<commit_message>
More data for Dublin and South Signed-off-by: Gerry Mulvenna <git@movingwifi.com>
</commit_message>
<xml_diff>
--- a/europarl/europarl-ireland-2019.xlsx
+++ b/europarl/europarl-ireland-2019.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="14220" windowHeight="8580" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="14220" windowHeight="8580" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Candidates" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="260">
   <si>
     <t>Candidate</t>
   </si>
@@ -791,6 +791,12 @@
   </si>
   <si>
     <t>Eames, Fidelma Healy</t>
+  </si>
+  <si>
+    <t>Count 15</t>
+  </si>
+  <si>
+    <t>Brennan, Allan eliminated</t>
   </si>
 </sst>
 </file>
@@ -2452,15 +2458,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD41"/>
+  <dimension ref="A1:AF41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="AA2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="AE2" sqref="AE2:AF20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>232</v>
       </c>
@@ -2509,8 +2518,11 @@
       <c r="AD1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AF1" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>3</v>
       </c>
@@ -2612,8 +2624,15 @@
       <c r="AD2" s="1">
         <v>59619</v>
       </c>
-    </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE2">
+        <f>IF(ISBLANK(AF2),-AD2,AF2-AD2)</f>
+        <v>3558</v>
+      </c>
+      <c r="AF2">
+        <v>63177</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>5</v>
       </c>
@@ -2715,8 +2734,15 @@
       <c r="AD3" s="1">
         <v>46704</v>
       </c>
-    </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE3">
+        <f>IF(ISBLANK(AF3),-AD3,AF3-AD3)</f>
+        <v>4928</v>
+      </c>
+      <c r="AF3">
+        <v>51632</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>9</v>
       </c>
@@ -2818,8 +2844,15 @@
       <c r="AD4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE4">
+        <f t="shared" ref="AE4:AE20" si="12">IF(ISBLANK(AF4),-AD4,AF4-AD4)</f>
+        <v>0</v>
+      </c>
+      <c r="AF4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2920,8 +2953,15 @@
       <c r="AD5" s="1">
         <v>73028</v>
       </c>
-    </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE5">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AF5" s="1">
+        <v>73028</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -3017,14 +3057,21 @@
         <v>52930</v>
       </c>
       <c r="AC6">
-        <f t="shared" ref="AC6:AC20" si="12">IF(ISBLANK(AD6),-AB6,AD6-AB6)</f>
+        <f t="shared" ref="AC6:AC20" si="13">IF(ISBLANK(AD6),-AB6,AD6-AB6)</f>
         <v>2822</v>
       </c>
       <c r="AD6" s="1">
         <v>55752</v>
       </c>
-    </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE6">
+        <f t="shared" si="12"/>
+        <v>9931</v>
+      </c>
+      <c r="AF6">
+        <v>65683</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>8</v>
       </c>
@@ -3120,14 +3167,21 @@
         <v>0</v>
       </c>
       <c r="AC7">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AD7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE7">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="AD7" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AF7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2</v>
       </c>
@@ -3223,14 +3277,21 @@
         <v>72446</v>
       </c>
       <c r="AC8">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>6134</v>
       </c>
       <c r="AD8" s="1">
         <v>78580</v>
       </c>
-    </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE8">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AF8" s="1">
+        <v>78580</v>
+      </c>
+    </row>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>6</v>
       </c>
@@ -3326,14 +3387,21 @@
         <v>25915</v>
       </c>
       <c r="AC9">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>3805</v>
       </c>
       <c r="AD9" s="1">
         <v>29720</v>
       </c>
-    </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE9">
+        <f t="shared" si="12"/>
+        <v>-29720</v>
+      </c>
+      <c r="AF9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>11</v>
       </c>
@@ -3429,14 +3497,21 @@
         <v>0</v>
       </c>
       <c r="AC10">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AD10" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE10">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="AD10" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AF10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>13</v>
       </c>
@@ -3532,14 +3607,21 @@
         <v>0</v>
       </c>
       <c r="AC11">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AD11" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE11">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="AD11" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AF11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -3635,14 +3717,21 @@
         <v>0</v>
       </c>
       <c r="AC12">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AD12" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE12">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="AD12" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AF12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>16</v>
       </c>
@@ -3738,14 +3827,21 @@
         <v>0</v>
       </c>
       <c r="AC13">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AD13">
+        <v>0</v>
+      </c>
+      <c r="AE13">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="AD13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AF13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>19</v>
       </c>
@@ -3841,14 +3937,21 @@
         <v>0</v>
       </c>
       <c r="AC14">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AD14">
+        <v>0</v>
+      </c>
+      <c r="AE14">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="AD14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AF14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>17</v>
       </c>
@@ -3944,14 +4047,21 @@
         <v>0</v>
       </c>
       <c r="AC15">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AD15">
+        <v>0</v>
+      </c>
+      <c r="AE15">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="AD15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AF15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>18</v>
       </c>
@@ -4047,14 +4157,21 @@
         <v>0</v>
       </c>
       <c r="AC16">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AD16">
+        <v>0</v>
+      </c>
+      <c r="AE16">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="AD16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AF16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -4150,14 +4267,21 @@
         <v>0</v>
       </c>
       <c r="AC17">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AD17">
+        <v>0</v>
+      </c>
+      <c r="AE17">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="AD17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AF17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>12</v>
       </c>
@@ -4253,14 +4377,21 @@
         <v>0</v>
       </c>
       <c r="AC18">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AD18">
+        <v>0</v>
+      </c>
+      <c r="AE18">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="AD18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AF18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>14</v>
       </c>
@@ -4356,14 +4487,21 @@
         <v>0</v>
       </c>
       <c r="AC19">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AD19">
+        <v>0</v>
+      </c>
+      <c r="AE19">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="AD19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AF19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>7</v>
       </c>
@@ -4459,14 +4597,21 @@
         <v>22205</v>
       </c>
       <c r="AC20">
+        <f t="shared" si="13"/>
+        <v>-22205</v>
+      </c>
+      <c r="AD20">
+        <v>0</v>
+      </c>
+      <c r="AE20">
         <f t="shared" si="12"/>
-        <v>-22205</v>
-      </c>
-      <c r="AD20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="AF20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>34</v>
       </c>
@@ -4487,192 +4632,192 @@
         <v>Ciaran Cuffe</v>
       </c>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>35</v>
       </c>
       <c r="D24">
-        <f t="shared" ref="D24:D41" si="13">FIND(",",B24)</f>
+        <f t="shared" ref="D24:D41" si="14">FIND(",",B24)</f>
         <v>11</v>
       </c>
       <c r="E24" t="str">
-        <f t="shared" ref="E24:E41" si="14">LEFT(B24,D24-1)</f>
+        <f t="shared" ref="E24:E41" si="15">LEFT(B24,D24-1)</f>
         <v>Fitzgerald</v>
       </c>
       <c r="F24" t="str">
-        <f t="shared" ref="F24:F41" si="15">RIGHT(B24,LEN(B24)-(D24+1))</f>
+        <f t="shared" ref="F24:F41" si="16">RIGHT(B24,LEN(B24)-(D24+1))</f>
         <v>Frances</v>
       </c>
       <c r="G24" t="str">
-        <f t="shared" ref="G24:G41" si="16">F24&amp;" "&amp;E24</f>
+        <f t="shared" ref="G24:G41" si="17">F24&amp;" "&amp;E24</f>
         <v>Frances Fitzgerald</v>
       </c>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>36</v>
       </c>
       <c r="D25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>8</v>
       </c>
       <c r="E25" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>Andrews</v>
       </c>
       <c r="F25" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>Barry</v>
       </c>
       <c r="G25" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>Barry Andrews</v>
       </c>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>37</v>
       </c>
       <c r="D26">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>5</v>
       </c>
       <c r="E26" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>Daly</v>
       </c>
       <c r="F26" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>Clare</v>
       </c>
       <c r="G26" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>Clare Daly</v>
       </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>38</v>
       </c>
       <c r="D27">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>7</v>
       </c>
       <c r="E27" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>Boylan</v>
       </c>
       <c r="F27" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>Lynn</v>
       </c>
       <c r="G27" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>Lynn Boylan</v>
       </c>
     </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>39</v>
       </c>
       <c r="D28">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>7</v>
       </c>
       <c r="E28" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>Gannon</v>
       </c>
       <c r="F28" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>Gary</v>
       </c>
       <c r="G28" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>Gary Gannon</v>
       </c>
     </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>40</v>
       </c>
       <c r="D29">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>6</v>
       </c>
       <c r="E29" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>White</v>
       </c>
       <c r="F29" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>Alex</v>
       </c>
       <c r="G29" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>Alex White</v>
       </c>
     </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>41</v>
       </c>
       <c r="D30">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>7</v>
       </c>
       <c r="E30" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>Durkan</v>
       </c>
       <c r="F30" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>Mark</v>
       </c>
       <c r="G30" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>Mark Durkan</v>
       </c>
     </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>42</v>
       </c>
       <c r="D31">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>6</v>
       </c>
       <c r="E31" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>Brien</v>
       </c>
       <c r="F31" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>Gillian</v>
       </c>
       <c r="G31" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>Gillian Brien</v>
       </c>
     </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>43</v>
       </c>
       <c r="D32">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>8</v>
       </c>
       <c r="E32" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>Higgins</v>
       </c>
       <c r="F32" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>Alice Mary</v>
       </c>
       <c r="G32" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>Alice Mary Higgins</v>
       </c>
     </row>
@@ -4681,19 +4826,19 @@
         <v>44</v>
       </c>
       <c r="D33">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>7</v>
       </c>
       <c r="E33" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>Gilroy</v>
       </c>
       <c r="F33" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>Ben</v>
       </c>
       <c r="G33" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>Ben Gilroy</v>
       </c>
     </row>
@@ -4702,19 +4847,19 @@
         <v>45</v>
       </c>
       <c r="D34">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>10</v>
       </c>
       <c r="E34" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>O'Doherty</v>
       </c>
       <c r="F34" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>Gemma</v>
       </c>
       <c r="G34" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>Gemma O'Doherty</v>
       </c>
     </row>
@@ -4723,19 +4868,19 @@
         <v>46</v>
       </c>
       <c r="D35">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>8</v>
       </c>
       <c r="E35" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>Harrold</v>
       </c>
       <c r="F35" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>Rita</v>
       </c>
       <c r="G35" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>Rita Harrold</v>
       </c>
     </row>
@@ -4744,19 +4889,19 @@
         <v>47</v>
       </c>
       <c r="D36">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>5</v>
       </c>
       <c r="E36" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>Ryan</v>
       </c>
       <c r="F36" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>Éilis</v>
       </c>
       <c r="G36" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>Éilis Ryan</v>
       </c>
     </row>
@@ -4765,19 +4910,19 @@
         <v>48</v>
       </c>
       <c r="D37">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>7</v>
       </c>
       <c r="E37" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>Murphy</v>
       </c>
       <c r="F37" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>Eamonn</v>
       </c>
       <c r="G37" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>Eamonn Murphy</v>
       </c>
     </row>
@@ -4786,19 +4931,19 @@
         <v>49</v>
       </c>
       <c r="D38">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>6</v>
       </c>
       <c r="E38" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>Kelly</v>
       </c>
       <c r="F38" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>Hermann</v>
       </c>
       <c r="G38" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>Hermann Kelly</v>
       </c>
     </row>
@@ -4807,19 +4952,19 @@
         <v>50</v>
       </c>
       <c r="D39">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>8</v>
       </c>
       <c r="E39" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>McNiffe</v>
       </c>
       <c r="F39" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>Aisling</v>
       </c>
       <c r="G39" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>Aisling McNiffe</v>
       </c>
     </row>
@@ -4828,19 +4973,19 @@
         <v>51</v>
       </c>
       <c r="D40">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>7</v>
       </c>
       <c r="E40" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>Mullan</v>
       </c>
       <c r="F40" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>Mark</v>
       </c>
       <c r="G40" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>Mark Mullan</v>
       </c>
     </row>
@@ -4849,19 +4994,19 @@
         <v>52</v>
       </c>
       <c r="D41">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>6</v>
       </c>
       <c r="E41" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>Lowth</v>
       </c>
       <c r="F41" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>Tony Bosco</v>
       </c>
       <c r="G41" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>Tony Bosco Lowth</v>
       </c>
     </row>
@@ -4919,28 +5064,28 @@
         <v>8130</v>
       </c>
       <c r="E2">
-        <f>IF(ISBLANK(F2),-D2,F2-D2)</f>
+        <f t="shared" ref="E2:E18" si="0">IF(ISBLANK(F2),-D2,F2-D2)</f>
         <v>96</v>
       </c>
       <c r="F2" s="1">
         <v>8226</v>
       </c>
       <c r="G2">
-        <f>IF(ISBLANK(H2),-F2,H2-F2)</f>
+        <f t="shared" ref="G2:G18" si="1">IF(ISBLANK(H2),-F2,H2-F2)</f>
         <v>20</v>
       </c>
       <c r="H2" s="1">
         <v>8246</v>
       </c>
       <c r="I2">
-        <f>IF(ISBLANK(J2),-H2,J2-H2)</f>
+        <f t="shared" ref="I2:I18" si="2">IF(ISBLANK(J2),-H2,J2-H2)</f>
         <v>91</v>
       </c>
       <c r="J2" s="1">
         <v>8337</v>
       </c>
       <c r="K2">
-        <f>IF(ISBLANK(L2),-J2,L2-J2)</f>
+        <f t="shared" ref="K2:K18" si="3">IF(ISBLANK(L2),-J2,L2-J2)</f>
         <v>28</v>
       </c>
       <c r="L2" s="1">
@@ -4959,28 +5104,28 @@
         <v>77619</v>
       </c>
       <c r="E3">
-        <f>IF(ISBLANK(F3),-D3,F3-D3)</f>
+        <f t="shared" si="0"/>
         <v>868</v>
       </c>
       <c r="F3" s="1">
         <v>78487</v>
       </c>
       <c r="G3">
-        <f>IF(ISBLANK(H3),-F3,H3-F3)</f>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="H3" s="1">
         <v>78513</v>
       </c>
       <c r="I3">
-        <f>IF(ISBLANK(J3),-H3,J3-H3)</f>
+        <f t="shared" si="2"/>
         <v>99</v>
       </c>
       <c r="J3" s="1">
         <v>78612</v>
       </c>
       <c r="K3">
-        <f>IF(ISBLANK(L3),-J3,L3-J3)</f>
+        <f t="shared" si="3"/>
         <v>41</v>
       </c>
       <c r="L3" s="1">
@@ -4999,28 +5144,28 @@
         <v>56650</v>
       </c>
       <c r="E4">
-        <f>IF(ISBLANK(F4),-D4,F4-D4)</f>
+        <f t="shared" si="0"/>
         <v>1198</v>
       </c>
       <c r="F4" s="1">
         <v>57848</v>
       </c>
       <c r="G4">
-        <f>IF(ISBLANK(H4),-F4,H4-F4)</f>
+        <f t="shared" si="1"/>
         <v>44</v>
       </c>
       <c r="H4" s="1">
         <v>57892</v>
       </c>
       <c r="I4">
-        <f>IF(ISBLANK(J4),-H4,J4-H4)</f>
+        <f t="shared" si="2"/>
         <v>142</v>
       </c>
       <c r="J4" s="1">
         <v>58034</v>
       </c>
       <c r="K4">
-        <f>IF(ISBLANK(L4),-J4,L4-J4)</f>
+        <f t="shared" si="3"/>
         <v>178</v>
       </c>
       <c r="L4" s="1">
@@ -5039,28 +5184,28 @@
         <v>15991</v>
       </c>
       <c r="E5">
-        <f>IF(ISBLANK(F5),-D5,F5-D5)</f>
+        <f t="shared" si="0"/>
         <v>477</v>
       </c>
       <c r="F5" s="1">
         <v>16468</v>
       </c>
       <c r="G5">
-        <f>IF(ISBLANK(H5),-F5,H5-F5)</f>
+        <f t="shared" si="1"/>
         <v>47</v>
       </c>
       <c r="H5" s="1">
         <v>16515</v>
       </c>
       <c r="I5">
-        <f>IF(ISBLANK(J5),-H5,J5-H5)</f>
+        <f t="shared" si="2"/>
         <v>106</v>
       </c>
       <c r="J5" s="1">
         <v>16621</v>
       </c>
       <c r="K5">
-        <f>IF(ISBLANK(L5),-J5,L5-J5)</f>
+        <f t="shared" si="3"/>
         <v>143</v>
       </c>
       <c r="L5" s="1">
@@ -5079,28 +5224,28 @@
         <v>85034</v>
       </c>
       <c r="E6">
-        <f>IF(ISBLANK(F6),-D6,F6-D6)</f>
+        <f t="shared" si="0"/>
         <v>1872</v>
       </c>
       <c r="F6" s="1">
         <v>86906</v>
       </c>
       <c r="G6">
-        <f>IF(ISBLANK(H6),-F6,H6-F6)</f>
+        <f t="shared" si="1"/>
         <v>102</v>
       </c>
       <c r="H6" s="1">
         <v>87008</v>
       </c>
       <c r="I6">
-        <f>IF(ISBLANK(J6),-H6,J6-H6)</f>
+        <f t="shared" si="2"/>
         <v>180</v>
       </c>
       <c r="J6" s="1">
         <v>87188</v>
       </c>
       <c r="K6">
-        <f>IF(ISBLANK(L6),-J6,L6-J6)</f>
+        <f t="shared" si="3"/>
         <v>145</v>
       </c>
       <c r="L6" s="1">
@@ -5119,28 +5264,28 @@
         <v>1352</v>
       </c>
       <c r="E7">
-        <f>IF(ISBLANK(F7),-D7,F7-D7)</f>
+        <f t="shared" si="0"/>
         <v>48</v>
       </c>
       <c r="F7" s="1">
         <v>1400</v>
       </c>
       <c r="G7">
-        <f>IF(ISBLANK(H7),-F7,H7-F7)</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="H7" s="1">
         <v>1412</v>
       </c>
       <c r="I7">
-        <f>IF(ISBLANK(J7),-H7,J7-H7)</f>
+        <f t="shared" si="2"/>
         <v>-1412</v>
       </c>
       <c r="J7" s="1">
         <v>0</v>
       </c>
       <c r="K7">
-        <f>IF(ISBLANK(L7),-J7,L7-J7)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L7" s="1">
@@ -5159,28 +5304,28 @@
         <v>12378</v>
       </c>
       <c r="E8">
-        <f>IF(ISBLANK(F8),-D8,F8-D8)</f>
+        <f t="shared" si="0"/>
         <v>653</v>
       </c>
       <c r="F8" s="1">
         <v>13031</v>
       </c>
       <c r="G8">
-        <f>IF(ISBLANK(H8),-F8,H8-F8)</f>
+        <f t="shared" si="1"/>
         <v>34</v>
       </c>
       <c r="H8" s="1">
         <v>13065</v>
       </c>
       <c r="I8">
-        <f>IF(ISBLANK(J8),-H8,J8-H8)</f>
+        <f t="shared" si="2"/>
         <v>85</v>
       </c>
       <c r="J8" s="1">
         <v>13150</v>
       </c>
       <c r="K8">
-        <f>IF(ISBLANK(L8),-J8,L8-J8)</f>
+        <f t="shared" si="3"/>
         <v>47</v>
       </c>
       <c r="L8" s="1">
@@ -5199,28 +5344,28 @@
         <v>2450</v>
       </c>
       <c r="E9">
-        <f>IF(ISBLANK(F9),-D9,F9-D9)</f>
+        <f t="shared" si="0"/>
         <v>112</v>
       </c>
       <c r="F9" s="1">
         <v>2562</v>
       </c>
       <c r="G9">
-        <f>IF(ISBLANK(H9),-F9,H9-F9)</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="H9" s="1">
         <v>2577</v>
       </c>
       <c r="I9">
-        <f>IF(ISBLANK(J9),-H9,J9-H9)</f>
+        <f t="shared" si="2"/>
         <v>77</v>
       </c>
       <c r="J9" s="1">
         <v>2654</v>
       </c>
       <c r="K9">
-        <f>IF(ISBLANK(L9),-J9,L9-J9)</f>
+        <f t="shared" si="3"/>
         <v>40</v>
       </c>
       <c r="L9" s="1">
@@ -5239,28 +5384,28 @@
         <v>134630</v>
       </c>
       <c r="E10">
-        <f>IF(ISBLANK(F10),-D10,F10-D10)</f>
+        <f t="shared" si="0"/>
         <v>-15644</v>
       </c>
       <c r="F10">
         <v>118986</v>
       </c>
       <c r="G10">
-        <f>IF(ISBLANK(H10),-F10,H10-F10)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H10">
         <v>118986</v>
       </c>
       <c r="I10">
-        <f>IF(ISBLANK(J10),-H10,J10-H10)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J10">
         <v>118986</v>
       </c>
       <c r="K10">
-        <f>IF(ISBLANK(L10),-J10,L10-J10)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L10">
@@ -5279,28 +5424,28 @@
         <v>51019</v>
       </c>
       <c r="E11">
-        <f>IF(ISBLANK(F11),-D11,F11-D11)</f>
+        <f t="shared" si="0"/>
         <v>1712</v>
       </c>
       <c r="F11" s="1">
         <v>52731</v>
       </c>
       <c r="G11">
-        <f>IF(ISBLANK(H11),-F11,H11-F11)</f>
+        <f t="shared" si="1"/>
         <v>90</v>
       </c>
       <c r="H11" s="1">
         <v>52821</v>
       </c>
       <c r="I11">
-        <f>IF(ISBLANK(J11),-H11,J11-H11)</f>
+        <f t="shared" si="2"/>
         <v>155</v>
       </c>
       <c r="J11" s="1">
         <v>52976</v>
       </c>
       <c r="K11">
-        <f>IF(ISBLANK(L11),-J11,L11-J11)</f>
+        <f t="shared" si="3"/>
         <v>92</v>
       </c>
       <c r="L11" s="1">
@@ -5319,28 +5464,28 @@
         <v>1322</v>
       </c>
       <c r="E12">
-        <f>IF(ISBLANK(F12),-D12,F12-D12)</f>
+        <f t="shared" si="0"/>
         <v>53</v>
       </c>
       <c r="F12" s="1">
         <v>1375</v>
       </c>
       <c r="G12">
-        <f>IF(ISBLANK(H12),-F12,H12-F12)</f>
+        <f t="shared" si="1"/>
         <v>71</v>
       </c>
       <c r="H12" s="1">
         <v>1446</v>
       </c>
       <c r="I12">
-        <f>IF(ISBLANK(J12),-H12,J12-H12)</f>
+        <f t="shared" si="2"/>
         <v>44</v>
       </c>
       <c r="J12" s="1">
         <v>1490</v>
       </c>
       <c r="K12">
-        <f>IF(ISBLANK(L12),-J12,L12-J12)</f>
+        <f t="shared" si="3"/>
         <v>-1490</v>
       </c>
       <c r="L12" s="1">
@@ -5359,28 +5504,28 @@
         <v>789</v>
       </c>
       <c r="E13">
-        <f>IF(ISBLANK(F13),-D13,F13-D13)</f>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="F13">
         <v>811</v>
       </c>
       <c r="G13">
-        <f>IF(ISBLANK(H13),-F13,H13-F13)</f>
+        <f t="shared" si="1"/>
         <v>-811</v>
       </c>
       <c r="H13" s="1">
         <v>0</v>
       </c>
       <c r="I13">
-        <f>IF(ISBLANK(J13),-H13,J13-H13)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J13" s="1">
         <v>0</v>
       </c>
       <c r="K13">
-        <f>IF(ISBLANK(L13),-J13,L13-J13)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L13" s="1">
@@ -5399,28 +5544,28 @@
         <v>3132</v>
       </c>
       <c r="E14">
-        <f>IF(ISBLANK(F14),-D14,F14-D14)</f>
+        <f t="shared" si="0"/>
         <v>104</v>
       </c>
       <c r="F14" s="1">
         <v>3236</v>
       </c>
       <c r="G14">
-        <f>IF(ISBLANK(H14),-F14,H14-F14)</f>
+        <f t="shared" si="1"/>
         <v>77</v>
       </c>
       <c r="H14" s="1">
         <v>3313</v>
       </c>
       <c r="I14">
-        <f>IF(ISBLANK(J14),-H14,J14-H14)</f>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="J14" s="1">
         <v>3326</v>
       </c>
       <c r="K14">
-        <f>IF(ISBLANK(L14),-J14,L14-J14)</f>
+        <f t="shared" si="3"/>
         <v>151</v>
       </c>
       <c r="L14" s="1">
@@ -5439,28 +5584,28 @@
         <v>6897</v>
       </c>
       <c r="E15">
-        <f>IF(ISBLANK(F15),-D15,F15-D15)</f>
+        <f t="shared" si="0"/>
         <v>303</v>
       </c>
       <c r="F15" s="1">
         <v>7200</v>
       </c>
       <c r="G15">
-        <f>IF(ISBLANK(H15),-F15,H15-F15)</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="H15" s="1">
         <v>7220</v>
       </c>
       <c r="I15">
-        <f>IF(ISBLANK(J15),-H15,J15-H15)</f>
+        <f t="shared" si="2"/>
         <v>84</v>
       </c>
       <c r="J15" s="1">
         <v>7304</v>
       </c>
       <c r="K15">
-        <f>IF(ISBLANK(L15),-J15,L15-J15)</f>
+        <f t="shared" si="3"/>
         <v>141</v>
       </c>
       <c r="L15" s="1">
@@ -5479,28 +5624,28 @@
         <v>30220</v>
       </c>
       <c r="E16">
-        <f>IF(ISBLANK(F16),-D16,F16-D16)</f>
+        <f t="shared" si="0"/>
         <v>864</v>
       </c>
       <c r="F16" s="1">
         <v>31084</v>
       </c>
       <c r="G16">
-        <f>IF(ISBLANK(H16),-F16,H16-F16)</f>
+        <f t="shared" si="1"/>
         <v>38</v>
       </c>
       <c r="H16" s="1">
         <v>31122</v>
       </c>
       <c r="I16">
-        <f>IF(ISBLANK(J16),-H16,J16-H16)</f>
+        <f t="shared" si="2"/>
         <v>21</v>
       </c>
       <c r="J16" s="1">
         <v>31143</v>
       </c>
       <c r="K16">
-        <f>IF(ISBLANK(L16),-J16,L16-J16)</f>
+        <f t="shared" si="3"/>
         <v>55</v>
       </c>
       <c r="L16" s="1">
@@ -5519,28 +5664,28 @@
         <v>42814</v>
       </c>
       <c r="E17">
-        <f>IF(ISBLANK(F17),-D17,F17-D17)</f>
+        <f t="shared" si="0"/>
         <v>1226</v>
       </c>
       <c r="F17" s="1">
         <v>44040</v>
       </c>
       <c r="G17">
-        <f>IF(ISBLANK(H17),-F17,H17-F17)</f>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="H17" s="1">
         <v>44059</v>
       </c>
       <c r="I17">
-        <f>IF(ISBLANK(J17),-H17,J17-H17)</f>
+        <f t="shared" si="2"/>
         <v>17</v>
       </c>
       <c r="J17" s="1">
         <v>44076</v>
       </c>
       <c r="K17">
-        <f>IF(ISBLANK(L17),-J17,L17-J17)</f>
+        <f t="shared" si="3"/>
         <v>54</v>
       </c>
       <c r="L17" s="1">
@@ -5559,28 +5704,28 @@
         <v>64500</v>
       </c>
       <c r="E18">
-        <f>IF(ISBLANK(F18),-D18,F18-D18)</f>
+        <f t="shared" si="0"/>
         <v>6036</v>
       </c>
       <c r="F18" s="1">
         <v>70536</v>
       </c>
       <c r="G18">
-        <f>IF(ISBLANK(H18),-F18,H18-F18)</f>
+        <f t="shared" si="1"/>
         <v>83</v>
       </c>
       <c r="H18" s="1">
         <v>70619</v>
       </c>
       <c r="I18">
-        <f>IF(ISBLANK(J18),-H18,J18-H18)</f>
+        <f t="shared" si="2"/>
         <v>41</v>
       </c>
       <c r="J18" s="1">
         <v>70660</v>
       </c>
       <c r="K18">
-        <f>IF(ISBLANK(L18),-J18,L18-J18)</f>
+        <f t="shared" si="3"/>
         <v>71</v>
       </c>
       <c r="L18" s="1">
@@ -5634,19 +5779,19 @@
         <v>197</v>
       </c>
       <c r="D21">
-        <f t="shared" ref="D21:D36" si="0">FIND(",",B21)</f>
+        <f t="shared" ref="D21:D36" si="4">FIND(",",B21)</f>
         <v>9</v>
       </c>
       <c r="E21" t="str">
-        <f t="shared" ref="E21:E36" si="1">LEFT(B21,D21-1)</f>
+        <f t="shared" ref="E21:E36" si="5">LEFT(B21,D21-1)</f>
         <v>Flanagan</v>
       </c>
       <c r="F21" t="str">
-        <f t="shared" ref="F21:F36" si="2">RIGHT(B21,LEN(B21)-(D21+1))</f>
+        <f t="shared" ref="F21:F36" si="6">RIGHT(B21,LEN(B21)-(D21+1))</f>
         <v>Luke 'Ming'</v>
       </c>
       <c r="G21" t="str">
-        <f t="shared" ref="G21:G36" si="3">F21&amp;" "&amp;E21</f>
+        <f t="shared" ref="G21:G36" si="7">F21&amp;" "&amp;E21</f>
         <v>Luke 'Ming' Flanagan</v>
       </c>
       <c r="J21" t="s">
@@ -5664,19 +5809,19 @@
         <v>198</v>
       </c>
       <c r="D22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
       <c r="E22" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>Carthy</v>
       </c>
       <c r="F22" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>Matt</v>
       </c>
       <c r="G22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>Matt Carthy</v>
       </c>
       <c r="J22" t="s">
@@ -5706,19 +5851,19 @@
         <v>199</v>
       </c>
       <c r="D23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="E23" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>Walsh</v>
       </c>
       <c r="F23" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>Maria</v>
       </c>
       <c r="G23" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>Maria Walsh</v>
       </c>
       <c r="J23" t="s">
@@ -5748,19 +5893,19 @@
         <v>200</v>
       </c>
       <c r="D24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="E24" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>Casey</v>
       </c>
       <c r="F24" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>Peter</v>
       </c>
       <c r="G24" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>Peter Casey</v>
       </c>
       <c r="J24" t="s">
@@ -5790,19 +5935,19 @@
         <v>201</v>
       </c>
       <c r="D25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
       <c r="E25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>McHugh</v>
       </c>
       <c r="F25" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>Saoirse</v>
       </c>
       <c r="G25" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>Saoirse McHugh</v>
       </c>
       <c r="J25" t="s">
@@ -5832,19 +5977,19 @@
         <v>202</v>
       </c>
       <c r="D26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="E26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>Smith</v>
       </c>
       <c r="F26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>Brendan</v>
       </c>
       <c r="G26" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>Brendan Smith</v>
       </c>
       <c r="J26" t="s">
@@ -5874,19 +6019,19 @@
         <v>203</v>
       </c>
       <c r="D27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>9</v>
       </c>
       <c r="E27" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>Rabbitte</v>
       </c>
       <c r="F27" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>Anne</v>
       </c>
       <c r="G27" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>Anne Rabbitte</v>
       </c>
       <c r="J27" t="s">
@@ -5916,19 +6061,19 @@
         <v>204</v>
       </c>
       <c r="D28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
       <c r="E28" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>Healy Eames</v>
       </c>
       <c r="F28" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>Fidelma</v>
       </c>
       <c r="G28" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>Fidelma Healy Eames</v>
       </c>
       <c r="J28" t="s">
@@ -5958,19 +6103,19 @@
         <v>205</v>
       </c>
       <c r="D29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>9</v>
       </c>
       <c r="E29" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>Hannigan</v>
       </c>
       <c r="F29" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>Dominic</v>
       </c>
       <c r="G29" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>Dominic Hannigan</v>
       </c>
       <c r="J29" t="s">
@@ -6000,19 +6145,19 @@
         <v>206</v>
       </c>
       <c r="D30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="E30" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>Brennan</v>
       </c>
       <c r="F30" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>Cyril</v>
       </c>
       <c r="G30" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>Cyril Brennan</v>
       </c>
       <c r="J30" t="s">
@@ -6042,19 +6187,19 @@
         <v>207</v>
       </c>
       <c r="D31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
       <c r="E31" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>O'Dowd</v>
       </c>
       <c r="F31" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>Michael</v>
       </c>
       <c r="G31" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>Michael O'Dowd</v>
       </c>
       <c r="J31" t="s">
@@ -6084,19 +6229,19 @@
         <v>208</v>
       </c>
       <c r="D32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>9</v>
       </c>
       <c r="E32" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>O'Connor</v>
       </c>
       <c r="F32" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>Olive</v>
       </c>
       <c r="G32" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>Olive O'Connor</v>
       </c>
       <c r="J32" t="s">
@@ -6126,19 +6271,19 @@
         <v>209</v>
       </c>
       <c r="D33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="E33" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>Mahapatra</v>
       </c>
       <c r="F33" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>Dilip</v>
       </c>
       <c r="G33" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>Dilip Mahapatra</v>
       </c>
       <c r="J33" t="s">
@@ -6168,19 +6313,19 @@
         <v>210</v>
       </c>
       <c r="D34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
       <c r="E34" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>Greene</v>
       </c>
       <c r="F34" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>Patrick</v>
       </c>
       <c r="G34" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>Patrick Greene</v>
       </c>
       <c r="J34" t="s">
@@ -6210,19 +6355,19 @@
         <v>211</v>
       </c>
       <c r="D35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
       <c r="E35" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>Miller</v>
       </c>
       <c r="F35" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>James</v>
       </c>
       <c r="G35" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>James Miller</v>
       </c>
       <c r="J35" t="s">
@@ -6246,19 +6391,19 @@
         <v>212</v>
       </c>
       <c r="D36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="E36" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>Mulcahy</v>
       </c>
       <c r="F36" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>Diarmaid</v>
       </c>
       <c r="G36" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>Diarmaid Mulcahy</v>
       </c>
       <c r="J36" t="s">
@@ -6306,8 +6451,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD49"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2:R24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6377,46 +6522,53 @@
         <v>4665</v>
       </c>
       <c r="E2">
-        <f t="shared" ref="E2:E24" si="0">IF(ISBLANK(F2),-D2,F2-D2)</f>
+        <f>IF(ISBLANK(F2),-D2,F2-D2)</f>
         <v>26</v>
       </c>
       <c r="F2" s="1">
         <v>4691</v>
       </c>
       <c r="G2">
-        <f t="shared" ref="G2:G24" si="1">IF(ISBLANK(H2),-F2,H2-F2)</f>
+        <f>IF(ISBLANK(H2),-F2,H2-F2)</f>
         <v>43</v>
       </c>
       <c r="H2" s="1">
         <v>4734</v>
       </c>
       <c r="I2">
-        <f t="shared" ref="I2:I24" si="2">IF(ISBLANK(J2),-H2,J2-H2)</f>
+        <f>IF(ISBLANK(J2),-H2,J2-H2)</f>
         <v>57</v>
       </c>
       <c r="J2" s="1">
         <v>4791</v>
       </c>
       <c r="K2">
-        <f t="shared" ref="K2:K24" si="3">IF(ISBLANK(L2),-J2,L2-J2)</f>
+        <f>IF(ISBLANK(L2),-J2,L2-J2)</f>
         <v>50</v>
       </c>
       <c r="L2" s="1">
         <v>4841</v>
       </c>
       <c r="M2">
-        <f t="shared" ref="M2:M24" si="4">IF(ISBLANK(N2),-L2,N2-L2)</f>
+        <f>IF(ISBLANK(N2),-L2,N2-L2)</f>
         <v>115</v>
       </c>
       <c r="N2" s="1">
         <v>4956</v>
       </c>
       <c r="O2">
-        <f t="shared" ref="O2:O24" si="5">IF(ISBLANK(P2),-N2,P2-N2)</f>
+        <f>IF(ISBLANK(P2),-N2,P2-N2)</f>
         <v>72</v>
       </c>
       <c r="P2" s="1">
         <v>5028</v>
+      </c>
+      <c r="Q2">
+        <f>IF(ISBLANK(R2),-P2,R2-P2)</f>
+        <v>104</v>
+      </c>
+      <c r="R2" s="1">
+        <v>5132</v>
       </c>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.25">
@@ -6430,46 +6582,53 @@
         <v>69166</v>
       </c>
       <c r="E3">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F3),-D3,F3-D3)</f>
         <v>35</v>
       </c>
       <c r="F3" s="1">
         <v>69201</v>
       </c>
       <c r="G3">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H3),-F3,H3-F3)</f>
         <v>71</v>
       </c>
       <c r="H3" s="1">
         <v>69272</v>
       </c>
       <c r="I3">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J3),-H3,J3-H3)</f>
         <v>44</v>
       </c>
       <c r="J3" s="1">
         <v>69316</v>
       </c>
       <c r="K3">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L3),-J3,L3-J3)</f>
         <v>66</v>
       </c>
       <c r="L3" s="1">
         <v>69382</v>
       </c>
       <c r="M3">
-        <f t="shared" si="4"/>
+        <f>IF(ISBLANK(N3),-L3,N3-L3)</f>
         <v>129</v>
       </c>
       <c r="N3" s="1">
         <v>69511</v>
       </c>
       <c r="O3">
-        <f t="shared" si="5"/>
+        <f>IF(ISBLANK(P3),-N3,P3-N3)</f>
         <v>45</v>
       </c>
       <c r="P3" s="1">
         <v>69556</v>
+      </c>
+      <c r="Q3">
+        <f>IF(ISBLANK(R3),-P3,R3-P3)</f>
+        <v>116</v>
+      </c>
+      <c r="R3" s="1">
+        <v>69672</v>
       </c>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.25">
@@ -6483,46 +6642,53 @@
         <v>10582</v>
       </c>
       <c r="E4">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F4),-D4,F4-D4)</f>
         <v>57</v>
       </c>
       <c r="F4" s="1">
         <v>10639</v>
       </c>
       <c r="G4">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H4),-F4,H4-F4)</f>
         <v>106</v>
       </c>
       <c r="H4" s="1">
         <v>10745</v>
       </c>
       <c r="I4">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J4),-H4,J4-H4)</f>
         <v>138</v>
       </c>
       <c r="J4" s="1">
         <v>10883</v>
       </c>
       <c r="K4">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L4),-J4,L4-J4)</f>
         <v>54</v>
       </c>
       <c r="L4" s="1">
         <v>10937</v>
       </c>
       <c r="M4">
-        <f t="shared" si="4"/>
+        <f>IF(ISBLANK(N4),-L4,N4-L4)</f>
         <v>300</v>
       </c>
       <c r="N4" s="1">
         <v>11237</v>
       </c>
       <c r="O4">
-        <f t="shared" si="5"/>
+        <f>IF(ISBLANK(P4),-N4,P4-N4)</f>
         <v>159</v>
       </c>
       <c r="P4" s="1">
         <v>11396</v>
+      </c>
+      <c r="Q4">
+        <f>IF(ISBLANK(R4),-P4,R4-P4)</f>
+        <v>322</v>
+      </c>
+      <c r="R4" s="1">
+        <v>11718</v>
       </c>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.25">
@@ -6536,46 +6702,53 @@
         <v>64605</v>
       </c>
       <c r="E5">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F5),-D5,F5-D5)</f>
         <v>26</v>
       </c>
       <c r="F5" s="1">
         <v>64631</v>
       </c>
       <c r="G5">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H5),-F5,H5-F5)</f>
         <v>61</v>
       </c>
       <c r="H5" s="1">
         <v>64692</v>
       </c>
       <c r="I5">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J5),-H5,J5-H5)</f>
         <v>71</v>
       </c>
       <c r="J5" s="1">
         <v>64763</v>
       </c>
       <c r="K5">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L5),-J5,L5-J5)</f>
         <v>136</v>
       </c>
       <c r="L5" s="1">
         <v>64899</v>
       </c>
       <c r="M5">
-        <f t="shared" si="4"/>
+        <f>IF(ISBLANK(N5),-L5,N5-L5)</f>
         <v>106</v>
       </c>
       <c r="N5" s="1">
         <v>65005</v>
       </c>
       <c r="O5">
-        <f t="shared" si="5"/>
+        <f>IF(ISBLANK(P5),-N5,P5-N5)</f>
         <v>110</v>
       </c>
       <c r="P5" s="1">
         <v>65115</v>
+      </c>
+      <c r="Q5">
+        <f>IF(ISBLANK(R5),-P5,R5-P5)</f>
+        <v>137</v>
+      </c>
+      <c r="R5" s="1">
+        <v>65252</v>
       </c>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.25">
@@ -6589,46 +6762,53 @@
         <v>38738</v>
       </c>
       <c r="E6">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F6),-D6,F6-D6)</f>
         <v>17</v>
       </c>
       <c r="F6" s="1">
         <v>38755</v>
       </c>
       <c r="G6">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H6),-F6,H6-F6)</f>
         <v>33</v>
       </c>
       <c r="H6" s="1">
         <v>38788</v>
       </c>
       <c r="I6">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J6),-H6,J6-H6)</f>
         <v>16</v>
       </c>
       <c r="J6" s="1">
         <v>38804</v>
       </c>
       <c r="K6">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L6),-J6,L6-J6)</f>
         <v>38</v>
       </c>
       <c r="L6" s="1">
         <v>38842</v>
       </c>
       <c r="M6">
-        <f t="shared" si="4"/>
+        <f>IF(ISBLANK(N6),-L6,N6-L6)</f>
         <v>84</v>
       </c>
       <c r="N6" s="1">
         <v>38926</v>
       </c>
       <c r="O6">
-        <f t="shared" si="5"/>
+        <f>IF(ISBLANK(P6),-N6,P6-N6)</f>
         <v>24</v>
       </c>
       <c r="P6" s="1">
         <v>38950</v>
+      </c>
+      <c r="Q6">
+        <f>IF(ISBLANK(R6),-P6,R6-P6)</f>
+        <v>46</v>
+      </c>
+      <c r="R6" s="1">
+        <v>38996</v>
       </c>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.25">
@@ -6642,45 +6822,52 @@
         <v>3182</v>
       </c>
       <c r="E7">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F7),-D7,F7-D7)</f>
         <v>15</v>
       </c>
       <c r="F7" s="1">
         <v>3197</v>
       </c>
       <c r="G7">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H7),-F7,H7-F7)</f>
         <v>60</v>
       </c>
       <c r="H7" s="1">
         <v>3257</v>
       </c>
       <c r="I7">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J7),-H7,J7-H7)</f>
         <v>43</v>
       </c>
       <c r="J7" s="1">
         <v>3300</v>
       </c>
       <c r="K7">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L7),-J7,L7-J7)</f>
         <v>32</v>
       </c>
       <c r="L7" s="1">
         <v>3332</v>
       </c>
       <c r="M7">
-        <f t="shared" si="4"/>
+        <f>IF(ISBLANK(N7),-L7,N7-L7)</f>
         <v>-3332</v>
       </c>
       <c r="N7" s="1">
         <v>0</v>
       </c>
       <c r="O7">
-        <f t="shared" si="5"/>
+        <f>IF(ISBLANK(P7),-N7,P7-N7)</f>
         <v>0</v>
       </c>
       <c r="P7" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <f>IF(ISBLANK(R7),-P7,R7-P7)</f>
+        <v>0</v>
+      </c>
+      <c r="R7" s="1">
         <v>0</v>
       </c>
     </row>
@@ -6695,46 +6882,53 @@
         <v>9306</v>
       </c>
       <c r="E8">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F8),-D8,F8-D8)</f>
         <v>25</v>
       </c>
       <c r="F8" s="1">
         <v>9331</v>
       </c>
       <c r="G8">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H8),-F8,H8-F8)</f>
         <v>70</v>
       </c>
       <c r="H8" s="1">
         <v>9401</v>
       </c>
       <c r="I8">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J8),-H8,J8-H8)</f>
         <v>35</v>
       </c>
       <c r="J8" s="1">
         <v>9436</v>
       </c>
       <c r="K8">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L8),-J8,L8-J8)</f>
         <v>60</v>
       </c>
       <c r="L8" s="1">
         <v>9496</v>
       </c>
       <c r="M8">
-        <f t="shared" si="4"/>
+        <f>IF(ISBLANK(N8),-L8,N8-L8)</f>
         <v>228</v>
       </c>
       <c r="N8" s="1">
         <v>9724</v>
       </c>
       <c r="O8">
-        <f t="shared" si="5"/>
+        <f>IF(ISBLANK(P8),-N8,P8-N8)</f>
         <v>145</v>
       </c>
       <c r="P8" s="1">
         <v>9869</v>
+      </c>
+      <c r="Q8">
+        <f>IF(ISBLANK(R8),-P8,R8-P8)</f>
+        <v>106</v>
+      </c>
+      <c r="R8" s="1">
+        <v>9975</v>
       </c>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.25">
@@ -6748,46 +6942,53 @@
         <v>7475</v>
       </c>
       <c r="E9">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F9),-D9,F9-D9)</f>
         <v>23</v>
       </c>
       <c r="F9" s="1">
         <v>7498</v>
       </c>
       <c r="G9">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H9),-F9,H9-F9)</f>
         <v>98</v>
       </c>
       <c r="H9" s="1">
         <v>7596</v>
       </c>
       <c r="I9">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J9),-H9,J9-H9)</f>
         <v>142</v>
       </c>
       <c r="J9" s="1">
         <v>7738</v>
       </c>
       <c r="K9">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L9),-J9,L9-J9)</f>
         <v>70</v>
       </c>
       <c r="L9" s="1">
         <v>7808</v>
       </c>
       <c r="M9">
-        <f t="shared" si="4"/>
+        <f>IF(ISBLANK(N9),-L9,N9-L9)</f>
         <v>197</v>
       </c>
       <c r="N9" s="1">
         <v>8005</v>
       </c>
       <c r="O9">
-        <f t="shared" si="5"/>
+        <f>IF(ISBLANK(P9),-N9,P9-N9)</f>
         <v>192</v>
       </c>
       <c r="P9" s="1">
         <v>8197</v>
+      </c>
+      <c r="Q9">
+        <f>IF(ISBLANK(R9),-P9,R9-P9)</f>
+        <v>176</v>
+      </c>
+      <c r="R9" s="1">
+        <v>8373</v>
       </c>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.25">
@@ -6801,46 +7002,53 @@
         <v>84083</v>
       </c>
       <c r="E10">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F10),-D10,F10-D10)</f>
         <v>23</v>
       </c>
       <c r="F10" s="1">
         <v>84106</v>
       </c>
       <c r="G10">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H10),-F10,H10-F10)</f>
         <v>58</v>
       </c>
       <c r="H10" s="1">
         <v>84164</v>
       </c>
       <c r="I10">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J10),-H10,J10-H10)</f>
         <v>74</v>
       </c>
       <c r="J10" s="1">
         <v>84238</v>
       </c>
       <c r="K10">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L10),-J10,L10-J10)</f>
         <v>150</v>
       </c>
       <c r="L10" s="1">
         <v>84388</v>
       </c>
       <c r="M10">
-        <f t="shared" si="4"/>
+        <f>IF(ISBLANK(N10),-L10,N10-L10)</f>
         <v>171</v>
       </c>
       <c r="N10" s="1">
         <v>84559</v>
       </c>
       <c r="O10">
-        <f t="shared" si="5"/>
+        <f>IF(ISBLANK(P10),-N10,P10-N10)</f>
         <v>95</v>
       </c>
       <c r="P10" s="1">
         <v>84654</v>
+      </c>
+      <c r="Q10">
+        <f>IF(ISBLANK(R10),-P10,R10-P10)</f>
+        <v>187</v>
+      </c>
+      <c r="R10" s="1">
+        <v>84841</v>
       </c>
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.25">
@@ -6854,46 +7062,53 @@
         <v>118444</v>
       </c>
       <c r="E11">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F11),-D11,F11-D11)</f>
         <v>45</v>
       </c>
       <c r="F11" s="1">
         <v>118489</v>
       </c>
       <c r="G11">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H11),-F11,H11-F11)</f>
         <v>186</v>
       </c>
       <c r="H11" s="1">
         <v>118675</v>
       </c>
       <c r="I11">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J11),-H11,J11-H11)</f>
         <v>98</v>
       </c>
       <c r="J11" s="1">
         <v>118773</v>
       </c>
       <c r="K11">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L11),-J11,L11-J11)</f>
         <v>350</v>
       </c>
       <c r="L11" s="1">
         <v>119123</v>
       </c>
       <c r="M11">
-        <f t="shared" si="4"/>
+        <f>IF(ISBLANK(N11),-L11,N11-L11)</f>
         <v>257</v>
       </c>
       <c r="N11" s="1">
         <v>119380</v>
       </c>
       <c r="O11">
-        <f t="shared" si="5"/>
+        <f>IF(ISBLANK(P11),-N11,P11-N11)</f>
         <v>165</v>
       </c>
       <c r="P11" s="1">
         <v>119545</v>
+      </c>
+      <c r="Q11">
+        <f>IF(ISBLANK(R11),-P11,R11-P11)</f>
+        <v>170</v>
+      </c>
+      <c r="R11" s="1">
+        <v>119715</v>
       </c>
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.25">
@@ -6907,45 +7122,52 @@
         <v>2395</v>
       </c>
       <c r="E12">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F12),-D12,F12-D12)</f>
         <v>14</v>
       </c>
       <c r="F12" s="1">
         <v>2409</v>
       </c>
       <c r="G12">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H12),-F12,H12-F12)</f>
         <v>-2409</v>
       </c>
       <c r="H12" s="1">
         <v>0</v>
       </c>
       <c r="I12">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J12),-H12,J12-H12)</f>
         <v>0</v>
       </c>
       <c r="J12" s="1">
         <v>0</v>
       </c>
       <c r="K12">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L12),-J12,L12-J12)</f>
         <v>0</v>
       </c>
       <c r="L12" s="1">
         <v>0</v>
       </c>
       <c r="M12">
-        <f t="shared" si="4"/>
+        <f>IF(ISBLANK(N12),-L12,N12-L12)</f>
         <v>0</v>
       </c>
       <c r="N12" s="1">
         <v>0</v>
       </c>
       <c r="O12">
-        <f t="shared" si="5"/>
+        <f>IF(ISBLANK(P12),-N12,P12-N12)</f>
         <v>0</v>
       </c>
       <c r="P12" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <f>IF(ISBLANK(R12),-P12,R12-P12)</f>
+        <v>0</v>
+      </c>
+      <c r="R12" s="1">
         <v>0</v>
       </c>
     </row>
@@ -6960,46 +7182,53 @@
         <v>9423</v>
       </c>
       <c r="E13">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F13),-D13,F13-D13)</f>
         <v>32</v>
       </c>
       <c r="F13" s="1">
         <v>9455</v>
       </c>
       <c r="G13">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H13),-F13,H13-F13)</f>
         <v>325</v>
       </c>
       <c r="H13" s="1">
         <v>9780</v>
       </c>
       <c r="I13">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J13),-H13,J13-H13)</f>
         <v>75</v>
       </c>
       <c r="J13" s="1">
         <v>9855</v>
       </c>
       <c r="K13">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L13),-J13,L13-J13)</f>
         <v>114</v>
       </c>
       <c r="L13" s="1">
         <v>9969</v>
       </c>
       <c r="M13">
-        <f t="shared" si="4"/>
+        <f>IF(ISBLANK(N13),-L13,N13-L13)</f>
         <v>280</v>
       </c>
       <c r="N13" s="1">
         <v>10249</v>
       </c>
       <c r="O13">
-        <f t="shared" si="5"/>
+        <f>IF(ISBLANK(P13),-N13,P13-N13)</f>
         <v>78</v>
       </c>
       <c r="P13" s="1">
         <v>10327</v>
+      </c>
+      <c r="Q13">
+        <f>IF(ISBLANK(R13),-P13,R13-P13)</f>
+        <v>137</v>
+      </c>
+      <c r="R13" s="1">
+        <v>10464</v>
       </c>
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.25">
@@ -7013,46 +7242,53 @@
         <v>79072</v>
       </c>
       <c r="E14">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F14),-D14,F14-D14)</f>
         <v>68</v>
       </c>
       <c r="F14" s="1">
         <v>79140</v>
       </c>
       <c r="G14">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H14),-F14,H14-F14)</f>
         <v>142</v>
       </c>
       <c r="H14" s="1">
         <v>79282</v>
       </c>
       <c r="I14">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J14),-H14,J14-H14)</f>
         <v>105</v>
       </c>
       <c r="J14" s="1">
         <v>79387</v>
       </c>
       <c r="K14">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L14),-J14,L14-J14)</f>
         <v>186</v>
       </c>
       <c r="L14" s="1">
         <v>79573</v>
       </c>
       <c r="M14">
-        <f t="shared" si="4"/>
+        <f>IF(ISBLANK(N14),-L14,N14-L14)</f>
         <v>168</v>
       </c>
       <c r="N14" s="1">
         <v>79741</v>
       </c>
       <c r="O14">
-        <f t="shared" si="5"/>
+        <f>IF(ISBLANK(P14),-N14,P14-N14)</f>
         <v>204</v>
       </c>
       <c r="P14" s="1">
         <v>79945</v>
+      </c>
+      <c r="Q14">
+        <f>IF(ISBLANK(R14),-P14,R14-P14)</f>
+        <v>305</v>
+      </c>
+      <c r="R14" s="1">
+        <v>80250</v>
       </c>
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.25">
@@ -7066,46 +7302,53 @@
         <v>22075</v>
       </c>
       <c r="E15">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F15),-D15,F15-D15)</f>
         <v>38</v>
       </c>
       <c r="F15" s="1">
         <v>22113</v>
       </c>
       <c r="G15">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H15),-F15,H15-F15)</f>
         <v>80</v>
       </c>
       <c r="H15" s="1">
         <v>22193</v>
       </c>
       <c r="I15">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J15),-H15,J15-H15)</f>
         <v>58</v>
       </c>
       <c r="J15" s="1">
         <v>22251</v>
       </c>
       <c r="K15">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L15),-J15,L15-J15)</f>
         <v>70</v>
       </c>
       <c r="L15" s="1">
         <v>22321</v>
       </c>
       <c r="M15">
-        <f t="shared" si="4"/>
+        <f>IF(ISBLANK(N15),-L15,N15-L15)</f>
         <v>62</v>
       </c>
       <c r="N15" s="1">
         <v>22383</v>
       </c>
       <c r="O15">
-        <f t="shared" si="5"/>
+        <f>IF(ISBLANK(P15),-N15,P15-N15)</f>
         <v>70</v>
       </c>
       <c r="P15" s="1">
         <v>22453</v>
+      </c>
+      <c r="Q15">
+        <f>IF(ISBLANK(R15),-P15,R15-P15)</f>
+        <v>173</v>
+      </c>
+      <c r="R15" s="1">
+        <v>22626</v>
       </c>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.25">
@@ -7119,49 +7362,56 @@
         <v>9823</v>
       </c>
       <c r="E16">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F16),-D16,F16-D16)</f>
         <v>37</v>
       </c>
       <c r="F16" s="1">
         <v>9860</v>
       </c>
       <c r="G16">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H16),-F16,H16-F16)</f>
         <v>76</v>
       </c>
       <c r="H16" s="1">
         <v>9936</v>
       </c>
       <c r="I16">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J16),-H16,J16-H16)</f>
         <v>54</v>
       </c>
       <c r="J16" s="1">
         <v>9990</v>
       </c>
       <c r="K16">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L16),-J16,L16-J16)</f>
         <v>184</v>
       </c>
       <c r="L16" s="1">
         <v>10174</v>
       </c>
       <c r="M16">
-        <f t="shared" si="4"/>
+        <f>IF(ISBLANK(N16),-L16,N16-L16)</f>
         <v>52</v>
       </c>
       <c r="N16" s="1">
         <v>10226</v>
       </c>
       <c r="O16">
-        <f t="shared" si="5"/>
+        <f>IF(ISBLANK(P16),-N16,P16-N16)</f>
         <v>168</v>
       </c>
       <c r="P16" s="1">
         <v>10394</v>
       </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q16">
+        <f>IF(ISBLANK(R16),-P16,R16-P16)</f>
+        <v>214</v>
+      </c>
+      <c r="R16" s="1">
+        <v>10608</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>17</v>
       </c>
@@ -7172,49 +7422,56 @@
         <v>3682</v>
       </c>
       <c r="E17">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F17),-D17,F17-D17)</f>
         <v>77</v>
       </c>
       <c r="F17" s="1">
         <v>3759</v>
       </c>
       <c r="G17">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H17),-F17,H17-F17)</f>
         <v>44</v>
       </c>
       <c r="H17" s="1">
         <v>3803</v>
       </c>
       <c r="I17">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J17),-H17,J17-H17)</f>
         <v>116</v>
       </c>
       <c r="J17" s="1">
         <v>3919</v>
       </c>
       <c r="K17">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L17),-J17,L17-J17)</f>
         <v>87</v>
       </c>
       <c r="L17" s="1">
         <v>4006</v>
       </c>
       <c r="M17">
-        <f t="shared" si="4"/>
+        <f>IF(ISBLANK(N17),-L17,N17-L17)</f>
         <v>41</v>
       </c>
       <c r="N17" s="1">
         <v>4047</v>
       </c>
       <c r="O17">
-        <f t="shared" si="5"/>
+        <f>IF(ISBLANK(P17),-N17,P17-N17)</f>
         <v>134</v>
       </c>
       <c r="P17" s="1">
         <v>4181</v>
       </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q17">
+        <f>IF(ISBLANK(R17),-P17,R17-P17)</f>
+        <v>-4181</v>
+      </c>
+      <c r="R17" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>5</v>
       </c>
@@ -7225,49 +7482,56 @@
         <v>75946</v>
       </c>
       <c r="E18">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F18),-D18,F18-D18)</f>
         <v>100</v>
       </c>
       <c r="F18" s="1">
         <v>76046</v>
       </c>
       <c r="G18">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H18),-F18,H18-F18)</f>
         <v>201</v>
       </c>
       <c r="H18" s="1">
         <v>76247</v>
       </c>
       <c r="I18">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J18),-H18,J18-H18)</f>
         <v>126</v>
       </c>
       <c r="J18" s="1">
         <v>76373</v>
       </c>
       <c r="K18">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L18),-J18,L18-J18)</f>
         <v>272</v>
       </c>
       <c r="L18" s="1">
         <v>76645</v>
       </c>
       <c r="M18">
-        <f t="shared" si="4"/>
+        <f>IF(ISBLANK(N18),-L18,N18-L18)</f>
         <v>74</v>
       </c>
       <c r="N18" s="1">
         <v>76719</v>
       </c>
       <c r="O18">
-        <f t="shared" si="5"/>
+        <f>IF(ISBLANK(P18),-N18,P18-N18)</f>
         <v>301</v>
       </c>
       <c r="P18" s="1">
         <v>77020</v>
       </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q18">
+        <f>IF(ISBLANK(R18),-P18,R18-P18)</f>
+        <v>283</v>
+      </c>
+      <c r="R18" s="1">
+        <v>77303</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>20</v>
       </c>
@@ -7278,49 +7542,56 @@
         <v>2864</v>
       </c>
       <c r="E19">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F19),-D19,F19-D19)</f>
         <v>34</v>
       </c>
       <c r="F19" s="1">
         <v>2898</v>
       </c>
       <c r="G19">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H19),-F19,H19-F19)</f>
         <v>21</v>
       </c>
       <c r="H19" s="1">
         <v>2919</v>
       </c>
       <c r="I19">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J19),-H19,J19-H19)</f>
         <v>148</v>
       </c>
       <c r="J19" s="1">
         <v>3067</v>
       </c>
       <c r="K19">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L19),-J19,L19-J19)</f>
         <v>-3067</v>
       </c>
       <c r="L19" s="1">
         <v>0</v>
       </c>
       <c r="M19">
-        <f t="shared" si="4"/>
+        <f>IF(ISBLANK(N19),-L19,N19-L19)</f>
         <v>0</v>
       </c>
       <c r="N19" s="1">
         <v>0</v>
       </c>
       <c r="O19">
-        <f t="shared" si="5"/>
+        <f>IF(ISBLANK(P19),-N19,P19-N19)</f>
         <v>0</v>
       </c>
       <c r="P19" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q19">
+        <f>IF(ISBLANK(R19),-P19,R19-P19)</f>
+        <v>0</v>
+      </c>
+      <c r="R19" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>21</v>
       </c>
@@ -7331,49 +7602,56 @@
         <v>2416</v>
       </c>
       <c r="E20">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F20),-D20,F20-D20)</f>
         <v>48</v>
       </c>
       <c r="F20" s="1">
         <v>2464</v>
       </c>
       <c r="G20">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H20),-F20,H20-F20)</f>
         <v>78</v>
       </c>
       <c r="H20" s="1">
         <v>2542</v>
       </c>
       <c r="I20">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J20),-H20,J20-H20)</f>
         <v>-2542</v>
       </c>
       <c r="J20" s="1">
         <v>0</v>
       </c>
       <c r="K20">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L20),-J20,L20-J20)</f>
         <v>0</v>
       </c>
       <c r="L20" s="1">
         <v>0</v>
       </c>
       <c r="M20">
-        <f t="shared" si="4"/>
+        <f>IF(ISBLANK(N20),-L20,N20-L20)</f>
         <v>0</v>
       </c>
       <c r="N20" s="1">
         <v>0</v>
       </c>
       <c r="O20">
-        <f t="shared" si="5"/>
+        <f>IF(ISBLANK(P20),-N20,P20-N20)</f>
         <v>0</v>
       </c>
       <c r="P20" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q20">
+        <f>IF(ISBLANK(R20),-P20,R20-P20)</f>
+        <v>0</v>
+      </c>
+      <c r="R20" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>23</v>
       </c>
@@ -7384,49 +7662,56 @@
         <v>1423</v>
       </c>
       <c r="E21">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F21),-D21,F21-D21)</f>
         <v>-1423</v>
       </c>
       <c r="F21" s="1">
         <v>0</v>
       </c>
       <c r="G21">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H21),-F21,H21-F21)</f>
         <v>0</v>
       </c>
       <c r="H21" s="1">
         <v>0</v>
       </c>
       <c r="I21">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J21),-H21,J21-H21)</f>
         <v>0</v>
       </c>
       <c r="J21" s="1">
         <v>0</v>
       </c>
       <c r="K21">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L21),-J21,L21-J21)</f>
         <v>0</v>
       </c>
       <c r="L21" s="1">
         <v>0</v>
       </c>
       <c r="M21">
-        <f t="shared" si="4"/>
+        <f>IF(ISBLANK(N21),-L21,N21-L21)</f>
         <v>0</v>
       </c>
       <c r="N21" s="1">
         <v>0</v>
       </c>
       <c r="O21">
-        <f t="shared" si="5"/>
+        <f>IF(ISBLANK(P21),-N21,P21-N21)</f>
         <v>0</v>
       </c>
       <c r="P21" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q21">
+        <f>IF(ISBLANK(R21),-P21,R21-P21)</f>
+        <v>0</v>
+      </c>
+      <c r="R21" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>10</v>
       </c>
@@ -7437,49 +7722,56 @@
         <v>14802</v>
       </c>
       <c r="E22">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F22),-D22,F22-D22)</f>
         <v>156</v>
       </c>
       <c r="F22" s="1">
         <v>14958</v>
       </c>
       <c r="G22">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H22),-F22,H22-F22)</f>
         <v>51</v>
       </c>
       <c r="H22" s="1">
         <v>15009</v>
       </c>
       <c r="I22">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J22),-H22,J22-H22)</f>
         <v>198</v>
       </c>
       <c r="J22" s="1">
         <v>15207</v>
       </c>
       <c r="K22">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L22),-J22,L22-J22)</f>
         <v>146</v>
       </c>
       <c r="L22" s="1">
         <v>15353</v>
       </c>
       <c r="M22">
-        <f t="shared" si="4"/>
+        <f>IF(ISBLANK(N22),-L22,N22-L22)</f>
         <v>41</v>
       </c>
       <c r="N22" s="1">
         <v>15394</v>
       </c>
       <c r="O22">
-        <f t="shared" si="5"/>
+        <f>IF(ISBLANK(P22),-N22,P22-N22)</f>
         <v>392</v>
       </c>
       <c r="P22" s="1">
         <v>15786</v>
       </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q22">
+        <f>IF(ISBLANK(R22),-P22,R22-P22)</f>
+        <v>321</v>
+      </c>
+      <c r="R22" s="1">
+        <v>16107</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>3</v>
       </c>
@@ -7490,49 +7782,56 @@
         <v>81741</v>
       </c>
       <c r="E23">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F23),-D23,F23-D23)</f>
         <v>253</v>
       </c>
       <c r="F23" s="1">
         <v>81994</v>
       </c>
       <c r="G23">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H23),-F23,H23-F23)</f>
         <v>130</v>
       </c>
       <c r="H23" s="1">
         <v>82124</v>
       </c>
       <c r="I23">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J23),-H23,J23-H23)</f>
         <v>211</v>
       </c>
       <c r="J23" s="1">
         <v>82335</v>
       </c>
       <c r="K23">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L23),-J23,L23-J23)</f>
         <v>323</v>
       </c>
       <c r="L23" s="1">
         <v>82658</v>
       </c>
       <c r="M23">
-        <f t="shared" si="4"/>
+        <f>IF(ISBLANK(N23),-L23,N23-L23)</f>
         <v>206</v>
       </c>
       <c r="N23" s="1">
         <v>82864</v>
       </c>
       <c r="O23">
-        <f t="shared" si="5"/>
+        <f>IF(ISBLANK(P23),-N23,P23-N23)</f>
         <v>556</v>
       </c>
       <c r="P23" s="1">
         <v>83420</v>
       </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q23">
+        <f>IF(ISBLANK(R23),-P23,R23-P23)</f>
+        <v>351</v>
+      </c>
+      <c r="R23" s="1">
+        <v>83771</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>18</v>
       </c>
@@ -7543,49 +7842,56 @@
         <v>3286</v>
       </c>
       <c r="E24">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F24),-D24,F24-D24)</f>
         <v>21</v>
       </c>
       <c r="F24" s="1">
         <v>3307</v>
       </c>
       <c r="G24">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H24),-F24,H24-F24)</f>
         <v>13</v>
       </c>
       <c r="H24" s="1">
         <v>3320</v>
       </c>
       <c r="I24">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J24),-H24,J24-H24)</f>
         <v>232</v>
       </c>
       <c r="J24" s="1">
         <v>3552</v>
       </c>
       <c r="K24">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L24),-J24,L24-J24)</f>
         <v>102</v>
       </c>
       <c r="L24" s="1">
         <v>3654</v>
       </c>
       <c r="M24">
-        <f t="shared" si="4"/>
+        <f>IF(ISBLANK(N24),-L24,N24-L24)</f>
         <v>60</v>
       </c>
       <c r="N24" s="1">
         <v>3714</v>
       </c>
       <c r="O24">
-        <f t="shared" si="5"/>
+        <f>IF(ISBLANK(P24),-N24,P24-N24)</f>
         <v>-3714</v>
       </c>
       <c r="P24" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q24">
+        <f>IF(ISBLANK(R24),-P24,R24-P24)</f>
+        <v>0</v>
+      </c>
+      <c r="R24" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>147</v>
       </c>
@@ -7626,25 +7932,49 @@
       <c r="P26" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q26" t="s">
+        <v>0</v>
+      </c>
+      <c r="R26" t="s">
+        <v>10</v>
+      </c>
+      <c r="S26" t="s">
+        <v>11</v>
+      </c>
+      <c r="T26" t="s">
+        <v>12</v>
+      </c>
+      <c r="U26" t="s">
+        <v>13</v>
+      </c>
+      <c r="V26" t="s">
+        <v>14</v>
+      </c>
+      <c r="W26" t="s">
+        <v>1</v>
+      </c>
+      <c r="X26" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>148</v>
       </c>
       <c r="E27">
-        <f t="shared" ref="E27:E48" si="6">FIND(",",B27)</f>
+        <f t="shared" ref="E27:E48" si="0">FIND(",",B27)</f>
         <v>9</v>
       </c>
       <c r="F27" t="str">
-        <f t="shared" ref="F27:F48" si="7">LEFT(B27,E27-1)</f>
+        <f t="shared" ref="F27:F48" si="1">LEFT(B27,E27-1)</f>
         <v>Kelleher</v>
       </c>
       <c r="G27" t="str">
-        <f t="shared" ref="G27:G48" si="8">RIGHT(B27,LEN(B27)-(E27+1))</f>
+        <f t="shared" ref="G27:G48" si="2">RIGHT(B27,LEN(B27)-(E27+1))</f>
         <v>Billy</v>
       </c>
       <c r="H27" t="str">
-        <f t="shared" ref="H27:H48" si="9">G27&amp;" "&amp;F27</f>
+        <f t="shared" ref="H27:H48" si="3">G27&amp;" "&amp;F27</f>
         <v>Billy Kelleher</v>
       </c>
       <c r="J27" t="s">
@@ -7662,25 +7992,49 @@
       <c r="N27" s="1">
         <v>119123</v>
       </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q27" t="s">
+        <v>124</v>
+      </c>
+      <c r="R27" s="1">
+        <v>118489</v>
+      </c>
+      <c r="S27" s="1">
+        <v>118675</v>
+      </c>
+      <c r="T27" s="1">
+        <v>118773</v>
+      </c>
+      <c r="U27" s="1">
+        <v>119123</v>
+      </c>
+      <c r="V27" s="1">
+        <v>119380</v>
+      </c>
+      <c r="W27" s="1">
+        <v>119545</v>
+      </c>
+      <c r="X27" s="1">
+        <v>119715</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>149</v>
       </c>
       <c r="E28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="F28" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="1"/>
         <v>Wallace</v>
       </c>
       <c r="G28" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>Mick</v>
       </c>
       <c r="H28" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="3"/>
         <v>Mick Wallace</v>
       </c>
       <c r="J28" t="s">
@@ -7698,25 +8052,49 @@
       <c r="N28" s="1">
         <v>84388</v>
       </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q28" t="s">
+        <v>125</v>
+      </c>
+      <c r="R28" s="1">
+        <v>84106</v>
+      </c>
+      <c r="S28" s="1">
+        <v>84164</v>
+      </c>
+      <c r="T28" s="1">
+        <v>84238</v>
+      </c>
+      <c r="U28" s="1">
+        <v>84388</v>
+      </c>
+      <c r="V28" s="1">
+        <v>84559</v>
+      </c>
+      <c r="W28" s="1">
+        <v>84654</v>
+      </c>
+      <c r="X28" s="1">
+        <v>84841</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>150</v>
       </c>
       <c r="E29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="F29" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="1"/>
         <v>Ní Riada</v>
       </c>
       <c r="G29" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>Liadh</v>
       </c>
       <c r="H29" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="3"/>
         <v>Liadh Ní Riada</v>
       </c>
       <c r="J29" t="s">
@@ -7734,25 +8112,49 @@
       <c r="N29" s="1">
         <v>82658</v>
       </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q29" t="s">
+        <v>126</v>
+      </c>
+      <c r="R29" s="1">
+        <v>81994</v>
+      </c>
+      <c r="S29" s="1">
+        <v>82124</v>
+      </c>
+      <c r="T29" s="1">
+        <v>82335</v>
+      </c>
+      <c r="U29" s="1">
+        <v>82658</v>
+      </c>
+      <c r="V29" s="1">
+        <v>82864</v>
+      </c>
+      <c r="W29" s="1">
+        <v>83420</v>
+      </c>
+      <c r="X29" s="1">
+        <v>83771</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>151</v>
       </c>
       <c r="E30">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="F30" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="1"/>
         <v>O'Sullivan</v>
       </c>
       <c r="G30" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>Grace</v>
       </c>
       <c r="H30" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="3"/>
         <v>Grace O'Sullivan</v>
       </c>
       <c r="J30" t="s">
@@ -7770,25 +8172,49 @@
       <c r="N30" s="1">
         <v>79573</v>
       </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q30" t="s">
+        <v>127</v>
+      </c>
+      <c r="R30" s="1">
+        <v>79140</v>
+      </c>
+      <c r="S30" s="1">
+        <v>79282</v>
+      </c>
+      <c r="T30" s="1">
+        <v>79387</v>
+      </c>
+      <c r="U30" s="1">
+        <v>79573</v>
+      </c>
+      <c r="V30" s="1">
+        <v>79741</v>
+      </c>
+      <c r="W30" s="1">
+        <v>79945</v>
+      </c>
+      <c r="X30" s="1">
+        <v>80250</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>152</v>
       </c>
       <c r="E31">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="F31" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="1"/>
         <v>Byrne</v>
       </c>
       <c r="G31" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>Malcolm</v>
       </c>
       <c r="H31" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="3"/>
         <v>Malcolm Byrne</v>
       </c>
       <c r="J31" t="s">
@@ -7806,25 +8232,49 @@
       <c r="N31" s="1">
         <v>76645</v>
       </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q31" t="s">
+        <v>128</v>
+      </c>
+      <c r="R31" s="1">
+        <v>76046</v>
+      </c>
+      <c r="S31" s="1">
+        <v>76247</v>
+      </c>
+      <c r="T31" s="1">
+        <v>76373</v>
+      </c>
+      <c r="U31" s="1">
+        <v>76645</v>
+      </c>
+      <c r="V31" s="1">
+        <v>76719</v>
+      </c>
+      <c r="W31" s="1">
+        <v>77020</v>
+      </c>
+      <c r="X31" s="1">
+        <v>77303</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>153</v>
       </c>
       <c r="E32">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="F32" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="1"/>
         <v>Clune</v>
       </c>
       <c r="G32" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>Deirdre</v>
       </c>
       <c r="H32" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="3"/>
         <v>Deirdre Clune</v>
       </c>
       <c r="J32" t="s">
@@ -7842,25 +8292,49 @@
       <c r="N32" s="1">
         <v>69382</v>
       </c>
-    </row>
-    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="Q32" t="s">
+        <v>129</v>
+      </c>
+      <c r="R32" s="1">
+        <v>69201</v>
+      </c>
+      <c r="S32" s="1">
+        <v>69272</v>
+      </c>
+      <c r="T32" s="1">
+        <v>69316</v>
+      </c>
+      <c r="U32" s="1">
+        <v>69382</v>
+      </c>
+      <c r="V32" s="1">
+        <v>69511</v>
+      </c>
+      <c r="W32" s="1">
+        <v>69556</v>
+      </c>
+      <c r="X32" s="1">
+        <v>69672</v>
+      </c>
+    </row>
+    <row r="33" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>154</v>
       </c>
       <c r="E33">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="F33" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="1"/>
         <v>Doyle</v>
       </c>
       <c r="G33" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>Andrew</v>
       </c>
       <c r="H33" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="3"/>
         <v>Andrew Doyle</v>
       </c>
       <c r="J33" t="s">
@@ -7878,25 +8352,49 @@
       <c r="N33" s="1">
         <v>64899</v>
       </c>
-    </row>
-    <row r="34" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="Q33" t="s">
+        <v>130</v>
+      </c>
+      <c r="R33" s="1">
+        <v>64631</v>
+      </c>
+      <c r="S33" s="1">
+        <v>64692</v>
+      </c>
+      <c r="T33" s="1">
+        <v>64763</v>
+      </c>
+      <c r="U33" s="1">
+        <v>64899</v>
+      </c>
+      <c r="V33" s="1">
+        <v>65005</v>
+      </c>
+      <c r="W33" s="1">
+        <v>65115</v>
+      </c>
+      <c r="X33" s="1">
+        <v>65252</v>
+      </c>
+    </row>
+    <row r="34" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>155</v>
       </c>
       <c r="E34">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="F34" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="1"/>
         <v>Nunan</v>
       </c>
       <c r="G34" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>Sheila</v>
       </c>
       <c r="H34" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="3"/>
         <v>Sheila Nunan</v>
       </c>
       <c r="J34" t="s">
@@ -7914,25 +8412,49 @@
       <c r="N34" s="1">
         <v>38842</v>
       </c>
-    </row>
-    <row r="35" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="Q34" t="s">
+        <v>131</v>
+      </c>
+      <c r="R34" s="1">
+        <v>38755</v>
+      </c>
+      <c r="S34" s="1">
+        <v>38788</v>
+      </c>
+      <c r="T34" s="1">
+        <v>38804</v>
+      </c>
+      <c r="U34" s="1">
+        <v>38842</v>
+      </c>
+      <c r="V34" s="1">
+        <v>38926</v>
+      </c>
+      <c r="W34" s="1">
+        <v>38950</v>
+      </c>
+      <c r="X34" s="1">
+        <v>38996</v>
+      </c>
+    </row>
+    <row r="35" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>156</v>
       </c>
       <c r="E35">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="F35" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="1"/>
         <v>Wallace</v>
       </c>
       <c r="G35" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>Adrienne</v>
       </c>
       <c r="H35" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="3"/>
         <v>Adrienne Wallace</v>
       </c>
       <c r="J35" t="s">
@@ -7950,25 +8472,49 @@
       <c r="N35" s="1">
         <v>22321</v>
       </c>
-    </row>
-    <row r="36" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="Q35" t="s">
+        <v>132</v>
+      </c>
+      <c r="R35" s="1">
+        <v>22113</v>
+      </c>
+      <c r="S35" s="1">
+        <v>22193</v>
+      </c>
+      <c r="T35" s="1">
+        <v>22251</v>
+      </c>
+      <c r="U35" s="1">
+        <v>22321</v>
+      </c>
+      <c r="V35" s="1">
+        <v>22383</v>
+      </c>
+      <c r="W35" s="1">
+        <v>22453</v>
+      </c>
+      <c r="X35" s="1">
+        <v>22626</v>
+      </c>
+    </row>
+    <row r="36" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>157</v>
       </c>
       <c r="E36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="F36" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="1"/>
         <v>Cahill</v>
       </c>
       <c r="G36" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>Dolores</v>
       </c>
       <c r="H36" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="3"/>
         <v>Dolores Cahill</v>
       </c>
       <c r="J36" t="s">
@@ -7986,25 +8532,49 @@
       <c r="N36" s="1">
         <v>15353</v>
       </c>
-    </row>
-    <row r="37" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="Q36" t="s">
+        <v>133</v>
+      </c>
+      <c r="R36" s="1">
+        <v>14958</v>
+      </c>
+      <c r="S36" s="1">
+        <v>15009</v>
+      </c>
+      <c r="T36" s="1">
+        <v>15207</v>
+      </c>
+      <c r="U36" s="1">
+        <v>15353</v>
+      </c>
+      <c r="V36" s="1">
+        <v>15394</v>
+      </c>
+      <c r="W36" s="1">
+        <v>15786</v>
+      </c>
+      <c r="X36" s="1">
+        <v>16107</v>
+      </c>
+    </row>
+    <row r="37" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>158</v>
       </c>
       <c r="E37">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="F37" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="1"/>
         <v>O'Flynn</v>
       </c>
       <c r="G37" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>Diarmuid Patrick</v>
       </c>
       <c r="H37" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="3"/>
         <v>Diarmuid Patrick O'Flynn</v>
       </c>
       <c r="J37" t="s">
@@ -8022,25 +8592,49 @@
       <c r="N37" s="1">
         <v>10937</v>
       </c>
-    </row>
-    <row r="38" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="Q37" t="s">
+        <v>134</v>
+      </c>
+      <c r="R37" s="1">
+        <v>10639</v>
+      </c>
+      <c r="S37" s="1">
+        <v>10745</v>
+      </c>
+      <c r="T37" s="1">
+        <v>10883</v>
+      </c>
+      <c r="U37" s="1">
+        <v>10937</v>
+      </c>
+      <c r="V37" s="1">
+        <v>11237</v>
+      </c>
+      <c r="W37" s="1">
+        <v>11396</v>
+      </c>
+      <c r="X37" s="1">
+        <v>11718</v>
+      </c>
+    </row>
+    <row r="38" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>159</v>
       </c>
       <c r="E38">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="F38" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="1"/>
         <v>Minehan</v>
       </c>
       <c r="G38" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>Liam</v>
       </c>
       <c r="H38" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="3"/>
         <v>Liam Minehan</v>
       </c>
       <c r="J38" t="s">
@@ -8058,25 +8652,49 @@
       <c r="N38" s="1">
         <v>10174</v>
       </c>
-    </row>
-    <row r="39" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="Q38" t="s">
+        <v>135</v>
+      </c>
+      <c r="R38" s="1">
+        <v>9860</v>
+      </c>
+      <c r="S38" s="1">
+        <v>9936</v>
+      </c>
+      <c r="T38" s="1">
+        <v>9990</v>
+      </c>
+      <c r="U38" s="1">
+        <v>10174</v>
+      </c>
+      <c r="V38" s="1">
+        <v>10226</v>
+      </c>
+      <c r="W38" s="1">
+        <v>10394</v>
+      </c>
+      <c r="X38" s="1">
+        <v>10608</v>
+      </c>
+    </row>
+    <row r="39" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>160</v>
       </c>
       <c r="E39">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="F39" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="1"/>
         <v>Gardner</v>
       </c>
       <c r="G39" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>Breda Patricia</v>
       </c>
       <c r="H39" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="3"/>
         <v>Breda Patricia Gardner</v>
       </c>
       <c r="J39" t="s">
@@ -8094,25 +8712,49 @@
       <c r="N39" s="1">
         <v>9969</v>
       </c>
-    </row>
-    <row r="40" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="Q39" t="s">
+        <v>136</v>
+      </c>
+      <c r="R39" s="1">
+        <v>9455</v>
+      </c>
+      <c r="S39" s="1">
+        <v>9780</v>
+      </c>
+      <c r="T39" s="1">
+        <v>9855</v>
+      </c>
+      <c r="U39" s="1">
+        <v>9969</v>
+      </c>
+      <c r="V39" s="1">
+        <v>10249</v>
+      </c>
+      <c r="W39" s="1">
+        <v>10327</v>
+      </c>
+      <c r="X39" s="1">
+        <v>10464</v>
+      </c>
+    </row>
+    <row r="40" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>161</v>
       </c>
       <c r="E40">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="F40" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="1"/>
         <v>Heaney</v>
       </c>
       <c r="G40" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>Theresa</v>
       </c>
       <c r="H40" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="3"/>
         <v>Theresa Heaney</v>
       </c>
       <c r="J40" t="s">
@@ -8130,25 +8772,49 @@
       <c r="N40" s="1">
         <v>9496</v>
       </c>
-    </row>
-    <row r="41" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="Q40" t="s">
+        <v>137</v>
+      </c>
+      <c r="R40" s="1">
+        <v>9331</v>
+      </c>
+      <c r="S40" s="1">
+        <v>9401</v>
+      </c>
+      <c r="T40" s="1">
+        <v>9436</v>
+      </c>
+      <c r="U40" s="1">
+        <v>9496</v>
+      </c>
+      <c r="V40" s="1">
+        <v>9724</v>
+      </c>
+      <c r="W40" s="1">
+        <v>9869</v>
+      </c>
+      <c r="X40" s="1">
+        <v>9975</v>
+      </c>
+    </row>
+    <row r="41" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>162</v>
       </c>
       <c r="E41">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="F41" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="1"/>
         <v>Brennan</v>
       </c>
       <c r="G41" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>Allan</v>
       </c>
       <c r="H41" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="3"/>
         <v>Allan Brennan</v>
       </c>
       <c r="J41" t="s">
@@ -8166,25 +8832,49 @@
       <c r="N41" s="1">
         <v>7808</v>
       </c>
-    </row>
-    <row r="42" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="Q41" t="s">
+        <v>138</v>
+      </c>
+      <c r="R41" s="1">
+        <v>7498</v>
+      </c>
+      <c r="S41" s="1">
+        <v>7596</v>
+      </c>
+      <c r="T41" s="1">
+        <v>7738</v>
+      </c>
+      <c r="U41" s="1">
+        <v>7808</v>
+      </c>
+      <c r="V41" s="1">
+        <v>8005</v>
+      </c>
+      <c r="W41" s="1">
+        <v>8197</v>
+      </c>
+      <c r="X41" s="1">
+        <v>8373</v>
+      </c>
+    </row>
+    <row r="42" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>163</v>
       </c>
       <c r="E42">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="F42" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="1"/>
         <v>O'Loughlin</v>
       </c>
       <c r="G42" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>Peter</v>
       </c>
       <c r="H42" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="3"/>
         <v>Peter O'Loughlin</v>
       </c>
       <c r="J42" t="s">
@@ -8202,25 +8892,49 @@
       <c r="N42" s="1">
         <v>4841</v>
       </c>
-    </row>
-    <row r="43" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="Q42" t="s">
+        <v>259</v>
+      </c>
+      <c r="R42" s="1">
+        <v>4691</v>
+      </c>
+      <c r="S42" s="1">
+        <v>4734</v>
+      </c>
+      <c r="T42" s="1">
+        <v>4791</v>
+      </c>
+      <c r="U42" s="1">
+        <v>4841</v>
+      </c>
+      <c r="V42" s="1">
+        <v>4956</v>
+      </c>
+      <c r="W42" s="1">
+        <v>5028</v>
+      </c>
+      <c r="X42" s="1">
+        <v>5132</v>
+      </c>
+    </row>
+    <row r="43" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>164</v>
       </c>
       <c r="E43">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="F43" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="1"/>
         <v>Worthington</v>
       </c>
       <c r="G43" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>Colleen</v>
       </c>
       <c r="H43" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="3"/>
         <v>Colleen Worthington</v>
       </c>
       <c r="J43" t="s">
@@ -8238,25 +8952,46 @@
       <c r="N43" s="1">
         <v>4006</v>
       </c>
-    </row>
-    <row r="44" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="Q43" t="s">
+        <v>236</v>
+      </c>
+      <c r="R43" s="1">
+        <v>3759</v>
+      </c>
+      <c r="S43" s="1">
+        <v>3803</v>
+      </c>
+      <c r="T43" s="1">
+        <v>3919</v>
+      </c>
+      <c r="U43" s="1">
+        <v>4006</v>
+      </c>
+      <c r="V43" s="1">
+        <v>4047</v>
+      </c>
+      <c r="W43" s="1">
+        <v>4181</v>
+      </c>
+    </row>
+    <row r="44" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>165</v>
       </c>
       <c r="E44">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="F44" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="1"/>
         <v>Fitzgerald</v>
       </c>
       <c r="G44" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>Paddy</v>
       </c>
       <c r="H44" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="3"/>
         <v>Paddy Fitzgerald</v>
       </c>
       <c r="J44" t="s">
@@ -8274,25 +9009,43 @@
       <c r="N44" s="1">
         <v>3654</v>
       </c>
-    </row>
-    <row r="45" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="Q44" t="s">
+        <v>237</v>
+      </c>
+      <c r="R44" s="1">
+        <v>3307</v>
+      </c>
+      <c r="S44" s="1">
+        <v>3320</v>
+      </c>
+      <c r="T44" s="1">
+        <v>3552</v>
+      </c>
+      <c r="U44" s="1">
+        <v>3654</v>
+      </c>
+      <c r="V44" s="1">
+        <v>3714</v>
+      </c>
+    </row>
+    <row r="45" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>166</v>
       </c>
       <c r="E45">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="F45" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="1"/>
         <v>Ryan-Purcell</v>
       </c>
       <c r="G45" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>Walter</v>
       </c>
       <c r="H45" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="3"/>
         <v>Walter Ryan-Purcell</v>
       </c>
       <c r="J45" t="s">
@@ -8310,25 +9063,40 @@
       <c r="N45" s="1">
         <v>3332</v>
       </c>
-    </row>
-    <row r="46" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="Q45" t="s">
+        <v>142</v>
+      </c>
+      <c r="R45" s="1">
+        <v>3197</v>
+      </c>
+      <c r="S45" s="1">
+        <v>3257</v>
+      </c>
+      <c r="T45" s="1">
+        <v>3300</v>
+      </c>
+      <c r="U45" s="1">
+        <v>3332</v>
+      </c>
+    </row>
+    <row r="46" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>167</v>
       </c>
       <c r="E46">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="F46" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="1"/>
         <v>Sexton</v>
       </c>
       <c r="G46" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>Joesph</v>
       </c>
       <c r="H46" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="3"/>
         <v>Joesph Sexton</v>
       </c>
       <c r="J46" t="s">
@@ -8343,25 +9111,37 @@
       <c r="M46" s="1">
         <v>3067</v>
       </c>
-    </row>
-    <row r="47" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="Q46" t="s">
+        <v>143</v>
+      </c>
+      <c r="R46" s="1">
+        <v>2898</v>
+      </c>
+      <c r="S46" s="1">
+        <v>2919</v>
+      </c>
+      <c r="T46" s="1">
+        <v>3067</v>
+      </c>
+    </row>
+    <row r="47" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>168</v>
       </c>
       <c r="E47">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="F47" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="1"/>
         <v>Madden</v>
       </c>
       <c r="G47" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>Peter</v>
       </c>
       <c r="H47" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="3"/>
         <v>Peter Madden</v>
       </c>
       <c r="J47" t="s">
@@ -8373,25 +9153,34 @@
       <c r="L47" s="1">
         <v>2542</v>
       </c>
-    </row>
-    <row r="48" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="Q47" t="s">
+        <v>144</v>
+      </c>
+      <c r="R47" s="1">
+        <v>2464</v>
+      </c>
+      <c r="S47" s="1">
+        <v>2542</v>
+      </c>
+    </row>
+    <row r="48" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>169</v>
       </c>
       <c r="E48">
-        <f t="shared" si="6"/>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="F48" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="1"/>
         <v>Van de Ven</v>
       </c>
       <c r="G48" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>Jan</v>
       </c>
       <c r="H48" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="3"/>
         <v>Jan Van de Ven</v>
       </c>
       <c r="J48" t="s">
@@ -8400,16 +9189,26 @@
       <c r="K48" s="1">
         <v>2409</v>
       </c>
-    </row>
-    <row r="49" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="Q48" t="s">
+        <v>145</v>
+      </c>
+      <c r="R48" s="1">
+        <v>2409</v>
+      </c>
+    </row>
+    <row r="49" spans="10:17" x14ac:dyDescent="0.25">
       <c r="J49" t="s">
         <v>146</v>
       </c>
+      <c r="Q49" t="s">
+        <v>146</v>
+      </c>
     </row>
   </sheetData>
-  <sortState ref="A2:P24">
+  <sortState ref="A2:R24">
     <sortCondition ref="B2:B24"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Count 6 Midlands added Signed-off-by: Gerry Mulvenna <git@movingwifi.com>
</commit_message>
<xml_diff>
--- a/europarl/europarl-ireland-2019.xlsx
+++ b/europarl/europarl-ireland-2019.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="14220" windowHeight="8580" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="14220" windowHeight="8580" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Candidates" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="260">
   <si>
     <t>Candidate</t>
   </si>
@@ -5021,15 +5021,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P37"/>
+  <dimension ref="A1:Y37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2:N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>256</v>
       </c>
@@ -5052,7 +5052,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>11</v>
       </c>
@@ -5064,35 +5064,42 @@
         <v>8130</v>
       </c>
       <c r="E2">
-        <f t="shared" ref="E2:E18" si="0">IF(ISBLANK(F2),-D2,F2-D2)</f>
+        <f>IF(ISBLANK(F2),-D2,F2-D2)</f>
         <v>96</v>
       </c>
       <c r="F2" s="1">
         <v>8226</v>
       </c>
       <c r="G2">
-        <f t="shared" ref="G2:G18" si="1">IF(ISBLANK(H2),-F2,H2-F2)</f>
+        <f>IF(ISBLANK(H2),-F2,H2-F2)</f>
         <v>20</v>
       </c>
       <c r="H2" s="1">
         <v>8246</v>
       </c>
       <c r="I2">
-        <f t="shared" ref="I2:I18" si="2">IF(ISBLANK(J2),-H2,J2-H2)</f>
+        <f>IF(ISBLANK(J2),-H2,J2-H2)</f>
         <v>91</v>
       </c>
       <c r="J2" s="1">
         <v>8337</v>
       </c>
       <c r="K2">
-        <f t="shared" ref="K2:K18" si="3">IF(ISBLANK(L2),-J2,L2-J2)</f>
+        <f>IF(ISBLANK(L2),-J2,L2-J2)</f>
         <v>28</v>
       </c>
       <c r="L2" s="1">
         <v>8365</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M2">
+        <f>IF(ISBLANK(N2),-L2,N2-L2)</f>
+        <v>188</v>
+      </c>
+      <c r="N2" s="1">
+        <v>8553</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
@@ -5104,35 +5111,42 @@
         <v>77619</v>
       </c>
       <c r="E3">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F3),-D3,F3-D3)</f>
         <v>868</v>
       </c>
       <c r="F3" s="1">
         <v>78487</v>
       </c>
       <c r="G3">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H3),-F3,H3-F3)</f>
         <v>26</v>
       </c>
       <c r="H3" s="1">
         <v>78513</v>
       </c>
       <c r="I3">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J3),-H3,J3-H3)</f>
         <v>99</v>
       </c>
       <c r="J3" s="1">
         <v>78612</v>
       </c>
       <c r="K3">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L3),-J3,L3-J3)</f>
         <v>41</v>
       </c>
       <c r="L3" s="1">
         <v>78653</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M3">
+        <f>IF(ISBLANK(N3),-L3,N3-L3)</f>
+        <v>375</v>
+      </c>
+      <c r="N3" s="1">
+        <v>79028</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>5</v>
       </c>
@@ -5144,35 +5158,42 @@
         <v>56650</v>
       </c>
       <c r="E4">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F4),-D4,F4-D4)</f>
         <v>1198</v>
       </c>
       <c r="F4" s="1">
         <v>57848</v>
       </c>
       <c r="G4">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H4),-F4,H4-F4)</f>
         <v>44</v>
       </c>
       <c r="H4" s="1">
         <v>57892</v>
       </c>
       <c r="I4">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J4),-H4,J4-H4)</f>
         <v>142</v>
       </c>
       <c r="J4" s="1">
         <v>58034</v>
       </c>
       <c r="K4">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L4),-J4,L4-J4)</f>
         <v>178</v>
       </c>
       <c r="L4" s="1">
         <v>58212</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M4">
+        <f>IF(ISBLANK(N4),-L4,N4-L4)</f>
+        <v>390</v>
+      </c>
+      <c r="N4" s="1">
+        <v>58602</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>9</v>
       </c>
@@ -5184,35 +5205,42 @@
         <v>15991</v>
       </c>
       <c r="E5">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F5),-D5,F5-D5)</f>
         <v>477</v>
       </c>
       <c r="F5" s="1">
         <v>16468</v>
       </c>
       <c r="G5">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H5),-F5,H5-F5)</f>
         <v>47</v>
       </c>
       <c r="H5" s="1">
         <v>16515</v>
       </c>
       <c r="I5">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J5),-H5,J5-H5)</f>
         <v>106</v>
       </c>
       <c r="J5" s="1">
         <v>16621</v>
       </c>
       <c r="K5">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L5),-J5,L5-J5)</f>
         <v>143</v>
       </c>
       <c r="L5" s="1">
         <v>16764</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M5">
+        <f>IF(ISBLANK(N5),-L5,N5-L5)</f>
+        <v>826</v>
+      </c>
+      <c r="N5" s="1">
+        <v>17590</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -5224,35 +5252,42 @@
         <v>85034</v>
       </c>
       <c r="E6">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F6),-D6,F6-D6)</f>
         <v>1872</v>
       </c>
       <c r="F6" s="1">
         <v>86906</v>
       </c>
       <c r="G6">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H6),-F6,H6-F6)</f>
         <v>102</v>
       </c>
       <c r="H6" s="1">
         <v>87008</v>
       </c>
       <c r="I6">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J6),-H6,J6-H6)</f>
         <v>180</v>
       </c>
       <c r="J6" s="1">
         <v>87188</v>
       </c>
       <c r="K6">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L6),-J6,L6-J6)</f>
         <v>145</v>
       </c>
       <c r="L6" s="1">
         <v>87333</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M6">
+        <f>IF(ISBLANK(N6),-L6,N6-L6)</f>
+        <v>631</v>
+      </c>
+      <c r="N6" s="1">
+        <v>87964</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>15</v>
       </c>
@@ -5264,35 +5299,42 @@
         <v>1352</v>
       </c>
       <c r="E7">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F7),-D7,F7-D7)</f>
         <v>48</v>
       </c>
       <c r="F7" s="1">
         <v>1400</v>
       </c>
       <c r="G7">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H7),-F7,H7-F7)</f>
         <v>12</v>
       </c>
       <c r="H7" s="1">
         <v>1412</v>
       </c>
       <c r="I7">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J7),-H7,J7-H7)</f>
         <v>-1412</v>
       </c>
       <c r="J7" s="1">
         <v>0</v>
       </c>
       <c r="K7">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L7),-J7,L7-J7)</f>
         <v>0</v>
       </c>
       <c r="L7" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M7">
+        <f>IF(ISBLANK(N7),-L7,N7-L7)</f>
+        <v>0</v>
+      </c>
+      <c r="N7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>10</v>
       </c>
@@ -5304,35 +5346,42 @@
         <v>12378</v>
       </c>
       <c r="E8">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F8),-D8,F8-D8)</f>
         <v>653</v>
       </c>
       <c r="F8" s="1">
         <v>13031</v>
       </c>
       <c r="G8">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H8),-F8,H8-F8)</f>
         <v>34</v>
       </c>
       <c r="H8" s="1">
         <v>13065</v>
       </c>
       <c r="I8">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J8),-H8,J8-H8)</f>
         <v>85</v>
       </c>
       <c r="J8" s="1">
         <v>13150</v>
       </c>
       <c r="K8">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L8),-J8,L8-J8)</f>
         <v>47</v>
       </c>
       <c r="L8" s="1">
         <v>13197</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M8">
+        <f>IF(ISBLANK(N8),-L8,N8-L8)</f>
+        <v>211</v>
+      </c>
+      <c r="N8" s="1">
+        <v>13408</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>14</v>
       </c>
@@ -5344,35 +5393,42 @@
         <v>2450</v>
       </c>
       <c r="E9">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F9),-D9,F9-D9)</f>
         <v>112</v>
       </c>
       <c r="F9" s="1">
         <v>2562</v>
       </c>
       <c r="G9">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H9),-F9,H9-F9)</f>
         <v>15</v>
       </c>
       <c r="H9" s="1">
         <v>2577</v>
       </c>
       <c r="I9">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J9),-H9,J9-H9)</f>
         <v>77</v>
       </c>
       <c r="J9" s="1">
         <v>2654</v>
       </c>
       <c r="K9">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L9),-J9,L9-J9)</f>
         <v>40</v>
       </c>
       <c r="L9" s="1">
         <v>2694</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M9">
+        <f>IF(ISBLANK(N9),-L9,N9-L9)</f>
+        <v>-2694</v>
+      </c>
+      <c r="N9" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
@@ -5384,35 +5440,42 @@
         <v>134630</v>
       </c>
       <c r="E10">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F10),-D10,F10-D10)</f>
         <v>-15644</v>
       </c>
       <c r="F10">
         <v>118986</v>
       </c>
       <c r="G10">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H10),-F10,H10-F10)</f>
         <v>0</v>
       </c>
       <c r="H10">
         <v>118986</v>
       </c>
       <c r="I10">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J10),-H10,J10-H10)</f>
         <v>0</v>
       </c>
       <c r="J10">
         <v>118986</v>
       </c>
       <c r="K10">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L10),-J10,L10-J10)</f>
         <v>0</v>
       </c>
       <c r="L10">
         <v>118986</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M10">
+        <f>IF(ISBLANK(N10),-L10,N10-L10)</f>
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>118986</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>6</v>
       </c>
@@ -5424,35 +5487,42 @@
         <v>51019</v>
       </c>
       <c r="E11">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F11),-D11,F11-D11)</f>
         <v>1712</v>
       </c>
       <c r="F11" s="1">
         <v>52731</v>
       </c>
       <c r="G11">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H11),-F11,H11-F11)</f>
         <v>90</v>
       </c>
       <c r="H11" s="1">
         <v>52821</v>
       </c>
       <c r="I11">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J11),-H11,J11-H11)</f>
         <v>155</v>
       </c>
       <c r="J11" s="1">
         <v>52976</v>
       </c>
       <c r="K11">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L11),-J11,L11-J11)</f>
         <v>92</v>
       </c>
       <c r="L11" s="1">
         <v>53068</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M11">
+        <f>IF(ISBLANK(N11),-L11,N11-L11)</f>
+        <v>898</v>
+      </c>
+      <c r="N11" s="1">
+        <v>53966</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>16</v>
       </c>
@@ -5464,35 +5534,42 @@
         <v>1322</v>
       </c>
       <c r="E12">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F12),-D12,F12-D12)</f>
         <v>53</v>
       </c>
       <c r="F12" s="1">
         <v>1375</v>
       </c>
       <c r="G12">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H12),-F12,H12-F12)</f>
         <v>71</v>
       </c>
       <c r="H12" s="1">
         <v>1446</v>
       </c>
       <c r="I12">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J12),-H12,J12-H12)</f>
         <v>44</v>
       </c>
       <c r="J12" s="1">
         <v>1490</v>
       </c>
       <c r="K12">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L12),-J12,L12-J12)</f>
         <v>-1490</v>
       </c>
       <c r="L12" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M12">
+        <f>IF(ISBLANK(N12),-L12,N12-L12)</f>
+        <v>0</v>
+      </c>
+      <c r="N12" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>17</v>
       </c>
@@ -5504,35 +5581,42 @@
         <v>789</v>
       </c>
       <c r="E13">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F13),-D13,F13-D13)</f>
         <v>22</v>
       </c>
       <c r="F13">
         <v>811</v>
       </c>
       <c r="G13">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H13),-F13,H13-F13)</f>
         <v>-811</v>
       </c>
       <c r="H13" s="1">
         <v>0</v>
       </c>
       <c r="I13">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J13),-H13,J13-H13)</f>
         <v>0</v>
       </c>
       <c r="J13" s="1">
         <v>0</v>
       </c>
       <c r="K13">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L13),-J13,L13-J13)</f>
         <v>0</v>
       </c>
       <c r="L13" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M13">
+        <f>IF(ISBLANK(N13),-L13,N13-L13)</f>
+        <v>0</v>
+      </c>
+      <c r="N13" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -5544,35 +5628,42 @@
         <v>3132</v>
       </c>
       <c r="E14">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F14),-D14,F14-D14)</f>
         <v>104</v>
       </c>
       <c r="F14" s="1">
         <v>3236</v>
       </c>
       <c r="G14">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H14),-F14,H14-F14)</f>
         <v>77</v>
       </c>
       <c r="H14" s="1">
         <v>3313</v>
       </c>
       <c r="I14">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J14),-H14,J14-H14)</f>
         <v>13</v>
       </c>
       <c r="J14" s="1">
         <v>3326</v>
       </c>
       <c r="K14">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L14),-J14,L14-J14)</f>
         <v>151</v>
       </c>
       <c r="L14" s="1">
         <v>3477</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M14">
+        <f>IF(ISBLANK(N14),-L14,N14-L14)</f>
+        <v>-3477</v>
+      </c>
+      <c r="N14" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>12</v>
       </c>
@@ -5584,35 +5675,42 @@
         <v>6897</v>
       </c>
       <c r="E15">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F15),-D15,F15-D15)</f>
         <v>303</v>
       </c>
       <c r="F15" s="1">
         <v>7200</v>
       </c>
       <c r="G15">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H15),-F15,H15-F15)</f>
         <v>20</v>
       </c>
       <c r="H15" s="1">
         <v>7220</v>
       </c>
       <c r="I15">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J15),-H15,J15-H15)</f>
         <v>84</v>
       </c>
       <c r="J15" s="1">
         <v>7304</v>
       </c>
       <c r="K15">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L15),-J15,L15-J15)</f>
         <v>141</v>
       </c>
       <c r="L15" s="1">
         <v>7445</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M15">
+        <f>IF(ISBLANK(N15),-L15,N15-L15)</f>
+        <v>232</v>
+      </c>
+      <c r="N15" s="1">
+        <v>7677</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>8</v>
       </c>
@@ -5624,35 +5722,42 @@
         <v>30220</v>
       </c>
       <c r="E16">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F16),-D16,F16-D16)</f>
         <v>864</v>
       </c>
       <c r="F16" s="1">
         <v>31084</v>
       </c>
       <c r="G16">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H16),-F16,H16-F16)</f>
         <v>38</v>
       </c>
       <c r="H16" s="1">
         <v>31122</v>
       </c>
       <c r="I16">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J16),-H16,J16-H16)</f>
         <v>21</v>
       </c>
       <c r="J16" s="1">
         <v>31143</v>
       </c>
       <c r="K16">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L16),-J16,L16-J16)</f>
         <v>55</v>
       </c>
       <c r="L16" s="1">
         <v>31198</v>
       </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M16">
+        <f>IF(ISBLANK(N16),-L16,N16-L16)</f>
+        <v>273</v>
+      </c>
+      <c r="N16" s="1">
+        <v>31471</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>7</v>
       </c>
@@ -5664,35 +5769,42 @@
         <v>42814</v>
       </c>
       <c r="E17">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F17),-D17,F17-D17)</f>
         <v>1226</v>
       </c>
       <c r="F17" s="1">
         <v>44040</v>
       </c>
       <c r="G17">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H17),-F17,H17-F17)</f>
         <v>19</v>
       </c>
       <c r="H17" s="1">
         <v>44059</v>
       </c>
       <c r="I17">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J17),-H17,J17-H17)</f>
         <v>17</v>
       </c>
       <c r="J17" s="1">
         <v>44076</v>
       </c>
       <c r="K17">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L17),-J17,L17-J17)</f>
         <v>54</v>
       </c>
       <c r="L17" s="1">
         <v>44130</v>
       </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M17">
+        <f>IF(ISBLANK(N17),-L17,N17-L17)</f>
+        <v>125</v>
+      </c>
+      <c r="N17" s="1">
+        <v>44255</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>4</v>
       </c>
@@ -5704,35 +5816,42 @@
         <v>64500</v>
       </c>
       <c r="E18">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F18),-D18,F18-D18)</f>
         <v>6036</v>
       </c>
       <c r="F18" s="1">
         <v>70536</v>
       </c>
       <c r="G18">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H18),-F18,H18-F18)</f>
         <v>83</v>
       </c>
       <c r="H18" s="1">
         <v>70619</v>
       </c>
       <c r="I18">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J18),-H18,J18-H18)</f>
         <v>41</v>
       </c>
       <c r="J18" s="1">
         <v>70660</v>
       </c>
       <c r="K18">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L18),-J18,L18-J18)</f>
         <v>71</v>
       </c>
       <c r="L18" s="1">
         <v>70731</v>
       </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M18">
+        <f>IF(ISBLANK(N18),-L18,N18-L18)</f>
+        <v>694</v>
+      </c>
+      <c r="N18" s="1">
+        <v>71425</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>196</v>
       </c>
@@ -5773,25 +5892,28 @@
       <c r="P20" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Y20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>197</v>
       </c>
       <c r="D21">
-        <f t="shared" ref="D21:D36" si="4">FIND(",",B21)</f>
+        <f t="shared" ref="D21:D36" si="0">FIND(",",B21)</f>
         <v>9</v>
       </c>
       <c r="E21" t="str">
-        <f t="shared" ref="E21:E36" si="5">LEFT(B21,D21-1)</f>
+        <f t="shared" ref="E21:E36" si="1">LEFT(B21,D21-1)</f>
         <v>Flanagan</v>
       </c>
       <c r="F21" t="str">
-        <f t="shared" ref="F21:F36" si="6">RIGHT(B21,LEN(B21)-(D21+1))</f>
+        <f t="shared" ref="F21:F36" si="2">RIGHT(B21,LEN(B21)-(D21+1))</f>
         <v>Luke 'Ming'</v>
       </c>
       <c r="G21" t="str">
-        <f t="shared" ref="G21:G36" si="7">F21&amp;" "&amp;E21</f>
+        <f t="shared" ref="G21:G36" si="3">F21&amp;" "&amp;E21</f>
         <v>Luke 'Ming' Flanagan</v>
       </c>
       <c r="J21" t="s">
@@ -5803,25 +5925,27 @@
       <c r="L21" s="1">
         <v>134630</v>
       </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="S21" s="2"/>
+      <c r="T21" s="1"/>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>198</v>
       </c>
       <c r="D22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="E22" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>Carthy</v>
       </c>
       <c r="F22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="2"/>
         <v>Matt</v>
       </c>
       <c r="G22" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v>Matt Carthy</v>
       </c>
       <c r="J22" t="s">
@@ -5845,25 +5969,34 @@
       <c r="P22" s="1">
         <v>87333</v>
       </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="S22" s="2"/>
+      <c r="T22" s="1"/>
+      <c r="U22" s="1"/>
+      <c r="V22" s="1"/>
+      <c r="W22" s="1"/>
+      <c r="X22" s="1"/>
+      <c r="Y22" s="1">
+        <v>87964</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>199</v>
       </c>
       <c r="D23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="E23" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>Walsh</v>
       </c>
       <c r="F23" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="2"/>
         <v>Maria</v>
       </c>
       <c r="G23" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v>Maria Walsh</v>
       </c>
       <c r="J23" t="s">
@@ -5887,25 +6020,34 @@
       <c r="P23" s="1">
         <v>78653</v>
       </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="S23" s="2"/>
+      <c r="T23" s="1"/>
+      <c r="U23" s="1"/>
+      <c r="V23" s="1"/>
+      <c r="W23" s="1"/>
+      <c r="X23" s="1"/>
+      <c r="Y23" s="1">
+        <v>79028</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>200</v>
       </c>
       <c r="D24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="E24" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>Casey</v>
       </c>
       <c r="F24" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="2"/>
         <v>Peter</v>
       </c>
       <c r="G24" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v>Peter Casey</v>
       </c>
       <c r="J24" t="s">
@@ -5929,25 +6071,34 @@
       <c r="P24" s="1">
         <v>70731</v>
       </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="S24" s="2"/>
+      <c r="T24" s="1"/>
+      <c r="U24" s="1"/>
+      <c r="V24" s="1"/>
+      <c r="W24" s="1"/>
+      <c r="X24" s="1"/>
+      <c r="Y24" s="1">
+        <v>71425</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>201</v>
       </c>
       <c r="D25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="E25" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>McHugh</v>
       </c>
       <c r="F25" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="2"/>
         <v>Saoirse</v>
       </c>
       <c r="G25" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v>Saoirse McHugh</v>
       </c>
       <c r="J25" t="s">
@@ -5971,25 +6122,34 @@
       <c r="P25" s="1">
         <v>58212</v>
       </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="S25" s="2"/>
+      <c r="T25" s="1"/>
+      <c r="U25" s="1"/>
+      <c r="V25" s="1"/>
+      <c r="W25" s="1"/>
+      <c r="X25" s="1"/>
+      <c r="Y25" s="1">
+        <v>58602</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>202</v>
       </c>
       <c r="D26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="E26" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>Smith</v>
       </c>
       <c r="F26" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="2"/>
         <v>Brendan</v>
       </c>
       <c r="G26" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v>Brendan Smith</v>
       </c>
       <c r="J26" t="s">
@@ -6013,25 +6173,34 @@
       <c r="P26" s="1">
         <v>53068</v>
       </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="S26" s="2"/>
+      <c r="T26" s="1"/>
+      <c r="U26" s="1"/>
+      <c r="V26" s="1"/>
+      <c r="W26" s="1"/>
+      <c r="X26" s="1"/>
+      <c r="Y26" s="1">
+        <v>53966</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>203</v>
       </c>
       <c r="D27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="E27" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>Rabbitte</v>
       </c>
       <c r="F27" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="2"/>
         <v>Anne</v>
       </c>
       <c r="G27" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v>Anne Rabbitte</v>
       </c>
       <c r="J27" t="s">
@@ -6055,25 +6224,34 @@
       <c r="P27" s="1">
         <v>44130</v>
       </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="S27" s="2"/>
+      <c r="T27" s="1"/>
+      <c r="U27" s="1"/>
+      <c r="V27" s="1"/>
+      <c r="W27" s="1"/>
+      <c r="X27" s="1"/>
+      <c r="Y27" s="1">
+        <v>44255</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>204</v>
       </c>
       <c r="D28">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="E28" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>Healy Eames</v>
       </c>
       <c r="F28" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="2"/>
         <v>Fidelma</v>
       </c>
       <c r="G28" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v>Fidelma Healy Eames</v>
       </c>
       <c r="J28" t="s">
@@ -6097,25 +6275,34 @@
       <c r="P28" s="1">
         <v>31198</v>
       </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="S28" s="2"/>
+      <c r="T28" s="1"/>
+      <c r="U28" s="1"/>
+      <c r="V28" s="1"/>
+      <c r="W28" s="1"/>
+      <c r="X28" s="1"/>
+      <c r="Y28" s="1">
+        <v>31471</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>205</v>
       </c>
       <c r="D29">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="E29" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>Hannigan</v>
       </c>
       <c r="F29" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="2"/>
         <v>Dominic</v>
       </c>
       <c r="G29" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v>Dominic Hannigan</v>
       </c>
       <c r="J29" t="s">
@@ -6139,25 +6326,34 @@
       <c r="P29" s="1">
         <v>16764</v>
       </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="S29" s="2"/>
+      <c r="T29" s="1"/>
+      <c r="U29" s="1"/>
+      <c r="V29" s="1"/>
+      <c r="W29" s="1"/>
+      <c r="X29" s="1"/>
+      <c r="Y29" s="1">
+        <v>17590</v>
+      </c>
+    </row>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>206</v>
       </c>
       <c r="D30">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="E30" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>Brennan</v>
       </c>
       <c r="F30" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="2"/>
         <v>Cyril</v>
       </c>
       <c r="G30" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v>Cyril Brennan</v>
       </c>
       <c r="J30" t="s">
@@ -6181,25 +6377,34 @@
       <c r="P30" s="1">
         <v>13197</v>
       </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="S30" s="2"/>
+      <c r="T30" s="1"/>
+      <c r="U30" s="1"/>
+      <c r="V30" s="1"/>
+      <c r="W30" s="1"/>
+      <c r="X30" s="1"/>
+      <c r="Y30" s="1">
+        <v>13408</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>207</v>
       </c>
       <c r="D31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="E31" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>O'Dowd</v>
       </c>
       <c r="F31" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="2"/>
         <v>Michael</v>
       </c>
       <c r="G31" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v>Michael O'Dowd</v>
       </c>
       <c r="J31" t="s">
@@ -6223,25 +6428,34 @@
       <c r="P31" s="1">
         <v>8365</v>
       </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="S31" s="2"/>
+      <c r="T31" s="1"/>
+      <c r="U31" s="1"/>
+      <c r="V31" s="1"/>
+      <c r="W31" s="1"/>
+      <c r="X31" s="1"/>
+      <c r="Y31" s="1">
+        <v>8553</v>
+      </c>
+    </row>
+    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>208</v>
       </c>
       <c r="D32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="E32" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>O'Connor</v>
       </c>
       <c r="F32" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="2"/>
         <v>Olive</v>
       </c>
       <c r="G32" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v>Olive O'Connor</v>
       </c>
       <c r="J32" t="s">
@@ -6265,25 +6479,34 @@
       <c r="P32" s="1">
         <v>7445</v>
       </c>
-    </row>
-    <row r="33" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="S32" s="2"/>
+      <c r="T32" s="1"/>
+      <c r="U32" s="1"/>
+      <c r="V32" s="1"/>
+      <c r="W32" s="1"/>
+      <c r="X32" s="1"/>
+      <c r="Y32" s="1">
+        <v>7677</v>
+      </c>
+    </row>
+    <row r="33" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>209</v>
       </c>
       <c r="D33">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="E33" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>Mahapatra</v>
       </c>
       <c r="F33" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="2"/>
         <v>Dilip</v>
       </c>
       <c r="G33" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v>Dilip Mahapatra</v>
       </c>
       <c r="J33" t="s">
@@ -6307,25 +6530,31 @@
       <c r="P33" s="1">
         <v>3477</v>
       </c>
-    </row>
-    <row r="34" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="S33" s="2"/>
+      <c r="T33" s="1"/>
+      <c r="U33" s="1"/>
+      <c r="V33" s="1"/>
+      <c r="W33" s="1"/>
+      <c r="X33" s="1"/>
+    </row>
+    <row r="34" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>210</v>
       </c>
       <c r="D34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="E34" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>Greene</v>
       </c>
       <c r="F34" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="2"/>
         <v>Patrick</v>
       </c>
       <c r="G34" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v>Patrick Greene</v>
       </c>
       <c r="J34" t="s">
@@ -6349,25 +6578,31 @@
       <c r="P34" s="1">
         <v>2694</v>
       </c>
-    </row>
-    <row r="35" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="S34" s="2"/>
+      <c r="T34" s="1"/>
+      <c r="U34" s="1"/>
+      <c r="V34" s="1"/>
+      <c r="W34" s="1"/>
+      <c r="X34" s="1"/>
+    </row>
+    <row r="35" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>211</v>
       </c>
       <c r="D35">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="E35" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>Miller</v>
       </c>
       <c r="F35" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="2"/>
         <v>James</v>
       </c>
       <c r="G35" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v>James Miller</v>
       </c>
       <c r="J35" t="s">
@@ -6385,25 +6620,29 @@
       <c r="N35" s="1">
         <v>1412</v>
       </c>
-    </row>
-    <row r="36" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="S35" s="2"/>
+      <c r="T35" s="1"/>
+      <c r="U35" s="1"/>
+      <c r="V35" s="1"/>
+    </row>
+    <row r="36" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>212</v>
       </c>
       <c r="D36">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="E36" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>Mulcahy</v>
       </c>
       <c r="F36" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="2"/>
         <v>Diarmaid</v>
       </c>
       <c r="G36" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v>Diarmaid Mulcahy</v>
       </c>
       <c r="J36" t="s">
@@ -6424,8 +6663,13 @@
       <c r="O36" s="1">
         <v>1490</v>
       </c>
-    </row>
-    <row r="37" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="S36" s="2"/>
+      <c r="T36" s="1"/>
+      <c r="U36" s="1"/>
+      <c r="V36" s="1"/>
+      <c r="W36" s="1"/>
+    </row>
+    <row r="37" spans="2:24" x14ac:dyDescent="0.25">
       <c r="J37" t="s">
         <v>255</v>
       </c>
@@ -6438,9 +6682,10 @@
       <c r="M37">
         <v>811</v>
       </c>
+      <c r="S37" s="2"/>
     </row>
   </sheetData>
-  <sortState ref="A2:L18">
+  <sortState ref="A2:N18">
     <sortCondition ref="B2:B18"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6451,7 +6696,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+    <sheetView topLeftCell="L1" workbookViewId="0">
       <selection activeCell="Q2" sqref="Q2:R24"/>
     </sheetView>
   </sheetViews>
@@ -6522,49 +6767,49 @@
         <v>4665</v>
       </c>
       <c r="E2">
-        <f>IF(ISBLANK(F2),-D2,F2-D2)</f>
+        <f t="shared" ref="E2:E24" si="0">IF(ISBLANK(F2),-D2,F2-D2)</f>
         <v>26</v>
       </c>
       <c r="F2" s="1">
         <v>4691</v>
       </c>
       <c r="G2">
-        <f>IF(ISBLANK(H2),-F2,H2-F2)</f>
+        <f t="shared" ref="G2:G24" si="1">IF(ISBLANK(H2),-F2,H2-F2)</f>
         <v>43</v>
       </c>
       <c r="H2" s="1">
         <v>4734</v>
       </c>
       <c r="I2">
-        <f>IF(ISBLANK(J2),-H2,J2-H2)</f>
+        <f t="shared" ref="I2:I24" si="2">IF(ISBLANK(J2),-H2,J2-H2)</f>
         <v>57</v>
       </c>
       <c r="J2" s="1">
         <v>4791</v>
       </c>
       <c r="K2">
-        <f>IF(ISBLANK(L2),-J2,L2-J2)</f>
+        <f t="shared" ref="K2:K24" si="3">IF(ISBLANK(L2),-J2,L2-J2)</f>
         <v>50</v>
       </c>
       <c r="L2" s="1">
         <v>4841</v>
       </c>
       <c r="M2">
-        <f>IF(ISBLANK(N2),-L2,N2-L2)</f>
+        <f t="shared" ref="M2:M24" si="4">IF(ISBLANK(N2),-L2,N2-L2)</f>
         <v>115</v>
       </c>
       <c r="N2" s="1">
         <v>4956</v>
       </c>
       <c r="O2">
-        <f>IF(ISBLANK(P2),-N2,P2-N2)</f>
+        <f t="shared" ref="O2:O24" si="5">IF(ISBLANK(P2),-N2,P2-N2)</f>
         <v>72</v>
       </c>
       <c r="P2" s="1">
         <v>5028</v>
       </c>
       <c r="Q2">
-        <f>IF(ISBLANK(R2),-P2,R2-P2)</f>
+        <f t="shared" ref="Q2:Q24" si="6">IF(ISBLANK(R2),-P2,R2-P2)</f>
         <v>104</v>
       </c>
       <c r="R2" s="1">
@@ -6582,49 +6827,49 @@
         <v>69166</v>
       </c>
       <c r="E3">
-        <f>IF(ISBLANK(F3),-D3,F3-D3)</f>
+        <f t="shared" si="0"/>
         <v>35</v>
       </c>
       <c r="F3" s="1">
         <v>69201</v>
       </c>
       <c r="G3">
-        <f>IF(ISBLANK(H3),-F3,H3-F3)</f>
+        <f t="shared" si="1"/>
         <v>71</v>
       </c>
       <c r="H3" s="1">
         <v>69272</v>
       </c>
       <c r="I3">
-        <f>IF(ISBLANK(J3),-H3,J3-H3)</f>
+        <f t="shared" si="2"/>
         <v>44</v>
       </c>
       <c r="J3" s="1">
         <v>69316</v>
       </c>
       <c r="K3">
-        <f>IF(ISBLANK(L3),-J3,L3-J3)</f>
+        <f t="shared" si="3"/>
         <v>66</v>
       </c>
       <c r="L3" s="1">
         <v>69382</v>
       </c>
       <c r="M3">
-        <f>IF(ISBLANK(N3),-L3,N3-L3)</f>
+        <f t="shared" si="4"/>
         <v>129</v>
       </c>
       <c r="N3" s="1">
         <v>69511</v>
       </c>
       <c r="O3">
-        <f>IF(ISBLANK(P3),-N3,P3-N3)</f>
+        <f t="shared" si="5"/>
         <v>45</v>
       </c>
       <c r="P3" s="1">
         <v>69556</v>
       </c>
       <c r="Q3">
-        <f>IF(ISBLANK(R3),-P3,R3-P3)</f>
+        <f t="shared" si="6"/>
         <v>116</v>
       </c>
       <c r="R3" s="1">
@@ -6642,49 +6887,49 @@
         <v>10582</v>
       </c>
       <c r="E4">
-        <f>IF(ISBLANK(F4),-D4,F4-D4)</f>
+        <f t="shared" si="0"/>
         <v>57</v>
       </c>
       <c r="F4" s="1">
         <v>10639</v>
       </c>
       <c r="G4">
-        <f>IF(ISBLANK(H4),-F4,H4-F4)</f>
+        <f t="shared" si="1"/>
         <v>106</v>
       </c>
       <c r="H4" s="1">
         <v>10745</v>
       </c>
       <c r="I4">
-        <f>IF(ISBLANK(J4),-H4,J4-H4)</f>
+        <f t="shared" si="2"/>
         <v>138</v>
       </c>
       <c r="J4" s="1">
         <v>10883</v>
       </c>
       <c r="K4">
-        <f>IF(ISBLANK(L4),-J4,L4-J4)</f>
+        <f t="shared" si="3"/>
         <v>54</v>
       </c>
       <c r="L4" s="1">
         <v>10937</v>
       </c>
       <c r="M4">
-        <f>IF(ISBLANK(N4),-L4,N4-L4)</f>
+        <f t="shared" si="4"/>
         <v>300</v>
       </c>
       <c r="N4" s="1">
         <v>11237</v>
       </c>
       <c r="O4">
-        <f>IF(ISBLANK(P4),-N4,P4-N4)</f>
+        <f t="shared" si="5"/>
         <v>159</v>
       </c>
       <c r="P4" s="1">
         <v>11396</v>
       </c>
       <c r="Q4">
-        <f>IF(ISBLANK(R4),-P4,R4-P4)</f>
+        <f t="shared" si="6"/>
         <v>322</v>
       </c>
       <c r="R4" s="1">
@@ -6702,49 +6947,49 @@
         <v>64605</v>
       </c>
       <c r="E5">
-        <f>IF(ISBLANK(F5),-D5,F5-D5)</f>
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="F5" s="1">
         <v>64631</v>
       </c>
       <c r="G5">
-        <f>IF(ISBLANK(H5),-F5,H5-F5)</f>
+        <f t="shared" si="1"/>
         <v>61</v>
       </c>
       <c r="H5" s="1">
         <v>64692</v>
       </c>
       <c r="I5">
-        <f>IF(ISBLANK(J5),-H5,J5-H5)</f>
+        <f t="shared" si="2"/>
         <v>71</v>
       </c>
       <c r="J5" s="1">
         <v>64763</v>
       </c>
       <c r="K5">
-        <f>IF(ISBLANK(L5),-J5,L5-J5)</f>
+        <f t="shared" si="3"/>
         <v>136</v>
       </c>
       <c r="L5" s="1">
         <v>64899</v>
       </c>
       <c r="M5">
-        <f>IF(ISBLANK(N5),-L5,N5-L5)</f>
+        <f t="shared" si="4"/>
         <v>106</v>
       </c>
       <c r="N5" s="1">
         <v>65005</v>
       </c>
       <c r="O5">
-        <f>IF(ISBLANK(P5),-N5,P5-N5)</f>
+        <f t="shared" si="5"/>
         <v>110</v>
       </c>
       <c r="P5" s="1">
         <v>65115</v>
       </c>
       <c r="Q5">
-        <f>IF(ISBLANK(R5),-P5,R5-P5)</f>
+        <f t="shared" si="6"/>
         <v>137</v>
       </c>
       <c r="R5" s="1">
@@ -6762,49 +7007,49 @@
         <v>38738</v>
       </c>
       <c r="E6">
-        <f>IF(ISBLANK(F6),-D6,F6-D6)</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="F6" s="1">
         <v>38755</v>
       </c>
       <c r="G6">
-        <f>IF(ISBLANK(H6),-F6,H6-F6)</f>
+        <f t="shared" si="1"/>
         <v>33</v>
       </c>
       <c r="H6" s="1">
         <v>38788</v>
       </c>
       <c r="I6">
-        <f>IF(ISBLANK(J6),-H6,J6-H6)</f>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="J6" s="1">
         <v>38804</v>
       </c>
       <c r="K6">
-        <f>IF(ISBLANK(L6),-J6,L6-J6)</f>
+        <f t="shared" si="3"/>
         <v>38</v>
       </c>
       <c r="L6" s="1">
         <v>38842</v>
       </c>
       <c r="M6">
-        <f>IF(ISBLANK(N6),-L6,N6-L6)</f>
+        <f t="shared" si="4"/>
         <v>84</v>
       </c>
       <c r="N6" s="1">
         <v>38926</v>
       </c>
       <c r="O6">
-        <f>IF(ISBLANK(P6),-N6,P6-N6)</f>
+        <f t="shared" si="5"/>
         <v>24</v>
       </c>
       <c r="P6" s="1">
         <v>38950</v>
       </c>
       <c r="Q6">
-        <f>IF(ISBLANK(R6),-P6,R6-P6)</f>
+        <f t="shared" si="6"/>
         <v>46</v>
       </c>
       <c r="R6" s="1">
@@ -6822,49 +7067,49 @@
         <v>3182</v>
       </c>
       <c r="E7">
-        <f>IF(ISBLANK(F7),-D7,F7-D7)</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="F7" s="1">
         <v>3197</v>
       </c>
       <c r="G7">
-        <f>IF(ISBLANK(H7),-F7,H7-F7)</f>
+        <f t="shared" si="1"/>
         <v>60</v>
       </c>
       <c r="H7" s="1">
         <v>3257</v>
       </c>
       <c r="I7">
-        <f>IF(ISBLANK(J7),-H7,J7-H7)</f>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="J7" s="1">
         <v>3300</v>
       </c>
       <c r="K7">
-        <f>IF(ISBLANK(L7),-J7,L7-J7)</f>
+        <f t="shared" si="3"/>
         <v>32</v>
       </c>
       <c r="L7" s="1">
         <v>3332</v>
       </c>
       <c r="M7">
-        <f>IF(ISBLANK(N7),-L7,N7-L7)</f>
+        <f t="shared" si="4"/>
         <v>-3332</v>
       </c>
       <c r="N7" s="1">
         <v>0</v>
       </c>
       <c r="O7">
-        <f>IF(ISBLANK(P7),-N7,P7-N7)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P7" s="1">
         <v>0</v>
       </c>
       <c r="Q7">
-        <f>IF(ISBLANK(R7),-P7,R7-P7)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="R7" s="1">
@@ -6882,49 +7127,49 @@
         <v>9306</v>
       </c>
       <c r="E8">
-        <f>IF(ISBLANK(F8),-D8,F8-D8)</f>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="F8" s="1">
         <v>9331</v>
       </c>
       <c r="G8">
-        <f>IF(ISBLANK(H8),-F8,H8-F8)</f>
+        <f t="shared" si="1"/>
         <v>70</v>
       </c>
       <c r="H8" s="1">
         <v>9401</v>
       </c>
       <c r="I8">
-        <f>IF(ISBLANK(J8),-H8,J8-H8)</f>
+        <f t="shared" si="2"/>
         <v>35</v>
       </c>
       <c r="J8" s="1">
         <v>9436</v>
       </c>
       <c r="K8">
-        <f>IF(ISBLANK(L8),-J8,L8-J8)</f>
+        <f t="shared" si="3"/>
         <v>60</v>
       </c>
       <c r="L8" s="1">
         <v>9496</v>
       </c>
       <c r="M8">
-        <f>IF(ISBLANK(N8),-L8,N8-L8)</f>
+        <f t="shared" si="4"/>
         <v>228</v>
       </c>
       <c r="N8" s="1">
         <v>9724</v>
       </c>
       <c r="O8">
-        <f>IF(ISBLANK(P8),-N8,P8-N8)</f>
+        <f t="shared" si="5"/>
         <v>145</v>
       </c>
       <c r="P8" s="1">
         <v>9869</v>
       </c>
       <c r="Q8">
-        <f>IF(ISBLANK(R8),-P8,R8-P8)</f>
+        <f t="shared" si="6"/>
         <v>106</v>
       </c>
       <c r="R8" s="1">
@@ -6942,49 +7187,49 @@
         <v>7475</v>
       </c>
       <c r="E9">
-        <f>IF(ISBLANK(F9),-D9,F9-D9)</f>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="F9" s="1">
         <v>7498</v>
       </c>
       <c r="G9">
-        <f>IF(ISBLANK(H9),-F9,H9-F9)</f>
+        <f t="shared" si="1"/>
         <v>98</v>
       </c>
       <c r="H9" s="1">
         <v>7596</v>
       </c>
       <c r="I9">
-        <f>IF(ISBLANK(J9),-H9,J9-H9)</f>
+        <f t="shared" si="2"/>
         <v>142</v>
       </c>
       <c r="J9" s="1">
         <v>7738</v>
       </c>
       <c r="K9">
-        <f>IF(ISBLANK(L9),-J9,L9-J9)</f>
+        <f t="shared" si="3"/>
         <v>70</v>
       </c>
       <c r="L9" s="1">
         <v>7808</v>
       </c>
       <c r="M9">
-        <f>IF(ISBLANK(N9),-L9,N9-L9)</f>
+        <f t="shared" si="4"/>
         <v>197</v>
       </c>
       <c r="N9" s="1">
         <v>8005</v>
       </c>
       <c r="O9">
-        <f>IF(ISBLANK(P9),-N9,P9-N9)</f>
+        <f t="shared" si="5"/>
         <v>192</v>
       </c>
       <c r="P9" s="1">
         <v>8197</v>
       </c>
       <c r="Q9">
-        <f>IF(ISBLANK(R9),-P9,R9-P9)</f>
+        <f t="shared" si="6"/>
         <v>176</v>
       </c>
       <c r="R9" s="1">
@@ -7002,49 +7247,49 @@
         <v>84083</v>
       </c>
       <c r="E10">
-        <f>IF(ISBLANK(F10),-D10,F10-D10)</f>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="F10" s="1">
         <v>84106</v>
       </c>
       <c r="G10">
-        <f>IF(ISBLANK(H10),-F10,H10-F10)</f>
+        <f t="shared" si="1"/>
         <v>58</v>
       </c>
       <c r="H10" s="1">
         <v>84164</v>
       </c>
       <c r="I10">
-        <f>IF(ISBLANK(J10),-H10,J10-H10)</f>
+        <f t="shared" si="2"/>
         <v>74</v>
       </c>
       <c r="J10" s="1">
         <v>84238</v>
       </c>
       <c r="K10">
-        <f>IF(ISBLANK(L10),-J10,L10-J10)</f>
+        <f t="shared" si="3"/>
         <v>150</v>
       </c>
       <c r="L10" s="1">
         <v>84388</v>
       </c>
       <c r="M10">
-        <f>IF(ISBLANK(N10),-L10,N10-L10)</f>
+        <f t="shared" si="4"/>
         <v>171</v>
       </c>
       <c r="N10" s="1">
         <v>84559</v>
       </c>
       <c r="O10">
-        <f>IF(ISBLANK(P10),-N10,P10-N10)</f>
+        <f t="shared" si="5"/>
         <v>95</v>
       </c>
       <c r="P10" s="1">
         <v>84654</v>
       </c>
       <c r="Q10">
-        <f>IF(ISBLANK(R10),-P10,R10-P10)</f>
+        <f t="shared" si="6"/>
         <v>187</v>
       </c>
       <c r="R10" s="1">
@@ -7062,49 +7307,49 @@
         <v>118444</v>
       </c>
       <c r="E11">
-        <f>IF(ISBLANK(F11),-D11,F11-D11)</f>
+        <f t="shared" si="0"/>
         <v>45</v>
       </c>
       <c r="F11" s="1">
         <v>118489</v>
       </c>
       <c r="G11">
-        <f>IF(ISBLANK(H11),-F11,H11-F11)</f>
+        <f t="shared" si="1"/>
         <v>186</v>
       </c>
       <c r="H11" s="1">
         <v>118675</v>
       </c>
       <c r="I11">
-        <f>IF(ISBLANK(J11),-H11,J11-H11)</f>
+        <f t="shared" si="2"/>
         <v>98</v>
       </c>
       <c r="J11" s="1">
         <v>118773</v>
       </c>
       <c r="K11">
-        <f>IF(ISBLANK(L11),-J11,L11-J11)</f>
+        <f t="shared" si="3"/>
         <v>350</v>
       </c>
       <c r="L11" s="1">
         <v>119123</v>
       </c>
       <c r="M11">
-        <f>IF(ISBLANK(N11),-L11,N11-L11)</f>
+        <f t="shared" si="4"/>
         <v>257</v>
       </c>
       <c r="N11" s="1">
         <v>119380</v>
       </c>
       <c r="O11">
-        <f>IF(ISBLANK(P11),-N11,P11-N11)</f>
+        <f t="shared" si="5"/>
         <v>165</v>
       </c>
       <c r="P11" s="1">
         <v>119545</v>
       </c>
       <c r="Q11">
-        <f>IF(ISBLANK(R11),-P11,R11-P11)</f>
+        <f t="shared" si="6"/>
         <v>170</v>
       </c>
       <c r="R11" s="1">
@@ -7122,49 +7367,49 @@
         <v>2395</v>
       </c>
       <c r="E12">
-        <f>IF(ISBLANK(F12),-D12,F12-D12)</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="F12" s="1">
         <v>2409</v>
       </c>
       <c r="G12">
-        <f>IF(ISBLANK(H12),-F12,H12-F12)</f>
+        <f t="shared" si="1"/>
         <v>-2409</v>
       </c>
       <c r="H12" s="1">
         <v>0</v>
       </c>
       <c r="I12">
-        <f>IF(ISBLANK(J12),-H12,J12-H12)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J12" s="1">
         <v>0</v>
       </c>
       <c r="K12">
-        <f>IF(ISBLANK(L12),-J12,L12-J12)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L12" s="1">
         <v>0</v>
       </c>
       <c r="M12">
-        <f>IF(ISBLANK(N12),-L12,N12-L12)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N12" s="1">
         <v>0</v>
       </c>
       <c r="O12">
-        <f>IF(ISBLANK(P12),-N12,P12-N12)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P12" s="1">
         <v>0</v>
       </c>
       <c r="Q12">
-        <f>IF(ISBLANK(R12),-P12,R12-P12)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="R12" s="1">
@@ -7182,49 +7427,49 @@
         <v>9423</v>
       </c>
       <c r="E13">
-        <f>IF(ISBLANK(F13),-D13,F13-D13)</f>
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="F13" s="1">
         <v>9455</v>
       </c>
       <c r="G13">
-        <f>IF(ISBLANK(H13),-F13,H13-F13)</f>
+        <f t="shared" si="1"/>
         <v>325</v>
       </c>
       <c r="H13" s="1">
         <v>9780</v>
       </c>
       <c r="I13">
-        <f>IF(ISBLANK(J13),-H13,J13-H13)</f>
+        <f t="shared" si="2"/>
         <v>75</v>
       </c>
       <c r="J13" s="1">
         <v>9855</v>
       </c>
       <c r="K13">
-        <f>IF(ISBLANK(L13),-J13,L13-J13)</f>
+        <f t="shared" si="3"/>
         <v>114</v>
       </c>
       <c r="L13" s="1">
         <v>9969</v>
       </c>
       <c r="M13">
-        <f>IF(ISBLANK(N13),-L13,N13-L13)</f>
+        <f t="shared" si="4"/>
         <v>280</v>
       </c>
       <c r="N13" s="1">
         <v>10249</v>
       </c>
       <c r="O13">
-        <f>IF(ISBLANK(P13),-N13,P13-N13)</f>
+        <f t="shared" si="5"/>
         <v>78</v>
       </c>
       <c r="P13" s="1">
         <v>10327</v>
       </c>
       <c r="Q13">
-        <f>IF(ISBLANK(R13),-P13,R13-P13)</f>
+        <f t="shared" si="6"/>
         <v>137</v>
       </c>
       <c r="R13" s="1">
@@ -7242,49 +7487,49 @@
         <v>79072</v>
       </c>
       <c r="E14">
-        <f>IF(ISBLANK(F14),-D14,F14-D14)</f>
+        <f t="shared" si="0"/>
         <v>68</v>
       </c>
       <c r="F14" s="1">
         <v>79140</v>
       </c>
       <c r="G14">
-        <f>IF(ISBLANK(H14),-F14,H14-F14)</f>
+        <f t="shared" si="1"/>
         <v>142</v>
       </c>
       <c r="H14" s="1">
         <v>79282</v>
       </c>
       <c r="I14">
-        <f>IF(ISBLANK(J14),-H14,J14-H14)</f>
+        <f t="shared" si="2"/>
         <v>105</v>
       </c>
       <c r="J14" s="1">
         <v>79387</v>
       </c>
       <c r="K14">
-        <f>IF(ISBLANK(L14),-J14,L14-J14)</f>
+        <f t="shared" si="3"/>
         <v>186</v>
       </c>
       <c r="L14" s="1">
         <v>79573</v>
       </c>
       <c r="M14">
-        <f>IF(ISBLANK(N14),-L14,N14-L14)</f>
+        <f t="shared" si="4"/>
         <v>168</v>
       </c>
       <c r="N14" s="1">
         <v>79741</v>
       </c>
       <c r="O14">
-        <f>IF(ISBLANK(P14),-N14,P14-N14)</f>
+        <f t="shared" si="5"/>
         <v>204</v>
       </c>
       <c r="P14" s="1">
         <v>79945</v>
       </c>
       <c r="Q14">
-        <f>IF(ISBLANK(R14),-P14,R14-P14)</f>
+        <f t="shared" si="6"/>
         <v>305</v>
       </c>
       <c r="R14" s="1">
@@ -7302,49 +7547,49 @@
         <v>22075</v>
       </c>
       <c r="E15">
-        <f>IF(ISBLANK(F15),-D15,F15-D15)</f>
+        <f t="shared" si="0"/>
         <v>38</v>
       </c>
       <c r="F15" s="1">
         <v>22113</v>
       </c>
       <c r="G15">
-        <f>IF(ISBLANK(H15),-F15,H15-F15)</f>
+        <f t="shared" si="1"/>
         <v>80</v>
       </c>
       <c r="H15" s="1">
         <v>22193</v>
       </c>
       <c r="I15">
-        <f>IF(ISBLANK(J15),-H15,J15-H15)</f>
+        <f t="shared" si="2"/>
         <v>58</v>
       </c>
       <c r="J15" s="1">
         <v>22251</v>
       </c>
       <c r="K15">
-        <f>IF(ISBLANK(L15),-J15,L15-J15)</f>
+        <f t="shared" si="3"/>
         <v>70</v>
       </c>
       <c r="L15" s="1">
         <v>22321</v>
       </c>
       <c r="M15">
-        <f>IF(ISBLANK(N15),-L15,N15-L15)</f>
+        <f t="shared" si="4"/>
         <v>62</v>
       </c>
       <c r="N15" s="1">
         <v>22383</v>
       </c>
       <c r="O15">
-        <f>IF(ISBLANK(P15),-N15,P15-N15)</f>
+        <f t="shared" si="5"/>
         <v>70</v>
       </c>
       <c r="P15" s="1">
         <v>22453</v>
       </c>
       <c r="Q15">
-        <f>IF(ISBLANK(R15),-P15,R15-P15)</f>
+        <f t="shared" si="6"/>
         <v>173</v>
       </c>
       <c r="R15" s="1">
@@ -7362,49 +7607,49 @@
         <v>9823</v>
       </c>
       <c r="E16">
-        <f>IF(ISBLANK(F16),-D16,F16-D16)</f>
+        <f t="shared" si="0"/>
         <v>37</v>
       </c>
       <c r="F16" s="1">
         <v>9860</v>
       </c>
       <c r="G16">
-        <f>IF(ISBLANK(H16),-F16,H16-F16)</f>
+        <f t="shared" si="1"/>
         <v>76</v>
       </c>
       <c r="H16" s="1">
         <v>9936</v>
       </c>
       <c r="I16">
-        <f>IF(ISBLANK(J16),-H16,J16-H16)</f>
+        <f t="shared" si="2"/>
         <v>54</v>
       </c>
       <c r="J16" s="1">
         <v>9990</v>
       </c>
       <c r="K16">
-        <f>IF(ISBLANK(L16),-J16,L16-J16)</f>
+        <f t="shared" si="3"/>
         <v>184</v>
       </c>
       <c r="L16" s="1">
         <v>10174</v>
       </c>
       <c r="M16">
-        <f>IF(ISBLANK(N16),-L16,N16-L16)</f>
+        <f t="shared" si="4"/>
         <v>52</v>
       </c>
       <c r="N16" s="1">
         <v>10226</v>
       </c>
       <c r="O16">
-        <f>IF(ISBLANK(P16),-N16,P16-N16)</f>
+        <f t="shared" si="5"/>
         <v>168</v>
       </c>
       <c r="P16" s="1">
         <v>10394</v>
       </c>
       <c r="Q16">
-        <f>IF(ISBLANK(R16),-P16,R16-P16)</f>
+        <f t="shared" si="6"/>
         <v>214</v>
       </c>
       <c r="R16" s="1">
@@ -7422,49 +7667,49 @@
         <v>3682</v>
       </c>
       <c r="E17">
-        <f>IF(ISBLANK(F17),-D17,F17-D17)</f>
+        <f t="shared" si="0"/>
         <v>77</v>
       </c>
       <c r="F17" s="1">
         <v>3759</v>
       </c>
       <c r="G17">
-        <f>IF(ISBLANK(H17),-F17,H17-F17)</f>
+        <f t="shared" si="1"/>
         <v>44</v>
       </c>
       <c r="H17" s="1">
         <v>3803</v>
       </c>
       <c r="I17">
-        <f>IF(ISBLANK(J17),-H17,J17-H17)</f>
+        <f t="shared" si="2"/>
         <v>116</v>
       </c>
       <c r="J17" s="1">
         <v>3919</v>
       </c>
       <c r="K17">
-        <f>IF(ISBLANK(L17),-J17,L17-J17)</f>
+        <f t="shared" si="3"/>
         <v>87</v>
       </c>
       <c r="L17" s="1">
         <v>4006</v>
       </c>
       <c r="M17">
-        <f>IF(ISBLANK(N17),-L17,N17-L17)</f>
+        <f t="shared" si="4"/>
         <v>41</v>
       </c>
       <c r="N17" s="1">
         <v>4047</v>
       </c>
       <c r="O17">
-        <f>IF(ISBLANK(P17),-N17,P17-N17)</f>
+        <f t="shared" si="5"/>
         <v>134</v>
       </c>
       <c r="P17" s="1">
         <v>4181</v>
       </c>
       <c r="Q17">
-        <f>IF(ISBLANK(R17),-P17,R17-P17)</f>
+        <f t="shared" si="6"/>
         <v>-4181</v>
       </c>
       <c r="R17" s="1">
@@ -7482,49 +7727,49 @@
         <v>75946</v>
       </c>
       <c r="E18">
-        <f>IF(ISBLANK(F18),-D18,F18-D18)</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="F18" s="1">
         <v>76046</v>
       </c>
       <c r="G18">
-        <f>IF(ISBLANK(H18),-F18,H18-F18)</f>
+        <f t="shared" si="1"/>
         <v>201</v>
       </c>
       <c r="H18" s="1">
         <v>76247</v>
       </c>
       <c r="I18">
-        <f>IF(ISBLANK(J18),-H18,J18-H18)</f>
+        <f t="shared" si="2"/>
         <v>126</v>
       </c>
       <c r="J18" s="1">
         <v>76373</v>
       </c>
       <c r="K18">
-        <f>IF(ISBLANK(L18),-J18,L18-J18)</f>
+        <f t="shared" si="3"/>
         <v>272</v>
       </c>
       <c r="L18" s="1">
         <v>76645</v>
       </c>
       <c r="M18">
-        <f>IF(ISBLANK(N18),-L18,N18-L18)</f>
+        <f t="shared" si="4"/>
         <v>74</v>
       </c>
       <c r="N18" s="1">
         <v>76719</v>
       </c>
       <c r="O18">
-        <f>IF(ISBLANK(P18),-N18,P18-N18)</f>
+        <f t="shared" si="5"/>
         <v>301</v>
       </c>
       <c r="P18" s="1">
         <v>77020</v>
       </c>
       <c r="Q18">
-        <f>IF(ISBLANK(R18),-P18,R18-P18)</f>
+        <f t="shared" si="6"/>
         <v>283</v>
       </c>
       <c r="R18" s="1">
@@ -7542,49 +7787,49 @@
         <v>2864</v>
       </c>
       <c r="E19">
-        <f>IF(ISBLANK(F19),-D19,F19-D19)</f>
+        <f t="shared" si="0"/>
         <v>34</v>
       </c>
       <c r="F19" s="1">
         <v>2898</v>
       </c>
       <c r="G19">
-        <f>IF(ISBLANK(H19),-F19,H19-F19)</f>
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="H19" s="1">
         <v>2919</v>
       </c>
       <c r="I19">
-        <f>IF(ISBLANK(J19),-H19,J19-H19)</f>
+        <f t="shared" si="2"/>
         <v>148</v>
       </c>
       <c r="J19" s="1">
         <v>3067</v>
       </c>
       <c r="K19">
-        <f>IF(ISBLANK(L19),-J19,L19-J19)</f>
+        <f t="shared" si="3"/>
         <v>-3067</v>
       </c>
       <c r="L19" s="1">
         <v>0</v>
       </c>
       <c r="M19">
-        <f>IF(ISBLANK(N19),-L19,N19-L19)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N19" s="1">
         <v>0</v>
       </c>
       <c r="O19">
-        <f>IF(ISBLANK(P19),-N19,P19-N19)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P19" s="1">
         <v>0</v>
       </c>
       <c r="Q19">
-        <f>IF(ISBLANK(R19),-P19,R19-P19)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="R19" s="1">
@@ -7602,49 +7847,49 @@
         <v>2416</v>
       </c>
       <c r="E20">
-        <f>IF(ISBLANK(F20),-D20,F20-D20)</f>
+        <f t="shared" si="0"/>
         <v>48</v>
       </c>
       <c r="F20" s="1">
         <v>2464</v>
       </c>
       <c r="G20">
-        <f>IF(ISBLANK(H20),-F20,H20-F20)</f>
+        <f t="shared" si="1"/>
         <v>78</v>
       </c>
       <c r="H20" s="1">
         <v>2542</v>
       </c>
       <c r="I20">
-        <f>IF(ISBLANK(J20),-H20,J20-H20)</f>
+        <f t="shared" si="2"/>
         <v>-2542</v>
       </c>
       <c r="J20" s="1">
         <v>0</v>
       </c>
       <c r="K20">
-        <f>IF(ISBLANK(L20),-J20,L20-J20)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L20" s="1">
         <v>0</v>
       </c>
       <c r="M20">
-        <f>IF(ISBLANK(N20),-L20,N20-L20)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N20" s="1">
         <v>0</v>
       </c>
       <c r="O20">
-        <f>IF(ISBLANK(P20),-N20,P20-N20)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P20" s="1">
         <v>0</v>
       </c>
       <c r="Q20">
-        <f>IF(ISBLANK(R20),-P20,R20-P20)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="R20" s="1">
@@ -7662,49 +7907,49 @@
         <v>1423</v>
       </c>
       <c r="E21">
-        <f>IF(ISBLANK(F21),-D21,F21-D21)</f>
+        <f t="shared" si="0"/>
         <v>-1423</v>
       </c>
       <c r="F21" s="1">
         <v>0</v>
       </c>
       <c r="G21">
-        <f>IF(ISBLANK(H21),-F21,H21-F21)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H21" s="1">
         <v>0</v>
       </c>
       <c r="I21">
-        <f>IF(ISBLANK(J21),-H21,J21-H21)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J21" s="1">
         <v>0</v>
       </c>
       <c r="K21">
-        <f>IF(ISBLANK(L21),-J21,L21-J21)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L21" s="1">
         <v>0</v>
       </c>
       <c r="M21">
-        <f>IF(ISBLANK(N21),-L21,N21-L21)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N21" s="1">
         <v>0</v>
       </c>
       <c r="O21">
-        <f>IF(ISBLANK(P21),-N21,P21-N21)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P21" s="1">
         <v>0</v>
       </c>
       <c r="Q21">
-        <f>IF(ISBLANK(R21),-P21,R21-P21)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="R21" s="1">
@@ -7722,49 +7967,49 @@
         <v>14802</v>
       </c>
       <c r="E22">
-        <f>IF(ISBLANK(F22),-D22,F22-D22)</f>
+        <f t="shared" si="0"/>
         <v>156</v>
       </c>
       <c r="F22" s="1">
         <v>14958</v>
       </c>
       <c r="G22">
-        <f>IF(ISBLANK(H22),-F22,H22-F22)</f>
+        <f t="shared" si="1"/>
         <v>51</v>
       </c>
       <c r="H22" s="1">
         <v>15009</v>
       </c>
       <c r="I22">
-        <f>IF(ISBLANK(J22),-H22,J22-H22)</f>
+        <f t="shared" si="2"/>
         <v>198</v>
       </c>
       <c r="J22" s="1">
         <v>15207</v>
       </c>
       <c r="K22">
-        <f>IF(ISBLANK(L22),-J22,L22-J22)</f>
+        <f t="shared" si="3"/>
         <v>146</v>
       </c>
       <c r="L22" s="1">
         <v>15353</v>
       </c>
       <c r="M22">
-        <f>IF(ISBLANK(N22),-L22,N22-L22)</f>
+        <f t="shared" si="4"/>
         <v>41</v>
       </c>
       <c r="N22" s="1">
         <v>15394</v>
       </c>
       <c r="O22">
-        <f>IF(ISBLANK(P22),-N22,P22-N22)</f>
+        <f t="shared" si="5"/>
         <v>392</v>
       </c>
       <c r="P22" s="1">
         <v>15786</v>
       </c>
       <c r="Q22">
-        <f>IF(ISBLANK(R22),-P22,R22-P22)</f>
+        <f t="shared" si="6"/>
         <v>321</v>
       </c>
       <c r="R22" s="1">
@@ -7782,49 +8027,49 @@
         <v>81741</v>
       </c>
       <c r="E23">
-        <f>IF(ISBLANK(F23),-D23,F23-D23)</f>
+        <f t="shared" si="0"/>
         <v>253</v>
       </c>
       <c r="F23" s="1">
         <v>81994</v>
       </c>
       <c r="G23">
-        <f>IF(ISBLANK(H23),-F23,H23-F23)</f>
+        <f t="shared" si="1"/>
         <v>130</v>
       </c>
       <c r="H23" s="1">
         <v>82124</v>
       </c>
       <c r="I23">
-        <f>IF(ISBLANK(J23),-H23,J23-H23)</f>
+        <f t="shared" si="2"/>
         <v>211</v>
       </c>
       <c r="J23" s="1">
         <v>82335</v>
       </c>
       <c r="K23">
-        <f>IF(ISBLANK(L23),-J23,L23-J23)</f>
+        <f t="shared" si="3"/>
         <v>323</v>
       </c>
       <c r="L23" s="1">
         <v>82658</v>
       </c>
       <c r="M23">
-        <f>IF(ISBLANK(N23),-L23,N23-L23)</f>
+        <f t="shared" si="4"/>
         <v>206</v>
       </c>
       <c r="N23" s="1">
         <v>82864</v>
       </c>
       <c r="O23">
-        <f>IF(ISBLANK(P23),-N23,P23-N23)</f>
+        <f t="shared" si="5"/>
         <v>556</v>
       </c>
       <c r="P23" s="1">
         <v>83420</v>
       </c>
       <c r="Q23">
-        <f>IF(ISBLANK(R23),-P23,R23-P23)</f>
+        <f t="shared" si="6"/>
         <v>351</v>
       </c>
       <c r="R23" s="1">
@@ -7842,49 +8087,49 @@
         <v>3286</v>
       </c>
       <c r="E24">
-        <f>IF(ISBLANK(F24),-D24,F24-D24)</f>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="F24" s="1">
         <v>3307</v>
       </c>
       <c r="G24">
-        <f>IF(ISBLANK(H24),-F24,H24-F24)</f>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="H24" s="1">
         <v>3320</v>
       </c>
       <c r="I24">
-        <f>IF(ISBLANK(J24),-H24,J24-H24)</f>
+        <f t="shared" si="2"/>
         <v>232</v>
       </c>
       <c r="J24" s="1">
         <v>3552</v>
       </c>
       <c r="K24">
-        <f>IF(ISBLANK(L24),-J24,L24-J24)</f>
+        <f t="shared" si="3"/>
         <v>102</v>
       </c>
       <c r="L24" s="1">
         <v>3654</v>
       </c>
       <c r="M24">
-        <f>IF(ISBLANK(N24),-L24,N24-L24)</f>
+        <f t="shared" si="4"/>
         <v>60</v>
       </c>
       <c r="N24" s="1">
         <v>3714</v>
       </c>
       <c r="O24">
-        <f>IF(ISBLANK(P24),-N24,P24-N24)</f>
+        <f t="shared" si="5"/>
         <v>-3714</v>
       </c>
       <c r="P24" s="1">
         <v>0</v>
       </c>
       <c r="Q24">
-        <f>IF(ISBLANK(R24),-P24,R24-P24)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="R24" s="1">
@@ -7962,19 +8207,19 @@
         <v>148</v>
       </c>
       <c r="E27">
-        <f t="shared" ref="E27:E48" si="0">FIND(",",B27)</f>
+        <f t="shared" ref="E27:E48" si="7">FIND(",",B27)</f>
         <v>9</v>
       </c>
       <c r="F27" t="str">
-        <f t="shared" ref="F27:F48" si="1">LEFT(B27,E27-1)</f>
+        <f t="shared" ref="F27:F48" si="8">LEFT(B27,E27-1)</f>
         <v>Kelleher</v>
       </c>
       <c r="G27" t="str">
-        <f t="shared" ref="G27:G48" si="2">RIGHT(B27,LEN(B27)-(E27+1))</f>
+        <f t="shared" ref="G27:G48" si="9">RIGHT(B27,LEN(B27)-(E27+1))</f>
         <v>Billy</v>
       </c>
       <c r="H27" t="str">
-        <f t="shared" ref="H27:H48" si="3">G27&amp;" "&amp;F27</f>
+        <f t="shared" ref="H27:H48" si="10">G27&amp;" "&amp;F27</f>
         <v>Billy Kelleher</v>
       </c>
       <c r="J27" t="s">
@@ -8022,19 +8267,19 @@
         <v>149</v>
       </c>
       <c r="E28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="7"/>
         <v>8</v>
       </c>
       <c r="F28" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>Wallace</v>
       </c>
       <c r="G28" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>Mick</v>
       </c>
       <c r="H28" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>Mick Wallace</v>
       </c>
       <c r="J28" t="s">
@@ -8082,19 +8327,19 @@
         <v>150</v>
       </c>
       <c r="E29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="7"/>
         <v>9</v>
       </c>
       <c r="F29" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>Ní Riada</v>
       </c>
       <c r="G29" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>Liadh</v>
       </c>
       <c r="H29" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>Liadh Ní Riada</v>
       </c>
       <c r="J29" t="s">
@@ -8142,19 +8387,19 @@
         <v>151</v>
       </c>
       <c r="E30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="7"/>
         <v>11</v>
       </c>
       <c r="F30" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>O'Sullivan</v>
       </c>
       <c r="G30" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>Grace</v>
       </c>
       <c r="H30" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>Grace O'Sullivan</v>
       </c>
       <c r="J30" t="s">
@@ -8202,19 +8447,19 @@
         <v>152</v>
       </c>
       <c r="E31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="7"/>
         <v>6</v>
       </c>
       <c r="F31" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>Byrne</v>
       </c>
       <c r="G31" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>Malcolm</v>
       </c>
       <c r="H31" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>Malcolm Byrne</v>
       </c>
       <c r="J31" t="s">
@@ -8262,19 +8507,19 @@
         <v>153</v>
       </c>
       <c r="E32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="7"/>
         <v>6</v>
       </c>
       <c r="F32" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>Clune</v>
       </c>
       <c r="G32" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>Deirdre</v>
       </c>
       <c r="H32" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>Deirdre Clune</v>
       </c>
       <c r="J32" t="s">
@@ -8322,19 +8567,19 @@
         <v>154</v>
       </c>
       <c r="E33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="7"/>
         <v>6</v>
       </c>
       <c r="F33" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>Doyle</v>
       </c>
       <c r="G33" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>Andrew</v>
       </c>
       <c r="H33" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>Andrew Doyle</v>
       </c>
       <c r="J33" t="s">
@@ -8382,19 +8627,19 @@
         <v>155</v>
       </c>
       <c r="E34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="7"/>
         <v>6</v>
       </c>
       <c r="F34" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>Nunan</v>
       </c>
       <c r="G34" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>Sheila</v>
       </c>
       <c r="H34" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>Sheila Nunan</v>
       </c>
       <c r="J34" t="s">
@@ -8442,19 +8687,19 @@
         <v>156</v>
       </c>
       <c r="E35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="7"/>
         <v>8</v>
       </c>
       <c r="F35" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>Wallace</v>
       </c>
       <c r="G35" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>Adrienne</v>
       </c>
       <c r="H35" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>Adrienne Wallace</v>
       </c>
       <c r="J35" t="s">
@@ -8502,19 +8747,19 @@
         <v>157</v>
       </c>
       <c r="E36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="7"/>
         <v>7</v>
       </c>
       <c r="F36" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>Cahill</v>
       </c>
       <c r="G36" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>Dolores</v>
       </c>
       <c r="H36" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>Dolores Cahill</v>
       </c>
       <c r="J36" t="s">
@@ -8562,19 +8807,19 @@
         <v>158</v>
       </c>
       <c r="E37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="7"/>
         <v>8</v>
       </c>
       <c r="F37" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>O'Flynn</v>
       </c>
       <c r="G37" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>Diarmuid Patrick</v>
       </c>
       <c r="H37" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>Diarmuid Patrick O'Flynn</v>
       </c>
       <c r="J37" t="s">
@@ -8622,19 +8867,19 @@
         <v>159</v>
       </c>
       <c r="E38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="7"/>
         <v>8</v>
       </c>
       <c r="F38" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>Minehan</v>
       </c>
       <c r="G38" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>Liam</v>
       </c>
       <c r="H38" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>Liam Minehan</v>
       </c>
       <c r="J38" t="s">
@@ -8682,19 +8927,19 @@
         <v>160</v>
       </c>
       <c r="E39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="7"/>
         <v>8</v>
       </c>
       <c r="F39" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>Gardner</v>
       </c>
       <c r="G39" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>Breda Patricia</v>
       </c>
       <c r="H39" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>Breda Patricia Gardner</v>
       </c>
       <c r="J39" t="s">
@@ -8742,19 +8987,19 @@
         <v>161</v>
       </c>
       <c r="E40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="7"/>
         <v>7</v>
       </c>
       <c r="F40" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>Heaney</v>
       </c>
       <c r="G40" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>Theresa</v>
       </c>
       <c r="H40" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>Theresa Heaney</v>
       </c>
       <c r="J40" t="s">
@@ -8802,19 +9047,19 @@
         <v>162</v>
       </c>
       <c r="E41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="7"/>
         <v>8</v>
       </c>
       <c r="F41" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>Brennan</v>
       </c>
       <c r="G41" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>Allan</v>
       </c>
       <c r="H41" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>Allan Brennan</v>
       </c>
       <c r="J41" t="s">
@@ -8862,19 +9107,19 @@
         <v>163</v>
       </c>
       <c r="E42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="7"/>
         <v>11</v>
       </c>
       <c r="F42" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>O'Loughlin</v>
       </c>
       <c r="G42" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>Peter</v>
       </c>
       <c r="H42" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>Peter O'Loughlin</v>
       </c>
       <c r="J42" t="s">
@@ -8922,19 +9167,19 @@
         <v>164</v>
       </c>
       <c r="E43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="7"/>
         <v>12</v>
       </c>
       <c r="F43" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>Worthington</v>
       </c>
       <c r="G43" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>Colleen</v>
       </c>
       <c r="H43" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>Colleen Worthington</v>
       </c>
       <c r="J43" t="s">
@@ -8979,19 +9224,19 @@
         <v>165</v>
       </c>
       <c r="E44">
-        <f t="shared" si="0"/>
+        <f t="shared" si="7"/>
         <v>11</v>
       </c>
       <c r="F44" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>Fitzgerald</v>
       </c>
       <c r="G44" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>Paddy</v>
       </c>
       <c r="H44" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>Paddy Fitzgerald</v>
       </c>
       <c r="J44" t="s">
@@ -9033,19 +9278,19 @@
         <v>166</v>
       </c>
       <c r="E45">
-        <f t="shared" si="0"/>
+        <f t="shared" si="7"/>
         <v>13</v>
       </c>
       <c r="F45" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>Ryan-Purcell</v>
       </c>
       <c r="G45" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>Walter</v>
       </c>
       <c r="H45" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>Walter Ryan-Purcell</v>
       </c>
       <c r="J45" t="s">
@@ -9084,19 +9329,19 @@
         <v>167</v>
       </c>
       <c r="E46">
-        <f t="shared" si="0"/>
+        <f t="shared" si="7"/>
         <v>7</v>
       </c>
       <c r="F46" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>Sexton</v>
       </c>
       <c r="G46" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>Joesph</v>
       </c>
       <c r="H46" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>Joesph Sexton</v>
       </c>
       <c r="J46" t="s">
@@ -9129,19 +9374,19 @@
         <v>168</v>
       </c>
       <c r="E47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="7"/>
         <v>7</v>
       </c>
       <c r="F47" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>Madden</v>
       </c>
       <c r="G47" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>Peter</v>
       </c>
       <c r="H47" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>Peter Madden</v>
       </c>
       <c r="J47" t="s">
@@ -9168,19 +9413,19 @@
         <v>169</v>
       </c>
       <c r="E48">
-        <f t="shared" si="0"/>
+        <f t="shared" si="7"/>
         <v>11</v>
       </c>
       <c r="F48" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>Van de Ven</v>
       </c>
       <c r="G48" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>Jan</v>
       </c>
       <c r="H48" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>Jan Van de Ven</v>
       </c>
       <c r="J48" t="s">

</xml_diff>

<commit_message>
Count 9 south added Signed-off-by: Gerry Mulvenna <git@movingwifi.com>
</commit_message>
<xml_diff>
--- a/europarl/europarl-ireland-2019.xlsx
+++ b/europarl/europarl-ireland-2019.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="14220" windowHeight="8580" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="14220" windowHeight="8580" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Candidates" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="260">
   <si>
     <t>Candidate</t>
   </si>
@@ -5023,7 +5023,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView topLeftCell="G1" workbookViewId="0">
       <selection activeCell="M2" sqref="M2:N18"/>
     </sheetView>
   </sheetViews>
@@ -5064,35 +5064,35 @@
         <v>8130</v>
       </c>
       <c r="E2">
-        <f>IF(ISBLANK(F2),-D2,F2-D2)</f>
+        <f t="shared" ref="E2:E18" si="0">IF(ISBLANK(F2),-D2,F2-D2)</f>
         <v>96</v>
       </c>
       <c r="F2" s="1">
         <v>8226</v>
       </c>
       <c r="G2">
-        <f>IF(ISBLANK(H2),-F2,H2-F2)</f>
+        <f t="shared" ref="G2:G18" si="1">IF(ISBLANK(H2),-F2,H2-F2)</f>
         <v>20</v>
       </c>
       <c r="H2" s="1">
         <v>8246</v>
       </c>
       <c r="I2">
-        <f>IF(ISBLANK(J2),-H2,J2-H2)</f>
+        <f t="shared" ref="I2:I18" si="2">IF(ISBLANK(J2),-H2,J2-H2)</f>
         <v>91</v>
       </c>
       <c r="J2" s="1">
         <v>8337</v>
       </c>
       <c r="K2">
-        <f>IF(ISBLANK(L2),-J2,L2-J2)</f>
+        <f t="shared" ref="K2:K18" si="3">IF(ISBLANK(L2),-J2,L2-J2)</f>
         <v>28</v>
       </c>
       <c r="L2" s="1">
         <v>8365</v>
       </c>
       <c r="M2">
-        <f>IF(ISBLANK(N2),-L2,N2-L2)</f>
+        <f t="shared" ref="M2:M18" si="4">IF(ISBLANK(N2),-L2,N2-L2)</f>
         <v>188</v>
       </c>
       <c r="N2" s="1">
@@ -5111,35 +5111,35 @@
         <v>77619</v>
       </c>
       <c r="E3">
-        <f>IF(ISBLANK(F3),-D3,F3-D3)</f>
+        <f t="shared" si="0"/>
         <v>868</v>
       </c>
       <c r="F3" s="1">
         <v>78487</v>
       </c>
       <c r="G3">
-        <f>IF(ISBLANK(H3),-F3,H3-F3)</f>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="H3" s="1">
         <v>78513</v>
       </c>
       <c r="I3">
-        <f>IF(ISBLANK(J3),-H3,J3-H3)</f>
+        <f t="shared" si="2"/>
         <v>99</v>
       </c>
       <c r="J3" s="1">
         <v>78612</v>
       </c>
       <c r="K3">
-        <f>IF(ISBLANK(L3),-J3,L3-J3)</f>
+        <f t="shared" si="3"/>
         <v>41</v>
       </c>
       <c r="L3" s="1">
         <v>78653</v>
       </c>
       <c r="M3">
-        <f>IF(ISBLANK(N3),-L3,N3-L3)</f>
+        <f t="shared" si="4"/>
         <v>375</v>
       </c>
       <c r="N3" s="1">
@@ -5158,35 +5158,35 @@
         <v>56650</v>
       </c>
       <c r="E4">
-        <f>IF(ISBLANK(F4),-D4,F4-D4)</f>
+        <f t="shared" si="0"/>
         <v>1198</v>
       </c>
       <c r="F4" s="1">
         <v>57848</v>
       </c>
       <c r="G4">
-        <f>IF(ISBLANK(H4),-F4,H4-F4)</f>
+        <f t="shared" si="1"/>
         <v>44</v>
       </c>
       <c r="H4" s="1">
         <v>57892</v>
       </c>
       <c r="I4">
-        <f>IF(ISBLANK(J4),-H4,J4-H4)</f>
+        <f t="shared" si="2"/>
         <v>142</v>
       </c>
       <c r="J4" s="1">
         <v>58034</v>
       </c>
       <c r="K4">
-        <f>IF(ISBLANK(L4),-J4,L4-J4)</f>
+        <f t="shared" si="3"/>
         <v>178</v>
       </c>
       <c r="L4" s="1">
         <v>58212</v>
       </c>
       <c r="M4">
-        <f>IF(ISBLANK(N4),-L4,N4-L4)</f>
+        <f t="shared" si="4"/>
         <v>390</v>
       </c>
       <c r="N4" s="1">
@@ -5205,35 +5205,35 @@
         <v>15991</v>
       </c>
       <c r="E5">
-        <f>IF(ISBLANK(F5),-D5,F5-D5)</f>
+        <f t="shared" si="0"/>
         <v>477</v>
       </c>
       <c r="F5" s="1">
         <v>16468</v>
       </c>
       <c r="G5">
-        <f>IF(ISBLANK(H5),-F5,H5-F5)</f>
+        <f t="shared" si="1"/>
         <v>47</v>
       </c>
       <c r="H5" s="1">
         <v>16515</v>
       </c>
       <c r="I5">
-        <f>IF(ISBLANK(J5),-H5,J5-H5)</f>
+        <f t="shared" si="2"/>
         <v>106</v>
       </c>
       <c r="J5" s="1">
         <v>16621</v>
       </c>
       <c r="K5">
-        <f>IF(ISBLANK(L5),-J5,L5-J5)</f>
+        <f t="shared" si="3"/>
         <v>143</v>
       </c>
       <c r="L5" s="1">
         <v>16764</v>
       </c>
       <c r="M5">
-        <f>IF(ISBLANK(N5),-L5,N5-L5)</f>
+        <f t="shared" si="4"/>
         <v>826</v>
       </c>
       <c r="N5" s="1">
@@ -5252,35 +5252,35 @@
         <v>85034</v>
       </c>
       <c r="E6">
-        <f>IF(ISBLANK(F6),-D6,F6-D6)</f>
+        <f t="shared" si="0"/>
         <v>1872</v>
       </c>
       <c r="F6" s="1">
         <v>86906</v>
       </c>
       <c r="G6">
-        <f>IF(ISBLANK(H6),-F6,H6-F6)</f>
+        <f t="shared" si="1"/>
         <v>102</v>
       </c>
       <c r="H6" s="1">
         <v>87008</v>
       </c>
       <c r="I6">
-        <f>IF(ISBLANK(J6),-H6,J6-H6)</f>
+        <f t="shared" si="2"/>
         <v>180</v>
       </c>
       <c r="J6" s="1">
         <v>87188</v>
       </c>
       <c r="K6">
-        <f>IF(ISBLANK(L6),-J6,L6-J6)</f>
+        <f t="shared" si="3"/>
         <v>145</v>
       </c>
       <c r="L6" s="1">
         <v>87333</v>
       </c>
       <c r="M6">
-        <f>IF(ISBLANK(N6),-L6,N6-L6)</f>
+        <f t="shared" si="4"/>
         <v>631</v>
       </c>
       <c r="N6" s="1">
@@ -5299,35 +5299,35 @@
         <v>1352</v>
       </c>
       <c r="E7">
-        <f>IF(ISBLANK(F7),-D7,F7-D7)</f>
+        <f t="shared" si="0"/>
         <v>48</v>
       </c>
       <c r="F7" s="1">
         <v>1400</v>
       </c>
       <c r="G7">
-        <f>IF(ISBLANK(H7),-F7,H7-F7)</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="H7" s="1">
         <v>1412</v>
       </c>
       <c r="I7">
-        <f>IF(ISBLANK(J7),-H7,J7-H7)</f>
+        <f t="shared" si="2"/>
         <v>-1412</v>
       </c>
       <c r="J7" s="1">
         <v>0</v>
       </c>
       <c r="K7">
-        <f>IF(ISBLANK(L7),-J7,L7-J7)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L7" s="1">
         <v>0</v>
       </c>
       <c r="M7">
-        <f>IF(ISBLANK(N7),-L7,N7-L7)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N7" s="1">
@@ -5346,35 +5346,35 @@
         <v>12378</v>
       </c>
       <c r="E8">
-        <f>IF(ISBLANK(F8),-D8,F8-D8)</f>
+        <f t="shared" si="0"/>
         <v>653</v>
       </c>
       <c r="F8" s="1">
         <v>13031</v>
       </c>
       <c r="G8">
-        <f>IF(ISBLANK(H8),-F8,H8-F8)</f>
+        <f t="shared" si="1"/>
         <v>34</v>
       </c>
       <c r="H8" s="1">
         <v>13065</v>
       </c>
       <c r="I8">
-        <f>IF(ISBLANK(J8),-H8,J8-H8)</f>
+        <f t="shared" si="2"/>
         <v>85</v>
       </c>
       <c r="J8" s="1">
         <v>13150</v>
       </c>
       <c r="K8">
-        <f>IF(ISBLANK(L8),-J8,L8-J8)</f>
+        <f t="shared" si="3"/>
         <v>47</v>
       </c>
       <c r="L8" s="1">
         <v>13197</v>
       </c>
       <c r="M8">
-        <f>IF(ISBLANK(N8),-L8,N8-L8)</f>
+        <f t="shared" si="4"/>
         <v>211</v>
       </c>
       <c r="N8" s="1">
@@ -5393,35 +5393,35 @@
         <v>2450</v>
       </c>
       <c r="E9">
-        <f>IF(ISBLANK(F9),-D9,F9-D9)</f>
+        <f t="shared" si="0"/>
         <v>112</v>
       </c>
       <c r="F9" s="1">
         <v>2562</v>
       </c>
       <c r="G9">
-        <f>IF(ISBLANK(H9),-F9,H9-F9)</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="H9" s="1">
         <v>2577</v>
       </c>
       <c r="I9">
-        <f>IF(ISBLANK(J9),-H9,J9-H9)</f>
+        <f t="shared" si="2"/>
         <v>77</v>
       </c>
       <c r="J9" s="1">
         <v>2654</v>
       </c>
       <c r="K9">
-        <f>IF(ISBLANK(L9),-J9,L9-J9)</f>
+        <f t="shared" si="3"/>
         <v>40</v>
       </c>
       <c r="L9" s="1">
         <v>2694</v>
       </c>
       <c r="M9">
-        <f>IF(ISBLANK(N9),-L9,N9-L9)</f>
+        <f t="shared" si="4"/>
         <v>-2694</v>
       </c>
       <c r="N9" s="1">
@@ -5440,35 +5440,35 @@
         <v>134630</v>
       </c>
       <c r="E10">
-        <f>IF(ISBLANK(F10),-D10,F10-D10)</f>
+        <f t="shared" si="0"/>
         <v>-15644</v>
       </c>
       <c r="F10">
         <v>118986</v>
       </c>
       <c r="G10">
-        <f>IF(ISBLANK(H10),-F10,H10-F10)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H10">
         <v>118986</v>
       </c>
       <c r="I10">
-        <f>IF(ISBLANK(J10),-H10,J10-H10)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J10">
         <v>118986</v>
       </c>
       <c r="K10">
-        <f>IF(ISBLANK(L10),-J10,L10-J10)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L10">
         <v>118986</v>
       </c>
       <c r="M10">
-        <f>IF(ISBLANK(N10),-L10,N10-L10)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N10">
@@ -5487,35 +5487,35 @@
         <v>51019</v>
       </c>
       <c r="E11">
-        <f>IF(ISBLANK(F11),-D11,F11-D11)</f>
+        <f t="shared" si="0"/>
         <v>1712</v>
       </c>
       <c r="F11" s="1">
         <v>52731</v>
       </c>
       <c r="G11">
-        <f>IF(ISBLANK(H11),-F11,H11-F11)</f>
+        <f t="shared" si="1"/>
         <v>90</v>
       </c>
       <c r="H11" s="1">
         <v>52821</v>
       </c>
       <c r="I11">
-        <f>IF(ISBLANK(J11),-H11,J11-H11)</f>
+        <f t="shared" si="2"/>
         <v>155</v>
       </c>
       <c r="J11" s="1">
         <v>52976</v>
       </c>
       <c r="K11">
-        <f>IF(ISBLANK(L11),-J11,L11-J11)</f>
+        <f t="shared" si="3"/>
         <v>92</v>
       </c>
       <c r="L11" s="1">
         <v>53068</v>
       </c>
       <c r="M11">
-        <f>IF(ISBLANK(N11),-L11,N11-L11)</f>
+        <f t="shared" si="4"/>
         <v>898</v>
       </c>
       <c r="N11" s="1">
@@ -5534,35 +5534,35 @@
         <v>1322</v>
       </c>
       <c r="E12">
-        <f>IF(ISBLANK(F12),-D12,F12-D12)</f>
+        <f t="shared" si="0"/>
         <v>53</v>
       </c>
       <c r="F12" s="1">
         <v>1375</v>
       </c>
       <c r="G12">
-        <f>IF(ISBLANK(H12),-F12,H12-F12)</f>
+        <f t="shared" si="1"/>
         <v>71</v>
       </c>
       <c r="H12" s="1">
         <v>1446</v>
       </c>
       <c r="I12">
-        <f>IF(ISBLANK(J12),-H12,J12-H12)</f>
+        <f t="shared" si="2"/>
         <v>44</v>
       </c>
       <c r="J12" s="1">
         <v>1490</v>
       </c>
       <c r="K12">
-        <f>IF(ISBLANK(L12),-J12,L12-J12)</f>
+        <f t="shared" si="3"/>
         <v>-1490</v>
       </c>
       <c r="L12" s="1">
         <v>0</v>
       </c>
       <c r="M12">
-        <f>IF(ISBLANK(N12),-L12,N12-L12)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N12" s="1">
@@ -5581,35 +5581,35 @@
         <v>789</v>
       </c>
       <c r="E13">
-        <f>IF(ISBLANK(F13),-D13,F13-D13)</f>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="F13">
         <v>811</v>
       </c>
       <c r="G13">
-        <f>IF(ISBLANK(H13),-F13,H13-F13)</f>
+        <f t="shared" si="1"/>
         <v>-811</v>
       </c>
       <c r="H13" s="1">
         <v>0</v>
       </c>
       <c r="I13">
-        <f>IF(ISBLANK(J13),-H13,J13-H13)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J13" s="1">
         <v>0</v>
       </c>
       <c r="K13">
-        <f>IF(ISBLANK(L13),-J13,L13-J13)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L13" s="1">
         <v>0</v>
       </c>
       <c r="M13">
-        <f>IF(ISBLANK(N13),-L13,N13-L13)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N13" s="1">
@@ -5628,35 +5628,35 @@
         <v>3132</v>
       </c>
       <c r="E14">
-        <f>IF(ISBLANK(F14),-D14,F14-D14)</f>
+        <f t="shared" si="0"/>
         <v>104</v>
       </c>
       <c r="F14" s="1">
         <v>3236</v>
       </c>
       <c r="G14">
-        <f>IF(ISBLANK(H14),-F14,H14-F14)</f>
+        <f t="shared" si="1"/>
         <v>77</v>
       </c>
       <c r="H14" s="1">
         <v>3313</v>
       </c>
       <c r="I14">
-        <f>IF(ISBLANK(J14),-H14,J14-H14)</f>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="J14" s="1">
         <v>3326</v>
       </c>
       <c r="K14">
-        <f>IF(ISBLANK(L14),-J14,L14-J14)</f>
+        <f t="shared" si="3"/>
         <v>151</v>
       </c>
       <c r="L14" s="1">
         <v>3477</v>
       </c>
       <c r="M14">
-        <f>IF(ISBLANK(N14),-L14,N14-L14)</f>
+        <f t="shared" si="4"/>
         <v>-3477</v>
       </c>
       <c r="N14" s="1">
@@ -5675,35 +5675,35 @@
         <v>6897</v>
       </c>
       <c r="E15">
-        <f>IF(ISBLANK(F15),-D15,F15-D15)</f>
+        <f t="shared" si="0"/>
         <v>303</v>
       </c>
       <c r="F15" s="1">
         <v>7200</v>
       </c>
       <c r="G15">
-        <f>IF(ISBLANK(H15),-F15,H15-F15)</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="H15" s="1">
         <v>7220</v>
       </c>
       <c r="I15">
-        <f>IF(ISBLANK(J15),-H15,J15-H15)</f>
+        <f t="shared" si="2"/>
         <v>84</v>
       </c>
       <c r="J15" s="1">
         <v>7304</v>
       </c>
       <c r="K15">
-        <f>IF(ISBLANK(L15),-J15,L15-J15)</f>
+        <f t="shared" si="3"/>
         <v>141</v>
       </c>
       <c r="L15" s="1">
         <v>7445</v>
       </c>
       <c r="M15">
-        <f>IF(ISBLANK(N15),-L15,N15-L15)</f>
+        <f t="shared" si="4"/>
         <v>232</v>
       </c>
       <c r="N15" s="1">
@@ -5722,35 +5722,35 @@
         <v>30220</v>
       </c>
       <c r="E16">
-        <f>IF(ISBLANK(F16),-D16,F16-D16)</f>
+        <f t="shared" si="0"/>
         <v>864</v>
       </c>
       <c r="F16" s="1">
         <v>31084</v>
       </c>
       <c r="G16">
-        <f>IF(ISBLANK(H16),-F16,H16-F16)</f>
+        <f t="shared" si="1"/>
         <v>38</v>
       </c>
       <c r="H16" s="1">
         <v>31122</v>
       </c>
       <c r="I16">
-        <f>IF(ISBLANK(J16),-H16,J16-H16)</f>
+        <f t="shared" si="2"/>
         <v>21</v>
       </c>
       <c r="J16" s="1">
         <v>31143</v>
       </c>
       <c r="K16">
-        <f>IF(ISBLANK(L16),-J16,L16-J16)</f>
+        <f t="shared" si="3"/>
         <v>55</v>
       </c>
       <c r="L16" s="1">
         <v>31198</v>
       </c>
       <c r="M16">
-        <f>IF(ISBLANK(N16),-L16,N16-L16)</f>
+        <f t="shared" si="4"/>
         <v>273</v>
       </c>
       <c r="N16" s="1">
@@ -5769,35 +5769,35 @@
         <v>42814</v>
       </c>
       <c r="E17">
-        <f>IF(ISBLANK(F17),-D17,F17-D17)</f>
+        <f t="shared" si="0"/>
         <v>1226</v>
       </c>
       <c r="F17" s="1">
         <v>44040</v>
       </c>
       <c r="G17">
-        <f>IF(ISBLANK(H17),-F17,H17-F17)</f>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="H17" s="1">
         <v>44059</v>
       </c>
       <c r="I17">
-        <f>IF(ISBLANK(J17),-H17,J17-H17)</f>
+        <f t="shared" si="2"/>
         <v>17</v>
       </c>
       <c r="J17" s="1">
         <v>44076</v>
       </c>
       <c r="K17">
-        <f>IF(ISBLANK(L17),-J17,L17-J17)</f>
+        <f t="shared" si="3"/>
         <v>54</v>
       </c>
       <c r="L17" s="1">
         <v>44130</v>
       </c>
       <c r="M17">
-        <f>IF(ISBLANK(N17),-L17,N17-L17)</f>
+        <f t="shared" si="4"/>
         <v>125</v>
       </c>
       <c r="N17" s="1">
@@ -5816,35 +5816,35 @@
         <v>64500</v>
       </c>
       <c r="E18">
-        <f>IF(ISBLANK(F18),-D18,F18-D18)</f>
+        <f t="shared" si="0"/>
         <v>6036</v>
       </c>
       <c r="F18" s="1">
         <v>70536</v>
       </c>
       <c r="G18">
-        <f>IF(ISBLANK(H18),-F18,H18-F18)</f>
+        <f t="shared" si="1"/>
         <v>83</v>
       </c>
       <c r="H18" s="1">
         <v>70619</v>
       </c>
       <c r="I18">
-        <f>IF(ISBLANK(J18),-H18,J18-H18)</f>
+        <f t="shared" si="2"/>
         <v>41</v>
       </c>
       <c r="J18" s="1">
         <v>70660</v>
       </c>
       <c r="K18">
-        <f>IF(ISBLANK(L18),-J18,L18-J18)</f>
+        <f t="shared" si="3"/>
         <v>71</v>
       </c>
       <c r="L18" s="1">
         <v>70731</v>
       </c>
       <c r="M18">
-        <f>IF(ISBLANK(N18),-L18,N18-L18)</f>
+        <f t="shared" si="4"/>
         <v>694</v>
       </c>
       <c r="N18" s="1">
@@ -5901,19 +5901,19 @@
         <v>197</v>
       </c>
       <c r="D21">
-        <f t="shared" ref="D21:D36" si="0">FIND(",",B21)</f>
+        <f t="shared" ref="D21:D36" si="5">FIND(",",B21)</f>
         <v>9</v>
       </c>
       <c r="E21" t="str">
-        <f t="shared" ref="E21:E36" si="1">LEFT(B21,D21-1)</f>
+        <f t="shared" ref="E21:E36" si="6">LEFT(B21,D21-1)</f>
         <v>Flanagan</v>
       </c>
       <c r="F21" t="str">
-        <f t="shared" ref="F21:F36" si="2">RIGHT(B21,LEN(B21)-(D21+1))</f>
+        <f t="shared" ref="F21:F36" si="7">RIGHT(B21,LEN(B21)-(D21+1))</f>
         <v>Luke 'Ming'</v>
       </c>
       <c r="G21" t="str">
-        <f t="shared" ref="G21:G36" si="3">F21&amp;" "&amp;E21</f>
+        <f t="shared" ref="G21:G36" si="8">F21&amp;" "&amp;E21</f>
         <v>Luke 'Ming' Flanagan</v>
       </c>
       <c r="J21" t="s">
@@ -5933,19 +5933,19 @@
         <v>198</v>
       </c>
       <c r="D22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
       <c r="E22" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>Carthy</v>
       </c>
       <c r="F22" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>Matt</v>
       </c>
       <c r="G22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>Matt Carthy</v>
       </c>
       <c r="J22" t="s">
@@ -5984,19 +5984,19 @@
         <v>199</v>
       </c>
       <c r="D23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="E23" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>Walsh</v>
       </c>
       <c r="F23" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>Maria</v>
       </c>
       <c r="G23" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>Maria Walsh</v>
       </c>
       <c r="J23" t="s">
@@ -6035,19 +6035,19 @@
         <v>200</v>
       </c>
       <c r="D24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="E24" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>Casey</v>
       </c>
       <c r="F24" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>Peter</v>
       </c>
       <c r="G24" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>Peter Casey</v>
       </c>
       <c r="J24" t="s">
@@ -6086,19 +6086,19 @@
         <v>201</v>
       </c>
       <c r="D25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
       <c r="E25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>McHugh</v>
       </c>
       <c r="F25" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>Saoirse</v>
       </c>
       <c r="G25" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>Saoirse McHugh</v>
       </c>
       <c r="J25" t="s">
@@ -6137,19 +6137,19 @@
         <v>202</v>
       </c>
       <c r="D26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="E26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>Smith</v>
       </c>
       <c r="F26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>Brendan</v>
       </c>
       <c r="G26" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>Brendan Smith</v>
       </c>
       <c r="J26" t="s">
@@ -6188,19 +6188,19 @@
         <v>203</v>
       </c>
       <c r="D27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>9</v>
       </c>
       <c r="E27" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>Rabbitte</v>
       </c>
       <c r="F27" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>Anne</v>
       </c>
       <c r="G27" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>Anne Rabbitte</v>
       </c>
       <c r="J27" t="s">
@@ -6239,19 +6239,19 @@
         <v>204</v>
       </c>
       <c r="D28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>12</v>
       </c>
       <c r="E28" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>Healy Eames</v>
       </c>
       <c r="F28" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>Fidelma</v>
       </c>
       <c r="G28" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>Fidelma Healy Eames</v>
       </c>
       <c r="J28" t="s">
@@ -6290,19 +6290,19 @@
         <v>205</v>
       </c>
       <c r="D29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>9</v>
       </c>
       <c r="E29" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>Hannigan</v>
       </c>
       <c r="F29" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>Dominic</v>
       </c>
       <c r="G29" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>Dominic Hannigan</v>
       </c>
       <c r="J29" t="s">
@@ -6341,19 +6341,19 @@
         <v>206</v>
       </c>
       <c r="D30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="E30" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>Brennan</v>
       </c>
       <c r="F30" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>Cyril</v>
       </c>
       <c r="G30" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>Cyril Brennan</v>
       </c>
       <c r="J30" t="s">
@@ -6392,19 +6392,19 @@
         <v>207</v>
       </c>
       <c r="D31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
       <c r="E31" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>O'Dowd</v>
       </c>
       <c r="F31" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>Michael</v>
       </c>
       <c r="G31" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>Michael O'Dowd</v>
       </c>
       <c r="J31" t="s">
@@ -6443,19 +6443,19 @@
         <v>208</v>
       </c>
       <c r="D32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>9</v>
       </c>
       <c r="E32" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>O'Connor</v>
       </c>
       <c r="F32" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>Olive</v>
       </c>
       <c r="G32" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>Olive O'Connor</v>
       </c>
       <c r="J32" t="s">
@@ -6494,19 +6494,19 @@
         <v>209</v>
       </c>
       <c r="D33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="E33" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>Mahapatra</v>
       </c>
       <c r="F33" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>Dilip</v>
       </c>
       <c r="G33" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>Dilip Mahapatra</v>
       </c>
       <c r="J33" t="s">
@@ -6542,19 +6542,19 @@
         <v>210</v>
       </c>
       <c r="D34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
       <c r="E34" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>Greene</v>
       </c>
       <c r="F34" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>Patrick</v>
       </c>
       <c r="G34" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>Patrick Greene</v>
       </c>
       <c r="J34" t="s">
@@ -6590,19 +6590,19 @@
         <v>211</v>
       </c>
       <c r="D35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
       <c r="E35" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>Miller</v>
       </c>
       <c r="F35" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>James</v>
       </c>
       <c r="G35" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>James Miller</v>
       </c>
       <c r="J35" t="s">
@@ -6630,19 +6630,19 @@
         <v>212</v>
       </c>
       <c r="D36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="E36" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>Mulcahy</v>
       </c>
       <c r="F36" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>Diarmaid</v>
       </c>
       <c r="G36" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>Diarmaid Mulcahy</v>
       </c>
       <c r="J36" t="s">
@@ -6696,8 +6696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD49"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2:R24"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="S2" sqref="S2:T24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6767,53 +6767,60 @@
         <v>4665</v>
       </c>
       <c r="E2">
-        <f t="shared" ref="E2:E24" si="0">IF(ISBLANK(F2),-D2,F2-D2)</f>
+        <f>IF(ISBLANK(F2),-D2,F2-D2)</f>
         <v>26</v>
       </c>
       <c r="F2" s="1">
         <v>4691</v>
       </c>
       <c r="G2">
-        <f t="shared" ref="G2:G24" si="1">IF(ISBLANK(H2),-F2,H2-F2)</f>
+        <f>IF(ISBLANK(H2),-F2,H2-F2)</f>
         <v>43</v>
       </c>
       <c r="H2" s="1">
         <v>4734</v>
       </c>
       <c r="I2">
-        <f t="shared" ref="I2:I24" si="2">IF(ISBLANK(J2),-H2,J2-H2)</f>
+        <f>IF(ISBLANK(J2),-H2,J2-H2)</f>
         <v>57</v>
       </c>
       <c r="J2" s="1">
         <v>4791</v>
       </c>
       <c r="K2">
-        <f t="shared" ref="K2:K24" si="3">IF(ISBLANK(L2),-J2,L2-J2)</f>
+        <f>IF(ISBLANK(L2),-J2,L2-J2)</f>
         <v>50</v>
       </c>
       <c r="L2" s="1">
         <v>4841</v>
       </c>
       <c r="M2">
-        <f t="shared" ref="M2:M24" si="4">IF(ISBLANK(N2),-L2,N2-L2)</f>
+        <f>IF(ISBLANK(N2),-L2,N2-L2)</f>
         <v>115</v>
       </c>
       <c r="N2" s="1">
         <v>4956</v>
       </c>
       <c r="O2">
-        <f t="shared" ref="O2:O24" si="5">IF(ISBLANK(P2),-N2,P2-N2)</f>
+        <f>IF(ISBLANK(P2),-N2,P2-N2)</f>
         <v>72</v>
       </c>
       <c r="P2" s="1">
         <v>5028</v>
       </c>
       <c r="Q2">
-        <f t="shared" ref="Q2:Q24" si="6">IF(ISBLANK(R2),-P2,R2-P2)</f>
+        <f>IF(ISBLANK(R2),-P2,R2-P2)</f>
         <v>104</v>
       </c>
       <c r="R2" s="1">
         <v>5132</v>
+      </c>
+      <c r="S2">
+        <f>IF(ISBLANK(T2),-R2,T2-R2)</f>
+        <v>-5132</v>
+      </c>
+      <c r="T2" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.25">
@@ -6827,53 +6834,60 @@
         <v>69166</v>
       </c>
       <c r="E3">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F3),-D3,F3-D3)</f>
         <v>35</v>
       </c>
       <c r="F3" s="1">
         <v>69201</v>
       </c>
       <c r="G3">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H3),-F3,H3-F3)</f>
         <v>71</v>
       </c>
       <c r="H3" s="1">
         <v>69272</v>
       </c>
       <c r="I3">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J3),-H3,J3-H3)</f>
         <v>44</v>
       </c>
       <c r="J3" s="1">
         <v>69316</v>
       </c>
       <c r="K3">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L3),-J3,L3-J3)</f>
         <v>66</v>
       </c>
       <c r="L3" s="1">
         <v>69382</v>
       </c>
       <c r="M3">
-        <f t="shared" si="4"/>
+        <f>IF(ISBLANK(N3),-L3,N3-L3)</f>
         <v>129</v>
       </c>
       <c r="N3" s="1">
         <v>69511</v>
       </c>
       <c r="O3">
-        <f t="shared" si="5"/>
+        <f>IF(ISBLANK(P3),-N3,P3-N3)</f>
         <v>45</v>
       </c>
       <c r="P3" s="1">
         <v>69556</v>
       </c>
       <c r="Q3">
-        <f t="shared" si="6"/>
+        <f>IF(ISBLANK(R3),-P3,R3-P3)</f>
         <v>116</v>
       </c>
       <c r="R3" s="1">
         <v>69672</v>
+      </c>
+      <c r="S3">
+        <f>IF(ISBLANK(T3),-R3,T3-R3)</f>
+        <v>1226</v>
+      </c>
+      <c r="T3" s="1">
+        <v>70898</v>
       </c>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.25">
@@ -6887,53 +6901,60 @@
         <v>10582</v>
       </c>
       <c r="E4">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F4),-D4,F4-D4)</f>
         <v>57</v>
       </c>
       <c r="F4" s="1">
         <v>10639</v>
       </c>
       <c r="G4">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H4),-F4,H4-F4)</f>
         <v>106</v>
       </c>
       <c r="H4" s="1">
         <v>10745</v>
       </c>
       <c r="I4">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J4),-H4,J4-H4)</f>
         <v>138</v>
       </c>
       <c r="J4" s="1">
         <v>10883</v>
       </c>
       <c r="K4">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L4),-J4,L4-J4)</f>
         <v>54</v>
       </c>
       <c r="L4" s="1">
         <v>10937</v>
       </c>
       <c r="M4">
-        <f t="shared" si="4"/>
+        <f>IF(ISBLANK(N4),-L4,N4-L4)</f>
         <v>300</v>
       </c>
       <c r="N4" s="1">
         <v>11237</v>
       </c>
       <c r="O4">
-        <f t="shared" si="5"/>
+        <f>IF(ISBLANK(P4),-N4,P4-N4)</f>
         <v>159</v>
       </c>
       <c r="P4" s="1">
         <v>11396</v>
       </c>
       <c r="Q4">
-        <f t="shared" si="6"/>
+        <f>IF(ISBLANK(R4),-P4,R4-P4)</f>
         <v>322</v>
       </c>
       <c r="R4" s="1">
         <v>11718</v>
+      </c>
+      <c r="S4">
+        <f>IF(ISBLANK(T4),-R4,T4-R4)</f>
+        <v>908</v>
+      </c>
+      <c r="T4" s="1">
+        <v>12626</v>
       </c>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.25">
@@ -6947,53 +6968,60 @@
         <v>64605</v>
       </c>
       <c r="E5">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F5),-D5,F5-D5)</f>
         <v>26</v>
       </c>
       <c r="F5" s="1">
         <v>64631</v>
       </c>
       <c r="G5">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H5),-F5,H5-F5)</f>
         <v>61</v>
       </c>
       <c r="H5" s="1">
         <v>64692</v>
       </c>
       <c r="I5">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J5),-H5,J5-H5)</f>
         <v>71</v>
       </c>
       <c r="J5" s="1">
         <v>64763</v>
       </c>
       <c r="K5">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L5),-J5,L5-J5)</f>
         <v>136</v>
       </c>
       <c r="L5" s="1">
         <v>64899</v>
       </c>
       <c r="M5">
-        <f t="shared" si="4"/>
+        <f>IF(ISBLANK(N5),-L5,N5-L5)</f>
         <v>106</v>
       </c>
       <c r="N5" s="1">
         <v>65005</v>
       </c>
       <c r="O5">
-        <f t="shared" si="5"/>
+        <f>IF(ISBLANK(P5),-N5,P5-N5)</f>
         <v>110</v>
       </c>
       <c r="P5" s="1">
         <v>65115</v>
       </c>
       <c r="Q5">
-        <f t="shared" si="6"/>
+        <f>IF(ISBLANK(R5),-P5,R5-P5)</f>
         <v>137</v>
       </c>
       <c r="R5" s="1">
         <v>65252</v>
+      </c>
+      <c r="S5">
+        <f>IF(ISBLANK(T5),-R5,T5-R5)</f>
+        <v>306</v>
+      </c>
+      <c r="T5" s="1">
+        <v>65558</v>
       </c>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.25">
@@ -7007,53 +7035,60 @@
         <v>38738</v>
       </c>
       <c r="E6">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F6),-D6,F6-D6)</f>
         <v>17</v>
       </c>
       <c r="F6" s="1">
         <v>38755</v>
       </c>
       <c r="G6">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H6),-F6,H6-F6)</f>
         <v>33</v>
       </c>
       <c r="H6" s="1">
         <v>38788</v>
       </c>
       <c r="I6">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J6),-H6,J6-H6)</f>
         <v>16</v>
       </c>
       <c r="J6" s="1">
         <v>38804</v>
       </c>
       <c r="K6">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L6),-J6,L6-J6)</f>
         <v>38</v>
       </c>
       <c r="L6" s="1">
         <v>38842</v>
       </c>
       <c r="M6">
-        <f t="shared" si="4"/>
+        <f>IF(ISBLANK(N6),-L6,N6-L6)</f>
         <v>84</v>
       </c>
       <c r="N6" s="1">
         <v>38926</v>
       </c>
       <c r="O6">
-        <f t="shared" si="5"/>
+        <f>IF(ISBLANK(P6),-N6,P6-N6)</f>
         <v>24</v>
       </c>
       <c r="P6" s="1">
         <v>38950</v>
       </c>
       <c r="Q6">
-        <f t="shared" si="6"/>
+        <f>IF(ISBLANK(R6),-P6,R6-P6)</f>
         <v>46</v>
       </c>
       <c r="R6" s="1">
         <v>38996</v>
+      </c>
+      <c r="S6">
+        <f>IF(ISBLANK(T6),-R6,T6-R6)</f>
+        <v>298</v>
+      </c>
+      <c r="T6" s="1">
+        <v>39294</v>
       </c>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.25">
@@ -7067,52 +7102,59 @@
         <v>3182</v>
       </c>
       <c r="E7">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F7),-D7,F7-D7)</f>
         <v>15</v>
       </c>
       <c r="F7" s="1">
         <v>3197</v>
       </c>
       <c r="G7">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H7),-F7,H7-F7)</f>
         <v>60</v>
       </c>
       <c r="H7" s="1">
         <v>3257</v>
       </c>
       <c r="I7">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J7),-H7,J7-H7)</f>
         <v>43</v>
       </c>
       <c r="J7" s="1">
         <v>3300</v>
       </c>
       <c r="K7">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L7),-J7,L7-J7)</f>
         <v>32</v>
       </c>
       <c r="L7" s="1">
         <v>3332</v>
       </c>
       <c r="M7">
-        <f t="shared" si="4"/>
+        <f>IF(ISBLANK(N7),-L7,N7-L7)</f>
         <v>-3332</v>
       </c>
       <c r="N7" s="1">
         <v>0</v>
       </c>
       <c r="O7">
-        <f t="shared" si="5"/>
+        <f>IF(ISBLANK(P7),-N7,P7-N7)</f>
         <v>0</v>
       </c>
       <c r="P7" s="1">
         <v>0</v>
       </c>
       <c r="Q7">
-        <f t="shared" si="6"/>
+        <f>IF(ISBLANK(R7),-P7,R7-P7)</f>
         <v>0</v>
       </c>
       <c r="R7" s="1">
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <f>IF(ISBLANK(T7),-R7,T7-R7)</f>
+        <v>0</v>
+      </c>
+      <c r="T7" s="1">
         <v>0</v>
       </c>
     </row>
@@ -7127,53 +7169,60 @@
         <v>9306</v>
       </c>
       <c r="E8">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F8),-D8,F8-D8)</f>
         <v>25</v>
       </c>
       <c r="F8" s="1">
         <v>9331</v>
       </c>
       <c r="G8">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H8),-F8,H8-F8)</f>
         <v>70</v>
       </c>
       <c r="H8" s="1">
         <v>9401</v>
       </c>
       <c r="I8">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J8),-H8,J8-H8)</f>
         <v>35</v>
       </c>
       <c r="J8" s="1">
         <v>9436</v>
       </c>
       <c r="K8">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L8),-J8,L8-J8)</f>
         <v>60</v>
       </c>
       <c r="L8" s="1">
         <v>9496</v>
       </c>
       <c r="M8">
-        <f t="shared" si="4"/>
+        <f>IF(ISBLANK(N8),-L8,N8-L8)</f>
         <v>228</v>
       </c>
       <c r="N8" s="1">
         <v>9724</v>
       </c>
       <c r="O8">
-        <f t="shared" si="5"/>
+        <f>IF(ISBLANK(P8),-N8,P8-N8)</f>
         <v>145</v>
       </c>
       <c r="P8" s="1">
         <v>9869</v>
       </c>
       <c r="Q8">
-        <f t="shared" si="6"/>
+        <f>IF(ISBLANK(R8),-P8,R8-P8)</f>
         <v>106</v>
       </c>
       <c r="R8" s="1">
         <v>9975</v>
+      </c>
+      <c r="S8">
+        <f>IF(ISBLANK(T8),-R8,T8-R8)</f>
+        <v>247</v>
+      </c>
+      <c r="T8" s="1">
+        <v>10222</v>
       </c>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.25">
@@ -7187,53 +7236,60 @@
         <v>7475</v>
       </c>
       <c r="E9">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F9),-D9,F9-D9)</f>
         <v>23</v>
       </c>
       <c r="F9" s="1">
         <v>7498</v>
       </c>
       <c r="G9">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H9),-F9,H9-F9)</f>
         <v>98</v>
       </c>
       <c r="H9" s="1">
         <v>7596</v>
       </c>
       <c r="I9">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J9),-H9,J9-H9)</f>
         <v>142</v>
       </c>
       <c r="J9" s="1">
         <v>7738</v>
       </c>
       <c r="K9">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L9),-J9,L9-J9)</f>
         <v>70</v>
       </c>
       <c r="L9" s="1">
         <v>7808</v>
       </c>
       <c r="M9">
-        <f t="shared" si="4"/>
+        <f>IF(ISBLANK(N9),-L9,N9-L9)</f>
         <v>197</v>
       </c>
       <c r="N9" s="1">
         <v>8005</v>
       </c>
       <c r="O9">
-        <f t="shared" si="5"/>
+        <f>IF(ISBLANK(P9),-N9,P9-N9)</f>
         <v>192</v>
       </c>
       <c r="P9" s="1">
         <v>8197</v>
       </c>
       <c r="Q9">
-        <f t="shared" si="6"/>
+        <f>IF(ISBLANK(R9),-P9,R9-P9)</f>
         <v>176</v>
       </c>
       <c r="R9" s="1">
         <v>8373</v>
+      </c>
+      <c r="S9">
+        <f>IF(ISBLANK(T9),-R9,T9-R9)</f>
+        <v>188</v>
+      </c>
+      <c r="T9" s="1">
+        <v>8561</v>
       </c>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.25">
@@ -7247,53 +7303,60 @@
         <v>84083</v>
       </c>
       <c r="E10">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F10),-D10,F10-D10)</f>
         <v>23</v>
       </c>
       <c r="F10" s="1">
         <v>84106</v>
       </c>
       <c r="G10">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H10),-F10,H10-F10)</f>
         <v>58</v>
       </c>
       <c r="H10" s="1">
         <v>84164</v>
       </c>
       <c r="I10">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J10),-H10,J10-H10)</f>
         <v>74</v>
       </c>
       <c r="J10" s="1">
         <v>84238</v>
       </c>
       <c r="K10">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L10),-J10,L10-J10)</f>
         <v>150</v>
       </c>
       <c r="L10" s="1">
         <v>84388</v>
       </c>
       <c r="M10">
-        <f t="shared" si="4"/>
+        <f>IF(ISBLANK(N10),-L10,N10-L10)</f>
         <v>171</v>
       </c>
       <c r="N10" s="1">
         <v>84559</v>
       </c>
       <c r="O10">
-        <f t="shared" si="5"/>
+        <f>IF(ISBLANK(P10),-N10,P10-N10)</f>
         <v>95</v>
       </c>
       <c r="P10" s="1">
         <v>84654</v>
       </c>
       <c r="Q10">
-        <f t="shared" si="6"/>
+        <f>IF(ISBLANK(R10),-P10,R10-P10)</f>
         <v>187</v>
       </c>
       <c r="R10" s="1">
         <v>84841</v>
+      </c>
+      <c r="S10">
+        <f>IF(ISBLANK(T10),-R10,T10-R10)</f>
+        <v>130</v>
+      </c>
+      <c r="T10" s="1">
+        <v>84971</v>
       </c>
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.25">
@@ -7307,53 +7370,60 @@
         <v>118444</v>
       </c>
       <c r="E11">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F11),-D11,F11-D11)</f>
         <v>45</v>
       </c>
       <c r="F11" s="1">
         <v>118489</v>
       </c>
       <c r="G11">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H11),-F11,H11-F11)</f>
         <v>186</v>
       </c>
       <c r="H11" s="1">
         <v>118675</v>
       </c>
       <c r="I11">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J11),-H11,J11-H11)</f>
         <v>98</v>
       </c>
       <c r="J11" s="1">
         <v>118773</v>
       </c>
       <c r="K11">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L11),-J11,L11-J11)</f>
         <v>350</v>
       </c>
       <c r="L11" s="1">
         <v>119123</v>
       </c>
       <c r="M11">
-        <f t="shared" si="4"/>
+        <f>IF(ISBLANK(N11),-L11,N11-L11)</f>
         <v>257</v>
       </c>
       <c r="N11" s="1">
         <v>119380</v>
       </c>
       <c r="O11">
-        <f t="shared" si="5"/>
+        <f>IF(ISBLANK(P11),-N11,P11-N11)</f>
         <v>165</v>
       </c>
       <c r="P11" s="1">
         <v>119545</v>
       </c>
       <c r="Q11">
-        <f t="shared" si="6"/>
+        <f>IF(ISBLANK(R11),-P11,R11-P11)</f>
         <v>170</v>
       </c>
       <c r="R11" s="1">
         <v>119715</v>
+      </c>
+      <c r="S11">
+        <f>IF(ISBLANK(T11),-R11,T11-R11)</f>
+        <v>168</v>
+      </c>
+      <c r="T11" s="1">
+        <v>119883</v>
       </c>
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.25">
@@ -7367,52 +7437,59 @@
         <v>2395</v>
       </c>
       <c r="E12">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F12),-D12,F12-D12)</f>
         <v>14</v>
       </c>
       <c r="F12" s="1">
         <v>2409</v>
       </c>
       <c r="G12">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H12),-F12,H12-F12)</f>
         <v>-2409</v>
       </c>
       <c r="H12" s="1">
         <v>0</v>
       </c>
       <c r="I12">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J12),-H12,J12-H12)</f>
         <v>0</v>
       </c>
       <c r="J12" s="1">
         <v>0</v>
       </c>
       <c r="K12">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L12),-J12,L12-J12)</f>
         <v>0</v>
       </c>
       <c r="L12" s="1">
         <v>0</v>
       </c>
       <c r="M12">
-        <f t="shared" si="4"/>
+        <f>IF(ISBLANK(N12),-L12,N12-L12)</f>
         <v>0</v>
       </c>
       <c r="N12" s="1">
         <v>0</v>
       </c>
       <c r="O12">
-        <f t="shared" si="5"/>
+        <f>IF(ISBLANK(P12),-N12,P12-N12)</f>
         <v>0</v>
       </c>
       <c r="P12" s="1">
         <v>0</v>
       </c>
       <c r="Q12">
-        <f t="shared" si="6"/>
+        <f>IF(ISBLANK(R12),-P12,R12-P12)</f>
         <v>0</v>
       </c>
       <c r="R12" s="1">
+        <v>0</v>
+      </c>
+      <c r="S12">
+        <f>IF(ISBLANK(T12),-R12,T12-R12)</f>
+        <v>0</v>
+      </c>
+      <c r="T12" s="1">
         <v>0</v>
       </c>
     </row>
@@ -7427,53 +7504,60 @@
         <v>9423</v>
       </c>
       <c r="E13">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F13),-D13,F13-D13)</f>
         <v>32</v>
       </c>
       <c r="F13" s="1">
         <v>9455</v>
       </c>
       <c r="G13">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H13),-F13,H13-F13)</f>
         <v>325</v>
       </c>
       <c r="H13" s="1">
         <v>9780</v>
       </c>
       <c r="I13">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J13),-H13,J13-H13)</f>
         <v>75</v>
       </c>
       <c r="J13" s="1">
         <v>9855</v>
       </c>
       <c r="K13">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L13),-J13,L13-J13)</f>
         <v>114</v>
       </c>
       <c r="L13" s="1">
         <v>9969</v>
       </c>
       <c r="M13">
-        <f t="shared" si="4"/>
+        <f>IF(ISBLANK(N13),-L13,N13-L13)</f>
         <v>280</v>
       </c>
       <c r="N13" s="1">
         <v>10249</v>
       </c>
       <c r="O13">
-        <f t="shared" si="5"/>
+        <f>IF(ISBLANK(P13),-N13,P13-N13)</f>
         <v>78</v>
       </c>
       <c r="P13" s="1">
         <v>10327</v>
       </c>
       <c r="Q13">
-        <f t="shared" si="6"/>
+        <f>IF(ISBLANK(R13),-P13,R13-P13)</f>
         <v>137</v>
       </c>
       <c r="R13" s="1">
         <v>10464</v>
+      </c>
+      <c r="S13">
+        <f>IF(ISBLANK(T13),-R13,T13-R13)</f>
+        <v>79</v>
+      </c>
+      <c r="T13" s="1">
+        <v>10543</v>
       </c>
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.25">
@@ -7487,53 +7571,60 @@
         <v>79072</v>
       </c>
       <c r="E14">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F14),-D14,F14-D14)</f>
         <v>68</v>
       </c>
       <c r="F14" s="1">
         <v>79140</v>
       </c>
       <c r="G14">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H14),-F14,H14-F14)</f>
         <v>142</v>
       </c>
       <c r="H14" s="1">
         <v>79282</v>
       </c>
       <c r="I14">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J14),-H14,J14-H14)</f>
         <v>105</v>
       </c>
       <c r="J14" s="1">
         <v>79387</v>
       </c>
       <c r="K14">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L14),-J14,L14-J14)</f>
         <v>186</v>
       </c>
       <c r="L14" s="1">
         <v>79573</v>
       </c>
       <c r="M14">
-        <f t="shared" si="4"/>
+        <f>IF(ISBLANK(N14),-L14,N14-L14)</f>
         <v>168</v>
       </c>
       <c r="N14" s="1">
         <v>79741</v>
       </c>
       <c r="O14">
-        <f t="shared" si="5"/>
+        <f>IF(ISBLANK(P14),-N14,P14-N14)</f>
         <v>204</v>
       </c>
       <c r="P14" s="1">
         <v>79945</v>
       </c>
       <c r="Q14">
-        <f t="shared" si="6"/>
+        <f>IF(ISBLANK(R14),-P14,R14-P14)</f>
         <v>305</v>
       </c>
       <c r="R14" s="1">
         <v>80250</v>
+      </c>
+      <c r="S14">
+        <f>IF(ISBLANK(T14),-R14,T14-R14)</f>
+        <v>127</v>
+      </c>
+      <c r="T14" s="1">
+        <v>80377</v>
       </c>
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.25">
@@ -7547,53 +7638,60 @@
         <v>22075</v>
       </c>
       <c r="E15">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F15),-D15,F15-D15)</f>
         <v>38</v>
       </c>
       <c r="F15" s="1">
         <v>22113</v>
       </c>
       <c r="G15">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H15),-F15,H15-F15)</f>
         <v>80</v>
       </c>
       <c r="H15" s="1">
         <v>22193</v>
       </c>
       <c r="I15">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J15),-H15,J15-H15)</f>
         <v>58</v>
       </c>
       <c r="J15" s="1">
         <v>22251</v>
       </c>
       <c r="K15">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L15),-J15,L15-J15)</f>
         <v>70</v>
       </c>
       <c r="L15" s="1">
         <v>22321</v>
       </c>
       <c r="M15">
-        <f t="shared" si="4"/>
+        <f>IF(ISBLANK(N15),-L15,N15-L15)</f>
         <v>62</v>
       </c>
       <c r="N15" s="1">
         <v>22383</v>
       </c>
       <c r="O15">
-        <f t="shared" si="5"/>
+        <f>IF(ISBLANK(P15),-N15,P15-N15)</f>
         <v>70</v>
       </c>
       <c r="P15" s="1">
         <v>22453</v>
       </c>
       <c r="Q15">
-        <f t="shared" si="6"/>
+        <f>IF(ISBLANK(R15),-P15,R15-P15)</f>
         <v>173</v>
       </c>
       <c r="R15" s="1">
         <v>22626</v>
+      </c>
+      <c r="S15">
+        <f>IF(ISBLANK(T15),-R15,T15-R15)</f>
+        <v>74</v>
+      </c>
+      <c r="T15" s="1">
+        <v>22700</v>
       </c>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.25">
@@ -7607,56 +7705,63 @@
         <v>9823</v>
       </c>
       <c r="E16">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F16),-D16,F16-D16)</f>
         <v>37</v>
       </c>
       <c r="F16" s="1">
         <v>9860</v>
       </c>
       <c r="G16">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H16),-F16,H16-F16)</f>
         <v>76</v>
       </c>
       <c r="H16" s="1">
         <v>9936</v>
       </c>
       <c r="I16">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J16),-H16,J16-H16)</f>
         <v>54</v>
       </c>
       <c r="J16" s="1">
         <v>9990</v>
       </c>
       <c r="K16">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L16),-J16,L16-J16)</f>
         <v>184</v>
       </c>
       <c r="L16" s="1">
         <v>10174</v>
       </c>
       <c r="M16">
-        <f t="shared" si="4"/>
+        <f>IF(ISBLANK(N16),-L16,N16-L16)</f>
         <v>52</v>
       </c>
       <c r="N16" s="1">
         <v>10226</v>
       </c>
       <c r="O16">
-        <f t="shared" si="5"/>
+        <f>IF(ISBLANK(P16),-N16,P16-N16)</f>
         <v>168</v>
       </c>
       <c r="P16" s="1">
         <v>10394</v>
       </c>
       <c r="Q16">
-        <f t="shared" si="6"/>
+        <f>IF(ISBLANK(R16),-P16,R16-P16)</f>
         <v>214</v>
       </c>
       <c r="R16" s="1">
         <v>10608</v>
       </c>
-    </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="S16">
+        <f>IF(ISBLANK(T16),-R16,T16-R16)</f>
+        <v>48</v>
+      </c>
+      <c r="T16" s="1">
+        <v>10656</v>
+      </c>
+    </row>
+    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>17</v>
       </c>
@@ -7667,56 +7772,63 @@
         <v>3682</v>
       </c>
       <c r="E17">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F17),-D17,F17-D17)</f>
         <v>77</v>
       </c>
       <c r="F17" s="1">
         <v>3759</v>
       </c>
       <c r="G17">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H17),-F17,H17-F17)</f>
         <v>44</v>
       </c>
       <c r="H17" s="1">
         <v>3803</v>
       </c>
       <c r="I17">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J17),-H17,J17-H17)</f>
         <v>116</v>
       </c>
       <c r="J17" s="1">
         <v>3919</v>
       </c>
       <c r="K17">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L17),-J17,L17-J17)</f>
         <v>87</v>
       </c>
       <c r="L17" s="1">
         <v>4006</v>
       </c>
       <c r="M17">
-        <f t="shared" si="4"/>
+        <f>IF(ISBLANK(N17),-L17,N17-L17)</f>
         <v>41</v>
       </c>
       <c r="N17" s="1">
         <v>4047</v>
       </c>
       <c r="O17">
-        <f t="shared" si="5"/>
+        <f>IF(ISBLANK(P17),-N17,P17-N17)</f>
         <v>134</v>
       </c>
       <c r="P17" s="1">
         <v>4181</v>
       </c>
       <c r="Q17">
-        <f t="shared" si="6"/>
+        <f>IF(ISBLANK(R17),-P17,R17-P17)</f>
         <v>-4181</v>
       </c>
       <c r="R17" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="S17">
+        <f>IF(ISBLANK(T17),-R17,T17-R17)</f>
+        <v>0</v>
+      </c>
+      <c r="T17" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>5</v>
       </c>
@@ -7727,56 +7839,63 @@
         <v>75946</v>
       </c>
       <c r="E18">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F18),-D18,F18-D18)</f>
         <v>100</v>
       </c>
       <c r="F18" s="1">
         <v>76046</v>
       </c>
       <c r="G18">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H18),-F18,H18-F18)</f>
         <v>201</v>
       </c>
       <c r="H18" s="1">
         <v>76247</v>
       </c>
       <c r="I18">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J18),-H18,J18-H18)</f>
         <v>126</v>
       </c>
       <c r="J18" s="1">
         <v>76373</v>
       </c>
       <c r="K18">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L18),-J18,L18-J18)</f>
         <v>272</v>
       </c>
       <c r="L18" s="1">
         <v>76645</v>
       </c>
       <c r="M18">
-        <f t="shared" si="4"/>
+        <f>IF(ISBLANK(N18),-L18,N18-L18)</f>
         <v>74</v>
       </c>
       <c r="N18" s="1">
         <v>76719</v>
       </c>
       <c r="O18">
-        <f t="shared" si="5"/>
+        <f>IF(ISBLANK(P18),-N18,P18-N18)</f>
         <v>301</v>
       </c>
       <c r="P18" s="1">
         <v>77020</v>
       </c>
       <c r="Q18">
-        <f t="shared" si="6"/>
+        <f>IF(ISBLANK(R18),-P18,R18-P18)</f>
         <v>283</v>
       </c>
       <c r="R18" s="1">
         <v>77303</v>
       </c>
-    </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="S18">
+        <f>IF(ISBLANK(T18),-R18,T18-R18)</f>
+        <v>112</v>
+      </c>
+      <c r="T18" s="1">
+        <v>77415</v>
+      </c>
+    </row>
+    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>20</v>
       </c>
@@ -7787,56 +7906,63 @@
         <v>2864</v>
       </c>
       <c r="E19">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F19),-D19,F19-D19)</f>
         <v>34</v>
       </c>
       <c r="F19" s="1">
         <v>2898</v>
       </c>
       <c r="G19">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H19),-F19,H19-F19)</f>
         <v>21</v>
       </c>
       <c r="H19" s="1">
         <v>2919</v>
       </c>
       <c r="I19">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J19),-H19,J19-H19)</f>
         <v>148</v>
       </c>
       <c r="J19" s="1">
         <v>3067</v>
       </c>
       <c r="K19">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L19),-J19,L19-J19)</f>
         <v>-3067</v>
       </c>
       <c r="L19" s="1">
         <v>0</v>
       </c>
       <c r="M19">
-        <f t="shared" si="4"/>
+        <f>IF(ISBLANK(N19),-L19,N19-L19)</f>
         <v>0</v>
       </c>
       <c r="N19" s="1">
         <v>0</v>
       </c>
       <c r="O19">
-        <f t="shared" si="5"/>
+        <f>IF(ISBLANK(P19),-N19,P19-N19)</f>
         <v>0</v>
       </c>
       <c r="P19" s="1">
         <v>0</v>
       </c>
       <c r="Q19">
-        <f t="shared" si="6"/>
+        <f>IF(ISBLANK(R19),-P19,R19-P19)</f>
         <v>0</v>
       </c>
       <c r="R19" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="S19">
+        <f>IF(ISBLANK(T19),-R19,T19-R19)</f>
+        <v>0</v>
+      </c>
+      <c r="T19" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>21</v>
       </c>
@@ -7847,56 +7973,63 @@
         <v>2416</v>
       </c>
       <c r="E20">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F20),-D20,F20-D20)</f>
         <v>48</v>
       </c>
       <c r="F20" s="1">
         <v>2464</v>
       </c>
       <c r="G20">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H20),-F20,H20-F20)</f>
         <v>78</v>
       </c>
       <c r="H20" s="1">
         <v>2542</v>
       </c>
       <c r="I20">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J20),-H20,J20-H20)</f>
         <v>-2542</v>
       </c>
       <c r="J20" s="1">
         <v>0</v>
       </c>
       <c r="K20">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L20),-J20,L20-J20)</f>
         <v>0</v>
       </c>
       <c r="L20" s="1">
         <v>0</v>
       </c>
       <c r="M20">
-        <f t="shared" si="4"/>
+        <f>IF(ISBLANK(N20),-L20,N20-L20)</f>
         <v>0</v>
       </c>
       <c r="N20" s="1">
         <v>0</v>
       </c>
       <c r="O20">
-        <f t="shared" si="5"/>
+        <f>IF(ISBLANK(P20),-N20,P20-N20)</f>
         <v>0</v>
       </c>
       <c r="P20" s="1">
         <v>0</v>
       </c>
       <c r="Q20">
-        <f t="shared" si="6"/>
+        <f>IF(ISBLANK(R20),-P20,R20-P20)</f>
         <v>0</v>
       </c>
       <c r="R20" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="S20">
+        <f>IF(ISBLANK(T20),-R20,T20-R20)</f>
+        <v>0</v>
+      </c>
+      <c r="T20" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>23</v>
       </c>
@@ -7907,56 +8040,63 @@
         <v>1423</v>
       </c>
       <c r="E21">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F21),-D21,F21-D21)</f>
         <v>-1423</v>
       </c>
       <c r="F21" s="1">
         <v>0</v>
       </c>
       <c r="G21">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H21),-F21,H21-F21)</f>
         <v>0</v>
       </c>
       <c r="H21" s="1">
         <v>0</v>
       </c>
       <c r="I21">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J21),-H21,J21-H21)</f>
         <v>0</v>
       </c>
       <c r="J21" s="1">
         <v>0</v>
       </c>
       <c r="K21">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L21),-J21,L21-J21)</f>
         <v>0</v>
       </c>
       <c r="L21" s="1">
         <v>0</v>
       </c>
       <c r="M21">
-        <f t="shared" si="4"/>
+        <f>IF(ISBLANK(N21),-L21,N21-L21)</f>
         <v>0</v>
       </c>
       <c r="N21" s="1">
         <v>0</v>
       </c>
       <c r="O21">
-        <f t="shared" si="5"/>
+        <f>IF(ISBLANK(P21),-N21,P21-N21)</f>
         <v>0</v>
       </c>
       <c r="P21" s="1">
         <v>0</v>
       </c>
       <c r="Q21">
-        <f t="shared" si="6"/>
+        <f>IF(ISBLANK(R21),-P21,R21-P21)</f>
         <v>0</v>
       </c>
       <c r="R21" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="S21">
+        <f>IF(ISBLANK(T21),-R21,T21-R21)</f>
+        <v>0</v>
+      </c>
+      <c r="T21" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>10</v>
       </c>
@@ -7967,56 +8107,63 @@
         <v>14802</v>
       </c>
       <c r="E22">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F22),-D22,F22-D22)</f>
         <v>156</v>
       </c>
       <c r="F22" s="1">
         <v>14958</v>
       </c>
       <c r="G22">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H22),-F22,H22-F22)</f>
         <v>51</v>
       </c>
       <c r="H22" s="1">
         <v>15009</v>
       </c>
       <c r="I22">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J22),-H22,J22-H22)</f>
         <v>198</v>
       </c>
       <c r="J22" s="1">
         <v>15207</v>
       </c>
       <c r="K22">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L22),-J22,L22-J22)</f>
         <v>146</v>
       </c>
       <c r="L22" s="1">
         <v>15353</v>
       </c>
       <c r="M22">
-        <f t="shared" si="4"/>
+        <f>IF(ISBLANK(N22),-L22,N22-L22)</f>
         <v>41</v>
       </c>
       <c r="N22" s="1">
         <v>15394</v>
       </c>
       <c r="O22">
-        <f t="shared" si="5"/>
+        <f>IF(ISBLANK(P22),-N22,P22-N22)</f>
         <v>392</v>
       </c>
       <c r="P22" s="1">
         <v>15786</v>
       </c>
       <c r="Q22">
-        <f t="shared" si="6"/>
+        <f>IF(ISBLANK(R22),-P22,R22-P22)</f>
         <v>321</v>
       </c>
       <c r="R22" s="1">
         <v>16107</v>
       </c>
-    </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="S22">
+        <f>IF(ISBLANK(T22),-R22,T22-R22)</f>
+        <v>101</v>
+      </c>
+      <c r="T22" s="1">
+        <v>16208</v>
+      </c>
+    </row>
+    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>3</v>
       </c>
@@ -8027,56 +8174,63 @@
         <v>81741</v>
       </c>
       <c r="E23">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F23),-D23,F23-D23)</f>
         <v>253</v>
       </c>
       <c r="F23" s="1">
         <v>81994</v>
       </c>
       <c r="G23">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H23),-F23,H23-F23)</f>
         <v>130</v>
       </c>
       <c r="H23" s="1">
         <v>82124</v>
       </c>
       <c r="I23">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J23),-H23,J23-H23)</f>
         <v>211</v>
       </c>
       <c r="J23" s="1">
         <v>82335</v>
       </c>
       <c r="K23">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L23),-J23,L23-J23)</f>
         <v>323</v>
       </c>
       <c r="L23" s="1">
         <v>82658</v>
       </c>
       <c r="M23">
-        <f t="shared" si="4"/>
+        <f>IF(ISBLANK(N23),-L23,N23-L23)</f>
         <v>206</v>
       </c>
       <c r="N23" s="1">
         <v>82864</v>
       </c>
       <c r="O23">
-        <f t="shared" si="5"/>
+        <f>IF(ISBLANK(P23),-N23,P23-N23)</f>
         <v>556</v>
       </c>
       <c r="P23" s="1">
         <v>83420</v>
       </c>
       <c r="Q23">
-        <f t="shared" si="6"/>
+        <f>IF(ISBLANK(R23),-P23,R23-P23)</f>
         <v>351</v>
       </c>
       <c r="R23" s="1">
         <v>83771</v>
       </c>
-    </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="S23">
+        <f>IF(ISBLANK(T23),-R23,T23-R23)</f>
+        <v>217</v>
+      </c>
+      <c r="T23" s="1">
+        <v>83988</v>
+      </c>
+    </row>
+    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>18</v>
       </c>
@@ -8087,56 +8241,63 @@
         <v>3286</v>
       </c>
       <c r="E24">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F24),-D24,F24-D24)</f>
         <v>21</v>
       </c>
       <c r="F24" s="1">
         <v>3307</v>
       </c>
       <c r="G24">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H24),-F24,H24-F24)</f>
         <v>13</v>
       </c>
       <c r="H24" s="1">
         <v>3320</v>
       </c>
       <c r="I24">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J24),-H24,J24-H24)</f>
         <v>232</v>
       </c>
       <c r="J24" s="1">
         <v>3552</v>
       </c>
       <c r="K24">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L24),-J24,L24-J24)</f>
         <v>102</v>
       </c>
       <c r="L24" s="1">
         <v>3654</v>
       </c>
       <c r="M24">
-        <f t="shared" si="4"/>
+        <f>IF(ISBLANK(N24),-L24,N24-L24)</f>
         <v>60</v>
       </c>
       <c r="N24" s="1">
         <v>3714</v>
       </c>
       <c r="O24">
-        <f t="shared" si="5"/>
+        <f>IF(ISBLANK(P24),-N24,P24-N24)</f>
         <v>-3714</v>
       </c>
       <c r="P24" s="1">
         <v>0</v>
       </c>
       <c r="Q24">
-        <f t="shared" si="6"/>
+        <f>IF(ISBLANK(R24),-P24,R24-P24)</f>
         <v>0</v>
       </c>
       <c r="R24" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="S24">
+        <f>IF(ISBLANK(T24),-R24,T24-R24)</f>
+        <v>0</v>
+      </c>
+      <c r="T24" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>147</v>
       </c>
@@ -8201,25 +8362,28 @@
       <c r="X26" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y26" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>148</v>
       </c>
       <c r="E27">
-        <f t="shared" ref="E27:E48" si="7">FIND(",",B27)</f>
+        <f t="shared" ref="E27:E48" si="0">FIND(",",B27)</f>
         <v>9</v>
       </c>
       <c r="F27" t="str">
-        <f t="shared" ref="F27:F48" si="8">LEFT(B27,E27-1)</f>
+        <f t="shared" ref="F27:F48" si="1">LEFT(B27,E27-1)</f>
         <v>Kelleher</v>
       </c>
       <c r="G27" t="str">
-        <f t="shared" ref="G27:G48" si="9">RIGHT(B27,LEN(B27)-(E27+1))</f>
+        <f t="shared" ref="G27:G48" si="2">RIGHT(B27,LEN(B27)-(E27+1))</f>
         <v>Billy</v>
       </c>
       <c r="H27" t="str">
-        <f t="shared" ref="H27:H48" si="10">G27&amp;" "&amp;F27</f>
+        <f t="shared" ref="H27:H48" si="3">G27&amp;" "&amp;F27</f>
         <v>Billy Kelleher</v>
       </c>
       <c r="J27" t="s">
@@ -8261,25 +8425,33 @@
       <c r="X27" s="1">
         <v>119715</v>
       </c>
-    </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y27" s="1">
+        <v>119883</v>
+      </c>
+      <c r="Z27" s="1"/>
+      <c r="AA27" s="1"/>
+      <c r="AB27" s="1"/>
+      <c r="AC27" s="1"/>
+      <c r="AD27" s="1"/>
+    </row>
+    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>149</v>
       </c>
       <c r="E28">
-        <f t="shared" si="7"/>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="F28" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="1"/>
         <v>Wallace</v>
       </c>
       <c r="G28" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="2"/>
         <v>Mick</v>
       </c>
       <c r="H28" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>Mick Wallace</v>
       </c>
       <c r="J28" t="s">
@@ -8321,25 +8493,33 @@
       <c r="X28" s="1">
         <v>84841</v>
       </c>
-    </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y28" s="1">
+        <v>84971</v>
+      </c>
+      <c r="Z28" s="1"/>
+      <c r="AA28" s="1"/>
+      <c r="AB28" s="1"/>
+      <c r="AC28" s="1"/>
+      <c r="AD28" s="1"/>
+    </row>
+    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>150</v>
       </c>
       <c r="E29">
-        <f t="shared" si="7"/>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="F29" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="1"/>
         <v>Ní Riada</v>
       </c>
       <c r="G29" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="2"/>
         <v>Liadh</v>
       </c>
       <c r="H29" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>Liadh Ní Riada</v>
       </c>
       <c r="J29" t="s">
@@ -8381,25 +8561,33 @@
       <c r="X29" s="1">
         <v>83771</v>
       </c>
-    </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y29" s="1">
+        <v>83988</v>
+      </c>
+      <c r="Z29" s="1"/>
+      <c r="AA29" s="1"/>
+      <c r="AB29" s="1"/>
+      <c r="AC29" s="1"/>
+      <c r="AD29" s="1"/>
+    </row>
+    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>151</v>
       </c>
       <c r="E30">
-        <f t="shared" si="7"/>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="F30" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="1"/>
         <v>O'Sullivan</v>
       </c>
       <c r="G30" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="2"/>
         <v>Grace</v>
       </c>
       <c r="H30" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>Grace O'Sullivan</v>
       </c>
       <c r="J30" t="s">
@@ -8441,25 +8629,33 @@
       <c r="X30" s="1">
         <v>80250</v>
       </c>
-    </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y30" s="1">
+        <v>80377</v>
+      </c>
+      <c r="Z30" s="1"/>
+      <c r="AA30" s="1"/>
+      <c r="AB30" s="1"/>
+      <c r="AC30" s="1"/>
+      <c r="AD30" s="1"/>
+    </row>
+    <row r="31" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>152</v>
       </c>
       <c r="E31">
-        <f t="shared" si="7"/>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="F31" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="1"/>
         <v>Byrne</v>
       </c>
       <c r="G31" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="2"/>
         <v>Malcolm</v>
       </c>
       <c r="H31" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>Malcolm Byrne</v>
       </c>
       <c r="J31" t="s">
@@ -8501,25 +8697,33 @@
       <c r="X31" s="1">
         <v>77303</v>
       </c>
-    </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y31" s="1">
+        <v>77415</v>
+      </c>
+      <c r="Z31" s="1"/>
+      <c r="AA31" s="1"/>
+      <c r="AB31" s="1"/>
+      <c r="AC31" s="1"/>
+      <c r="AD31" s="1"/>
+    </row>
+    <row r="32" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>153</v>
       </c>
       <c r="E32">
-        <f t="shared" si="7"/>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="F32" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="1"/>
         <v>Clune</v>
       </c>
       <c r="G32" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="2"/>
         <v>Deirdre</v>
       </c>
       <c r="H32" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>Deirdre Clune</v>
       </c>
       <c r="J32" t="s">
@@ -8561,25 +8765,33 @@
       <c r="X32" s="1">
         <v>69672</v>
       </c>
-    </row>
-    <row r="33" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="Y32" s="1">
+        <v>70898</v>
+      </c>
+      <c r="Z32" s="1"/>
+      <c r="AA32" s="1"/>
+      <c r="AB32" s="1"/>
+      <c r="AC32" s="1"/>
+      <c r="AD32" s="1"/>
+    </row>
+    <row r="33" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>154</v>
       </c>
       <c r="E33">
-        <f t="shared" si="7"/>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="F33" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="1"/>
         <v>Doyle</v>
       </c>
       <c r="G33" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="2"/>
         <v>Andrew</v>
       </c>
       <c r="H33" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>Andrew Doyle</v>
       </c>
       <c r="J33" t="s">
@@ -8621,25 +8833,33 @@
       <c r="X33" s="1">
         <v>65252</v>
       </c>
-    </row>
-    <row r="34" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="Y33" s="1">
+        <v>65558</v>
+      </c>
+      <c r="Z33" s="1"/>
+      <c r="AA33" s="1"/>
+      <c r="AB33" s="1"/>
+      <c r="AC33" s="1"/>
+      <c r="AD33" s="1"/>
+    </row>
+    <row r="34" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>155</v>
       </c>
       <c r="E34">
-        <f t="shared" si="7"/>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="F34" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="1"/>
         <v>Nunan</v>
       </c>
       <c r="G34" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="2"/>
         <v>Sheila</v>
       </c>
       <c r="H34" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>Sheila Nunan</v>
       </c>
       <c r="J34" t="s">
@@ -8681,25 +8901,33 @@
       <c r="X34" s="1">
         <v>38996</v>
       </c>
-    </row>
-    <row r="35" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="Y34" s="1">
+        <v>39294</v>
+      </c>
+      <c r="Z34" s="1"/>
+      <c r="AA34" s="1"/>
+      <c r="AB34" s="1"/>
+      <c r="AC34" s="1"/>
+      <c r="AD34" s="1"/>
+    </row>
+    <row r="35" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>156</v>
       </c>
       <c r="E35">
-        <f t="shared" si="7"/>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="F35" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="1"/>
         <v>Wallace</v>
       </c>
       <c r="G35" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="2"/>
         <v>Adrienne</v>
       </c>
       <c r="H35" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>Adrienne Wallace</v>
       </c>
       <c r="J35" t="s">
@@ -8741,25 +8969,33 @@
       <c r="X35" s="1">
         <v>22626</v>
       </c>
-    </row>
-    <row r="36" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="Y35" s="1">
+        <v>22700</v>
+      </c>
+      <c r="Z35" s="1"/>
+      <c r="AA35" s="1"/>
+      <c r="AB35" s="1"/>
+      <c r="AC35" s="1"/>
+      <c r="AD35" s="1"/>
+    </row>
+    <row r="36" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>157</v>
       </c>
       <c r="E36">
-        <f t="shared" si="7"/>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="F36" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="1"/>
         <v>Cahill</v>
       </c>
       <c r="G36" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="2"/>
         <v>Dolores</v>
       </c>
       <c r="H36" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>Dolores Cahill</v>
       </c>
       <c r="J36" t="s">
@@ -8801,25 +9037,33 @@
       <c r="X36" s="1">
         <v>16107</v>
       </c>
-    </row>
-    <row r="37" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="Y36" s="1">
+        <v>16208</v>
+      </c>
+      <c r="Z36" s="1"/>
+      <c r="AA36" s="1"/>
+      <c r="AB36" s="1"/>
+      <c r="AC36" s="1"/>
+      <c r="AD36" s="1"/>
+    </row>
+    <row r="37" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>158</v>
       </c>
       <c r="E37">
-        <f t="shared" si="7"/>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="F37" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="1"/>
         <v>O'Flynn</v>
       </c>
       <c r="G37" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="2"/>
         <v>Diarmuid Patrick</v>
       </c>
       <c r="H37" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>Diarmuid Patrick O'Flynn</v>
       </c>
       <c r="J37" t="s">
@@ -8861,25 +9105,33 @@
       <c r="X37" s="1">
         <v>11718</v>
       </c>
-    </row>
-    <row r="38" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="Y37" s="1">
+        <v>12626</v>
+      </c>
+      <c r="Z37" s="1"/>
+      <c r="AA37" s="1"/>
+      <c r="AB37" s="1"/>
+      <c r="AC37" s="1"/>
+      <c r="AD37" s="1"/>
+    </row>
+    <row r="38" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>159</v>
       </c>
       <c r="E38">
-        <f t="shared" si="7"/>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="F38" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="1"/>
         <v>Minehan</v>
       </c>
       <c r="G38" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="2"/>
         <v>Liam</v>
       </c>
       <c r="H38" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>Liam Minehan</v>
       </c>
       <c r="J38" t="s">
@@ -8921,25 +9173,33 @@
       <c r="X38" s="1">
         <v>10608</v>
       </c>
-    </row>
-    <row r="39" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="Y38" s="1">
+        <v>10656</v>
+      </c>
+      <c r="Z38" s="1"/>
+      <c r="AA38" s="1"/>
+      <c r="AB38" s="1"/>
+      <c r="AC38" s="1"/>
+      <c r="AD38" s="1"/>
+    </row>
+    <row r="39" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>160</v>
       </c>
       <c r="E39">
-        <f t="shared" si="7"/>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="F39" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="1"/>
         <v>Gardner</v>
       </c>
       <c r="G39" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="2"/>
         <v>Breda Patricia</v>
       </c>
       <c r="H39" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>Breda Patricia Gardner</v>
       </c>
       <c r="J39" t="s">
@@ -8981,25 +9241,33 @@
       <c r="X39" s="1">
         <v>10464</v>
       </c>
-    </row>
-    <row r="40" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="Y39" s="1">
+        <v>10543</v>
+      </c>
+      <c r="Z39" s="1"/>
+      <c r="AA39" s="1"/>
+      <c r="AB39" s="1"/>
+      <c r="AC39" s="1"/>
+      <c r="AD39" s="1"/>
+    </row>
+    <row r="40" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>161</v>
       </c>
       <c r="E40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="F40" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="1"/>
         <v>Heaney</v>
       </c>
       <c r="G40" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="2"/>
         <v>Theresa</v>
       </c>
       <c r="H40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>Theresa Heaney</v>
       </c>
       <c r="J40" t="s">
@@ -9041,25 +9309,33 @@
       <c r="X40" s="1">
         <v>9975</v>
       </c>
-    </row>
-    <row r="41" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="Y40" s="1">
+        <v>10222</v>
+      </c>
+      <c r="Z40" s="1"/>
+      <c r="AA40" s="1"/>
+      <c r="AB40" s="1"/>
+      <c r="AC40" s="1"/>
+      <c r="AD40" s="1"/>
+    </row>
+    <row r="41" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>162</v>
       </c>
       <c r="E41">
-        <f t="shared" si="7"/>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="F41" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="1"/>
         <v>Brennan</v>
       </c>
       <c r="G41" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="2"/>
         <v>Allan</v>
       </c>
       <c r="H41" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>Allan Brennan</v>
       </c>
       <c r="J41" t="s">
@@ -9101,25 +9377,33 @@
       <c r="X41" s="1">
         <v>8373</v>
       </c>
-    </row>
-    <row r="42" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="Y41" s="1">
+        <v>8561</v>
+      </c>
+      <c r="Z41" s="1"/>
+      <c r="AA41" s="1"/>
+      <c r="AB41" s="1"/>
+      <c r="AC41" s="1"/>
+      <c r="AD41" s="1"/>
+    </row>
+    <row r="42" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>163</v>
       </c>
       <c r="E42">
-        <f t="shared" si="7"/>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="F42" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="1"/>
         <v>O'Loughlin</v>
       </c>
       <c r="G42" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="2"/>
         <v>Peter</v>
       </c>
       <c r="H42" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>Peter O'Loughlin</v>
       </c>
       <c r="J42" t="s">
@@ -9161,25 +9445,30 @@
       <c r="X42" s="1">
         <v>5132</v>
       </c>
-    </row>
-    <row r="43" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="Z42" s="1"/>
+      <c r="AA42" s="1"/>
+      <c r="AB42" s="1"/>
+      <c r="AC42" s="1"/>
+      <c r="AD42" s="1"/>
+    </row>
+    <row r="43" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>164</v>
       </c>
       <c r="E43">
-        <f t="shared" si="7"/>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="F43" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="1"/>
         <v>Worthington</v>
       </c>
       <c r="G43" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="2"/>
         <v>Colleen</v>
       </c>
       <c r="H43" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>Colleen Worthington</v>
       </c>
       <c r="J43" t="s">
@@ -9218,25 +9507,29 @@
       <c r="W43" s="1">
         <v>4181</v>
       </c>
-    </row>
-    <row r="44" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="Z43" s="1"/>
+      <c r="AA43" s="1"/>
+      <c r="AB43" s="1"/>
+      <c r="AC43" s="1"/>
+    </row>
+    <row r="44" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>165</v>
       </c>
       <c r="E44">
-        <f t="shared" si="7"/>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="F44" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="1"/>
         <v>Fitzgerald</v>
       </c>
       <c r="G44" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="2"/>
         <v>Paddy</v>
       </c>
       <c r="H44" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>Paddy Fitzgerald</v>
       </c>
       <c r="J44" t="s">
@@ -9272,25 +9565,28 @@
       <c r="V44" s="1">
         <v>3714</v>
       </c>
-    </row>
-    <row r="45" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="Z44" s="1"/>
+      <c r="AA44" s="1"/>
+      <c r="AB44" s="1"/>
+    </row>
+    <row r="45" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>166</v>
       </c>
       <c r="E45">
-        <f t="shared" si="7"/>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="F45" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="1"/>
         <v>Ryan-Purcell</v>
       </c>
       <c r="G45" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="2"/>
         <v>Walter</v>
       </c>
       <c r="H45" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>Walter Ryan-Purcell</v>
       </c>
       <c r="J45" t="s">
@@ -9323,25 +9619,27 @@
       <c r="U45" s="1">
         <v>3332</v>
       </c>
-    </row>
-    <row r="46" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="Z45" s="1"/>
+      <c r="AA45" s="1"/>
+    </row>
+    <row r="46" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>167</v>
       </c>
       <c r="E46">
-        <f t="shared" si="7"/>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="F46" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="1"/>
         <v>Sexton</v>
       </c>
       <c r="G46" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="2"/>
         <v>Joesph</v>
       </c>
       <c r="H46" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>Joesph Sexton</v>
       </c>
       <c r="J46" t="s">
@@ -9368,25 +9666,26 @@
       <c r="T46" s="1">
         <v>3067</v>
       </c>
-    </row>
-    <row r="47" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="Z46" s="1"/>
+    </row>
+    <row r="47" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>168</v>
       </c>
       <c r="E47">
-        <f t="shared" si="7"/>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="F47" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="1"/>
         <v>Madden</v>
       </c>
       <c r="G47" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="2"/>
         <v>Peter</v>
       </c>
       <c r="H47" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>Peter Madden</v>
       </c>
       <c r="J47" t="s">
@@ -9408,24 +9707,24 @@
         <v>2542</v>
       </c>
     </row>
-    <row r="48" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>169</v>
       </c>
       <c r="E48">
-        <f t="shared" si="7"/>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="F48" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="1"/>
         <v>Van de Ven</v>
       </c>
       <c r="G48" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="2"/>
         <v>Jan</v>
       </c>
       <c r="H48" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>Jan Van de Ven</v>
       </c>
       <c r="J48" t="s">
@@ -9450,7 +9749,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:R24">
+  <sortState ref="A2:T24">
     <sortCondition ref="B2:B24"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Stage 7 midlands added Signed-off-by: Gerry Mulvenna <git@movingwifi.com>
</commit_message>
<xml_diff>
--- a/europarl/europarl-ireland-2019.xlsx
+++ b/europarl/europarl-ireland-2019.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="14220" windowHeight="8580" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="14220" windowHeight="8580" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Candidates" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="262">
   <si>
     <t>Candidate</t>
   </si>
@@ -797,6 +797,12 @@
   </si>
   <si>
     <t>Brennan, Allan eliminated</t>
+  </si>
+  <si>
+    <t>Brennan, Cyril eliminated</t>
+  </si>
+  <si>
+    <t>O'Dowd, Michael eliminated</t>
   </si>
 </sst>
 </file>
@@ -5021,15 +5027,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y37"/>
+  <dimension ref="A1:AF37"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2:N18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>256</v>
       </c>
@@ -5051,572 +5057,662 @@
       <c r="L1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1">
-        <v>8130</v>
+        <v>134630</v>
       </c>
       <c r="E2">
-        <f t="shared" ref="E2:E18" si="0">IF(ISBLANK(F2),-D2,F2-D2)</f>
-        <v>96</v>
-      </c>
-      <c r="F2" s="1">
-        <v>8226</v>
+        <f>IF(ISBLANK(F2),-D2,F2-D2)</f>
+        <v>-15644</v>
+      </c>
+      <c r="F2">
+        <v>118986</v>
       </c>
       <c r="G2">
-        <f t="shared" ref="G2:G18" si="1">IF(ISBLANK(H2),-F2,H2-F2)</f>
-        <v>20</v>
-      </c>
-      <c r="H2" s="1">
-        <v>8246</v>
+        <f>IF(ISBLANK(H2),-F2,H2-F2)</f>
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>118986</v>
       </c>
       <c r="I2">
-        <f t="shared" ref="I2:I18" si="2">IF(ISBLANK(J2),-H2,J2-H2)</f>
-        <v>91</v>
-      </c>
-      <c r="J2" s="1">
-        <v>8337</v>
+        <f>IF(ISBLANK(J2),-H2,J2-H2)</f>
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>118986</v>
       </c>
       <c r="K2">
-        <f t="shared" ref="K2:K18" si="3">IF(ISBLANK(L2),-J2,L2-J2)</f>
-        <v>28</v>
-      </c>
-      <c r="L2" s="1">
-        <v>8365</v>
+        <f>IF(ISBLANK(L2),-J2,L2-J2)</f>
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>118986</v>
       </c>
       <c r="M2">
-        <f t="shared" ref="M2:M18" si="4">IF(ISBLANK(N2),-L2,N2-L2)</f>
-        <v>188</v>
-      </c>
-      <c r="N2" s="1">
-        <v>8553</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+        <f>IF(ISBLANK(N2),-L2,N2-L2)</f>
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>118986</v>
+      </c>
+      <c r="O2">
+        <f>IF(ISBLANK(P2),-N2,P2-N2)</f>
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>118986</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="1">
-        <v>77619</v>
+        <v>85034</v>
       </c>
       <c r="E3">
-        <f t="shared" si="0"/>
-        <v>868</v>
+        <f>IF(ISBLANK(F3),-D3,F3-D3)</f>
+        <v>1872</v>
       </c>
       <c r="F3" s="1">
-        <v>78487</v>
+        <v>86906</v>
       </c>
       <c r="G3">
-        <f t="shared" si="1"/>
-        <v>26</v>
+        <f>IF(ISBLANK(H3),-F3,H3-F3)</f>
+        <v>102</v>
       </c>
       <c r="H3" s="1">
-        <v>78513</v>
+        <v>87008</v>
       </c>
       <c r="I3">
-        <f t="shared" si="2"/>
-        <v>99</v>
+        <f>IF(ISBLANK(J3),-H3,J3-H3)</f>
+        <v>180</v>
       </c>
       <c r="J3" s="1">
-        <v>78612</v>
+        <v>87188</v>
       </c>
       <c r="K3">
-        <f t="shared" si="3"/>
-        <v>41</v>
+        <f>IF(ISBLANK(L3),-J3,L3-J3)</f>
+        <v>145</v>
       </c>
       <c r="L3" s="1">
-        <v>78653</v>
+        <v>87333</v>
       </c>
       <c r="M3">
-        <f t="shared" si="4"/>
-        <v>375</v>
+        <f>IF(ISBLANK(N3),-L3,N3-L3)</f>
+        <v>631</v>
       </c>
       <c r="N3" s="1">
-        <v>79028</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+        <v>87964</v>
+      </c>
+      <c r="O3">
+        <f>IF(ISBLANK(P3),-N3,P3-N3)</f>
+        <v>579</v>
+      </c>
+      <c r="P3" s="1">
+        <v>88543</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="1">
-        <v>56650</v>
+        <v>77619</v>
       </c>
       <c r="E4">
-        <f t="shared" si="0"/>
-        <v>1198</v>
+        <f>IF(ISBLANK(F4),-D4,F4-D4)</f>
+        <v>868</v>
       </c>
       <c r="F4" s="1">
-        <v>57848</v>
+        <v>78487</v>
       </c>
       <c r="G4">
-        <f t="shared" si="1"/>
-        <v>44</v>
+        <f>IF(ISBLANK(H4),-F4,H4-F4)</f>
+        <v>26</v>
       </c>
       <c r="H4" s="1">
-        <v>57892</v>
+        <v>78513</v>
       </c>
       <c r="I4">
-        <f t="shared" si="2"/>
-        <v>142</v>
+        <f>IF(ISBLANK(J4),-H4,J4-H4)</f>
+        <v>99</v>
       </c>
       <c r="J4" s="1">
-        <v>58034</v>
+        <v>78612</v>
       </c>
       <c r="K4">
-        <f t="shared" si="3"/>
-        <v>178</v>
+        <f>IF(ISBLANK(L4),-J4,L4-J4)</f>
+        <v>41</v>
       </c>
       <c r="L4" s="1">
-        <v>58212</v>
+        <v>78653</v>
       </c>
       <c r="M4">
-        <f t="shared" si="4"/>
-        <v>390</v>
+        <f>IF(ISBLANK(N4),-L4,N4-L4)</f>
+        <v>375</v>
       </c>
       <c r="N4" s="1">
-        <v>58602</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+        <v>79028</v>
+      </c>
+      <c r="O4">
+        <f>IF(ISBLANK(P4),-N4,P4-N4)</f>
+        <v>409</v>
+      </c>
+      <c r="P4" s="1">
+        <v>79437</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>257</v>
+        <v>199</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="1">
-        <v>15991</v>
+        <v>64500</v>
       </c>
       <c r="E5">
-        <f t="shared" si="0"/>
-        <v>477</v>
+        <f>IF(ISBLANK(F5),-D5,F5-D5)</f>
+        <v>6036</v>
       </c>
       <c r="F5" s="1">
-        <v>16468</v>
+        <v>70536</v>
       </c>
       <c r="G5">
-        <f t="shared" si="1"/>
-        <v>47</v>
+        <f>IF(ISBLANK(H5),-F5,H5-F5)</f>
+        <v>83</v>
       </c>
       <c r="H5" s="1">
-        <v>16515</v>
+        <v>70619</v>
       </c>
       <c r="I5">
-        <f t="shared" si="2"/>
-        <v>106</v>
+        <f>IF(ISBLANK(J5),-H5,J5-H5)</f>
+        <v>41</v>
       </c>
       <c r="J5" s="1">
-        <v>16621</v>
+        <v>70660</v>
       </c>
       <c r="K5">
-        <f t="shared" si="3"/>
-        <v>143</v>
+        <f>IF(ISBLANK(L5),-J5,L5-J5)</f>
+        <v>71</v>
       </c>
       <c r="L5" s="1">
-        <v>16764</v>
+        <v>70731</v>
       </c>
       <c r="M5">
-        <f t="shared" si="4"/>
-        <v>826</v>
+        <f>IF(ISBLANK(N5),-L5,N5-L5)</f>
+        <v>694</v>
       </c>
       <c r="N5" s="1">
-        <v>17590</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+        <v>71425</v>
+      </c>
+      <c r="O5">
+        <f>IF(ISBLANK(P5),-N5,P5-N5)</f>
+        <v>368</v>
+      </c>
+      <c r="P5" s="1">
+        <v>71793</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="1">
-        <v>85034</v>
+        <v>56650</v>
       </c>
       <c r="E6">
-        <f t="shared" si="0"/>
-        <v>1872</v>
+        <f>IF(ISBLANK(F6),-D6,F6-D6)</f>
+        <v>1198</v>
       </c>
       <c r="F6" s="1">
-        <v>86906</v>
+        <v>57848</v>
       </c>
       <c r="G6">
-        <f t="shared" si="1"/>
-        <v>102</v>
+        <f>IF(ISBLANK(H6),-F6,H6-F6)</f>
+        <v>44</v>
       </c>
       <c r="H6" s="1">
-        <v>87008</v>
+        <v>57892</v>
       </c>
       <c r="I6">
-        <f t="shared" si="2"/>
-        <v>180</v>
+        <f>IF(ISBLANK(J6),-H6,J6-H6)</f>
+        <v>142</v>
       </c>
       <c r="J6" s="1">
-        <v>87188</v>
+        <v>58034</v>
       </c>
       <c r="K6">
-        <f t="shared" si="3"/>
-        <v>145</v>
+        <f>IF(ISBLANK(L6),-J6,L6-J6)</f>
+        <v>178</v>
       </c>
       <c r="L6" s="1">
-        <v>87333</v>
+        <v>58212</v>
       </c>
       <c r="M6">
-        <f t="shared" si="4"/>
-        <v>631</v>
+        <f>IF(ISBLANK(N6),-L6,N6-L6)</f>
+        <v>390</v>
       </c>
       <c r="N6" s="1">
-        <v>87964</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+        <v>58602</v>
+      </c>
+      <c r="O6">
+        <f>IF(ISBLANK(P6),-N6,P6-N6)</f>
+        <v>1033</v>
+      </c>
+      <c r="P6" s="1">
+        <v>59635</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="1">
-        <v>1352</v>
+        <v>51019</v>
       </c>
       <c r="E7">
-        <f t="shared" si="0"/>
-        <v>48</v>
+        <f>IF(ISBLANK(F7),-D7,F7-D7)</f>
+        <v>1712</v>
       </c>
       <c r="F7" s="1">
-        <v>1400</v>
+        <v>52731</v>
       </c>
       <c r="G7">
-        <f t="shared" si="1"/>
-        <v>12</v>
+        <f>IF(ISBLANK(H7),-F7,H7-F7)</f>
+        <v>90</v>
       </c>
       <c r="H7" s="1">
-        <v>1412</v>
+        <v>52821</v>
       </c>
       <c r="I7">
-        <f t="shared" si="2"/>
-        <v>-1412</v>
+        <f>IF(ISBLANK(J7),-H7,J7-H7)</f>
+        <v>155</v>
       </c>
       <c r="J7" s="1">
-        <v>0</v>
+        <v>52976</v>
       </c>
       <c r="K7">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f>IF(ISBLANK(L7),-J7,L7-J7)</f>
+        <v>92</v>
       </c>
       <c r="L7" s="1">
-        <v>0</v>
+        <v>53068</v>
       </c>
       <c r="M7">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f>IF(ISBLANK(N7),-L7,N7-L7)</f>
+        <v>898</v>
       </c>
       <c r="N7" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+        <v>53966</v>
+      </c>
+      <c r="O7">
+        <f>IF(ISBLANK(P7),-N7,P7-N7)</f>
+        <v>582</v>
+      </c>
+      <c r="P7" s="1">
+        <v>54548</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="1">
-        <v>12378</v>
+        <v>42814</v>
       </c>
       <c r="E8">
-        <f t="shared" si="0"/>
-        <v>653</v>
+        <f>IF(ISBLANK(F8),-D8,F8-D8)</f>
+        <v>1226</v>
       </c>
       <c r="F8" s="1">
-        <v>13031</v>
+        <v>44040</v>
       </c>
       <c r="G8">
-        <f t="shared" si="1"/>
-        <v>34</v>
+        <f>IF(ISBLANK(H8),-F8,H8-F8)</f>
+        <v>19</v>
       </c>
       <c r="H8" s="1">
-        <v>13065</v>
+        <v>44059</v>
       </c>
       <c r="I8">
-        <f t="shared" si="2"/>
-        <v>85</v>
+        <f>IF(ISBLANK(J8),-H8,J8-H8)</f>
+        <v>17</v>
       </c>
       <c r="J8" s="1">
-        <v>13150</v>
+        <v>44076</v>
       </c>
       <c r="K8">
-        <f t="shared" si="3"/>
-        <v>47</v>
+        <f>IF(ISBLANK(L8),-J8,L8-J8)</f>
+        <v>54</v>
       </c>
       <c r="L8" s="1">
-        <v>13197</v>
+        <v>44130</v>
       </c>
       <c r="M8">
-        <f t="shared" si="4"/>
-        <v>211</v>
+        <f>IF(ISBLANK(N8),-L8,N8-L8)</f>
+        <v>125</v>
       </c>
       <c r="N8" s="1">
-        <v>13408</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+        <v>44255</v>
+      </c>
+      <c r="O8">
+        <f>IF(ISBLANK(P8),-N8,P8-N8)</f>
+        <v>437</v>
+      </c>
+      <c r="P8" s="1">
+        <v>44692</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="1">
-        <v>2450</v>
+        <v>30220</v>
       </c>
       <c r="E9">
-        <f t="shared" si="0"/>
-        <v>112</v>
+        <f>IF(ISBLANK(F9),-D9,F9-D9)</f>
+        <v>864</v>
       </c>
       <c r="F9" s="1">
-        <v>2562</v>
+        <v>31084</v>
       </c>
       <c r="G9">
-        <f t="shared" si="1"/>
-        <v>15</v>
+        <f>IF(ISBLANK(H9),-F9,H9-F9)</f>
+        <v>38</v>
       </c>
       <c r="H9" s="1">
-        <v>2577</v>
+        <v>31122</v>
       </c>
       <c r="I9">
-        <f t="shared" si="2"/>
-        <v>77</v>
+        <f>IF(ISBLANK(J9),-H9,J9-H9)</f>
+        <v>21</v>
       </c>
       <c r="J9" s="1">
-        <v>2654</v>
+        <v>31143</v>
       </c>
       <c r="K9">
-        <f t="shared" si="3"/>
-        <v>40</v>
+        <f>IF(ISBLANK(L9),-J9,L9-J9)</f>
+        <v>55</v>
       </c>
       <c r="L9" s="1">
-        <v>2694</v>
+        <v>31198</v>
       </c>
       <c r="M9">
-        <f t="shared" si="4"/>
-        <v>-2694</v>
+        <f>IF(ISBLANK(N9),-L9,N9-L9)</f>
+        <v>273</v>
       </c>
       <c r="N9" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+        <v>31471</v>
+      </c>
+      <c r="O9">
+        <f>IF(ISBLANK(P9),-N9,P9-N9)</f>
+        <v>422</v>
+      </c>
+      <c r="P9" s="1">
+        <v>31893</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>196</v>
+        <v>257</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="1">
-        <v>134630</v>
+        <v>15991</v>
       </c>
       <c r="E10">
-        <f t="shared" si="0"/>
-        <v>-15644</v>
-      </c>
-      <c r="F10">
-        <v>118986</v>
+        <f>IF(ISBLANK(F10),-D10,F10-D10)</f>
+        <v>477</v>
+      </c>
+      <c r="F10" s="1">
+        <v>16468</v>
       </c>
       <c r="G10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H10">
-        <v>118986</v>
+        <f>IF(ISBLANK(H10),-F10,H10-F10)</f>
+        <v>47</v>
+      </c>
+      <c r="H10" s="1">
+        <v>16515</v>
       </c>
       <c r="I10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J10">
-        <v>118986</v>
+        <f>IF(ISBLANK(J10),-H10,J10-H10)</f>
+        <v>106</v>
+      </c>
+      <c r="J10" s="1">
+        <v>16621</v>
       </c>
       <c r="K10">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L10">
-        <v>118986</v>
+        <f>IF(ISBLANK(L10),-J10,L10-J10)</f>
+        <v>143</v>
+      </c>
+      <c r="L10" s="1">
+        <v>16764</v>
       </c>
       <c r="M10">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="N10">
-        <v>118986</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+        <f>IF(ISBLANK(N10),-L10,N10-L10)</f>
+        <v>826</v>
+      </c>
+      <c r="N10" s="1">
+        <v>17590</v>
+      </c>
+      <c r="O10">
+        <f>IF(ISBLANK(P10),-N10,P10-N10)</f>
+        <v>1722</v>
+      </c>
+      <c r="P10" s="1">
+        <v>19312</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="1">
-        <v>51019</v>
+        <v>12378</v>
       </c>
       <c r="E11">
-        <f t="shared" si="0"/>
-        <v>1712</v>
+        <f>IF(ISBLANK(F11),-D11,F11-D11)</f>
+        <v>653</v>
       </c>
       <c r="F11" s="1">
-        <v>52731</v>
+        <v>13031</v>
       </c>
       <c r="G11">
-        <f t="shared" si="1"/>
-        <v>90</v>
+        <f>IF(ISBLANK(H11),-F11,H11-F11)</f>
+        <v>34</v>
       </c>
       <c r="H11" s="1">
-        <v>52821</v>
+        <v>13065</v>
       </c>
       <c r="I11">
-        <f t="shared" si="2"/>
-        <v>155</v>
+        <f>IF(ISBLANK(J11),-H11,J11-H11)</f>
+        <v>85</v>
       </c>
       <c r="J11" s="1">
-        <v>52976</v>
+        <v>13150</v>
       </c>
       <c r="K11">
-        <f t="shared" si="3"/>
-        <v>92</v>
+        <f>IF(ISBLANK(L11),-J11,L11-J11)</f>
+        <v>47</v>
       </c>
       <c r="L11" s="1">
-        <v>53068</v>
+        <v>13197</v>
       </c>
       <c r="M11">
-        <f t="shared" si="4"/>
-        <v>898</v>
+        <f>IF(ISBLANK(N11),-L11,N11-L11)</f>
+        <v>211</v>
       </c>
       <c r="N11" s="1">
-        <v>53966</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+        <v>13408</v>
+      </c>
+      <c r="O11">
+        <f>IF(ISBLANK(P11),-N11,P11-N11)</f>
+        <v>315</v>
+      </c>
+      <c r="P11" s="1">
+        <v>13723</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="1">
-        <v>1322</v>
+        <v>8130</v>
       </c>
       <c r="E12">
-        <f t="shared" si="0"/>
-        <v>53</v>
+        <f>IF(ISBLANK(F12),-D12,F12-D12)</f>
+        <v>96</v>
       </c>
       <c r="F12" s="1">
-        <v>1375</v>
+        <v>8226</v>
       </c>
       <c r="G12">
-        <f t="shared" si="1"/>
-        <v>71</v>
+        <f>IF(ISBLANK(H12),-F12,H12-F12)</f>
+        <v>20</v>
       </c>
       <c r="H12" s="1">
-        <v>1446</v>
+        <v>8246</v>
       </c>
       <c r="I12">
-        <f t="shared" si="2"/>
-        <v>44</v>
+        <f>IF(ISBLANK(J12),-H12,J12-H12)</f>
+        <v>91</v>
       </c>
       <c r="J12" s="1">
-        <v>1490</v>
+        <v>8337</v>
       </c>
       <c r="K12">
-        <f t="shared" si="3"/>
-        <v>-1490</v>
+        <f>IF(ISBLANK(L12),-J12,L12-J12)</f>
+        <v>28</v>
       </c>
       <c r="L12" s="1">
-        <v>0</v>
+        <v>8365</v>
       </c>
       <c r="M12">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f>IF(ISBLANK(N12),-L12,N12-L12)</f>
+        <v>188</v>
       </c>
       <c r="N12" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+        <v>8553</v>
+      </c>
+      <c r="O12">
+        <f>IF(ISBLANK(P12),-N12,P12-N12)</f>
+        <v>146</v>
+      </c>
+      <c r="P12" s="1">
+        <v>8699</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="C13" s="2"/>
-      <c r="D13">
-        <v>789</v>
+      <c r="D13" s="1">
+        <v>6897</v>
       </c>
       <c r="E13">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="F13">
-        <v>811</v>
+        <f>IF(ISBLANK(F13),-D13,F13-D13)</f>
+        <v>303</v>
+      </c>
+      <c r="F13" s="1">
+        <v>7200</v>
       </c>
       <c r="G13">
-        <f t="shared" si="1"/>
-        <v>-811</v>
+        <f>IF(ISBLANK(H13),-F13,H13-F13)</f>
+        <v>20</v>
       </c>
       <c r="H13" s="1">
-        <v>0</v>
+        <v>7220</v>
       </c>
       <c r="I13">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>IF(ISBLANK(J13),-H13,J13-H13)</f>
+        <v>84</v>
       </c>
       <c r="J13" s="1">
-        <v>0</v>
+        <v>7304</v>
       </c>
       <c r="K13">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f>IF(ISBLANK(L13),-J13,L13-J13)</f>
+        <v>141</v>
       </c>
       <c r="L13" s="1">
-        <v>0</v>
+        <v>7445</v>
       </c>
       <c r="M13">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f>IF(ISBLANK(N13),-L13,N13-L13)</f>
+        <v>232</v>
       </c>
       <c r="N13" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+        <v>7677</v>
+      </c>
+      <c r="O13">
+        <f>IF(ISBLANK(P13),-N13,P13-N13)</f>
+        <v>-7677</v>
+      </c>
+      <c r="P13" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -5628,230 +5724,265 @@
         <v>3132</v>
       </c>
       <c r="E14">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F14),-D14,F14-D14)</f>
         <v>104</v>
       </c>
       <c r="F14" s="1">
         <v>3236</v>
       </c>
       <c r="G14">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H14),-F14,H14-F14)</f>
         <v>77</v>
       </c>
       <c r="H14" s="1">
         <v>3313</v>
       </c>
       <c r="I14">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J14),-H14,J14-H14)</f>
         <v>13</v>
       </c>
       <c r="J14" s="1">
         <v>3326</v>
       </c>
       <c r="K14">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L14),-J14,L14-J14)</f>
         <v>151</v>
       </c>
       <c r="L14" s="1">
         <v>3477</v>
       </c>
       <c r="M14">
-        <f t="shared" si="4"/>
+        <f>IF(ISBLANK(N14),-L14,N14-L14)</f>
         <v>-3477</v>
       </c>
       <c r="N14" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O14">
+        <f>IF(ISBLANK(P14),-N14,P14-N14)</f>
+        <v>0</v>
+      </c>
+      <c r="P14" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="1">
-        <v>6897</v>
+        <v>2450</v>
       </c>
       <c r="E15">
-        <f t="shared" si="0"/>
-        <v>303</v>
+        <f>IF(ISBLANK(F15),-D15,F15-D15)</f>
+        <v>112</v>
       </c>
       <c r="F15" s="1">
-        <v>7200</v>
+        <v>2562</v>
       </c>
       <c r="G15">
-        <f t="shared" si="1"/>
-        <v>20</v>
+        <f>IF(ISBLANK(H15),-F15,H15-F15)</f>
+        <v>15</v>
       </c>
       <c r="H15" s="1">
-        <v>7220</v>
+        <v>2577</v>
       </c>
       <c r="I15">
-        <f t="shared" si="2"/>
-        <v>84</v>
+        <f>IF(ISBLANK(J15),-H15,J15-H15)</f>
+        <v>77</v>
       </c>
       <c r="J15" s="1">
-        <v>7304</v>
+        <v>2654</v>
       </c>
       <c r="K15">
-        <f t="shared" si="3"/>
-        <v>141</v>
+        <f>IF(ISBLANK(L15),-J15,L15-J15)</f>
+        <v>40</v>
       </c>
       <c r="L15" s="1">
-        <v>7445</v>
+        <v>2694</v>
       </c>
       <c r="M15">
-        <f t="shared" si="4"/>
-        <v>232</v>
+        <f>IF(ISBLANK(N15),-L15,N15-L15)</f>
+        <v>-2694</v>
       </c>
       <c r="N15" s="1">
-        <v>7677</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <f>IF(ISBLANK(P15),-N15,P15-N15)</f>
+        <v>0</v>
+      </c>
+      <c r="P15" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="1">
-        <v>30220</v>
+        <v>1352</v>
       </c>
       <c r="E16">
-        <f t="shared" si="0"/>
-        <v>864</v>
+        <f>IF(ISBLANK(F16),-D16,F16-D16)</f>
+        <v>48</v>
       </c>
       <c r="F16" s="1">
-        <v>31084</v>
+        <v>1400</v>
       </c>
       <c r="G16">
-        <f t="shared" si="1"/>
-        <v>38</v>
+        <f>IF(ISBLANK(H16),-F16,H16-F16)</f>
+        <v>12</v>
       </c>
       <c r="H16" s="1">
-        <v>31122</v>
+        <v>1412</v>
       </c>
       <c r="I16">
-        <f t="shared" si="2"/>
-        <v>21</v>
+        <f>IF(ISBLANK(J16),-H16,J16-H16)</f>
+        <v>-1412</v>
       </c>
       <c r="J16" s="1">
-        <v>31143</v>
+        <v>0</v>
       </c>
       <c r="K16">
-        <f t="shared" si="3"/>
-        <v>55</v>
+        <f>IF(ISBLANK(L16),-J16,L16-J16)</f>
+        <v>0</v>
       </c>
       <c r="L16" s="1">
-        <v>31198</v>
+        <v>0</v>
       </c>
       <c r="M16">
-        <f t="shared" si="4"/>
-        <v>273</v>
+        <f>IF(ISBLANK(N16),-L16,N16-L16)</f>
+        <v>0</v>
       </c>
       <c r="N16" s="1">
-        <v>31471</v>
-      </c>
-    </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <f>IF(ISBLANK(P16),-N16,P16-N16)</f>
+        <v>0</v>
+      </c>
+      <c r="P16" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>202</v>
+        <v>211</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="1">
-        <v>42814</v>
+        <v>1322</v>
       </c>
       <c r="E17">
-        <f t="shared" si="0"/>
-        <v>1226</v>
+        <f>IF(ISBLANK(F17),-D17,F17-D17)</f>
+        <v>53</v>
       </c>
       <c r="F17" s="1">
-        <v>44040</v>
+        <v>1375</v>
       </c>
       <c r="G17">
-        <f t="shared" si="1"/>
-        <v>19</v>
+        <f>IF(ISBLANK(H17),-F17,H17-F17)</f>
+        <v>71</v>
       </c>
       <c r="H17" s="1">
-        <v>44059</v>
+        <v>1446</v>
       </c>
       <c r="I17">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J17),-H17,J17-H17)</f>
+        <v>44</v>
+      </c>
+      <c r="J17" s="1">
+        <v>1490</v>
+      </c>
+      <c r="K17">
+        <f>IF(ISBLANK(L17),-J17,L17-J17)</f>
+        <v>-1490</v>
+      </c>
+      <c r="L17" s="1">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <f>IF(ISBLANK(N17),-L17,N17-L17)</f>
+        <v>0</v>
+      </c>
+      <c r="N17" s="1">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <f>IF(ISBLANK(P17),-N17,P17-N17)</f>
+        <v>0</v>
+      </c>
+      <c r="P17" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A18">
         <v>17</v>
       </c>
-      <c r="J17" s="1">
-        <v>44076</v>
-      </c>
-      <c r="K17">
-        <f t="shared" si="3"/>
-        <v>54</v>
-      </c>
-      <c r="L17" s="1">
-        <v>44130</v>
-      </c>
-      <c r="M17">
-        <f t="shared" si="4"/>
-        <v>125</v>
-      </c>
-      <c r="N17" s="1">
-        <v>44255</v>
-      </c>
-    </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>4</v>
-      </c>
       <c r="B18" t="s">
-        <v>199</v>
+        <v>212</v>
       </c>
       <c r="C18" s="2"/>
-      <c r="D18" s="1">
-        <v>64500</v>
+      <c r="D18">
+        <v>789</v>
       </c>
       <c r="E18">
-        <f t="shared" si="0"/>
-        <v>6036</v>
-      </c>
-      <c r="F18" s="1">
-        <v>70536</v>
+        <f>IF(ISBLANK(F18),-D18,F18-D18)</f>
+        <v>22</v>
+      </c>
+      <c r="F18">
+        <v>811</v>
       </c>
       <c r="G18">
-        <f t="shared" si="1"/>
-        <v>83</v>
+        <f>IF(ISBLANK(H18),-F18,H18-F18)</f>
+        <v>-811</v>
       </c>
       <c r="H18" s="1">
-        <v>70619</v>
+        <v>0</v>
       </c>
       <c r="I18">
-        <f t="shared" si="2"/>
-        <v>41</v>
+        <f>IF(ISBLANK(J18),-H18,J18-H18)</f>
+        <v>0</v>
       </c>
       <c r="J18" s="1">
-        <v>70660</v>
+        <v>0</v>
       </c>
       <c r="K18">
-        <f t="shared" si="3"/>
-        <v>71</v>
+        <f>IF(ISBLANK(L18),-J18,L18-J18)</f>
+        <v>0</v>
       </c>
       <c r="L18" s="1">
-        <v>70731</v>
+        <v>0</v>
       </c>
       <c r="M18">
-        <f t="shared" si="4"/>
-        <v>694</v>
+        <f>IF(ISBLANK(N18),-L18,N18-L18)</f>
+        <v>0</v>
       </c>
       <c r="N18" s="1">
-        <v>71425</v>
-      </c>
-    </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <f>IF(ISBLANK(P18),-N18,P18-N18)</f>
+        <v>0</v>
+      </c>
+      <c r="P18" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>196</v>
       </c>
@@ -5892,28 +6023,52 @@
       <c r="P20" t="s">
         <v>13</v>
       </c>
-      <c r="Y20" t="s">
+      <c r="Q20" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="R20" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z20" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA20" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB20" t="s">
+        <v>10</v>
+      </c>
+      <c r="AC20" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD20" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE20" t="s">
+        <v>13</v>
+      </c>
+      <c r="AF20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>197</v>
       </c>
       <c r="D21">
-        <f t="shared" ref="D21:D36" si="5">FIND(",",B21)</f>
+        <f t="shared" ref="D21:D36" si="0">FIND(",",B21)</f>
         <v>9</v>
       </c>
       <c r="E21" t="str">
-        <f t="shared" ref="E21:E36" si="6">LEFT(B21,D21-1)</f>
+        <f t="shared" ref="E21:E36" si="1">LEFT(B21,D21-1)</f>
         <v>Flanagan</v>
       </c>
       <c r="F21" t="str">
-        <f t="shared" ref="F21:F36" si="7">RIGHT(B21,LEN(B21)-(D21+1))</f>
+        <f t="shared" ref="F21:F36" si="2">RIGHT(B21,LEN(B21)-(D21+1))</f>
         <v>Luke 'Ming'</v>
       </c>
       <c r="G21" t="str">
-        <f t="shared" ref="G21:G36" si="8">F21&amp;" "&amp;E21</f>
+        <f t="shared" ref="G21:G36" si="3">F21&amp;" "&amp;E21</f>
         <v>Luke 'Ming' Flanagan</v>
       </c>
       <c r="J21" t="s">
@@ -5927,25 +6082,31 @@
       </c>
       <c r="S21" s="2"/>
       <c r="T21" s="1"/>
-    </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z21" t="s">
+        <v>239</v>
+      </c>
+      <c r="AA21" s="1">
+        <v>134630</v>
+      </c>
+    </row>
+    <row r="22" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>198</v>
       </c>
       <c r="D22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="E22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>Carthy</v>
       </c>
       <c r="F22" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>Matt</v>
       </c>
       <c r="G22" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>Matt Carthy</v>
       </c>
       <c r="J22" t="s">
@@ -5968,6 +6129,12 @@
       </c>
       <c r="P22" s="1">
         <v>87333</v>
+      </c>
+      <c r="Q22" s="1">
+        <v>87964</v>
+      </c>
+      <c r="R22" s="1">
+        <v>88543</v>
       </c>
       <c r="S22" s="2"/>
       <c r="T22" s="1"/>
@@ -5975,28 +6142,46 @@
       <c r="V22" s="1"/>
       <c r="W22" s="1"/>
       <c r="X22" s="1"/>
-      <c r="Y22" s="1">
+      <c r="Z22" t="s">
+        <v>240</v>
+      </c>
+      <c r="AA22" s="1">
+        <v>85034</v>
+      </c>
+      <c r="AB22" s="1">
+        <v>86906</v>
+      </c>
+      <c r="AC22" s="1">
+        <v>87008</v>
+      </c>
+      <c r="AD22" s="1">
+        <v>87188</v>
+      </c>
+      <c r="AE22" s="1">
+        <v>87333</v>
+      </c>
+      <c r="AF22" s="1">
         <v>87964</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>199</v>
       </c>
       <c r="D23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="E23" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>Walsh</v>
       </c>
       <c r="F23" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>Maria</v>
       </c>
       <c r="G23" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>Maria Walsh</v>
       </c>
       <c r="J23" t="s">
@@ -6019,6 +6204,12 @@
       </c>
       <c r="P23" s="1">
         <v>78653</v>
+      </c>
+      <c r="Q23" s="1">
+        <v>79028</v>
+      </c>
+      <c r="R23" s="1">
+        <v>79437</v>
       </c>
       <c r="S23" s="2"/>
       <c r="T23" s="1"/>
@@ -6026,28 +6217,46 @@
       <c r="V23" s="1"/>
       <c r="W23" s="1"/>
       <c r="X23" s="1"/>
-      <c r="Y23" s="1">
+      <c r="Z23" t="s">
+        <v>241</v>
+      </c>
+      <c r="AA23" s="1">
+        <v>77619</v>
+      </c>
+      <c r="AB23" s="1">
+        <v>78487</v>
+      </c>
+      <c r="AC23" s="1">
+        <v>78513</v>
+      </c>
+      <c r="AD23" s="1">
+        <v>78612</v>
+      </c>
+      <c r="AE23" s="1">
+        <v>78653</v>
+      </c>
+      <c r="AF23" s="1">
         <v>79028</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>200</v>
       </c>
       <c r="D24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="E24" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>Casey</v>
       </c>
       <c r="F24" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>Peter</v>
       </c>
       <c r="G24" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>Peter Casey</v>
       </c>
       <c r="J24" t="s">
@@ -6070,6 +6279,12 @@
       </c>
       <c r="P24" s="1">
         <v>70731</v>
+      </c>
+      <c r="Q24" s="1">
+        <v>71425</v>
+      </c>
+      <c r="R24" s="1">
+        <v>71793</v>
       </c>
       <c r="S24" s="2"/>
       <c r="T24" s="1"/>
@@ -6077,28 +6292,46 @@
       <c r="V24" s="1"/>
       <c r="W24" s="1"/>
       <c r="X24" s="1"/>
-      <c r="Y24" s="1">
+      <c r="Z24" t="s">
+        <v>242</v>
+      </c>
+      <c r="AA24" s="1">
+        <v>64500</v>
+      </c>
+      <c r="AB24" s="1">
+        <v>70536</v>
+      </c>
+      <c r="AC24" s="1">
+        <v>70619</v>
+      </c>
+      <c r="AD24" s="1">
+        <v>70660</v>
+      </c>
+      <c r="AE24" s="1">
+        <v>70731</v>
+      </c>
+      <c r="AF24" s="1">
         <v>71425</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>201</v>
       </c>
       <c r="D25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="E25" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>McHugh</v>
       </c>
       <c r="F25" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>Saoirse</v>
       </c>
       <c r="G25" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>Saoirse McHugh</v>
       </c>
       <c r="J25" t="s">
@@ -6121,6 +6354,12 @@
       </c>
       <c r="P25" s="1">
         <v>58212</v>
+      </c>
+      <c r="Q25" s="1">
+        <v>58602</v>
+      </c>
+      <c r="R25" s="1">
+        <v>59635</v>
       </c>
       <c r="S25" s="2"/>
       <c r="T25" s="1"/>
@@ -6128,28 +6367,46 @@
       <c r="V25" s="1"/>
       <c r="W25" s="1"/>
       <c r="X25" s="1"/>
-      <c r="Y25" s="1">
+      <c r="Z25" t="s">
+        <v>243</v>
+      </c>
+      <c r="AA25" s="1">
+        <v>56650</v>
+      </c>
+      <c r="AB25" s="1">
+        <v>57848</v>
+      </c>
+      <c r="AC25" s="1">
+        <v>57892</v>
+      </c>
+      <c r="AD25" s="1">
+        <v>58034</v>
+      </c>
+      <c r="AE25" s="1">
+        <v>58212</v>
+      </c>
+      <c r="AF25" s="1">
         <v>58602</v>
       </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>202</v>
       </c>
       <c r="D26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="E26" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>Smith</v>
       </c>
       <c r="F26" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>Brendan</v>
       </c>
       <c r="G26" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>Brendan Smith</v>
       </c>
       <c r="J26" t="s">
@@ -6172,6 +6429,12 @@
       </c>
       <c r="P26" s="1">
         <v>53068</v>
+      </c>
+      <c r="Q26" s="1">
+        <v>53966</v>
+      </c>
+      <c r="R26" s="1">
+        <v>54548</v>
       </c>
       <c r="S26" s="2"/>
       <c r="T26" s="1"/>
@@ -6179,28 +6442,46 @@
       <c r="V26" s="1"/>
       <c r="W26" s="1"/>
       <c r="X26" s="1"/>
-      <c r="Y26" s="1">
+      <c r="Z26" t="s">
+        <v>244</v>
+      </c>
+      <c r="AA26" s="1">
+        <v>51019</v>
+      </c>
+      <c r="AB26" s="1">
+        <v>52731</v>
+      </c>
+      <c r="AC26" s="1">
+        <v>52821</v>
+      </c>
+      <c r="AD26" s="1">
+        <v>52976</v>
+      </c>
+      <c r="AE26" s="1">
+        <v>53068</v>
+      </c>
+      <c r="AF26" s="1">
         <v>53966</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>203</v>
       </c>
       <c r="D27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="E27" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>Rabbitte</v>
       </c>
       <c r="F27" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>Anne</v>
       </c>
       <c r="G27" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>Anne Rabbitte</v>
       </c>
       <c r="J27" t="s">
@@ -6223,6 +6504,12 @@
       </c>
       <c r="P27" s="1">
         <v>44130</v>
+      </c>
+      <c r="Q27" s="1">
+        <v>44255</v>
+      </c>
+      <c r="R27" s="1">
+        <v>44692</v>
       </c>
       <c r="S27" s="2"/>
       <c r="T27" s="1"/>
@@ -6230,28 +6517,46 @@
       <c r="V27" s="1"/>
       <c r="W27" s="1"/>
       <c r="X27" s="1"/>
-      <c r="Y27" s="1">
+      <c r="Z27" t="s">
+        <v>245</v>
+      </c>
+      <c r="AA27" s="1">
+        <v>42814</v>
+      </c>
+      <c r="AB27" s="1">
+        <v>44040</v>
+      </c>
+      <c r="AC27" s="1">
+        <v>44059</v>
+      </c>
+      <c r="AD27" s="1">
+        <v>44076</v>
+      </c>
+      <c r="AE27" s="1">
+        <v>44130</v>
+      </c>
+      <c r="AF27" s="1">
         <v>44255</v>
       </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>204</v>
       </c>
       <c r="D28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="E28" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>Healy Eames</v>
       </c>
       <c r="F28" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>Fidelma</v>
       </c>
       <c r="G28" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>Fidelma Healy Eames</v>
       </c>
       <c r="J28" t="s">
@@ -6274,6 +6579,12 @@
       </c>
       <c r="P28" s="1">
         <v>31198</v>
+      </c>
+      <c r="Q28" s="1">
+        <v>31471</v>
+      </c>
+      <c r="R28" s="1">
+        <v>31893</v>
       </c>
       <c r="S28" s="2"/>
       <c r="T28" s="1"/>
@@ -6281,28 +6592,46 @@
       <c r="V28" s="1"/>
       <c r="W28" s="1"/>
       <c r="X28" s="1"/>
-      <c r="Y28" s="1">
+      <c r="Z28" t="s">
+        <v>246</v>
+      </c>
+      <c r="AA28" s="1">
+        <v>30220</v>
+      </c>
+      <c r="AB28" s="1">
+        <v>31084</v>
+      </c>
+      <c r="AC28" s="1">
+        <v>31122</v>
+      </c>
+      <c r="AD28" s="1">
+        <v>31143</v>
+      </c>
+      <c r="AE28" s="1">
+        <v>31198</v>
+      </c>
+      <c r="AF28" s="1">
         <v>31471</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>205</v>
       </c>
       <c r="D29">
-        <f t="shared" si="5"/>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="E29" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>Hannigan</v>
       </c>
       <c r="F29" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>Dominic</v>
       </c>
       <c r="G29" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>Dominic Hannigan</v>
       </c>
       <c r="J29" t="s">
@@ -6325,6 +6654,12 @@
       </c>
       <c r="P29" s="1">
         <v>16764</v>
+      </c>
+      <c r="Q29" s="1">
+        <v>17590</v>
+      </c>
+      <c r="R29" s="1">
+        <v>19312</v>
       </c>
       <c r="S29" s="2"/>
       <c r="T29" s="1"/>
@@ -6332,28 +6667,46 @@
       <c r="V29" s="1"/>
       <c r="W29" s="1"/>
       <c r="X29" s="1"/>
-      <c r="Y29" s="1">
+      <c r="Z29" t="s">
+        <v>247</v>
+      </c>
+      <c r="AA29" s="1">
+        <v>15991</v>
+      </c>
+      <c r="AB29" s="1">
+        <v>16468</v>
+      </c>
+      <c r="AC29" s="1">
+        <v>16515</v>
+      </c>
+      <c r="AD29" s="1">
+        <v>16621</v>
+      </c>
+      <c r="AE29" s="1">
+        <v>16764</v>
+      </c>
+      <c r="AF29" s="1">
         <v>17590</v>
       </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>206</v>
       </c>
       <c r="D30">
-        <f t="shared" si="5"/>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="E30" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>Brennan</v>
       </c>
       <c r="F30" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>Cyril</v>
       </c>
       <c r="G30" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>Cyril Brennan</v>
       </c>
       <c r="J30" t="s">
@@ -6376,6 +6729,12 @@
       </c>
       <c r="P30" s="1">
         <v>13197</v>
+      </c>
+      <c r="Q30" s="1">
+        <v>13408</v>
+      </c>
+      <c r="R30" s="1">
+        <v>13723</v>
       </c>
       <c r="S30" s="2"/>
       <c r="T30" s="1"/>
@@ -6383,28 +6742,46 @@
       <c r="V30" s="1"/>
       <c r="W30" s="1"/>
       <c r="X30" s="1"/>
-      <c r="Y30" s="1">
+      <c r="Z30" t="s">
+        <v>248</v>
+      </c>
+      <c r="AA30" s="1">
+        <v>12378</v>
+      </c>
+      <c r="AB30" s="1">
+        <v>13031</v>
+      </c>
+      <c r="AC30" s="1">
+        <v>13065</v>
+      </c>
+      <c r="AD30" s="1">
+        <v>13150</v>
+      </c>
+      <c r="AE30" s="1">
+        <v>13197</v>
+      </c>
+      <c r="AF30" s="1">
         <v>13408</v>
       </c>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>207</v>
       </c>
       <c r="D31">
-        <f t="shared" si="5"/>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="E31" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>O'Dowd</v>
       </c>
       <c r="F31" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>Michael</v>
       </c>
       <c r="G31" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>Michael O'Dowd</v>
       </c>
       <c r="J31" t="s">
@@ -6427,6 +6804,12 @@
       </c>
       <c r="P31" s="1">
         <v>8365</v>
+      </c>
+      <c r="Q31" s="1">
+        <v>8553</v>
+      </c>
+      <c r="R31" s="1">
+        <v>8699</v>
       </c>
       <c r="S31" s="2"/>
       <c r="T31" s="1"/>
@@ -6434,28 +6817,46 @@
       <c r="V31" s="1"/>
       <c r="W31" s="1"/>
       <c r="X31" s="1"/>
-      <c r="Y31" s="1">
+      <c r="Z31" t="s">
+        <v>260</v>
+      </c>
+      <c r="AA31" s="1">
+        <v>8130</v>
+      </c>
+      <c r="AB31" s="1">
+        <v>8226</v>
+      </c>
+      <c r="AC31" s="1">
+        <v>8246</v>
+      </c>
+      <c r="AD31" s="1">
+        <v>8337</v>
+      </c>
+      <c r="AE31" s="1">
+        <v>8365</v>
+      </c>
+      <c r="AF31" s="1">
         <v>8553</v>
       </c>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>208</v>
       </c>
       <c r="D32">
-        <f t="shared" si="5"/>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="E32" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>O'Connor</v>
       </c>
       <c r="F32" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>Olive</v>
       </c>
       <c r="G32" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>Olive O'Connor</v>
       </c>
       <c r="J32" t="s">
@@ -6478,6 +6879,9 @@
       </c>
       <c r="P32" s="1">
         <v>7445</v>
+      </c>
+      <c r="Q32" s="1">
+        <v>7677</v>
       </c>
       <c r="S32" s="2"/>
       <c r="T32" s="1"/>
@@ -6485,28 +6889,46 @@
       <c r="V32" s="1"/>
       <c r="W32" s="1"/>
       <c r="X32" s="1"/>
-      <c r="Y32" s="1">
+      <c r="Z32" t="s">
+        <v>261</v>
+      </c>
+      <c r="AA32" s="1">
+        <v>6897</v>
+      </c>
+      <c r="AB32" s="1">
+        <v>7200</v>
+      </c>
+      <c r="AC32" s="1">
+        <v>7220</v>
+      </c>
+      <c r="AD32" s="1">
+        <v>7304</v>
+      </c>
+      <c r="AE32" s="1">
+        <v>7445</v>
+      </c>
+      <c r="AF32" s="1">
         <v>7677</v>
       </c>
     </row>
-    <row r="33" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>209</v>
       </c>
       <c r="D33">
-        <f t="shared" si="5"/>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="E33" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>Mahapatra</v>
       </c>
       <c r="F33" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>Dilip</v>
       </c>
       <c r="G33" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>Dilip Mahapatra</v>
       </c>
       <c r="J33" t="s">
@@ -6536,25 +6958,43 @@
       <c r="V33" s="1"/>
       <c r="W33" s="1"/>
       <c r="X33" s="1"/>
-    </row>
-    <row r="34" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="Z33" t="s">
+        <v>251</v>
+      </c>
+      <c r="AA33" s="1">
+        <v>3132</v>
+      </c>
+      <c r="AB33" s="1">
+        <v>3236</v>
+      </c>
+      <c r="AC33" s="1">
+        <v>3313</v>
+      </c>
+      <c r="AD33" s="1">
+        <v>3326</v>
+      </c>
+      <c r="AE33" s="1">
+        <v>3477</v>
+      </c>
+    </row>
+    <row r="34" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>210</v>
       </c>
       <c r="D34">
-        <f t="shared" si="5"/>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="E34" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>Greene</v>
       </c>
       <c r="F34" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>Patrick</v>
       </c>
       <c r="G34" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>Patrick Greene</v>
       </c>
       <c r="J34" t="s">
@@ -6584,25 +7024,43 @@
       <c r="V34" s="1"/>
       <c r="W34" s="1"/>
       <c r="X34" s="1"/>
-    </row>
-    <row r="35" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="Z34" t="s">
+        <v>252</v>
+      </c>
+      <c r="AA34" s="1">
+        <v>2450</v>
+      </c>
+      <c r="AB34" s="1">
+        <v>2562</v>
+      </c>
+      <c r="AC34" s="1">
+        <v>2577</v>
+      </c>
+      <c r="AD34" s="1">
+        <v>2654</v>
+      </c>
+      <c r="AE34" s="1">
+        <v>2694</v>
+      </c>
+    </row>
+    <row r="35" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>211</v>
       </c>
       <c r="D35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="E35" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>Miller</v>
       </c>
       <c r="F35" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>James</v>
       </c>
       <c r="G35" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>James Miller</v>
       </c>
       <c r="J35" t="s">
@@ -6624,25 +7082,37 @@
       <c r="T35" s="1"/>
       <c r="U35" s="1"/>
       <c r="V35" s="1"/>
-    </row>
-    <row r="36" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="Z35" t="s">
+        <v>253</v>
+      </c>
+      <c r="AA35" s="1">
+        <v>1352</v>
+      </c>
+      <c r="AB35" s="1">
+        <v>1400</v>
+      </c>
+      <c r="AC35" s="1">
+        <v>1412</v>
+      </c>
+    </row>
+    <row r="36" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>212</v>
       </c>
       <c r="D36">
-        <f t="shared" si="5"/>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="E36" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>Mulcahy</v>
       </c>
       <c r="F36" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>Diarmaid</v>
       </c>
       <c r="G36" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>Diarmaid Mulcahy</v>
       </c>
       <c r="J36" t="s">
@@ -6668,8 +7138,23 @@
       <c r="U36" s="1"/>
       <c r="V36" s="1"/>
       <c r="W36" s="1"/>
-    </row>
-    <row r="37" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="Z36" t="s">
+        <v>254</v>
+      </c>
+      <c r="AA36" s="1">
+        <v>1322</v>
+      </c>
+      <c r="AB36" s="1">
+        <v>1375</v>
+      </c>
+      <c r="AC36" s="1">
+        <v>1446</v>
+      </c>
+      <c r="AD36" s="1">
+        <v>1490</v>
+      </c>
+    </row>
+    <row r="37" spans="2:31" x14ac:dyDescent="0.25">
       <c r="J37" t="s">
         <v>255</v>
       </c>
@@ -6683,10 +7168,19 @@
         <v>811</v>
       </c>
       <c r="S37" s="2"/>
+      <c r="Z37" t="s">
+        <v>255</v>
+      </c>
+      <c r="AA37">
+        <v>789</v>
+      </c>
+      <c r="AB37">
+        <v>811</v>
+      </c>
     </row>
   </sheetData>
-  <sortState ref="A2:N18">
-    <sortCondition ref="B2:B18"/>
+  <sortState ref="A2:P18">
+    <sortCondition ref="A2:A18"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6696,7 +7190,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+    <sheetView topLeftCell="N1" workbookViewId="0">
       <selection activeCell="S2" sqref="S2:T24"/>
     </sheetView>
   </sheetViews>
@@ -6767,56 +7261,56 @@
         <v>4665</v>
       </c>
       <c r="E2">
-        <f>IF(ISBLANK(F2),-D2,F2-D2)</f>
+        <f t="shared" ref="E2:E24" si="0">IF(ISBLANK(F2),-D2,F2-D2)</f>
         <v>26</v>
       </c>
       <c r="F2" s="1">
         <v>4691</v>
       </c>
       <c r="G2">
-        <f>IF(ISBLANK(H2),-F2,H2-F2)</f>
+        <f t="shared" ref="G2:G24" si="1">IF(ISBLANK(H2),-F2,H2-F2)</f>
         <v>43</v>
       </c>
       <c r="H2" s="1">
         <v>4734</v>
       </c>
       <c r="I2">
-        <f>IF(ISBLANK(J2),-H2,J2-H2)</f>
+        <f t="shared" ref="I2:I24" si="2">IF(ISBLANK(J2),-H2,J2-H2)</f>
         <v>57</v>
       </c>
       <c r="J2" s="1">
         <v>4791</v>
       </c>
       <c r="K2">
-        <f>IF(ISBLANK(L2),-J2,L2-J2)</f>
+        <f t="shared" ref="K2:K24" si="3">IF(ISBLANK(L2),-J2,L2-J2)</f>
         <v>50</v>
       </c>
       <c r="L2" s="1">
         <v>4841</v>
       </c>
       <c r="M2">
-        <f>IF(ISBLANK(N2),-L2,N2-L2)</f>
+        <f t="shared" ref="M2:M24" si="4">IF(ISBLANK(N2),-L2,N2-L2)</f>
         <v>115</v>
       </c>
       <c r="N2" s="1">
         <v>4956</v>
       </c>
       <c r="O2">
-        <f>IF(ISBLANK(P2),-N2,P2-N2)</f>
+        <f t="shared" ref="O2:O24" si="5">IF(ISBLANK(P2),-N2,P2-N2)</f>
         <v>72</v>
       </c>
       <c r="P2" s="1">
         <v>5028</v>
       </c>
       <c r="Q2">
-        <f>IF(ISBLANK(R2),-P2,R2-P2)</f>
+        <f t="shared" ref="Q2:Q24" si="6">IF(ISBLANK(R2),-P2,R2-P2)</f>
         <v>104</v>
       </c>
       <c r="R2" s="1">
         <v>5132</v>
       </c>
       <c r="S2">
-        <f>IF(ISBLANK(T2),-R2,T2-R2)</f>
+        <f t="shared" ref="S2:S24" si="7">IF(ISBLANK(T2),-R2,T2-R2)</f>
         <v>-5132</v>
       </c>
       <c r="T2" s="1">
@@ -6834,56 +7328,56 @@
         <v>69166</v>
       </c>
       <c r="E3">
-        <f>IF(ISBLANK(F3),-D3,F3-D3)</f>
+        <f t="shared" si="0"/>
         <v>35</v>
       </c>
       <c r="F3" s="1">
         <v>69201</v>
       </c>
       <c r="G3">
-        <f>IF(ISBLANK(H3),-F3,H3-F3)</f>
+        <f t="shared" si="1"/>
         <v>71</v>
       </c>
       <c r="H3" s="1">
         <v>69272</v>
       </c>
       <c r="I3">
-        <f>IF(ISBLANK(J3),-H3,J3-H3)</f>
+        <f t="shared" si="2"/>
         <v>44</v>
       </c>
       <c r="J3" s="1">
         <v>69316</v>
       </c>
       <c r="K3">
-        <f>IF(ISBLANK(L3),-J3,L3-J3)</f>
+        <f t="shared" si="3"/>
         <v>66</v>
       </c>
       <c r="L3" s="1">
         <v>69382</v>
       </c>
       <c r="M3">
-        <f>IF(ISBLANK(N3),-L3,N3-L3)</f>
+        <f t="shared" si="4"/>
         <v>129</v>
       </c>
       <c r="N3" s="1">
         <v>69511</v>
       </c>
       <c r="O3">
-        <f>IF(ISBLANK(P3),-N3,P3-N3)</f>
+        <f t="shared" si="5"/>
         <v>45</v>
       </c>
       <c r="P3" s="1">
         <v>69556</v>
       </c>
       <c r="Q3">
-        <f>IF(ISBLANK(R3),-P3,R3-P3)</f>
+        <f t="shared" si="6"/>
         <v>116</v>
       </c>
       <c r="R3" s="1">
         <v>69672</v>
       </c>
       <c r="S3">
-        <f>IF(ISBLANK(T3),-R3,T3-R3)</f>
+        <f t="shared" si="7"/>
         <v>1226</v>
       </c>
       <c r="T3" s="1">
@@ -6901,56 +7395,56 @@
         <v>10582</v>
       </c>
       <c r="E4">
-        <f>IF(ISBLANK(F4),-D4,F4-D4)</f>
+        <f t="shared" si="0"/>
         <v>57</v>
       </c>
       <c r="F4" s="1">
         <v>10639</v>
       </c>
       <c r="G4">
-        <f>IF(ISBLANK(H4),-F4,H4-F4)</f>
+        <f t="shared" si="1"/>
         <v>106</v>
       </c>
       <c r="H4" s="1">
         <v>10745</v>
       </c>
       <c r="I4">
-        <f>IF(ISBLANK(J4),-H4,J4-H4)</f>
+        <f t="shared" si="2"/>
         <v>138</v>
       </c>
       <c r="J4" s="1">
         <v>10883</v>
       </c>
       <c r="K4">
-        <f>IF(ISBLANK(L4),-J4,L4-J4)</f>
+        <f t="shared" si="3"/>
         <v>54</v>
       </c>
       <c r="L4" s="1">
         <v>10937</v>
       </c>
       <c r="M4">
-        <f>IF(ISBLANK(N4),-L4,N4-L4)</f>
+        <f t="shared" si="4"/>
         <v>300</v>
       </c>
       <c r="N4" s="1">
         <v>11237</v>
       </c>
       <c r="O4">
-        <f>IF(ISBLANK(P4),-N4,P4-N4)</f>
+        <f t="shared" si="5"/>
         <v>159</v>
       </c>
       <c r="P4" s="1">
         <v>11396</v>
       </c>
       <c r="Q4">
-        <f>IF(ISBLANK(R4),-P4,R4-P4)</f>
+        <f t="shared" si="6"/>
         <v>322</v>
       </c>
       <c r="R4" s="1">
         <v>11718</v>
       </c>
       <c r="S4">
-        <f>IF(ISBLANK(T4),-R4,T4-R4)</f>
+        <f t="shared" si="7"/>
         <v>908</v>
       </c>
       <c r="T4" s="1">
@@ -6968,56 +7462,56 @@
         <v>64605</v>
       </c>
       <c r="E5">
-        <f>IF(ISBLANK(F5),-D5,F5-D5)</f>
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="F5" s="1">
         <v>64631</v>
       </c>
       <c r="G5">
-        <f>IF(ISBLANK(H5),-F5,H5-F5)</f>
+        <f t="shared" si="1"/>
         <v>61</v>
       </c>
       <c r="H5" s="1">
         <v>64692</v>
       </c>
       <c r="I5">
-        <f>IF(ISBLANK(J5),-H5,J5-H5)</f>
+        <f t="shared" si="2"/>
         <v>71</v>
       </c>
       <c r="J5" s="1">
         <v>64763</v>
       </c>
       <c r="K5">
-        <f>IF(ISBLANK(L5),-J5,L5-J5)</f>
+        <f t="shared" si="3"/>
         <v>136</v>
       </c>
       <c r="L5" s="1">
         <v>64899</v>
       </c>
       <c r="M5">
-        <f>IF(ISBLANK(N5),-L5,N5-L5)</f>
+        <f t="shared" si="4"/>
         <v>106</v>
       </c>
       <c r="N5" s="1">
         <v>65005</v>
       </c>
       <c r="O5">
-        <f>IF(ISBLANK(P5),-N5,P5-N5)</f>
+        <f t="shared" si="5"/>
         <v>110</v>
       </c>
       <c r="P5" s="1">
         <v>65115</v>
       </c>
       <c r="Q5">
-        <f>IF(ISBLANK(R5),-P5,R5-P5)</f>
+        <f t="shared" si="6"/>
         <v>137</v>
       </c>
       <c r="R5" s="1">
         <v>65252</v>
       </c>
       <c r="S5">
-        <f>IF(ISBLANK(T5),-R5,T5-R5)</f>
+        <f t="shared" si="7"/>
         <v>306</v>
       </c>
       <c r="T5" s="1">
@@ -7035,56 +7529,56 @@
         <v>38738</v>
       </c>
       <c r="E6">
-        <f>IF(ISBLANK(F6),-D6,F6-D6)</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="F6" s="1">
         <v>38755</v>
       </c>
       <c r="G6">
-        <f>IF(ISBLANK(H6),-F6,H6-F6)</f>
+        <f t="shared" si="1"/>
         <v>33</v>
       </c>
       <c r="H6" s="1">
         <v>38788</v>
       </c>
       <c r="I6">
-        <f>IF(ISBLANK(J6),-H6,J6-H6)</f>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="J6" s="1">
         <v>38804</v>
       </c>
       <c r="K6">
-        <f>IF(ISBLANK(L6),-J6,L6-J6)</f>
+        <f t="shared" si="3"/>
         <v>38</v>
       </c>
       <c r="L6" s="1">
         <v>38842</v>
       </c>
       <c r="M6">
-        <f>IF(ISBLANK(N6),-L6,N6-L6)</f>
+        <f t="shared" si="4"/>
         <v>84</v>
       </c>
       <c r="N6" s="1">
         <v>38926</v>
       </c>
       <c r="O6">
-        <f>IF(ISBLANK(P6),-N6,P6-N6)</f>
+        <f t="shared" si="5"/>
         <v>24</v>
       </c>
       <c r="P6" s="1">
         <v>38950</v>
       </c>
       <c r="Q6">
-        <f>IF(ISBLANK(R6),-P6,R6-P6)</f>
+        <f t="shared" si="6"/>
         <v>46</v>
       </c>
       <c r="R6" s="1">
         <v>38996</v>
       </c>
       <c r="S6">
-        <f>IF(ISBLANK(T6),-R6,T6-R6)</f>
+        <f t="shared" si="7"/>
         <v>298</v>
       </c>
       <c r="T6" s="1">
@@ -7102,56 +7596,56 @@
         <v>3182</v>
       </c>
       <c r="E7">
-        <f>IF(ISBLANK(F7),-D7,F7-D7)</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="F7" s="1">
         <v>3197</v>
       </c>
       <c r="G7">
-        <f>IF(ISBLANK(H7),-F7,H7-F7)</f>
+        <f t="shared" si="1"/>
         <v>60</v>
       </c>
       <c r="H7" s="1">
         <v>3257</v>
       </c>
       <c r="I7">
-        <f>IF(ISBLANK(J7),-H7,J7-H7)</f>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="J7" s="1">
         <v>3300</v>
       </c>
       <c r="K7">
-        <f>IF(ISBLANK(L7),-J7,L7-J7)</f>
+        <f t="shared" si="3"/>
         <v>32</v>
       </c>
       <c r="L7" s="1">
         <v>3332</v>
       </c>
       <c r="M7">
-        <f>IF(ISBLANK(N7),-L7,N7-L7)</f>
+        <f t="shared" si="4"/>
         <v>-3332</v>
       </c>
       <c r="N7" s="1">
         <v>0</v>
       </c>
       <c r="O7">
-        <f>IF(ISBLANK(P7),-N7,P7-N7)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P7" s="1">
         <v>0</v>
       </c>
       <c r="Q7">
-        <f>IF(ISBLANK(R7),-P7,R7-P7)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="R7" s="1">
         <v>0</v>
       </c>
       <c r="S7">
-        <f>IF(ISBLANK(T7),-R7,T7-R7)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="T7" s="1">
@@ -7169,56 +7663,56 @@
         <v>9306</v>
       </c>
       <c r="E8">
-        <f>IF(ISBLANK(F8),-D8,F8-D8)</f>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="F8" s="1">
         <v>9331</v>
       </c>
       <c r="G8">
-        <f>IF(ISBLANK(H8),-F8,H8-F8)</f>
+        <f t="shared" si="1"/>
         <v>70</v>
       </c>
       <c r="H8" s="1">
         <v>9401</v>
       </c>
       <c r="I8">
-        <f>IF(ISBLANK(J8),-H8,J8-H8)</f>
+        <f t="shared" si="2"/>
         <v>35</v>
       </c>
       <c r="J8" s="1">
         <v>9436</v>
       </c>
       <c r="K8">
-        <f>IF(ISBLANK(L8),-J8,L8-J8)</f>
+        <f t="shared" si="3"/>
         <v>60</v>
       </c>
       <c r="L8" s="1">
         <v>9496</v>
       </c>
       <c r="M8">
-        <f>IF(ISBLANK(N8),-L8,N8-L8)</f>
+        <f t="shared" si="4"/>
         <v>228</v>
       </c>
       <c r="N8" s="1">
         <v>9724</v>
       </c>
       <c r="O8">
-        <f>IF(ISBLANK(P8),-N8,P8-N8)</f>
+        <f t="shared" si="5"/>
         <v>145</v>
       </c>
       <c r="P8" s="1">
         <v>9869</v>
       </c>
       <c r="Q8">
-        <f>IF(ISBLANK(R8),-P8,R8-P8)</f>
+        <f t="shared" si="6"/>
         <v>106</v>
       </c>
       <c r="R8" s="1">
         <v>9975</v>
       </c>
       <c r="S8">
-        <f>IF(ISBLANK(T8),-R8,T8-R8)</f>
+        <f t="shared" si="7"/>
         <v>247</v>
       </c>
       <c r="T8" s="1">
@@ -7236,56 +7730,56 @@
         <v>7475</v>
       </c>
       <c r="E9">
-        <f>IF(ISBLANK(F9),-D9,F9-D9)</f>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="F9" s="1">
         <v>7498</v>
       </c>
       <c r="G9">
-        <f>IF(ISBLANK(H9),-F9,H9-F9)</f>
+        <f t="shared" si="1"/>
         <v>98</v>
       </c>
       <c r="H9" s="1">
         <v>7596</v>
       </c>
       <c r="I9">
-        <f>IF(ISBLANK(J9),-H9,J9-H9)</f>
+        <f t="shared" si="2"/>
         <v>142</v>
       </c>
       <c r="J9" s="1">
         <v>7738</v>
       </c>
       <c r="K9">
-        <f>IF(ISBLANK(L9),-J9,L9-J9)</f>
+        <f t="shared" si="3"/>
         <v>70</v>
       </c>
       <c r="L9" s="1">
         <v>7808</v>
       </c>
       <c r="M9">
-        <f>IF(ISBLANK(N9),-L9,N9-L9)</f>
+        <f t="shared" si="4"/>
         <v>197</v>
       </c>
       <c r="N9" s="1">
         <v>8005</v>
       </c>
       <c r="O9">
-        <f>IF(ISBLANK(P9),-N9,P9-N9)</f>
+        <f t="shared" si="5"/>
         <v>192</v>
       </c>
       <c r="P9" s="1">
         <v>8197</v>
       </c>
       <c r="Q9">
-        <f>IF(ISBLANK(R9),-P9,R9-P9)</f>
+        <f t="shared" si="6"/>
         <v>176</v>
       </c>
       <c r="R9" s="1">
         <v>8373</v>
       </c>
       <c r="S9">
-        <f>IF(ISBLANK(T9),-R9,T9-R9)</f>
+        <f t="shared" si="7"/>
         <v>188</v>
       </c>
       <c r="T9" s="1">
@@ -7303,56 +7797,56 @@
         <v>84083</v>
       </c>
       <c r="E10">
-        <f>IF(ISBLANK(F10),-D10,F10-D10)</f>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="F10" s="1">
         <v>84106</v>
       </c>
       <c r="G10">
-        <f>IF(ISBLANK(H10),-F10,H10-F10)</f>
+        <f t="shared" si="1"/>
         <v>58</v>
       </c>
       <c r="H10" s="1">
         <v>84164</v>
       </c>
       <c r="I10">
-        <f>IF(ISBLANK(J10),-H10,J10-H10)</f>
+        <f t="shared" si="2"/>
         <v>74</v>
       </c>
       <c r="J10" s="1">
         <v>84238</v>
       </c>
       <c r="K10">
-        <f>IF(ISBLANK(L10),-J10,L10-J10)</f>
+        <f t="shared" si="3"/>
         <v>150</v>
       </c>
       <c r="L10" s="1">
         <v>84388</v>
       </c>
       <c r="M10">
-        <f>IF(ISBLANK(N10),-L10,N10-L10)</f>
+        <f t="shared" si="4"/>
         <v>171</v>
       </c>
       <c r="N10" s="1">
         <v>84559</v>
       </c>
       <c r="O10">
-        <f>IF(ISBLANK(P10),-N10,P10-N10)</f>
+        <f t="shared" si="5"/>
         <v>95</v>
       </c>
       <c r="P10" s="1">
         <v>84654</v>
       </c>
       <c r="Q10">
-        <f>IF(ISBLANK(R10),-P10,R10-P10)</f>
+        <f t="shared" si="6"/>
         <v>187</v>
       </c>
       <c r="R10" s="1">
         <v>84841</v>
       </c>
       <c r="S10">
-        <f>IF(ISBLANK(T10),-R10,T10-R10)</f>
+        <f t="shared" si="7"/>
         <v>130</v>
       </c>
       <c r="T10" s="1">
@@ -7370,56 +7864,56 @@
         <v>118444</v>
       </c>
       <c r="E11">
-        <f>IF(ISBLANK(F11),-D11,F11-D11)</f>
+        <f t="shared" si="0"/>
         <v>45</v>
       </c>
       <c r="F11" s="1">
         <v>118489</v>
       </c>
       <c r="G11">
-        <f>IF(ISBLANK(H11),-F11,H11-F11)</f>
+        <f t="shared" si="1"/>
         <v>186</v>
       </c>
       <c r="H11" s="1">
         <v>118675</v>
       </c>
       <c r="I11">
-        <f>IF(ISBLANK(J11),-H11,J11-H11)</f>
+        <f t="shared" si="2"/>
         <v>98</v>
       </c>
       <c r="J11" s="1">
         <v>118773</v>
       </c>
       <c r="K11">
-        <f>IF(ISBLANK(L11),-J11,L11-J11)</f>
+        <f t="shared" si="3"/>
         <v>350</v>
       </c>
       <c r="L11" s="1">
         <v>119123</v>
       </c>
       <c r="M11">
-        <f>IF(ISBLANK(N11),-L11,N11-L11)</f>
+        <f t="shared" si="4"/>
         <v>257</v>
       </c>
       <c r="N11" s="1">
         <v>119380</v>
       </c>
       <c r="O11">
-        <f>IF(ISBLANK(P11),-N11,P11-N11)</f>
+        <f t="shared" si="5"/>
         <v>165</v>
       </c>
       <c r="P11" s="1">
         <v>119545</v>
       </c>
       <c r="Q11">
-        <f>IF(ISBLANK(R11),-P11,R11-P11)</f>
+        <f t="shared" si="6"/>
         <v>170</v>
       </c>
       <c r="R11" s="1">
         <v>119715</v>
       </c>
       <c r="S11">
-        <f>IF(ISBLANK(T11),-R11,T11-R11)</f>
+        <f t="shared" si="7"/>
         <v>168</v>
       </c>
       <c r="T11" s="1">
@@ -7437,56 +7931,56 @@
         <v>2395</v>
       </c>
       <c r="E12">
-        <f>IF(ISBLANK(F12),-D12,F12-D12)</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="F12" s="1">
         <v>2409</v>
       </c>
       <c r="G12">
-        <f>IF(ISBLANK(H12),-F12,H12-F12)</f>
+        <f t="shared" si="1"/>
         <v>-2409</v>
       </c>
       <c r="H12" s="1">
         <v>0</v>
       </c>
       <c r="I12">
-        <f>IF(ISBLANK(J12),-H12,J12-H12)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J12" s="1">
         <v>0</v>
       </c>
       <c r="K12">
-        <f>IF(ISBLANK(L12),-J12,L12-J12)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L12" s="1">
         <v>0</v>
       </c>
       <c r="M12">
-        <f>IF(ISBLANK(N12),-L12,N12-L12)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N12" s="1">
         <v>0</v>
       </c>
       <c r="O12">
-        <f>IF(ISBLANK(P12),-N12,P12-N12)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P12" s="1">
         <v>0</v>
       </c>
       <c r="Q12">
-        <f>IF(ISBLANK(R12),-P12,R12-P12)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="R12" s="1">
         <v>0</v>
       </c>
       <c r="S12">
-        <f>IF(ISBLANK(T12),-R12,T12-R12)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="T12" s="1">
@@ -7504,56 +7998,56 @@
         <v>9423</v>
       </c>
       <c r="E13">
-        <f>IF(ISBLANK(F13),-D13,F13-D13)</f>
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="F13" s="1">
         <v>9455</v>
       </c>
       <c r="G13">
-        <f>IF(ISBLANK(H13),-F13,H13-F13)</f>
+        <f t="shared" si="1"/>
         <v>325</v>
       </c>
       <c r="H13" s="1">
         <v>9780</v>
       </c>
       <c r="I13">
-        <f>IF(ISBLANK(J13),-H13,J13-H13)</f>
+        <f t="shared" si="2"/>
         <v>75</v>
       </c>
       <c r="J13" s="1">
         <v>9855</v>
       </c>
       <c r="K13">
-        <f>IF(ISBLANK(L13),-J13,L13-J13)</f>
+        <f t="shared" si="3"/>
         <v>114</v>
       </c>
       <c r="L13" s="1">
         <v>9969</v>
       </c>
       <c r="M13">
-        <f>IF(ISBLANK(N13),-L13,N13-L13)</f>
+        <f t="shared" si="4"/>
         <v>280</v>
       </c>
       <c r="N13" s="1">
         <v>10249</v>
       </c>
       <c r="O13">
-        <f>IF(ISBLANK(P13),-N13,P13-N13)</f>
+        <f t="shared" si="5"/>
         <v>78</v>
       </c>
       <c r="P13" s="1">
         <v>10327</v>
       </c>
       <c r="Q13">
-        <f>IF(ISBLANK(R13),-P13,R13-P13)</f>
+        <f t="shared" si="6"/>
         <v>137</v>
       </c>
       <c r="R13" s="1">
         <v>10464</v>
       </c>
       <c r="S13">
-        <f>IF(ISBLANK(T13),-R13,T13-R13)</f>
+        <f t="shared" si="7"/>
         <v>79</v>
       </c>
       <c r="T13" s="1">
@@ -7571,56 +8065,56 @@
         <v>79072</v>
       </c>
       <c r="E14">
-        <f>IF(ISBLANK(F14),-D14,F14-D14)</f>
+        <f t="shared" si="0"/>
         <v>68</v>
       </c>
       <c r="F14" s="1">
         <v>79140</v>
       </c>
       <c r="G14">
-        <f>IF(ISBLANK(H14),-F14,H14-F14)</f>
+        <f t="shared" si="1"/>
         <v>142</v>
       </c>
       <c r="H14" s="1">
         <v>79282</v>
       </c>
       <c r="I14">
-        <f>IF(ISBLANK(J14),-H14,J14-H14)</f>
+        <f t="shared" si="2"/>
         <v>105</v>
       </c>
       <c r="J14" s="1">
         <v>79387</v>
       </c>
       <c r="K14">
-        <f>IF(ISBLANK(L14),-J14,L14-J14)</f>
+        <f t="shared" si="3"/>
         <v>186</v>
       </c>
       <c r="L14" s="1">
         <v>79573</v>
       </c>
       <c r="M14">
-        <f>IF(ISBLANK(N14),-L14,N14-L14)</f>
+        <f t="shared" si="4"/>
         <v>168</v>
       </c>
       <c r="N14" s="1">
         <v>79741</v>
       </c>
       <c r="O14">
-        <f>IF(ISBLANK(P14),-N14,P14-N14)</f>
+        <f t="shared" si="5"/>
         <v>204</v>
       </c>
       <c r="P14" s="1">
         <v>79945</v>
       </c>
       <c r="Q14">
-        <f>IF(ISBLANK(R14),-P14,R14-P14)</f>
+        <f t="shared" si="6"/>
         <v>305</v>
       </c>
       <c r="R14" s="1">
         <v>80250</v>
       </c>
       <c r="S14">
-        <f>IF(ISBLANK(T14),-R14,T14-R14)</f>
+        <f t="shared" si="7"/>
         <v>127</v>
       </c>
       <c r="T14" s="1">
@@ -7638,56 +8132,56 @@
         <v>22075</v>
       </c>
       <c r="E15">
-        <f>IF(ISBLANK(F15),-D15,F15-D15)</f>
+        <f t="shared" si="0"/>
         <v>38</v>
       </c>
       <c r="F15" s="1">
         <v>22113</v>
       </c>
       <c r="G15">
-        <f>IF(ISBLANK(H15),-F15,H15-F15)</f>
+        <f t="shared" si="1"/>
         <v>80</v>
       </c>
       <c r="H15" s="1">
         <v>22193</v>
       </c>
       <c r="I15">
-        <f>IF(ISBLANK(J15),-H15,J15-H15)</f>
+        <f t="shared" si="2"/>
         <v>58</v>
       </c>
       <c r="J15" s="1">
         <v>22251</v>
       </c>
       <c r="K15">
-        <f>IF(ISBLANK(L15),-J15,L15-J15)</f>
+        <f t="shared" si="3"/>
         <v>70</v>
       </c>
       <c r="L15" s="1">
         <v>22321</v>
       </c>
       <c r="M15">
-        <f>IF(ISBLANK(N15),-L15,N15-L15)</f>
+        <f t="shared" si="4"/>
         <v>62</v>
       </c>
       <c r="N15" s="1">
         <v>22383</v>
       </c>
       <c r="O15">
-        <f>IF(ISBLANK(P15),-N15,P15-N15)</f>
+        <f t="shared" si="5"/>
         <v>70</v>
       </c>
       <c r="P15" s="1">
         <v>22453</v>
       </c>
       <c r="Q15">
-        <f>IF(ISBLANK(R15),-P15,R15-P15)</f>
+        <f t="shared" si="6"/>
         <v>173</v>
       </c>
       <c r="R15" s="1">
         <v>22626</v>
       </c>
       <c r="S15">
-        <f>IF(ISBLANK(T15),-R15,T15-R15)</f>
+        <f t="shared" si="7"/>
         <v>74</v>
       </c>
       <c r="T15" s="1">
@@ -7705,56 +8199,56 @@
         <v>9823</v>
       </c>
       <c r="E16">
-        <f>IF(ISBLANK(F16),-D16,F16-D16)</f>
+        <f t="shared" si="0"/>
         <v>37</v>
       </c>
       <c r="F16" s="1">
         <v>9860</v>
       </c>
       <c r="G16">
-        <f>IF(ISBLANK(H16),-F16,H16-F16)</f>
+        <f t="shared" si="1"/>
         <v>76</v>
       </c>
       <c r="H16" s="1">
         <v>9936</v>
       </c>
       <c r="I16">
-        <f>IF(ISBLANK(J16),-H16,J16-H16)</f>
+        <f t="shared" si="2"/>
         <v>54</v>
       </c>
       <c r="J16" s="1">
         <v>9990</v>
       </c>
       <c r="K16">
-        <f>IF(ISBLANK(L16),-J16,L16-J16)</f>
+        <f t="shared" si="3"/>
         <v>184</v>
       </c>
       <c r="L16" s="1">
         <v>10174</v>
       </c>
       <c r="M16">
-        <f>IF(ISBLANK(N16),-L16,N16-L16)</f>
+        <f t="shared" si="4"/>
         <v>52</v>
       </c>
       <c r="N16" s="1">
         <v>10226</v>
       </c>
       <c r="O16">
-        <f>IF(ISBLANK(P16),-N16,P16-N16)</f>
+        <f t="shared" si="5"/>
         <v>168</v>
       </c>
       <c r="P16" s="1">
         <v>10394</v>
       </c>
       <c r="Q16">
-        <f>IF(ISBLANK(R16),-P16,R16-P16)</f>
+        <f t="shared" si="6"/>
         <v>214</v>
       </c>
       <c r="R16" s="1">
         <v>10608</v>
       </c>
       <c r="S16">
-        <f>IF(ISBLANK(T16),-R16,T16-R16)</f>
+        <f t="shared" si="7"/>
         <v>48</v>
       </c>
       <c r="T16" s="1">
@@ -7772,56 +8266,56 @@
         <v>3682</v>
       </c>
       <c r="E17">
-        <f>IF(ISBLANK(F17),-D17,F17-D17)</f>
+        <f t="shared" si="0"/>
         <v>77</v>
       </c>
       <c r="F17" s="1">
         <v>3759</v>
       </c>
       <c r="G17">
-        <f>IF(ISBLANK(H17),-F17,H17-F17)</f>
+        <f t="shared" si="1"/>
         <v>44</v>
       </c>
       <c r="H17" s="1">
         <v>3803</v>
       </c>
       <c r="I17">
-        <f>IF(ISBLANK(J17),-H17,J17-H17)</f>
+        <f t="shared" si="2"/>
         <v>116</v>
       </c>
       <c r="J17" s="1">
         <v>3919</v>
       </c>
       <c r="K17">
-        <f>IF(ISBLANK(L17),-J17,L17-J17)</f>
+        <f t="shared" si="3"/>
         <v>87</v>
       </c>
       <c r="L17" s="1">
         <v>4006</v>
       </c>
       <c r="M17">
-        <f>IF(ISBLANK(N17),-L17,N17-L17)</f>
+        <f t="shared" si="4"/>
         <v>41</v>
       </c>
       <c r="N17" s="1">
         <v>4047</v>
       </c>
       <c r="O17">
-        <f>IF(ISBLANK(P17),-N17,P17-N17)</f>
+        <f t="shared" si="5"/>
         <v>134</v>
       </c>
       <c r="P17" s="1">
         <v>4181</v>
       </c>
       <c r="Q17">
-        <f>IF(ISBLANK(R17),-P17,R17-P17)</f>
+        <f t="shared" si="6"/>
         <v>-4181</v>
       </c>
       <c r="R17" s="1">
         <v>0</v>
       </c>
       <c r="S17">
-        <f>IF(ISBLANK(T17),-R17,T17-R17)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="T17" s="1">
@@ -7839,56 +8333,56 @@
         <v>75946</v>
       </c>
       <c r="E18">
-        <f>IF(ISBLANK(F18),-D18,F18-D18)</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="F18" s="1">
         <v>76046</v>
       </c>
       <c r="G18">
-        <f>IF(ISBLANK(H18),-F18,H18-F18)</f>
+        <f t="shared" si="1"/>
         <v>201</v>
       </c>
       <c r="H18" s="1">
         <v>76247</v>
       </c>
       <c r="I18">
-        <f>IF(ISBLANK(J18),-H18,J18-H18)</f>
+        <f t="shared" si="2"/>
         <v>126</v>
       </c>
       <c r="J18" s="1">
         <v>76373</v>
       </c>
       <c r="K18">
-        <f>IF(ISBLANK(L18),-J18,L18-J18)</f>
+        <f t="shared" si="3"/>
         <v>272</v>
       </c>
       <c r="L18" s="1">
         <v>76645</v>
       </c>
       <c r="M18">
-        <f>IF(ISBLANK(N18),-L18,N18-L18)</f>
+        <f t="shared" si="4"/>
         <v>74</v>
       </c>
       <c r="N18" s="1">
         <v>76719</v>
       </c>
       <c r="O18">
-        <f>IF(ISBLANK(P18),-N18,P18-N18)</f>
+        <f t="shared" si="5"/>
         <v>301</v>
       </c>
       <c r="P18" s="1">
         <v>77020</v>
       </c>
       <c r="Q18">
-        <f>IF(ISBLANK(R18),-P18,R18-P18)</f>
+        <f t="shared" si="6"/>
         <v>283</v>
       </c>
       <c r="R18" s="1">
         <v>77303</v>
       </c>
       <c r="S18">
-        <f>IF(ISBLANK(T18),-R18,T18-R18)</f>
+        <f t="shared" si="7"/>
         <v>112</v>
       </c>
       <c r="T18" s="1">
@@ -7906,56 +8400,56 @@
         <v>2864</v>
       </c>
       <c r="E19">
-        <f>IF(ISBLANK(F19),-D19,F19-D19)</f>
+        <f t="shared" si="0"/>
         <v>34</v>
       </c>
       <c r="F19" s="1">
         <v>2898</v>
       </c>
       <c r="G19">
-        <f>IF(ISBLANK(H19),-F19,H19-F19)</f>
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="H19" s="1">
         <v>2919</v>
       </c>
       <c r="I19">
-        <f>IF(ISBLANK(J19),-H19,J19-H19)</f>
+        <f t="shared" si="2"/>
         <v>148</v>
       </c>
       <c r="J19" s="1">
         <v>3067</v>
       </c>
       <c r="K19">
-        <f>IF(ISBLANK(L19),-J19,L19-J19)</f>
+        <f t="shared" si="3"/>
         <v>-3067</v>
       </c>
       <c r="L19" s="1">
         <v>0</v>
       </c>
       <c r="M19">
-        <f>IF(ISBLANK(N19),-L19,N19-L19)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N19" s="1">
         <v>0</v>
       </c>
       <c r="O19">
-        <f>IF(ISBLANK(P19),-N19,P19-N19)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P19" s="1">
         <v>0</v>
       </c>
       <c r="Q19">
-        <f>IF(ISBLANK(R19),-P19,R19-P19)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="R19" s="1">
         <v>0</v>
       </c>
       <c r="S19">
-        <f>IF(ISBLANK(T19),-R19,T19-R19)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="T19" s="1">
@@ -7973,56 +8467,56 @@
         <v>2416</v>
       </c>
       <c r="E20">
-        <f>IF(ISBLANK(F20),-D20,F20-D20)</f>
+        <f t="shared" si="0"/>
         <v>48</v>
       </c>
       <c r="F20" s="1">
         <v>2464</v>
       </c>
       <c r="G20">
-        <f>IF(ISBLANK(H20),-F20,H20-F20)</f>
+        <f t="shared" si="1"/>
         <v>78</v>
       </c>
       <c r="H20" s="1">
         <v>2542</v>
       </c>
       <c r="I20">
-        <f>IF(ISBLANK(J20),-H20,J20-H20)</f>
+        <f t="shared" si="2"/>
         <v>-2542</v>
       </c>
       <c r="J20" s="1">
         <v>0</v>
       </c>
       <c r="K20">
-        <f>IF(ISBLANK(L20),-J20,L20-J20)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L20" s="1">
         <v>0</v>
       </c>
       <c r="M20">
-        <f>IF(ISBLANK(N20),-L20,N20-L20)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N20" s="1">
         <v>0</v>
       </c>
       <c r="O20">
-        <f>IF(ISBLANK(P20),-N20,P20-N20)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P20" s="1">
         <v>0</v>
       </c>
       <c r="Q20">
-        <f>IF(ISBLANK(R20),-P20,R20-P20)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="R20" s="1">
         <v>0</v>
       </c>
       <c r="S20">
-        <f>IF(ISBLANK(T20),-R20,T20-R20)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="T20" s="1">
@@ -8040,56 +8534,56 @@
         <v>1423</v>
       </c>
       <c r="E21">
-        <f>IF(ISBLANK(F21),-D21,F21-D21)</f>
+        <f t="shared" si="0"/>
         <v>-1423</v>
       </c>
       <c r="F21" s="1">
         <v>0</v>
       </c>
       <c r="G21">
-        <f>IF(ISBLANK(H21),-F21,H21-F21)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H21" s="1">
         <v>0</v>
       </c>
       <c r="I21">
-        <f>IF(ISBLANK(J21),-H21,J21-H21)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J21" s="1">
         <v>0</v>
       </c>
       <c r="K21">
-        <f>IF(ISBLANK(L21),-J21,L21-J21)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L21" s="1">
         <v>0</v>
       </c>
       <c r="M21">
-        <f>IF(ISBLANK(N21),-L21,N21-L21)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N21" s="1">
         <v>0</v>
       </c>
       <c r="O21">
-        <f>IF(ISBLANK(P21),-N21,P21-N21)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P21" s="1">
         <v>0</v>
       </c>
       <c r="Q21">
-        <f>IF(ISBLANK(R21),-P21,R21-P21)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="R21" s="1">
         <v>0</v>
       </c>
       <c r="S21">
-        <f>IF(ISBLANK(T21),-R21,T21-R21)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="T21" s="1">
@@ -8107,56 +8601,56 @@
         <v>14802</v>
       </c>
       <c r="E22">
-        <f>IF(ISBLANK(F22),-D22,F22-D22)</f>
+        <f t="shared" si="0"/>
         <v>156</v>
       </c>
       <c r="F22" s="1">
         <v>14958</v>
       </c>
       <c r="G22">
-        <f>IF(ISBLANK(H22),-F22,H22-F22)</f>
+        <f t="shared" si="1"/>
         <v>51</v>
       </c>
       <c r="H22" s="1">
         <v>15009</v>
       </c>
       <c r="I22">
-        <f>IF(ISBLANK(J22),-H22,J22-H22)</f>
+        <f t="shared" si="2"/>
         <v>198</v>
       </c>
       <c r="J22" s="1">
         <v>15207</v>
       </c>
       <c r="K22">
-        <f>IF(ISBLANK(L22),-J22,L22-J22)</f>
+        <f t="shared" si="3"/>
         <v>146</v>
       </c>
       <c r="L22" s="1">
         <v>15353</v>
       </c>
       <c r="M22">
-        <f>IF(ISBLANK(N22),-L22,N22-L22)</f>
+        <f t="shared" si="4"/>
         <v>41</v>
       </c>
       <c r="N22" s="1">
         <v>15394</v>
       </c>
       <c r="O22">
-        <f>IF(ISBLANK(P22),-N22,P22-N22)</f>
+        <f t="shared" si="5"/>
         <v>392</v>
       </c>
       <c r="P22" s="1">
         <v>15786</v>
       </c>
       <c r="Q22">
-        <f>IF(ISBLANK(R22),-P22,R22-P22)</f>
+        <f t="shared" si="6"/>
         <v>321</v>
       </c>
       <c r="R22" s="1">
         <v>16107</v>
       </c>
       <c r="S22">
-        <f>IF(ISBLANK(T22),-R22,T22-R22)</f>
+        <f t="shared" si="7"/>
         <v>101</v>
       </c>
       <c r="T22" s="1">
@@ -8174,56 +8668,56 @@
         <v>81741</v>
       </c>
       <c r="E23">
-        <f>IF(ISBLANK(F23),-D23,F23-D23)</f>
+        <f t="shared" si="0"/>
         <v>253</v>
       </c>
       <c r="F23" s="1">
         <v>81994</v>
       </c>
       <c r="G23">
-        <f>IF(ISBLANK(H23),-F23,H23-F23)</f>
+        <f t="shared" si="1"/>
         <v>130</v>
       </c>
       <c r="H23" s="1">
         <v>82124</v>
       </c>
       <c r="I23">
-        <f>IF(ISBLANK(J23),-H23,J23-H23)</f>
+        <f t="shared" si="2"/>
         <v>211</v>
       </c>
       <c r="J23" s="1">
         <v>82335</v>
       </c>
       <c r="K23">
-        <f>IF(ISBLANK(L23),-J23,L23-J23)</f>
+        <f t="shared" si="3"/>
         <v>323</v>
       </c>
       <c r="L23" s="1">
         <v>82658</v>
       </c>
       <c r="M23">
-        <f>IF(ISBLANK(N23),-L23,N23-L23)</f>
+        <f t="shared" si="4"/>
         <v>206</v>
       </c>
       <c r="N23" s="1">
         <v>82864</v>
       </c>
       <c r="O23">
-        <f>IF(ISBLANK(P23),-N23,P23-N23)</f>
+        <f t="shared" si="5"/>
         <v>556</v>
       </c>
       <c r="P23" s="1">
         <v>83420</v>
       </c>
       <c r="Q23">
-        <f>IF(ISBLANK(R23),-P23,R23-P23)</f>
+        <f t="shared" si="6"/>
         <v>351</v>
       </c>
       <c r="R23" s="1">
         <v>83771</v>
       </c>
       <c r="S23">
-        <f>IF(ISBLANK(T23),-R23,T23-R23)</f>
+        <f t="shared" si="7"/>
         <v>217</v>
       </c>
       <c r="T23" s="1">
@@ -8241,56 +8735,56 @@
         <v>3286</v>
       </c>
       <c r="E24">
-        <f>IF(ISBLANK(F24),-D24,F24-D24)</f>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="F24" s="1">
         <v>3307</v>
       </c>
       <c r="G24">
-        <f>IF(ISBLANK(H24),-F24,H24-F24)</f>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="H24" s="1">
         <v>3320</v>
       </c>
       <c r="I24">
-        <f>IF(ISBLANK(J24),-H24,J24-H24)</f>
+        <f t="shared" si="2"/>
         <v>232</v>
       </c>
       <c r="J24" s="1">
         <v>3552</v>
       </c>
       <c r="K24">
-        <f>IF(ISBLANK(L24),-J24,L24-J24)</f>
+        <f t="shared" si="3"/>
         <v>102</v>
       </c>
       <c r="L24" s="1">
         <v>3654</v>
       </c>
       <c r="M24">
-        <f>IF(ISBLANK(N24),-L24,N24-L24)</f>
+        <f t="shared" si="4"/>
         <v>60</v>
       </c>
       <c r="N24" s="1">
         <v>3714</v>
       </c>
       <c r="O24">
-        <f>IF(ISBLANK(P24),-N24,P24-N24)</f>
+        <f t="shared" si="5"/>
         <v>-3714</v>
       </c>
       <c r="P24" s="1">
         <v>0</v>
       </c>
       <c r="Q24">
-        <f>IF(ISBLANK(R24),-P24,R24-P24)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="R24" s="1">
         <v>0</v>
       </c>
       <c r="S24">
-        <f>IF(ISBLANK(T24),-R24,T24-R24)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="T24" s="1">
@@ -8371,19 +8865,19 @@
         <v>148</v>
       </c>
       <c r="E27">
-        <f t="shared" ref="E27:E48" si="0">FIND(",",B27)</f>
+        <f t="shared" ref="E27:E48" si="8">FIND(",",B27)</f>
         <v>9</v>
       </c>
       <c r="F27" t="str">
-        <f t="shared" ref="F27:F48" si="1">LEFT(B27,E27-1)</f>
+        <f t="shared" ref="F27:F48" si="9">LEFT(B27,E27-1)</f>
         <v>Kelleher</v>
       </c>
       <c r="G27" t="str">
-        <f t="shared" ref="G27:G48" si="2">RIGHT(B27,LEN(B27)-(E27+1))</f>
+        <f t="shared" ref="G27:G48" si="10">RIGHT(B27,LEN(B27)-(E27+1))</f>
         <v>Billy</v>
       </c>
       <c r="H27" t="str">
-        <f t="shared" ref="H27:H48" si="3">G27&amp;" "&amp;F27</f>
+        <f t="shared" ref="H27:H48" si="11">G27&amp;" "&amp;F27</f>
         <v>Billy Kelleher</v>
       </c>
       <c r="J27" t="s">
@@ -8439,19 +8933,19 @@
         <v>149</v>
       </c>
       <c r="E28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="8"/>
         <v>8</v>
       </c>
       <c r="F28" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>Wallace</v>
       </c>
       <c r="G28" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>Mick</v>
       </c>
       <c r="H28" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="11"/>
         <v>Mick Wallace</v>
       </c>
       <c r="J28" t="s">
@@ -8507,19 +9001,19 @@
         <v>150</v>
       </c>
       <c r="E29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="8"/>
         <v>9</v>
       </c>
       <c r="F29" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>Ní Riada</v>
       </c>
       <c r="G29" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>Liadh</v>
       </c>
       <c r="H29" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="11"/>
         <v>Liadh Ní Riada</v>
       </c>
       <c r="J29" t="s">
@@ -8575,19 +9069,19 @@
         <v>151</v>
       </c>
       <c r="E30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="8"/>
         <v>11</v>
       </c>
       <c r="F30" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>O'Sullivan</v>
       </c>
       <c r="G30" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>Grace</v>
       </c>
       <c r="H30" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="11"/>
         <v>Grace O'Sullivan</v>
       </c>
       <c r="J30" t="s">
@@ -8643,19 +9137,19 @@
         <v>152</v>
       </c>
       <c r="E31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="8"/>
         <v>6</v>
       </c>
       <c r="F31" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>Byrne</v>
       </c>
       <c r="G31" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>Malcolm</v>
       </c>
       <c r="H31" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="11"/>
         <v>Malcolm Byrne</v>
       </c>
       <c r="J31" t="s">
@@ -8711,19 +9205,19 @@
         <v>153</v>
       </c>
       <c r="E32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="8"/>
         <v>6</v>
       </c>
       <c r="F32" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>Clune</v>
       </c>
       <c r="G32" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>Deirdre</v>
       </c>
       <c r="H32" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="11"/>
         <v>Deirdre Clune</v>
       </c>
       <c r="J32" t="s">
@@ -8779,19 +9273,19 @@
         <v>154</v>
       </c>
       <c r="E33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="8"/>
         <v>6</v>
       </c>
       <c r="F33" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>Doyle</v>
       </c>
       <c r="G33" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>Andrew</v>
       </c>
       <c r="H33" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="11"/>
         <v>Andrew Doyle</v>
       </c>
       <c r="J33" t="s">
@@ -8847,19 +9341,19 @@
         <v>155</v>
       </c>
       <c r="E34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="8"/>
         <v>6</v>
       </c>
       <c r="F34" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>Nunan</v>
       </c>
       <c r="G34" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>Sheila</v>
       </c>
       <c r="H34" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="11"/>
         <v>Sheila Nunan</v>
       </c>
       <c r="J34" t="s">
@@ -8915,19 +9409,19 @@
         <v>156</v>
       </c>
       <c r="E35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="8"/>
         <v>8</v>
       </c>
       <c r="F35" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>Wallace</v>
       </c>
       <c r="G35" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>Adrienne</v>
       </c>
       <c r="H35" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="11"/>
         <v>Adrienne Wallace</v>
       </c>
       <c r="J35" t="s">
@@ -8983,19 +9477,19 @@
         <v>157</v>
       </c>
       <c r="E36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="8"/>
         <v>7</v>
       </c>
       <c r="F36" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>Cahill</v>
       </c>
       <c r="G36" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>Dolores</v>
       </c>
       <c r="H36" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="11"/>
         <v>Dolores Cahill</v>
       </c>
       <c r="J36" t="s">
@@ -9051,19 +9545,19 @@
         <v>158</v>
       </c>
       <c r="E37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="8"/>
         <v>8</v>
       </c>
       <c r="F37" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>O'Flynn</v>
       </c>
       <c r="G37" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>Diarmuid Patrick</v>
       </c>
       <c r="H37" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="11"/>
         <v>Diarmuid Patrick O'Flynn</v>
       </c>
       <c r="J37" t="s">
@@ -9119,19 +9613,19 @@
         <v>159</v>
       </c>
       <c r="E38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="8"/>
         <v>8</v>
       </c>
       <c r="F38" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>Minehan</v>
       </c>
       <c r="G38" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>Liam</v>
       </c>
       <c r="H38" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="11"/>
         <v>Liam Minehan</v>
       </c>
       <c r="J38" t="s">
@@ -9187,19 +9681,19 @@
         <v>160</v>
       </c>
       <c r="E39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="8"/>
         <v>8</v>
       </c>
       <c r="F39" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>Gardner</v>
       </c>
       <c r="G39" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>Breda Patricia</v>
       </c>
       <c r="H39" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="11"/>
         <v>Breda Patricia Gardner</v>
       </c>
       <c r="J39" t="s">
@@ -9255,19 +9749,19 @@
         <v>161</v>
       </c>
       <c r="E40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="8"/>
         <v>7</v>
       </c>
       <c r="F40" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>Heaney</v>
       </c>
       <c r="G40" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>Theresa</v>
       </c>
       <c r="H40" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="11"/>
         <v>Theresa Heaney</v>
       </c>
       <c r="J40" t="s">
@@ -9323,19 +9817,19 @@
         <v>162</v>
       </c>
       <c r="E41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="8"/>
         <v>8</v>
       </c>
       <c r="F41" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>Brennan</v>
       </c>
       <c r="G41" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>Allan</v>
       </c>
       <c r="H41" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="11"/>
         <v>Allan Brennan</v>
       </c>
       <c r="J41" t="s">
@@ -9391,19 +9885,19 @@
         <v>163</v>
       </c>
       <c r="E42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="8"/>
         <v>11</v>
       </c>
       <c r="F42" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>O'Loughlin</v>
       </c>
       <c r="G42" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>Peter</v>
       </c>
       <c r="H42" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="11"/>
         <v>Peter O'Loughlin</v>
       </c>
       <c r="J42" t="s">
@@ -9456,19 +9950,19 @@
         <v>164</v>
       </c>
       <c r="E43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="8"/>
         <v>12</v>
       </c>
       <c r="F43" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>Worthington</v>
       </c>
       <c r="G43" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>Colleen</v>
       </c>
       <c r="H43" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="11"/>
         <v>Colleen Worthington</v>
       </c>
       <c r="J43" t="s">
@@ -9517,19 +10011,19 @@
         <v>165</v>
       </c>
       <c r="E44">
-        <f t="shared" si="0"/>
+        <f t="shared" si="8"/>
         <v>11</v>
       </c>
       <c r="F44" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>Fitzgerald</v>
       </c>
       <c r="G44" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>Paddy</v>
       </c>
       <c r="H44" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="11"/>
         <v>Paddy Fitzgerald</v>
       </c>
       <c r="J44" t="s">
@@ -9574,19 +10068,19 @@
         <v>166</v>
       </c>
       <c r="E45">
-        <f t="shared" si="0"/>
+        <f t="shared" si="8"/>
         <v>13</v>
       </c>
       <c r="F45" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>Ryan-Purcell</v>
       </c>
       <c r="G45" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>Walter</v>
       </c>
       <c r="H45" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="11"/>
         <v>Walter Ryan-Purcell</v>
       </c>
       <c r="J45" t="s">
@@ -9627,19 +10121,19 @@
         <v>167</v>
       </c>
       <c r="E46">
-        <f t="shared" si="0"/>
+        <f t="shared" si="8"/>
         <v>7</v>
       </c>
       <c r="F46" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>Sexton</v>
       </c>
       <c r="G46" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>Joesph</v>
       </c>
       <c r="H46" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="11"/>
         <v>Joesph Sexton</v>
       </c>
       <c r="J46" t="s">
@@ -9673,19 +10167,19 @@
         <v>168</v>
       </c>
       <c r="E47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="8"/>
         <v>7</v>
       </c>
       <c r="F47" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>Madden</v>
       </c>
       <c r="G47" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>Peter</v>
       </c>
       <c r="H47" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="11"/>
         <v>Peter Madden</v>
       </c>
       <c r="J47" t="s">
@@ -9712,19 +10206,19 @@
         <v>169</v>
       </c>
       <c r="E48">
-        <f t="shared" si="0"/>
+        <f t="shared" si="8"/>
         <v>11</v>
       </c>
       <c r="F48" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>Van de Ven</v>
       </c>
       <c r="G48" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>Jan</v>
       </c>
       <c r="H48" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="11"/>
         <v>Jan Van de Ven</v>
       </c>
       <c r="J48" t="s">

</xml_diff>

<commit_message>
Stage 16 Dublin added Signed-off-by: Gerry Mulvenna <git@movingwifi.com>
</commit_message>
<xml_diff>
--- a/europarl/europarl-ireland-2019.xlsx
+++ b/europarl/europarl-ireland-2019.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="14220" windowHeight="8580" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="14220" windowHeight="8580" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Candidates" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="263">
   <si>
     <t>Candidate</t>
   </si>
@@ -803,6 +803,9 @@
   </si>
   <si>
     <t>O'Dowd, Michael eliminated</t>
+  </si>
+  <si>
+    <t>Count 16</t>
   </si>
 </sst>
 </file>
@@ -2464,18 +2467,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF41"/>
+  <dimension ref="A1:AH41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="AA2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="AF2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AE2" sqref="AE2:AF20"/>
+      <selection pane="bottomRight" activeCell="D2" sqref="D2:AH20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>232</v>
       </c>
@@ -2527,8 +2530,11 @@
       <c r="AF1" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AH1" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>3</v>
       </c>
@@ -2637,8 +2643,15 @@
       <c r="AF2">
         <v>63177</v>
       </c>
-    </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG2">
+        <f t="shared" ref="AG2:AG20" si="12">IF(ISBLANK(AH2),-AF2,AH2-AF2)</f>
+        <v>5775</v>
+      </c>
+      <c r="AH2">
+        <v>68952</v>
+      </c>
+    </row>
+    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>5</v>
       </c>
@@ -2747,8 +2760,15 @@
       <c r="AF3">
         <v>51632</v>
       </c>
-    </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG3">
+        <f t="shared" si="12"/>
+        <v>-51632</v>
+      </c>
+      <c r="AH3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>9</v>
       </c>
@@ -2851,14 +2871,21 @@
         <v>0</v>
       </c>
       <c r="AE4">
-        <f t="shared" ref="AE4:AE20" si="12">IF(ISBLANK(AF4),-AD4,AF4-AD4)</f>
+        <f t="shared" ref="AE4:AE20" si="13">IF(ISBLANK(AF4),-AD4,AF4-AD4)</f>
         <v>0</v>
       </c>
       <c r="AF4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG4">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AH4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2960,14 +2987,21 @@
         <v>73028</v>
       </c>
       <c r="AE5">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AF5" s="1">
         <v>73028</v>
       </c>
-    </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG5">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AH5" s="1">
+        <v>73028</v>
+      </c>
+    </row>
+    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -3063,21 +3097,28 @@
         <v>52930</v>
       </c>
       <c r="AC6">
-        <f t="shared" ref="AC6:AC20" si="13">IF(ISBLANK(AD6),-AB6,AD6-AB6)</f>
+        <f t="shared" ref="AC6:AC20" si="14">IF(ISBLANK(AD6),-AB6,AD6-AB6)</f>
         <v>2822</v>
       </c>
       <c r="AD6" s="1">
         <v>55752</v>
       </c>
       <c r="AE6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>9931</v>
       </c>
       <c r="AF6">
         <v>65683</v>
       </c>
-    </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG6">
+        <f t="shared" si="12"/>
+        <v>22087</v>
+      </c>
+      <c r="AH6">
+        <v>87770</v>
+      </c>
+    </row>
+    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>8</v>
       </c>
@@ -3173,21 +3214,28 @@
         <v>0</v>
       </c>
       <c r="AC7">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AD7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE7">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="AD7" s="1">
-        <v>0</v>
-      </c>
-      <c r="AE7">
+      <c r="AF7">
+        <v>0</v>
+      </c>
+      <c r="AG7">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="AF7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AH7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2</v>
       </c>
@@ -3283,21 +3331,27 @@
         <v>72446</v>
       </c>
       <c r="AC8">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>6134</v>
       </c>
       <c r="AD8" s="1">
         <v>78580</v>
       </c>
       <c r="AE8">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AF8" s="1">
         <v>78580</v>
       </c>
-    </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG8">
+        <v>0</v>
+      </c>
+      <c r="AH8" s="1">
+        <v>78580</v>
+      </c>
+    </row>
+    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>6</v>
       </c>
@@ -3393,21 +3447,28 @@
         <v>25915</v>
       </c>
       <c r="AC9">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>3805</v>
       </c>
       <c r="AD9" s="1">
         <v>29720</v>
       </c>
       <c r="AE9">
+        <f t="shared" si="13"/>
+        <v>-29720</v>
+      </c>
+      <c r="AF9">
+        <v>0</v>
+      </c>
+      <c r="AG9">
         <f t="shared" si="12"/>
-        <v>-29720</v>
-      </c>
-      <c r="AF9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="AH9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>11</v>
       </c>
@@ -3503,21 +3564,28 @@
         <v>0</v>
       </c>
       <c r="AC10">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AD10" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE10">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="AD10" s="1">
-        <v>0</v>
-      </c>
-      <c r="AE10">
+      <c r="AF10">
+        <v>0</v>
+      </c>
+      <c r="AG10">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="AF10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AH10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>13</v>
       </c>
@@ -3613,21 +3681,28 @@
         <v>0</v>
       </c>
       <c r="AC11">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AD11" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE11">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="AD11" s="1">
-        <v>0</v>
-      </c>
-      <c r="AE11">
+      <c r="AF11">
+        <v>0</v>
+      </c>
+      <c r="AG11">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="AF11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AH11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -3723,21 +3798,28 @@
         <v>0</v>
       </c>
       <c r="AC12">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AD12" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE12">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="AD12" s="1">
-        <v>0</v>
-      </c>
-      <c r="AE12">
+      <c r="AF12">
+        <v>0</v>
+      </c>
+      <c r="AG12">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="AF12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AH12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>16</v>
       </c>
@@ -3833,21 +3915,28 @@
         <v>0</v>
       </c>
       <c r="AC13">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AD13">
+        <v>0</v>
+      </c>
+      <c r="AE13">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="AD13">
-        <v>0</v>
-      </c>
-      <c r="AE13">
+      <c r="AF13">
+        <v>0</v>
+      </c>
+      <c r="AG13">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="AF13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AH13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>19</v>
       </c>
@@ -3943,21 +4032,28 @@
         <v>0</v>
       </c>
       <c r="AC14">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AD14">
+        <v>0</v>
+      </c>
+      <c r="AE14">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="AD14">
-        <v>0</v>
-      </c>
-      <c r="AE14">
+      <c r="AF14">
+        <v>0</v>
+      </c>
+      <c r="AG14">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="AF14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AH14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>17</v>
       </c>
@@ -4053,21 +4149,28 @@
         <v>0</v>
       </c>
       <c r="AC15">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AD15">
+        <v>0</v>
+      </c>
+      <c r="AE15">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="AD15">
-        <v>0</v>
-      </c>
-      <c r="AE15">
+      <c r="AF15">
+        <v>0</v>
+      </c>
+      <c r="AG15">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="AF15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AH15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>18</v>
       </c>
@@ -4163,21 +4266,28 @@
         <v>0</v>
       </c>
       <c r="AC16">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AD16">
+        <v>0</v>
+      </c>
+      <c r="AE16">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="AD16">
-        <v>0</v>
-      </c>
-      <c r="AE16">
+      <c r="AF16">
+        <v>0</v>
+      </c>
+      <c r="AG16">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="AF16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AH16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -4273,21 +4383,28 @@
         <v>0</v>
       </c>
       <c r="AC17">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AD17">
+        <v>0</v>
+      </c>
+      <c r="AE17">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="AD17">
-        <v>0</v>
-      </c>
-      <c r="AE17">
+      <c r="AF17">
+        <v>0</v>
+      </c>
+      <c r="AG17">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="AF17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AH17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>12</v>
       </c>
@@ -4383,21 +4500,28 @@
         <v>0</v>
       </c>
       <c r="AC18">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AD18">
+        <v>0</v>
+      </c>
+      <c r="AE18">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="AD18">
-        <v>0</v>
-      </c>
-      <c r="AE18">
+      <c r="AF18">
+        <v>0</v>
+      </c>
+      <c r="AG18">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="AF18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AH18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>14</v>
       </c>
@@ -4493,21 +4617,28 @@
         <v>0</v>
       </c>
       <c r="AC19">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AD19">
+        <v>0</v>
+      </c>
+      <c r="AE19">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="AD19">
-        <v>0</v>
-      </c>
-      <c r="AE19">
+      <c r="AF19">
+        <v>0</v>
+      </c>
+      <c r="AG19">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="AF19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AH19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>7</v>
       </c>
@@ -4603,21 +4734,28 @@
         <v>22205</v>
       </c>
       <c r="AC20">
+        <f t="shared" si="14"/>
+        <v>-22205</v>
+      </c>
+      <c r="AD20">
+        <v>0</v>
+      </c>
+      <c r="AE20">
         <f t="shared" si="13"/>
-        <v>-22205</v>
-      </c>
-      <c r="AD20">
-        <v>0</v>
-      </c>
-      <c r="AE20">
+        <v>0</v>
+      </c>
+      <c r="AF20">
+        <v>0</v>
+      </c>
+      <c r="AG20">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="AF20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AH20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:34" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>34</v>
       </c>
@@ -4638,192 +4776,192 @@
         <v>Ciaran Cuffe</v>
       </c>
     </row>
-    <row r="24" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:34" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>35</v>
       </c>
       <c r="D24">
-        <f t="shared" ref="D24:D41" si="14">FIND(",",B24)</f>
+        <f t="shared" ref="D24:D41" si="15">FIND(",",B24)</f>
         <v>11</v>
       </c>
       <c r="E24" t="str">
-        <f t="shared" ref="E24:E41" si="15">LEFT(B24,D24-1)</f>
+        <f t="shared" ref="E24:E41" si="16">LEFT(B24,D24-1)</f>
         <v>Fitzgerald</v>
       </c>
       <c r="F24" t="str">
-        <f t="shared" ref="F24:F41" si="16">RIGHT(B24,LEN(B24)-(D24+1))</f>
+        <f t="shared" ref="F24:F41" si="17">RIGHT(B24,LEN(B24)-(D24+1))</f>
         <v>Frances</v>
       </c>
       <c r="G24" t="str">
-        <f t="shared" ref="G24:G41" si="17">F24&amp;" "&amp;E24</f>
+        <f t="shared" ref="G24:G41" si="18">F24&amp;" "&amp;E24</f>
         <v>Frances Fitzgerald</v>
       </c>
     </row>
-    <row r="25" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:34" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>36</v>
       </c>
       <c r="D25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>8</v>
       </c>
       <c r="E25" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>Andrews</v>
       </c>
       <c r="F25" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>Barry</v>
       </c>
       <c r="G25" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>Barry Andrews</v>
       </c>
     </row>
-    <row r="26" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:34" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>37</v>
       </c>
       <c r="D26">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>5</v>
       </c>
       <c r="E26" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>Daly</v>
       </c>
       <c r="F26" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>Clare</v>
       </c>
       <c r="G26" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>Clare Daly</v>
       </c>
     </row>
-    <row r="27" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:34" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>38</v>
       </c>
       <c r="D27">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>7</v>
       </c>
       <c r="E27" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>Boylan</v>
       </c>
       <c r="F27" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>Lynn</v>
       </c>
       <c r="G27" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>Lynn Boylan</v>
       </c>
     </row>
-    <row r="28" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:34" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>39</v>
       </c>
       <c r="D28">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>7</v>
       </c>
       <c r="E28" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>Gannon</v>
       </c>
       <c r="F28" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>Gary</v>
       </c>
       <c r="G28" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>Gary Gannon</v>
       </c>
     </row>
-    <row r="29" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:34" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>40</v>
       </c>
       <c r="D29">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>6</v>
       </c>
       <c r="E29" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>White</v>
       </c>
       <c r="F29" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>Alex</v>
       </c>
       <c r="G29" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>Alex White</v>
       </c>
     </row>
-    <row r="30" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:34" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>41</v>
       </c>
       <c r="D30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>7</v>
       </c>
       <c r="E30" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>Durkan</v>
       </c>
       <c r="F30" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>Mark</v>
       </c>
       <c r="G30" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>Mark Durkan</v>
       </c>
     </row>
-    <row r="31" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:34" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>42</v>
       </c>
       <c r="D31">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>6</v>
       </c>
       <c r="E31" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>Brien</v>
       </c>
       <c r="F31" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>Gillian</v>
       </c>
       <c r="G31" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>Gillian Brien</v>
       </c>
     </row>
-    <row r="32" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:34" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>43</v>
       </c>
       <c r="D32">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>8</v>
       </c>
       <c r="E32" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>Higgins</v>
       </c>
       <c r="F32" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>Alice Mary</v>
       </c>
       <c r="G32" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>Alice Mary Higgins</v>
       </c>
     </row>
@@ -4832,19 +4970,19 @@
         <v>44</v>
       </c>
       <c r="D33">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>7</v>
       </c>
       <c r="E33" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>Gilroy</v>
       </c>
       <c r="F33" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>Ben</v>
       </c>
       <c r="G33" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>Ben Gilroy</v>
       </c>
     </row>
@@ -4853,19 +4991,19 @@
         <v>45</v>
       </c>
       <c r="D34">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>10</v>
       </c>
       <c r="E34" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>O'Doherty</v>
       </c>
       <c r="F34" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>Gemma</v>
       </c>
       <c r="G34" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>Gemma O'Doherty</v>
       </c>
     </row>
@@ -4874,19 +5012,19 @@
         <v>46</v>
       </c>
       <c r="D35">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>8</v>
       </c>
       <c r="E35" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>Harrold</v>
       </c>
       <c r="F35" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>Rita</v>
       </c>
       <c r="G35" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>Rita Harrold</v>
       </c>
     </row>
@@ -4895,19 +5033,19 @@
         <v>47</v>
       </c>
       <c r="D36">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>5</v>
       </c>
       <c r="E36" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>Ryan</v>
       </c>
       <c r="F36" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>Éilis</v>
       </c>
       <c r="G36" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>Éilis Ryan</v>
       </c>
     </row>
@@ -4916,19 +5054,19 @@
         <v>48</v>
       </c>
       <c r="D37">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>7</v>
       </c>
       <c r="E37" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>Murphy</v>
       </c>
       <c r="F37" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>Eamonn</v>
       </c>
       <c r="G37" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>Eamonn Murphy</v>
       </c>
     </row>
@@ -4937,19 +5075,19 @@
         <v>49</v>
       </c>
       <c r="D38">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>6</v>
       </c>
       <c r="E38" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>Kelly</v>
       </c>
       <c r="F38" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>Hermann</v>
       </c>
       <c r="G38" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>Hermann Kelly</v>
       </c>
     </row>
@@ -4958,19 +5096,19 @@
         <v>50</v>
       </c>
       <c r="D39">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>8</v>
       </c>
       <c r="E39" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>McNiffe</v>
       </c>
       <c r="F39" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>Aisling</v>
       </c>
       <c r="G39" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>Aisling McNiffe</v>
       </c>
     </row>
@@ -4979,19 +5117,19 @@
         <v>51</v>
       </c>
       <c r="D40">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>7</v>
       </c>
       <c r="E40" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>Mullan</v>
       </c>
       <c r="F40" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>Mark</v>
       </c>
       <c r="G40" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>Mark Mullan</v>
       </c>
     </row>
@@ -5000,19 +5138,19 @@
         <v>52</v>
       </c>
       <c r="D41">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>6</v>
       </c>
       <c r="E41" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>Lowth</v>
       </c>
       <c r="F41" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>Tony Bosco</v>
       </c>
       <c r="G41" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>Tony Bosco Lowth</v>
       </c>
     </row>
@@ -5029,7 +5167,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
@@ -5076,42 +5214,42 @@
         <v>134630</v>
       </c>
       <c r="E2">
-        <f>IF(ISBLANK(F2),-D2,F2-D2)</f>
+        <f t="shared" ref="E2:E18" si="0">IF(ISBLANK(F2),-D2,F2-D2)</f>
         <v>-15644</v>
       </c>
       <c r="F2">
         <v>118986</v>
       </c>
       <c r="G2">
-        <f>IF(ISBLANK(H2),-F2,H2-F2)</f>
+        <f t="shared" ref="G2:G18" si="1">IF(ISBLANK(H2),-F2,H2-F2)</f>
         <v>0</v>
       </c>
       <c r="H2">
         <v>118986</v>
       </c>
       <c r="I2">
-        <f>IF(ISBLANK(J2),-H2,J2-H2)</f>
+        <f t="shared" ref="I2:I18" si="2">IF(ISBLANK(J2),-H2,J2-H2)</f>
         <v>0</v>
       </c>
       <c r="J2">
         <v>118986</v>
       </c>
       <c r="K2">
-        <f>IF(ISBLANK(L2),-J2,L2-J2)</f>
+        <f t="shared" ref="K2:K18" si="3">IF(ISBLANK(L2),-J2,L2-J2)</f>
         <v>0</v>
       </c>
       <c r="L2">
         <v>118986</v>
       </c>
       <c r="M2">
-        <f>IF(ISBLANK(N2),-L2,N2-L2)</f>
+        <f t="shared" ref="M2:M18" si="4">IF(ISBLANK(N2),-L2,N2-L2)</f>
         <v>0</v>
       </c>
       <c r="N2">
         <v>118986</v>
       </c>
       <c r="O2">
-        <f>IF(ISBLANK(P2),-N2,P2-N2)</f>
+        <f t="shared" ref="O2:O18" si="5">IF(ISBLANK(P2),-N2,P2-N2)</f>
         <v>0</v>
       </c>
       <c r="P2">
@@ -5130,42 +5268,42 @@
         <v>85034</v>
       </c>
       <c r="E3">
-        <f>IF(ISBLANK(F3),-D3,F3-D3)</f>
+        <f t="shared" si="0"/>
         <v>1872</v>
       </c>
       <c r="F3" s="1">
         <v>86906</v>
       </c>
       <c r="G3">
-        <f>IF(ISBLANK(H3),-F3,H3-F3)</f>
+        <f t="shared" si="1"/>
         <v>102</v>
       </c>
       <c r="H3" s="1">
         <v>87008</v>
       </c>
       <c r="I3">
-        <f>IF(ISBLANK(J3),-H3,J3-H3)</f>
+        <f t="shared" si="2"/>
         <v>180</v>
       </c>
       <c r="J3" s="1">
         <v>87188</v>
       </c>
       <c r="K3">
-        <f>IF(ISBLANK(L3),-J3,L3-J3)</f>
+        <f t="shared" si="3"/>
         <v>145</v>
       </c>
       <c r="L3" s="1">
         <v>87333</v>
       </c>
       <c r="M3">
-        <f>IF(ISBLANK(N3),-L3,N3-L3)</f>
+        <f t="shared" si="4"/>
         <v>631</v>
       </c>
       <c r="N3" s="1">
         <v>87964</v>
       </c>
       <c r="O3">
-        <f>IF(ISBLANK(P3),-N3,P3-N3)</f>
+        <f t="shared" si="5"/>
         <v>579</v>
       </c>
       <c r="P3" s="1">
@@ -5184,42 +5322,42 @@
         <v>77619</v>
       </c>
       <c r="E4">
-        <f>IF(ISBLANK(F4),-D4,F4-D4)</f>
+        <f t="shared" si="0"/>
         <v>868</v>
       </c>
       <c r="F4" s="1">
         <v>78487</v>
       </c>
       <c r="G4">
-        <f>IF(ISBLANK(H4),-F4,H4-F4)</f>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="H4" s="1">
         <v>78513</v>
       </c>
       <c r="I4">
-        <f>IF(ISBLANK(J4),-H4,J4-H4)</f>
+        <f t="shared" si="2"/>
         <v>99</v>
       </c>
       <c r="J4" s="1">
         <v>78612</v>
       </c>
       <c r="K4">
-        <f>IF(ISBLANK(L4),-J4,L4-J4)</f>
+        <f t="shared" si="3"/>
         <v>41</v>
       </c>
       <c r="L4" s="1">
         <v>78653</v>
       </c>
       <c r="M4">
-        <f>IF(ISBLANK(N4),-L4,N4-L4)</f>
+        <f t="shared" si="4"/>
         <v>375</v>
       </c>
       <c r="N4" s="1">
         <v>79028</v>
       </c>
       <c r="O4">
-        <f>IF(ISBLANK(P4),-N4,P4-N4)</f>
+        <f t="shared" si="5"/>
         <v>409</v>
       </c>
       <c r="P4" s="1">
@@ -5238,42 +5376,42 @@
         <v>64500</v>
       </c>
       <c r="E5">
-        <f>IF(ISBLANK(F5),-D5,F5-D5)</f>
+        <f t="shared" si="0"/>
         <v>6036</v>
       </c>
       <c r="F5" s="1">
         <v>70536</v>
       </c>
       <c r="G5">
-        <f>IF(ISBLANK(H5),-F5,H5-F5)</f>
+        <f t="shared" si="1"/>
         <v>83</v>
       </c>
       <c r="H5" s="1">
         <v>70619</v>
       </c>
       <c r="I5">
-        <f>IF(ISBLANK(J5),-H5,J5-H5)</f>
+        <f t="shared" si="2"/>
         <v>41</v>
       </c>
       <c r="J5" s="1">
         <v>70660</v>
       </c>
       <c r="K5">
-        <f>IF(ISBLANK(L5),-J5,L5-J5)</f>
+        <f t="shared" si="3"/>
         <v>71</v>
       </c>
       <c r="L5" s="1">
         <v>70731</v>
       </c>
       <c r="M5">
-        <f>IF(ISBLANK(N5),-L5,N5-L5)</f>
+        <f t="shared" si="4"/>
         <v>694</v>
       </c>
       <c r="N5" s="1">
         <v>71425</v>
       </c>
       <c r="O5">
-        <f>IF(ISBLANK(P5),-N5,P5-N5)</f>
+        <f t="shared" si="5"/>
         <v>368</v>
       </c>
       <c r="P5" s="1">
@@ -5292,42 +5430,42 @@
         <v>56650</v>
       </c>
       <c r="E6">
-        <f>IF(ISBLANK(F6),-D6,F6-D6)</f>
+        <f t="shared" si="0"/>
         <v>1198</v>
       </c>
       <c r="F6" s="1">
         <v>57848</v>
       </c>
       <c r="G6">
-        <f>IF(ISBLANK(H6),-F6,H6-F6)</f>
+        <f t="shared" si="1"/>
         <v>44</v>
       </c>
       <c r="H6" s="1">
         <v>57892</v>
       </c>
       <c r="I6">
-        <f>IF(ISBLANK(J6),-H6,J6-H6)</f>
+        <f t="shared" si="2"/>
         <v>142</v>
       </c>
       <c r="J6" s="1">
         <v>58034</v>
       </c>
       <c r="K6">
-        <f>IF(ISBLANK(L6),-J6,L6-J6)</f>
+        <f t="shared" si="3"/>
         <v>178</v>
       </c>
       <c r="L6" s="1">
         <v>58212</v>
       </c>
       <c r="M6">
-        <f>IF(ISBLANK(N6),-L6,N6-L6)</f>
+        <f t="shared" si="4"/>
         <v>390</v>
       </c>
       <c r="N6" s="1">
         <v>58602</v>
       </c>
       <c r="O6">
-        <f>IF(ISBLANK(P6),-N6,P6-N6)</f>
+        <f t="shared" si="5"/>
         <v>1033</v>
       </c>
       <c r="P6" s="1">
@@ -5346,42 +5484,42 @@
         <v>51019</v>
       </c>
       <c r="E7">
-        <f>IF(ISBLANK(F7),-D7,F7-D7)</f>
+        <f t="shared" si="0"/>
         <v>1712</v>
       </c>
       <c r="F7" s="1">
         <v>52731</v>
       </c>
       <c r="G7">
-        <f>IF(ISBLANK(H7),-F7,H7-F7)</f>
+        <f t="shared" si="1"/>
         <v>90</v>
       </c>
       <c r="H7" s="1">
         <v>52821</v>
       </c>
       <c r="I7">
-        <f>IF(ISBLANK(J7),-H7,J7-H7)</f>
+        <f t="shared" si="2"/>
         <v>155</v>
       </c>
       <c r="J7" s="1">
         <v>52976</v>
       </c>
       <c r="K7">
-        <f>IF(ISBLANK(L7),-J7,L7-J7)</f>
+        <f t="shared" si="3"/>
         <v>92</v>
       </c>
       <c r="L7" s="1">
         <v>53068</v>
       </c>
       <c r="M7">
-        <f>IF(ISBLANK(N7),-L7,N7-L7)</f>
+        <f t="shared" si="4"/>
         <v>898</v>
       </c>
       <c r="N7" s="1">
         <v>53966</v>
       </c>
       <c r="O7">
-        <f>IF(ISBLANK(P7),-N7,P7-N7)</f>
+        <f t="shared" si="5"/>
         <v>582</v>
       </c>
       <c r="P7" s="1">
@@ -5400,42 +5538,42 @@
         <v>42814</v>
       </c>
       <c r="E8">
-        <f>IF(ISBLANK(F8),-D8,F8-D8)</f>
+        <f t="shared" si="0"/>
         <v>1226</v>
       </c>
       <c r="F8" s="1">
         <v>44040</v>
       </c>
       <c r="G8">
-        <f>IF(ISBLANK(H8),-F8,H8-F8)</f>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="H8" s="1">
         <v>44059</v>
       </c>
       <c r="I8">
-        <f>IF(ISBLANK(J8),-H8,J8-H8)</f>
+        <f t="shared" si="2"/>
         <v>17</v>
       </c>
       <c r="J8" s="1">
         <v>44076</v>
       </c>
       <c r="K8">
-        <f>IF(ISBLANK(L8),-J8,L8-J8)</f>
+        <f t="shared" si="3"/>
         <v>54</v>
       </c>
       <c r="L8" s="1">
         <v>44130</v>
       </c>
       <c r="M8">
-        <f>IF(ISBLANK(N8),-L8,N8-L8)</f>
+        <f t="shared" si="4"/>
         <v>125</v>
       </c>
       <c r="N8" s="1">
         <v>44255</v>
       </c>
       <c r="O8">
-        <f>IF(ISBLANK(P8),-N8,P8-N8)</f>
+        <f t="shared" si="5"/>
         <v>437</v>
       </c>
       <c r="P8" s="1">
@@ -5454,42 +5592,42 @@
         <v>30220</v>
       </c>
       <c r="E9">
-        <f>IF(ISBLANK(F9),-D9,F9-D9)</f>
+        <f t="shared" si="0"/>
         <v>864</v>
       </c>
       <c r="F9" s="1">
         <v>31084</v>
       </c>
       <c r="G9">
-        <f>IF(ISBLANK(H9),-F9,H9-F9)</f>
+        <f t="shared" si="1"/>
         <v>38</v>
       </c>
       <c r="H9" s="1">
         <v>31122</v>
       </c>
       <c r="I9">
-        <f>IF(ISBLANK(J9),-H9,J9-H9)</f>
+        <f t="shared" si="2"/>
         <v>21</v>
       </c>
       <c r="J9" s="1">
         <v>31143</v>
       </c>
       <c r="K9">
-        <f>IF(ISBLANK(L9),-J9,L9-J9)</f>
+        <f t="shared" si="3"/>
         <v>55</v>
       </c>
       <c r="L9" s="1">
         <v>31198</v>
       </c>
       <c r="M9">
-        <f>IF(ISBLANK(N9),-L9,N9-L9)</f>
+        <f t="shared" si="4"/>
         <v>273</v>
       </c>
       <c r="N9" s="1">
         <v>31471</v>
       </c>
       <c r="O9">
-        <f>IF(ISBLANK(P9),-N9,P9-N9)</f>
+        <f t="shared" si="5"/>
         <v>422</v>
       </c>
       <c r="P9" s="1">
@@ -5508,42 +5646,42 @@
         <v>15991</v>
       </c>
       <c r="E10">
-        <f>IF(ISBLANK(F10),-D10,F10-D10)</f>
+        <f t="shared" si="0"/>
         <v>477</v>
       </c>
       <c r="F10" s="1">
         <v>16468</v>
       </c>
       <c r="G10">
-        <f>IF(ISBLANK(H10),-F10,H10-F10)</f>
+        <f t="shared" si="1"/>
         <v>47</v>
       </c>
       <c r="H10" s="1">
         <v>16515</v>
       </c>
       <c r="I10">
-        <f>IF(ISBLANK(J10),-H10,J10-H10)</f>
+        <f t="shared" si="2"/>
         <v>106</v>
       </c>
       <c r="J10" s="1">
         <v>16621</v>
       </c>
       <c r="K10">
-        <f>IF(ISBLANK(L10),-J10,L10-J10)</f>
+        <f t="shared" si="3"/>
         <v>143</v>
       </c>
       <c r="L10" s="1">
         <v>16764</v>
       </c>
       <c r="M10">
-        <f>IF(ISBLANK(N10),-L10,N10-L10)</f>
+        <f t="shared" si="4"/>
         <v>826</v>
       </c>
       <c r="N10" s="1">
         <v>17590</v>
       </c>
       <c r="O10">
-        <f>IF(ISBLANK(P10),-N10,P10-N10)</f>
+        <f t="shared" si="5"/>
         <v>1722</v>
       </c>
       <c r="P10" s="1">
@@ -5562,42 +5700,42 @@
         <v>12378</v>
       </c>
       <c r="E11">
-        <f>IF(ISBLANK(F11),-D11,F11-D11)</f>
+        <f t="shared" si="0"/>
         <v>653</v>
       </c>
       <c r="F11" s="1">
         <v>13031</v>
       </c>
       <c r="G11">
-        <f>IF(ISBLANK(H11),-F11,H11-F11)</f>
+        <f t="shared" si="1"/>
         <v>34</v>
       </c>
       <c r="H11" s="1">
         <v>13065</v>
       </c>
       <c r="I11">
-        <f>IF(ISBLANK(J11),-H11,J11-H11)</f>
+        <f t="shared" si="2"/>
         <v>85</v>
       </c>
       <c r="J11" s="1">
         <v>13150</v>
       </c>
       <c r="K11">
-        <f>IF(ISBLANK(L11),-J11,L11-J11)</f>
+        <f t="shared" si="3"/>
         <v>47</v>
       </c>
       <c r="L11" s="1">
         <v>13197</v>
       </c>
       <c r="M11">
-        <f>IF(ISBLANK(N11),-L11,N11-L11)</f>
+        <f t="shared" si="4"/>
         <v>211</v>
       </c>
       <c r="N11" s="1">
         <v>13408</v>
       </c>
       <c r="O11">
-        <f>IF(ISBLANK(P11),-N11,P11-N11)</f>
+        <f t="shared" si="5"/>
         <v>315</v>
       </c>
       <c r="P11" s="1">
@@ -5616,42 +5754,42 @@
         <v>8130</v>
       </c>
       <c r="E12">
-        <f>IF(ISBLANK(F12),-D12,F12-D12)</f>
+        <f t="shared" si="0"/>
         <v>96</v>
       </c>
       <c r="F12" s="1">
         <v>8226</v>
       </c>
       <c r="G12">
-        <f>IF(ISBLANK(H12),-F12,H12-F12)</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="H12" s="1">
         <v>8246</v>
       </c>
       <c r="I12">
-        <f>IF(ISBLANK(J12),-H12,J12-H12)</f>
+        <f t="shared" si="2"/>
         <v>91</v>
       </c>
       <c r="J12" s="1">
         <v>8337</v>
       </c>
       <c r="K12">
-        <f>IF(ISBLANK(L12),-J12,L12-J12)</f>
+        <f t="shared" si="3"/>
         <v>28</v>
       </c>
       <c r="L12" s="1">
         <v>8365</v>
       </c>
       <c r="M12">
-        <f>IF(ISBLANK(N12),-L12,N12-L12)</f>
+        <f t="shared" si="4"/>
         <v>188</v>
       </c>
       <c r="N12" s="1">
         <v>8553</v>
       </c>
       <c r="O12">
-        <f>IF(ISBLANK(P12),-N12,P12-N12)</f>
+        <f t="shared" si="5"/>
         <v>146</v>
       </c>
       <c r="P12" s="1">
@@ -5670,42 +5808,42 @@
         <v>6897</v>
       </c>
       <c r="E13">
-        <f>IF(ISBLANK(F13),-D13,F13-D13)</f>
+        <f t="shared" si="0"/>
         <v>303</v>
       </c>
       <c r="F13" s="1">
         <v>7200</v>
       </c>
       <c r="G13">
-        <f>IF(ISBLANK(H13),-F13,H13-F13)</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="H13" s="1">
         <v>7220</v>
       </c>
       <c r="I13">
-        <f>IF(ISBLANK(J13),-H13,J13-H13)</f>
+        <f t="shared" si="2"/>
         <v>84</v>
       </c>
       <c r="J13" s="1">
         <v>7304</v>
       </c>
       <c r="K13">
-        <f>IF(ISBLANK(L13),-J13,L13-J13)</f>
+        <f t="shared" si="3"/>
         <v>141</v>
       </c>
       <c r="L13" s="1">
         <v>7445</v>
       </c>
       <c r="M13">
-        <f>IF(ISBLANK(N13),-L13,N13-L13)</f>
+        <f t="shared" si="4"/>
         <v>232</v>
       </c>
       <c r="N13" s="1">
         <v>7677</v>
       </c>
       <c r="O13">
-        <f>IF(ISBLANK(P13),-N13,P13-N13)</f>
+        <f t="shared" si="5"/>
         <v>-7677</v>
       </c>
       <c r="P13" s="1">
@@ -5724,42 +5862,42 @@
         <v>3132</v>
       </c>
       <c r="E14">
-        <f>IF(ISBLANK(F14),-D14,F14-D14)</f>
+        <f t="shared" si="0"/>
         <v>104</v>
       </c>
       <c r="F14" s="1">
         <v>3236</v>
       </c>
       <c r="G14">
-        <f>IF(ISBLANK(H14),-F14,H14-F14)</f>
+        <f t="shared" si="1"/>
         <v>77</v>
       </c>
       <c r="H14" s="1">
         <v>3313</v>
       </c>
       <c r="I14">
-        <f>IF(ISBLANK(J14),-H14,J14-H14)</f>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="J14" s="1">
         <v>3326</v>
       </c>
       <c r="K14">
-        <f>IF(ISBLANK(L14),-J14,L14-J14)</f>
+        <f t="shared" si="3"/>
         <v>151</v>
       </c>
       <c r="L14" s="1">
         <v>3477</v>
       </c>
       <c r="M14">
-        <f>IF(ISBLANK(N14),-L14,N14-L14)</f>
+        <f t="shared" si="4"/>
         <v>-3477</v>
       </c>
       <c r="N14" s="1">
         <v>0</v>
       </c>
       <c r="O14">
-        <f>IF(ISBLANK(P14),-N14,P14-N14)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P14" s="1">
@@ -5778,42 +5916,42 @@
         <v>2450</v>
       </c>
       <c r="E15">
-        <f>IF(ISBLANK(F15),-D15,F15-D15)</f>
+        <f t="shared" si="0"/>
         <v>112</v>
       </c>
       <c r="F15" s="1">
         <v>2562</v>
       </c>
       <c r="G15">
-        <f>IF(ISBLANK(H15),-F15,H15-F15)</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="H15" s="1">
         <v>2577</v>
       </c>
       <c r="I15">
-        <f>IF(ISBLANK(J15),-H15,J15-H15)</f>
+        <f t="shared" si="2"/>
         <v>77</v>
       </c>
       <c r="J15" s="1">
         <v>2654</v>
       </c>
       <c r="K15">
-        <f>IF(ISBLANK(L15),-J15,L15-J15)</f>
+        <f t="shared" si="3"/>
         <v>40</v>
       </c>
       <c r="L15" s="1">
         <v>2694</v>
       </c>
       <c r="M15">
-        <f>IF(ISBLANK(N15),-L15,N15-L15)</f>
+        <f t="shared" si="4"/>
         <v>-2694</v>
       </c>
       <c r="N15" s="1">
         <v>0</v>
       </c>
       <c r="O15">
-        <f>IF(ISBLANK(P15),-N15,P15-N15)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P15" s="1">
@@ -5832,42 +5970,42 @@
         <v>1352</v>
       </c>
       <c r="E16">
-        <f>IF(ISBLANK(F16),-D16,F16-D16)</f>
+        <f t="shared" si="0"/>
         <v>48</v>
       </c>
       <c r="F16" s="1">
         <v>1400</v>
       </c>
       <c r="G16">
-        <f>IF(ISBLANK(H16),-F16,H16-F16)</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="H16" s="1">
         <v>1412</v>
       </c>
       <c r="I16">
-        <f>IF(ISBLANK(J16),-H16,J16-H16)</f>
+        <f t="shared" si="2"/>
         <v>-1412</v>
       </c>
       <c r="J16" s="1">
         <v>0</v>
       </c>
       <c r="K16">
-        <f>IF(ISBLANK(L16),-J16,L16-J16)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L16" s="1">
         <v>0</v>
       </c>
       <c r="M16">
-        <f>IF(ISBLANK(N16),-L16,N16-L16)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N16" s="1">
         <v>0</v>
       </c>
       <c r="O16">
-        <f>IF(ISBLANK(P16),-N16,P16-N16)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P16" s="1">
@@ -5886,42 +6024,42 @@
         <v>1322</v>
       </c>
       <c r="E17">
-        <f>IF(ISBLANK(F17),-D17,F17-D17)</f>
+        <f t="shared" si="0"/>
         <v>53</v>
       </c>
       <c r="F17" s="1">
         <v>1375</v>
       </c>
       <c r="G17">
-        <f>IF(ISBLANK(H17),-F17,H17-F17)</f>
+        <f t="shared" si="1"/>
         <v>71</v>
       </c>
       <c r="H17" s="1">
         <v>1446</v>
       </c>
       <c r="I17">
-        <f>IF(ISBLANK(J17),-H17,J17-H17)</f>
+        <f t="shared" si="2"/>
         <v>44</v>
       </c>
       <c r="J17" s="1">
         <v>1490</v>
       </c>
       <c r="K17">
-        <f>IF(ISBLANK(L17),-J17,L17-J17)</f>
+        <f t="shared" si="3"/>
         <v>-1490</v>
       </c>
       <c r="L17" s="1">
         <v>0</v>
       </c>
       <c r="M17">
-        <f>IF(ISBLANK(N17),-L17,N17-L17)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N17" s="1">
         <v>0</v>
       </c>
       <c r="O17">
-        <f>IF(ISBLANK(P17),-N17,P17-N17)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P17" s="1">
@@ -5940,42 +6078,42 @@
         <v>789</v>
       </c>
       <c r="E18">
-        <f>IF(ISBLANK(F18),-D18,F18-D18)</f>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="F18">
         <v>811</v>
       </c>
       <c r="G18">
-        <f>IF(ISBLANK(H18),-F18,H18-F18)</f>
+        <f t="shared" si="1"/>
         <v>-811</v>
       </c>
       <c r="H18" s="1">
         <v>0</v>
       </c>
       <c r="I18">
-        <f>IF(ISBLANK(J18),-H18,J18-H18)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J18" s="1">
         <v>0</v>
       </c>
       <c r="K18">
-        <f>IF(ISBLANK(L18),-J18,L18-J18)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L18" s="1">
         <v>0</v>
       </c>
       <c r="M18">
-        <f>IF(ISBLANK(N18),-L18,N18-L18)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N18" s="1">
         <v>0</v>
       </c>
       <c r="O18">
-        <f>IF(ISBLANK(P18),-N18,P18-N18)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P18" s="1">
@@ -6056,19 +6194,19 @@
         <v>197</v>
       </c>
       <c r="D21">
-        <f t="shared" ref="D21:D36" si="0">FIND(",",B21)</f>
+        <f t="shared" ref="D21:D36" si="6">FIND(",",B21)</f>
         <v>9</v>
       </c>
       <c r="E21" t="str">
-        <f t="shared" ref="E21:E36" si="1">LEFT(B21,D21-1)</f>
+        <f t="shared" ref="E21:E36" si="7">LEFT(B21,D21-1)</f>
         <v>Flanagan</v>
       </c>
       <c r="F21" t="str">
-        <f t="shared" ref="F21:F36" si="2">RIGHT(B21,LEN(B21)-(D21+1))</f>
+        <f t="shared" ref="F21:F36" si="8">RIGHT(B21,LEN(B21)-(D21+1))</f>
         <v>Luke 'Ming'</v>
       </c>
       <c r="G21" t="str">
-        <f t="shared" ref="G21:G36" si="3">F21&amp;" "&amp;E21</f>
+        <f t="shared" ref="G21:G36" si="9">F21&amp;" "&amp;E21</f>
         <v>Luke 'Ming' Flanagan</v>
       </c>
       <c r="J21" t="s">
@@ -6094,19 +6232,19 @@
         <v>198</v>
       </c>
       <c r="D22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="E22" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>Carthy</v>
       </c>
       <c r="F22" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>Matt</v>
       </c>
       <c r="G22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>Matt Carthy</v>
       </c>
       <c r="J22" t="s">
@@ -6169,19 +6307,19 @@
         <v>199</v>
       </c>
       <c r="D23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="E23" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>Walsh</v>
       </c>
       <c r="F23" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>Maria</v>
       </c>
       <c r="G23" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>Maria Walsh</v>
       </c>
       <c r="J23" t="s">
@@ -6244,19 +6382,19 @@
         <v>200</v>
       </c>
       <c r="D24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="E24" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>Casey</v>
       </c>
       <c r="F24" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>Peter</v>
       </c>
       <c r="G24" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>Peter Casey</v>
       </c>
       <c r="J24" t="s">
@@ -6319,19 +6457,19 @@
         <v>201</v>
       </c>
       <c r="D25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="E25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>McHugh</v>
       </c>
       <c r="F25" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>Saoirse</v>
       </c>
       <c r="G25" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>Saoirse McHugh</v>
       </c>
       <c r="J25" t="s">
@@ -6394,19 +6532,19 @@
         <v>202</v>
       </c>
       <c r="D26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="E26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>Smith</v>
       </c>
       <c r="F26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>Brendan</v>
       </c>
       <c r="G26" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>Brendan Smith</v>
       </c>
       <c r="J26" t="s">
@@ -6469,19 +6607,19 @@
         <v>203</v>
       </c>
       <c r="D27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>9</v>
       </c>
       <c r="E27" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>Rabbitte</v>
       </c>
       <c r="F27" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>Anne</v>
       </c>
       <c r="G27" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>Anne Rabbitte</v>
       </c>
       <c r="J27" t="s">
@@ -6544,19 +6682,19 @@
         <v>204</v>
       </c>
       <c r="D28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>12</v>
       </c>
       <c r="E28" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>Healy Eames</v>
       </c>
       <c r="F28" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>Fidelma</v>
       </c>
       <c r="G28" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>Fidelma Healy Eames</v>
       </c>
       <c r="J28" t="s">
@@ -6619,19 +6757,19 @@
         <v>205</v>
       </c>
       <c r="D29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>9</v>
       </c>
       <c r="E29" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>Hannigan</v>
       </c>
       <c r="F29" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>Dominic</v>
       </c>
       <c r="G29" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>Dominic Hannigan</v>
       </c>
       <c r="J29" t="s">
@@ -6694,19 +6832,19 @@
         <v>206</v>
       </c>
       <c r="D30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="E30" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>Brennan</v>
       </c>
       <c r="F30" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>Cyril</v>
       </c>
       <c r="G30" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>Cyril Brennan</v>
       </c>
       <c r="J30" t="s">
@@ -6769,19 +6907,19 @@
         <v>207</v>
       </c>
       <c r="D31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="E31" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>O'Dowd</v>
       </c>
       <c r="F31" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>Michael</v>
       </c>
       <c r="G31" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>Michael O'Dowd</v>
       </c>
       <c r="J31" t="s">
@@ -6844,19 +6982,19 @@
         <v>208</v>
       </c>
       <c r="D32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>9</v>
       </c>
       <c r="E32" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>O'Connor</v>
       </c>
       <c r="F32" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>Olive</v>
       </c>
       <c r="G32" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>Olive O'Connor</v>
       </c>
       <c r="J32" t="s">
@@ -6916,19 +7054,19 @@
         <v>209</v>
       </c>
       <c r="D33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="E33" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>Mahapatra</v>
       </c>
       <c r="F33" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>Dilip</v>
       </c>
       <c r="G33" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>Dilip Mahapatra</v>
       </c>
       <c r="J33" t="s">
@@ -6982,19 +7120,19 @@
         <v>210</v>
       </c>
       <c r="D34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="E34" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>Greene</v>
       </c>
       <c r="F34" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>Patrick</v>
       </c>
       <c r="G34" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>Patrick Greene</v>
       </c>
       <c r="J34" t="s">
@@ -7048,19 +7186,19 @@
         <v>211</v>
       </c>
       <c r="D35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="E35" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>Miller</v>
       </c>
       <c r="F35" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>James</v>
       </c>
       <c r="G35" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>James Miller</v>
       </c>
       <c r="J35" t="s">
@@ -7100,19 +7238,19 @@
         <v>212</v>
       </c>
       <c r="D36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="E36" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>Mulcahy</v>
       </c>
       <c r="F36" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>Diarmaid</v>
       </c>
       <c r="G36" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>Diarmaid Mulcahy</v>
       </c>
       <c r="J36" t="s">

</xml_diff>

<commit_message>
Stage 10 South added Signed-off-by: Gerry Mulvenna <git@movingwifi.com>
</commit_message>
<xml_diff>
--- a/europarl/europarl-ireland-2019.xlsx
+++ b/europarl/europarl-ireland-2019.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="14220" windowHeight="8580" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="14220" windowHeight="8580" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Candidates" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="263">
   <si>
     <t>Candidate</t>
   </si>
@@ -2469,7 +2469,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="AF2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -7326,10 +7326,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD49"/>
+  <dimension ref="A1:AE49"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="S2" sqref="S2:T24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7390,1546 +7390,1707 @@
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
       <c r="D2" s="1">
-        <v>4665</v>
+        <v>118444</v>
       </c>
       <c r="E2">
-        <f t="shared" ref="E2:E24" si="0">IF(ISBLANK(F2),-D2,F2-D2)</f>
-        <v>26</v>
+        <f>IF(ISBLANK(F2),-D2,F2-D2)</f>
+        <v>45</v>
       </c>
       <c r="F2" s="1">
-        <v>4691</v>
+        <v>118489</v>
       </c>
       <c r="G2">
-        <f t="shared" ref="G2:G24" si="1">IF(ISBLANK(H2),-F2,H2-F2)</f>
-        <v>43</v>
+        <f>IF(ISBLANK(H2),-F2,H2-F2)</f>
+        <v>186</v>
       </c>
       <c r="H2" s="1">
-        <v>4734</v>
+        <v>118675</v>
       </c>
       <c r="I2">
-        <f t="shared" ref="I2:I24" si="2">IF(ISBLANK(J2),-H2,J2-H2)</f>
-        <v>57</v>
+        <f>IF(ISBLANK(J2),-H2,J2-H2)</f>
+        <v>98</v>
       </c>
       <c r="J2" s="1">
-        <v>4791</v>
+        <v>118773</v>
       </c>
       <c r="K2">
-        <f t="shared" ref="K2:K24" si="3">IF(ISBLANK(L2),-J2,L2-J2)</f>
-        <v>50</v>
+        <f>IF(ISBLANK(L2),-J2,L2-J2)</f>
+        <v>350</v>
       </c>
       <c r="L2" s="1">
-        <v>4841</v>
+        <v>119123</v>
       </c>
       <c r="M2">
-        <f t="shared" ref="M2:M24" si="4">IF(ISBLANK(N2),-L2,N2-L2)</f>
-        <v>115</v>
+        <f>IF(ISBLANK(N2),-L2,N2-L2)</f>
+        <v>257</v>
       </c>
       <c r="N2" s="1">
-        <v>4956</v>
+        <v>119380</v>
       </c>
       <c r="O2">
-        <f t="shared" ref="O2:O24" si="5">IF(ISBLANK(P2),-N2,P2-N2)</f>
-        <v>72</v>
+        <f>IF(ISBLANK(P2),-N2,P2-N2)</f>
+        <v>165</v>
       </c>
       <c r="P2" s="1">
-        <v>5028</v>
+        <v>119545</v>
       </c>
       <c r="Q2">
-        <f t="shared" ref="Q2:Q24" si="6">IF(ISBLANK(R2),-P2,R2-P2)</f>
-        <v>104</v>
+        <f>IF(ISBLANK(R2),-P2,R2-P2)</f>
+        <v>170</v>
       </c>
       <c r="R2" s="1">
-        <v>5132</v>
+        <v>119715</v>
       </c>
       <c r="S2">
-        <f t="shared" ref="S2:S24" si="7">IF(ISBLANK(T2),-R2,T2-R2)</f>
-        <v>-5132</v>
+        <f>IF(ISBLANK(T2),-R2,T2-R2)</f>
+        <v>168</v>
       </c>
       <c r="T2" s="1">
-        <v>0</v>
+        <v>119883</v>
+      </c>
+      <c r="U2">
+        <f>IF(ISBLANK(V2),-T2,V2-T2)</f>
+        <v>0</v>
+      </c>
+      <c r="V2" s="1">
+        <v>119883</v>
       </c>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D3" s="1">
-        <v>69166</v>
+        <v>84083</v>
       </c>
       <c r="E3">
-        <f t="shared" si="0"/>
-        <v>35</v>
+        <f>IF(ISBLANK(F3),-D3,F3-D3)</f>
+        <v>23</v>
       </c>
       <c r="F3" s="1">
-        <v>69201</v>
+        <v>84106</v>
       </c>
       <c r="G3">
-        <f t="shared" si="1"/>
-        <v>71</v>
+        <f>IF(ISBLANK(H3),-F3,H3-F3)</f>
+        <v>58</v>
       </c>
       <c r="H3" s="1">
-        <v>69272</v>
+        <v>84164</v>
       </c>
       <c r="I3">
-        <f t="shared" si="2"/>
-        <v>44</v>
+        <f>IF(ISBLANK(J3),-H3,J3-H3)</f>
+        <v>74</v>
       </c>
       <c r="J3" s="1">
-        <v>69316</v>
+        <v>84238</v>
       </c>
       <c r="K3">
-        <f t="shared" si="3"/>
-        <v>66</v>
+        <f>IF(ISBLANK(L3),-J3,L3-J3)</f>
+        <v>150</v>
       </c>
       <c r="L3" s="1">
-        <v>69382</v>
+        <v>84388</v>
       </c>
       <c r="M3">
-        <f t="shared" si="4"/>
-        <v>129</v>
+        <f>IF(ISBLANK(N3),-L3,N3-L3)</f>
+        <v>171</v>
       </c>
       <c r="N3" s="1">
-        <v>69511</v>
+        <v>84559</v>
       </c>
       <c r="O3">
-        <f t="shared" si="5"/>
-        <v>45</v>
+        <f>IF(ISBLANK(P3),-N3,P3-N3)</f>
+        <v>95</v>
       </c>
       <c r="P3" s="1">
-        <v>69556</v>
+        <v>84654</v>
       </c>
       <c r="Q3">
-        <f t="shared" si="6"/>
-        <v>116</v>
+        <f>IF(ISBLANK(R3),-P3,R3-P3)</f>
+        <v>187</v>
       </c>
       <c r="R3" s="1">
-        <v>69672</v>
+        <v>84841</v>
       </c>
       <c r="S3">
-        <f t="shared" si="7"/>
-        <v>1226</v>
+        <f>IF(ISBLANK(T3),-R3,T3-R3)</f>
+        <v>130</v>
       </c>
       <c r="T3" s="1">
-        <v>70898</v>
+        <v>84971</v>
+      </c>
+      <c r="U3">
+        <f>IF(ISBLANK(V3),-T3,V3-T3)</f>
+        <v>480</v>
+      </c>
+      <c r="V3" s="1">
+        <v>85451</v>
       </c>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="D4" s="1">
-        <v>10582</v>
+        <v>81741</v>
       </c>
       <c r="E4">
-        <f t="shared" si="0"/>
-        <v>57</v>
+        <f>IF(ISBLANK(F4),-D4,F4-D4)</f>
+        <v>253</v>
       </c>
       <c r="F4" s="1">
-        <v>10639</v>
+        <v>81994</v>
       </c>
       <c r="G4">
-        <f t="shared" si="1"/>
-        <v>106</v>
+        <f>IF(ISBLANK(H4),-F4,H4-F4)</f>
+        <v>130</v>
       </c>
       <c r="H4" s="1">
-        <v>10745</v>
+        <v>82124</v>
       </c>
       <c r="I4">
-        <f t="shared" si="2"/>
-        <v>138</v>
+        <f>IF(ISBLANK(J4),-H4,J4-H4)</f>
+        <v>211</v>
       </c>
       <c r="J4" s="1">
-        <v>10883</v>
+        <v>82335</v>
       </c>
       <c r="K4">
-        <f t="shared" si="3"/>
-        <v>54</v>
+        <f>IF(ISBLANK(L4),-J4,L4-J4)</f>
+        <v>323</v>
       </c>
       <c r="L4" s="1">
-        <v>10937</v>
+        <v>82658</v>
       </c>
       <c r="M4">
-        <f t="shared" si="4"/>
-        <v>300</v>
+        <f>IF(ISBLANK(N4),-L4,N4-L4)</f>
+        <v>206</v>
       </c>
       <c r="N4" s="1">
-        <v>11237</v>
+        <v>82864</v>
       </c>
       <c r="O4">
-        <f t="shared" si="5"/>
-        <v>159</v>
+        <f>IF(ISBLANK(P4),-N4,P4-N4)</f>
+        <v>556</v>
       </c>
       <c r="P4" s="1">
-        <v>11396</v>
+        <v>83420</v>
       </c>
       <c r="Q4">
-        <f t="shared" si="6"/>
-        <v>322</v>
+        <f>IF(ISBLANK(R4),-P4,R4-P4)</f>
+        <v>351</v>
       </c>
       <c r="R4" s="1">
-        <v>11718</v>
+        <v>83771</v>
       </c>
       <c r="S4">
-        <f t="shared" si="7"/>
-        <v>908</v>
+        <f>IF(ISBLANK(T4),-R4,T4-R4)</f>
+        <v>217</v>
       </c>
       <c r="T4" s="1">
-        <v>12626</v>
+        <v>83988</v>
+      </c>
+      <c r="U4">
+        <f>IF(ISBLANK(V4),-T4,V4-T4)</f>
+        <v>247</v>
+      </c>
+      <c r="V4" s="1">
+        <v>84235</v>
       </c>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D5" s="1">
-        <v>64605</v>
+        <v>79072</v>
       </c>
       <c r="E5">
-        <f t="shared" si="0"/>
-        <v>26</v>
+        <f>IF(ISBLANK(F5),-D5,F5-D5)</f>
+        <v>68</v>
       </c>
       <c r="F5" s="1">
-        <v>64631</v>
+        <v>79140</v>
       </c>
       <c r="G5">
-        <f t="shared" si="1"/>
-        <v>61</v>
+        <f>IF(ISBLANK(H5),-F5,H5-F5)</f>
+        <v>142</v>
       </c>
       <c r="H5" s="1">
-        <v>64692</v>
+        <v>79282</v>
       </c>
       <c r="I5">
-        <f t="shared" si="2"/>
-        <v>71</v>
+        <f>IF(ISBLANK(J5),-H5,J5-H5)</f>
+        <v>105</v>
       </c>
       <c r="J5" s="1">
-        <v>64763</v>
+        <v>79387</v>
       </c>
       <c r="K5">
-        <f t="shared" si="3"/>
-        <v>136</v>
+        <f>IF(ISBLANK(L5),-J5,L5-J5)</f>
+        <v>186</v>
       </c>
       <c r="L5" s="1">
-        <v>64899</v>
+        <v>79573</v>
       </c>
       <c r="M5">
-        <f t="shared" si="4"/>
-        <v>106</v>
+        <f>IF(ISBLANK(N5),-L5,N5-L5)</f>
+        <v>168</v>
       </c>
       <c r="N5" s="1">
-        <v>65005</v>
+        <v>79741</v>
       </c>
       <c r="O5">
-        <f t="shared" si="5"/>
-        <v>110</v>
+        <f>IF(ISBLANK(P5),-N5,P5-N5)</f>
+        <v>204</v>
       </c>
       <c r="P5" s="1">
-        <v>65115</v>
+        <v>79945</v>
       </c>
       <c r="Q5">
-        <f t="shared" si="6"/>
-        <v>137</v>
+        <f>IF(ISBLANK(R5),-P5,R5-P5)</f>
+        <v>305</v>
       </c>
       <c r="R5" s="1">
-        <v>65252</v>
+        <v>80250</v>
       </c>
       <c r="S5">
-        <f t="shared" si="7"/>
-        <v>306</v>
+        <f>IF(ISBLANK(T5),-R5,T5-R5)</f>
+        <v>127</v>
       </c>
       <c r="T5" s="1">
-        <v>65558</v>
+        <v>80377</v>
+      </c>
+      <c r="U5">
+        <f>IF(ISBLANK(V5),-T5,V5-T5)</f>
+        <v>446</v>
+      </c>
+      <c r="V5" s="1">
+        <v>80823</v>
       </c>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D6" s="1">
-        <v>38738</v>
+        <v>75946</v>
       </c>
       <c r="E6">
-        <f t="shared" si="0"/>
-        <v>17</v>
+        <f>IF(ISBLANK(F6),-D6,F6-D6)</f>
+        <v>100</v>
       </c>
       <c r="F6" s="1">
-        <v>38755</v>
+        <v>76046</v>
       </c>
       <c r="G6">
-        <f t="shared" si="1"/>
-        <v>33</v>
+        <f>IF(ISBLANK(H6),-F6,H6-F6)</f>
+        <v>201</v>
       </c>
       <c r="H6" s="1">
-        <v>38788</v>
+        <v>76247</v>
       </c>
       <c r="I6">
-        <f t="shared" si="2"/>
-        <v>16</v>
+        <f>IF(ISBLANK(J6),-H6,J6-H6)</f>
+        <v>126</v>
       </c>
       <c r="J6" s="1">
-        <v>38804</v>
+        <v>76373</v>
       </c>
       <c r="K6">
-        <f t="shared" si="3"/>
-        <v>38</v>
+        <f>IF(ISBLANK(L6),-J6,L6-J6)</f>
+        <v>272</v>
       </c>
       <c r="L6" s="1">
-        <v>38842</v>
+        <v>76645</v>
       </c>
       <c r="M6">
-        <f t="shared" si="4"/>
-        <v>84</v>
+        <f>IF(ISBLANK(N6),-L6,N6-L6)</f>
+        <v>74</v>
       </c>
       <c r="N6" s="1">
-        <v>38926</v>
+        <v>76719</v>
       </c>
       <c r="O6">
-        <f t="shared" si="5"/>
-        <v>24</v>
+        <f>IF(ISBLANK(P6),-N6,P6-N6)</f>
+        <v>301</v>
       </c>
       <c r="P6" s="1">
-        <v>38950</v>
+        <v>77020</v>
       </c>
       <c r="Q6">
-        <f t="shared" si="6"/>
-        <v>46</v>
+        <f>IF(ISBLANK(R6),-P6,R6-P6)</f>
+        <v>283</v>
       </c>
       <c r="R6" s="1">
-        <v>38996</v>
+        <v>77303</v>
       </c>
       <c r="S6">
-        <f t="shared" si="7"/>
-        <v>298</v>
+        <f>IF(ISBLANK(T6),-R6,T6-R6)</f>
+        <v>112</v>
       </c>
       <c r="T6" s="1">
-        <v>39294</v>
+        <v>77415</v>
+      </c>
+      <c r="U6">
+        <f>IF(ISBLANK(V6),-T6,V6-T6)</f>
+        <v>339</v>
+      </c>
+      <c r="V6" s="1">
+        <v>77754</v>
       </c>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="D7" s="1">
-        <v>3182</v>
+        <v>69166</v>
       </c>
       <c r="E7">
-        <f t="shared" si="0"/>
-        <v>15</v>
+        <f>IF(ISBLANK(F7),-D7,F7-D7)</f>
+        <v>35</v>
       </c>
       <c r="F7" s="1">
-        <v>3197</v>
+        <v>69201</v>
       </c>
       <c r="G7">
-        <f t="shared" si="1"/>
-        <v>60</v>
+        <f>IF(ISBLANK(H7),-F7,H7-F7)</f>
+        <v>71</v>
       </c>
       <c r="H7" s="1">
-        <v>3257</v>
+        <v>69272</v>
       </c>
       <c r="I7">
-        <f t="shared" si="2"/>
-        <v>43</v>
+        <f>IF(ISBLANK(J7),-H7,J7-H7)</f>
+        <v>44</v>
       </c>
       <c r="J7" s="1">
-        <v>3300</v>
+        <v>69316</v>
       </c>
       <c r="K7">
-        <f t="shared" si="3"/>
-        <v>32</v>
+        <f>IF(ISBLANK(L7),-J7,L7-J7)</f>
+        <v>66</v>
       </c>
       <c r="L7" s="1">
-        <v>3332</v>
+        <v>69382</v>
       </c>
       <c r="M7">
-        <f t="shared" si="4"/>
-        <v>-3332</v>
+        <f>IF(ISBLANK(N7),-L7,N7-L7)</f>
+        <v>129</v>
       </c>
       <c r="N7" s="1">
-        <v>0</v>
+        <v>69511</v>
       </c>
       <c r="O7">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f>IF(ISBLANK(P7),-N7,P7-N7)</f>
+        <v>45</v>
       </c>
       <c r="P7" s="1">
-        <v>0</v>
+        <v>69556</v>
       </c>
       <c r="Q7">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f>IF(ISBLANK(R7),-P7,R7-P7)</f>
+        <v>116</v>
       </c>
       <c r="R7" s="1">
-        <v>0</v>
+        <v>69672</v>
       </c>
       <c r="S7">
-        <f t="shared" si="7"/>
-        <v>0</v>
+        <f>IF(ISBLANK(T7),-R7,T7-R7)</f>
+        <v>1226</v>
       </c>
       <c r="T7" s="1">
-        <v>0</v>
+        <v>70898</v>
+      </c>
+      <c r="U7">
+        <f>IF(ISBLANK(V7),-T7,V7-T7)</f>
+        <v>270</v>
+      </c>
+      <c r="V7" s="1">
+        <v>71168</v>
       </c>
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>130</v>
+      </c>
+      <c r="D8" s="1">
+        <v>64605</v>
+      </c>
+      <c r="E8">
+        <f>IF(ISBLANK(F8),-D8,F8-D8)</f>
+        <v>26</v>
+      </c>
+      <c r="F8" s="1">
+        <v>64631</v>
+      </c>
+      <c r="G8">
+        <f>IF(ISBLANK(H8),-F8,H8-F8)</f>
+        <v>61</v>
+      </c>
+      <c r="H8" s="1">
+        <v>64692</v>
+      </c>
+      <c r="I8">
+        <f>IF(ISBLANK(J8),-H8,J8-H8)</f>
+        <v>71</v>
+      </c>
+      <c r="J8" s="1">
+        <v>64763</v>
+      </c>
+      <c r="K8">
+        <f>IF(ISBLANK(L8),-J8,L8-J8)</f>
+        <v>136</v>
+      </c>
+      <c r="L8" s="1">
+        <v>64899</v>
+      </c>
+      <c r="M8">
+        <f>IF(ISBLANK(N8),-L8,N8-L8)</f>
+        <v>106</v>
+      </c>
+      <c r="N8" s="1">
+        <v>65005</v>
+      </c>
+      <c r="O8">
+        <f>IF(ISBLANK(P8),-N8,P8-N8)</f>
+        <v>110</v>
+      </c>
+      <c r="P8" s="1">
+        <v>65115</v>
+      </c>
+      <c r="Q8">
+        <f>IF(ISBLANK(R8),-P8,R8-P8)</f>
         <v>137</v>
       </c>
-      <c r="D8" s="1">
-        <v>9306</v>
-      </c>
-      <c r="E8">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="F8" s="1">
-        <v>9331</v>
-      </c>
-      <c r="G8">
-        <f t="shared" si="1"/>
-        <v>70</v>
-      </c>
-      <c r="H8" s="1">
-        <v>9401</v>
-      </c>
-      <c r="I8">
-        <f t="shared" si="2"/>
-        <v>35</v>
-      </c>
-      <c r="J8" s="1">
-        <v>9436</v>
-      </c>
-      <c r="K8">
-        <f t="shared" si="3"/>
-        <v>60</v>
-      </c>
-      <c r="L8" s="1">
-        <v>9496</v>
-      </c>
-      <c r="M8">
-        <f t="shared" si="4"/>
-        <v>228</v>
-      </c>
-      <c r="N8" s="1">
-        <v>9724</v>
-      </c>
-      <c r="O8">
-        <f t="shared" si="5"/>
-        <v>145</v>
-      </c>
-      <c r="P8" s="1">
-        <v>9869</v>
-      </c>
-      <c r="Q8">
-        <f t="shared" si="6"/>
-        <v>106</v>
-      </c>
       <c r="R8" s="1">
-        <v>9975</v>
+        <v>65252</v>
       </c>
       <c r="S8">
-        <f t="shared" si="7"/>
-        <v>247</v>
+        <f>IF(ISBLANK(T8),-R8,T8-R8)</f>
+        <v>306</v>
       </c>
       <c r="T8" s="1">
-        <v>10222</v>
+        <v>65558</v>
+      </c>
+      <c r="U8">
+        <f>IF(ISBLANK(V8),-T8,V8-T8)</f>
+        <v>491</v>
+      </c>
+      <c r="V8" s="1">
+        <v>66049</v>
       </c>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="D9" s="1">
-        <v>7475</v>
+        <v>38738</v>
       </c>
       <c r="E9">
-        <f t="shared" si="0"/>
-        <v>23</v>
+        <f>IF(ISBLANK(F9),-D9,F9-D9)</f>
+        <v>17</v>
       </c>
       <c r="F9" s="1">
-        <v>7498</v>
+        <v>38755</v>
       </c>
       <c r="G9">
-        <f t="shared" si="1"/>
-        <v>98</v>
+        <f>IF(ISBLANK(H9),-F9,H9-F9)</f>
+        <v>33</v>
       </c>
       <c r="H9" s="1">
-        <v>7596</v>
+        <v>38788</v>
       </c>
       <c r="I9">
-        <f t="shared" si="2"/>
-        <v>142</v>
+        <f>IF(ISBLANK(J9),-H9,J9-H9)</f>
+        <v>16</v>
       </c>
       <c r="J9" s="1">
-        <v>7738</v>
+        <v>38804</v>
       </c>
       <c r="K9">
-        <f t="shared" si="3"/>
-        <v>70</v>
+        <f>IF(ISBLANK(L9),-J9,L9-J9)</f>
+        <v>38</v>
       </c>
       <c r="L9" s="1">
-        <v>7808</v>
+        <v>38842</v>
       </c>
       <c r="M9">
-        <f t="shared" si="4"/>
-        <v>197</v>
+        <f>IF(ISBLANK(N9),-L9,N9-L9)</f>
+        <v>84</v>
       </c>
       <c r="N9" s="1">
-        <v>8005</v>
+        <v>38926</v>
       </c>
       <c r="O9">
-        <f t="shared" si="5"/>
-        <v>192</v>
+        <f>IF(ISBLANK(P9),-N9,P9-N9)</f>
+        <v>24</v>
       </c>
       <c r="P9" s="1">
-        <v>8197</v>
+        <v>38950</v>
       </c>
       <c r="Q9">
-        <f t="shared" si="6"/>
-        <v>176</v>
+        <f>IF(ISBLANK(R9),-P9,R9-P9)</f>
+        <v>46</v>
       </c>
       <c r="R9" s="1">
-        <v>8373</v>
+        <v>38996</v>
       </c>
       <c r="S9">
-        <f t="shared" si="7"/>
-        <v>188</v>
+        <f>IF(ISBLANK(T9),-R9,T9-R9)</f>
+        <v>298</v>
       </c>
       <c r="T9" s="1">
-        <v>8561</v>
+        <v>39294</v>
+      </c>
+      <c r="U9">
+        <f>IF(ISBLANK(V9),-T9,V9-T9)</f>
+        <v>135</v>
+      </c>
+      <c r="V9" s="1">
+        <v>39429</v>
       </c>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="D10" s="1">
-        <v>84083</v>
+        <v>22075</v>
       </c>
       <c r="E10">
-        <f t="shared" si="0"/>
-        <v>23</v>
+        <f>IF(ISBLANK(F10),-D10,F10-D10)</f>
+        <v>38</v>
       </c>
       <c r="F10" s="1">
-        <v>84106</v>
+        <v>22113</v>
       </c>
       <c r="G10">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H10),-F10,H10-F10)</f>
+        <v>80</v>
+      </c>
+      <c r="H10" s="1">
+        <v>22193</v>
+      </c>
+      <c r="I10">
+        <f>IF(ISBLANK(J10),-H10,J10-H10)</f>
         <v>58</v>
       </c>
-      <c r="H10" s="1">
-        <v>84164</v>
-      </c>
-      <c r="I10">
-        <f t="shared" si="2"/>
+      <c r="J10" s="1">
+        <v>22251</v>
+      </c>
+      <c r="K10">
+        <f>IF(ISBLANK(L10),-J10,L10-J10)</f>
+        <v>70</v>
+      </c>
+      <c r="L10" s="1">
+        <v>22321</v>
+      </c>
+      <c r="M10">
+        <f>IF(ISBLANK(N10),-L10,N10-L10)</f>
+        <v>62</v>
+      </c>
+      <c r="N10" s="1">
+        <v>22383</v>
+      </c>
+      <c r="O10">
+        <f>IF(ISBLANK(P10),-N10,P10-N10)</f>
+        <v>70</v>
+      </c>
+      <c r="P10" s="1">
+        <v>22453</v>
+      </c>
+      <c r="Q10">
+        <f>IF(ISBLANK(R10),-P10,R10-P10)</f>
+        <v>173</v>
+      </c>
+      <c r="R10" s="1">
+        <v>22626</v>
+      </c>
+      <c r="S10">
+        <f>IF(ISBLANK(T10),-R10,T10-R10)</f>
         <v>74</v>
       </c>
-      <c r="J10" s="1">
-        <v>84238</v>
-      </c>
-      <c r="K10">
-        <f t="shared" si="3"/>
-        <v>150</v>
-      </c>
-      <c r="L10" s="1">
-        <v>84388</v>
-      </c>
-      <c r="M10">
-        <f t="shared" si="4"/>
-        <v>171</v>
-      </c>
-      <c r="N10" s="1">
-        <v>84559</v>
-      </c>
-      <c r="O10">
-        <f t="shared" si="5"/>
-        <v>95</v>
-      </c>
-      <c r="P10" s="1">
-        <v>84654</v>
-      </c>
-      <c r="Q10">
-        <f t="shared" si="6"/>
-        <v>187</v>
-      </c>
-      <c r="R10" s="1">
-        <v>84841</v>
-      </c>
-      <c r="S10">
-        <f t="shared" si="7"/>
-        <v>130</v>
-      </c>
       <c r="T10" s="1">
-        <v>84971</v>
+        <v>22700</v>
+      </c>
+      <c r="U10">
+        <f>IF(ISBLANK(V10),-T10,V10-T10)</f>
+        <v>193</v>
+      </c>
+      <c r="V10" s="1">
+        <v>22893</v>
       </c>
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="D11" s="1">
-        <v>118444</v>
+        <v>14802</v>
       </c>
       <c r="E11">
-        <f t="shared" si="0"/>
-        <v>45</v>
+        <f>IF(ISBLANK(F11),-D11,F11-D11)</f>
+        <v>156</v>
       </c>
       <c r="F11" s="1">
-        <v>118489</v>
+        <v>14958</v>
       </c>
       <c r="G11">
-        <f t="shared" si="1"/>
-        <v>186</v>
+        <f>IF(ISBLANK(H11),-F11,H11-F11)</f>
+        <v>51</v>
       </c>
       <c r="H11" s="1">
-        <v>118675</v>
+        <v>15009</v>
       </c>
       <c r="I11">
-        <f t="shared" si="2"/>
-        <v>98</v>
+        <f>IF(ISBLANK(J11),-H11,J11-H11)</f>
+        <v>198</v>
       </c>
       <c r="J11" s="1">
-        <v>118773</v>
+        <v>15207</v>
       </c>
       <c r="K11">
-        <f t="shared" si="3"/>
-        <v>350</v>
+        <f>IF(ISBLANK(L11),-J11,L11-J11)</f>
+        <v>146</v>
       </c>
       <c r="L11" s="1">
-        <v>119123</v>
+        <v>15353</v>
       </c>
       <c r="M11">
-        <f t="shared" si="4"/>
-        <v>257</v>
+        <f>IF(ISBLANK(N11),-L11,N11-L11)</f>
+        <v>41</v>
       </c>
       <c r="N11" s="1">
-        <v>119380</v>
+        <v>15394</v>
       </c>
       <c r="O11">
-        <f t="shared" si="5"/>
-        <v>165</v>
+        <f>IF(ISBLANK(P11),-N11,P11-N11)</f>
+        <v>392</v>
       </c>
       <c r="P11" s="1">
-        <v>119545</v>
+        <v>15786</v>
       </c>
       <c r="Q11">
-        <f t="shared" si="6"/>
+        <f>IF(ISBLANK(R11),-P11,R11-P11)</f>
+        <v>321</v>
+      </c>
+      <c r="R11" s="1">
+        <v>16107</v>
+      </c>
+      <c r="S11">
+        <f>IF(ISBLANK(T11),-R11,T11-R11)</f>
+        <v>101</v>
+      </c>
+      <c r="T11" s="1">
+        <v>16208</v>
+      </c>
+      <c r="U11">
+        <f>IF(ISBLANK(V11),-T11,V11-T11)</f>
         <v>170</v>
       </c>
-      <c r="R11" s="1">
-        <v>119715</v>
-      </c>
-      <c r="S11">
-        <f t="shared" si="7"/>
-        <v>168</v>
-      </c>
-      <c r="T11" s="1">
-        <v>119883</v>
+      <c r="V11" s="1">
+        <v>16378</v>
       </c>
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="D12" s="1">
-        <v>2395</v>
+        <v>10582</v>
       </c>
       <c r="E12">
-        <f t="shared" si="0"/>
-        <v>14</v>
+        <f>IF(ISBLANK(F12),-D12,F12-D12)</f>
+        <v>57</v>
       </c>
       <c r="F12" s="1">
-        <v>2409</v>
+        <v>10639</v>
       </c>
       <c r="G12">
-        <f t="shared" si="1"/>
-        <v>-2409</v>
+        <f>IF(ISBLANK(H12),-F12,H12-F12)</f>
+        <v>106</v>
       </c>
       <c r="H12" s="1">
-        <v>0</v>
+        <v>10745</v>
       </c>
       <c r="I12">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>IF(ISBLANK(J12),-H12,J12-H12)</f>
+        <v>138</v>
       </c>
       <c r="J12" s="1">
-        <v>0</v>
+        <v>10883</v>
       </c>
       <c r="K12">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f>IF(ISBLANK(L12),-J12,L12-J12)</f>
+        <v>54</v>
       </c>
       <c r="L12" s="1">
-        <v>0</v>
+        <v>10937</v>
       </c>
       <c r="M12">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f>IF(ISBLANK(N12),-L12,N12-L12)</f>
+        <v>300</v>
       </c>
       <c r="N12" s="1">
-        <v>0</v>
+        <v>11237</v>
       </c>
       <c r="O12">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f>IF(ISBLANK(P12),-N12,P12-N12)</f>
+        <v>159</v>
       </c>
       <c r="P12" s="1">
-        <v>0</v>
+        <v>11396</v>
       </c>
       <c r="Q12">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f>IF(ISBLANK(R12),-P12,R12-P12)</f>
+        <v>322</v>
       </c>
       <c r="R12" s="1">
-        <v>0</v>
+        <v>11718</v>
       </c>
       <c r="S12">
-        <f t="shared" si="7"/>
-        <v>0</v>
+        <f>IF(ISBLANK(T12),-R12,T12-R12)</f>
+        <v>908</v>
       </c>
       <c r="T12" s="1">
-        <v>0</v>
+        <v>12626</v>
+      </c>
+      <c r="U12">
+        <f>IF(ISBLANK(V12),-T12,V12-T12)</f>
+        <v>1585</v>
+      </c>
+      <c r="V12" s="1">
+        <v>14211</v>
       </c>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D13" s="1">
-        <v>9423</v>
+        <v>9823</v>
       </c>
       <c r="E13">
-        <f t="shared" si="0"/>
-        <v>32</v>
+        <f>IF(ISBLANK(F13),-D13,F13-D13)</f>
+        <v>37</v>
       </c>
       <c r="F13" s="1">
-        <v>9455</v>
+        <v>9860</v>
       </c>
       <c r="G13">
-        <f t="shared" si="1"/>
-        <v>325</v>
+        <f>IF(ISBLANK(H13),-F13,H13-F13)</f>
+        <v>76</v>
       </c>
       <c r="H13" s="1">
-        <v>9780</v>
+        <v>9936</v>
       </c>
       <c r="I13">
-        <f t="shared" si="2"/>
-        <v>75</v>
+        <f>IF(ISBLANK(J13),-H13,J13-H13)</f>
+        <v>54</v>
       </c>
       <c r="J13" s="1">
-        <v>9855</v>
+        <v>9990</v>
       </c>
       <c r="K13">
-        <f t="shared" si="3"/>
-        <v>114</v>
+        <f>IF(ISBLANK(L13),-J13,L13-J13)</f>
+        <v>184</v>
       </c>
       <c r="L13" s="1">
-        <v>9969</v>
+        <v>10174</v>
       </c>
       <c r="M13">
-        <f t="shared" si="4"/>
-        <v>280</v>
+        <f>IF(ISBLANK(N13),-L13,N13-L13)</f>
+        <v>52</v>
       </c>
       <c r="N13" s="1">
-        <v>10249</v>
+        <v>10226</v>
       </c>
       <c r="O13">
-        <f t="shared" si="5"/>
-        <v>78</v>
+        <f>IF(ISBLANK(P13),-N13,P13-N13)</f>
+        <v>168</v>
       </c>
       <c r="P13" s="1">
-        <v>10327</v>
+        <v>10394</v>
       </c>
       <c r="Q13">
-        <f t="shared" si="6"/>
-        <v>137</v>
+        <f>IF(ISBLANK(R13),-P13,R13-P13)</f>
+        <v>214</v>
       </c>
       <c r="R13" s="1">
-        <v>10464</v>
+        <v>10608</v>
       </c>
       <c r="S13">
-        <f t="shared" si="7"/>
-        <v>79</v>
+        <f>IF(ISBLANK(T13),-R13,T13-R13)</f>
+        <v>48</v>
       </c>
       <c r="T13" s="1">
-        <v>10543</v>
+        <v>10656</v>
+      </c>
+      <c r="U13">
+        <f>IF(ISBLANK(V13),-T13,V13-T13)</f>
+        <v>286</v>
+      </c>
+      <c r="V13" s="1">
+        <v>10942</v>
       </c>
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
       <c r="D14" s="1">
-        <v>79072</v>
+        <v>9423</v>
       </c>
       <c r="E14">
-        <f t="shared" si="0"/>
-        <v>68</v>
+        <f>IF(ISBLANK(F14),-D14,F14-D14)</f>
+        <v>32</v>
       </c>
       <c r="F14" s="1">
-        <v>79140</v>
+        <v>9455</v>
       </c>
       <c r="G14">
-        <f t="shared" si="1"/>
-        <v>142</v>
+        <f>IF(ISBLANK(H14),-F14,H14-F14)</f>
+        <v>325</v>
       </c>
       <c r="H14" s="1">
-        <v>79282</v>
+        <v>9780</v>
       </c>
       <c r="I14">
-        <f t="shared" si="2"/>
-        <v>105</v>
+        <f>IF(ISBLANK(J14),-H14,J14-H14)</f>
+        <v>75</v>
       </c>
       <c r="J14" s="1">
-        <v>79387</v>
+        <v>9855</v>
       </c>
       <c r="K14">
-        <f t="shared" si="3"/>
-        <v>186</v>
+        <f>IF(ISBLANK(L14),-J14,L14-J14)</f>
+        <v>114</v>
       </c>
       <c r="L14" s="1">
-        <v>79573</v>
+        <v>9969</v>
       </c>
       <c r="M14">
-        <f t="shared" si="4"/>
-        <v>168</v>
+        <f>IF(ISBLANK(N14),-L14,N14-L14)</f>
+        <v>280</v>
       </c>
       <c r="N14" s="1">
-        <v>79741</v>
+        <v>10249</v>
       </c>
       <c r="O14">
-        <f t="shared" si="5"/>
-        <v>204</v>
+        <f>IF(ISBLANK(P14),-N14,P14-N14)</f>
+        <v>78</v>
       </c>
       <c r="P14" s="1">
-        <v>79945</v>
+        <v>10327</v>
       </c>
       <c r="Q14">
-        <f t="shared" si="6"/>
-        <v>305</v>
+        <f>IF(ISBLANK(R14),-P14,R14-P14)</f>
+        <v>137</v>
       </c>
       <c r="R14" s="1">
-        <v>80250</v>
+        <v>10464</v>
       </c>
       <c r="S14">
-        <f t="shared" si="7"/>
-        <v>127</v>
+        <f>IF(ISBLANK(T14),-R14,T14-R14)</f>
+        <v>79</v>
       </c>
       <c r="T14" s="1">
-        <v>80377</v>
+        <v>10543</v>
+      </c>
+      <c r="U14">
+        <f>IF(ISBLANK(V14),-T14,V14-T14)</f>
+        <v>1160</v>
+      </c>
+      <c r="V14" s="1">
+        <v>11703</v>
       </c>
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="D15" s="1">
-        <v>22075</v>
+        <v>9306</v>
       </c>
       <c r="E15">
-        <f t="shared" si="0"/>
-        <v>38</v>
+        <f>IF(ISBLANK(F15),-D15,F15-D15)</f>
+        <v>25</v>
       </c>
       <c r="F15" s="1">
-        <v>22113</v>
+        <v>9331</v>
       </c>
       <c r="G15">
-        <f t="shared" si="1"/>
-        <v>80</v>
+        <f>IF(ISBLANK(H15),-F15,H15-F15)</f>
+        <v>70</v>
       </c>
       <c r="H15" s="1">
-        <v>22193</v>
+        <v>9401</v>
       </c>
       <c r="I15">
-        <f t="shared" si="2"/>
-        <v>58</v>
+        <f>IF(ISBLANK(J15),-H15,J15-H15)</f>
+        <v>35</v>
       </c>
       <c r="J15" s="1">
-        <v>22251</v>
+        <v>9436</v>
       </c>
       <c r="K15">
-        <f t="shared" si="3"/>
-        <v>70</v>
+        <f>IF(ISBLANK(L15),-J15,L15-J15)</f>
+        <v>60</v>
       </c>
       <c r="L15" s="1">
-        <v>22321</v>
+        <v>9496</v>
       </c>
       <c r="M15">
-        <f t="shared" si="4"/>
-        <v>62</v>
+        <f>IF(ISBLANK(N15),-L15,N15-L15)</f>
+        <v>228</v>
       </c>
       <c r="N15" s="1">
-        <v>22383</v>
+        <v>9724</v>
       </c>
       <c r="O15">
-        <f t="shared" si="5"/>
-        <v>70</v>
+        <f>IF(ISBLANK(P15),-N15,P15-N15)</f>
+        <v>145</v>
       </c>
       <c r="P15" s="1">
-        <v>22453</v>
+        <v>9869</v>
       </c>
       <c r="Q15">
-        <f t="shared" si="6"/>
-        <v>173</v>
+        <f>IF(ISBLANK(R15),-P15,R15-P15)</f>
+        <v>106</v>
       </c>
       <c r="R15" s="1">
-        <v>22626</v>
+        <v>9975</v>
       </c>
       <c r="S15">
-        <f t="shared" si="7"/>
-        <v>74</v>
+        <f>IF(ISBLANK(T15),-R15,T15-R15)</f>
+        <v>247</v>
       </c>
       <c r="T15" s="1">
-        <v>22700</v>
+        <v>10222</v>
+      </c>
+      <c r="U15">
+        <f>IF(ISBLANK(V15),-T15,V15-T15)</f>
+        <v>616</v>
+      </c>
+      <c r="V15" s="1">
+        <v>10838</v>
       </c>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D16" s="1">
-        <v>9823</v>
+        <v>7475</v>
       </c>
       <c r="E16">
-        <f t="shared" si="0"/>
-        <v>37</v>
+        <f>IF(ISBLANK(F16),-D16,F16-D16)</f>
+        <v>23</v>
       </c>
       <c r="F16" s="1">
-        <v>9860</v>
+        <v>7498</v>
       </c>
       <c r="G16">
-        <f t="shared" si="1"/>
-        <v>76</v>
+        <f>IF(ISBLANK(H16),-F16,H16-F16)</f>
+        <v>98</v>
       </c>
       <c r="H16" s="1">
-        <v>9936</v>
+        <v>7596</v>
       </c>
       <c r="I16">
-        <f t="shared" si="2"/>
-        <v>54</v>
+        <f>IF(ISBLANK(J16),-H16,J16-H16)</f>
+        <v>142</v>
       </c>
       <c r="J16" s="1">
-        <v>9990</v>
+        <v>7738</v>
       </c>
       <c r="K16">
-        <f t="shared" si="3"/>
-        <v>184</v>
+        <f>IF(ISBLANK(L16),-J16,L16-J16)</f>
+        <v>70</v>
       </c>
       <c r="L16" s="1">
-        <v>10174</v>
+        <v>7808</v>
       </c>
       <c r="M16">
-        <f t="shared" si="4"/>
-        <v>52</v>
+        <f>IF(ISBLANK(N16),-L16,N16-L16)</f>
+        <v>197</v>
       </c>
       <c r="N16" s="1">
-        <v>10226</v>
+        <v>8005</v>
       </c>
       <c r="O16">
-        <f t="shared" si="5"/>
-        <v>168</v>
+        <f>IF(ISBLANK(P16),-N16,P16-N16)</f>
+        <v>192</v>
       </c>
       <c r="P16" s="1">
-        <v>10394</v>
+        <v>8197</v>
       </c>
       <c r="Q16">
-        <f t="shared" si="6"/>
-        <v>214</v>
+        <f>IF(ISBLANK(R16),-P16,R16-P16)</f>
+        <v>176</v>
       </c>
       <c r="R16" s="1">
-        <v>10608</v>
+        <v>8373</v>
       </c>
       <c r="S16">
-        <f t="shared" si="7"/>
+        <f>IF(ISBLANK(T16),-R16,T16-R16)</f>
+        <v>188</v>
+      </c>
+      <c r="T16" s="1">
+        <v>8561</v>
+      </c>
+      <c r="U16">
+        <f>IF(ISBLANK(V16),-T16,V16-T16)</f>
+        <v>-8561</v>
+      </c>
+      <c r="V16" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>139</v>
+      </c>
+      <c r="D17" s="1">
+        <v>4665</v>
+      </c>
+      <c r="E17">
+        <f>IF(ISBLANK(F17),-D17,F17-D17)</f>
+        <v>26</v>
+      </c>
+      <c r="F17" s="1">
+        <v>4691</v>
+      </c>
+      <c r="G17">
+        <f>IF(ISBLANK(H17),-F17,H17-F17)</f>
+        <v>43</v>
+      </c>
+      <c r="H17" s="1">
+        <v>4734</v>
+      </c>
+      <c r="I17">
+        <f>IF(ISBLANK(J17),-H17,J17-H17)</f>
+        <v>57</v>
+      </c>
+      <c r="J17" s="1">
+        <v>4791</v>
+      </c>
+      <c r="K17">
+        <f>IF(ISBLANK(L17),-J17,L17-J17)</f>
+        <v>50</v>
+      </c>
+      <c r="L17" s="1">
+        <v>4841</v>
+      </c>
+      <c r="M17">
+        <f>IF(ISBLANK(N17),-L17,N17-L17)</f>
+        <v>115</v>
+      </c>
+      <c r="N17" s="1">
+        <v>4956</v>
+      </c>
+      <c r="O17">
+        <f>IF(ISBLANK(P17),-N17,P17-N17)</f>
+        <v>72</v>
+      </c>
+      <c r="P17" s="1">
+        <v>5028</v>
+      </c>
+      <c r="Q17">
+        <f>IF(ISBLANK(R17),-P17,R17-P17)</f>
+        <v>104</v>
+      </c>
+      <c r="R17" s="1">
+        <v>5132</v>
+      </c>
+      <c r="S17">
+        <f>IF(ISBLANK(T17),-R17,T17-R17)</f>
+        <v>-5132</v>
+      </c>
+      <c r="T17" s="1">
+        <v>0</v>
+      </c>
+      <c r="U17">
+        <f>IF(ISBLANK(V17),-T17,V17-T17)</f>
+        <v>0</v>
+      </c>
+      <c r="V17" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>140</v>
+      </c>
+      <c r="D18" s="1">
+        <v>3682</v>
+      </c>
+      <c r="E18">
+        <f>IF(ISBLANK(F18),-D18,F18-D18)</f>
+        <v>77</v>
+      </c>
+      <c r="F18" s="1">
+        <v>3759</v>
+      </c>
+      <c r="G18">
+        <f>IF(ISBLANK(H18),-F18,H18-F18)</f>
+        <v>44</v>
+      </c>
+      <c r="H18" s="1">
+        <v>3803</v>
+      </c>
+      <c r="I18">
+        <f>IF(ISBLANK(J18),-H18,J18-H18)</f>
+        <v>116</v>
+      </c>
+      <c r="J18" s="1">
+        <v>3919</v>
+      </c>
+      <c r="K18">
+        <f>IF(ISBLANK(L18),-J18,L18-J18)</f>
+        <v>87</v>
+      </c>
+      <c r="L18" s="1">
+        <v>4006</v>
+      </c>
+      <c r="M18">
+        <f>IF(ISBLANK(N18),-L18,N18-L18)</f>
+        <v>41</v>
+      </c>
+      <c r="N18" s="1">
+        <v>4047</v>
+      </c>
+      <c r="O18">
+        <f>IF(ISBLANK(P18),-N18,P18-N18)</f>
+        <v>134</v>
+      </c>
+      <c r="P18" s="1">
+        <v>4181</v>
+      </c>
+      <c r="Q18">
+        <f>IF(ISBLANK(R18),-P18,R18-P18)</f>
+        <v>-4181</v>
+      </c>
+      <c r="R18" s="1">
+        <v>0</v>
+      </c>
+      <c r="S18">
+        <f>IF(ISBLANK(T18),-R18,T18-R18)</f>
+        <v>0</v>
+      </c>
+      <c r="T18" s="1">
+        <v>0</v>
+      </c>
+      <c r="U18">
+        <f>IF(ISBLANK(V18),-T18,V18-T18)</f>
+        <v>0</v>
+      </c>
+      <c r="V18" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>141</v>
+      </c>
+      <c r="D19" s="1">
+        <v>3286</v>
+      </c>
+      <c r="E19">
+        <f>IF(ISBLANK(F19),-D19,F19-D19)</f>
+        <v>21</v>
+      </c>
+      <c r="F19" s="1">
+        <v>3307</v>
+      </c>
+      <c r="G19">
+        <f>IF(ISBLANK(H19),-F19,H19-F19)</f>
+        <v>13</v>
+      </c>
+      <c r="H19" s="1">
+        <v>3320</v>
+      </c>
+      <c r="I19">
+        <f>IF(ISBLANK(J19),-H19,J19-H19)</f>
+        <v>232</v>
+      </c>
+      <c r="J19" s="1">
+        <v>3552</v>
+      </c>
+      <c r="K19">
+        <f>IF(ISBLANK(L19),-J19,L19-J19)</f>
+        <v>102</v>
+      </c>
+      <c r="L19" s="1">
+        <v>3654</v>
+      </c>
+      <c r="M19">
+        <f>IF(ISBLANK(N19),-L19,N19-L19)</f>
+        <v>60</v>
+      </c>
+      <c r="N19" s="1">
+        <v>3714</v>
+      </c>
+      <c r="O19">
+        <f>IF(ISBLANK(P19),-N19,P19-N19)</f>
+        <v>-3714</v>
+      </c>
+      <c r="P19" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q19">
+        <f>IF(ISBLANK(R19),-P19,R19-P19)</f>
+        <v>0</v>
+      </c>
+      <c r="R19" s="1">
+        <v>0</v>
+      </c>
+      <c r="S19">
+        <f>IF(ISBLANK(T19),-R19,T19-R19)</f>
+        <v>0</v>
+      </c>
+      <c r="T19" s="1">
+        <v>0</v>
+      </c>
+      <c r="U19">
+        <f>IF(ISBLANK(V19),-T19,V19-T19)</f>
+        <v>0</v>
+      </c>
+      <c r="V19" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>142</v>
+      </c>
+      <c r="D20" s="1">
+        <v>3182</v>
+      </c>
+      <c r="E20">
+        <f>IF(ISBLANK(F20),-D20,F20-D20)</f>
+        <v>15</v>
+      </c>
+      <c r="F20" s="1">
+        <v>3197</v>
+      </c>
+      <c r="G20">
+        <f>IF(ISBLANK(H20),-F20,H20-F20)</f>
+        <v>60</v>
+      </c>
+      <c r="H20" s="1">
+        <v>3257</v>
+      </c>
+      <c r="I20">
+        <f>IF(ISBLANK(J20),-H20,J20-H20)</f>
+        <v>43</v>
+      </c>
+      <c r="J20" s="1">
+        <v>3300</v>
+      </c>
+      <c r="K20">
+        <f>IF(ISBLANK(L20),-J20,L20-J20)</f>
+        <v>32</v>
+      </c>
+      <c r="L20" s="1">
+        <v>3332</v>
+      </c>
+      <c r="M20">
+        <f>IF(ISBLANK(N20),-L20,N20-L20)</f>
+        <v>-3332</v>
+      </c>
+      <c r="N20" s="1">
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <f>IF(ISBLANK(P20),-N20,P20-N20)</f>
+        <v>0</v>
+      </c>
+      <c r="P20" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q20">
+        <f>IF(ISBLANK(R20),-P20,R20-P20)</f>
+        <v>0</v>
+      </c>
+      <c r="R20" s="1">
+        <v>0</v>
+      </c>
+      <c r="S20">
+        <f>IF(ISBLANK(T20),-R20,T20-R20)</f>
+        <v>0</v>
+      </c>
+      <c r="T20" s="1">
+        <v>0</v>
+      </c>
+      <c r="U20">
+        <f>IF(ISBLANK(V20),-T20,V20-T20)</f>
+        <v>0</v>
+      </c>
+      <c r="V20" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>143</v>
+      </c>
+      <c r="D21" s="1">
+        <v>2864</v>
+      </c>
+      <c r="E21">
+        <f>IF(ISBLANK(F21),-D21,F21-D21)</f>
+        <v>34</v>
+      </c>
+      <c r="F21" s="1">
+        <v>2898</v>
+      </c>
+      <c r="G21">
+        <f>IF(ISBLANK(H21),-F21,H21-F21)</f>
+        <v>21</v>
+      </c>
+      <c r="H21" s="1">
+        <v>2919</v>
+      </c>
+      <c r="I21">
+        <f>IF(ISBLANK(J21),-H21,J21-H21)</f>
+        <v>148</v>
+      </c>
+      <c r="J21" s="1">
+        <v>3067</v>
+      </c>
+      <c r="K21">
+        <f>IF(ISBLANK(L21),-J21,L21-J21)</f>
+        <v>-3067</v>
+      </c>
+      <c r="L21" s="1">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <f>IF(ISBLANK(N21),-L21,N21-L21)</f>
+        <v>0</v>
+      </c>
+      <c r="N21" s="1">
+        <v>0</v>
+      </c>
+      <c r="O21">
+        <f>IF(ISBLANK(P21),-N21,P21-N21)</f>
+        <v>0</v>
+      </c>
+      <c r="P21" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q21">
+        <f>IF(ISBLANK(R21),-P21,R21-P21)</f>
+        <v>0</v>
+      </c>
+      <c r="R21" s="1">
+        <v>0</v>
+      </c>
+      <c r="S21">
+        <f>IF(ISBLANK(T21),-R21,T21-R21)</f>
+        <v>0</v>
+      </c>
+      <c r="T21" s="1">
+        <v>0</v>
+      </c>
+      <c r="U21">
+        <f>IF(ISBLANK(V21),-T21,V21-T21)</f>
+        <v>0</v>
+      </c>
+      <c r="V21" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>144</v>
+      </c>
+      <c r="D22" s="1">
+        <v>2416</v>
+      </c>
+      <c r="E22">
+        <f>IF(ISBLANK(F22),-D22,F22-D22)</f>
         <v>48</v>
       </c>
-      <c r="T16" s="1">
-        <v>10656</v>
-      </c>
-    </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>17</v>
-      </c>
-      <c r="B17" t="s">
-        <v>140</v>
-      </c>
-      <c r="D17" s="1">
-        <v>3682</v>
-      </c>
-      <c r="E17">
-        <f t="shared" si="0"/>
-        <v>77</v>
-      </c>
-      <c r="F17" s="1">
-        <v>3759</v>
-      </c>
-      <c r="G17">
-        <f t="shared" si="1"/>
-        <v>44</v>
-      </c>
-      <c r="H17" s="1">
-        <v>3803</v>
-      </c>
-      <c r="I17">
-        <f t="shared" si="2"/>
-        <v>116</v>
-      </c>
-      <c r="J17" s="1">
-        <v>3919</v>
-      </c>
-      <c r="K17">
-        <f t="shared" si="3"/>
-        <v>87</v>
-      </c>
-      <c r="L17" s="1">
-        <v>4006</v>
-      </c>
-      <c r="M17">
-        <f t="shared" si="4"/>
-        <v>41</v>
-      </c>
-      <c r="N17" s="1">
-        <v>4047</v>
-      </c>
-      <c r="O17">
-        <f t="shared" si="5"/>
-        <v>134</v>
-      </c>
-      <c r="P17" s="1">
-        <v>4181</v>
-      </c>
-      <c r="Q17">
-        <f t="shared" si="6"/>
-        <v>-4181</v>
-      </c>
-      <c r="R17" s="1">
-        <v>0</v>
-      </c>
-      <c r="S17">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="T17" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>5</v>
-      </c>
-      <c r="B18" t="s">
-        <v>128</v>
-      </c>
-      <c r="D18" s="1">
-        <v>75946</v>
-      </c>
-      <c r="E18">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="F18" s="1">
-        <v>76046</v>
-      </c>
-      <c r="G18">
-        <f t="shared" si="1"/>
-        <v>201</v>
-      </c>
-      <c r="H18" s="1">
-        <v>76247</v>
-      </c>
-      <c r="I18">
-        <f t="shared" si="2"/>
-        <v>126</v>
-      </c>
-      <c r="J18" s="1">
-        <v>76373</v>
-      </c>
-      <c r="K18">
-        <f t="shared" si="3"/>
-        <v>272</v>
-      </c>
-      <c r="L18" s="1">
-        <v>76645</v>
-      </c>
-      <c r="M18">
-        <f t="shared" si="4"/>
-        <v>74</v>
-      </c>
-      <c r="N18" s="1">
-        <v>76719</v>
-      </c>
-      <c r="O18">
-        <f t="shared" si="5"/>
-        <v>301</v>
-      </c>
-      <c r="P18" s="1">
-        <v>77020</v>
-      </c>
-      <c r="Q18">
-        <f t="shared" si="6"/>
-        <v>283</v>
-      </c>
-      <c r="R18" s="1">
-        <v>77303</v>
-      </c>
-      <c r="S18">
-        <f t="shared" si="7"/>
-        <v>112</v>
-      </c>
-      <c r="T18" s="1">
-        <v>77415</v>
-      </c>
-    </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>20</v>
-      </c>
-      <c r="B19" t="s">
-        <v>143</v>
-      </c>
-      <c r="D19" s="1">
-        <v>2864</v>
-      </c>
-      <c r="E19">
-        <f t="shared" si="0"/>
-        <v>34</v>
-      </c>
-      <c r="F19" s="1">
-        <v>2898</v>
-      </c>
-      <c r="G19">
-        <f t="shared" si="1"/>
-        <v>21</v>
-      </c>
-      <c r="H19" s="1">
-        <v>2919</v>
-      </c>
-      <c r="I19">
-        <f t="shared" si="2"/>
-        <v>148</v>
-      </c>
-      <c r="J19" s="1">
-        <v>3067</v>
-      </c>
-      <c r="K19">
-        <f t="shared" si="3"/>
-        <v>-3067</v>
-      </c>
-      <c r="L19" s="1">
-        <v>0</v>
-      </c>
-      <c r="M19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="N19" s="1">
-        <v>0</v>
-      </c>
-      <c r="O19">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="P19" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="R19" s="1">
-        <v>0</v>
-      </c>
-      <c r="S19">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="T19" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>21</v>
-      </c>
-      <c r="B20" t="s">
-        <v>144</v>
-      </c>
-      <c r="D20" s="1">
-        <v>2416</v>
-      </c>
-      <c r="E20">
-        <f t="shared" si="0"/>
-        <v>48</v>
-      </c>
-      <c r="F20" s="1">
+      <c r="F22" s="1">
         <v>2464</v>
       </c>
-      <c r="G20">
-        <f t="shared" si="1"/>
+      <c r="G22">
+        <f>IF(ISBLANK(H22),-F22,H22-F22)</f>
         <v>78</v>
       </c>
-      <c r="H20" s="1">
+      <c r="H22" s="1">
         <v>2542</v>
       </c>
-      <c r="I20">
-        <f t="shared" si="2"/>
+      <c r="I22">
+        <f>IF(ISBLANK(J22),-H22,J22-H22)</f>
         <v>-2542</v>
       </c>
-      <c r="J20" s="1">
-        <v>0</v>
-      </c>
-      <c r="K20">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L20" s="1">
-        <v>0</v>
-      </c>
-      <c r="M20">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="N20" s="1">
-        <v>0</v>
-      </c>
-      <c r="O20">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="P20" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q20">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="R20" s="1">
-        <v>0</v>
-      </c>
-      <c r="S20">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="T20" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A21">
+      <c r="J22" s="1">
+        <v>0</v>
+      </c>
+      <c r="K22">
+        <f>IF(ISBLANK(L22),-J22,L22-J22)</f>
+        <v>0</v>
+      </c>
+      <c r="L22" s="1">
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <f>IF(ISBLANK(N22),-L22,N22-L22)</f>
+        <v>0</v>
+      </c>
+      <c r="N22" s="1">
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <f>IF(ISBLANK(P22),-N22,P22-N22)</f>
+        <v>0</v>
+      </c>
+      <c r="P22" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q22">
+        <f>IF(ISBLANK(R22),-P22,R22-P22)</f>
+        <v>0</v>
+      </c>
+      <c r="R22" s="1">
+        <v>0</v>
+      </c>
+      <c r="S22">
+        <f>IF(ISBLANK(T22),-R22,T22-R22)</f>
+        <v>0</v>
+      </c>
+      <c r="T22" s="1">
+        <v>0</v>
+      </c>
+      <c r="U22">
+        <f>IF(ISBLANK(V22),-T22,V22-T22)</f>
+        <v>0</v>
+      </c>
+      <c r="V22" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>145</v>
+      </c>
+      <c r="D23" s="1">
+        <v>2395</v>
+      </c>
+      <c r="E23">
+        <f>IF(ISBLANK(F23),-D23,F23-D23)</f>
+        <v>14</v>
+      </c>
+      <c r="F23" s="1">
+        <v>2409</v>
+      </c>
+      <c r="G23">
+        <f>IF(ISBLANK(H23),-F23,H23-F23)</f>
+        <v>-2409</v>
+      </c>
+      <c r="H23" s="1">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <f>IF(ISBLANK(J23),-H23,J23-H23)</f>
+        <v>0</v>
+      </c>
+      <c r="J23" s="1">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <f>IF(ISBLANK(L23),-J23,L23-J23)</f>
+        <v>0</v>
+      </c>
+      <c r="L23" s="1">
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <f>IF(ISBLANK(N23),-L23,N23-L23)</f>
+        <v>0</v>
+      </c>
+      <c r="N23" s="1">
+        <v>0</v>
+      </c>
+      <c r="O23">
+        <f>IF(ISBLANK(P23),-N23,P23-N23)</f>
+        <v>0</v>
+      </c>
+      <c r="P23" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q23">
+        <f>IF(ISBLANK(R23),-P23,R23-P23)</f>
+        <v>0</v>
+      </c>
+      <c r="R23" s="1">
+        <v>0</v>
+      </c>
+      <c r="S23">
+        <f>IF(ISBLANK(T23),-R23,T23-R23)</f>
+        <v>0</v>
+      </c>
+      <c r="T23" s="1">
+        <v>0</v>
+      </c>
+      <c r="U23">
+        <f>IF(ISBLANK(V23),-T23,V23-T23)</f>
+        <v>0</v>
+      </c>
+      <c r="V23" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A24">
         <v>23</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B24" t="s">
         <v>146</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D24" s="1">
         <v>1423</v>
       </c>
-      <c r="E21">
-        <f t="shared" si="0"/>
+      <c r="E24">
+        <f>IF(ISBLANK(F24),-D24,F24-D24)</f>
         <v>-1423</v>
       </c>
-      <c r="F21" s="1">
-        <v>0</v>
-      </c>
-      <c r="G21">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H21" s="1">
-        <v>0</v>
-      </c>
-      <c r="I21">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J21" s="1">
-        <v>0</v>
-      </c>
-      <c r="K21">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L21" s="1">
-        <v>0</v>
-      </c>
-      <c r="M21">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="N21" s="1">
-        <v>0</v>
-      </c>
-      <c r="O21">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="P21" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q21">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="R21" s="1">
-        <v>0</v>
-      </c>
-      <c r="S21">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="T21" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>10</v>
-      </c>
-      <c r="B22" t="s">
-        <v>133</v>
-      </c>
-      <c r="D22" s="1">
-        <v>14802</v>
-      </c>
-      <c r="E22">
-        <f t="shared" si="0"/>
-        <v>156</v>
-      </c>
-      <c r="F22" s="1">
-        <v>14958</v>
-      </c>
-      <c r="G22">
-        <f t="shared" si="1"/>
-        <v>51</v>
-      </c>
-      <c r="H22" s="1">
-        <v>15009</v>
-      </c>
-      <c r="I22">
-        <f t="shared" si="2"/>
-        <v>198</v>
-      </c>
-      <c r="J22" s="1">
-        <v>15207</v>
-      </c>
-      <c r="K22">
-        <f t="shared" si="3"/>
-        <v>146</v>
-      </c>
-      <c r="L22" s="1">
-        <v>15353</v>
-      </c>
-      <c r="M22">
-        <f t="shared" si="4"/>
-        <v>41</v>
-      </c>
-      <c r="N22" s="1">
-        <v>15394</v>
-      </c>
-      <c r="O22">
-        <f t="shared" si="5"/>
-        <v>392</v>
-      </c>
-      <c r="P22" s="1">
-        <v>15786</v>
-      </c>
-      <c r="Q22">
-        <f t="shared" si="6"/>
-        <v>321</v>
-      </c>
-      <c r="R22" s="1">
-        <v>16107</v>
-      </c>
-      <c r="S22">
-        <f t="shared" si="7"/>
-        <v>101</v>
-      </c>
-      <c r="T22" s="1">
-        <v>16208</v>
-      </c>
-    </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>3</v>
-      </c>
-      <c r="B23" t="s">
-        <v>126</v>
-      </c>
-      <c r="D23" s="1">
-        <v>81741</v>
-      </c>
-      <c r="E23">
-        <f t="shared" si="0"/>
-        <v>253</v>
-      </c>
-      <c r="F23" s="1">
-        <v>81994</v>
-      </c>
-      <c r="G23">
-        <f t="shared" si="1"/>
-        <v>130</v>
-      </c>
-      <c r="H23" s="1">
-        <v>82124</v>
-      </c>
-      <c r="I23">
-        <f t="shared" si="2"/>
-        <v>211</v>
-      </c>
-      <c r="J23" s="1">
-        <v>82335</v>
-      </c>
-      <c r="K23">
-        <f t="shared" si="3"/>
-        <v>323</v>
-      </c>
-      <c r="L23" s="1">
-        <v>82658</v>
-      </c>
-      <c r="M23">
-        <f t="shared" si="4"/>
-        <v>206</v>
-      </c>
-      <c r="N23" s="1">
-        <v>82864</v>
-      </c>
-      <c r="O23">
-        <f t="shared" si="5"/>
-        <v>556</v>
-      </c>
-      <c r="P23" s="1">
-        <v>83420</v>
-      </c>
-      <c r="Q23">
-        <f t="shared" si="6"/>
-        <v>351</v>
-      </c>
-      <c r="R23" s="1">
-        <v>83771</v>
-      </c>
-      <c r="S23">
-        <f t="shared" si="7"/>
-        <v>217</v>
-      </c>
-      <c r="T23" s="1">
-        <v>83988</v>
-      </c>
-    </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>18</v>
-      </c>
-      <c r="B24" t="s">
-        <v>141</v>
-      </c>
-      <c r="D24" s="1">
-        <v>3286</v>
-      </c>
-      <c r="E24">
-        <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
       <c r="F24" s="1">
-        <v>3307</v>
+        <v>0</v>
       </c>
       <c r="G24">
-        <f t="shared" si="1"/>
-        <v>13</v>
+        <f>IF(ISBLANK(H24),-F24,H24-F24)</f>
+        <v>0</v>
       </c>
       <c r="H24" s="1">
-        <v>3320</v>
+        <v>0</v>
       </c>
       <c r="I24">
-        <f t="shared" si="2"/>
-        <v>232</v>
+        <f>IF(ISBLANK(J24),-H24,J24-H24)</f>
+        <v>0</v>
       </c>
       <c r="J24" s="1">
-        <v>3552</v>
+        <v>0</v>
       </c>
       <c r="K24">
-        <f t="shared" si="3"/>
-        <v>102</v>
+        <f>IF(ISBLANK(L24),-J24,L24-J24)</f>
+        <v>0</v>
       </c>
       <c r="L24" s="1">
-        <v>3654</v>
+        <v>0</v>
       </c>
       <c r="M24">
-        <f t="shared" si="4"/>
-        <v>60</v>
+        <f>IF(ISBLANK(N24),-L24,N24-L24)</f>
+        <v>0</v>
       </c>
       <c r="N24" s="1">
-        <v>3714</v>
+        <v>0</v>
       </c>
       <c r="O24">
-        <f t="shared" si="5"/>
-        <v>-3714</v>
+        <f>IF(ISBLANK(P24),-N24,P24-N24)</f>
+        <v>0</v>
       </c>
       <c r="P24" s="1">
         <v>0</v>
       </c>
       <c r="Q24">
-        <f t="shared" si="6"/>
+        <f>IF(ISBLANK(R24),-P24,R24-P24)</f>
         <v>0</v>
       </c>
       <c r="R24" s="1">
         <v>0</v>
       </c>
       <c r="S24">
-        <f t="shared" si="7"/>
+        <f>IF(ISBLANK(T24),-R24,T24-R24)</f>
         <v>0</v>
       </c>
       <c r="T24" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="U24">
+        <f>IF(ISBLANK(V24),-T24,V24-T24)</f>
+        <v>0</v>
+      </c>
+      <c r="V24" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>147</v>
       </c>
@@ -8997,25 +9158,28 @@
       <c r="Y26" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="Z26" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>148</v>
       </c>
       <c r="E27">
-        <f t="shared" ref="E27:E48" si="8">FIND(",",B27)</f>
+        <f t="shared" ref="E27:E48" si="0">FIND(",",B27)</f>
         <v>9</v>
       </c>
       <c r="F27" t="str">
-        <f t="shared" ref="F27:F48" si="9">LEFT(B27,E27-1)</f>
+        <f t="shared" ref="F27:F48" si="1">LEFT(B27,E27-1)</f>
         <v>Kelleher</v>
       </c>
       <c r="G27" t="str">
-        <f t="shared" ref="G27:G48" si="10">RIGHT(B27,LEN(B27)-(E27+1))</f>
+        <f t="shared" ref="G27:G48" si="2">RIGHT(B27,LEN(B27)-(E27+1))</f>
         <v>Billy</v>
       </c>
       <c r="H27" t="str">
-        <f t="shared" ref="H27:H48" si="11">G27&amp;" "&amp;F27</f>
+        <f t="shared" ref="H27:H48" si="3">G27&amp;" "&amp;F27</f>
         <v>Billy Kelleher</v>
       </c>
       <c r="J27" t="s">
@@ -9060,30 +9224,30 @@
       <c r="Y27" s="1">
         <v>119883</v>
       </c>
-      <c r="Z27" s="1"/>
       <c r="AA27" s="1"/>
       <c r="AB27" s="1"/>
       <c r="AC27" s="1"/>
       <c r="AD27" s="1"/>
-    </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE27" s="1"/>
+    </row>
+    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>149</v>
       </c>
       <c r="E28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="F28" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>Wallace</v>
       </c>
       <c r="G28" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="2"/>
         <v>Mick</v>
       </c>
       <c r="H28" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v>Mick Wallace</v>
       </c>
       <c r="J28" t="s">
@@ -9128,30 +9292,33 @@
       <c r="Y28" s="1">
         <v>84971</v>
       </c>
-      <c r="Z28" s="1"/>
+      <c r="Z28" s="1">
+        <v>85451</v>
+      </c>
       <c r="AA28" s="1"/>
       <c r="AB28" s="1"/>
       <c r="AC28" s="1"/>
       <c r="AD28" s="1"/>
-    </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE28" s="1"/>
+    </row>
+    <row r="29" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>150</v>
       </c>
       <c r="E29">
-        <f t="shared" si="8"/>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="F29" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>Ní Riada</v>
       </c>
       <c r="G29" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="2"/>
         <v>Liadh</v>
       </c>
       <c r="H29" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v>Liadh Ní Riada</v>
       </c>
       <c r="J29" t="s">
@@ -9196,30 +9363,33 @@
       <c r="Y29" s="1">
         <v>83988</v>
       </c>
-      <c r="Z29" s="1"/>
+      <c r="Z29" s="1">
+        <v>84235</v>
+      </c>
       <c r="AA29" s="1"/>
       <c r="AB29" s="1"/>
       <c r="AC29" s="1"/>
       <c r="AD29" s="1"/>
-    </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE29" s="1"/>
+    </row>
+    <row r="30" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>151</v>
       </c>
       <c r="E30">
-        <f t="shared" si="8"/>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="F30" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>O'Sullivan</v>
       </c>
       <c r="G30" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="2"/>
         <v>Grace</v>
       </c>
       <c r="H30" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v>Grace O'Sullivan</v>
       </c>
       <c r="J30" t="s">
@@ -9264,30 +9434,33 @@
       <c r="Y30" s="1">
         <v>80377</v>
       </c>
-      <c r="Z30" s="1"/>
+      <c r="Z30" s="1">
+        <v>80823</v>
+      </c>
       <c r="AA30" s="1"/>
       <c r="AB30" s="1"/>
       <c r="AC30" s="1"/>
       <c r="AD30" s="1"/>
-    </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE30" s="1"/>
+    </row>
+    <row r="31" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>152</v>
       </c>
       <c r="E31">
-        <f t="shared" si="8"/>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="F31" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>Byrne</v>
       </c>
       <c r="G31" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="2"/>
         <v>Malcolm</v>
       </c>
       <c r="H31" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v>Malcolm Byrne</v>
       </c>
       <c r="J31" t="s">
@@ -9332,30 +9505,33 @@
       <c r="Y31" s="1">
         <v>77415</v>
       </c>
-      <c r="Z31" s="1"/>
+      <c r="Z31" s="1">
+        <v>77754</v>
+      </c>
       <c r="AA31" s="1"/>
       <c r="AB31" s="1"/>
       <c r="AC31" s="1"/>
       <c r="AD31" s="1"/>
-    </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE31" s="1"/>
+    </row>
+    <row r="32" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>153</v>
       </c>
       <c r="E32">
-        <f t="shared" si="8"/>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="F32" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>Clune</v>
       </c>
       <c r="G32" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="2"/>
         <v>Deirdre</v>
       </c>
       <c r="H32" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v>Deirdre Clune</v>
       </c>
       <c r="J32" t="s">
@@ -9400,30 +9576,33 @@
       <c r="Y32" s="1">
         <v>70898</v>
       </c>
-      <c r="Z32" s="1"/>
+      <c r="Z32" s="1">
+        <v>71168</v>
+      </c>
       <c r="AA32" s="1"/>
       <c r="AB32" s="1"/>
       <c r="AC32" s="1"/>
       <c r="AD32" s="1"/>
-    </row>
-    <row r="33" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE32" s="1"/>
+    </row>
+    <row r="33" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>154</v>
       </c>
       <c r="E33">
-        <f t="shared" si="8"/>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="F33" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>Doyle</v>
       </c>
       <c r="G33" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="2"/>
         <v>Andrew</v>
       </c>
       <c r="H33" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v>Andrew Doyle</v>
       </c>
       <c r="J33" t="s">
@@ -9468,30 +9647,33 @@
       <c r="Y33" s="1">
         <v>65558</v>
       </c>
-      <c r="Z33" s="1"/>
+      <c r="Z33" s="1">
+        <v>66049</v>
+      </c>
       <c r="AA33" s="1"/>
       <c r="AB33" s="1"/>
       <c r="AC33" s="1"/>
       <c r="AD33" s="1"/>
-    </row>
-    <row r="34" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE33" s="1"/>
+    </row>
+    <row r="34" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>155</v>
       </c>
       <c r="E34">
-        <f t="shared" si="8"/>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="F34" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>Nunan</v>
       </c>
       <c r="G34" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="2"/>
         <v>Sheila</v>
       </c>
       <c r="H34" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v>Sheila Nunan</v>
       </c>
       <c r="J34" t="s">
@@ -9536,30 +9718,33 @@
       <c r="Y34" s="1">
         <v>39294</v>
       </c>
-      <c r="Z34" s="1"/>
+      <c r="Z34" s="1">
+        <v>39429</v>
+      </c>
       <c r="AA34" s="1"/>
       <c r="AB34" s="1"/>
       <c r="AC34" s="1"/>
       <c r="AD34" s="1"/>
-    </row>
-    <row r="35" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE34" s="1"/>
+    </row>
+    <row r="35" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>156</v>
       </c>
       <c r="E35">
-        <f t="shared" si="8"/>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="F35" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>Wallace</v>
       </c>
       <c r="G35" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="2"/>
         <v>Adrienne</v>
       </c>
       <c r="H35" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v>Adrienne Wallace</v>
       </c>
       <c r="J35" t="s">
@@ -9604,30 +9789,33 @@
       <c r="Y35" s="1">
         <v>22700</v>
       </c>
-      <c r="Z35" s="1"/>
+      <c r="Z35" s="1">
+        <v>22893</v>
+      </c>
       <c r="AA35" s="1"/>
       <c r="AB35" s="1"/>
       <c r="AC35" s="1"/>
       <c r="AD35" s="1"/>
-    </row>
-    <row r="36" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE35" s="1"/>
+    </row>
+    <row r="36" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>157</v>
       </c>
       <c r="E36">
-        <f t="shared" si="8"/>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="F36" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>Cahill</v>
       </c>
       <c r="G36" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="2"/>
         <v>Dolores</v>
       </c>
       <c r="H36" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v>Dolores Cahill</v>
       </c>
       <c r="J36" t="s">
@@ -9672,30 +9860,33 @@
       <c r="Y36" s="1">
         <v>16208</v>
       </c>
-      <c r="Z36" s="1"/>
+      <c r="Z36" s="1">
+        <v>16378</v>
+      </c>
       <c r="AA36" s="1"/>
       <c r="AB36" s="1"/>
       <c r="AC36" s="1"/>
       <c r="AD36" s="1"/>
-    </row>
-    <row r="37" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE36" s="1"/>
+    </row>
+    <row r="37" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>158</v>
       </c>
       <c r="E37">
-        <f t="shared" si="8"/>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="F37" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>O'Flynn</v>
       </c>
       <c r="G37" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="2"/>
         <v>Diarmuid Patrick</v>
       </c>
       <c r="H37" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v>Diarmuid Patrick O'Flynn</v>
       </c>
       <c r="J37" t="s">
@@ -9740,30 +9931,33 @@
       <c r="Y37" s="1">
         <v>12626</v>
       </c>
-      <c r="Z37" s="1"/>
+      <c r="Z37" s="1">
+        <v>14211</v>
+      </c>
       <c r="AA37" s="1"/>
       <c r="AB37" s="1"/>
       <c r="AC37" s="1"/>
       <c r="AD37" s="1"/>
-    </row>
-    <row r="38" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE37" s="1"/>
+    </row>
+    <row r="38" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>159</v>
       </c>
       <c r="E38">
-        <f t="shared" si="8"/>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="F38" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>Minehan</v>
       </c>
       <c r="G38" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="2"/>
         <v>Liam</v>
       </c>
       <c r="H38" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v>Liam Minehan</v>
       </c>
       <c r="J38" t="s">
@@ -9808,30 +10002,33 @@
       <c r="Y38" s="1">
         <v>10656</v>
       </c>
-      <c r="Z38" s="1"/>
+      <c r="Z38" s="1">
+        <v>10942</v>
+      </c>
       <c r="AA38" s="1"/>
       <c r="AB38" s="1"/>
       <c r="AC38" s="1"/>
       <c r="AD38" s="1"/>
-    </row>
-    <row r="39" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE38" s="1"/>
+    </row>
+    <row r="39" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>160</v>
       </c>
       <c r="E39">
-        <f t="shared" si="8"/>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="F39" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>Gardner</v>
       </c>
       <c r="G39" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="2"/>
         <v>Breda Patricia</v>
       </c>
       <c r="H39" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v>Breda Patricia Gardner</v>
       </c>
       <c r="J39" t="s">
@@ -9876,30 +10073,33 @@
       <c r="Y39" s="1">
         <v>10543</v>
       </c>
-      <c r="Z39" s="1"/>
+      <c r="Z39" s="1">
+        <v>11703</v>
+      </c>
       <c r="AA39" s="1"/>
       <c r="AB39" s="1"/>
       <c r="AC39" s="1"/>
       <c r="AD39" s="1"/>
-    </row>
-    <row r="40" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE39" s="1"/>
+    </row>
+    <row r="40" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>161</v>
       </c>
       <c r="E40">
-        <f t="shared" si="8"/>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="F40" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>Heaney</v>
       </c>
       <c r="G40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="2"/>
         <v>Theresa</v>
       </c>
       <c r="H40" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v>Theresa Heaney</v>
       </c>
       <c r="J40" t="s">
@@ -9944,30 +10144,33 @@
       <c r="Y40" s="1">
         <v>10222</v>
       </c>
-      <c r="Z40" s="1"/>
+      <c r="Z40" s="1">
+        <v>10838</v>
+      </c>
       <c r="AA40" s="1"/>
       <c r="AB40" s="1"/>
       <c r="AC40" s="1"/>
       <c r="AD40" s="1"/>
-    </row>
-    <row r="41" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE40" s="1"/>
+    </row>
+    <row r="41" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>162</v>
       </c>
       <c r="E41">
-        <f t="shared" si="8"/>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="F41" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>Brennan</v>
       </c>
       <c r="G41" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="2"/>
         <v>Allan</v>
       </c>
       <c r="H41" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v>Allan Brennan</v>
       </c>
       <c r="J41" t="s">
@@ -10017,25 +10220,26 @@
       <c r="AB41" s="1"/>
       <c r="AC41" s="1"/>
       <c r="AD41" s="1"/>
-    </row>
-    <row r="42" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="AE41" s="1"/>
+    </row>
+    <row r="42" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>163</v>
       </c>
       <c r="E42">
-        <f t="shared" si="8"/>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="F42" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>O'Loughlin</v>
       </c>
       <c r="G42" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="2"/>
         <v>Peter</v>
       </c>
       <c r="H42" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v>Peter O'Loughlin</v>
       </c>
       <c r="J42" t="s">
@@ -10083,24 +10287,24 @@
       <c r="AC42" s="1"/>
       <c r="AD42" s="1"/>
     </row>
-    <row r="43" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>164</v>
       </c>
       <c r="E43">
-        <f t="shared" si="8"/>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="F43" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>Worthington</v>
       </c>
       <c r="G43" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="2"/>
         <v>Colleen</v>
       </c>
       <c r="H43" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v>Colleen Worthington</v>
       </c>
       <c r="J43" t="s">
@@ -10144,24 +10348,24 @@
       <c r="AB43" s="1"/>
       <c r="AC43" s="1"/>
     </row>
-    <row r="44" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>165</v>
       </c>
       <c r="E44">
-        <f t="shared" si="8"/>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="F44" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>Fitzgerald</v>
       </c>
       <c r="G44" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="2"/>
         <v>Paddy</v>
       </c>
       <c r="H44" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v>Paddy Fitzgerald</v>
       </c>
       <c r="J44" t="s">
@@ -10201,24 +10405,24 @@
       <c r="AA44" s="1"/>
       <c r="AB44" s="1"/>
     </row>
-    <row r="45" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>166</v>
       </c>
       <c r="E45">
-        <f t="shared" si="8"/>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="F45" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>Ryan-Purcell</v>
       </c>
       <c r="G45" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="2"/>
         <v>Walter</v>
       </c>
       <c r="H45" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v>Walter Ryan-Purcell</v>
       </c>
       <c r="J45" t="s">
@@ -10254,24 +10458,24 @@
       <c r="Z45" s="1"/>
       <c r="AA45" s="1"/>
     </row>
-    <row r="46" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>167</v>
       </c>
       <c r="E46">
-        <f t="shared" si="8"/>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="F46" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>Sexton</v>
       </c>
       <c r="G46" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="2"/>
         <v>Joesph</v>
       </c>
       <c r="H46" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v>Joesph Sexton</v>
       </c>
       <c r="J46" t="s">
@@ -10300,24 +10504,24 @@
       </c>
       <c r="Z46" s="1"/>
     </row>
-    <row r="47" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>168</v>
       </c>
       <c r="E47">
-        <f t="shared" si="8"/>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="F47" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>Madden</v>
       </c>
       <c r="G47" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="2"/>
         <v>Peter</v>
       </c>
       <c r="H47" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v>Peter Madden</v>
       </c>
       <c r="J47" t="s">
@@ -10339,24 +10543,24 @@
         <v>2542</v>
       </c>
     </row>
-    <row r="48" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>169</v>
       </c>
       <c r="E48">
-        <f t="shared" si="8"/>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="F48" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>Van de Ven</v>
       </c>
       <c r="G48" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="2"/>
         <v>Jan</v>
       </c>
       <c r="H48" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v>Jan Van de Ven</v>
       </c>
       <c r="J48" t="s">
@@ -10381,8 +10585,8 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:T24">
-    <sortCondition ref="B2:B24"/>
+  <sortState ref="A2:V24">
+    <sortCondition ref="A2:A24"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Ack Irish candidate data, Stage 11 South added Signed-off-by: Gerry Mulvenna <git@movingwifi.com>
</commit_message>
<xml_diff>
--- a/europarl/europarl-ireland-2019.xlsx
+++ b/europarl/europarl-ireland-2019.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="263">
   <si>
     <t>Candidate</t>
   </si>
@@ -7326,10 +7326,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE49"/>
+  <dimension ref="A1:AG49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection sqref="A1:X24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7461,6 +7461,13 @@
       <c r="V2" s="1">
         <v>119883</v>
       </c>
+      <c r="W2">
+        <f>IF(ISBLANK(X2),-V2,X2-V2)</f>
+        <v>0</v>
+      </c>
+      <c r="X2" s="1">
+        <v>119883</v>
+      </c>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -7535,6 +7542,13 @@
       <c r="V3" s="1">
         <v>85451</v>
       </c>
+      <c r="W3">
+        <f>IF(ISBLANK(X3),-V3,X3-V3)</f>
+        <v>575</v>
+      </c>
+      <c r="X3" s="1">
+        <v>86026</v>
+      </c>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -7609,6 +7623,13 @@
       <c r="V4" s="1">
         <v>84235</v>
       </c>
+      <c r="W4">
+        <f>IF(ISBLANK(X4),-V4,X4-V4)</f>
+        <v>1001</v>
+      </c>
+      <c r="X4" s="1">
+        <v>85236</v>
+      </c>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -7683,6 +7704,13 @@
       <c r="V5" s="1">
         <v>80823</v>
       </c>
+      <c r="W5">
+        <f>IF(ISBLANK(X5),-V5,X5-V5)</f>
+        <v>991</v>
+      </c>
+      <c r="X5" s="1">
+        <v>81814</v>
+      </c>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -7757,6 +7785,13 @@
       <c r="V6" s="1">
         <v>77754</v>
       </c>
+      <c r="W6">
+        <f>IF(ISBLANK(X6),-V6,X6-V6)</f>
+        <v>1066</v>
+      </c>
+      <c r="X6" s="1">
+        <v>78820</v>
+      </c>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -7831,6 +7866,13 @@
       <c r="V7" s="1">
         <v>71168</v>
       </c>
+      <c r="W7">
+        <f>IF(ISBLANK(X7),-V7,X7-V7)</f>
+        <v>674</v>
+      </c>
+      <c r="X7" s="1">
+        <v>71842</v>
+      </c>
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -7905,6 +7947,13 @@
       <c r="V8" s="1">
         <v>66049</v>
       </c>
+      <c r="W8">
+        <f>IF(ISBLANK(X8),-V8,X8-V8)</f>
+        <v>683</v>
+      </c>
+      <c r="X8" s="1">
+        <v>66732</v>
+      </c>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -7979,6 +8028,13 @@
       <c r="V9" s="1">
         <v>39429</v>
       </c>
+      <c r="W9">
+        <f>IF(ISBLANK(X9),-V9,X9-V9)</f>
+        <v>426</v>
+      </c>
+      <c r="X9" s="1">
+        <v>39855</v>
+      </c>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -8053,6 +8109,13 @@
       <c r="V10" s="1">
         <v>22893</v>
       </c>
+      <c r="W10">
+        <f>IF(ISBLANK(X10),-V10,X10-V10)</f>
+        <v>626</v>
+      </c>
+      <c r="X10" s="1">
+        <v>23519</v>
+      </c>
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -8127,6 +8190,13 @@
       <c r="V11" s="1">
         <v>16378</v>
       </c>
+      <c r="W11">
+        <f>IF(ISBLANK(X11),-V11,X11-V11)</f>
+        <v>530</v>
+      </c>
+      <c r="X11" s="1">
+        <v>16908</v>
+      </c>
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -8201,6 +8271,13 @@
       <c r="V12" s="1">
         <v>14211</v>
       </c>
+      <c r="W12">
+        <f>IF(ISBLANK(X12),-V12,X12-V12)</f>
+        <v>826</v>
+      </c>
+      <c r="X12" s="1">
+        <v>15037</v>
+      </c>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -8275,6 +8352,13 @@
       <c r="V13" s="1">
         <v>10942</v>
       </c>
+      <c r="W13">
+        <f>IF(ISBLANK(X13),-V13,X13-V13)</f>
+        <v>208</v>
+      </c>
+      <c r="X13" s="1">
+        <v>11150</v>
+      </c>
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -8349,6 +8433,13 @@
       <c r="V14" s="1">
         <v>11703</v>
       </c>
+      <c r="W14">
+        <f>IF(ISBLANK(X14),-V14,X14-V14)</f>
+        <v>568</v>
+      </c>
+      <c r="X14" s="1">
+        <v>12271</v>
+      </c>
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15">
@@ -8423,6 +8514,13 @@
       <c r="V15" s="1">
         <v>10838</v>
       </c>
+      <c r="W15">
+        <f>IF(ISBLANK(X15),-V15,X15-V15)</f>
+        <v>-10838</v>
+      </c>
+      <c r="X15" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16">
@@ -8497,8 +8595,15 @@
       <c r="V16" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="W16">
+        <f>IF(ISBLANK(X16),-V16,X16-V16)</f>
+        <v>0</v>
+      </c>
+      <c r="X16" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -8571,8 +8676,15 @@
       <c r="V17" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="W17">
+        <f>IF(ISBLANK(X17),-V17,X17-V17)</f>
+        <v>0</v>
+      </c>
+      <c r="X17" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -8645,8 +8757,15 @@
       <c r="V18" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="W18">
+        <f>IF(ISBLANK(X18),-V18,X18-V18)</f>
+        <v>0</v>
+      </c>
+      <c r="X18" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -8719,8 +8838,15 @@
       <c r="V19" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="W19">
+        <f>IF(ISBLANK(X19),-V19,X19-V19)</f>
+        <v>0</v>
+      </c>
+      <c r="X19" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -8793,8 +8919,15 @@
       <c r="V20" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="W20">
+        <f>IF(ISBLANK(X20),-V20,X20-V20)</f>
+        <v>0</v>
+      </c>
+      <c r="X20" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -8867,8 +9000,15 @@
       <c r="V21" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="W21">
+        <f>IF(ISBLANK(X21),-V21,X21-V21)</f>
+        <v>0</v>
+      </c>
+      <c r="X21" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -8941,8 +9081,15 @@
       <c r="V22" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="W22">
+        <f>IF(ISBLANK(X22),-V22,X22-V22)</f>
+        <v>0</v>
+      </c>
+      <c r="X22" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -9015,8 +9162,15 @@
       <c r="V23" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="W23">
+        <f>IF(ISBLANK(X23),-V23,X23-V23)</f>
+        <v>0</v>
+      </c>
+      <c r="X23" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -9089,8 +9243,15 @@
       <c r="V24" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="W24">
+        <f>IF(ISBLANK(X24),-V24,X24-V24)</f>
+        <v>0</v>
+      </c>
+      <c r="X24" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>147</v>
       </c>
@@ -9161,8 +9322,11 @@
       <c r="Z26" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AA26" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>148</v>
       </c>
@@ -9224,13 +9388,13 @@
       <c r="Y27" s="1">
         <v>119883</v>
       </c>
-      <c r="AA27" s="1"/>
       <c r="AB27" s="1"/>
       <c r="AC27" s="1"/>
       <c r="AD27" s="1"/>
       <c r="AE27" s="1"/>
-    </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AF27" s="1"/>
+    </row>
+    <row r="28" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>149</v>
       </c>
@@ -9295,13 +9459,17 @@
       <c r="Z28" s="1">
         <v>85451</v>
       </c>
-      <c r="AA28" s="1"/>
+      <c r="AA28" s="1">
+        <v>86026</v>
+      </c>
       <c r="AB28" s="1"/>
       <c r="AC28" s="1"/>
       <c r="AD28" s="1"/>
       <c r="AE28" s="1"/>
-    </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AF28" s="1"/>
+      <c r="AG28" s="1"/>
+    </row>
+    <row r="29" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>150</v>
       </c>
@@ -9366,13 +9534,17 @@
       <c r="Z29" s="1">
         <v>84235</v>
       </c>
-      <c r="AA29" s="1"/>
+      <c r="AA29" s="1">
+        <v>85236</v>
+      </c>
       <c r="AB29" s="1"/>
       <c r="AC29" s="1"/>
       <c r="AD29" s="1"/>
       <c r="AE29" s="1"/>
-    </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AF29" s="1"/>
+      <c r="AG29" s="1"/>
+    </row>
+    <row r="30" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>151</v>
       </c>
@@ -9437,13 +9609,17 @@
       <c r="Z30" s="1">
         <v>80823</v>
       </c>
-      <c r="AA30" s="1"/>
+      <c r="AA30" s="1">
+        <v>81814</v>
+      </c>
       <c r="AB30" s="1"/>
       <c r="AC30" s="1"/>
       <c r="AD30" s="1"/>
       <c r="AE30" s="1"/>
-    </row>
-    <row r="31" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AF30" s="1"/>
+      <c r="AG30" s="1"/>
+    </row>
+    <row r="31" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>152</v>
       </c>
@@ -9508,13 +9684,17 @@
       <c r="Z31" s="1">
         <v>77754</v>
       </c>
-      <c r="AA31" s="1"/>
+      <c r="AA31" s="1">
+        <v>78820</v>
+      </c>
       <c r="AB31" s="1"/>
       <c r="AC31" s="1"/>
       <c r="AD31" s="1"/>
       <c r="AE31" s="1"/>
-    </row>
-    <row r="32" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AF31" s="1"/>
+      <c r="AG31" s="1"/>
+    </row>
+    <row r="32" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>153</v>
       </c>
@@ -9579,13 +9759,17 @@
       <c r="Z32" s="1">
         <v>71168</v>
       </c>
-      <c r="AA32" s="1"/>
+      <c r="AA32" s="1">
+        <v>71842</v>
+      </c>
       <c r="AB32" s="1"/>
       <c r="AC32" s="1"/>
       <c r="AD32" s="1"/>
       <c r="AE32" s="1"/>
-    </row>
-    <row r="33" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AF32" s="1"/>
+      <c r="AG32" s="1"/>
+    </row>
+    <row r="33" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>154</v>
       </c>
@@ -9650,13 +9834,17 @@
       <c r="Z33" s="1">
         <v>66049</v>
       </c>
-      <c r="AA33" s="1"/>
+      <c r="AA33" s="1">
+        <v>66732</v>
+      </c>
       <c r="AB33" s="1"/>
       <c r="AC33" s="1"/>
       <c r="AD33" s="1"/>
       <c r="AE33" s="1"/>
-    </row>
-    <row r="34" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AF33" s="1"/>
+      <c r="AG33" s="1"/>
+    </row>
+    <row r="34" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>155</v>
       </c>
@@ -9721,13 +9909,17 @@
       <c r="Z34" s="1">
         <v>39429</v>
       </c>
-      <c r="AA34" s="1"/>
+      <c r="AA34" s="1">
+        <v>39855</v>
+      </c>
       <c r="AB34" s="1"/>
       <c r="AC34" s="1"/>
       <c r="AD34" s="1"/>
       <c r="AE34" s="1"/>
-    </row>
-    <row r="35" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AF34" s="1"/>
+      <c r="AG34" s="1"/>
+    </row>
+    <row r="35" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>156</v>
       </c>
@@ -9792,13 +9984,17 @@
       <c r="Z35" s="1">
         <v>22893</v>
       </c>
-      <c r="AA35" s="1"/>
+      <c r="AA35" s="1">
+        <v>23519</v>
+      </c>
       <c r="AB35" s="1"/>
       <c r="AC35" s="1"/>
       <c r="AD35" s="1"/>
       <c r="AE35" s="1"/>
-    </row>
-    <row r="36" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AF35" s="1"/>
+      <c r="AG35" s="1"/>
+    </row>
+    <row r="36" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>157</v>
       </c>
@@ -9863,13 +10059,17 @@
       <c r="Z36" s="1">
         <v>16378</v>
       </c>
-      <c r="AA36" s="1"/>
+      <c r="AA36" s="1">
+        <v>16908</v>
+      </c>
       <c r="AB36" s="1"/>
       <c r="AC36" s="1"/>
       <c r="AD36" s="1"/>
       <c r="AE36" s="1"/>
-    </row>
-    <row r="37" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AF36" s="1"/>
+      <c r="AG36" s="1"/>
+    </row>
+    <row r="37" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>158</v>
       </c>
@@ -9934,13 +10134,17 @@
       <c r="Z37" s="1">
         <v>14211</v>
       </c>
-      <c r="AA37" s="1"/>
+      <c r="AA37" s="1">
+        <v>15037</v>
+      </c>
       <c r="AB37" s="1"/>
       <c r="AC37" s="1"/>
       <c r="AD37" s="1"/>
       <c r="AE37" s="1"/>
-    </row>
-    <row r="38" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AF37" s="1"/>
+      <c r="AG37" s="1"/>
+    </row>
+    <row r="38" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>159</v>
       </c>
@@ -10005,13 +10209,17 @@
       <c r="Z38" s="1">
         <v>10942</v>
       </c>
-      <c r="AA38" s="1"/>
+      <c r="AA38" s="1">
+        <v>11150</v>
+      </c>
       <c r="AB38" s="1"/>
       <c r="AC38" s="1"/>
       <c r="AD38" s="1"/>
       <c r="AE38" s="1"/>
-    </row>
-    <row r="39" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AF38" s="1"/>
+      <c r="AG38" s="1"/>
+    </row>
+    <row r="39" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>160</v>
       </c>
@@ -10076,13 +10284,17 @@
       <c r="Z39" s="1">
         <v>11703</v>
       </c>
-      <c r="AA39" s="1"/>
+      <c r="AA39" s="1">
+        <v>12271</v>
+      </c>
       <c r="AB39" s="1"/>
       <c r="AC39" s="1"/>
       <c r="AD39" s="1"/>
       <c r="AE39" s="1"/>
-    </row>
-    <row r="40" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AF39" s="1"/>
+      <c r="AG39" s="1"/>
+    </row>
+    <row r="40" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>161</v>
       </c>
@@ -10152,8 +10364,10 @@
       <c r="AC40" s="1"/>
       <c r="AD40" s="1"/>
       <c r="AE40" s="1"/>
-    </row>
-    <row r="41" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AF40" s="1"/>
+      <c r="AG40" s="1"/>
+    </row>
+    <row r="41" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>162</v>
       </c>
@@ -10221,8 +10435,9 @@
       <c r="AC41" s="1"/>
       <c r="AD41" s="1"/>
       <c r="AE41" s="1"/>
-    </row>
-    <row r="42" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AF41" s="1"/>
+    </row>
+    <row r="42" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>163</v>
       </c>
@@ -10286,8 +10501,9 @@
       <c r="AB42" s="1"/>
       <c r="AC42" s="1"/>
       <c r="AD42" s="1"/>
-    </row>
-    <row r="43" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AE42" s="1"/>
+    </row>
+    <row r="43" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>164</v>
       </c>
@@ -10347,8 +10563,9 @@
       <c r="AA43" s="1"/>
       <c r="AB43" s="1"/>
       <c r="AC43" s="1"/>
-    </row>
-    <row r="44" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AD43" s="1"/>
+    </row>
+    <row r="44" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>165</v>
       </c>
@@ -10404,8 +10621,9 @@
       <c r="Z44" s="1"/>
       <c r="AA44" s="1"/>
       <c r="AB44" s="1"/>
-    </row>
-    <row r="45" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AC44" s="1"/>
+    </row>
+    <row r="45" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>166</v>
       </c>
@@ -10457,8 +10675,9 @@
       </c>
       <c r="Z45" s="1"/>
       <c r="AA45" s="1"/>
-    </row>
-    <row r="46" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AB45" s="1"/>
+    </row>
+    <row r="46" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>167</v>
       </c>
@@ -10504,7 +10723,7 @@
       </c>
       <c r="Z46" s="1"/>
     </row>
-    <row r="47" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>168</v>
       </c>
@@ -10543,7 +10762,7 @@
         <v>2542</v>
       </c>
     </row>
-    <row r="48" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>169</v>
       </c>
@@ -10585,7 +10804,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:V24">
+  <sortState ref="A2:X24">
     <sortCondition ref="A2:A24"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Stage 10 Midlands added Signed-off-by: Gerry Mulvenna <git@movingwifi.com>
</commit_message>
<xml_diff>
--- a/europarl/europarl-ireland-2019.xlsx
+++ b/europarl/europarl-ireland-2019.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="14220" windowHeight="8580" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="14220" windowHeight="8580" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Candidates" sheetId="1" r:id="rId1"/>
@@ -5161,8 +5161,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:V18"/>
+    <sheetView topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2:V18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5217,63 +5217,63 @@
         <v>8130</v>
       </c>
       <c r="E2">
-        <f>IF(ISBLANK(F2),-D2,F2-D2)</f>
+        <f t="shared" ref="E2:E18" si="0">IF(ISBLANK(F2),-D2,F2-D2)</f>
         <v>96</v>
       </c>
       <c r="F2" s="1">
         <v>8226</v>
       </c>
       <c r="G2">
-        <f>IF(ISBLANK(H2),-F2,H2-F2)</f>
+        <f t="shared" ref="G2:G18" si="1">IF(ISBLANK(H2),-F2,H2-F2)</f>
         <v>20</v>
       </c>
       <c r="H2" s="1">
         <v>8246</v>
       </c>
       <c r="I2">
-        <f>IF(ISBLANK(J2),-H2,J2-H2)</f>
+        <f t="shared" ref="I2:I18" si="2">IF(ISBLANK(J2),-H2,J2-H2)</f>
         <v>91</v>
       </c>
       <c r="J2" s="1">
         <v>8337</v>
       </c>
       <c r="K2">
-        <f>IF(ISBLANK(L2),-J2,L2-J2)</f>
+        <f t="shared" ref="K2:K18" si="3">IF(ISBLANK(L2),-J2,L2-J2)</f>
         <v>28</v>
       </c>
       <c r="L2" s="1">
         <v>8365</v>
       </c>
       <c r="M2">
-        <f>IF(ISBLANK(N2),-L2,N2-L2)</f>
+        <f t="shared" ref="M2:M18" si="4">IF(ISBLANK(N2),-L2,N2-L2)</f>
         <v>188</v>
       </c>
       <c r="N2" s="1">
         <v>8553</v>
       </c>
       <c r="O2">
-        <f>IF(ISBLANK(P2),-N2,P2-N2)</f>
+        <f t="shared" ref="O2:O18" si="5">IF(ISBLANK(P2),-N2,P2-N2)</f>
         <v>146</v>
       </c>
       <c r="P2" s="1">
         <v>8699</v>
       </c>
       <c r="Q2">
-        <f>IF(ISBLANK(R2),-P2,R2-P2)</f>
+        <f t="shared" ref="Q2:Q18" si="6">IF(ISBLANK(R2),-P2,R2-P2)</f>
         <v>-8699</v>
       </c>
       <c r="R2" s="1">
         <v>0</v>
       </c>
       <c r="S2">
-        <f>IF(ISBLANK(T2),-R2,T2-R2)</f>
+        <f t="shared" ref="S2:S18" si="7">IF(ISBLANK(T2),-R2,T2-R2)</f>
         <v>0</v>
       </c>
       <c r="T2" s="1">
         <v>0</v>
       </c>
       <c r="U2">
-        <f>IF(ISBLANK(V2),-T2,V2-T2)</f>
+        <f t="shared" ref="U2:U18" si="8">IF(ISBLANK(V2),-T2,V2-T2)</f>
         <v>0</v>
       </c>
       <c r="V2" s="1">
@@ -5292,63 +5292,63 @@
         <v>77619</v>
       </c>
       <c r="E3">
-        <f>IF(ISBLANK(F3),-D3,F3-D3)</f>
+        <f t="shared" si="0"/>
         <v>868</v>
       </c>
       <c r="F3" s="1">
         <v>78487</v>
       </c>
       <c r="G3">
-        <f>IF(ISBLANK(H3),-F3,H3-F3)</f>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="H3" s="1">
         <v>78513</v>
       </c>
       <c r="I3">
-        <f>IF(ISBLANK(J3),-H3,J3-H3)</f>
+        <f t="shared" si="2"/>
         <v>99</v>
       </c>
       <c r="J3" s="1">
         <v>78612</v>
       </c>
       <c r="K3">
-        <f>IF(ISBLANK(L3),-J3,L3-J3)</f>
+        <f t="shared" si="3"/>
         <v>41</v>
       </c>
       <c r="L3" s="1">
         <v>78653</v>
       </c>
       <c r="M3">
-        <f>IF(ISBLANK(N3),-L3,N3-L3)</f>
+        <f t="shared" si="4"/>
         <v>375</v>
       </c>
       <c r="N3" s="1">
         <v>79028</v>
       </c>
       <c r="O3">
-        <f>IF(ISBLANK(P3),-N3,P3-N3)</f>
+        <f t="shared" si="5"/>
         <v>409</v>
       </c>
       <c r="P3" s="1">
         <v>79437</v>
       </c>
       <c r="Q3">
-        <f>IF(ISBLANK(R3),-P3,R3-P3)</f>
+        <f t="shared" si="6"/>
         <v>2107</v>
       </c>
       <c r="R3" s="1">
         <v>81544</v>
       </c>
       <c r="S3">
-        <f>IF(ISBLANK(T3),-R3,T3-R3)</f>
+        <f t="shared" si="7"/>
         <v>1377</v>
       </c>
       <c r="T3" s="1">
         <v>82921</v>
       </c>
       <c r="U3">
-        <f>IF(ISBLANK(V3),-T3,V3-T3)</f>
+        <f t="shared" si="8"/>
         <v>930</v>
       </c>
       <c r="V3" s="1">
@@ -5367,63 +5367,63 @@
         <v>56650</v>
       </c>
       <c r="E4">
-        <f>IF(ISBLANK(F4),-D4,F4-D4)</f>
+        <f t="shared" si="0"/>
         <v>1198</v>
       </c>
       <c r="F4" s="1">
         <v>57848</v>
       </c>
       <c r="G4">
-        <f>IF(ISBLANK(H4),-F4,H4-F4)</f>
+        <f t="shared" si="1"/>
         <v>44</v>
       </c>
       <c r="H4" s="1">
         <v>57892</v>
       </c>
       <c r="I4">
-        <f>IF(ISBLANK(J4),-H4,J4-H4)</f>
+        <f t="shared" si="2"/>
         <v>142</v>
       </c>
       <c r="J4" s="1">
         <v>58034</v>
       </c>
       <c r="K4">
-        <f>IF(ISBLANK(L4),-J4,L4-J4)</f>
+        <f t="shared" si="3"/>
         <v>178</v>
       </c>
       <c r="L4" s="1">
         <v>58212</v>
       </c>
       <c r="M4">
-        <f>IF(ISBLANK(N4),-L4,N4-L4)</f>
+        <f t="shared" si="4"/>
         <v>390</v>
       </c>
       <c r="N4" s="1">
         <v>58602</v>
       </c>
       <c r="O4">
-        <f>IF(ISBLANK(P4),-N4,P4-N4)</f>
+        <f t="shared" si="5"/>
         <v>1033</v>
       </c>
       <c r="P4" s="1">
         <v>59635</v>
       </c>
       <c r="Q4">
-        <f>IF(ISBLANK(R4),-P4,R4-P4)</f>
+        <f t="shared" si="6"/>
         <v>1124</v>
       </c>
       <c r="R4" s="1">
         <v>60759</v>
       </c>
       <c r="S4">
-        <f>IF(ISBLANK(T4),-R4,T4-R4)</f>
+        <f t="shared" si="7"/>
         <v>857</v>
       </c>
       <c r="T4" s="1">
         <v>61616</v>
       </c>
       <c r="U4">
-        <f>IF(ISBLANK(V4),-T4,V4-T4)</f>
+        <f t="shared" si="8"/>
         <v>3074</v>
       </c>
       <c r="V4" s="1">
@@ -5442,63 +5442,63 @@
         <v>15991</v>
       </c>
       <c r="E5">
-        <f>IF(ISBLANK(F5),-D5,F5-D5)</f>
+        <f t="shared" si="0"/>
         <v>477</v>
       </c>
       <c r="F5" s="1">
         <v>16468</v>
       </c>
       <c r="G5">
-        <f>IF(ISBLANK(H5),-F5,H5-F5)</f>
+        <f t="shared" si="1"/>
         <v>47</v>
       </c>
       <c r="H5" s="1">
         <v>16515</v>
       </c>
       <c r="I5">
-        <f>IF(ISBLANK(J5),-H5,J5-H5)</f>
+        <f t="shared" si="2"/>
         <v>106</v>
       </c>
       <c r="J5" s="1">
         <v>16621</v>
       </c>
       <c r="K5">
-        <f>IF(ISBLANK(L5),-J5,L5-J5)</f>
+        <f t="shared" si="3"/>
         <v>143</v>
       </c>
       <c r="L5" s="1">
         <v>16764</v>
       </c>
       <c r="M5">
-        <f>IF(ISBLANK(N5),-L5,N5-L5)</f>
+        <f t="shared" si="4"/>
         <v>826</v>
       </c>
       <c r="N5" s="1">
         <v>17590</v>
       </c>
       <c r="O5">
-        <f>IF(ISBLANK(P5),-N5,P5-N5)</f>
+        <f t="shared" si="5"/>
         <v>1722</v>
       </c>
       <c r="P5" s="1">
         <v>19312</v>
       </c>
       <c r="Q5">
-        <f>IF(ISBLANK(R5),-P5,R5-P5)</f>
+        <f t="shared" si="6"/>
         <v>382</v>
       </c>
       <c r="R5" s="1">
         <v>19694</v>
       </c>
       <c r="S5">
-        <f>IF(ISBLANK(T5),-R5,T5-R5)</f>
+        <f t="shared" si="7"/>
         <v>716</v>
       </c>
       <c r="T5" s="1">
         <v>20410</v>
       </c>
       <c r="U5">
-        <f>IF(ISBLANK(V5),-T5,V5-T5)</f>
+        <f t="shared" si="8"/>
         <v>-20410</v>
       </c>
       <c r="V5" s="1">
@@ -5517,63 +5517,63 @@
         <v>85034</v>
       </c>
       <c r="E6">
-        <f>IF(ISBLANK(F6),-D6,F6-D6)</f>
+        <f t="shared" si="0"/>
         <v>1872</v>
       </c>
       <c r="F6" s="1">
         <v>86906</v>
       </c>
       <c r="G6">
-        <f>IF(ISBLANK(H6),-F6,H6-F6)</f>
+        <f t="shared" si="1"/>
         <v>102</v>
       </c>
       <c r="H6" s="1">
         <v>87008</v>
       </c>
       <c r="I6">
-        <f>IF(ISBLANK(J6),-H6,J6-H6)</f>
+        <f t="shared" si="2"/>
         <v>180</v>
       </c>
       <c r="J6" s="1">
         <v>87188</v>
       </c>
       <c r="K6">
-        <f>IF(ISBLANK(L6),-J6,L6-J6)</f>
+        <f t="shared" si="3"/>
         <v>145</v>
       </c>
       <c r="L6" s="1">
         <v>87333</v>
       </c>
       <c r="M6">
-        <f>IF(ISBLANK(N6),-L6,N6-L6)</f>
+        <f t="shared" si="4"/>
         <v>631</v>
       </c>
       <c r="N6" s="1">
         <v>87964</v>
       </c>
       <c r="O6">
-        <f>IF(ISBLANK(P6),-N6,P6-N6)</f>
+        <f t="shared" si="5"/>
         <v>579</v>
       </c>
       <c r="P6" s="1">
         <v>88543</v>
       </c>
       <c r="Q6">
-        <f>IF(ISBLANK(R6),-P6,R6-P6)</f>
+        <f t="shared" si="6"/>
         <v>1644</v>
       </c>
       <c r="R6" s="1">
         <v>90187</v>
       </c>
       <c r="S6">
-        <f>IF(ISBLANK(T6),-R6,T6-R6)</f>
+        <f t="shared" si="7"/>
         <v>1560</v>
       </c>
       <c r="T6" s="1">
         <v>91747</v>
       </c>
       <c r="U6">
-        <f>IF(ISBLANK(V6),-T6,V6-T6)</f>
+        <f t="shared" si="8"/>
         <v>2606</v>
       </c>
       <c r="V6" s="1">
@@ -5592,63 +5592,63 @@
         <v>1352</v>
       </c>
       <c r="E7">
-        <f>IF(ISBLANK(F7),-D7,F7-D7)</f>
+        <f t="shared" si="0"/>
         <v>48</v>
       </c>
       <c r="F7" s="1">
         <v>1400</v>
       </c>
       <c r="G7">
-        <f>IF(ISBLANK(H7),-F7,H7-F7)</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="H7" s="1">
         <v>1412</v>
       </c>
       <c r="I7">
-        <f>IF(ISBLANK(J7),-H7,J7-H7)</f>
+        <f t="shared" si="2"/>
         <v>-1412</v>
       </c>
       <c r="J7" s="1">
         <v>0</v>
       </c>
       <c r="K7">
-        <f>IF(ISBLANK(L7),-J7,L7-J7)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L7" s="1">
         <v>0</v>
       </c>
       <c r="M7">
-        <f>IF(ISBLANK(N7),-L7,N7-L7)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N7" s="1">
         <v>0</v>
       </c>
       <c r="O7">
-        <f>IF(ISBLANK(P7),-N7,P7-N7)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P7" s="1">
         <v>0</v>
       </c>
       <c r="Q7">
-        <f>IF(ISBLANK(R7),-P7,R7-P7)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="R7" s="1">
         <v>0</v>
       </c>
       <c r="S7">
-        <f>IF(ISBLANK(T7),-R7,T7-R7)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="T7" s="1">
         <v>0</v>
       </c>
       <c r="U7">
-        <f>IF(ISBLANK(V7),-T7,V7-T7)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="V7" s="1">
@@ -5667,63 +5667,63 @@
         <v>12378</v>
       </c>
       <c r="E8">
-        <f>IF(ISBLANK(F8),-D8,F8-D8)</f>
+        <f t="shared" si="0"/>
         <v>653</v>
       </c>
       <c r="F8" s="1">
         <v>13031</v>
       </c>
       <c r="G8">
-        <f>IF(ISBLANK(H8),-F8,H8-F8)</f>
+        <f t="shared" si="1"/>
         <v>34</v>
       </c>
       <c r="H8" s="1">
         <v>13065</v>
       </c>
       <c r="I8">
-        <f>IF(ISBLANK(J8),-H8,J8-H8)</f>
+        <f t="shared" si="2"/>
         <v>85</v>
       </c>
       <c r="J8" s="1">
         <v>13150</v>
       </c>
       <c r="K8">
-        <f>IF(ISBLANK(L8),-J8,L8-J8)</f>
+        <f t="shared" si="3"/>
         <v>47</v>
       </c>
       <c r="L8" s="1">
         <v>13197</v>
       </c>
       <c r="M8">
-        <f>IF(ISBLANK(N8),-L8,N8-L8)</f>
+        <f t="shared" si="4"/>
         <v>211</v>
       </c>
       <c r="N8" s="1">
         <v>13408</v>
       </c>
       <c r="O8">
-        <f>IF(ISBLANK(P8),-N8,P8-N8)</f>
+        <f t="shared" si="5"/>
         <v>315</v>
       </c>
       <c r="P8" s="1">
         <v>13723</v>
       </c>
       <c r="Q8">
-        <f>IF(ISBLANK(R8),-P8,R8-P8)</f>
+        <f t="shared" si="6"/>
         <v>366</v>
       </c>
       <c r="R8" s="1">
         <v>14089</v>
       </c>
       <c r="S8">
-        <f>IF(ISBLANK(T8),-R8,T8-R8)</f>
+        <f t="shared" si="7"/>
         <v>-14089</v>
       </c>
       <c r="T8" s="1">
         <v>0</v>
       </c>
       <c r="U8">
-        <f>IF(ISBLANK(V8),-T8,V8-T8)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="V8" s="1">
@@ -5742,63 +5742,63 @@
         <v>2450</v>
       </c>
       <c r="E9">
-        <f>IF(ISBLANK(F9),-D9,F9-D9)</f>
+        <f t="shared" si="0"/>
         <v>112</v>
       </c>
       <c r="F9" s="1">
         <v>2562</v>
       </c>
       <c r="G9">
-        <f>IF(ISBLANK(H9),-F9,H9-F9)</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="H9" s="1">
         <v>2577</v>
       </c>
       <c r="I9">
-        <f>IF(ISBLANK(J9),-H9,J9-H9)</f>
+        <f t="shared" si="2"/>
         <v>77</v>
       </c>
       <c r="J9" s="1">
         <v>2654</v>
       </c>
       <c r="K9">
-        <f>IF(ISBLANK(L9),-J9,L9-J9)</f>
+        <f t="shared" si="3"/>
         <v>40</v>
       </c>
       <c r="L9" s="1">
         <v>2694</v>
       </c>
       <c r="M9">
-        <f>IF(ISBLANK(N9),-L9,N9-L9)</f>
+        <f t="shared" si="4"/>
         <v>-2694</v>
       </c>
       <c r="N9" s="1">
         <v>0</v>
       </c>
       <c r="O9">
-        <f>IF(ISBLANK(P9),-N9,P9-N9)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P9" s="1">
         <v>0</v>
       </c>
       <c r="Q9">
-        <f>IF(ISBLANK(R9),-P9,R9-P9)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="R9" s="1">
         <v>0</v>
       </c>
       <c r="S9">
-        <f>IF(ISBLANK(T9),-R9,T9-R9)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="T9" s="1">
         <v>0</v>
       </c>
       <c r="U9">
-        <f>IF(ISBLANK(V9),-T9,V9-T9)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="V9" s="1">
@@ -5817,63 +5817,63 @@
         <v>134630</v>
       </c>
       <c r="E10">
-        <f>IF(ISBLANK(F10),-D10,F10-D10)</f>
+        <f t="shared" si="0"/>
         <v>-15644</v>
       </c>
       <c r="F10">
         <v>118986</v>
       </c>
       <c r="G10">
-        <f>IF(ISBLANK(H10),-F10,H10-F10)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H10">
         <v>118986</v>
       </c>
       <c r="I10">
-        <f>IF(ISBLANK(J10),-H10,J10-H10)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J10">
         <v>118986</v>
       </c>
       <c r="K10">
-        <f>IF(ISBLANK(L10),-J10,L10-J10)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L10">
         <v>118986</v>
       </c>
       <c r="M10">
-        <f>IF(ISBLANK(N10),-L10,N10-L10)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N10">
         <v>118986</v>
       </c>
       <c r="O10">
-        <f>IF(ISBLANK(P10),-N10,P10-N10)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P10">
         <v>118986</v>
       </c>
       <c r="Q10">
-        <f>IF(ISBLANK(R10),-P10,R10-P10)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="R10">
         <v>118986</v>
       </c>
       <c r="S10">
-        <f>IF(ISBLANK(T10),-R10,T10-R10)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="T10">
         <v>118986</v>
       </c>
       <c r="U10">
-        <f>IF(ISBLANK(V10),-T10,V10-T10)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="V10">
@@ -5892,63 +5892,63 @@
         <v>51019</v>
       </c>
       <c r="E11">
-        <f>IF(ISBLANK(F11),-D11,F11-D11)</f>
+        <f t="shared" si="0"/>
         <v>1712</v>
       </c>
       <c r="F11" s="1">
         <v>52731</v>
       </c>
       <c r="G11">
-        <f>IF(ISBLANK(H11),-F11,H11-F11)</f>
+        <f t="shared" si="1"/>
         <v>90</v>
       </c>
       <c r="H11" s="1">
         <v>52821</v>
       </c>
       <c r="I11">
-        <f>IF(ISBLANK(J11),-H11,J11-H11)</f>
+        <f t="shared" si="2"/>
         <v>155</v>
       </c>
       <c r="J11" s="1">
         <v>52976</v>
       </c>
       <c r="K11">
-        <f>IF(ISBLANK(L11),-J11,L11-J11)</f>
+        <f t="shared" si="3"/>
         <v>92</v>
       </c>
       <c r="L11" s="1">
         <v>53068</v>
       </c>
       <c r="M11">
-        <f>IF(ISBLANK(N11),-L11,N11-L11)</f>
+        <f t="shared" si="4"/>
         <v>898</v>
       </c>
       <c r="N11" s="1">
         <v>53966</v>
       </c>
       <c r="O11">
-        <f>IF(ISBLANK(P11),-N11,P11-N11)</f>
+        <f t="shared" si="5"/>
         <v>582</v>
       </c>
       <c r="P11" s="1">
         <v>54548</v>
       </c>
       <c r="Q11">
-        <f>IF(ISBLANK(R11),-P11,R11-P11)</f>
+        <f t="shared" si="6"/>
         <v>907</v>
       </c>
       <c r="R11" s="1">
         <v>55455</v>
       </c>
       <c r="S11">
-        <f>IF(ISBLANK(T11),-R11,T11-R11)</f>
+        <f t="shared" si="7"/>
         <v>3187</v>
       </c>
       <c r="T11" s="1">
         <v>58642</v>
       </c>
       <c r="U11">
-        <f>IF(ISBLANK(V11),-T11,V11-T11)</f>
+        <f t="shared" si="8"/>
         <v>2136</v>
       </c>
       <c r="V11" s="1">
@@ -5967,63 +5967,63 @@
         <v>1322</v>
       </c>
       <c r="E12">
-        <f>IF(ISBLANK(F12),-D12,F12-D12)</f>
+        <f t="shared" si="0"/>
         <v>53</v>
       </c>
       <c r="F12" s="1">
         <v>1375</v>
       </c>
       <c r="G12">
-        <f>IF(ISBLANK(H12),-F12,H12-F12)</f>
+        <f t="shared" si="1"/>
         <v>71</v>
       </c>
       <c r="H12" s="1">
         <v>1446</v>
       </c>
       <c r="I12">
-        <f>IF(ISBLANK(J12),-H12,J12-H12)</f>
+        <f t="shared" si="2"/>
         <v>44</v>
       </c>
       <c r="J12" s="1">
         <v>1490</v>
       </c>
       <c r="K12">
-        <f>IF(ISBLANK(L12),-J12,L12-J12)</f>
+        <f t="shared" si="3"/>
         <v>-1490</v>
       </c>
       <c r="L12" s="1">
         <v>0</v>
       </c>
       <c r="M12">
-        <f>IF(ISBLANK(N12),-L12,N12-L12)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N12" s="1">
         <v>0</v>
       </c>
       <c r="O12">
-        <f>IF(ISBLANK(P12),-N12,P12-N12)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P12" s="1">
         <v>0</v>
       </c>
       <c r="Q12">
-        <f>IF(ISBLANK(R12),-P12,R12-P12)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="R12" s="1">
         <v>0</v>
       </c>
       <c r="S12">
-        <f>IF(ISBLANK(T12),-R12,T12-R12)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="T12" s="1">
         <v>0</v>
       </c>
       <c r="U12">
-        <f>IF(ISBLANK(V12),-T12,V12-T12)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="V12" s="1">
@@ -6042,63 +6042,63 @@
         <v>789</v>
       </c>
       <c r="E13">
-        <f>IF(ISBLANK(F13),-D13,F13-D13)</f>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="F13">
         <v>811</v>
       </c>
       <c r="G13">
-        <f>IF(ISBLANK(H13),-F13,H13-F13)</f>
+        <f t="shared" si="1"/>
         <v>-811</v>
       </c>
       <c r="H13" s="1">
         <v>0</v>
       </c>
       <c r="I13">
-        <f>IF(ISBLANK(J13),-H13,J13-H13)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J13" s="1">
         <v>0</v>
       </c>
       <c r="K13">
-        <f>IF(ISBLANK(L13),-J13,L13-J13)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L13" s="1">
         <v>0</v>
       </c>
       <c r="M13">
-        <f>IF(ISBLANK(N13),-L13,N13-L13)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N13" s="1">
         <v>0</v>
       </c>
       <c r="O13">
-        <f>IF(ISBLANK(P13),-N13,P13-N13)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P13" s="1">
         <v>0</v>
       </c>
       <c r="Q13">
-        <f>IF(ISBLANK(R13),-P13,R13-P13)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="R13" s="1">
         <v>0</v>
       </c>
       <c r="S13">
-        <f>IF(ISBLANK(T13),-R13,T13-R13)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="T13" s="1">
         <v>0</v>
       </c>
       <c r="U13">
-        <f>IF(ISBLANK(V13),-T13,V13-T13)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="V13" s="1">
@@ -6117,63 +6117,63 @@
         <v>3132</v>
       </c>
       <c r="E14">
-        <f>IF(ISBLANK(F14),-D14,F14-D14)</f>
+        <f t="shared" si="0"/>
         <v>104</v>
       </c>
       <c r="F14" s="1">
         <v>3236</v>
       </c>
       <c r="G14">
-        <f>IF(ISBLANK(H14),-F14,H14-F14)</f>
+        <f t="shared" si="1"/>
         <v>77</v>
       </c>
       <c r="H14" s="1">
         <v>3313</v>
       </c>
       <c r="I14">
-        <f>IF(ISBLANK(J14),-H14,J14-H14)</f>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="J14" s="1">
         <v>3326</v>
       </c>
       <c r="K14">
-        <f>IF(ISBLANK(L14),-J14,L14-J14)</f>
+        <f t="shared" si="3"/>
         <v>151</v>
       </c>
       <c r="L14" s="1">
         <v>3477</v>
       </c>
       <c r="M14">
-        <f>IF(ISBLANK(N14),-L14,N14-L14)</f>
+        <f t="shared" si="4"/>
         <v>-3477</v>
       </c>
       <c r="N14" s="1">
         <v>0</v>
       </c>
       <c r="O14">
-        <f>IF(ISBLANK(P14),-N14,P14-N14)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P14" s="1">
         <v>0</v>
       </c>
       <c r="Q14">
-        <f>IF(ISBLANK(R14),-P14,R14-P14)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="R14" s="1">
         <v>0</v>
       </c>
       <c r="S14">
-        <f>IF(ISBLANK(T14),-R14,T14-R14)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="T14" s="1">
         <v>0</v>
       </c>
       <c r="U14">
-        <f>IF(ISBLANK(V14),-T14,V14-T14)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="V14" s="1">
@@ -6192,63 +6192,63 @@
         <v>6897</v>
       </c>
       <c r="E15">
-        <f>IF(ISBLANK(F15),-D15,F15-D15)</f>
+        <f t="shared" si="0"/>
         <v>303</v>
       </c>
       <c r="F15" s="1">
         <v>7200</v>
       </c>
       <c r="G15">
-        <f>IF(ISBLANK(H15),-F15,H15-F15)</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="H15" s="1">
         <v>7220</v>
       </c>
       <c r="I15">
-        <f>IF(ISBLANK(J15),-H15,J15-H15)</f>
+        <f t="shared" si="2"/>
         <v>84</v>
       </c>
       <c r="J15" s="1">
         <v>7304</v>
       </c>
       <c r="K15">
-        <f>IF(ISBLANK(L15),-J15,L15-J15)</f>
+        <f t="shared" si="3"/>
         <v>141</v>
       </c>
       <c r="L15" s="1">
         <v>7445</v>
       </c>
       <c r="M15">
-        <f>IF(ISBLANK(N15),-L15,N15-L15)</f>
+        <f t="shared" si="4"/>
         <v>232</v>
       </c>
       <c r="N15" s="1">
         <v>7677</v>
       </c>
       <c r="O15">
-        <f>IF(ISBLANK(P15),-N15,P15-N15)</f>
+        <f t="shared" si="5"/>
         <v>-7677</v>
       </c>
       <c r="P15" s="1">
         <v>0</v>
       </c>
       <c r="Q15">
-        <f>IF(ISBLANK(R15),-P15,R15-P15)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="R15" s="1">
         <v>0</v>
       </c>
       <c r="S15">
-        <f>IF(ISBLANK(T15),-R15,T15-R15)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="T15" s="1">
         <v>0</v>
       </c>
       <c r="U15">
-        <f>IF(ISBLANK(V15),-T15,V15-T15)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="V15" s="1">
@@ -6267,63 +6267,63 @@
         <v>30220</v>
       </c>
       <c r="E16">
-        <f>IF(ISBLANK(F16),-D16,F16-D16)</f>
+        <f t="shared" si="0"/>
         <v>864</v>
       </c>
       <c r="F16" s="1">
         <v>31084</v>
       </c>
       <c r="G16">
-        <f>IF(ISBLANK(H16),-F16,H16-F16)</f>
+        <f t="shared" si="1"/>
         <v>38</v>
       </c>
       <c r="H16" s="1">
         <v>31122</v>
       </c>
       <c r="I16">
-        <f>IF(ISBLANK(J16),-H16,J16-H16)</f>
+        <f t="shared" si="2"/>
         <v>21</v>
       </c>
       <c r="J16" s="1">
         <v>31143</v>
       </c>
       <c r="K16">
-        <f>IF(ISBLANK(L16),-J16,L16-J16)</f>
+        <f t="shared" si="3"/>
         <v>55</v>
       </c>
       <c r="L16" s="1">
         <v>31198</v>
       </c>
       <c r="M16">
-        <f>IF(ISBLANK(N16),-L16,N16-L16)</f>
+        <f t="shared" si="4"/>
         <v>273</v>
       </c>
       <c r="N16" s="1">
         <v>31471</v>
       </c>
       <c r="O16">
-        <f>IF(ISBLANK(P16),-N16,P16-N16)</f>
+        <f t="shared" si="5"/>
         <v>422</v>
       </c>
       <c r="P16" s="1">
         <v>31893</v>
       </c>
       <c r="Q16">
-        <f>IF(ISBLANK(R16),-P16,R16-P16)</f>
+        <f t="shared" si="6"/>
         <v>148</v>
       </c>
       <c r="R16" s="1">
         <v>32041</v>
       </c>
       <c r="S16">
-        <f>IF(ISBLANK(T16),-R16,T16-R16)</f>
+        <f t="shared" si="7"/>
         <v>673</v>
       </c>
       <c r="T16" s="1">
         <v>32714</v>
       </c>
       <c r="U16">
-        <f>IF(ISBLANK(V16),-T16,V16-T16)</f>
+        <f t="shared" si="8"/>
         <v>1896</v>
       </c>
       <c r="V16" s="1">
@@ -6342,63 +6342,63 @@
         <v>42814</v>
       </c>
       <c r="E17">
-        <f>IF(ISBLANK(F17),-D17,F17-D17)</f>
+        <f t="shared" si="0"/>
         <v>1226</v>
       </c>
       <c r="F17" s="1">
         <v>44040</v>
       </c>
       <c r="G17">
-        <f>IF(ISBLANK(H17),-F17,H17-F17)</f>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="H17" s="1">
         <v>44059</v>
       </c>
       <c r="I17">
-        <f>IF(ISBLANK(J17),-H17,J17-H17)</f>
+        <f t="shared" si="2"/>
         <v>17</v>
       </c>
       <c r="J17" s="1">
         <v>44076</v>
       </c>
       <c r="K17">
-        <f>IF(ISBLANK(L17),-J17,L17-J17)</f>
+        <f t="shared" si="3"/>
         <v>54</v>
       </c>
       <c r="L17" s="1">
         <v>44130</v>
       </c>
       <c r="M17">
-        <f>IF(ISBLANK(N17),-L17,N17-L17)</f>
+        <f t="shared" si="4"/>
         <v>125</v>
       </c>
       <c r="N17" s="1">
         <v>44255</v>
       </c>
       <c r="O17">
-        <f>IF(ISBLANK(P17),-N17,P17-N17)</f>
+        <f t="shared" si="5"/>
         <v>437</v>
       </c>
       <c r="P17" s="1">
         <v>44692</v>
       </c>
       <c r="Q17">
-        <f>IF(ISBLANK(R17),-P17,R17-P17)</f>
+        <f t="shared" si="6"/>
         <v>144</v>
       </c>
       <c r="R17" s="1">
         <v>44836</v>
       </c>
       <c r="S17">
-        <f>IF(ISBLANK(T17),-R17,T17-R17)</f>
+        <f t="shared" si="7"/>
         <v>399</v>
       </c>
       <c r="T17" s="1">
         <v>45235</v>
       </c>
       <c r="U17">
-        <f>IF(ISBLANK(V17),-T17,V17-T17)</f>
+        <f t="shared" si="8"/>
         <v>1585</v>
       </c>
       <c r="V17" s="1">
@@ -6417,63 +6417,63 @@
         <v>64500</v>
       </c>
       <c r="E18">
-        <f>IF(ISBLANK(F18),-D18,F18-D18)</f>
+        <f t="shared" si="0"/>
         <v>6036</v>
       </c>
       <c r="F18" s="1">
         <v>70536</v>
       </c>
       <c r="G18">
-        <f>IF(ISBLANK(H18),-F18,H18-F18)</f>
+        <f t="shared" si="1"/>
         <v>83</v>
       </c>
       <c r="H18" s="1">
         <v>70619</v>
       </c>
       <c r="I18">
-        <f>IF(ISBLANK(J18),-H18,J18-H18)</f>
+        <f t="shared" si="2"/>
         <v>41</v>
       </c>
       <c r="J18" s="1">
         <v>70660</v>
       </c>
       <c r="K18">
-        <f>IF(ISBLANK(L18),-J18,L18-J18)</f>
+        <f t="shared" si="3"/>
         <v>71</v>
       </c>
       <c r="L18" s="1">
         <v>70731</v>
       </c>
       <c r="M18">
-        <f>IF(ISBLANK(N18),-L18,N18-L18)</f>
+        <f t="shared" si="4"/>
         <v>694</v>
       </c>
       <c r="N18" s="1">
         <v>71425</v>
       </c>
       <c r="O18">
-        <f>IF(ISBLANK(P18),-N18,P18-N18)</f>
+        <f t="shared" si="5"/>
         <v>368</v>
       </c>
       <c r="P18" s="1">
         <v>71793</v>
       </c>
       <c r="Q18">
-        <f>IF(ISBLANK(R18),-P18,R18-P18)</f>
+        <f t="shared" si="6"/>
         <v>472</v>
       </c>
       <c r="R18" s="1">
         <v>72265</v>
       </c>
       <c r="S18">
-        <f>IF(ISBLANK(T18),-R18,T18-R18)</f>
+        <f t="shared" si="7"/>
         <v>1851</v>
       </c>
       <c r="T18" s="1">
         <v>74116</v>
       </c>
       <c r="U18">
-        <f>IF(ISBLANK(V18),-T18,V18-T18)</f>
+        <f t="shared" si="8"/>
         <v>1940</v>
       </c>
       <c r="V18" s="1">
@@ -6542,19 +6542,19 @@
         <v>197</v>
       </c>
       <c r="D21">
-        <f t="shared" ref="D21:D36" si="0">FIND(",",B21)</f>
+        <f t="shared" ref="D21:D36" si="9">FIND(",",B21)</f>
         <v>9</v>
       </c>
       <c r="E21" t="str">
-        <f t="shared" ref="E21:E36" si="1">LEFT(B21,D21-1)</f>
+        <f t="shared" ref="E21:E36" si="10">LEFT(B21,D21-1)</f>
         <v>Flanagan</v>
       </c>
       <c r="F21" t="str">
-        <f t="shared" ref="F21:F36" si="2">RIGHT(B21,LEN(B21)-(D21+1))</f>
+        <f t="shared" ref="F21:F36" si="11">RIGHT(B21,LEN(B21)-(D21+1))</f>
         <v>Luke 'Ming'</v>
       </c>
       <c r="G21" t="str">
-        <f t="shared" ref="G21:G36" si="3">F21&amp;" "&amp;E21</f>
+        <f t="shared" ref="G21:G36" si="12">F21&amp;" "&amp;E21</f>
         <v>Luke 'Ming' Flanagan</v>
       </c>
       <c r="J21" t="s">
@@ -6573,19 +6573,19 @@
         <v>198</v>
       </c>
       <c r="D22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>7</v>
       </c>
       <c r="E22" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>Carthy</v>
       </c>
       <c r="F22" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>Matt</v>
       </c>
       <c r="G22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>Matt Carthy</v>
       </c>
       <c r="J22" t="s">
@@ -6638,19 +6638,19 @@
         <v>199</v>
       </c>
       <c r="D23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="E23" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>Walsh</v>
       </c>
       <c r="F23" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>Maria</v>
       </c>
       <c r="G23" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>Maria Walsh</v>
       </c>
       <c r="J23" t="s">
@@ -6703,19 +6703,19 @@
         <v>200</v>
       </c>
       <c r="D24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="E24" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>Casey</v>
       </c>
       <c r="F24" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>Peter</v>
       </c>
       <c r="G24" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>Peter Casey</v>
       </c>
       <c r="J24" t="s">
@@ -6768,19 +6768,19 @@
         <v>201</v>
       </c>
       <c r="D25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>7</v>
       </c>
       <c r="E25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>McHugh</v>
       </c>
       <c r="F25" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>Saoirse</v>
       </c>
       <c r="G25" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>Saoirse McHugh</v>
       </c>
       <c r="J25" t="s">
@@ -6833,19 +6833,19 @@
         <v>202</v>
       </c>
       <c r="D26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="E26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>Smith</v>
       </c>
       <c r="F26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>Brendan</v>
       </c>
       <c r="G26" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>Brendan Smith</v>
       </c>
       <c r="J26" t="s">
@@ -6898,19 +6898,19 @@
         <v>203</v>
       </c>
       <c r="D27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>9</v>
       </c>
       <c r="E27" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>Rabbitte</v>
       </c>
       <c r="F27" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>Anne</v>
       </c>
       <c r="G27" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>Anne Rabbitte</v>
       </c>
       <c r="J27" t="s">
@@ -6963,19 +6963,19 @@
         <v>204</v>
       </c>
       <c r="D28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>12</v>
       </c>
       <c r="E28" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>Healy Eames</v>
       </c>
       <c r="F28" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>Fidelma</v>
       </c>
       <c r="G28" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>Fidelma Healy Eames</v>
       </c>
       <c r="J28" t="s">
@@ -7028,19 +7028,19 @@
         <v>205</v>
       </c>
       <c r="D29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>9</v>
       </c>
       <c r="E29" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>Hannigan</v>
       </c>
       <c r="F29" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>Dominic</v>
       </c>
       <c r="G29" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>Dominic Hannigan</v>
       </c>
       <c r="J29" t="s">
@@ -7090,19 +7090,19 @@
         <v>206</v>
       </c>
       <c r="D30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
       <c r="E30" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>Brennan</v>
       </c>
       <c r="F30" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>Cyril</v>
       </c>
       <c r="G30" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>Cyril Brennan</v>
       </c>
       <c r="J30" t="s">
@@ -7149,19 +7149,19 @@
         <v>207</v>
       </c>
       <c r="D31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>7</v>
       </c>
       <c r="E31" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>O'Dowd</v>
       </c>
       <c r="F31" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>Michael</v>
       </c>
       <c r="G31" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>Michael O'Dowd</v>
       </c>
       <c r="J31" t="s">
@@ -7206,19 +7206,19 @@
         <v>208</v>
       </c>
       <c r="D32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>9</v>
       </c>
       <c r="E32" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>O'Connor</v>
       </c>
       <c r="F32" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>Olive</v>
       </c>
       <c r="G32" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>Olive O'Connor</v>
       </c>
       <c r="J32" t="s">
@@ -7260,19 +7260,19 @@
         <v>209</v>
       </c>
       <c r="D33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
       <c r="E33" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>Mahapatra</v>
       </c>
       <c r="F33" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>Dilip</v>
       </c>
       <c r="G33" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>Dilip Mahapatra</v>
       </c>
       <c r="J33" t="s">
@@ -7310,19 +7310,19 @@
         <v>210</v>
       </c>
       <c r="D34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>7</v>
       </c>
       <c r="E34" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>Greene</v>
       </c>
       <c r="F34" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>Patrick</v>
       </c>
       <c r="G34" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>Patrick Greene</v>
       </c>
       <c r="J34" t="s">
@@ -7360,19 +7360,19 @@
         <v>211</v>
       </c>
       <c r="D35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>7</v>
       </c>
       <c r="E35" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>Miller</v>
       </c>
       <c r="F35" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>James</v>
       </c>
       <c r="G35" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>James Miller</v>
       </c>
       <c r="J35" t="s">
@@ -7400,19 +7400,19 @@
         <v>212</v>
       </c>
       <c r="D36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
       <c r="E36" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>Mulcahy</v>
       </c>
       <c r="F36" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>Diarmaid</v>
       </c>
       <c r="G36" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="12"/>
         <v>Diarmaid Mulcahy</v>
       </c>
       <c r="J36" t="s">
@@ -7466,8 +7466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG49"/>
   <sheetViews>
-    <sheetView topLeftCell="W1" workbookViewId="0">
-      <selection activeCell="Y2" sqref="Y2:AD24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7528,1121 +7528,1121 @@
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
       <c r="D2" s="1">
-        <v>4665</v>
+        <v>118444</v>
       </c>
       <c r="E2">
         <f>IF(ISBLANK(F2),-D2,F2-D2)</f>
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="F2" s="1">
-        <v>4691</v>
+        <v>118489</v>
       </c>
       <c r="G2">
         <f>IF(ISBLANK(H2),-F2,H2-F2)</f>
-        <v>43</v>
+        <v>186</v>
       </c>
       <c r="H2" s="1">
-        <v>4734</v>
+        <v>118675</v>
       </c>
       <c r="I2">
         <f>IF(ISBLANK(J2),-H2,J2-H2)</f>
-        <v>57</v>
+        <v>98</v>
       </c>
       <c r="J2" s="1">
-        <v>4791</v>
+        <v>118773</v>
       </c>
       <c r="K2">
         <f>IF(ISBLANK(L2),-J2,L2-J2)</f>
-        <v>50</v>
+        <v>350</v>
       </c>
       <c r="L2" s="1">
-        <v>4841</v>
+        <v>119123</v>
       </c>
       <c r="M2">
         <f>IF(ISBLANK(N2),-L2,N2-L2)</f>
-        <v>115</v>
+        <v>257</v>
       </c>
       <c r="N2" s="1">
-        <v>4956</v>
+        <v>119380</v>
       </c>
       <c r="O2">
         <f>IF(ISBLANK(P2),-N2,P2-N2)</f>
-        <v>72</v>
+        <v>165</v>
       </c>
       <c r="P2" s="1">
-        <v>5028</v>
+        <v>119545</v>
       </c>
       <c r="Q2">
         <f>IF(ISBLANK(R2),-P2,R2-P2)</f>
-        <v>104</v>
+        <v>170</v>
       </c>
       <c r="R2" s="1">
-        <v>5132</v>
+        <v>119715</v>
       </c>
       <c r="S2">
         <f>IF(ISBLANK(T2),-R2,T2-R2)</f>
-        <v>-5132</v>
+        <v>168</v>
       </c>
       <c r="T2" s="1">
-        <v>0</v>
+        <v>119883</v>
       </c>
       <c r="U2">
         <f>IF(ISBLANK(V2),-T2,V2-T2)</f>
         <v>0</v>
       </c>
       <c r="V2" s="1">
-        <v>0</v>
+        <v>119883</v>
       </c>
       <c r="W2">
         <f>IF(ISBLANK(X2),-V2,X2-V2)</f>
         <v>0</v>
       </c>
       <c r="X2" s="1">
-        <v>0</v>
+        <v>119883</v>
       </c>
       <c r="Y2">
         <f>IF(ISBLANK(Z2),-X2,Z2-X2)</f>
         <v>0</v>
       </c>
       <c r="Z2" s="1">
-        <v>0</v>
+        <v>119883</v>
       </c>
       <c r="AA2">
         <f>IF(ISBLANK(AB2),-Z2,AB2-Z2)</f>
         <v>0</v>
       </c>
       <c r="AB2" s="1">
-        <v>0</v>
+        <v>119883</v>
       </c>
       <c r="AC2">
         <f>IF(ISBLANK(AD2),-AB2,AD2-AB2)</f>
         <v>0</v>
       </c>
       <c r="AD2" s="1">
-        <v>0</v>
+        <v>119883</v>
       </c>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D3" s="1">
-        <v>69166</v>
+        <v>84083</v>
       </c>
       <c r="E3">
         <f>IF(ISBLANK(F3),-D3,F3-D3)</f>
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="F3" s="1">
-        <v>69201</v>
+        <v>84106</v>
       </c>
       <c r="G3">
         <f>IF(ISBLANK(H3),-F3,H3-F3)</f>
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="H3" s="1">
-        <v>69272</v>
+        <v>84164</v>
       </c>
       <c r="I3">
         <f>IF(ISBLANK(J3),-H3,J3-H3)</f>
-        <v>44</v>
+        <v>74</v>
       </c>
       <c r="J3" s="1">
-        <v>69316</v>
+        <v>84238</v>
       </c>
       <c r="K3">
         <f>IF(ISBLANK(L3),-J3,L3-J3)</f>
-        <v>66</v>
+        <v>150</v>
       </c>
       <c r="L3" s="1">
-        <v>69382</v>
+        <v>84388</v>
       </c>
       <c r="M3">
         <f>IF(ISBLANK(N3),-L3,N3-L3)</f>
-        <v>129</v>
+        <v>171</v>
       </c>
       <c r="N3" s="1">
-        <v>69511</v>
+        <v>84559</v>
       </c>
       <c r="O3">
         <f>IF(ISBLANK(P3),-N3,P3-N3)</f>
-        <v>45</v>
+        <v>95</v>
       </c>
       <c r="P3" s="1">
-        <v>69556</v>
+        <v>84654</v>
       </c>
       <c r="Q3">
         <f>IF(ISBLANK(R3),-P3,R3-P3)</f>
-        <v>116</v>
+        <v>187</v>
       </c>
       <c r="R3" s="1">
-        <v>69672</v>
+        <v>84841</v>
       </c>
       <c r="S3">
         <f>IF(ISBLANK(T3),-R3,T3-R3)</f>
-        <v>1226</v>
+        <v>130</v>
       </c>
       <c r="T3" s="1">
-        <v>70898</v>
+        <v>84971</v>
       </c>
       <c r="U3">
         <f>IF(ISBLANK(V3),-T3,V3-T3)</f>
-        <v>270</v>
+        <v>480</v>
       </c>
       <c r="V3" s="1">
-        <v>71168</v>
+        <v>85451</v>
       </c>
       <c r="W3">
         <f>IF(ISBLANK(X3),-V3,X3-V3)</f>
-        <v>674</v>
+        <v>575</v>
       </c>
       <c r="X3" s="1">
-        <v>71842</v>
+        <v>86026</v>
       </c>
       <c r="Y3">
         <f>IF(ISBLANK(Z3),-X3,Z3-X3)</f>
-        <v>291</v>
+        <v>1010</v>
       </c>
       <c r="Z3" s="1">
-        <v>72133</v>
+        <v>87036</v>
       </c>
       <c r="AA3">
         <f>IF(ISBLANK(AB3),-Z3,AB3-Z3)</f>
-        <v>720</v>
+        <v>928</v>
       </c>
       <c r="AB3" s="1">
-        <v>72853</v>
+        <v>87964</v>
       </c>
       <c r="AC3">
         <f>IF(ISBLANK(AD3),-AB3,AD3-AB3)</f>
-        <v>929</v>
+        <v>637</v>
       </c>
       <c r="AD3" s="1">
-        <v>73782</v>
+        <v>88601</v>
       </c>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="D4" s="1">
-        <v>10582</v>
+        <v>81741</v>
       </c>
       <c r="E4">
         <f>IF(ISBLANK(F4),-D4,F4-D4)</f>
-        <v>57</v>
+        <v>253</v>
       </c>
       <c r="F4" s="1">
-        <v>10639</v>
+        <v>81994</v>
       </c>
       <c r="G4">
         <f>IF(ISBLANK(H4),-F4,H4-F4)</f>
-        <v>106</v>
+        <v>130</v>
       </c>
       <c r="H4" s="1">
-        <v>10745</v>
+        <v>82124</v>
       </c>
       <c r="I4">
         <f>IF(ISBLANK(J4),-H4,J4-H4)</f>
-        <v>138</v>
+        <v>211</v>
       </c>
       <c r="J4" s="1">
-        <v>10883</v>
+        <v>82335</v>
       </c>
       <c r="K4">
         <f>IF(ISBLANK(L4),-J4,L4-J4)</f>
-        <v>54</v>
+        <v>323</v>
       </c>
       <c r="L4" s="1">
-        <v>10937</v>
+        <v>82658</v>
       </c>
       <c r="M4">
         <f>IF(ISBLANK(N4),-L4,N4-L4)</f>
-        <v>300</v>
+        <v>206</v>
       </c>
       <c r="N4" s="1">
-        <v>11237</v>
+        <v>82864</v>
       </c>
       <c r="O4">
         <f>IF(ISBLANK(P4),-N4,P4-N4)</f>
-        <v>159</v>
+        <v>556</v>
       </c>
       <c r="P4" s="1">
-        <v>11396</v>
+        <v>83420</v>
       </c>
       <c r="Q4">
         <f>IF(ISBLANK(R4),-P4,R4-P4)</f>
-        <v>322</v>
+        <v>351</v>
       </c>
       <c r="R4" s="1">
-        <v>11718</v>
+        <v>83771</v>
       </c>
       <c r="S4">
         <f>IF(ISBLANK(T4),-R4,T4-R4)</f>
-        <v>908</v>
+        <v>217</v>
       </c>
       <c r="T4" s="1">
-        <v>12626</v>
+        <v>83988</v>
       </c>
       <c r="U4">
         <f>IF(ISBLANK(V4),-T4,V4-T4)</f>
-        <v>1585</v>
+        <v>247</v>
       </c>
       <c r="V4" s="1">
-        <v>14211</v>
+        <v>84235</v>
       </c>
       <c r="W4">
         <f>IF(ISBLANK(X4),-V4,X4-V4)</f>
-        <v>826</v>
+        <v>1001</v>
       </c>
       <c r="X4" s="1">
-        <v>15037</v>
+        <v>85236</v>
       </c>
       <c r="Y4">
         <f>IF(ISBLANK(Z4),-X4,Z4-X4)</f>
-        <v>429</v>
+        <v>2333</v>
       </c>
       <c r="Z4" s="1">
-        <v>15466</v>
+        <v>87569</v>
       </c>
       <c r="AA4">
         <f>IF(ISBLANK(AB4),-Z4,AB4-Z4)</f>
-        <v>1664</v>
+        <v>1190</v>
       </c>
       <c r="AB4" s="1">
-        <v>17130</v>
+        <v>88759</v>
       </c>
       <c r="AC4">
         <f>IF(ISBLANK(AD4),-AB4,AD4-AB4)</f>
-        <v>-17130</v>
+        <v>1476</v>
       </c>
       <c r="AD4" s="1">
-        <v>0</v>
+        <v>90235</v>
       </c>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D5" s="1">
-        <v>64605</v>
+        <v>79072</v>
       </c>
       <c r="E5">
         <f>IF(ISBLANK(F5),-D5,F5-D5)</f>
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="F5" s="1">
-        <v>64631</v>
+        <v>79140</v>
       </c>
       <c r="G5">
         <f>IF(ISBLANK(H5),-F5,H5-F5)</f>
-        <v>61</v>
+        <v>142</v>
       </c>
       <c r="H5" s="1">
-        <v>64692</v>
+        <v>79282</v>
       </c>
       <c r="I5">
         <f>IF(ISBLANK(J5),-H5,J5-H5)</f>
-        <v>71</v>
+        <v>105</v>
       </c>
       <c r="J5" s="1">
-        <v>64763</v>
+        <v>79387</v>
       </c>
       <c r="K5">
         <f>IF(ISBLANK(L5),-J5,L5-J5)</f>
-        <v>136</v>
+        <v>186</v>
       </c>
       <c r="L5" s="1">
-        <v>64899</v>
+        <v>79573</v>
       </c>
       <c r="M5">
         <f>IF(ISBLANK(N5),-L5,N5-L5)</f>
-        <v>106</v>
+        <v>168</v>
       </c>
       <c r="N5" s="1">
-        <v>65005</v>
+        <v>79741</v>
       </c>
       <c r="O5">
         <f>IF(ISBLANK(P5),-N5,P5-N5)</f>
-        <v>110</v>
+        <v>204</v>
       </c>
       <c r="P5" s="1">
-        <v>65115</v>
+        <v>79945</v>
       </c>
       <c r="Q5">
         <f>IF(ISBLANK(R5),-P5,R5-P5)</f>
-        <v>137</v>
+        <v>305</v>
       </c>
       <c r="R5" s="1">
-        <v>65252</v>
+        <v>80250</v>
       </c>
       <c r="S5">
         <f>IF(ISBLANK(T5),-R5,T5-R5)</f>
-        <v>306</v>
+        <v>127</v>
       </c>
       <c r="T5" s="1">
-        <v>65558</v>
+        <v>80377</v>
       </c>
       <c r="U5">
         <f>IF(ISBLANK(V5),-T5,V5-T5)</f>
-        <v>491</v>
+        <v>446</v>
       </c>
       <c r="V5" s="1">
-        <v>66049</v>
+        <v>80823</v>
       </c>
       <c r="W5">
         <f>IF(ISBLANK(X5),-V5,X5-V5)</f>
-        <v>683</v>
+        <v>991</v>
       </c>
       <c r="X5" s="1">
-        <v>66732</v>
+        <v>81814</v>
       </c>
       <c r="Y5">
         <f>IF(ISBLANK(Z5),-X5,Z5-X5)</f>
-        <v>542</v>
+        <v>1119</v>
       </c>
       <c r="Z5" s="1">
-        <v>67274</v>
+        <v>82933</v>
       </c>
       <c r="AA5">
         <f>IF(ISBLANK(AB5),-Z5,AB5-Z5)</f>
-        <v>622</v>
+        <v>958</v>
       </c>
       <c r="AB5" s="1">
-        <v>67896</v>
+        <v>83891</v>
       </c>
       <c r="AC5">
         <f>IF(ISBLANK(AD5),-AB5,AD5-AB5)</f>
-        <v>1194</v>
+        <v>1108</v>
       </c>
       <c r="AD5" s="1">
-        <v>69090</v>
+        <v>84999</v>
       </c>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D6" s="1">
-        <v>38738</v>
+        <v>75946</v>
       </c>
       <c r="E6">
         <f>IF(ISBLANK(F6),-D6,F6-D6)</f>
-        <v>17</v>
+        <v>100</v>
       </c>
       <c r="F6" s="1">
-        <v>38755</v>
+        <v>76046</v>
       </c>
       <c r="G6">
         <f>IF(ISBLANK(H6),-F6,H6-F6)</f>
-        <v>33</v>
+        <v>201</v>
       </c>
       <c r="H6" s="1">
-        <v>38788</v>
+        <v>76247</v>
       </c>
       <c r="I6">
         <f>IF(ISBLANK(J6),-H6,J6-H6)</f>
-        <v>16</v>
+        <v>126</v>
       </c>
       <c r="J6" s="1">
-        <v>38804</v>
+        <v>76373</v>
       </c>
       <c r="K6">
         <f>IF(ISBLANK(L6),-J6,L6-J6)</f>
-        <v>38</v>
+        <v>272</v>
       </c>
       <c r="L6" s="1">
-        <v>38842</v>
+        <v>76645</v>
       </c>
       <c r="M6">
         <f>IF(ISBLANK(N6),-L6,N6-L6)</f>
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="N6" s="1">
-        <v>38926</v>
+        <v>76719</v>
       </c>
       <c r="O6">
         <f>IF(ISBLANK(P6),-N6,P6-N6)</f>
-        <v>24</v>
+        <v>301</v>
       </c>
       <c r="P6" s="1">
-        <v>38950</v>
+        <v>77020</v>
       </c>
       <c r="Q6">
         <f>IF(ISBLANK(R6),-P6,R6-P6)</f>
-        <v>46</v>
+        <v>283</v>
       </c>
       <c r="R6" s="1">
-        <v>38996</v>
+        <v>77303</v>
       </c>
       <c r="S6">
         <f>IF(ISBLANK(T6),-R6,T6-R6)</f>
-        <v>298</v>
+        <v>112</v>
       </c>
       <c r="T6" s="1">
-        <v>39294</v>
+        <v>77415</v>
       </c>
       <c r="U6">
         <f>IF(ISBLANK(V6),-T6,V6-T6)</f>
-        <v>135</v>
+        <v>339</v>
       </c>
       <c r="V6" s="1">
-        <v>39429</v>
+        <v>77754</v>
       </c>
       <c r="W6">
         <f>IF(ISBLANK(X6),-V6,X6-V6)</f>
-        <v>426</v>
+        <v>1066</v>
       </c>
       <c r="X6" s="1">
-        <v>39855</v>
+        <v>78820</v>
       </c>
       <c r="Y6">
         <f>IF(ISBLANK(Z6),-X6,Z6-X6)</f>
-        <v>159</v>
+        <v>1295</v>
       </c>
       <c r="Z6" s="1">
-        <v>40014</v>
+        <v>80115</v>
       </c>
       <c r="AA6">
         <f>IF(ISBLANK(AB6),-Z6,AB6-Z6)</f>
-        <v>572</v>
+        <v>593</v>
       </c>
       <c r="AB6" s="1">
-        <v>40586</v>
+        <v>80708</v>
       </c>
       <c r="AC6">
         <f>IF(ISBLANK(AD6),-AB6,AD6-AB6)</f>
-        <v>483</v>
+        <v>1290</v>
       </c>
       <c r="AD6" s="1">
-        <v>41069</v>
+        <v>81998</v>
       </c>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="D7" s="1">
-        <v>3182</v>
+        <v>69166</v>
       </c>
       <c r="E7">
         <f>IF(ISBLANK(F7),-D7,F7-D7)</f>
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="F7" s="1">
-        <v>3197</v>
+        <v>69201</v>
       </c>
       <c r="G7">
         <f>IF(ISBLANK(H7),-F7,H7-F7)</f>
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="H7" s="1">
-        <v>3257</v>
+        <v>69272</v>
       </c>
       <c r="I7">
         <f>IF(ISBLANK(J7),-H7,J7-H7)</f>
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J7" s="1">
-        <v>3300</v>
+        <v>69316</v>
       </c>
       <c r="K7">
         <f>IF(ISBLANK(L7),-J7,L7-J7)</f>
-        <v>32</v>
+        <v>66</v>
       </c>
       <c r="L7" s="1">
-        <v>3332</v>
+        <v>69382</v>
       </c>
       <c r="M7">
         <f>IF(ISBLANK(N7),-L7,N7-L7)</f>
-        <v>-3332</v>
+        <v>129</v>
       </c>
       <c r="N7" s="1">
-        <v>0</v>
+        <v>69511</v>
       </c>
       <c r="O7">
         <f>IF(ISBLANK(P7),-N7,P7-N7)</f>
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="P7" s="1">
-        <v>0</v>
+        <v>69556</v>
       </c>
       <c r="Q7">
         <f>IF(ISBLANK(R7),-P7,R7-P7)</f>
-        <v>0</v>
+        <v>116</v>
       </c>
       <c r="R7" s="1">
-        <v>0</v>
+        <v>69672</v>
       </c>
       <c r="S7">
         <f>IF(ISBLANK(T7),-R7,T7-R7)</f>
-        <v>0</v>
+        <v>1226</v>
       </c>
       <c r="T7" s="1">
-        <v>0</v>
+        <v>70898</v>
       </c>
       <c r="U7">
         <f>IF(ISBLANK(V7),-T7,V7-T7)</f>
-        <v>0</v>
+        <v>270</v>
       </c>
       <c r="V7" s="1">
-        <v>0</v>
+        <v>71168</v>
       </c>
       <c r="W7">
         <f>IF(ISBLANK(X7),-V7,X7-V7)</f>
-        <v>0</v>
+        <v>674</v>
       </c>
       <c r="X7" s="1">
-        <v>0</v>
+        <v>71842</v>
       </c>
       <c r="Y7">
         <f>IF(ISBLANK(Z7),-X7,Z7-X7)</f>
-        <v>0</v>
+        <v>291</v>
       </c>
       <c r="Z7" s="1">
-        <v>0</v>
+        <v>72133</v>
       </c>
       <c r="AA7">
         <f>IF(ISBLANK(AB7),-Z7,AB7-Z7)</f>
-        <v>0</v>
+        <v>720</v>
       </c>
       <c r="AB7" s="1">
-        <v>0</v>
+        <v>72853</v>
       </c>
       <c r="AC7">
         <f>IF(ISBLANK(AD7),-AB7,AD7-AB7)</f>
-        <v>0</v>
+        <v>929</v>
       </c>
       <c r="AD7" s="1">
-        <v>0</v>
+        <v>73782</v>
       </c>
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="D8" s="1">
-        <v>9306</v>
+        <v>64605</v>
       </c>
       <c r="E8">
         <f>IF(ISBLANK(F8),-D8,F8-D8)</f>
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F8" s="1">
-        <v>9331</v>
+        <v>64631</v>
       </c>
       <c r="G8">
         <f>IF(ISBLANK(H8),-F8,H8-F8)</f>
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="H8" s="1">
-        <v>9401</v>
+        <v>64692</v>
       </c>
       <c r="I8">
         <f>IF(ISBLANK(J8),-H8,J8-H8)</f>
-        <v>35</v>
+        <v>71</v>
       </c>
       <c r="J8" s="1">
-        <v>9436</v>
+        <v>64763</v>
       </c>
       <c r="K8">
         <f>IF(ISBLANK(L8),-J8,L8-J8)</f>
-        <v>60</v>
+        <v>136</v>
       </c>
       <c r="L8" s="1">
-        <v>9496</v>
+        <v>64899</v>
       </c>
       <c r="M8">
         <f>IF(ISBLANK(N8),-L8,N8-L8)</f>
-        <v>228</v>
+        <v>106</v>
       </c>
       <c r="N8" s="1">
-        <v>9724</v>
+        <v>65005</v>
       </c>
       <c r="O8">
         <f>IF(ISBLANK(P8),-N8,P8-N8)</f>
-        <v>145</v>
+        <v>110</v>
       </c>
       <c r="P8" s="1">
-        <v>9869</v>
+        <v>65115</v>
       </c>
       <c r="Q8">
         <f>IF(ISBLANK(R8),-P8,R8-P8)</f>
-        <v>106</v>
+        <v>137</v>
       </c>
       <c r="R8" s="1">
-        <v>9975</v>
+        <v>65252</v>
       </c>
       <c r="S8">
         <f>IF(ISBLANK(T8),-R8,T8-R8)</f>
-        <v>247</v>
+        <v>306</v>
       </c>
       <c r="T8" s="1">
-        <v>10222</v>
+        <v>65558</v>
       </c>
       <c r="U8">
         <f>IF(ISBLANK(V8),-T8,V8-T8)</f>
-        <v>616</v>
+        <v>491</v>
       </c>
       <c r="V8" s="1">
-        <v>10838</v>
+        <v>66049</v>
       </c>
       <c r="W8">
         <f>IF(ISBLANK(X8),-V8,X8-V8)</f>
-        <v>-10838</v>
+        <v>683</v>
       </c>
       <c r="X8" s="1">
-        <v>0</v>
+        <v>66732</v>
       </c>
       <c r="Y8">
         <f>IF(ISBLANK(Z8),-X8,Z8-X8)</f>
-        <v>0</v>
+        <v>542</v>
       </c>
       <c r="Z8" s="1">
-        <v>0</v>
+        <v>67274</v>
       </c>
       <c r="AA8">
         <f>IF(ISBLANK(AB8),-Z8,AB8-Z8)</f>
-        <v>0</v>
+        <v>622</v>
       </c>
       <c r="AB8" s="1">
-        <v>0</v>
+        <v>67896</v>
       </c>
       <c r="AC8">
         <f>IF(ISBLANK(AD8),-AB8,AD8-AB8)</f>
-        <v>0</v>
+        <v>1194</v>
       </c>
       <c r="AD8" s="1">
-        <v>0</v>
+        <v>69090</v>
       </c>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="D9" s="1">
-        <v>7475</v>
+        <v>38738</v>
       </c>
       <c r="E9">
         <f>IF(ISBLANK(F9),-D9,F9-D9)</f>
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="F9" s="1">
-        <v>7498</v>
+        <v>38755</v>
       </c>
       <c r="G9">
         <f>IF(ISBLANK(H9),-F9,H9-F9)</f>
-        <v>98</v>
+        <v>33</v>
       </c>
       <c r="H9" s="1">
-        <v>7596</v>
+        <v>38788</v>
       </c>
       <c r="I9">
         <f>IF(ISBLANK(J9),-H9,J9-H9)</f>
-        <v>142</v>
+        <v>16</v>
       </c>
       <c r="J9" s="1">
-        <v>7738</v>
+        <v>38804</v>
       </c>
       <c r="K9">
         <f>IF(ISBLANK(L9),-J9,L9-J9)</f>
-        <v>70</v>
+        <v>38</v>
       </c>
       <c r="L9" s="1">
-        <v>7808</v>
+        <v>38842</v>
       </c>
       <c r="M9">
         <f>IF(ISBLANK(N9),-L9,N9-L9)</f>
-        <v>197</v>
+        <v>84</v>
       </c>
       <c r="N9" s="1">
-        <v>8005</v>
+        <v>38926</v>
       </c>
       <c r="O9">
         <f>IF(ISBLANK(P9),-N9,P9-N9)</f>
-        <v>192</v>
+        <v>24</v>
       </c>
       <c r="P9" s="1">
-        <v>8197</v>
+        <v>38950</v>
       </c>
       <c r="Q9">
         <f>IF(ISBLANK(R9),-P9,R9-P9)</f>
-        <v>176</v>
+        <v>46</v>
       </c>
       <c r="R9" s="1">
-        <v>8373</v>
+        <v>38996</v>
       </c>
       <c r="S9">
         <f>IF(ISBLANK(T9),-R9,T9-R9)</f>
-        <v>188</v>
+        <v>298</v>
       </c>
       <c r="T9" s="1">
-        <v>8561</v>
+        <v>39294</v>
       </c>
       <c r="U9">
         <f>IF(ISBLANK(V9),-T9,V9-T9)</f>
-        <v>-8561</v>
+        <v>135</v>
       </c>
       <c r="V9" s="1">
-        <v>0</v>
+        <v>39429</v>
       </c>
       <c r="W9">
         <f>IF(ISBLANK(X9),-V9,X9-V9)</f>
-        <v>0</v>
+        <v>426</v>
       </c>
       <c r="X9" s="1">
-        <v>0</v>
+        <v>39855</v>
       </c>
       <c r="Y9">
         <f>IF(ISBLANK(Z9),-X9,Z9-X9)</f>
-        <v>0</v>
+        <v>159</v>
       </c>
       <c r="Z9" s="1">
-        <v>0</v>
+        <v>40014</v>
       </c>
       <c r="AA9">
         <f>IF(ISBLANK(AB9),-Z9,AB9-Z9)</f>
-        <v>0</v>
+        <v>572</v>
       </c>
       <c r="AB9" s="1">
-        <v>0</v>
+        <v>40586</v>
       </c>
       <c r="AC9">
         <f>IF(ISBLANK(AD9),-AB9,AD9-AB9)</f>
-        <v>0</v>
+        <v>483</v>
       </c>
       <c r="AD9" s="1">
-        <v>0</v>
+        <v>41069</v>
       </c>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="D10" s="1">
-        <v>84083</v>
+        <v>22075</v>
       </c>
       <c r="E10">
         <f>IF(ISBLANK(F10),-D10,F10-D10)</f>
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="F10" s="1">
-        <v>84106</v>
+        <v>22113</v>
       </c>
       <c r="G10">
         <f>IF(ISBLANK(H10),-F10,H10-F10)</f>
-        <v>58</v>
+        <v>80</v>
       </c>
       <c r="H10" s="1">
-        <v>84164</v>
+        <v>22193</v>
       </c>
       <c r="I10">
         <f>IF(ISBLANK(J10),-H10,J10-H10)</f>
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="J10" s="1">
-        <v>84238</v>
+        <v>22251</v>
       </c>
       <c r="K10">
         <f>IF(ISBLANK(L10),-J10,L10-J10)</f>
-        <v>150</v>
+        <v>70</v>
       </c>
       <c r="L10" s="1">
-        <v>84388</v>
+        <v>22321</v>
       </c>
       <c r="M10">
         <f>IF(ISBLANK(N10),-L10,N10-L10)</f>
-        <v>171</v>
+        <v>62</v>
       </c>
       <c r="N10" s="1">
-        <v>84559</v>
+        <v>22383</v>
       </c>
       <c r="O10">
         <f>IF(ISBLANK(P10),-N10,P10-N10)</f>
-        <v>95</v>
+        <v>70</v>
       </c>
       <c r="P10" s="1">
-        <v>84654</v>
+        <v>22453</v>
       </c>
       <c r="Q10">
         <f>IF(ISBLANK(R10),-P10,R10-P10)</f>
-        <v>187</v>
+        <v>173</v>
       </c>
       <c r="R10" s="1">
-        <v>84841</v>
+        <v>22626</v>
       </c>
       <c r="S10">
         <f>IF(ISBLANK(T10),-R10,T10-R10)</f>
-        <v>130</v>
+        <v>74</v>
       </c>
       <c r="T10" s="1">
-        <v>84971</v>
+        <v>22700</v>
       </c>
       <c r="U10">
         <f>IF(ISBLANK(V10),-T10,V10-T10)</f>
-        <v>480</v>
+        <v>193</v>
       </c>
       <c r="V10" s="1">
-        <v>85451</v>
+        <v>22893</v>
       </c>
       <c r="W10">
         <f>IF(ISBLANK(X10),-V10,X10-V10)</f>
-        <v>575</v>
+        <v>626</v>
       </c>
       <c r="X10" s="1">
-        <v>86026</v>
+        <v>23519</v>
       </c>
       <c r="Y10">
         <f>IF(ISBLANK(Z10),-X10,Z10-X10)</f>
-        <v>1010</v>
+        <v>330</v>
       </c>
       <c r="Z10" s="1">
-        <v>87036</v>
+        <v>23849</v>
       </c>
       <c r="AA10">
         <f>IF(ISBLANK(AB10),-Z10,AB10-Z10)</f>
-        <v>928</v>
+        <v>483</v>
       </c>
       <c r="AB10" s="1">
-        <v>87964</v>
+        <v>24332</v>
       </c>
       <c r="AC10">
         <f>IF(ISBLANK(AD10),-AB10,AD10-AB10)</f>
-        <v>637</v>
+        <v>600</v>
       </c>
       <c r="AD10" s="1">
-        <v>88601</v>
+        <v>24932</v>
       </c>
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="D11" s="1">
-        <v>118444</v>
+        <v>14802</v>
       </c>
       <c r="E11">
         <f>IF(ISBLANK(F11),-D11,F11-D11)</f>
-        <v>45</v>
+        <v>156</v>
       </c>
       <c r="F11" s="1">
-        <v>118489</v>
+        <v>14958</v>
       </c>
       <c r="G11">
         <f>IF(ISBLANK(H11),-F11,H11-F11)</f>
-        <v>186</v>
+        <v>51</v>
       </c>
       <c r="H11" s="1">
-        <v>118675</v>
+        <v>15009</v>
       </c>
       <c r="I11">
         <f>IF(ISBLANK(J11),-H11,J11-H11)</f>
-        <v>98</v>
+        <v>198</v>
       </c>
       <c r="J11" s="1">
-        <v>118773</v>
+        <v>15207</v>
       </c>
       <c r="K11">
         <f>IF(ISBLANK(L11),-J11,L11-J11)</f>
-        <v>350</v>
+        <v>146</v>
       </c>
       <c r="L11" s="1">
-        <v>119123</v>
+        <v>15353</v>
       </c>
       <c r="M11">
         <f>IF(ISBLANK(N11),-L11,N11-L11)</f>
-        <v>257</v>
+        <v>41</v>
       </c>
       <c r="N11" s="1">
-        <v>119380</v>
+        <v>15394</v>
       </c>
       <c r="O11">
         <f>IF(ISBLANK(P11),-N11,P11-N11)</f>
-        <v>165</v>
+        <v>392</v>
       </c>
       <c r="P11" s="1">
-        <v>119545</v>
+        <v>15786</v>
       </c>
       <c r="Q11">
         <f>IF(ISBLANK(R11),-P11,R11-P11)</f>
-        <v>170</v>
+        <v>321</v>
       </c>
       <c r="R11" s="1">
-        <v>119715</v>
+        <v>16107</v>
       </c>
       <c r="S11">
         <f>IF(ISBLANK(T11),-R11,T11-R11)</f>
-        <v>168</v>
+        <v>101</v>
       </c>
       <c r="T11" s="1">
-        <v>119883</v>
+        <v>16208</v>
       </c>
       <c r="U11">
         <f>IF(ISBLANK(V11),-T11,V11-T11)</f>
-        <v>0</v>
+        <v>170</v>
       </c>
       <c r="V11" s="1">
-        <v>119883</v>
+        <v>16378</v>
       </c>
       <c r="W11">
         <f>IF(ISBLANK(X11),-V11,X11-V11)</f>
-        <v>0</v>
+        <v>530</v>
       </c>
       <c r="X11" s="1">
-        <v>119883</v>
+        <v>16908</v>
       </c>
       <c r="Y11">
         <f>IF(ISBLANK(Z11),-X11,Z11-X11)</f>
-        <v>0</v>
+        <v>490</v>
       </c>
       <c r="Z11" s="1">
-        <v>119883</v>
+        <v>17398</v>
       </c>
       <c r="AA11">
         <f>IF(ISBLANK(AB11),-Z11,AB11-Z11)</f>
-        <v>0</v>
+        <v>329</v>
       </c>
       <c r="AB11" s="1">
-        <v>119883</v>
+        <v>17727</v>
       </c>
       <c r="AC11">
         <f>IF(ISBLANK(AD11),-AB11,AD11-AB11)</f>
-        <v>0</v>
+        <v>749</v>
       </c>
       <c r="AD11" s="1">
-        <v>119883</v>
+        <v>18476</v>
       </c>
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="D12" s="1">
-        <v>2395</v>
+        <v>10582</v>
       </c>
       <c r="E12">
         <f>IF(ISBLANK(F12),-D12,F12-D12)</f>
-        <v>14</v>
+        <v>57</v>
       </c>
       <c r="F12" s="1">
-        <v>2409</v>
+        <v>10639</v>
       </c>
       <c r="G12">
         <f>IF(ISBLANK(H12),-F12,H12-F12)</f>
-        <v>-2409</v>
+        <v>106</v>
       </c>
       <c r="H12" s="1">
-        <v>0</v>
+        <v>10745</v>
       </c>
       <c r="I12">
         <f>IF(ISBLANK(J12),-H12,J12-H12)</f>
-        <v>0</v>
+        <v>138</v>
       </c>
       <c r="J12" s="1">
-        <v>0</v>
+        <v>10883</v>
       </c>
       <c r="K12">
         <f>IF(ISBLANK(L12),-J12,L12-J12)</f>
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="L12" s="1">
-        <v>0</v>
+        <v>10937</v>
       </c>
       <c r="M12">
         <f>IF(ISBLANK(N12),-L12,N12-L12)</f>
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="N12" s="1">
-        <v>0</v>
+        <v>11237</v>
       </c>
       <c r="O12">
         <f>IF(ISBLANK(P12),-N12,P12-N12)</f>
-        <v>0</v>
+        <v>159</v>
       </c>
       <c r="P12" s="1">
-        <v>0</v>
+        <v>11396</v>
       </c>
       <c r="Q12">
         <f>IF(ISBLANK(R12),-P12,R12-P12)</f>
-        <v>0</v>
+        <v>322</v>
       </c>
       <c r="R12" s="1">
-        <v>0</v>
+        <v>11718</v>
       </c>
       <c r="S12">
         <f>IF(ISBLANK(T12),-R12,T12-R12)</f>
-        <v>0</v>
+        <v>908</v>
       </c>
       <c r="T12" s="1">
-        <v>0</v>
+        <v>12626</v>
       </c>
       <c r="U12">
         <f>IF(ISBLANK(V12),-T12,V12-T12)</f>
-        <v>0</v>
+        <v>1585</v>
       </c>
       <c r="V12" s="1">
-        <v>0</v>
+        <v>14211</v>
       </c>
       <c r="W12">
         <f>IF(ISBLANK(X12),-V12,X12-V12)</f>
-        <v>0</v>
+        <v>826</v>
       </c>
       <c r="X12" s="1">
-        <v>0</v>
+        <v>15037</v>
       </c>
       <c r="Y12">
         <f>IF(ISBLANK(Z12),-X12,Z12-X12)</f>
-        <v>0</v>
+        <v>429</v>
       </c>
       <c r="Z12" s="1">
-        <v>0</v>
+        <v>15466</v>
       </c>
       <c r="AA12">
         <f>IF(ISBLANK(AB12),-Z12,AB12-Z12)</f>
-        <v>0</v>
+        <v>1664</v>
       </c>
       <c r="AB12" s="1">
-        <v>0</v>
+        <v>17130</v>
       </c>
       <c r="AC12">
         <f>IF(ISBLANK(AD12),-AB12,AD12-AB12)</f>
-        <v>0</v>
+        <v>-17130</v>
       </c>
       <c r="AD12" s="1">
         <v>0</v>
@@ -8650,94 +8650,94 @@
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D13" s="1">
-        <v>9423</v>
+        <v>9823</v>
       </c>
       <c r="E13">
         <f>IF(ISBLANK(F13),-D13,F13-D13)</f>
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="F13" s="1">
-        <v>9455</v>
+        <v>9860</v>
       </c>
       <c r="G13">
         <f>IF(ISBLANK(H13),-F13,H13-F13)</f>
-        <v>325</v>
+        <v>76</v>
       </c>
       <c r="H13" s="1">
-        <v>9780</v>
+        <v>9936</v>
       </c>
       <c r="I13">
         <f>IF(ISBLANK(J13),-H13,J13-H13)</f>
-        <v>75</v>
+        <v>54</v>
       </c>
       <c r="J13" s="1">
-        <v>9855</v>
+        <v>9990</v>
       </c>
       <c r="K13">
         <f>IF(ISBLANK(L13),-J13,L13-J13)</f>
-        <v>114</v>
+        <v>184</v>
       </c>
       <c r="L13" s="1">
-        <v>9969</v>
+        <v>10174</v>
       </c>
       <c r="M13">
         <f>IF(ISBLANK(N13),-L13,N13-L13)</f>
-        <v>280</v>
+        <v>52</v>
       </c>
       <c r="N13" s="1">
-        <v>10249</v>
+        <v>10226</v>
       </c>
       <c r="O13">
         <f>IF(ISBLANK(P13),-N13,P13-N13)</f>
-        <v>78</v>
+        <v>168</v>
       </c>
       <c r="P13" s="1">
-        <v>10327</v>
+        <v>10394</v>
       </c>
       <c r="Q13">
         <f>IF(ISBLANK(R13),-P13,R13-P13)</f>
-        <v>137</v>
+        <v>214</v>
       </c>
       <c r="R13" s="1">
-        <v>10464</v>
+        <v>10608</v>
       </c>
       <c r="S13">
         <f>IF(ISBLANK(T13),-R13,T13-R13)</f>
-        <v>79</v>
+        <v>48</v>
       </c>
       <c r="T13" s="1">
-        <v>10543</v>
+        <v>10656</v>
       </c>
       <c r="U13">
         <f>IF(ISBLANK(V13),-T13,V13-T13)</f>
-        <v>1160</v>
+        <v>286</v>
       </c>
       <c r="V13" s="1">
-        <v>11703</v>
+        <v>10942</v>
       </c>
       <c r="W13">
         <f>IF(ISBLANK(X13),-V13,X13-V13)</f>
-        <v>568</v>
+        <v>208</v>
       </c>
       <c r="X13" s="1">
-        <v>12271</v>
+        <v>11150</v>
       </c>
       <c r="Y13">
         <f>IF(ISBLANK(Z13),-X13,Z13-X13)</f>
-        <v>499</v>
+        <v>-11150</v>
       </c>
       <c r="Z13" s="1">
-        <v>12770</v>
+        <v>0</v>
       </c>
       <c r="AA13">
         <f>IF(ISBLANK(AB13),-Z13,AB13-Z13)</f>
-        <v>-12770</v>
+        <v>0</v>
       </c>
       <c r="AB13" s="1">
         <v>0</v>
@@ -8752,291 +8752,291 @@
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
       <c r="D14" s="1">
-        <v>79072</v>
+        <v>9423</v>
       </c>
       <c r="E14">
         <f>IF(ISBLANK(F14),-D14,F14-D14)</f>
-        <v>68</v>
+        <v>32</v>
       </c>
       <c r="F14" s="1">
-        <v>79140</v>
+        <v>9455</v>
       </c>
       <c r="G14">
         <f>IF(ISBLANK(H14),-F14,H14-F14)</f>
-        <v>142</v>
+        <v>325</v>
       </c>
       <c r="H14" s="1">
-        <v>79282</v>
+        <v>9780</v>
       </c>
       <c r="I14">
         <f>IF(ISBLANK(J14),-H14,J14-H14)</f>
-        <v>105</v>
+        <v>75</v>
       </c>
       <c r="J14" s="1">
-        <v>79387</v>
+        <v>9855</v>
       </c>
       <c r="K14">
         <f>IF(ISBLANK(L14),-J14,L14-J14)</f>
-        <v>186</v>
+        <v>114</v>
       </c>
       <c r="L14" s="1">
-        <v>79573</v>
+        <v>9969</v>
       </c>
       <c r="M14">
         <f>IF(ISBLANK(N14),-L14,N14-L14)</f>
-        <v>168</v>
+        <v>280</v>
       </c>
       <c r="N14" s="1">
-        <v>79741</v>
+        <v>10249</v>
       </c>
       <c r="O14">
         <f>IF(ISBLANK(P14),-N14,P14-N14)</f>
-        <v>204</v>
+        <v>78</v>
       </c>
       <c r="P14" s="1">
-        <v>79945</v>
+        <v>10327</v>
       </c>
       <c r="Q14">
         <f>IF(ISBLANK(R14),-P14,R14-P14)</f>
-        <v>305</v>
+        <v>137</v>
       </c>
       <c r="R14" s="1">
-        <v>80250</v>
+        <v>10464</v>
       </c>
       <c r="S14">
         <f>IF(ISBLANK(T14),-R14,T14-R14)</f>
-        <v>127</v>
+        <v>79</v>
       </c>
       <c r="T14" s="1">
-        <v>80377</v>
+        <v>10543</v>
       </c>
       <c r="U14">
         <f>IF(ISBLANK(V14),-T14,V14-T14)</f>
-        <v>446</v>
+        <v>1160</v>
       </c>
       <c r="V14" s="1">
-        <v>80823</v>
+        <v>11703</v>
       </c>
       <c r="W14">
         <f>IF(ISBLANK(X14),-V14,X14-V14)</f>
-        <v>991</v>
+        <v>568</v>
       </c>
       <c r="X14" s="1">
-        <v>81814</v>
+        <v>12271</v>
       </c>
       <c r="Y14">
         <f>IF(ISBLANK(Z14),-X14,Z14-X14)</f>
-        <v>1119</v>
+        <v>499</v>
       </c>
       <c r="Z14" s="1">
-        <v>82933</v>
+        <v>12770</v>
       </c>
       <c r="AA14">
         <f>IF(ISBLANK(AB14),-Z14,AB14-Z14)</f>
-        <v>958</v>
+        <v>-12770</v>
       </c>
       <c r="AB14" s="1">
-        <v>83891</v>
+        <v>0</v>
       </c>
       <c r="AC14">
         <f>IF(ISBLANK(AD14),-AB14,AD14-AB14)</f>
-        <v>1108</v>
+        <v>0</v>
       </c>
       <c r="AD14" s="1">
-        <v>84999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="D15" s="1">
-        <v>22075</v>
+        <v>9306</v>
       </c>
       <c r="E15">
         <f>IF(ISBLANK(F15),-D15,F15-D15)</f>
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="F15" s="1">
-        <v>22113</v>
+        <v>9331</v>
       </c>
       <c r="G15">
         <f>IF(ISBLANK(H15),-F15,H15-F15)</f>
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="H15" s="1">
-        <v>22193</v>
+        <v>9401</v>
       </c>
       <c r="I15">
         <f>IF(ISBLANK(J15),-H15,J15-H15)</f>
-        <v>58</v>
+        <v>35</v>
       </c>
       <c r="J15" s="1">
-        <v>22251</v>
+        <v>9436</v>
       </c>
       <c r="K15">
         <f>IF(ISBLANK(L15),-J15,L15-J15)</f>
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="L15" s="1">
-        <v>22321</v>
+        <v>9496</v>
       </c>
       <c r="M15">
         <f>IF(ISBLANK(N15),-L15,N15-L15)</f>
-        <v>62</v>
+        <v>228</v>
       </c>
       <c r="N15" s="1">
-        <v>22383</v>
+        <v>9724</v>
       </c>
       <c r="O15">
         <f>IF(ISBLANK(P15),-N15,P15-N15)</f>
-        <v>70</v>
+        <v>145</v>
       </c>
       <c r="P15" s="1">
-        <v>22453</v>
+        <v>9869</v>
       </c>
       <c r="Q15">
         <f>IF(ISBLANK(R15),-P15,R15-P15)</f>
-        <v>173</v>
+        <v>106</v>
       </c>
       <c r="R15" s="1">
-        <v>22626</v>
+        <v>9975</v>
       </c>
       <c r="S15">
         <f>IF(ISBLANK(T15),-R15,T15-R15)</f>
-        <v>74</v>
+        <v>247</v>
       </c>
       <c r="T15" s="1">
-        <v>22700</v>
+        <v>10222</v>
       </c>
       <c r="U15">
         <f>IF(ISBLANK(V15),-T15,V15-T15)</f>
-        <v>193</v>
+        <v>616</v>
       </c>
       <c r="V15" s="1">
-        <v>22893</v>
+        <v>10838</v>
       </c>
       <c r="W15">
         <f>IF(ISBLANK(X15),-V15,X15-V15)</f>
-        <v>626</v>
+        <v>-10838</v>
       </c>
       <c r="X15" s="1">
-        <v>23519</v>
+        <v>0</v>
       </c>
       <c r="Y15">
         <f>IF(ISBLANK(Z15),-X15,Z15-X15)</f>
-        <v>330</v>
+        <v>0</v>
       </c>
       <c r="Z15" s="1">
-        <v>23849</v>
+        <v>0</v>
       </c>
       <c r="AA15">
         <f>IF(ISBLANK(AB15),-Z15,AB15-Z15)</f>
-        <v>483</v>
+        <v>0</v>
       </c>
       <c r="AB15" s="1">
-        <v>24332</v>
+        <v>0</v>
       </c>
       <c r="AC15">
         <f>IF(ISBLANK(AD15),-AB15,AD15-AB15)</f>
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="AD15" s="1">
-        <v>24932</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D16" s="1">
-        <v>9823</v>
+        <v>7475</v>
       </c>
       <c r="E16">
         <f>IF(ISBLANK(F16),-D16,F16-D16)</f>
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="F16" s="1">
-        <v>9860</v>
+        <v>7498</v>
       </c>
       <c r="G16">
         <f>IF(ISBLANK(H16),-F16,H16-F16)</f>
-        <v>76</v>
+        <v>98</v>
       </c>
       <c r="H16" s="1">
-        <v>9936</v>
+        <v>7596</v>
       </c>
       <c r="I16">
         <f>IF(ISBLANK(J16),-H16,J16-H16)</f>
-        <v>54</v>
+        <v>142</v>
       </c>
       <c r="J16" s="1">
-        <v>9990</v>
+        <v>7738</v>
       </c>
       <c r="K16">
         <f>IF(ISBLANK(L16),-J16,L16-J16)</f>
-        <v>184</v>
+        <v>70</v>
       </c>
       <c r="L16" s="1">
-        <v>10174</v>
+        <v>7808</v>
       </c>
       <c r="M16">
         <f>IF(ISBLANK(N16),-L16,N16-L16)</f>
-        <v>52</v>
+        <v>197</v>
       </c>
       <c r="N16" s="1">
-        <v>10226</v>
+        <v>8005</v>
       </c>
       <c r="O16">
         <f>IF(ISBLANK(P16),-N16,P16-N16)</f>
-        <v>168</v>
+        <v>192</v>
       </c>
       <c r="P16" s="1">
-        <v>10394</v>
+        <v>8197</v>
       </c>
       <c r="Q16">
         <f>IF(ISBLANK(R16),-P16,R16-P16)</f>
-        <v>214</v>
+        <v>176</v>
       </c>
       <c r="R16" s="1">
-        <v>10608</v>
+        <v>8373</v>
       </c>
       <c r="S16">
         <f>IF(ISBLANK(T16),-R16,T16-R16)</f>
-        <v>48</v>
+        <v>188</v>
       </c>
       <c r="T16" s="1">
-        <v>10656</v>
+        <v>8561</v>
       </c>
       <c r="U16">
         <f>IF(ISBLANK(V16),-T16,V16-T16)</f>
-        <v>286</v>
+        <v>-8561</v>
       </c>
       <c r="V16" s="1">
-        <v>10942</v>
+        <v>0</v>
       </c>
       <c r="W16">
         <f>IF(ISBLANK(X16),-V16,X16-V16)</f>
-        <v>208</v>
+        <v>0</v>
       </c>
       <c r="X16" s="1">
-        <v>11150</v>
+        <v>0</v>
       </c>
       <c r="Y16">
         <f>IF(ISBLANK(Z16),-X16,Z16-X16)</f>
-        <v>-11150</v>
+        <v>0</v>
       </c>
       <c r="Z16" s="1">
         <v>0</v>
@@ -9058,66 +9058,66 @@
     </row>
     <row r="17" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D17" s="1">
-        <v>3682</v>
+        <v>4665</v>
       </c>
       <c r="E17">
         <f>IF(ISBLANK(F17),-D17,F17-D17)</f>
-        <v>77</v>
+        <v>26</v>
       </c>
       <c r="F17" s="1">
-        <v>3759</v>
+        <v>4691</v>
       </c>
       <c r="G17">
         <f>IF(ISBLANK(H17),-F17,H17-F17)</f>
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H17" s="1">
-        <v>3803</v>
+        <v>4734</v>
       </c>
       <c r="I17">
         <f>IF(ISBLANK(J17),-H17,J17-H17)</f>
-        <v>116</v>
+        <v>57</v>
       </c>
       <c r="J17" s="1">
-        <v>3919</v>
+        <v>4791</v>
       </c>
       <c r="K17">
         <f>IF(ISBLANK(L17),-J17,L17-J17)</f>
-        <v>87</v>
+        <v>50</v>
       </c>
       <c r="L17" s="1">
-        <v>4006</v>
+        <v>4841</v>
       </c>
       <c r="M17">
         <f>IF(ISBLANK(N17),-L17,N17-L17)</f>
-        <v>41</v>
+        <v>115</v>
       </c>
       <c r="N17" s="1">
-        <v>4047</v>
+        <v>4956</v>
       </c>
       <c r="O17">
         <f>IF(ISBLANK(P17),-N17,P17-N17)</f>
-        <v>134</v>
+        <v>72</v>
       </c>
       <c r="P17" s="1">
-        <v>4181</v>
+        <v>5028</v>
       </c>
       <c r="Q17">
         <f>IF(ISBLANK(R17),-P17,R17-P17)</f>
-        <v>-4181</v>
+        <v>104</v>
       </c>
       <c r="R17" s="1">
-        <v>0</v>
+        <v>5132</v>
       </c>
       <c r="S17">
         <f>IF(ISBLANK(T17),-R17,T17-R17)</f>
-        <v>0</v>
+        <v>-5132</v>
       </c>
       <c r="T17" s="1">
         <v>0</v>
@@ -9160,154 +9160,154 @@
     </row>
     <row r="18" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>128</v>
+        <v>140</v>
       </c>
       <c r="D18" s="1">
-        <v>75946</v>
+        <v>3682</v>
       </c>
       <c r="E18">
         <f>IF(ISBLANK(F18),-D18,F18-D18)</f>
-        <v>100</v>
+        <v>77</v>
       </c>
       <c r="F18" s="1">
-        <v>76046</v>
+        <v>3759</v>
       </c>
       <c r="G18">
         <f>IF(ISBLANK(H18),-F18,H18-F18)</f>
-        <v>201</v>
+        <v>44</v>
       </c>
       <c r="H18" s="1">
-        <v>76247</v>
+        <v>3803</v>
       </c>
       <c r="I18">
         <f>IF(ISBLANK(J18),-H18,J18-H18)</f>
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="J18" s="1">
-        <v>76373</v>
+        <v>3919</v>
       </c>
       <c r="K18">
         <f>IF(ISBLANK(L18),-J18,L18-J18)</f>
-        <v>272</v>
+        <v>87</v>
       </c>
       <c r="L18" s="1">
-        <v>76645</v>
+        <v>4006</v>
       </c>
       <c r="M18">
         <f>IF(ISBLANK(N18),-L18,N18-L18)</f>
-        <v>74</v>
+        <v>41</v>
       </c>
       <c r="N18" s="1">
-        <v>76719</v>
+        <v>4047</v>
       </c>
       <c r="O18">
         <f>IF(ISBLANK(P18),-N18,P18-N18)</f>
-        <v>301</v>
+        <v>134</v>
       </c>
       <c r="P18" s="1">
-        <v>77020</v>
+        <v>4181</v>
       </c>
       <c r="Q18">
         <f>IF(ISBLANK(R18),-P18,R18-P18)</f>
-        <v>283</v>
+        <v>-4181</v>
       </c>
       <c r="R18" s="1">
-        <v>77303</v>
+        <v>0</v>
       </c>
       <c r="S18">
         <f>IF(ISBLANK(T18),-R18,T18-R18)</f>
-        <v>112</v>
+        <v>0</v>
       </c>
       <c r="T18" s="1">
-        <v>77415</v>
+        <v>0</v>
       </c>
       <c r="U18">
         <f>IF(ISBLANK(V18),-T18,V18-T18)</f>
-        <v>339</v>
+        <v>0</v>
       </c>
       <c r="V18" s="1">
-        <v>77754</v>
+        <v>0</v>
       </c>
       <c r="W18">
         <f>IF(ISBLANK(X18),-V18,X18-V18)</f>
-        <v>1066</v>
+        <v>0</v>
       </c>
       <c r="X18" s="1">
-        <v>78820</v>
+        <v>0</v>
       </c>
       <c r="Y18">
         <f>IF(ISBLANK(Z18),-X18,Z18-X18)</f>
-        <v>1295</v>
+        <v>0</v>
       </c>
       <c r="Z18" s="1">
-        <v>80115</v>
+        <v>0</v>
       </c>
       <c r="AA18">
         <f>IF(ISBLANK(AB18),-Z18,AB18-Z18)</f>
-        <v>593</v>
+        <v>0</v>
       </c>
       <c r="AB18" s="1">
-        <v>80708</v>
+        <v>0</v>
       </c>
       <c r="AC18">
         <f>IF(ISBLANK(AD18),-AB18,AD18-AB18)</f>
-        <v>1290</v>
+        <v>0</v>
       </c>
       <c r="AD18" s="1">
-        <v>81998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D19" s="1">
-        <v>2864</v>
+        <v>3286</v>
       </c>
       <c r="E19">
         <f>IF(ISBLANK(F19),-D19,F19-D19)</f>
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="F19" s="1">
-        <v>2898</v>
+        <v>3307</v>
       </c>
       <c r="G19">
         <f>IF(ISBLANK(H19),-F19,H19-F19)</f>
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="H19" s="1">
-        <v>2919</v>
+        <v>3320</v>
       </c>
       <c r="I19">
         <f>IF(ISBLANK(J19),-H19,J19-H19)</f>
-        <v>148</v>
+        <v>232</v>
       </c>
       <c r="J19" s="1">
-        <v>3067</v>
+        <v>3552</v>
       </c>
       <c r="K19">
         <f>IF(ISBLANK(L19),-J19,L19-J19)</f>
-        <v>-3067</v>
+        <v>102</v>
       </c>
       <c r="L19" s="1">
-        <v>0</v>
+        <v>3654</v>
       </c>
       <c r="M19">
         <f>IF(ISBLANK(N19),-L19,N19-L19)</f>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="N19" s="1">
-        <v>0</v>
+        <v>3714</v>
       </c>
       <c r="O19">
         <f>IF(ISBLANK(P19),-N19,P19-N19)</f>
-        <v>0</v>
+        <v>-3714</v>
       </c>
       <c r="P19" s="1">
         <v>0</v>
@@ -9364,45 +9364,45 @@
     </row>
     <row r="20" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D20" s="1">
-        <v>2416</v>
+        <v>3182</v>
       </c>
       <c r="E20">
         <f>IF(ISBLANK(F20),-D20,F20-D20)</f>
-        <v>48</v>
+        <v>15</v>
       </c>
       <c r="F20" s="1">
-        <v>2464</v>
+        <v>3197</v>
       </c>
       <c r="G20">
         <f>IF(ISBLANK(H20),-F20,H20-F20)</f>
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="H20" s="1">
-        <v>2542</v>
+        <v>3257</v>
       </c>
       <c r="I20">
         <f>IF(ISBLANK(J20),-H20,J20-H20)</f>
-        <v>-2542</v>
+        <v>43</v>
       </c>
       <c r="J20" s="1">
-        <v>0</v>
+        <v>3300</v>
       </c>
       <c r="K20">
         <f>IF(ISBLANK(L20),-J20,L20-J20)</f>
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="L20" s="1">
-        <v>0</v>
+        <v>3332</v>
       </c>
       <c r="M20">
         <f>IF(ISBLANK(N20),-L20,N20-L20)</f>
-        <v>0</v>
+        <v>-3332</v>
       </c>
       <c r="N20" s="1">
         <v>0</v>
@@ -9466,38 +9466,38 @@
     </row>
     <row r="21" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D21" s="1">
-        <v>1423</v>
+        <v>2864</v>
       </c>
       <c r="E21">
         <f>IF(ISBLANK(F21),-D21,F21-D21)</f>
-        <v>-1423</v>
+        <v>34</v>
       </c>
       <c r="F21" s="1">
-        <v>0</v>
+        <v>2898</v>
       </c>
       <c r="G21">
         <f>IF(ISBLANK(H21),-F21,H21-F21)</f>
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="H21" s="1">
-        <v>0</v>
+        <v>2919</v>
       </c>
       <c r="I21">
         <f>IF(ISBLANK(J21),-H21,J21-H21)</f>
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="J21" s="1">
-        <v>0</v>
+        <v>3067</v>
       </c>
       <c r="K21">
         <f>IF(ISBLANK(L21),-J21,L21-J21)</f>
-        <v>0</v>
+        <v>-3067</v>
       </c>
       <c r="L21" s="1">
         <v>0</v>
@@ -9568,256 +9568,256 @@
     </row>
     <row r="22" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>133</v>
+        <v>144</v>
       </c>
       <c r="D22" s="1">
-        <v>14802</v>
+        <v>2416</v>
       </c>
       <c r="E22">
         <f>IF(ISBLANK(F22),-D22,F22-D22)</f>
-        <v>156</v>
+        <v>48</v>
       </c>
       <c r="F22" s="1">
-        <v>14958</v>
+        <v>2464</v>
       </c>
       <c r="G22">
         <f>IF(ISBLANK(H22),-F22,H22-F22)</f>
-        <v>51</v>
+        <v>78</v>
       </c>
       <c r="H22" s="1">
-        <v>15009</v>
+        <v>2542</v>
       </c>
       <c r="I22">
         <f>IF(ISBLANK(J22),-H22,J22-H22)</f>
-        <v>198</v>
+        <v>-2542</v>
       </c>
       <c r="J22" s="1">
-        <v>15207</v>
+        <v>0</v>
       </c>
       <c r="K22">
         <f>IF(ISBLANK(L22),-J22,L22-J22)</f>
-        <v>146</v>
+        <v>0</v>
       </c>
       <c r="L22" s="1">
-        <v>15353</v>
+        <v>0</v>
       </c>
       <c r="M22">
         <f>IF(ISBLANK(N22),-L22,N22-L22)</f>
-        <v>41</v>
+        <v>0</v>
       </c>
       <c r="N22" s="1">
-        <v>15394</v>
+        <v>0</v>
       </c>
       <c r="O22">
         <f>IF(ISBLANK(P22),-N22,P22-N22)</f>
-        <v>392</v>
+        <v>0</v>
       </c>
       <c r="P22" s="1">
-        <v>15786</v>
+        <v>0</v>
       </c>
       <c r="Q22">
         <f>IF(ISBLANK(R22),-P22,R22-P22)</f>
-        <v>321</v>
+        <v>0</v>
       </c>
       <c r="R22" s="1">
-        <v>16107</v>
+        <v>0</v>
       </c>
       <c r="S22">
         <f>IF(ISBLANK(T22),-R22,T22-R22)</f>
-        <v>101</v>
+        <v>0</v>
       </c>
       <c r="T22" s="1">
-        <v>16208</v>
+        <v>0</v>
       </c>
       <c r="U22">
         <f>IF(ISBLANK(V22),-T22,V22-T22)</f>
-        <v>170</v>
+        <v>0</v>
       </c>
       <c r="V22" s="1">
-        <v>16378</v>
+        <v>0</v>
       </c>
       <c r="W22">
         <f>IF(ISBLANK(X22),-V22,X22-V22)</f>
-        <v>530</v>
+        <v>0</v>
       </c>
       <c r="X22" s="1">
-        <v>16908</v>
+        <v>0</v>
       </c>
       <c r="Y22">
         <f>IF(ISBLANK(Z22),-X22,Z22-X22)</f>
-        <v>490</v>
+        <v>0</v>
       </c>
       <c r="Z22" s="1">
-        <v>17398</v>
+        <v>0</v>
       </c>
       <c r="AA22">
         <f>IF(ISBLANK(AB22),-Z22,AB22-Z22)</f>
-        <v>329</v>
+        <v>0</v>
       </c>
       <c r="AB22" s="1">
-        <v>17727</v>
+        <v>0</v>
       </c>
       <c r="AC22">
         <f>IF(ISBLANK(AD22),-AB22,AD22-AB22)</f>
-        <v>749</v>
+        <v>0</v>
       </c>
       <c r="AD22" s="1">
-        <v>18476</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>126</v>
+        <v>145</v>
       </c>
       <c r="D23" s="1">
-        <v>81741</v>
+        <v>2395</v>
       </c>
       <c r="E23">
         <f>IF(ISBLANK(F23),-D23,F23-D23)</f>
-        <v>253</v>
+        <v>14</v>
       </c>
       <c r="F23" s="1">
-        <v>81994</v>
+        <v>2409</v>
       </c>
       <c r="G23">
         <f>IF(ISBLANK(H23),-F23,H23-F23)</f>
-        <v>130</v>
+        <v>-2409</v>
       </c>
       <c r="H23" s="1">
-        <v>82124</v>
+        <v>0</v>
       </c>
       <c r="I23">
         <f>IF(ISBLANK(J23),-H23,J23-H23)</f>
-        <v>211</v>
+        <v>0</v>
       </c>
       <c r="J23" s="1">
-        <v>82335</v>
+        <v>0</v>
       </c>
       <c r="K23">
         <f>IF(ISBLANK(L23),-J23,L23-J23)</f>
-        <v>323</v>
+        <v>0</v>
       </c>
       <c r="L23" s="1">
-        <v>82658</v>
+        <v>0</v>
       </c>
       <c r="M23">
         <f>IF(ISBLANK(N23),-L23,N23-L23)</f>
-        <v>206</v>
+        <v>0</v>
       </c>
       <c r="N23" s="1">
-        <v>82864</v>
+        <v>0</v>
       </c>
       <c r="O23">
         <f>IF(ISBLANK(P23),-N23,P23-N23)</f>
-        <v>556</v>
+        <v>0</v>
       </c>
       <c r="P23" s="1">
-        <v>83420</v>
+        <v>0</v>
       </c>
       <c r="Q23">
         <f>IF(ISBLANK(R23),-P23,R23-P23)</f>
-        <v>351</v>
+        <v>0</v>
       </c>
       <c r="R23" s="1">
-        <v>83771</v>
+        <v>0</v>
       </c>
       <c r="S23">
         <f>IF(ISBLANK(T23),-R23,T23-R23)</f>
-        <v>217</v>
+        <v>0</v>
       </c>
       <c r="T23" s="1">
-        <v>83988</v>
+        <v>0</v>
       </c>
       <c r="U23">
         <f>IF(ISBLANK(V23),-T23,V23-T23)</f>
-        <v>247</v>
+        <v>0</v>
       </c>
       <c r="V23" s="1">
-        <v>84235</v>
+        <v>0</v>
       </c>
       <c r="W23">
         <f>IF(ISBLANK(X23),-V23,X23-V23)</f>
-        <v>1001</v>
+        <v>0</v>
       </c>
       <c r="X23" s="1">
-        <v>85236</v>
+        <v>0</v>
       </c>
       <c r="Y23">
         <f>IF(ISBLANK(Z23),-X23,Z23-X23)</f>
-        <v>2333</v>
+        <v>0</v>
       </c>
       <c r="Z23" s="1">
-        <v>87569</v>
+        <v>0</v>
       </c>
       <c r="AA23">
         <f>IF(ISBLANK(AB23),-Z23,AB23-Z23)</f>
-        <v>1190</v>
+        <v>0</v>
       </c>
       <c r="AB23" s="1">
-        <v>88759</v>
+        <v>0</v>
       </c>
       <c r="AC23">
         <f>IF(ISBLANK(AD23),-AB23,AD23-AB23)</f>
-        <v>1476</v>
+        <v>0</v>
       </c>
       <c r="AD23" s="1">
-        <v>90235</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="D24" s="1">
-        <v>3286</v>
+        <v>1423</v>
       </c>
       <c r="E24">
         <f>IF(ISBLANK(F24),-D24,F24-D24)</f>
-        <v>21</v>
+        <v>-1423</v>
       </c>
       <c r="F24" s="1">
-        <v>3307</v>
+        <v>0</v>
       </c>
       <c r="G24">
         <f>IF(ISBLANK(H24),-F24,H24-F24)</f>
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="H24" s="1">
-        <v>3320</v>
+        <v>0</v>
       </c>
       <c r="I24">
         <f>IF(ISBLANK(J24),-H24,J24-H24)</f>
-        <v>232</v>
+        <v>0</v>
       </c>
       <c r="J24" s="1">
-        <v>3552</v>
+        <v>0</v>
       </c>
       <c r="K24">
         <f>IF(ISBLANK(L24),-J24,L24-J24)</f>
-        <v>102</v>
+        <v>0</v>
       </c>
       <c r="L24" s="1">
-        <v>3654</v>
+        <v>0</v>
       </c>
       <c r="M24">
         <f>IF(ISBLANK(N24),-L24,N24-L24)</f>
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="N24" s="1">
-        <v>3714</v>
+        <v>0</v>
       </c>
       <c r="O24">
         <f>IF(ISBLANK(P24),-N24,P24-N24)</f>
-        <v>-3714</v>
+        <v>0</v>
       </c>
       <c r="P24" s="1">
         <v>0</v>
@@ -11486,7 +11486,7 @@
     </row>
   </sheetData>
   <sortState ref="A2:AD24">
-    <sortCondition ref="B2:B24"/>
+    <sortCondition ref="A2:A24"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Stage 11 midlands added Signed-off-by: Gerry Mulvenna <git@movingwifi.com>
</commit_message>
<xml_diff>
--- a/europarl/europarl-ireland-2019.xlsx
+++ b/europarl/europarl-ireland-2019.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="14220" windowHeight="8580" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="14220" windowHeight="8580" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Candidates" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="261">
   <si>
     <t>Candidate</t>
   </si>
@@ -5161,13 +5161,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF37"/>
   <sheetViews>
-    <sheetView topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2:V18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="S2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="W2" sqref="W2:X18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>256</v>
       </c>
@@ -5204,8 +5207,11 @@
       <c r="V1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="X1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>11</v>
       </c>
@@ -5273,14 +5279,21 @@
         <v>0</v>
       </c>
       <c r="U2">
-        <f t="shared" ref="U2:U18" si="8">IF(ISBLANK(V2),-T2,V2-T2)</f>
+        <f t="shared" ref="U2:W18" si="8">IF(ISBLANK(V2),-T2,V2-T2)</f>
         <v>0</v>
       </c>
       <c r="V2" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W2">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
@@ -5354,8 +5367,15 @@
       <c r="V3" s="1">
         <v>83851</v>
       </c>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W3">
+        <f t="shared" si="8"/>
+        <v>974</v>
+      </c>
+      <c r="X3" s="1">
+        <v>84825</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>5</v>
       </c>
@@ -5429,8 +5449,15 @@
       <c r="V4" s="1">
         <v>64690</v>
       </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W4">
+        <f t="shared" si="8"/>
+        <v>1875</v>
+      </c>
+      <c r="X4" s="1">
+        <v>66565</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>9</v>
       </c>
@@ -5504,8 +5531,15 @@
       <c r="V5" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W5">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="X5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -5579,8 +5613,15 @@
       <c r="V6" s="1">
         <v>94353</v>
       </c>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W6">
+        <f t="shared" si="8"/>
+        <v>2966</v>
+      </c>
+      <c r="X6" s="1">
+        <v>97319</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>15</v>
       </c>
@@ -5654,8 +5695,15 @@
       <c r="V7" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W7">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="X7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>10</v>
       </c>
@@ -5729,8 +5777,15 @@
       <c r="V8" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W8">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="X8" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>14</v>
       </c>
@@ -5804,8 +5859,15 @@
       <c r="V9" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W9">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="X9" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
@@ -5879,8 +5941,15 @@
       <c r="V10">
         <v>118986</v>
       </c>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W10">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="X10">
+        <v>118986</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>6</v>
       </c>
@@ -5954,8 +6023,15 @@
       <c r="V11" s="1">
         <v>60778</v>
       </c>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W11">
+        <f t="shared" si="8"/>
+        <v>1179</v>
+      </c>
+      <c r="X11" s="1">
+        <v>61957</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>16</v>
       </c>
@@ -6029,8 +6105,15 @@
       <c r="V12" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W12">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="X12" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>17</v>
       </c>
@@ -6104,8 +6187,15 @@
       <c r="V13" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W13">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="X13" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -6179,8 +6269,15 @@
       <c r="V14" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W14">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="X14" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>12</v>
       </c>
@@ -6254,8 +6351,15 @@
       <c r="V15" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W15">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="X15" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>8</v>
       </c>
@@ -6329,6 +6433,13 @@
       <c r="V16" s="1">
         <v>34610</v>
       </c>
+      <c r="W16">
+        <f t="shared" si="8"/>
+        <v>-34610</v>
+      </c>
+      <c r="X16" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A17">
@@ -6404,6 +6515,13 @@
       <c r="V17" s="1">
         <v>46820</v>
       </c>
+      <c r="W17">
+        <f t="shared" si="8"/>
+        <v>17712</v>
+      </c>
+      <c r="X17" s="1">
+        <v>64532</v>
+      </c>
     </row>
     <row r="18" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A18">
@@ -6478,6 +6596,13 @@
       </c>
       <c r="V18" s="1">
         <v>76056</v>
+      </c>
+      <c r="W18">
+        <f t="shared" si="8"/>
+        <v>4282</v>
+      </c>
+      <c r="X18" s="1">
+        <v>80338</v>
       </c>
     </row>
     <row r="20" spans="1:32" x14ac:dyDescent="0.25">
@@ -7466,7 +7591,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
@@ -7537,91 +7662,91 @@
         <v>118444</v>
       </c>
       <c r="E2">
-        <f>IF(ISBLANK(F2),-D2,F2-D2)</f>
+        <f t="shared" ref="E2:E24" si="0">IF(ISBLANK(F2),-D2,F2-D2)</f>
         <v>45</v>
       </c>
       <c r="F2" s="1">
         <v>118489</v>
       </c>
       <c r="G2">
-        <f>IF(ISBLANK(H2),-F2,H2-F2)</f>
+        <f t="shared" ref="G2:G24" si="1">IF(ISBLANK(H2),-F2,H2-F2)</f>
         <v>186</v>
       </c>
       <c r="H2" s="1">
         <v>118675</v>
       </c>
       <c r="I2">
-        <f>IF(ISBLANK(J2),-H2,J2-H2)</f>
+        <f t="shared" ref="I2:I24" si="2">IF(ISBLANK(J2),-H2,J2-H2)</f>
         <v>98</v>
       </c>
       <c r="J2" s="1">
         <v>118773</v>
       </c>
       <c r="K2">
-        <f>IF(ISBLANK(L2),-J2,L2-J2)</f>
+        <f t="shared" ref="K2:K24" si="3">IF(ISBLANK(L2),-J2,L2-J2)</f>
         <v>350</v>
       </c>
       <c r="L2" s="1">
         <v>119123</v>
       </c>
       <c r="M2">
-        <f>IF(ISBLANK(N2),-L2,N2-L2)</f>
+        <f t="shared" ref="M2:M24" si="4">IF(ISBLANK(N2),-L2,N2-L2)</f>
         <v>257</v>
       </c>
       <c r="N2" s="1">
         <v>119380</v>
       </c>
       <c r="O2">
-        <f>IF(ISBLANK(P2),-N2,P2-N2)</f>
+        <f t="shared" ref="O2:O24" si="5">IF(ISBLANK(P2),-N2,P2-N2)</f>
         <v>165</v>
       </c>
       <c r="P2" s="1">
         <v>119545</v>
       </c>
       <c r="Q2">
-        <f>IF(ISBLANK(R2),-P2,R2-P2)</f>
+        <f t="shared" ref="Q2:Q24" si="6">IF(ISBLANK(R2),-P2,R2-P2)</f>
         <v>170</v>
       </c>
       <c r="R2" s="1">
         <v>119715</v>
       </c>
       <c r="S2">
-        <f>IF(ISBLANK(T2),-R2,T2-R2)</f>
+        <f t="shared" ref="S2:S24" si="7">IF(ISBLANK(T2),-R2,T2-R2)</f>
         <v>168</v>
       </c>
       <c r="T2" s="1">
         <v>119883</v>
       </c>
       <c r="U2">
-        <f>IF(ISBLANK(V2),-T2,V2-T2)</f>
+        <f t="shared" ref="U2:U24" si="8">IF(ISBLANK(V2),-T2,V2-T2)</f>
         <v>0</v>
       </c>
       <c r="V2" s="1">
         <v>119883</v>
       </c>
       <c r="W2">
-        <f>IF(ISBLANK(X2),-V2,X2-V2)</f>
+        <f t="shared" ref="W2:W24" si="9">IF(ISBLANK(X2),-V2,X2-V2)</f>
         <v>0</v>
       </c>
       <c r="X2" s="1">
         <v>119883</v>
       </c>
       <c r="Y2">
-        <f>IF(ISBLANK(Z2),-X2,Z2-X2)</f>
+        <f t="shared" ref="Y2:Y24" si="10">IF(ISBLANK(Z2),-X2,Z2-X2)</f>
         <v>0</v>
       </c>
       <c r="Z2" s="1">
         <v>119883</v>
       </c>
       <c r="AA2">
-        <f>IF(ISBLANK(AB2),-Z2,AB2-Z2)</f>
+        <f t="shared" ref="AA2:AA24" si="11">IF(ISBLANK(AB2),-Z2,AB2-Z2)</f>
         <v>0</v>
       </c>
       <c r="AB2" s="1">
         <v>119883</v>
       </c>
       <c r="AC2">
-        <f>IF(ISBLANK(AD2),-AB2,AD2-AB2)</f>
+        <f t="shared" ref="AC2:AC24" si="12">IF(ISBLANK(AD2),-AB2,AD2-AB2)</f>
         <v>0</v>
       </c>
       <c r="AD2" s="1">
@@ -7639,91 +7764,91 @@
         <v>84083</v>
       </c>
       <c r="E3">
-        <f>IF(ISBLANK(F3),-D3,F3-D3)</f>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="F3" s="1">
         <v>84106</v>
       </c>
       <c r="G3">
-        <f>IF(ISBLANK(H3),-F3,H3-F3)</f>
+        <f t="shared" si="1"/>
         <v>58</v>
       </c>
       <c r="H3" s="1">
         <v>84164</v>
       </c>
       <c r="I3">
-        <f>IF(ISBLANK(J3),-H3,J3-H3)</f>
+        <f t="shared" si="2"/>
         <v>74</v>
       </c>
       <c r="J3" s="1">
         <v>84238</v>
       </c>
       <c r="K3">
-        <f>IF(ISBLANK(L3),-J3,L3-J3)</f>
+        <f t="shared" si="3"/>
         <v>150</v>
       </c>
       <c r="L3" s="1">
         <v>84388</v>
       </c>
       <c r="M3">
-        <f>IF(ISBLANK(N3),-L3,N3-L3)</f>
+        <f t="shared" si="4"/>
         <v>171</v>
       </c>
       <c r="N3" s="1">
         <v>84559</v>
       </c>
       <c r="O3">
-        <f>IF(ISBLANK(P3),-N3,P3-N3)</f>
+        <f t="shared" si="5"/>
         <v>95</v>
       </c>
       <c r="P3" s="1">
         <v>84654</v>
       </c>
       <c r="Q3">
-        <f>IF(ISBLANK(R3),-P3,R3-P3)</f>
+        <f t="shared" si="6"/>
         <v>187</v>
       </c>
       <c r="R3" s="1">
         <v>84841</v>
       </c>
       <c r="S3">
-        <f>IF(ISBLANK(T3),-R3,T3-R3)</f>
+        <f t="shared" si="7"/>
         <v>130</v>
       </c>
       <c r="T3" s="1">
         <v>84971</v>
       </c>
       <c r="U3">
-        <f>IF(ISBLANK(V3),-T3,V3-T3)</f>
+        <f t="shared" si="8"/>
         <v>480</v>
       </c>
       <c r="V3" s="1">
         <v>85451</v>
       </c>
       <c r="W3">
-        <f>IF(ISBLANK(X3),-V3,X3-V3)</f>
+        <f t="shared" si="9"/>
         <v>575</v>
       </c>
       <c r="X3" s="1">
         <v>86026</v>
       </c>
       <c r="Y3">
-        <f>IF(ISBLANK(Z3),-X3,Z3-X3)</f>
+        <f t="shared" si="10"/>
         <v>1010</v>
       </c>
       <c r="Z3" s="1">
         <v>87036</v>
       </c>
       <c r="AA3">
-        <f>IF(ISBLANK(AB3),-Z3,AB3-Z3)</f>
+        <f t="shared" si="11"/>
         <v>928</v>
       </c>
       <c r="AB3" s="1">
         <v>87964</v>
       </c>
       <c r="AC3">
-        <f>IF(ISBLANK(AD3),-AB3,AD3-AB3)</f>
+        <f t="shared" si="12"/>
         <v>637</v>
       </c>
       <c r="AD3" s="1">
@@ -7741,91 +7866,91 @@
         <v>81741</v>
       </c>
       <c r="E4">
-        <f>IF(ISBLANK(F4),-D4,F4-D4)</f>
+        <f t="shared" si="0"/>
         <v>253</v>
       </c>
       <c r="F4" s="1">
         <v>81994</v>
       </c>
       <c r="G4">
-        <f>IF(ISBLANK(H4),-F4,H4-F4)</f>
+        <f t="shared" si="1"/>
         <v>130</v>
       </c>
       <c r="H4" s="1">
         <v>82124</v>
       </c>
       <c r="I4">
-        <f>IF(ISBLANK(J4),-H4,J4-H4)</f>
+        <f t="shared" si="2"/>
         <v>211</v>
       </c>
       <c r="J4" s="1">
         <v>82335</v>
       </c>
       <c r="K4">
-        <f>IF(ISBLANK(L4),-J4,L4-J4)</f>
+        <f t="shared" si="3"/>
         <v>323</v>
       </c>
       <c r="L4" s="1">
         <v>82658</v>
       </c>
       <c r="M4">
-        <f>IF(ISBLANK(N4),-L4,N4-L4)</f>
+        <f t="shared" si="4"/>
         <v>206</v>
       </c>
       <c r="N4" s="1">
         <v>82864</v>
       </c>
       <c r="O4">
-        <f>IF(ISBLANK(P4),-N4,P4-N4)</f>
+        <f t="shared" si="5"/>
         <v>556</v>
       </c>
       <c r="P4" s="1">
         <v>83420</v>
       </c>
       <c r="Q4">
-        <f>IF(ISBLANK(R4),-P4,R4-P4)</f>
+        <f t="shared" si="6"/>
         <v>351</v>
       </c>
       <c r="R4" s="1">
         <v>83771</v>
       </c>
       <c r="S4">
-        <f>IF(ISBLANK(T4),-R4,T4-R4)</f>
+        <f t="shared" si="7"/>
         <v>217</v>
       </c>
       <c r="T4" s="1">
         <v>83988</v>
       </c>
       <c r="U4">
-        <f>IF(ISBLANK(V4),-T4,V4-T4)</f>
+        <f t="shared" si="8"/>
         <v>247</v>
       </c>
       <c r="V4" s="1">
         <v>84235</v>
       </c>
       <c r="W4">
-        <f>IF(ISBLANK(X4),-V4,X4-V4)</f>
+        <f t="shared" si="9"/>
         <v>1001</v>
       </c>
       <c r="X4" s="1">
         <v>85236</v>
       </c>
       <c r="Y4">
-        <f>IF(ISBLANK(Z4),-X4,Z4-X4)</f>
+        <f t="shared" si="10"/>
         <v>2333</v>
       </c>
       <c r="Z4" s="1">
         <v>87569</v>
       </c>
       <c r="AA4">
-        <f>IF(ISBLANK(AB4),-Z4,AB4-Z4)</f>
+        <f t="shared" si="11"/>
         <v>1190</v>
       </c>
       <c r="AB4" s="1">
         <v>88759</v>
       </c>
       <c r="AC4">
-        <f>IF(ISBLANK(AD4),-AB4,AD4-AB4)</f>
+        <f t="shared" si="12"/>
         <v>1476</v>
       </c>
       <c r="AD4" s="1">
@@ -7843,91 +7968,91 @@
         <v>79072</v>
       </c>
       <c r="E5">
-        <f>IF(ISBLANK(F5),-D5,F5-D5)</f>
+        <f t="shared" si="0"/>
         <v>68</v>
       </c>
       <c r="F5" s="1">
         <v>79140</v>
       </c>
       <c r="G5">
-        <f>IF(ISBLANK(H5),-F5,H5-F5)</f>
+        <f t="shared" si="1"/>
         <v>142</v>
       </c>
       <c r="H5" s="1">
         <v>79282</v>
       </c>
       <c r="I5">
-        <f>IF(ISBLANK(J5),-H5,J5-H5)</f>
+        <f t="shared" si="2"/>
         <v>105</v>
       </c>
       <c r="J5" s="1">
         <v>79387</v>
       </c>
       <c r="K5">
-        <f>IF(ISBLANK(L5),-J5,L5-J5)</f>
+        <f t="shared" si="3"/>
         <v>186</v>
       </c>
       <c r="L5" s="1">
         <v>79573</v>
       </c>
       <c r="M5">
-        <f>IF(ISBLANK(N5),-L5,N5-L5)</f>
+        <f t="shared" si="4"/>
         <v>168</v>
       </c>
       <c r="N5" s="1">
         <v>79741</v>
       </c>
       <c r="O5">
-        <f>IF(ISBLANK(P5),-N5,P5-N5)</f>
+        <f t="shared" si="5"/>
         <v>204</v>
       </c>
       <c r="P5" s="1">
         <v>79945</v>
       </c>
       <c r="Q5">
-        <f>IF(ISBLANK(R5),-P5,R5-P5)</f>
+        <f t="shared" si="6"/>
         <v>305</v>
       </c>
       <c r="R5" s="1">
         <v>80250</v>
       </c>
       <c r="S5">
-        <f>IF(ISBLANK(T5),-R5,T5-R5)</f>
+        <f t="shared" si="7"/>
         <v>127</v>
       </c>
       <c r="T5" s="1">
         <v>80377</v>
       </c>
       <c r="U5">
-        <f>IF(ISBLANK(V5),-T5,V5-T5)</f>
+        <f t="shared" si="8"/>
         <v>446</v>
       </c>
       <c r="V5" s="1">
         <v>80823</v>
       </c>
       <c r="W5">
-        <f>IF(ISBLANK(X5),-V5,X5-V5)</f>
+        <f t="shared" si="9"/>
         <v>991</v>
       </c>
       <c r="X5" s="1">
         <v>81814</v>
       </c>
       <c r="Y5">
-        <f>IF(ISBLANK(Z5),-X5,Z5-X5)</f>
+        <f t="shared" si="10"/>
         <v>1119</v>
       </c>
       <c r="Z5" s="1">
         <v>82933</v>
       </c>
       <c r="AA5">
-        <f>IF(ISBLANK(AB5),-Z5,AB5-Z5)</f>
+        <f t="shared" si="11"/>
         <v>958</v>
       </c>
       <c r="AB5" s="1">
         <v>83891</v>
       </c>
       <c r="AC5">
-        <f>IF(ISBLANK(AD5),-AB5,AD5-AB5)</f>
+        <f t="shared" si="12"/>
         <v>1108</v>
       </c>
       <c r="AD5" s="1">
@@ -7945,91 +8070,91 @@
         <v>75946</v>
       </c>
       <c r="E6">
-        <f>IF(ISBLANK(F6),-D6,F6-D6)</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="F6" s="1">
         <v>76046</v>
       </c>
       <c r="G6">
-        <f>IF(ISBLANK(H6),-F6,H6-F6)</f>
+        <f t="shared" si="1"/>
         <v>201</v>
       </c>
       <c r="H6" s="1">
         <v>76247</v>
       </c>
       <c r="I6">
-        <f>IF(ISBLANK(J6),-H6,J6-H6)</f>
+        <f t="shared" si="2"/>
         <v>126</v>
       </c>
       <c r="J6" s="1">
         <v>76373</v>
       </c>
       <c r="K6">
-        <f>IF(ISBLANK(L6),-J6,L6-J6)</f>
+        <f t="shared" si="3"/>
         <v>272</v>
       </c>
       <c r="L6" s="1">
         <v>76645</v>
       </c>
       <c r="M6">
-        <f>IF(ISBLANK(N6),-L6,N6-L6)</f>
+        <f t="shared" si="4"/>
         <v>74</v>
       </c>
       <c r="N6" s="1">
         <v>76719</v>
       </c>
       <c r="O6">
-        <f>IF(ISBLANK(P6),-N6,P6-N6)</f>
+        <f t="shared" si="5"/>
         <v>301</v>
       </c>
       <c r="P6" s="1">
         <v>77020</v>
       </c>
       <c r="Q6">
-        <f>IF(ISBLANK(R6),-P6,R6-P6)</f>
+        <f t="shared" si="6"/>
         <v>283</v>
       </c>
       <c r="R6" s="1">
         <v>77303</v>
       </c>
       <c r="S6">
-        <f>IF(ISBLANK(T6),-R6,T6-R6)</f>
+        <f t="shared" si="7"/>
         <v>112</v>
       </c>
       <c r="T6" s="1">
         <v>77415</v>
       </c>
       <c r="U6">
-        <f>IF(ISBLANK(V6),-T6,V6-T6)</f>
+        <f t="shared" si="8"/>
         <v>339</v>
       </c>
       <c r="V6" s="1">
         <v>77754</v>
       </c>
       <c r="W6">
-        <f>IF(ISBLANK(X6),-V6,X6-V6)</f>
+        <f t="shared" si="9"/>
         <v>1066</v>
       </c>
       <c r="X6" s="1">
         <v>78820</v>
       </c>
       <c r="Y6">
-        <f>IF(ISBLANK(Z6),-X6,Z6-X6)</f>
+        <f t="shared" si="10"/>
         <v>1295</v>
       </c>
       <c r="Z6" s="1">
         <v>80115</v>
       </c>
       <c r="AA6">
-        <f>IF(ISBLANK(AB6),-Z6,AB6-Z6)</f>
+        <f t="shared" si="11"/>
         <v>593</v>
       </c>
       <c r="AB6" s="1">
         <v>80708</v>
       </c>
       <c r="AC6">
-        <f>IF(ISBLANK(AD6),-AB6,AD6-AB6)</f>
+        <f t="shared" si="12"/>
         <v>1290</v>
       </c>
       <c r="AD6" s="1">
@@ -8047,91 +8172,91 @@
         <v>69166</v>
       </c>
       <c r="E7">
-        <f>IF(ISBLANK(F7),-D7,F7-D7)</f>
+        <f t="shared" si="0"/>
         <v>35</v>
       </c>
       <c r="F7" s="1">
         <v>69201</v>
       </c>
       <c r="G7">
-        <f>IF(ISBLANK(H7),-F7,H7-F7)</f>
+        <f t="shared" si="1"/>
         <v>71</v>
       </c>
       <c r="H7" s="1">
         <v>69272</v>
       </c>
       <c r="I7">
-        <f>IF(ISBLANK(J7),-H7,J7-H7)</f>
+        <f t="shared" si="2"/>
         <v>44</v>
       </c>
       <c r="J7" s="1">
         <v>69316</v>
       </c>
       <c r="K7">
-        <f>IF(ISBLANK(L7),-J7,L7-J7)</f>
+        <f t="shared" si="3"/>
         <v>66</v>
       </c>
       <c r="L7" s="1">
         <v>69382</v>
       </c>
       <c r="M7">
-        <f>IF(ISBLANK(N7),-L7,N7-L7)</f>
+        <f t="shared" si="4"/>
         <v>129</v>
       </c>
       <c r="N7" s="1">
         <v>69511</v>
       </c>
       <c r="O7">
-        <f>IF(ISBLANK(P7),-N7,P7-N7)</f>
+        <f t="shared" si="5"/>
         <v>45</v>
       </c>
       <c r="P7" s="1">
         <v>69556</v>
       </c>
       <c r="Q7">
-        <f>IF(ISBLANK(R7),-P7,R7-P7)</f>
+        <f t="shared" si="6"/>
         <v>116</v>
       </c>
       <c r="R7" s="1">
         <v>69672</v>
       </c>
       <c r="S7">
-        <f>IF(ISBLANK(T7),-R7,T7-R7)</f>
+        <f t="shared" si="7"/>
         <v>1226</v>
       </c>
       <c r="T7" s="1">
         <v>70898</v>
       </c>
       <c r="U7">
-        <f>IF(ISBLANK(V7),-T7,V7-T7)</f>
+        <f t="shared" si="8"/>
         <v>270</v>
       </c>
       <c r="V7" s="1">
         <v>71168</v>
       </c>
       <c r="W7">
-        <f>IF(ISBLANK(X7),-V7,X7-V7)</f>
+        <f t="shared" si="9"/>
         <v>674</v>
       </c>
       <c r="X7" s="1">
         <v>71842</v>
       </c>
       <c r="Y7">
-        <f>IF(ISBLANK(Z7),-X7,Z7-X7)</f>
+        <f t="shared" si="10"/>
         <v>291</v>
       </c>
       <c r="Z7" s="1">
         <v>72133</v>
       </c>
       <c r="AA7">
-        <f>IF(ISBLANK(AB7),-Z7,AB7-Z7)</f>
+        <f t="shared" si="11"/>
         <v>720</v>
       </c>
       <c r="AB7" s="1">
         <v>72853</v>
       </c>
       <c r="AC7">
-        <f>IF(ISBLANK(AD7),-AB7,AD7-AB7)</f>
+        <f t="shared" si="12"/>
         <v>929</v>
       </c>
       <c r="AD7" s="1">
@@ -8149,91 +8274,91 @@
         <v>64605</v>
       </c>
       <c r="E8">
-        <f>IF(ISBLANK(F8),-D8,F8-D8)</f>
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="F8" s="1">
         <v>64631</v>
       </c>
       <c r="G8">
-        <f>IF(ISBLANK(H8),-F8,H8-F8)</f>
+        <f t="shared" si="1"/>
         <v>61</v>
       </c>
       <c r="H8" s="1">
         <v>64692</v>
       </c>
       <c r="I8">
-        <f>IF(ISBLANK(J8),-H8,J8-H8)</f>
+        <f t="shared" si="2"/>
         <v>71</v>
       </c>
       <c r="J8" s="1">
         <v>64763</v>
       </c>
       <c r="K8">
-        <f>IF(ISBLANK(L8),-J8,L8-J8)</f>
+        <f t="shared" si="3"/>
         <v>136</v>
       </c>
       <c r="L8" s="1">
         <v>64899</v>
       </c>
       <c r="M8">
-        <f>IF(ISBLANK(N8),-L8,N8-L8)</f>
+        <f t="shared" si="4"/>
         <v>106</v>
       </c>
       <c r="N8" s="1">
         <v>65005</v>
       </c>
       <c r="O8">
-        <f>IF(ISBLANK(P8),-N8,P8-N8)</f>
+        <f t="shared" si="5"/>
         <v>110</v>
       </c>
       <c r="P8" s="1">
         <v>65115</v>
       </c>
       <c r="Q8">
-        <f>IF(ISBLANK(R8),-P8,R8-P8)</f>
+        <f t="shared" si="6"/>
         <v>137</v>
       </c>
       <c r="R8" s="1">
         <v>65252</v>
       </c>
       <c r="S8">
-        <f>IF(ISBLANK(T8),-R8,T8-R8)</f>
+        <f t="shared" si="7"/>
         <v>306</v>
       </c>
       <c r="T8" s="1">
         <v>65558</v>
       </c>
       <c r="U8">
-        <f>IF(ISBLANK(V8),-T8,V8-T8)</f>
+        <f t="shared" si="8"/>
         <v>491</v>
       </c>
       <c r="V8" s="1">
         <v>66049</v>
       </c>
       <c r="W8">
-        <f>IF(ISBLANK(X8),-V8,X8-V8)</f>
+        <f t="shared" si="9"/>
         <v>683</v>
       </c>
       <c r="X8" s="1">
         <v>66732</v>
       </c>
       <c r="Y8">
-        <f>IF(ISBLANK(Z8),-X8,Z8-X8)</f>
+        <f t="shared" si="10"/>
         <v>542</v>
       </c>
       <c r="Z8" s="1">
         <v>67274</v>
       </c>
       <c r="AA8">
-        <f>IF(ISBLANK(AB8),-Z8,AB8-Z8)</f>
+        <f t="shared" si="11"/>
         <v>622</v>
       </c>
       <c r="AB8" s="1">
         <v>67896</v>
       </c>
       <c r="AC8">
-        <f>IF(ISBLANK(AD8),-AB8,AD8-AB8)</f>
+        <f t="shared" si="12"/>
         <v>1194</v>
       </c>
       <c r="AD8" s="1">
@@ -8251,91 +8376,91 @@
         <v>38738</v>
       </c>
       <c r="E9">
-        <f>IF(ISBLANK(F9),-D9,F9-D9)</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="F9" s="1">
         <v>38755</v>
       </c>
       <c r="G9">
-        <f>IF(ISBLANK(H9),-F9,H9-F9)</f>
+        <f t="shared" si="1"/>
         <v>33</v>
       </c>
       <c r="H9" s="1">
         <v>38788</v>
       </c>
       <c r="I9">
-        <f>IF(ISBLANK(J9),-H9,J9-H9)</f>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="J9" s="1">
         <v>38804</v>
       </c>
       <c r="K9">
-        <f>IF(ISBLANK(L9),-J9,L9-J9)</f>
+        <f t="shared" si="3"/>
         <v>38</v>
       </c>
       <c r="L9" s="1">
         <v>38842</v>
       </c>
       <c r="M9">
-        <f>IF(ISBLANK(N9),-L9,N9-L9)</f>
+        <f t="shared" si="4"/>
         <v>84</v>
       </c>
       <c r="N9" s="1">
         <v>38926</v>
       </c>
       <c r="O9">
-        <f>IF(ISBLANK(P9),-N9,P9-N9)</f>
+        <f t="shared" si="5"/>
         <v>24</v>
       </c>
       <c r="P9" s="1">
         <v>38950</v>
       </c>
       <c r="Q9">
-        <f>IF(ISBLANK(R9),-P9,R9-P9)</f>
+        <f t="shared" si="6"/>
         <v>46</v>
       </c>
       <c r="R9" s="1">
         <v>38996</v>
       </c>
       <c r="S9">
-        <f>IF(ISBLANK(T9),-R9,T9-R9)</f>
+        <f t="shared" si="7"/>
         <v>298</v>
       </c>
       <c r="T9" s="1">
         <v>39294</v>
       </c>
       <c r="U9">
-        <f>IF(ISBLANK(V9),-T9,V9-T9)</f>
+        <f t="shared" si="8"/>
         <v>135</v>
       </c>
       <c r="V9" s="1">
         <v>39429</v>
       </c>
       <c r="W9">
-        <f>IF(ISBLANK(X9),-V9,X9-V9)</f>
+        <f t="shared" si="9"/>
         <v>426</v>
       </c>
       <c r="X9" s="1">
         <v>39855</v>
       </c>
       <c r="Y9">
-        <f>IF(ISBLANK(Z9),-X9,Z9-X9)</f>
+        <f t="shared" si="10"/>
         <v>159</v>
       </c>
       <c r="Z9" s="1">
         <v>40014</v>
       </c>
       <c r="AA9">
-        <f>IF(ISBLANK(AB9),-Z9,AB9-Z9)</f>
+        <f t="shared" si="11"/>
         <v>572</v>
       </c>
       <c r="AB9" s="1">
         <v>40586</v>
       </c>
       <c r="AC9">
-        <f>IF(ISBLANK(AD9),-AB9,AD9-AB9)</f>
+        <f t="shared" si="12"/>
         <v>483</v>
       </c>
       <c r="AD9" s="1">
@@ -8353,91 +8478,91 @@
         <v>22075</v>
       </c>
       <c r="E10">
-        <f>IF(ISBLANK(F10),-D10,F10-D10)</f>
+        <f t="shared" si="0"/>
         <v>38</v>
       </c>
       <c r="F10" s="1">
         <v>22113</v>
       </c>
       <c r="G10">
-        <f>IF(ISBLANK(H10),-F10,H10-F10)</f>
+        <f t="shared" si="1"/>
         <v>80</v>
       </c>
       <c r="H10" s="1">
         <v>22193</v>
       </c>
       <c r="I10">
-        <f>IF(ISBLANK(J10),-H10,J10-H10)</f>
+        <f t="shared" si="2"/>
         <v>58</v>
       </c>
       <c r="J10" s="1">
         <v>22251</v>
       </c>
       <c r="K10">
-        <f>IF(ISBLANK(L10),-J10,L10-J10)</f>
+        <f t="shared" si="3"/>
         <v>70</v>
       </c>
       <c r="L10" s="1">
         <v>22321</v>
       </c>
       <c r="M10">
-        <f>IF(ISBLANK(N10),-L10,N10-L10)</f>
+        <f t="shared" si="4"/>
         <v>62</v>
       </c>
       <c r="N10" s="1">
         <v>22383</v>
       </c>
       <c r="O10">
-        <f>IF(ISBLANK(P10),-N10,P10-N10)</f>
+        <f t="shared" si="5"/>
         <v>70</v>
       </c>
       <c r="P10" s="1">
         <v>22453</v>
       </c>
       <c r="Q10">
-        <f>IF(ISBLANK(R10),-P10,R10-P10)</f>
+        <f t="shared" si="6"/>
         <v>173</v>
       </c>
       <c r="R10" s="1">
         <v>22626</v>
       </c>
       <c r="S10">
-        <f>IF(ISBLANK(T10),-R10,T10-R10)</f>
+        <f t="shared" si="7"/>
         <v>74</v>
       </c>
       <c r="T10" s="1">
         <v>22700</v>
       </c>
       <c r="U10">
-        <f>IF(ISBLANK(V10),-T10,V10-T10)</f>
+        <f t="shared" si="8"/>
         <v>193</v>
       </c>
       <c r="V10" s="1">
         <v>22893</v>
       </c>
       <c r="W10">
-        <f>IF(ISBLANK(X10),-V10,X10-V10)</f>
+        <f t="shared" si="9"/>
         <v>626</v>
       </c>
       <c r="X10" s="1">
         <v>23519</v>
       </c>
       <c r="Y10">
-        <f>IF(ISBLANK(Z10),-X10,Z10-X10)</f>
+        <f t="shared" si="10"/>
         <v>330</v>
       </c>
       <c r="Z10" s="1">
         <v>23849</v>
       </c>
       <c r="AA10">
-        <f>IF(ISBLANK(AB10),-Z10,AB10-Z10)</f>
+        <f t="shared" si="11"/>
         <v>483</v>
       </c>
       <c r="AB10" s="1">
         <v>24332</v>
       </c>
       <c r="AC10">
-        <f>IF(ISBLANK(AD10),-AB10,AD10-AB10)</f>
+        <f t="shared" si="12"/>
         <v>600</v>
       </c>
       <c r="AD10" s="1">
@@ -8455,91 +8580,91 @@
         <v>14802</v>
       </c>
       <c r="E11">
-        <f>IF(ISBLANK(F11),-D11,F11-D11)</f>
+        <f t="shared" si="0"/>
         <v>156</v>
       </c>
       <c r="F11" s="1">
         <v>14958</v>
       </c>
       <c r="G11">
-        <f>IF(ISBLANK(H11),-F11,H11-F11)</f>
+        <f t="shared" si="1"/>
         <v>51</v>
       </c>
       <c r="H11" s="1">
         <v>15009</v>
       </c>
       <c r="I11">
-        <f>IF(ISBLANK(J11),-H11,J11-H11)</f>
+        <f t="shared" si="2"/>
         <v>198</v>
       </c>
       <c r="J11" s="1">
         <v>15207</v>
       </c>
       <c r="K11">
-        <f>IF(ISBLANK(L11),-J11,L11-J11)</f>
+        <f t="shared" si="3"/>
         <v>146</v>
       </c>
       <c r="L11" s="1">
         <v>15353</v>
       </c>
       <c r="M11">
-        <f>IF(ISBLANK(N11),-L11,N11-L11)</f>
+        <f t="shared" si="4"/>
         <v>41</v>
       </c>
       <c r="N11" s="1">
         <v>15394</v>
       </c>
       <c r="O11">
-        <f>IF(ISBLANK(P11),-N11,P11-N11)</f>
+        <f t="shared" si="5"/>
         <v>392</v>
       </c>
       <c r="P11" s="1">
         <v>15786</v>
       </c>
       <c r="Q11">
-        <f>IF(ISBLANK(R11),-P11,R11-P11)</f>
+        <f t="shared" si="6"/>
         <v>321</v>
       </c>
       <c r="R11" s="1">
         <v>16107</v>
       </c>
       <c r="S11">
-        <f>IF(ISBLANK(T11),-R11,T11-R11)</f>
+        <f t="shared" si="7"/>
         <v>101</v>
       </c>
       <c r="T11" s="1">
         <v>16208</v>
       </c>
       <c r="U11">
-        <f>IF(ISBLANK(V11),-T11,V11-T11)</f>
+        <f t="shared" si="8"/>
         <v>170</v>
       </c>
       <c r="V11" s="1">
         <v>16378</v>
       </c>
       <c r="W11">
-        <f>IF(ISBLANK(X11),-V11,X11-V11)</f>
+        <f t="shared" si="9"/>
         <v>530</v>
       </c>
       <c r="X11" s="1">
         <v>16908</v>
       </c>
       <c r="Y11">
-        <f>IF(ISBLANK(Z11),-X11,Z11-X11)</f>
+        <f t="shared" si="10"/>
         <v>490</v>
       </c>
       <c r="Z11" s="1">
         <v>17398</v>
       </c>
       <c r="AA11">
-        <f>IF(ISBLANK(AB11),-Z11,AB11-Z11)</f>
+        <f t="shared" si="11"/>
         <v>329</v>
       </c>
       <c r="AB11" s="1">
         <v>17727</v>
       </c>
       <c r="AC11">
-        <f>IF(ISBLANK(AD11),-AB11,AD11-AB11)</f>
+        <f t="shared" si="12"/>
         <v>749</v>
       </c>
       <c r="AD11" s="1">
@@ -8557,91 +8682,91 @@
         <v>10582</v>
       </c>
       <c r="E12">
-        <f>IF(ISBLANK(F12),-D12,F12-D12)</f>
+        <f t="shared" si="0"/>
         <v>57</v>
       </c>
       <c r="F12" s="1">
         <v>10639</v>
       </c>
       <c r="G12">
-        <f>IF(ISBLANK(H12),-F12,H12-F12)</f>
+        <f t="shared" si="1"/>
         <v>106</v>
       </c>
       <c r="H12" s="1">
         <v>10745</v>
       </c>
       <c r="I12">
-        <f>IF(ISBLANK(J12),-H12,J12-H12)</f>
+        <f t="shared" si="2"/>
         <v>138</v>
       </c>
       <c r="J12" s="1">
         <v>10883</v>
       </c>
       <c r="K12">
-        <f>IF(ISBLANK(L12),-J12,L12-J12)</f>
+        <f t="shared" si="3"/>
         <v>54</v>
       </c>
       <c r="L12" s="1">
         <v>10937</v>
       </c>
       <c r="M12">
-        <f>IF(ISBLANK(N12),-L12,N12-L12)</f>
+        <f t="shared" si="4"/>
         <v>300</v>
       </c>
       <c r="N12" s="1">
         <v>11237</v>
       </c>
       <c r="O12">
-        <f>IF(ISBLANK(P12),-N12,P12-N12)</f>
+        <f t="shared" si="5"/>
         <v>159</v>
       </c>
       <c r="P12" s="1">
         <v>11396</v>
       </c>
       <c r="Q12">
-        <f>IF(ISBLANK(R12),-P12,R12-P12)</f>
+        <f t="shared" si="6"/>
         <v>322</v>
       </c>
       <c r="R12" s="1">
         <v>11718</v>
       </c>
       <c r="S12">
-        <f>IF(ISBLANK(T12),-R12,T12-R12)</f>
+        <f t="shared" si="7"/>
         <v>908</v>
       </c>
       <c r="T12" s="1">
         <v>12626</v>
       </c>
       <c r="U12">
-        <f>IF(ISBLANK(V12),-T12,V12-T12)</f>
+        <f t="shared" si="8"/>
         <v>1585</v>
       </c>
       <c r="V12" s="1">
         <v>14211</v>
       </c>
       <c r="W12">
-        <f>IF(ISBLANK(X12),-V12,X12-V12)</f>
+        <f t="shared" si="9"/>
         <v>826</v>
       </c>
       <c r="X12" s="1">
         <v>15037</v>
       </c>
       <c r="Y12">
-        <f>IF(ISBLANK(Z12),-X12,Z12-X12)</f>
+        <f t="shared" si="10"/>
         <v>429</v>
       </c>
       <c r="Z12" s="1">
         <v>15466</v>
       </c>
       <c r="AA12">
-        <f>IF(ISBLANK(AB12),-Z12,AB12-Z12)</f>
+        <f t="shared" si="11"/>
         <v>1664</v>
       </c>
       <c r="AB12" s="1">
         <v>17130</v>
       </c>
       <c r="AC12">
-        <f>IF(ISBLANK(AD12),-AB12,AD12-AB12)</f>
+        <f t="shared" si="12"/>
         <v>-17130</v>
       </c>
       <c r="AD12" s="1">
@@ -8659,91 +8784,91 @@
         <v>9823</v>
       </c>
       <c r="E13">
-        <f>IF(ISBLANK(F13),-D13,F13-D13)</f>
+        <f t="shared" si="0"/>
         <v>37</v>
       </c>
       <c r="F13" s="1">
         <v>9860</v>
       </c>
       <c r="G13">
-        <f>IF(ISBLANK(H13),-F13,H13-F13)</f>
+        <f t="shared" si="1"/>
         <v>76</v>
       </c>
       <c r="H13" s="1">
         <v>9936</v>
       </c>
       <c r="I13">
-        <f>IF(ISBLANK(J13),-H13,J13-H13)</f>
+        <f t="shared" si="2"/>
         <v>54</v>
       </c>
       <c r="J13" s="1">
         <v>9990</v>
       </c>
       <c r="K13">
-        <f>IF(ISBLANK(L13),-J13,L13-J13)</f>
+        <f t="shared" si="3"/>
         <v>184</v>
       </c>
       <c r="L13" s="1">
         <v>10174</v>
       </c>
       <c r="M13">
-        <f>IF(ISBLANK(N13),-L13,N13-L13)</f>
+        <f t="shared" si="4"/>
         <v>52</v>
       </c>
       <c r="N13" s="1">
         <v>10226</v>
       </c>
       <c r="O13">
-        <f>IF(ISBLANK(P13),-N13,P13-N13)</f>
+        <f t="shared" si="5"/>
         <v>168</v>
       </c>
       <c r="P13" s="1">
         <v>10394</v>
       </c>
       <c r="Q13">
-        <f>IF(ISBLANK(R13),-P13,R13-P13)</f>
+        <f t="shared" si="6"/>
         <v>214</v>
       </c>
       <c r="R13" s="1">
         <v>10608</v>
       </c>
       <c r="S13">
-        <f>IF(ISBLANK(T13),-R13,T13-R13)</f>
+        <f t="shared" si="7"/>
         <v>48</v>
       </c>
       <c r="T13" s="1">
         <v>10656</v>
       </c>
       <c r="U13">
-        <f>IF(ISBLANK(V13),-T13,V13-T13)</f>
+        <f t="shared" si="8"/>
         <v>286</v>
       </c>
       <c r="V13" s="1">
         <v>10942</v>
       </c>
       <c r="W13">
-        <f>IF(ISBLANK(X13),-V13,X13-V13)</f>
+        <f t="shared" si="9"/>
         <v>208</v>
       </c>
       <c r="X13" s="1">
         <v>11150</v>
       </c>
       <c r="Y13">
-        <f>IF(ISBLANK(Z13),-X13,Z13-X13)</f>
+        <f t="shared" si="10"/>
         <v>-11150</v>
       </c>
       <c r="Z13" s="1">
         <v>0</v>
       </c>
       <c r="AA13">
-        <f>IF(ISBLANK(AB13),-Z13,AB13-Z13)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AB13" s="1">
         <v>0</v>
       </c>
       <c r="AC13">
-        <f>IF(ISBLANK(AD13),-AB13,AD13-AB13)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AD13" s="1">
@@ -8761,91 +8886,91 @@
         <v>9423</v>
       </c>
       <c r="E14">
-        <f>IF(ISBLANK(F14),-D14,F14-D14)</f>
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="F14" s="1">
         <v>9455</v>
       </c>
       <c r="G14">
-        <f>IF(ISBLANK(H14),-F14,H14-F14)</f>
+        <f t="shared" si="1"/>
         <v>325</v>
       </c>
       <c r="H14" s="1">
         <v>9780</v>
       </c>
       <c r="I14">
-        <f>IF(ISBLANK(J14),-H14,J14-H14)</f>
+        <f t="shared" si="2"/>
         <v>75</v>
       </c>
       <c r="J14" s="1">
         <v>9855</v>
       </c>
       <c r="K14">
-        <f>IF(ISBLANK(L14),-J14,L14-J14)</f>
+        <f t="shared" si="3"/>
         <v>114</v>
       </c>
       <c r="L14" s="1">
         <v>9969</v>
       </c>
       <c r="M14">
-        <f>IF(ISBLANK(N14),-L14,N14-L14)</f>
+        <f t="shared" si="4"/>
         <v>280</v>
       </c>
       <c r="N14" s="1">
         <v>10249</v>
       </c>
       <c r="O14">
-        <f>IF(ISBLANK(P14),-N14,P14-N14)</f>
+        <f t="shared" si="5"/>
         <v>78</v>
       </c>
       <c r="P14" s="1">
         <v>10327</v>
       </c>
       <c r="Q14">
-        <f>IF(ISBLANK(R14),-P14,R14-P14)</f>
+        <f t="shared" si="6"/>
         <v>137</v>
       </c>
       <c r="R14" s="1">
         <v>10464</v>
       </c>
       <c r="S14">
-        <f>IF(ISBLANK(T14),-R14,T14-R14)</f>
+        <f t="shared" si="7"/>
         <v>79</v>
       </c>
       <c r="T14" s="1">
         <v>10543</v>
       </c>
       <c r="U14">
-        <f>IF(ISBLANK(V14),-T14,V14-T14)</f>
+        <f t="shared" si="8"/>
         <v>1160</v>
       </c>
       <c r="V14" s="1">
         <v>11703</v>
       </c>
       <c r="W14">
-        <f>IF(ISBLANK(X14),-V14,X14-V14)</f>
+        <f t="shared" si="9"/>
         <v>568</v>
       </c>
       <c r="X14" s="1">
         <v>12271</v>
       </c>
       <c r="Y14">
-        <f>IF(ISBLANK(Z14),-X14,Z14-X14)</f>
+        <f t="shared" si="10"/>
         <v>499</v>
       </c>
       <c r="Z14" s="1">
         <v>12770</v>
       </c>
       <c r="AA14">
-        <f>IF(ISBLANK(AB14),-Z14,AB14-Z14)</f>
+        <f t="shared" si="11"/>
         <v>-12770</v>
       </c>
       <c r="AB14" s="1">
         <v>0</v>
       </c>
       <c r="AC14">
-        <f>IF(ISBLANK(AD14),-AB14,AD14-AB14)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AD14" s="1">
@@ -8863,91 +8988,91 @@
         <v>9306</v>
       </c>
       <c r="E15">
-        <f>IF(ISBLANK(F15),-D15,F15-D15)</f>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="F15" s="1">
         <v>9331</v>
       </c>
       <c r="G15">
-        <f>IF(ISBLANK(H15),-F15,H15-F15)</f>
+        <f t="shared" si="1"/>
         <v>70</v>
       </c>
       <c r="H15" s="1">
         <v>9401</v>
       </c>
       <c r="I15">
-        <f>IF(ISBLANK(J15),-H15,J15-H15)</f>
+        <f t="shared" si="2"/>
         <v>35</v>
       </c>
       <c r="J15" s="1">
         <v>9436</v>
       </c>
       <c r="K15">
-        <f>IF(ISBLANK(L15),-J15,L15-J15)</f>
+        <f t="shared" si="3"/>
         <v>60</v>
       </c>
       <c r="L15" s="1">
         <v>9496</v>
       </c>
       <c r="M15">
-        <f>IF(ISBLANK(N15),-L15,N15-L15)</f>
+        <f t="shared" si="4"/>
         <v>228</v>
       </c>
       <c r="N15" s="1">
         <v>9724</v>
       </c>
       <c r="O15">
-        <f>IF(ISBLANK(P15),-N15,P15-N15)</f>
+        <f t="shared" si="5"/>
         <v>145</v>
       </c>
       <c r="P15" s="1">
         <v>9869</v>
       </c>
       <c r="Q15">
-        <f>IF(ISBLANK(R15),-P15,R15-P15)</f>
+        <f t="shared" si="6"/>
         <v>106</v>
       </c>
       <c r="R15" s="1">
         <v>9975</v>
       </c>
       <c r="S15">
-        <f>IF(ISBLANK(T15),-R15,T15-R15)</f>
+        <f t="shared" si="7"/>
         <v>247</v>
       </c>
       <c r="T15" s="1">
         <v>10222</v>
       </c>
       <c r="U15">
-        <f>IF(ISBLANK(V15),-T15,V15-T15)</f>
+        <f t="shared" si="8"/>
         <v>616</v>
       </c>
       <c r="V15" s="1">
         <v>10838</v>
       </c>
       <c r="W15">
-        <f>IF(ISBLANK(X15),-V15,X15-V15)</f>
+        <f t="shared" si="9"/>
         <v>-10838</v>
       </c>
       <c r="X15" s="1">
         <v>0</v>
       </c>
       <c r="Y15">
-        <f>IF(ISBLANK(Z15),-X15,Z15-X15)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Z15" s="1">
         <v>0</v>
       </c>
       <c r="AA15">
-        <f>IF(ISBLANK(AB15),-Z15,AB15-Z15)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AB15" s="1">
         <v>0</v>
       </c>
       <c r="AC15">
-        <f>IF(ISBLANK(AD15),-AB15,AD15-AB15)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AD15" s="1">
@@ -8965,91 +9090,91 @@
         <v>7475</v>
       </c>
       <c r="E16">
-        <f>IF(ISBLANK(F16),-D16,F16-D16)</f>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="F16" s="1">
         <v>7498</v>
       </c>
       <c r="G16">
-        <f>IF(ISBLANK(H16),-F16,H16-F16)</f>
+        <f t="shared" si="1"/>
         <v>98</v>
       </c>
       <c r="H16" s="1">
         <v>7596</v>
       </c>
       <c r="I16">
-        <f>IF(ISBLANK(J16),-H16,J16-H16)</f>
+        <f t="shared" si="2"/>
         <v>142</v>
       </c>
       <c r="J16" s="1">
         <v>7738</v>
       </c>
       <c r="K16">
-        <f>IF(ISBLANK(L16),-J16,L16-J16)</f>
+        <f t="shared" si="3"/>
         <v>70</v>
       </c>
       <c r="L16" s="1">
         <v>7808</v>
       </c>
       <c r="M16">
-        <f>IF(ISBLANK(N16),-L16,N16-L16)</f>
+        <f t="shared" si="4"/>
         <v>197</v>
       </c>
       <c r="N16" s="1">
         <v>8005</v>
       </c>
       <c r="O16">
-        <f>IF(ISBLANK(P16),-N16,P16-N16)</f>
+        <f t="shared" si="5"/>
         <v>192</v>
       </c>
       <c r="P16" s="1">
         <v>8197</v>
       </c>
       <c r="Q16">
-        <f>IF(ISBLANK(R16),-P16,R16-P16)</f>
+        <f t="shared" si="6"/>
         <v>176</v>
       </c>
       <c r="R16" s="1">
         <v>8373</v>
       </c>
       <c r="S16">
-        <f>IF(ISBLANK(T16),-R16,T16-R16)</f>
+        <f t="shared" si="7"/>
         <v>188</v>
       </c>
       <c r="T16" s="1">
         <v>8561</v>
       </c>
       <c r="U16">
-        <f>IF(ISBLANK(V16),-T16,V16-T16)</f>
+        <f t="shared" si="8"/>
         <v>-8561</v>
       </c>
       <c r="V16" s="1">
         <v>0</v>
       </c>
       <c r="W16">
-        <f>IF(ISBLANK(X16),-V16,X16-V16)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="X16" s="1">
         <v>0</v>
       </c>
       <c r="Y16">
-        <f>IF(ISBLANK(Z16),-X16,Z16-X16)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Z16" s="1">
         <v>0</v>
       </c>
       <c r="AA16">
-        <f>IF(ISBLANK(AB16),-Z16,AB16-Z16)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AB16" s="1">
         <v>0</v>
       </c>
       <c r="AC16">
-        <f>IF(ISBLANK(AD16),-AB16,AD16-AB16)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AD16" s="1">
@@ -9067,91 +9192,91 @@
         <v>4665</v>
       </c>
       <c r="E17">
-        <f>IF(ISBLANK(F17),-D17,F17-D17)</f>
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="F17" s="1">
         <v>4691</v>
       </c>
       <c r="G17">
-        <f>IF(ISBLANK(H17),-F17,H17-F17)</f>
+        <f t="shared" si="1"/>
         <v>43</v>
       </c>
       <c r="H17" s="1">
         <v>4734</v>
       </c>
       <c r="I17">
-        <f>IF(ISBLANK(J17),-H17,J17-H17)</f>
+        <f t="shared" si="2"/>
         <v>57</v>
       </c>
       <c r="J17" s="1">
         <v>4791</v>
       </c>
       <c r="K17">
-        <f>IF(ISBLANK(L17),-J17,L17-J17)</f>
+        <f t="shared" si="3"/>
         <v>50</v>
       </c>
       <c r="L17" s="1">
         <v>4841</v>
       </c>
       <c r="M17">
-        <f>IF(ISBLANK(N17),-L17,N17-L17)</f>
+        <f t="shared" si="4"/>
         <v>115</v>
       </c>
       <c r="N17" s="1">
         <v>4956</v>
       </c>
       <c r="O17">
-        <f>IF(ISBLANK(P17),-N17,P17-N17)</f>
+        <f t="shared" si="5"/>
         <v>72</v>
       </c>
       <c r="P17" s="1">
         <v>5028</v>
       </c>
       <c r="Q17">
-        <f>IF(ISBLANK(R17),-P17,R17-P17)</f>
+        <f t="shared" si="6"/>
         <v>104</v>
       </c>
       <c r="R17" s="1">
         <v>5132</v>
       </c>
       <c r="S17">
-        <f>IF(ISBLANK(T17),-R17,T17-R17)</f>
+        <f t="shared" si="7"/>
         <v>-5132</v>
       </c>
       <c r="T17" s="1">
         <v>0</v>
       </c>
       <c r="U17">
-        <f>IF(ISBLANK(V17),-T17,V17-T17)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="V17" s="1">
         <v>0</v>
       </c>
       <c r="W17">
-        <f>IF(ISBLANK(X17),-V17,X17-V17)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="X17" s="1">
         <v>0</v>
       </c>
       <c r="Y17">
-        <f>IF(ISBLANK(Z17),-X17,Z17-X17)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Z17" s="1">
         <v>0</v>
       </c>
       <c r="AA17">
-        <f>IF(ISBLANK(AB17),-Z17,AB17-Z17)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AB17" s="1">
         <v>0</v>
       </c>
       <c r="AC17">
-        <f>IF(ISBLANK(AD17),-AB17,AD17-AB17)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AD17" s="1">
@@ -9169,91 +9294,91 @@
         <v>3682</v>
       </c>
       <c r="E18">
-        <f>IF(ISBLANK(F18),-D18,F18-D18)</f>
+        <f t="shared" si="0"/>
         <v>77</v>
       </c>
       <c r="F18" s="1">
         <v>3759</v>
       </c>
       <c r="G18">
-        <f>IF(ISBLANK(H18),-F18,H18-F18)</f>
+        <f t="shared" si="1"/>
         <v>44</v>
       </c>
       <c r="H18" s="1">
         <v>3803</v>
       </c>
       <c r="I18">
-        <f>IF(ISBLANK(J18),-H18,J18-H18)</f>
+        <f t="shared" si="2"/>
         <v>116</v>
       </c>
       <c r="J18" s="1">
         <v>3919</v>
       </c>
       <c r="K18">
-        <f>IF(ISBLANK(L18),-J18,L18-J18)</f>
+        <f t="shared" si="3"/>
         <v>87</v>
       </c>
       <c r="L18" s="1">
         <v>4006</v>
       </c>
       <c r="M18">
-        <f>IF(ISBLANK(N18),-L18,N18-L18)</f>
+        <f t="shared" si="4"/>
         <v>41</v>
       </c>
       <c r="N18" s="1">
         <v>4047</v>
       </c>
       <c r="O18">
-        <f>IF(ISBLANK(P18),-N18,P18-N18)</f>
+        <f t="shared" si="5"/>
         <v>134</v>
       </c>
       <c r="P18" s="1">
         <v>4181</v>
       </c>
       <c r="Q18">
-        <f>IF(ISBLANK(R18),-P18,R18-P18)</f>
+        <f t="shared" si="6"/>
         <v>-4181</v>
       </c>
       <c r="R18" s="1">
         <v>0</v>
       </c>
       <c r="S18">
-        <f>IF(ISBLANK(T18),-R18,T18-R18)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="T18" s="1">
         <v>0</v>
       </c>
       <c r="U18">
-        <f>IF(ISBLANK(V18),-T18,V18-T18)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="V18" s="1">
         <v>0</v>
       </c>
       <c r="W18">
-        <f>IF(ISBLANK(X18),-V18,X18-V18)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="X18" s="1">
         <v>0</v>
       </c>
       <c r="Y18">
-        <f>IF(ISBLANK(Z18),-X18,Z18-X18)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Z18" s="1">
         <v>0</v>
       </c>
       <c r="AA18">
-        <f>IF(ISBLANK(AB18),-Z18,AB18-Z18)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AB18" s="1">
         <v>0</v>
       </c>
       <c r="AC18">
-        <f>IF(ISBLANK(AD18),-AB18,AD18-AB18)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AD18" s="1">
@@ -9271,91 +9396,91 @@
         <v>3286</v>
       </c>
       <c r="E19">
-        <f>IF(ISBLANK(F19),-D19,F19-D19)</f>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="F19" s="1">
         <v>3307</v>
       </c>
       <c r="G19">
-        <f>IF(ISBLANK(H19),-F19,H19-F19)</f>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="H19" s="1">
         <v>3320</v>
       </c>
       <c r="I19">
-        <f>IF(ISBLANK(J19),-H19,J19-H19)</f>
+        <f t="shared" si="2"/>
         <v>232</v>
       </c>
       <c r="J19" s="1">
         <v>3552</v>
       </c>
       <c r="K19">
-        <f>IF(ISBLANK(L19),-J19,L19-J19)</f>
+        <f t="shared" si="3"/>
         <v>102</v>
       </c>
       <c r="L19" s="1">
         <v>3654</v>
       </c>
       <c r="M19">
-        <f>IF(ISBLANK(N19),-L19,N19-L19)</f>
+        <f t="shared" si="4"/>
         <v>60</v>
       </c>
       <c r="N19" s="1">
         <v>3714</v>
       </c>
       <c r="O19">
-        <f>IF(ISBLANK(P19),-N19,P19-N19)</f>
+        <f t="shared" si="5"/>
         <v>-3714</v>
       </c>
       <c r="P19" s="1">
         <v>0</v>
       </c>
       <c r="Q19">
-        <f>IF(ISBLANK(R19),-P19,R19-P19)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="R19" s="1">
         <v>0</v>
       </c>
       <c r="S19">
-        <f>IF(ISBLANK(T19),-R19,T19-R19)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="T19" s="1">
         <v>0</v>
       </c>
       <c r="U19">
-        <f>IF(ISBLANK(V19),-T19,V19-T19)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="V19" s="1">
         <v>0</v>
       </c>
       <c r="W19">
-        <f>IF(ISBLANK(X19),-V19,X19-V19)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="X19" s="1">
         <v>0</v>
       </c>
       <c r="Y19">
-        <f>IF(ISBLANK(Z19),-X19,Z19-X19)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Z19" s="1">
         <v>0</v>
       </c>
       <c r="AA19">
-        <f>IF(ISBLANK(AB19),-Z19,AB19-Z19)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AB19" s="1">
         <v>0</v>
       </c>
       <c r="AC19">
-        <f>IF(ISBLANK(AD19),-AB19,AD19-AB19)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AD19" s="1">
@@ -9373,91 +9498,91 @@
         <v>3182</v>
       </c>
       <c r="E20">
-        <f>IF(ISBLANK(F20),-D20,F20-D20)</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="F20" s="1">
         <v>3197</v>
       </c>
       <c r="G20">
-        <f>IF(ISBLANK(H20),-F20,H20-F20)</f>
+        <f t="shared" si="1"/>
         <v>60</v>
       </c>
       <c r="H20" s="1">
         <v>3257</v>
       </c>
       <c r="I20">
-        <f>IF(ISBLANK(J20),-H20,J20-H20)</f>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="J20" s="1">
         <v>3300</v>
       </c>
       <c r="K20">
-        <f>IF(ISBLANK(L20),-J20,L20-J20)</f>
+        <f t="shared" si="3"/>
         <v>32</v>
       </c>
       <c r="L20" s="1">
         <v>3332</v>
       </c>
       <c r="M20">
-        <f>IF(ISBLANK(N20),-L20,N20-L20)</f>
+        <f t="shared" si="4"/>
         <v>-3332</v>
       </c>
       <c r="N20" s="1">
         <v>0</v>
       </c>
       <c r="O20">
-        <f>IF(ISBLANK(P20),-N20,P20-N20)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P20" s="1">
         <v>0</v>
       </c>
       <c r="Q20">
-        <f>IF(ISBLANK(R20),-P20,R20-P20)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="R20" s="1">
         <v>0</v>
       </c>
       <c r="S20">
-        <f>IF(ISBLANK(T20),-R20,T20-R20)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="T20" s="1">
         <v>0</v>
       </c>
       <c r="U20">
-        <f>IF(ISBLANK(V20),-T20,V20-T20)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="V20" s="1">
         <v>0</v>
       </c>
       <c r="W20">
-        <f>IF(ISBLANK(X20),-V20,X20-V20)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="X20" s="1">
         <v>0</v>
       </c>
       <c r="Y20">
-        <f>IF(ISBLANK(Z20),-X20,Z20-X20)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Z20" s="1">
         <v>0</v>
       </c>
       <c r="AA20">
-        <f>IF(ISBLANK(AB20),-Z20,AB20-Z20)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AB20" s="1">
         <v>0</v>
       </c>
       <c r="AC20">
-        <f>IF(ISBLANK(AD20),-AB20,AD20-AB20)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AD20" s="1">
@@ -9475,91 +9600,91 @@
         <v>2864</v>
       </c>
       <c r="E21">
-        <f>IF(ISBLANK(F21),-D21,F21-D21)</f>
+        <f t="shared" si="0"/>
         <v>34</v>
       </c>
       <c r="F21" s="1">
         <v>2898</v>
       </c>
       <c r="G21">
-        <f>IF(ISBLANK(H21),-F21,H21-F21)</f>
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="H21" s="1">
         <v>2919</v>
       </c>
       <c r="I21">
-        <f>IF(ISBLANK(J21),-H21,J21-H21)</f>
+        <f t="shared" si="2"/>
         <v>148</v>
       </c>
       <c r="J21" s="1">
         <v>3067</v>
       </c>
       <c r="K21">
-        <f>IF(ISBLANK(L21),-J21,L21-J21)</f>
+        <f t="shared" si="3"/>
         <v>-3067</v>
       </c>
       <c r="L21" s="1">
         <v>0</v>
       </c>
       <c r="M21">
-        <f>IF(ISBLANK(N21),-L21,N21-L21)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N21" s="1">
         <v>0</v>
       </c>
       <c r="O21">
-        <f>IF(ISBLANK(P21),-N21,P21-N21)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P21" s="1">
         <v>0</v>
       </c>
       <c r="Q21">
-        <f>IF(ISBLANK(R21),-P21,R21-P21)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="R21" s="1">
         <v>0</v>
       </c>
       <c r="S21">
-        <f>IF(ISBLANK(T21),-R21,T21-R21)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="T21" s="1">
         <v>0</v>
       </c>
       <c r="U21">
-        <f>IF(ISBLANK(V21),-T21,V21-T21)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="V21" s="1">
         <v>0</v>
       </c>
       <c r="W21">
-        <f>IF(ISBLANK(X21),-V21,X21-V21)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="X21" s="1">
         <v>0</v>
       </c>
       <c r="Y21">
-        <f>IF(ISBLANK(Z21),-X21,Z21-X21)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Z21" s="1">
         <v>0</v>
       </c>
       <c r="AA21">
-        <f>IF(ISBLANK(AB21),-Z21,AB21-Z21)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AB21" s="1">
         <v>0</v>
       </c>
       <c r="AC21">
-        <f>IF(ISBLANK(AD21),-AB21,AD21-AB21)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AD21" s="1">
@@ -9577,91 +9702,91 @@
         <v>2416</v>
       </c>
       <c r="E22">
-        <f>IF(ISBLANK(F22),-D22,F22-D22)</f>
+        <f t="shared" si="0"/>
         <v>48</v>
       </c>
       <c r="F22" s="1">
         <v>2464</v>
       </c>
       <c r="G22">
-        <f>IF(ISBLANK(H22),-F22,H22-F22)</f>
+        <f t="shared" si="1"/>
         <v>78</v>
       </c>
       <c r="H22" s="1">
         <v>2542</v>
       </c>
       <c r="I22">
-        <f>IF(ISBLANK(J22),-H22,J22-H22)</f>
+        <f t="shared" si="2"/>
         <v>-2542</v>
       </c>
       <c r="J22" s="1">
         <v>0</v>
       </c>
       <c r="K22">
-        <f>IF(ISBLANK(L22),-J22,L22-J22)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L22" s="1">
         <v>0</v>
       </c>
       <c r="M22">
-        <f>IF(ISBLANK(N22),-L22,N22-L22)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N22" s="1">
         <v>0</v>
       </c>
       <c r="O22">
-        <f>IF(ISBLANK(P22),-N22,P22-N22)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P22" s="1">
         <v>0</v>
       </c>
       <c r="Q22">
-        <f>IF(ISBLANK(R22),-P22,R22-P22)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="R22" s="1">
         <v>0</v>
       </c>
       <c r="S22">
-        <f>IF(ISBLANK(T22),-R22,T22-R22)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="T22" s="1">
         <v>0</v>
       </c>
       <c r="U22">
-        <f>IF(ISBLANK(V22),-T22,V22-T22)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="V22" s="1">
         <v>0</v>
       </c>
       <c r="W22">
-        <f>IF(ISBLANK(X22),-V22,X22-V22)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="X22" s="1">
         <v>0</v>
       </c>
       <c r="Y22">
-        <f>IF(ISBLANK(Z22),-X22,Z22-X22)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Z22" s="1">
         <v>0</v>
       </c>
       <c r="AA22">
-        <f>IF(ISBLANK(AB22),-Z22,AB22-Z22)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AB22" s="1">
         <v>0</v>
       </c>
       <c r="AC22">
-        <f>IF(ISBLANK(AD22),-AB22,AD22-AB22)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AD22" s="1">
@@ -9679,91 +9804,91 @@
         <v>2395</v>
       </c>
       <c r="E23">
-        <f>IF(ISBLANK(F23),-D23,F23-D23)</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="F23" s="1">
         <v>2409</v>
       </c>
       <c r="G23">
-        <f>IF(ISBLANK(H23),-F23,H23-F23)</f>
+        <f t="shared" si="1"/>
         <v>-2409</v>
       </c>
       <c r="H23" s="1">
         <v>0</v>
       </c>
       <c r="I23">
-        <f>IF(ISBLANK(J23),-H23,J23-H23)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J23" s="1">
         <v>0</v>
       </c>
       <c r="K23">
-        <f>IF(ISBLANK(L23),-J23,L23-J23)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L23" s="1">
         <v>0</v>
       </c>
       <c r="M23">
-        <f>IF(ISBLANK(N23),-L23,N23-L23)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N23" s="1">
         <v>0</v>
       </c>
       <c r="O23">
-        <f>IF(ISBLANK(P23),-N23,P23-N23)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P23" s="1">
         <v>0</v>
       </c>
       <c r="Q23">
-        <f>IF(ISBLANK(R23),-P23,R23-P23)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="R23" s="1">
         <v>0</v>
       </c>
       <c r="S23">
-        <f>IF(ISBLANK(T23),-R23,T23-R23)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="T23" s="1">
         <v>0</v>
       </c>
       <c r="U23">
-        <f>IF(ISBLANK(V23),-T23,V23-T23)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="V23" s="1">
         <v>0</v>
       </c>
       <c r="W23">
-        <f>IF(ISBLANK(X23),-V23,X23-V23)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="X23" s="1">
         <v>0</v>
       </c>
       <c r="Y23">
-        <f>IF(ISBLANK(Z23),-X23,Z23-X23)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Z23" s="1">
         <v>0</v>
       </c>
       <c r="AA23">
-        <f>IF(ISBLANK(AB23),-Z23,AB23-Z23)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AB23" s="1">
         <v>0</v>
       </c>
       <c r="AC23">
-        <f>IF(ISBLANK(AD23),-AB23,AD23-AB23)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AD23" s="1">
@@ -9781,91 +9906,91 @@
         <v>1423</v>
       </c>
       <c r="E24">
-        <f>IF(ISBLANK(F24),-D24,F24-D24)</f>
+        <f t="shared" si="0"/>
         <v>-1423</v>
       </c>
       <c r="F24" s="1">
         <v>0</v>
       </c>
       <c r="G24">
-        <f>IF(ISBLANK(H24),-F24,H24-F24)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H24" s="1">
         <v>0</v>
       </c>
       <c r="I24">
-        <f>IF(ISBLANK(J24),-H24,J24-H24)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J24" s="1">
         <v>0</v>
       </c>
       <c r="K24">
-        <f>IF(ISBLANK(L24),-J24,L24-J24)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L24" s="1">
         <v>0</v>
       </c>
       <c r="M24">
-        <f>IF(ISBLANK(N24),-L24,N24-L24)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N24" s="1">
         <v>0</v>
       </c>
       <c r="O24">
-        <f>IF(ISBLANK(P24),-N24,P24-N24)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P24" s="1">
         <v>0</v>
       </c>
       <c r="Q24">
-        <f>IF(ISBLANK(R24),-P24,R24-P24)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="R24" s="1">
         <v>0</v>
       </c>
       <c r="S24">
-        <f>IF(ISBLANK(T24),-R24,T24-R24)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="T24" s="1">
         <v>0</v>
       </c>
       <c r="U24">
-        <f>IF(ISBLANK(V24),-T24,V24-T24)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="V24" s="1">
         <v>0</v>
       </c>
       <c r="W24">
-        <f>IF(ISBLANK(X24),-V24,X24-V24)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="X24" s="1">
         <v>0</v>
       </c>
       <c r="Y24">
-        <f>IF(ISBLANK(Z24),-X24,Z24-X24)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Z24" s="1">
         <v>0</v>
       </c>
       <c r="AA24">
-        <f>IF(ISBLANK(AB24),-Z24,AB24-Z24)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AB24" s="1">
         <v>0</v>
       </c>
       <c r="AC24">
-        <f>IF(ISBLANK(AD24),-AB24,AD24-AB24)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AD24" s="1">
@@ -9961,19 +10086,19 @@
         <v>148</v>
       </c>
       <c r="E27">
-        <f t="shared" ref="E27:E48" si="0">FIND(",",B27)</f>
+        <f t="shared" ref="E27:E48" si="13">FIND(",",B27)</f>
         <v>9</v>
       </c>
       <c r="F27" t="str">
-        <f t="shared" ref="F27:F48" si="1">LEFT(B27,E27-1)</f>
+        <f t="shared" ref="F27:F48" si="14">LEFT(B27,E27-1)</f>
         <v>Kelleher</v>
       </c>
       <c r="G27" t="str">
-        <f t="shared" ref="G27:G48" si="2">RIGHT(B27,LEN(B27)-(E27+1))</f>
+        <f t="shared" ref="G27:G48" si="15">RIGHT(B27,LEN(B27)-(E27+1))</f>
         <v>Billy</v>
       </c>
       <c r="H27" t="str">
-        <f t="shared" ref="H27:H48" si="3">G27&amp;" "&amp;F27</f>
+        <f t="shared" ref="H27:H48" si="16">G27&amp;" "&amp;F27</f>
         <v>Billy Kelleher</v>
       </c>
       <c r="J27" t="s">
@@ -10026,19 +10151,19 @@
         <v>149</v>
       </c>
       <c r="E28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="13"/>
         <v>8</v>
       </c>
       <c r="F28" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="14"/>
         <v>Wallace</v>
       </c>
       <c r="G28" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="15"/>
         <v>Mick</v>
       </c>
       <c r="H28" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="16"/>
         <v>Mick Wallace</v>
       </c>
       <c r="J28" t="s">
@@ -10107,19 +10232,19 @@
         <v>150</v>
       </c>
       <c r="E29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="13"/>
         <v>9</v>
       </c>
       <c r="F29" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="14"/>
         <v>Ní Riada</v>
       </c>
       <c r="G29" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="15"/>
         <v>Liadh</v>
       </c>
       <c r="H29" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="16"/>
         <v>Liadh Ní Riada</v>
       </c>
       <c r="J29" t="s">
@@ -10188,19 +10313,19 @@
         <v>151</v>
       </c>
       <c r="E30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="13"/>
         <v>11</v>
       </c>
       <c r="F30" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="14"/>
         <v>O'Sullivan</v>
       </c>
       <c r="G30" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="15"/>
         <v>Grace</v>
       </c>
       <c r="H30" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="16"/>
         <v>Grace O'Sullivan</v>
       </c>
       <c r="J30" t="s">
@@ -10269,19 +10394,19 @@
         <v>152</v>
       </c>
       <c r="E31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="13"/>
         <v>6</v>
       </c>
       <c r="F31" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="14"/>
         <v>Byrne</v>
       </c>
       <c r="G31" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="15"/>
         <v>Malcolm</v>
       </c>
       <c r="H31" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="16"/>
         <v>Malcolm Byrne</v>
       </c>
       <c r="J31" t="s">
@@ -10350,19 +10475,19 @@
         <v>153</v>
       </c>
       <c r="E32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="13"/>
         <v>6</v>
       </c>
       <c r="F32" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="14"/>
         <v>Clune</v>
       </c>
       <c r="G32" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="15"/>
         <v>Deirdre</v>
       </c>
       <c r="H32" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="16"/>
         <v>Deirdre Clune</v>
       </c>
       <c r="J32" t="s">
@@ -10431,19 +10556,19 @@
         <v>154</v>
       </c>
       <c r="E33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="13"/>
         <v>6</v>
       </c>
       <c r="F33" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="14"/>
         <v>Doyle</v>
       </c>
       <c r="G33" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="15"/>
         <v>Andrew</v>
       </c>
       <c r="H33" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="16"/>
         <v>Andrew Doyle</v>
       </c>
       <c r="J33" t="s">
@@ -10512,19 +10637,19 @@
         <v>155</v>
       </c>
       <c r="E34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="13"/>
         <v>6</v>
       </c>
       <c r="F34" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="14"/>
         <v>Nunan</v>
       </c>
       <c r="G34" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="15"/>
         <v>Sheila</v>
       </c>
       <c r="H34" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="16"/>
         <v>Sheila Nunan</v>
       </c>
       <c r="J34" t="s">
@@ -10593,19 +10718,19 @@
         <v>156</v>
       </c>
       <c r="E35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="13"/>
         <v>8</v>
       </c>
       <c r="F35" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="14"/>
         <v>Wallace</v>
       </c>
       <c r="G35" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="15"/>
         <v>Adrienne</v>
       </c>
       <c r="H35" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="16"/>
         <v>Adrienne Wallace</v>
       </c>
       <c r="J35" t="s">
@@ -10674,19 +10799,19 @@
         <v>157</v>
       </c>
       <c r="E36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="13"/>
         <v>7</v>
       </c>
       <c r="F36" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="14"/>
         <v>Cahill</v>
       </c>
       <c r="G36" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="15"/>
         <v>Dolores</v>
       </c>
       <c r="H36" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="16"/>
         <v>Dolores Cahill</v>
       </c>
       <c r="J36" t="s">
@@ -10755,19 +10880,19 @@
         <v>158</v>
       </c>
       <c r="E37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="13"/>
         <v>8</v>
       </c>
       <c r="F37" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="14"/>
         <v>O'Flynn</v>
       </c>
       <c r="G37" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="15"/>
         <v>Diarmuid Patrick</v>
       </c>
       <c r="H37" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="16"/>
         <v>Diarmuid Patrick O'Flynn</v>
       </c>
       <c r="J37" t="s">
@@ -10833,19 +10958,19 @@
         <v>159</v>
       </c>
       <c r="E38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="13"/>
         <v>8</v>
       </c>
       <c r="F38" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="14"/>
         <v>Minehan</v>
       </c>
       <c r="G38" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="15"/>
         <v>Liam</v>
       </c>
       <c r="H38" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="16"/>
         <v>Liam Minehan</v>
       </c>
       <c r="J38" t="s">
@@ -10905,19 +11030,19 @@
         <v>160</v>
       </c>
       <c r="E39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="13"/>
         <v>8</v>
       </c>
       <c r="F39" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="14"/>
         <v>Gardner</v>
       </c>
       <c r="G39" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="15"/>
         <v>Breda Patricia</v>
       </c>
       <c r="H39" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="16"/>
         <v>Breda Patricia Gardner</v>
       </c>
       <c r="J39" t="s">
@@ -10980,19 +11105,19 @@
         <v>161</v>
       </c>
       <c r="E40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="13"/>
         <v>7</v>
       </c>
       <c r="F40" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="14"/>
         <v>Heaney</v>
       </c>
       <c r="G40" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="15"/>
         <v>Theresa</v>
       </c>
       <c r="H40" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="16"/>
         <v>Theresa Heaney</v>
       </c>
       <c r="J40" t="s">
@@ -11053,19 +11178,19 @@
         <v>162</v>
       </c>
       <c r="E41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="13"/>
         <v>8</v>
       </c>
       <c r="F41" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="14"/>
         <v>Brennan</v>
       </c>
       <c r="G41" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="15"/>
         <v>Allan</v>
       </c>
       <c r="H41" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="16"/>
         <v>Allan Brennan</v>
       </c>
       <c r="J41" t="s">
@@ -11123,19 +11248,19 @@
         <v>163</v>
       </c>
       <c r="E42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="13"/>
         <v>11</v>
       </c>
       <c r="F42" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="14"/>
         <v>O'Loughlin</v>
       </c>
       <c r="G42" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="15"/>
         <v>Peter</v>
       </c>
       <c r="H42" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="16"/>
         <v>Peter O'Loughlin</v>
       </c>
       <c r="J42" t="s">
@@ -11189,19 +11314,19 @@
         <v>164</v>
       </c>
       <c r="E43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="13"/>
         <v>12</v>
       </c>
       <c r="F43" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="14"/>
         <v>Worthington</v>
       </c>
       <c r="G43" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="15"/>
         <v>Colleen</v>
       </c>
       <c r="H43" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="16"/>
         <v>Colleen Worthington</v>
       </c>
       <c r="J43" t="s">
@@ -11251,19 +11376,19 @@
         <v>165</v>
       </c>
       <c r="E44">
-        <f t="shared" si="0"/>
+        <f t="shared" si="13"/>
         <v>11</v>
       </c>
       <c r="F44" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="14"/>
         <v>Fitzgerald</v>
       </c>
       <c r="G44" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="15"/>
         <v>Paddy</v>
       </c>
       <c r="H44" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="16"/>
         <v>Paddy Fitzgerald</v>
       </c>
       <c r="J44" t="s">
@@ -11309,19 +11434,19 @@
         <v>166</v>
       </c>
       <c r="E45">
-        <f t="shared" si="0"/>
+        <f t="shared" si="13"/>
         <v>13</v>
       </c>
       <c r="F45" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="14"/>
         <v>Ryan-Purcell</v>
       </c>
       <c r="G45" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="15"/>
         <v>Walter</v>
       </c>
       <c r="H45" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="16"/>
         <v>Walter Ryan-Purcell</v>
       </c>
       <c r="J45" t="s">
@@ -11363,19 +11488,19 @@
         <v>167</v>
       </c>
       <c r="E46">
-        <f t="shared" si="0"/>
+        <f t="shared" si="13"/>
         <v>7</v>
       </c>
       <c r="F46" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="14"/>
         <v>Sexton</v>
       </c>
       <c r="G46" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="15"/>
         <v>Joesph</v>
       </c>
       <c r="H46" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="16"/>
         <v>Joesph Sexton</v>
       </c>
       <c r="J46" t="s">
@@ -11409,19 +11534,19 @@
         <v>168</v>
       </c>
       <c r="E47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="13"/>
         <v>7</v>
       </c>
       <c r="F47" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="14"/>
         <v>Madden</v>
       </c>
       <c r="G47" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="15"/>
         <v>Peter</v>
       </c>
       <c r="H47" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="16"/>
         <v>Peter Madden</v>
       </c>
       <c r="J47" t="s">
@@ -11448,19 +11573,19 @@
         <v>169</v>
       </c>
       <c r="E48">
-        <f t="shared" si="0"/>
+        <f t="shared" si="13"/>
         <v>11</v>
       </c>
       <c r="F48" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="14"/>
         <v>Van de Ven</v>
       </c>
       <c r="G48" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="15"/>
         <v>Jan</v>
       </c>
       <c r="H48" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="16"/>
         <v>Jan Van de Ven</v>
       </c>
       <c r="J48" t="s">

</xml_diff>

<commit_message>
Stage 15 South added Signed-off-by: Gerry Mulvenna <git@movingwifi.com>
</commit_message>
<xml_diff>
--- a/europarl/europarl-ireland-2019.xlsx
+++ b/europarl/europarl-ireland-2019.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="14220" windowHeight="8580" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="14220" windowHeight="8580" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Candidates" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="261">
   <si>
     <t>Candidate</t>
   </si>
@@ -5161,7 +5161,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="S2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -7589,10 +7589,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG49"/>
+  <dimension ref="A1:AM49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7601,7 +7601,7 @@
     <col min="3" max="3" width="4.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>232</v>
       </c>
@@ -7650,8 +7650,11 @@
       <c r="AD1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AF1" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -7662,98 +7665,107 @@
         <v>118444</v>
       </c>
       <c r="E2">
-        <f t="shared" ref="E2:E24" si="0">IF(ISBLANK(F2),-D2,F2-D2)</f>
+        <f>IF(ISBLANK(F2),-D2,F2-D2)</f>
         <v>45</v>
       </c>
       <c r="F2" s="1">
         <v>118489</v>
       </c>
       <c r="G2">
-        <f t="shared" ref="G2:G24" si="1">IF(ISBLANK(H2),-F2,H2-F2)</f>
+        <f>IF(ISBLANK(H2),-F2,H2-F2)</f>
         <v>186</v>
       </c>
       <c r="H2" s="1">
         <v>118675</v>
       </c>
       <c r="I2">
-        <f t="shared" ref="I2:I24" si="2">IF(ISBLANK(J2),-H2,J2-H2)</f>
+        <f>IF(ISBLANK(J2),-H2,J2-H2)</f>
         <v>98</v>
       </c>
       <c r="J2" s="1">
         <v>118773</v>
       </c>
       <c r="K2">
-        <f t="shared" ref="K2:K24" si="3">IF(ISBLANK(L2),-J2,L2-J2)</f>
+        <f>IF(ISBLANK(L2),-J2,L2-J2)</f>
         <v>350</v>
       </c>
       <c r="L2" s="1">
         <v>119123</v>
       </c>
       <c r="M2">
-        <f t="shared" ref="M2:M24" si="4">IF(ISBLANK(N2),-L2,N2-L2)</f>
+        <f>IF(ISBLANK(N2),-L2,N2-L2)</f>
         <v>257</v>
       </c>
       <c r="N2" s="1">
         <v>119380</v>
       </c>
       <c r="O2">
-        <f t="shared" ref="O2:O24" si="5">IF(ISBLANK(P2),-N2,P2-N2)</f>
+        <f>IF(ISBLANK(P2),-N2,P2-N2)</f>
         <v>165</v>
       </c>
       <c r="P2" s="1">
         <v>119545</v>
       </c>
       <c r="Q2">
-        <f t="shared" ref="Q2:Q24" si="6">IF(ISBLANK(R2),-P2,R2-P2)</f>
+        <f>IF(ISBLANK(R2),-P2,R2-P2)</f>
         <v>170</v>
       </c>
       <c r="R2" s="1">
         <v>119715</v>
       </c>
       <c r="S2">
-        <f t="shared" ref="S2:S24" si="7">IF(ISBLANK(T2),-R2,T2-R2)</f>
+        <f>IF(ISBLANK(T2),-R2,T2-R2)</f>
         <v>168</v>
       </c>
       <c r="T2" s="1">
         <v>119883</v>
       </c>
       <c r="U2">
-        <f t="shared" ref="U2:U24" si="8">IF(ISBLANK(V2),-T2,V2-T2)</f>
+        <f>IF(ISBLANK(V2),-T2,V2-T2)</f>
         <v>0</v>
       </c>
       <c r="V2" s="1">
         <v>119883</v>
       </c>
       <c r="W2">
-        <f t="shared" ref="W2:W24" si="9">IF(ISBLANK(X2),-V2,X2-V2)</f>
+        <f>IF(ISBLANK(X2),-V2,X2-V2)</f>
         <v>0</v>
       </c>
       <c r="X2" s="1">
         <v>119883</v>
       </c>
       <c r="Y2">
-        <f t="shared" ref="Y2:Y24" si="10">IF(ISBLANK(Z2),-X2,Z2-X2)</f>
+        <f>IF(ISBLANK(Z2),-X2,Z2-X2)</f>
         <v>0</v>
       </c>
       <c r="Z2" s="1">
         <v>119883</v>
       </c>
       <c r="AA2">
-        <f t="shared" ref="AA2:AA24" si="11">IF(ISBLANK(AB2),-Z2,AB2-Z2)</f>
+        <f>IF(ISBLANK(AB2),-Z2,AB2-Z2)</f>
         <v>0</v>
       </c>
       <c r="AB2" s="1">
         <v>119883</v>
       </c>
       <c r="AC2">
-        <f t="shared" ref="AC2:AC24" si="12">IF(ISBLANK(AD2),-AB2,AD2-AB2)</f>
+        <f>IF(ISBLANK(AD2),-AB2,AD2-AB2)</f>
         <v>0</v>
       </c>
       <c r="AD2" s="1">
         <v>119883</v>
       </c>
-    </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE2">
+        <f>IF(ISBLANK(AF2),-AD2,AF2-AD2)</f>
+        <v>0</v>
+      </c>
+      <c r="AF2" s="1">
+        <v>119883</v>
+      </c>
+      <c r="AG2" s="1"/>
+      <c r="AH2" s="1"/>
+    </row>
+    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -7764,98 +7776,112 @@
         <v>84083</v>
       </c>
       <c r="E3">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F3),-D3,F3-D3)</f>
         <v>23</v>
       </c>
       <c r="F3" s="1">
         <v>84106</v>
       </c>
       <c r="G3">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H3),-F3,H3-F3)</f>
         <v>58</v>
       </c>
       <c r="H3" s="1">
         <v>84164</v>
       </c>
       <c r="I3">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J3),-H3,J3-H3)</f>
         <v>74</v>
       </c>
       <c r="J3" s="1">
         <v>84238</v>
       </c>
       <c r="K3">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L3),-J3,L3-J3)</f>
         <v>150</v>
       </c>
       <c r="L3" s="1">
         <v>84388</v>
       </c>
       <c r="M3">
-        <f t="shared" si="4"/>
+        <f>IF(ISBLANK(N3),-L3,N3-L3)</f>
         <v>171</v>
       </c>
       <c r="N3" s="1">
         <v>84559</v>
       </c>
       <c r="O3">
-        <f t="shared" si="5"/>
+        <f>IF(ISBLANK(P3),-N3,P3-N3)</f>
         <v>95</v>
       </c>
       <c r="P3" s="1">
         <v>84654</v>
       </c>
       <c r="Q3">
-        <f t="shared" si="6"/>
+        <f>IF(ISBLANK(R3),-P3,R3-P3)</f>
         <v>187</v>
       </c>
       <c r="R3" s="1">
         <v>84841</v>
       </c>
       <c r="S3">
-        <f t="shared" si="7"/>
+        <f>IF(ISBLANK(T3),-R3,T3-R3)</f>
         <v>130</v>
       </c>
       <c r="T3" s="1">
         <v>84971</v>
       </c>
       <c r="U3">
-        <f t="shared" si="8"/>
+        <f>IF(ISBLANK(V3),-T3,V3-T3)</f>
         <v>480</v>
       </c>
       <c r="V3" s="1">
         <v>85451</v>
       </c>
       <c r="W3">
-        <f t="shared" si="9"/>
+        <f>IF(ISBLANK(X3),-V3,X3-V3)</f>
         <v>575</v>
       </c>
       <c r="X3" s="1">
         <v>86026</v>
       </c>
       <c r="Y3">
-        <f t="shared" si="10"/>
+        <f>IF(ISBLANK(Z3),-X3,Z3-X3)</f>
         <v>1010</v>
       </c>
       <c r="Z3" s="1">
         <v>87036</v>
       </c>
       <c r="AA3">
-        <f t="shared" si="11"/>
+        <f>IF(ISBLANK(AB3),-Z3,AB3-Z3)</f>
         <v>928</v>
       </c>
       <c r="AB3" s="1">
         <v>87964</v>
       </c>
       <c r="AC3">
-        <f t="shared" si="12"/>
+        <f>IF(ISBLANK(AD3),-AB3,AD3-AB3)</f>
         <v>637</v>
       </c>
       <c r="AD3" s="1">
         <v>88601</v>
       </c>
-    </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE3">
+        <f>IF(ISBLANK(AF3),-AD3,AF3-AD3)</f>
+        <v>435</v>
+      </c>
+      <c r="AF3" s="1">
+        <v>89036</v>
+      </c>
+      <c r="AG3" s="1"/>
+      <c r="AH3" s="1"/>
+      <c r="AI3" s="1"/>
+      <c r="AJ3" s="1"/>
+      <c r="AK3" s="1"/>
+      <c r="AL3" s="1"/>
+      <c r="AM3" s="1"/>
+    </row>
+    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -7866,98 +7892,112 @@
         <v>81741</v>
       </c>
       <c r="E4">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F4),-D4,F4-D4)</f>
         <v>253</v>
       </c>
       <c r="F4" s="1">
         <v>81994</v>
       </c>
       <c r="G4">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H4),-F4,H4-F4)</f>
         <v>130</v>
       </c>
       <c r="H4" s="1">
         <v>82124</v>
       </c>
       <c r="I4">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J4),-H4,J4-H4)</f>
         <v>211</v>
       </c>
       <c r="J4" s="1">
         <v>82335</v>
       </c>
       <c r="K4">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L4),-J4,L4-J4)</f>
         <v>323</v>
       </c>
       <c r="L4" s="1">
         <v>82658</v>
       </c>
       <c r="M4">
-        <f t="shared" si="4"/>
+        <f>IF(ISBLANK(N4),-L4,N4-L4)</f>
         <v>206</v>
       </c>
       <c r="N4" s="1">
         <v>82864</v>
       </c>
       <c r="O4">
-        <f t="shared" si="5"/>
+        <f>IF(ISBLANK(P4),-N4,P4-N4)</f>
         <v>556</v>
       </c>
       <c r="P4" s="1">
         <v>83420</v>
       </c>
       <c r="Q4">
-        <f t="shared" si="6"/>
+        <f>IF(ISBLANK(R4),-P4,R4-P4)</f>
         <v>351</v>
       </c>
       <c r="R4" s="1">
         <v>83771</v>
       </c>
       <c r="S4">
-        <f t="shared" si="7"/>
+        <f>IF(ISBLANK(T4),-R4,T4-R4)</f>
         <v>217</v>
       </c>
       <c r="T4" s="1">
         <v>83988</v>
       </c>
       <c r="U4">
-        <f t="shared" si="8"/>
+        <f>IF(ISBLANK(V4),-T4,V4-T4)</f>
         <v>247</v>
       </c>
       <c r="V4" s="1">
         <v>84235</v>
       </c>
       <c r="W4">
-        <f t="shared" si="9"/>
+        <f>IF(ISBLANK(X4),-V4,X4-V4)</f>
         <v>1001</v>
       </c>
       <c r="X4" s="1">
         <v>85236</v>
       </c>
       <c r="Y4">
-        <f t="shared" si="10"/>
+        <f>IF(ISBLANK(Z4),-X4,Z4-X4)</f>
         <v>2333</v>
       </c>
       <c r="Z4" s="1">
         <v>87569</v>
       </c>
       <c r="AA4">
-        <f t="shared" si="11"/>
+        <f>IF(ISBLANK(AB4),-Z4,AB4-Z4)</f>
         <v>1190</v>
       </c>
       <c r="AB4" s="1">
         <v>88759</v>
       </c>
       <c r="AC4">
-        <f t="shared" si="12"/>
+        <f>IF(ISBLANK(AD4),-AB4,AD4-AB4)</f>
         <v>1476</v>
       </c>
       <c r="AD4" s="1">
         <v>90235</v>
       </c>
-    </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE4">
+        <f>IF(ISBLANK(AF4),-AD4,AF4-AD4)</f>
+        <v>5545</v>
+      </c>
+      <c r="AF4" s="1">
+        <v>95780</v>
+      </c>
+      <c r="AG4" s="1"/>
+      <c r="AH4" s="1"/>
+      <c r="AI4" s="1"/>
+      <c r="AJ4" s="1"/>
+      <c r="AK4" s="1"/>
+      <c r="AL4" s="1"/>
+      <c r="AM4" s="1"/>
+    </row>
+    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -7968,98 +8008,112 @@
         <v>79072</v>
       </c>
       <c r="E5">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F5),-D5,F5-D5)</f>
         <v>68</v>
       </c>
       <c r="F5" s="1">
         <v>79140</v>
       </c>
       <c r="G5">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H5),-F5,H5-F5)</f>
         <v>142</v>
       </c>
       <c r="H5" s="1">
         <v>79282</v>
       </c>
       <c r="I5">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J5),-H5,J5-H5)</f>
         <v>105</v>
       </c>
       <c r="J5" s="1">
         <v>79387</v>
       </c>
       <c r="K5">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L5),-J5,L5-J5)</f>
         <v>186</v>
       </c>
       <c r="L5" s="1">
         <v>79573</v>
       </c>
       <c r="M5">
-        <f t="shared" si="4"/>
+        <f>IF(ISBLANK(N5),-L5,N5-L5)</f>
         <v>168</v>
       </c>
       <c r="N5" s="1">
         <v>79741</v>
       </c>
       <c r="O5">
-        <f t="shared" si="5"/>
+        <f>IF(ISBLANK(P5),-N5,P5-N5)</f>
         <v>204</v>
       </c>
       <c r="P5" s="1">
         <v>79945</v>
       </c>
       <c r="Q5">
-        <f t="shared" si="6"/>
+        <f>IF(ISBLANK(R5),-P5,R5-P5)</f>
         <v>305</v>
       </c>
       <c r="R5" s="1">
         <v>80250</v>
       </c>
       <c r="S5">
-        <f t="shared" si="7"/>
+        <f>IF(ISBLANK(T5),-R5,T5-R5)</f>
         <v>127</v>
       </c>
       <c r="T5" s="1">
         <v>80377</v>
       </c>
       <c r="U5">
-        <f t="shared" si="8"/>
+        <f>IF(ISBLANK(V5),-T5,V5-T5)</f>
         <v>446</v>
       </c>
       <c r="V5" s="1">
         <v>80823</v>
       </c>
       <c r="W5">
-        <f t="shared" si="9"/>
+        <f>IF(ISBLANK(X5),-V5,X5-V5)</f>
         <v>991</v>
       </c>
       <c r="X5" s="1">
         <v>81814</v>
       </c>
       <c r="Y5">
-        <f t="shared" si="10"/>
+        <f>IF(ISBLANK(Z5),-X5,Z5-X5)</f>
         <v>1119</v>
       </c>
       <c r="Z5" s="1">
         <v>82933</v>
       </c>
       <c r="AA5">
-        <f t="shared" si="11"/>
+        <f>IF(ISBLANK(AB5),-Z5,AB5-Z5)</f>
         <v>958</v>
       </c>
       <c r="AB5" s="1">
         <v>83891</v>
       </c>
       <c r="AC5">
-        <f t="shared" si="12"/>
+        <f>IF(ISBLANK(AD5),-AB5,AD5-AB5)</f>
         <v>1108</v>
       </c>
       <c r="AD5" s="1">
         <v>84999</v>
       </c>
-    </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE5">
+        <f>IF(ISBLANK(AF5),-AD5,AF5-AD5)</f>
+        <v>2323</v>
+      </c>
+      <c r="AF5" s="1">
+        <v>87322</v>
+      </c>
+      <c r="AG5" s="1"/>
+      <c r="AH5" s="1"/>
+      <c r="AI5" s="1"/>
+      <c r="AJ5" s="1"/>
+      <c r="AK5" s="1"/>
+      <c r="AL5" s="1"/>
+      <c r="AM5" s="1"/>
+    </row>
+    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -8070,98 +8124,112 @@
         <v>75946</v>
       </c>
       <c r="E6">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F6),-D6,F6-D6)</f>
         <v>100</v>
       </c>
       <c r="F6" s="1">
         <v>76046</v>
       </c>
       <c r="G6">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H6),-F6,H6-F6)</f>
         <v>201</v>
       </c>
       <c r="H6" s="1">
         <v>76247</v>
       </c>
       <c r="I6">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J6),-H6,J6-H6)</f>
         <v>126</v>
       </c>
       <c r="J6" s="1">
         <v>76373</v>
       </c>
       <c r="K6">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L6),-J6,L6-J6)</f>
         <v>272</v>
       </c>
       <c r="L6" s="1">
         <v>76645</v>
       </c>
       <c r="M6">
-        <f t="shared" si="4"/>
+        <f>IF(ISBLANK(N6),-L6,N6-L6)</f>
         <v>74</v>
       </c>
       <c r="N6" s="1">
         <v>76719</v>
       </c>
       <c r="O6">
-        <f t="shared" si="5"/>
+        <f>IF(ISBLANK(P6),-N6,P6-N6)</f>
         <v>301</v>
       </c>
       <c r="P6" s="1">
         <v>77020</v>
       </c>
       <c r="Q6">
-        <f t="shared" si="6"/>
+        <f>IF(ISBLANK(R6),-P6,R6-P6)</f>
         <v>283</v>
       </c>
       <c r="R6" s="1">
         <v>77303</v>
       </c>
       <c r="S6">
-        <f t="shared" si="7"/>
+        <f>IF(ISBLANK(T6),-R6,T6-R6)</f>
         <v>112</v>
       </c>
       <c r="T6" s="1">
         <v>77415</v>
       </c>
       <c r="U6">
-        <f t="shared" si="8"/>
+        <f>IF(ISBLANK(V6),-T6,V6-T6)</f>
         <v>339</v>
       </c>
       <c r="V6" s="1">
         <v>77754</v>
       </c>
       <c r="W6">
-        <f t="shared" si="9"/>
+        <f>IF(ISBLANK(X6),-V6,X6-V6)</f>
         <v>1066</v>
       </c>
       <c r="X6" s="1">
         <v>78820</v>
       </c>
       <c r="Y6">
-        <f t="shared" si="10"/>
+        <f>IF(ISBLANK(Z6),-X6,Z6-X6)</f>
         <v>1295</v>
       </c>
       <c r="Z6" s="1">
         <v>80115</v>
       </c>
       <c r="AA6">
-        <f t="shared" si="11"/>
+        <f>IF(ISBLANK(AB6),-Z6,AB6-Z6)</f>
         <v>593</v>
       </c>
       <c r="AB6" s="1">
         <v>80708</v>
       </c>
       <c r="AC6">
-        <f t="shared" si="12"/>
+        <f>IF(ISBLANK(AD6),-AB6,AD6-AB6)</f>
         <v>1290</v>
       </c>
       <c r="AD6" s="1">
         <v>81998</v>
       </c>
-    </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE6">
+        <f>IF(ISBLANK(AF6),-AD6,AF6-AD6)</f>
+        <v>2743</v>
+      </c>
+      <c r="AF6" s="1">
+        <v>84741</v>
+      </c>
+      <c r="AG6" s="1"/>
+      <c r="AH6" s="1"/>
+      <c r="AI6" s="1"/>
+      <c r="AJ6" s="1"/>
+      <c r="AK6" s="1"/>
+      <c r="AL6" s="1"/>
+      <c r="AM6" s="1"/>
+    </row>
+    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -8172,98 +8240,112 @@
         <v>69166</v>
       </c>
       <c r="E7">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F7),-D7,F7-D7)</f>
         <v>35</v>
       </c>
       <c r="F7" s="1">
         <v>69201</v>
       </c>
       <c r="G7">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H7),-F7,H7-F7)</f>
         <v>71</v>
       </c>
       <c r="H7" s="1">
         <v>69272</v>
       </c>
       <c r="I7">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J7),-H7,J7-H7)</f>
         <v>44</v>
       </c>
       <c r="J7" s="1">
         <v>69316</v>
       </c>
       <c r="K7">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L7),-J7,L7-J7)</f>
         <v>66</v>
       </c>
       <c r="L7" s="1">
         <v>69382</v>
       </c>
       <c r="M7">
-        <f t="shared" si="4"/>
+        <f>IF(ISBLANK(N7),-L7,N7-L7)</f>
         <v>129</v>
       </c>
       <c r="N7" s="1">
         <v>69511</v>
       </c>
       <c r="O7">
-        <f t="shared" si="5"/>
+        <f>IF(ISBLANK(P7),-N7,P7-N7)</f>
         <v>45</v>
       </c>
       <c r="P7" s="1">
         <v>69556</v>
       </c>
       <c r="Q7">
-        <f t="shared" si="6"/>
+        <f>IF(ISBLANK(R7),-P7,R7-P7)</f>
         <v>116</v>
       </c>
       <c r="R7" s="1">
         <v>69672</v>
       </c>
       <c r="S7">
-        <f t="shared" si="7"/>
+        <f>IF(ISBLANK(T7),-R7,T7-R7)</f>
         <v>1226</v>
       </c>
       <c r="T7" s="1">
         <v>70898</v>
       </c>
       <c r="U7">
-        <f t="shared" si="8"/>
+        <f>IF(ISBLANK(V7),-T7,V7-T7)</f>
         <v>270</v>
       </c>
       <c r="V7" s="1">
         <v>71168</v>
       </c>
       <c r="W7">
-        <f t="shared" si="9"/>
+        <f>IF(ISBLANK(X7),-V7,X7-V7)</f>
         <v>674</v>
       </c>
       <c r="X7" s="1">
         <v>71842</v>
       </c>
       <c r="Y7">
-        <f t="shared" si="10"/>
+        <f>IF(ISBLANK(Z7),-X7,Z7-X7)</f>
         <v>291</v>
       </c>
       <c r="Z7" s="1">
         <v>72133</v>
       </c>
       <c r="AA7">
-        <f t="shared" si="11"/>
+        <f>IF(ISBLANK(AB7),-Z7,AB7-Z7)</f>
         <v>720</v>
       </c>
       <c r="AB7" s="1">
         <v>72853</v>
       </c>
       <c r="AC7">
-        <f t="shared" si="12"/>
+        <f>IF(ISBLANK(AD7),-AB7,AD7-AB7)</f>
         <v>929</v>
       </c>
       <c r="AD7" s="1">
         <v>73782</v>
       </c>
-    </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE7">
+        <f>IF(ISBLANK(AF7),-AD7,AF7-AD7)</f>
+        <v>588</v>
+      </c>
+      <c r="AF7" s="1">
+        <v>74370</v>
+      </c>
+      <c r="AG7" s="1"/>
+      <c r="AH7" s="1"/>
+      <c r="AI7" s="1"/>
+      <c r="AJ7" s="1"/>
+      <c r="AK7" s="1"/>
+      <c r="AL7" s="1"/>
+      <c r="AM7" s="1"/>
+    </row>
+    <row r="8" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -8274,98 +8356,112 @@
         <v>64605</v>
       </c>
       <c r="E8">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F8),-D8,F8-D8)</f>
         <v>26</v>
       </c>
       <c r="F8" s="1">
         <v>64631</v>
       </c>
       <c r="G8">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H8),-F8,H8-F8)</f>
         <v>61</v>
       </c>
       <c r="H8" s="1">
         <v>64692</v>
       </c>
       <c r="I8">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J8),-H8,J8-H8)</f>
         <v>71</v>
       </c>
       <c r="J8" s="1">
         <v>64763</v>
       </c>
       <c r="K8">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L8),-J8,L8-J8)</f>
         <v>136</v>
       </c>
       <c r="L8" s="1">
         <v>64899</v>
       </c>
       <c r="M8">
-        <f t="shared" si="4"/>
+        <f>IF(ISBLANK(N8),-L8,N8-L8)</f>
         <v>106</v>
       </c>
       <c r="N8" s="1">
         <v>65005</v>
       </c>
       <c r="O8">
-        <f t="shared" si="5"/>
+        <f>IF(ISBLANK(P8),-N8,P8-N8)</f>
         <v>110</v>
       </c>
       <c r="P8" s="1">
         <v>65115</v>
       </c>
       <c r="Q8">
-        <f t="shared" si="6"/>
+        <f>IF(ISBLANK(R8),-P8,R8-P8)</f>
         <v>137</v>
       </c>
       <c r="R8" s="1">
         <v>65252</v>
       </c>
       <c r="S8">
-        <f t="shared" si="7"/>
+        <f>IF(ISBLANK(T8),-R8,T8-R8)</f>
         <v>306</v>
       </c>
       <c r="T8" s="1">
         <v>65558</v>
       </c>
       <c r="U8">
-        <f t="shared" si="8"/>
+        <f>IF(ISBLANK(V8),-T8,V8-T8)</f>
         <v>491</v>
       </c>
       <c r="V8" s="1">
         <v>66049</v>
       </c>
       <c r="W8">
-        <f t="shared" si="9"/>
+        <f>IF(ISBLANK(X8),-V8,X8-V8)</f>
         <v>683</v>
       </c>
       <c r="X8" s="1">
         <v>66732</v>
       </c>
       <c r="Y8">
-        <f t="shared" si="10"/>
+        <f>IF(ISBLANK(Z8),-X8,Z8-X8)</f>
         <v>542</v>
       </c>
       <c r="Z8" s="1">
         <v>67274</v>
       </c>
       <c r="AA8">
-        <f t="shared" si="11"/>
+        <f>IF(ISBLANK(AB8),-Z8,AB8-Z8)</f>
         <v>622</v>
       </c>
       <c r="AB8" s="1">
         <v>67896</v>
       </c>
       <c r="AC8">
-        <f t="shared" si="12"/>
+        <f>IF(ISBLANK(AD8),-AB8,AD8-AB8)</f>
         <v>1194</v>
       </c>
       <c r="AD8" s="1">
         <v>69090</v>
       </c>
-    </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE8">
+        <f>IF(ISBLANK(AF8),-AD8,AF8-AD8)</f>
+        <v>470</v>
+      </c>
+      <c r="AF8" s="1">
+        <v>69560</v>
+      </c>
+      <c r="AG8" s="1"/>
+      <c r="AH8" s="1"/>
+      <c r="AI8" s="1"/>
+      <c r="AJ8" s="1"/>
+      <c r="AK8" s="1"/>
+      <c r="AL8" s="1"/>
+      <c r="AM8" s="1"/>
+    </row>
+    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -8376,98 +8472,112 @@
         <v>38738</v>
       </c>
       <c r="E9">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F9),-D9,F9-D9)</f>
         <v>17</v>
       </c>
       <c r="F9" s="1">
         <v>38755</v>
       </c>
       <c r="G9">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H9),-F9,H9-F9)</f>
         <v>33</v>
       </c>
       <c r="H9" s="1">
         <v>38788</v>
       </c>
       <c r="I9">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J9),-H9,J9-H9)</f>
         <v>16</v>
       </c>
       <c r="J9" s="1">
         <v>38804</v>
       </c>
       <c r="K9">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L9),-J9,L9-J9)</f>
         <v>38</v>
       </c>
       <c r="L9" s="1">
         <v>38842</v>
       </c>
       <c r="M9">
-        <f t="shared" si="4"/>
+        <f>IF(ISBLANK(N9),-L9,N9-L9)</f>
         <v>84</v>
       </c>
       <c r="N9" s="1">
         <v>38926</v>
       </c>
       <c r="O9">
-        <f t="shared" si="5"/>
+        <f>IF(ISBLANK(P9),-N9,P9-N9)</f>
         <v>24</v>
       </c>
       <c r="P9" s="1">
         <v>38950</v>
       </c>
       <c r="Q9">
-        <f t="shared" si="6"/>
+        <f>IF(ISBLANK(R9),-P9,R9-P9)</f>
         <v>46</v>
       </c>
       <c r="R9" s="1">
         <v>38996</v>
       </c>
       <c r="S9">
-        <f t="shared" si="7"/>
+        <f>IF(ISBLANK(T9),-R9,T9-R9)</f>
         <v>298</v>
       </c>
       <c r="T9" s="1">
         <v>39294</v>
       </c>
       <c r="U9">
-        <f t="shared" si="8"/>
+        <f>IF(ISBLANK(V9),-T9,V9-T9)</f>
         <v>135</v>
       </c>
       <c r="V9" s="1">
         <v>39429</v>
       </c>
       <c r="W9">
-        <f t="shared" si="9"/>
+        <f>IF(ISBLANK(X9),-V9,X9-V9)</f>
         <v>426</v>
       </c>
       <c r="X9" s="1">
         <v>39855</v>
       </c>
       <c r="Y9">
-        <f t="shared" si="10"/>
+        <f>IF(ISBLANK(Z9),-X9,Z9-X9)</f>
         <v>159</v>
       </c>
       <c r="Z9" s="1">
         <v>40014</v>
       </c>
       <c r="AA9">
-        <f t="shared" si="11"/>
+        <f>IF(ISBLANK(AB9),-Z9,AB9-Z9)</f>
         <v>572</v>
       </c>
       <c r="AB9" s="1">
         <v>40586</v>
       </c>
       <c r="AC9">
-        <f t="shared" si="12"/>
+        <f>IF(ISBLANK(AD9),-AB9,AD9-AB9)</f>
         <v>483</v>
       </c>
       <c r="AD9" s="1">
         <v>41069</v>
       </c>
-    </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE9">
+        <f>IF(ISBLANK(AF9),-AD9,AF9-AD9)</f>
+        <v>347</v>
+      </c>
+      <c r="AF9" s="1">
+        <v>41416</v>
+      </c>
+      <c r="AG9" s="1"/>
+      <c r="AH9" s="1"/>
+      <c r="AI9" s="1"/>
+      <c r="AJ9" s="1"/>
+      <c r="AK9" s="1"/>
+      <c r="AL9" s="1"/>
+      <c r="AM9" s="1"/>
+    </row>
+    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -8478,98 +8588,112 @@
         <v>22075</v>
       </c>
       <c r="E10">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F10),-D10,F10-D10)</f>
         <v>38</v>
       </c>
       <c r="F10" s="1">
         <v>22113</v>
       </c>
       <c r="G10">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H10),-F10,H10-F10)</f>
         <v>80</v>
       </c>
       <c r="H10" s="1">
         <v>22193</v>
       </c>
       <c r="I10">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J10),-H10,J10-H10)</f>
         <v>58</v>
       </c>
       <c r="J10" s="1">
         <v>22251</v>
       </c>
       <c r="K10">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L10),-J10,L10-J10)</f>
         <v>70</v>
       </c>
       <c r="L10" s="1">
         <v>22321</v>
       </c>
       <c r="M10">
-        <f t="shared" si="4"/>
+        <f>IF(ISBLANK(N10),-L10,N10-L10)</f>
         <v>62</v>
       </c>
       <c r="N10" s="1">
         <v>22383</v>
       </c>
       <c r="O10">
-        <f t="shared" si="5"/>
+        <f>IF(ISBLANK(P10),-N10,P10-N10)</f>
         <v>70</v>
       </c>
       <c r="P10" s="1">
         <v>22453</v>
       </c>
       <c r="Q10">
-        <f t="shared" si="6"/>
+        <f>IF(ISBLANK(R10),-P10,R10-P10)</f>
         <v>173</v>
       </c>
       <c r="R10" s="1">
         <v>22626</v>
       </c>
       <c r="S10">
-        <f t="shared" si="7"/>
+        <f>IF(ISBLANK(T10),-R10,T10-R10)</f>
         <v>74</v>
       </c>
       <c r="T10" s="1">
         <v>22700</v>
       </c>
       <c r="U10">
-        <f t="shared" si="8"/>
+        <f>IF(ISBLANK(V10),-T10,V10-T10)</f>
         <v>193</v>
       </c>
       <c r="V10" s="1">
         <v>22893</v>
       </c>
       <c r="W10">
-        <f t="shared" si="9"/>
+        <f>IF(ISBLANK(X10),-V10,X10-V10)</f>
         <v>626</v>
       </c>
       <c r="X10" s="1">
         <v>23519</v>
       </c>
       <c r="Y10">
-        <f t="shared" si="10"/>
+        <f>IF(ISBLANK(Z10),-X10,Z10-X10)</f>
         <v>330</v>
       </c>
       <c r="Z10" s="1">
         <v>23849</v>
       </c>
       <c r="AA10">
-        <f t="shared" si="11"/>
+        <f>IF(ISBLANK(AB10),-Z10,AB10-Z10)</f>
         <v>483</v>
       </c>
       <c r="AB10" s="1">
         <v>24332</v>
       </c>
       <c r="AC10">
-        <f t="shared" si="12"/>
+        <f>IF(ISBLANK(AD10),-AB10,AD10-AB10)</f>
         <v>600</v>
       </c>
       <c r="AD10" s="1">
         <v>24932</v>
       </c>
-    </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE10">
+        <f>IF(ISBLANK(AF10),-AD10,AF10-AD10)</f>
+        <v>1026</v>
+      </c>
+      <c r="AF10" s="1">
+        <v>25958</v>
+      </c>
+      <c r="AG10" s="1"/>
+      <c r="AH10" s="1"/>
+      <c r="AI10" s="1"/>
+      <c r="AJ10" s="1"/>
+      <c r="AK10" s="1"/>
+      <c r="AL10" s="1"/>
+      <c r="AM10" s="1"/>
+    </row>
+    <row r="11" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -8580,98 +8704,112 @@
         <v>14802</v>
       </c>
       <c r="E11">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F11),-D11,F11-D11)</f>
         <v>156</v>
       </c>
       <c r="F11" s="1">
         <v>14958</v>
       </c>
       <c r="G11">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H11),-F11,H11-F11)</f>
         <v>51</v>
       </c>
       <c r="H11" s="1">
         <v>15009</v>
       </c>
       <c r="I11">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J11),-H11,J11-H11)</f>
         <v>198</v>
       </c>
       <c r="J11" s="1">
         <v>15207</v>
       </c>
       <c r="K11">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L11),-J11,L11-J11)</f>
         <v>146</v>
       </c>
       <c r="L11" s="1">
         <v>15353</v>
       </c>
       <c r="M11">
-        <f t="shared" si="4"/>
+        <f>IF(ISBLANK(N11),-L11,N11-L11)</f>
         <v>41</v>
       </c>
       <c r="N11" s="1">
         <v>15394</v>
       </c>
       <c r="O11">
-        <f t="shared" si="5"/>
+        <f>IF(ISBLANK(P11),-N11,P11-N11)</f>
         <v>392</v>
       </c>
       <c r="P11" s="1">
         <v>15786</v>
       </c>
       <c r="Q11">
-        <f t="shared" si="6"/>
+        <f>IF(ISBLANK(R11),-P11,R11-P11)</f>
         <v>321</v>
       </c>
       <c r="R11" s="1">
         <v>16107</v>
       </c>
       <c r="S11">
-        <f t="shared" si="7"/>
+        <f>IF(ISBLANK(T11),-R11,T11-R11)</f>
         <v>101</v>
       </c>
       <c r="T11" s="1">
         <v>16208</v>
       </c>
       <c r="U11">
-        <f t="shared" si="8"/>
+        <f>IF(ISBLANK(V11),-T11,V11-T11)</f>
         <v>170</v>
       </c>
       <c r="V11" s="1">
         <v>16378</v>
       </c>
       <c r="W11">
-        <f t="shared" si="9"/>
+        <f>IF(ISBLANK(X11),-V11,X11-V11)</f>
         <v>530</v>
       </c>
       <c r="X11" s="1">
         <v>16908</v>
       </c>
       <c r="Y11">
-        <f t="shared" si="10"/>
+        <f>IF(ISBLANK(Z11),-X11,Z11-X11)</f>
         <v>490</v>
       </c>
       <c r="Z11" s="1">
         <v>17398</v>
       </c>
       <c r="AA11">
-        <f t="shared" si="11"/>
+        <f>IF(ISBLANK(AB11),-Z11,AB11-Z11)</f>
         <v>329</v>
       </c>
       <c r="AB11" s="1">
         <v>17727</v>
       </c>
       <c r="AC11">
-        <f t="shared" si="12"/>
+        <f>IF(ISBLANK(AD11),-AB11,AD11-AB11)</f>
         <v>749</v>
       </c>
       <c r="AD11" s="1">
         <v>18476</v>
       </c>
-    </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE11">
+        <f>IF(ISBLANK(AF11),-AD11,AF11-AD11)</f>
+        <v>-18476</v>
+      </c>
+      <c r="AF11" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG11" s="1"/>
+      <c r="AH11" s="1"/>
+      <c r="AI11" s="1"/>
+      <c r="AJ11" s="1"/>
+      <c r="AK11" s="1"/>
+      <c r="AL11" s="1"/>
+      <c r="AM11" s="1"/>
+    </row>
+    <row r="12" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -8682,98 +8820,111 @@
         <v>10582</v>
       </c>
       <c r="E12">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F12),-D12,F12-D12)</f>
         <v>57</v>
       </c>
       <c r="F12" s="1">
         <v>10639</v>
       </c>
       <c r="G12">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H12),-F12,H12-F12)</f>
         <v>106</v>
       </c>
       <c r="H12" s="1">
         <v>10745</v>
       </c>
       <c r="I12">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J12),-H12,J12-H12)</f>
         <v>138</v>
       </c>
       <c r="J12" s="1">
         <v>10883</v>
       </c>
       <c r="K12">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L12),-J12,L12-J12)</f>
         <v>54</v>
       </c>
       <c r="L12" s="1">
         <v>10937</v>
       </c>
       <c r="M12">
-        <f t="shared" si="4"/>
+        <f>IF(ISBLANK(N12),-L12,N12-L12)</f>
         <v>300</v>
       </c>
       <c r="N12" s="1">
         <v>11237</v>
       </c>
       <c r="O12">
-        <f t="shared" si="5"/>
+        <f>IF(ISBLANK(P12),-N12,P12-N12)</f>
         <v>159</v>
       </c>
       <c r="P12" s="1">
         <v>11396</v>
       </c>
       <c r="Q12">
-        <f t="shared" si="6"/>
+        <f>IF(ISBLANK(R12),-P12,R12-P12)</f>
         <v>322</v>
       </c>
       <c r="R12" s="1">
         <v>11718</v>
       </c>
       <c r="S12">
-        <f t="shared" si="7"/>
+        <f>IF(ISBLANK(T12),-R12,T12-R12)</f>
         <v>908</v>
       </c>
       <c r="T12" s="1">
         <v>12626</v>
       </c>
       <c r="U12">
-        <f t="shared" si="8"/>
+        <f>IF(ISBLANK(V12),-T12,V12-T12)</f>
         <v>1585</v>
       </c>
       <c r="V12" s="1">
         <v>14211</v>
       </c>
       <c r="W12">
-        <f t="shared" si="9"/>
+        <f>IF(ISBLANK(X12),-V12,X12-V12)</f>
         <v>826</v>
       </c>
       <c r="X12" s="1">
         <v>15037</v>
       </c>
       <c r="Y12">
-        <f t="shared" si="10"/>
+        <f>IF(ISBLANK(Z12),-X12,Z12-X12)</f>
         <v>429</v>
       </c>
       <c r="Z12" s="1">
         <v>15466</v>
       </c>
       <c r="AA12">
-        <f t="shared" si="11"/>
+        <f>IF(ISBLANK(AB12),-Z12,AB12-Z12)</f>
         <v>1664</v>
       </c>
       <c r="AB12" s="1">
         <v>17130</v>
       </c>
       <c r="AC12">
-        <f t="shared" si="12"/>
+        <f>IF(ISBLANK(AD12),-AB12,AD12-AB12)</f>
         <v>-17130</v>
       </c>
       <c r="AD12" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE12">
+        <f>IF(ISBLANK(AF12),-AD12,AF12-AD12)</f>
+        <v>0</v>
+      </c>
+      <c r="AF12" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG12" s="1"/>
+      <c r="AH12" s="1"/>
+      <c r="AI12" s="1"/>
+      <c r="AJ12" s="1"/>
+      <c r="AK12" s="1"/>
+      <c r="AL12" s="1"/>
+    </row>
+    <row r="13" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -8784,98 +8935,109 @@
         <v>9823</v>
       </c>
       <c r="E13">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F13),-D13,F13-D13)</f>
         <v>37</v>
       </c>
       <c r="F13" s="1">
         <v>9860</v>
       </c>
       <c r="G13">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H13),-F13,H13-F13)</f>
         <v>76</v>
       </c>
       <c r="H13" s="1">
         <v>9936</v>
       </c>
       <c r="I13">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J13),-H13,J13-H13)</f>
         <v>54</v>
       </c>
       <c r="J13" s="1">
         <v>9990</v>
       </c>
       <c r="K13">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L13),-J13,L13-J13)</f>
         <v>184</v>
       </c>
       <c r="L13" s="1">
         <v>10174</v>
       </c>
       <c r="M13">
-        <f t="shared" si="4"/>
+        <f>IF(ISBLANK(N13),-L13,N13-L13)</f>
         <v>52</v>
       </c>
       <c r="N13" s="1">
         <v>10226</v>
       </c>
       <c r="O13">
-        <f t="shared" si="5"/>
+        <f>IF(ISBLANK(P13),-N13,P13-N13)</f>
         <v>168</v>
       </c>
       <c r="P13" s="1">
         <v>10394</v>
       </c>
       <c r="Q13">
-        <f t="shared" si="6"/>
+        <f>IF(ISBLANK(R13),-P13,R13-P13)</f>
         <v>214</v>
       </c>
       <c r="R13" s="1">
         <v>10608</v>
       </c>
       <c r="S13">
-        <f t="shared" si="7"/>
+        <f>IF(ISBLANK(T13),-R13,T13-R13)</f>
         <v>48</v>
       </c>
       <c r="T13" s="1">
         <v>10656</v>
       </c>
       <c r="U13">
-        <f t="shared" si="8"/>
+        <f>IF(ISBLANK(V13),-T13,V13-T13)</f>
         <v>286</v>
       </c>
       <c r="V13" s="1">
         <v>10942</v>
       </c>
       <c r="W13">
-        <f t="shared" si="9"/>
+        <f>IF(ISBLANK(X13),-V13,X13-V13)</f>
         <v>208</v>
       </c>
       <c r="X13" s="1">
         <v>11150</v>
       </c>
       <c r="Y13">
-        <f t="shared" si="10"/>
+        <f>IF(ISBLANK(Z13),-X13,Z13-X13)</f>
         <v>-11150</v>
       </c>
       <c r="Z13" s="1">
         <v>0</v>
       </c>
       <c r="AA13">
-        <f t="shared" si="11"/>
+        <f>IF(ISBLANK(AB13),-Z13,AB13-Z13)</f>
         <v>0</v>
       </c>
       <c r="AB13" s="1">
         <v>0</v>
       </c>
       <c r="AC13">
-        <f t="shared" si="12"/>
+        <f>IF(ISBLANK(AD13),-AB13,AD13-AB13)</f>
         <v>0</v>
       </c>
       <c r="AD13" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE13">
+        <f>IF(ISBLANK(AF13),-AD13,AF13-AD13)</f>
+        <v>0</v>
+      </c>
+      <c r="AF13" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG13" s="1"/>
+      <c r="AH13" s="1"/>
+      <c r="AI13" s="1"/>
+      <c r="AJ13" s="1"/>
+    </row>
+    <row r="14" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -8886,98 +9048,110 @@
         <v>9423</v>
       </c>
       <c r="E14">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F14),-D14,F14-D14)</f>
         <v>32</v>
       </c>
       <c r="F14" s="1">
         <v>9455</v>
       </c>
       <c r="G14">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H14),-F14,H14-F14)</f>
         <v>325</v>
       </c>
       <c r="H14" s="1">
         <v>9780</v>
       </c>
       <c r="I14">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J14),-H14,J14-H14)</f>
         <v>75</v>
       </c>
       <c r="J14" s="1">
         <v>9855</v>
       </c>
       <c r="K14">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L14),-J14,L14-J14)</f>
         <v>114</v>
       </c>
       <c r="L14" s="1">
         <v>9969</v>
       </c>
       <c r="M14">
-        <f t="shared" si="4"/>
+        <f>IF(ISBLANK(N14),-L14,N14-L14)</f>
         <v>280</v>
       </c>
       <c r="N14" s="1">
         <v>10249</v>
       </c>
       <c r="O14">
-        <f t="shared" si="5"/>
+        <f>IF(ISBLANK(P14),-N14,P14-N14)</f>
         <v>78</v>
       </c>
       <c r="P14" s="1">
         <v>10327</v>
       </c>
       <c r="Q14">
-        <f t="shared" si="6"/>
+        <f>IF(ISBLANK(R14),-P14,R14-P14)</f>
         <v>137</v>
       </c>
       <c r="R14" s="1">
         <v>10464</v>
       </c>
       <c r="S14">
-        <f t="shared" si="7"/>
+        <f>IF(ISBLANK(T14),-R14,T14-R14)</f>
         <v>79</v>
       </c>
       <c r="T14" s="1">
         <v>10543</v>
       </c>
       <c r="U14">
-        <f t="shared" si="8"/>
+        <f>IF(ISBLANK(V14),-T14,V14-T14)</f>
         <v>1160</v>
       </c>
       <c r="V14" s="1">
         <v>11703</v>
       </c>
       <c r="W14">
-        <f t="shared" si="9"/>
+        <f>IF(ISBLANK(X14),-V14,X14-V14)</f>
         <v>568</v>
       </c>
       <c r="X14" s="1">
         <v>12271</v>
       </c>
       <c r="Y14">
-        <f t="shared" si="10"/>
+        <f>IF(ISBLANK(Z14),-X14,Z14-X14)</f>
         <v>499</v>
       </c>
       <c r="Z14" s="1">
         <v>12770</v>
       </c>
       <c r="AA14">
-        <f t="shared" si="11"/>
+        <f>IF(ISBLANK(AB14),-Z14,AB14-Z14)</f>
         <v>-12770</v>
       </c>
       <c r="AB14" s="1">
         <v>0</v>
       </c>
       <c r="AC14">
-        <f t="shared" si="12"/>
+        <f>IF(ISBLANK(AD14),-AB14,AD14-AB14)</f>
         <v>0</v>
       </c>
       <c r="AD14" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE14">
+        <f>IF(ISBLANK(AF14),-AD14,AF14-AD14)</f>
+        <v>0</v>
+      </c>
+      <c r="AF14" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG14" s="1"/>
+      <c r="AH14" s="1"/>
+      <c r="AI14" s="1"/>
+      <c r="AJ14" s="1"/>
+      <c r="AK14" s="1"/>
+    </row>
+    <row r="15" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -8988,98 +9162,108 @@
         <v>9306</v>
       </c>
       <c r="E15">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F15),-D15,F15-D15)</f>
         <v>25</v>
       </c>
       <c r="F15" s="1">
         <v>9331</v>
       </c>
       <c r="G15">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H15),-F15,H15-F15)</f>
         <v>70</v>
       </c>
       <c r="H15" s="1">
         <v>9401</v>
       </c>
       <c r="I15">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J15),-H15,J15-H15)</f>
         <v>35</v>
       </c>
       <c r="J15" s="1">
         <v>9436</v>
       </c>
       <c r="K15">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L15),-J15,L15-J15)</f>
         <v>60</v>
       </c>
       <c r="L15" s="1">
         <v>9496</v>
       </c>
       <c r="M15">
-        <f t="shared" si="4"/>
+        <f>IF(ISBLANK(N15),-L15,N15-L15)</f>
         <v>228</v>
       </c>
       <c r="N15" s="1">
         <v>9724</v>
       </c>
       <c r="O15">
-        <f t="shared" si="5"/>
+        <f>IF(ISBLANK(P15),-N15,P15-N15)</f>
         <v>145</v>
       </c>
       <c r="P15" s="1">
         <v>9869</v>
       </c>
       <c r="Q15">
-        <f t="shared" si="6"/>
+        <f>IF(ISBLANK(R15),-P15,R15-P15)</f>
         <v>106</v>
       </c>
       <c r="R15" s="1">
         <v>9975</v>
       </c>
       <c r="S15">
-        <f t="shared" si="7"/>
+        <f>IF(ISBLANK(T15),-R15,T15-R15)</f>
         <v>247</v>
       </c>
       <c r="T15" s="1">
         <v>10222</v>
       </c>
       <c r="U15">
-        <f t="shared" si="8"/>
+        <f>IF(ISBLANK(V15),-T15,V15-T15)</f>
         <v>616</v>
       </c>
       <c r="V15" s="1">
         <v>10838</v>
       </c>
       <c r="W15">
-        <f t="shared" si="9"/>
+        <f>IF(ISBLANK(X15),-V15,X15-V15)</f>
         <v>-10838</v>
       </c>
       <c r="X15" s="1">
         <v>0</v>
       </c>
       <c r="Y15">
-        <f t="shared" si="10"/>
+        <f>IF(ISBLANK(Z15),-X15,Z15-X15)</f>
         <v>0</v>
       </c>
       <c r="Z15" s="1">
         <v>0</v>
       </c>
       <c r="AA15">
-        <f t="shared" si="11"/>
+        <f>IF(ISBLANK(AB15),-Z15,AB15-Z15)</f>
         <v>0</v>
       </c>
       <c r="AB15" s="1">
         <v>0</v>
       </c>
       <c r="AC15">
-        <f t="shared" si="12"/>
+        <f>IF(ISBLANK(AD15),-AB15,AD15-AB15)</f>
         <v>0</v>
       </c>
       <c r="AD15" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE15">
+        <f>IF(ISBLANK(AF15),-AD15,AF15-AD15)</f>
+        <v>0</v>
+      </c>
+      <c r="AF15" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG15" s="1"/>
+      <c r="AH15" s="1"/>
+      <c r="AI15" s="1"/>
+    </row>
+    <row r="16" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -9090,96 +9274,105 @@
         <v>7475</v>
       </c>
       <c r="E16">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F16),-D16,F16-D16)</f>
         <v>23</v>
       </c>
       <c r="F16" s="1">
         <v>7498</v>
       </c>
       <c r="G16">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H16),-F16,H16-F16)</f>
         <v>98</v>
       </c>
       <c r="H16" s="1">
         <v>7596</v>
       </c>
       <c r="I16">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J16),-H16,J16-H16)</f>
         <v>142</v>
       </c>
       <c r="J16" s="1">
         <v>7738</v>
       </c>
       <c r="K16">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L16),-J16,L16-J16)</f>
         <v>70</v>
       </c>
       <c r="L16" s="1">
         <v>7808</v>
       </c>
       <c r="M16">
-        <f t="shared" si="4"/>
+        <f>IF(ISBLANK(N16),-L16,N16-L16)</f>
         <v>197</v>
       </c>
       <c r="N16" s="1">
         <v>8005</v>
       </c>
       <c r="O16">
-        <f t="shared" si="5"/>
+        <f>IF(ISBLANK(P16),-N16,P16-N16)</f>
         <v>192</v>
       </c>
       <c r="P16" s="1">
         <v>8197</v>
       </c>
       <c r="Q16">
-        <f t="shared" si="6"/>
+        <f>IF(ISBLANK(R16),-P16,R16-P16)</f>
         <v>176</v>
       </c>
       <c r="R16" s="1">
         <v>8373</v>
       </c>
       <c r="S16">
-        <f t="shared" si="7"/>
+        <f>IF(ISBLANK(T16),-R16,T16-R16)</f>
         <v>188</v>
       </c>
       <c r="T16" s="1">
         <v>8561</v>
       </c>
       <c r="U16">
-        <f t="shared" si="8"/>
+        <f>IF(ISBLANK(V16),-T16,V16-T16)</f>
         <v>-8561</v>
       </c>
       <c r="V16" s="1">
         <v>0</v>
       </c>
       <c r="W16">
-        <f t="shared" si="9"/>
+        <f>IF(ISBLANK(X16),-V16,X16-V16)</f>
         <v>0</v>
       </c>
       <c r="X16" s="1">
         <v>0</v>
       </c>
       <c r="Y16">
-        <f t="shared" si="10"/>
+        <f>IF(ISBLANK(Z16),-X16,Z16-X16)</f>
         <v>0</v>
       </c>
       <c r="Z16" s="1">
         <v>0</v>
       </c>
       <c r="AA16">
-        <f t="shared" si="11"/>
+        <f>IF(ISBLANK(AB16),-Z16,AB16-Z16)</f>
         <v>0</v>
       </c>
       <c r="AB16" s="1">
         <v>0</v>
       </c>
       <c r="AC16">
-        <f t="shared" si="12"/>
+        <f>IF(ISBLANK(AD16),-AB16,AD16-AB16)</f>
         <v>0</v>
       </c>
       <c r="AD16" s="1">
         <v>0</v>
       </c>
+      <c r="AE16">
+        <f>IF(ISBLANK(AF16),-AD16,AF16-AD16)</f>
+        <v>0</v>
+      </c>
+      <c r="AF16" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG16" s="1"/>
+      <c r="AH16" s="1"/>
     </row>
     <row r="17" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A17">
@@ -9192,96 +9385,104 @@
         <v>4665</v>
       </c>
       <c r="E17">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F17),-D17,F17-D17)</f>
         <v>26</v>
       </c>
       <c r="F17" s="1">
         <v>4691</v>
       </c>
       <c r="G17">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H17),-F17,H17-F17)</f>
         <v>43</v>
       </c>
       <c r="H17" s="1">
         <v>4734</v>
       </c>
       <c r="I17">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J17),-H17,J17-H17)</f>
         <v>57</v>
       </c>
       <c r="J17" s="1">
         <v>4791</v>
       </c>
       <c r="K17">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L17),-J17,L17-J17)</f>
         <v>50</v>
       </c>
       <c r="L17" s="1">
         <v>4841</v>
       </c>
       <c r="M17">
-        <f t="shared" si="4"/>
+        <f>IF(ISBLANK(N17),-L17,N17-L17)</f>
         <v>115</v>
       </c>
       <c r="N17" s="1">
         <v>4956</v>
       </c>
       <c r="O17">
-        <f t="shared" si="5"/>
+        <f>IF(ISBLANK(P17),-N17,P17-N17)</f>
         <v>72</v>
       </c>
       <c r="P17" s="1">
         <v>5028</v>
       </c>
       <c r="Q17">
-        <f t="shared" si="6"/>
+        <f>IF(ISBLANK(R17),-P17,R17-P17)</f>
         <v>104</v>
       </c>
       <c r="R17" s="1">
         <v>5132</v>
       </c>
       <c r="S17">
-        <f t="shared" si="7"/>
+        <f>IF(ISBLANK(T17),-R17,T17-R17)</f>
         <v>-5132</v>
       </c>
       <c r="T17" s="1">
         <v>0</v>
       </c>
       <c r="U17">
-        <f t="shared" si="8"/>
+        <f>IF(ISBLANK(V17),-T17,V17-T17)</f>
         <v>0</v>
       </c>
       <c r="V17" s="1">
         <v>0</v>
       </c>
       <c r="W17">
-        <f t="shared" si="9"/>
+        <f>IF(ISBLANK(X17),-V17,X17-V17)</f>
         <v>0</v>
       </c>
       <c r="X17" s="1">
         <v>0</v>
       </c>
       <c r="Y17">
-        <f t="shared" si="10"/>
+        <f>IF(ISBLANK(Z17),-X17,Z17-X17)</f>
         <v>0</v>
       </c>
       <c r="Z17" s="1">
         <v>0</v>
       </c>
       <c r="AA17">
-        <f t="shared" si="11"/>
+        <f>IF(ISBLANK(AB17),-Z17,AB17-Z17)</f>
         <v>0</v>
       </c>
       <c r="AB17" s="1">
         <v>0</v>
       </c>
       <c r="AC17">
-        <f t="shared" si="12"/>
+        <f>IF(ISBLANK(AD17),-AB17,AD17-AB17)</f>
         <v>0</v>
       </c>
       <c r="AD17" s="1">
         <v>0</v>
       </c>
+      <c r="AE17">
+        <f>IF(ISBLANK(AF17),-AD17,AF17-AD17)</f>
+        <v>0</v>
+      </c>
+      <c r="AF17" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG17" s="1"/>
     </row>
     <row r="18" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A18">
@@ -9294,94 +9495,101 @@
         <v>3682</v>
       </c>
       <c r="E18">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F18),-D18,F18-D18)</f>
         <v>77</v>
       </c>
       <c r="F18" s="1">
         <v>3759</v>
       </c>
       <c r="G18">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H18),-F18,H18-F18)</f>
         <v>44</v>
       </c>
       <c r="H18" s="1">
         <v>3803</v>
       </c>
       <c r="I18">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J18),-H18,J18-H18)</f>
         <v>116</v>
       </c>
       <c r="J18" s="1">
         <v>3919</v>
       </c>
       <c r="K18">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L18),-J18,L18-J18)</f>
         <v>87</v>
       </c>
       <c r="L18" s="1">
         <v>4006</v>
       </c>
       <c r="M18">
-        <f t="shared" si="4"/>
+        <f>IF(ISBLANK(N18),-L18,N18-L18)</f>
         <v>41</v>
       </c>
       <c r="N18" s="1">
         <v>4047</v>
       </c>
       <c r="O18">
-        <f t="shared" si="5"/>
+        <f>IF(ISBLANK(P18),-N18,P18-N18)</f>
         <v>134</v>
       </c>
       <c r="P18" s="1">
         <v>4181</v>
       </c>
       <c r="Q18">
-        <f t="shared" si="6"/>
+        <f>IF(ISBLANK(R18),-P18,R18-P18)</f>
         <v>-4181</v>
       </c>
       <c r="R18" s="1">
         <v>0</v>
       </c>
       <c r="S18">
-        <f t="shared" si="7"/>
+        <f>IF(ISBLANK(T18),-R18,T18-R18)</f>
         <v>0</v>
       </c>
       <c r="T18" s="1">
         <v>0</v>
       </c>
       <c r="U18">
-        <f t="shared" si="8"/>
+        <f>IF(ISBLANK(V18),-T18,V18-T18)</f>
         <v>0</v>
       </c>
       <c r="V18" s="1">
         <v>0</v>
       </c>
       <c r="W18">
-        <f t="shared" si="9"/>
+        <f>IF(ISBLANK(X18),-V18,X18-V18)</f>
         <v>0</v>
       </c>
       <c r="X18" s="1">
         <v>0</v>
       </c>
       <c r="Y18">
-        <f t="shared" si="10"/>
+        <f>IF(ISBLANK(Z18),-X18,Z18-X18)</f>
         <v>0</v>
       </c>
       <c r="Z18" s="1">
         <v>0</v>
       </c>
       <c r="AA18">
-        <f t="shared" si="11"/>
+        <f>IF(ISBLANK(AB18),-Z18,AB18-Z18)</f>
         <v>0</v>
       </c>
       <c r="AB18" s="1">
         <v>0</v>
       </c>
       <c r="AC18">
-        <f t="shared" si="12"/>
+        <f>IF(ISBLANK(AD18),-AB18,AD18-AB18)</f>
         <v>0</v>
       </c>
       <c r="AD18" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE18">
+        <f>IF(ISBLANK(AF18),-AD18,AF18-AD18)</f>
+        <v>0</v>
+      </c>
+      <c r="AF18" s="1">
         <v>0</v>
       </c>
     </row>
@@ -9396,94 +9604,101 @@
         <v>3286</v>
       </c>
       <c r="E19">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F19),-D19,F19-D19)</f>
         <v>21</v>
       </c>
       <c r="F19" s="1">
         <v>3307</v>
       </c>
       <c r="G19">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H19),-F19,H19-F19)</f>
         <v>13</v>
       </c>
       <c r="H19" s="1">
         <v>3320</v>
       </c>
       <c r="I19">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J19),-H19,J19-H19)</f>
         <v>232</v>
       </c>
       <c r="J19" s="1">
         <v>3552</v>
       </c>
       <c r="K19">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L19),-J19,L19-J19)</f>
         <v>102</v>
       </c>
       <c r="L19" s="1">
         <v>3654</v>
       </c>
       <c r="M19">
-        <f t="shared" si="4"/>
+        <f>IF(ISBLANK(N19),-L19,N19-L19)</f>
         <v>60</v>
       </c>
       <c r="N19" s="1">
         <v>3714</v>
       </c>
       <c r="O19">
-        <f t="shared" si="5"/>
+        <f>IF(ISBLANK(P19),-N19,P19-N19)</f>
         <v>-3714</v>
       </c>
       <c r="P19" s="1">
         <v>0</v>
       </c>
       <c r="Q19">
-        <f t="shared" si="6"/>
+        <f>IF(ISBLANK(R19),-P19,R19-P19)</f>
         <v>0</v>
       </c>
       <c r="R19" s="1">
         <v>0</v>
       </c>
       <c r="S19">
-        <f t="shared" si="7"/>
+        <f>IF(ISBLANK(T19),-R19,T19-R19)</f>
         <v>0</v>
       </c>
       <c r="T19" s="1">
         <v>0</v>
       </c>
       <c r="U19">
-        <f t="shared" si="8"/>
+        <f>IF(ISBLANK(V19),-T19,V19-T19)</f>
         <v>0</v>
       </c>
       <c r="V19" s="1">
         <v>0</v>
       </c>
       <c r="W19">
-        <f t="shared" si="9"/>
+        <f>IF(ISBLANK(X19),-V19,X19-V19)</f>
         <v>0</v>
       </c>
       <c r="X19" s="1">
         <v>0</v>
       </c>
       <c r="Y19">
-        <f t="shared" si="10"/>
+        <f>IF(ISBLANK(Z19),-X19,Z19-X19)</f>
         <v>0</v>
       </c>
       <c r="Z19" s="1">
         <v>0</v>
       </c>
       <c r="AA19">
-        <f t="shared" si="11"/>
+        <f>IF(ISBLANK(AB19),-Z19,AB19-Z19)</f>
         <v>0</v>
       </c>
       <c r="AB19" s="1">
         <v>0</v>
       </c>
       <c r="AC19">
-        <f t="shared" si="12"/>
+        <f>IF(ISBLANK(AD19),-AB19,AD19-AB19)</f>
         <v>0</v>
       </c>
       <c r="AD19" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE19">
+        <f>IF(ISBLANK(AF19),-AD19,AF19-AD19)</f>
+        <v>0</v>
+      </c>
+      <c r="AF19" s="1">
         <v>0</v>
       </c>
     </row>
@@ -9498,94 +9713,101 @@
         <v>3182</v>
       </c>
       <c r="E20">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F20),-D20,F20-D20)</f>
         <v>15</v>
       </c>
       <c r="F20" s="1">
         <v>3197</v>
       </c>
       <c r="G20">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H20),-F20,H20-F20)</f>
         <v>60</v>
       </c>
       <c r="H20" s="1">
         <v>3257</v>
       </c>
       <c r="I20">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J20),-H20,J20-H20)</f>
         <v>43</v>
       </c>
       <c r="J20" s="1">
         <v>3300</v>
       </c>
       <c r="K20">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L20),-J20,L20-J20)</f>
         <v>32</v>
       </c>
       <c r="L20" s="1">
         <v>3332</v>
       </c>
       <c r="M20">
-        <f t="shared" si="4"/>
+        <f>IF(ISBLANK(N20),-L20,N20-L20)</f>
         <v>-3332</v>
       </c>
       <c r="N20" s="1">
         <v>0</v>
       </c>
       <c r="O20">
-        <f t="shared" si="5"/>
+        <f>IF(ISBLANK(P20),-N20,P20-N20)</f>
         <v>0</v>
       </c>
       <c r="P20" s="1">
         <v>0</v>
       </c>
       <c r="Q20">
-        <f t="shared" si="6"/>
+        <f>IF(ISBLANK(R20),-P20,R20-P20)</f>
         <v>0</v>
       </c>
       <c r="R20" s="1">
         <v>0</v>
       </c>
       <c r="S20">
-        <f t="shared" si="7"/>
+        <f>IF(ISBLANK(T20),-R20,T20-R20)</f>
         <v>0</v>
       </c>
       <c r="T20" s="1">
         <v>0</v>
       </c>
       <c r="U20">
-        <f t="shared" si="8"/>
+        <f>IF(ISBLANK(V20),-T20,V20-T20)</f>
         <v>0</v>
       </c>
       <c r="V20" s="1">
         <v>0</v>
       </c>
       <c r="W20">
-        <f t="shared" si="9"/>
+        <f>IF(ISBLANK(X20),-V20,X20-V20)</f>
         <v>0</v>
       </c>
       <c r="X20" s="1">
         <v>0</v>
       </c>
       <c r="Y20">
-        <f t="shared" si="10"/>
+        <f>IF(ISBLANK(Z20),-X20,Z20-X20)</f>
         <v>0</v>
       </c>
       <c r="Z20" s="1">
         <v>0</v>
       </c>
       <c r="AA20">
-        <f t="shared" si="11"/>
+        <f>IF(ISBLANK(AB20),-Z20,AB20-Z20)</f>
         <v>0</v>
       </c>
       <c r="AB20" s="1">
         <v>0</v>
       </c>
       <c r="AC20">
-        <f t="shared" si="12"/>
+        <f>IF(ISBLANK(AD20),-AB20,AD20-AB20)</f>
         <v>0</v>
       </c>
       <c r="AD20" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE20">
+        <f>IF(ISBLANK(AF20),-AD20,AF20-AD20)</f>
+        <v>0</v>
+      </c>
+      <c r="AF20" s="1">
         <v>0</v>
       </c>
     </row>
@@ -9600,94 +9822,101 @@
         <v>2864</v>
       </c>
       <c r="E21">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F21),-D21,F21-D21)</f>
         <v>34</v>
       </c>
       <c r="F21" s="1">
         <v>2898</v>
       </c>
       <c r="G21">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H21),-F21,H21-F21)</f>
         <v>21</v>
       </c>
       <c r="H21" s="1">
         <v>2919</v>
       </c>
       <c r="I21">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J21),-H21,J21-H21)</f>
         <v>148</v>
       </c>
       <c r="J21" s="1">
         <v>3067</v>
       </c>
       <c r="K21">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L21),-J21,L21-J21)</f>
         <v>-3067</v>
       </c>
       <c r="L21" s="1">
         <v>0</v>
       </c>
       <c r="M21">
-        <f t="shared" si="4"/>
+        <f>IF(ISBLANK(N21),-L21,N21-L21)</f>
         <v>0</v>
       </c>
       <c r="N21" s="1">
         <v>0</v>
       </c>
       <c r="O21">
-        <f t="shared" si="5"/>
+        <f>IF(ISBLANK(P21),-N21,P21-N21)</f>
         <v>0</v>
       </c>
       <c r="P21" s="1">
         <v>0</v>
       </c>
       <c r="Q21">
-        <f t="shared" si="6"/>
+        <f>IF(ISBLANK(R21),-P21,R21-P21)</f>
         <v>0</v>
       </c>
       <c r="R21" s="1">
         <v>0</v>
       </c>
       <c r="S21">
-        <f t="shared" si="7"/>
+        <f>IF(ISBLANK(T21),-R21,T21-R21)</f>
         <v>0</v>
       </c>
       <c r="T21" s="1">
         <v>0</v>
       </c>
       <c r="U21">
-        <f t="shared" si="8"/>
+        <f>IF(ISBLANK(V21),-T21,V21-T21)</f>
         <v>0</v>
       </c>
       <c r="V21" s="1">
         <v>0</v>
       </c>
       <c r="W21">
-        <f t="shared" si="9"/>
+        <f>IF(ISBLANK(X21),-V21,X21-V21)</f>
         <v>0</v>
       </c>
       <c r="X21" s="1">
         <v>0</v>
       </c>
       <c r="Y21">
-        <f t="shared" si="10"/>
+        <f>IF(ISBLANK(Z21),-X21,Z21-X21)</f>
         <v>0</v>
       </c>
       <c r="Z21" s="1">
         <v>0</v>
       </c>
       <c r="AA21">
-        <f t="shared" si="11"/>
+        <f>IF(ISBLANK(AB21),-Z21,AB21-Z21)</f>
         <v>0</v>
       </c>
       <c r="AB21" s="1">
         <v>0</v>
       </c>
       <c r="AC21">
-        <f t="shared" si="12"/>
+        <f>IF(ISBLANK(AD21),-AB21,AD21-AB21)</f>
         <v>0</v>
       </c>
       <c r="AD21" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE21">
+        <f>IF(ISBLANK(AF21),-AD21,AF21-AD21)</f>
+        <v>0</v>
+      </c>
+      <c r="AF21" s="1">
         <v>0</v>
       </c>
     </row>
@@ -9702,94 +9931,101 @@
         <v>2416</v>
       </c>
       <c r="E22">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F22),-D22,F22-D22)</f>
         <v>48</v>
       </c>
       <c r="F22" s="1">
         <v>2464</v>
       </c>
       <c r="G22">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H22),-F22,H22-F22)</f>
         <v>78</v>
       </c>
       <c r="H22" s="1">
         <v>2542</v>
       </c>
       <c r="I22">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J22),-H22,J22-H22)</f>
         <v>-2542</v>
       </c>
       <c r="J22" s="1">
         <v>0</v>
       </c>
       <c r="K22">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L22),-J22,L22-J22)</f>
         <v>0</v>
       </c>
       <c r="L22" s="1">
         <v>0</v>
       </c>
       <c r="M22">
-        <f t="shared" si="4"/>
+        <f>IF(ISBLANK(N22),-L22,N22-L22)</f>
         <v>0</v>
       </c>
       <c r="N22" s="1">
         <v>0</v>
       </c>
       <c r="O22">
-        <f t="shared" si="5"/>
+        <f>IF(ISBLANK(P22),-N22,P22-N22)</f>
         <v>0</v>
       </c>
       <c r="P22" s="1">
         <v>0</v>
       </c>
       <c r="Q22">
-        <f t="shared" si="6"/>
+        <f>IF(ISBLANK(R22),-P22,R22-P22)</f>
         <v>0</v>
       </c>
       <c r="R22" s="1">
         <v>0</v>
       </c>
       <c r="S22">
-        <f t="shared" si="7"/>
+        <f>IF(ISBLANK(T22),-R22,T22-R22)</f>
         <v>0</v>
       </c>
       <c r="T22" s="1">
         <v>0</v>
       </c>
       <c r="U22">
-        <f t="shared" si="8"/>
+        <f>IF(ISBLANK(V22),-T22,V22-T22)</f>
         <v>0</v>
       </c>
       <c r="V22" s="1">
         <v>0</v>
       </c>
       <c r="W22">
-        <f t="shared" si="9"/>
+        <f>IF(ISBLANK(X22),-V22,X22-V22)</f>
         <v>0</v>
       </c>
       <c r="X22" s="1">
         <v>0</v>
       </c>
       <c r="Y22">
-        <f t="shared" si="10"/>
+        <f>IF(ISBLANK(Z22),-X22,Z22-X22)</f>
         <v>0</v>
       </c>
       <c r="Z22" s="1">
         <v>0</v>
       </c>
       <c r="AA22">
-        <f t="shared" si="11"/>
+        <f>IF(ISBLANK(AB22),-Z22,AB22-Z22)</f>
         <v>0</v>
       </c>
       <c r="AB22" s="1">
         <v>0</v>
       </c>
       <c r="AC22">
-        <f t="shared" si="12"/>
+        <f>IF(ISBLANK(AD22),-AB22,AD22-AB22)</f>
         <v>0</v>
       </c>
       <c r="AD22" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE22">
+        <f>IF(ISBLANK(AF22),-AD22,AF22-AD22)</f>
+        <v>0</v>
+      </c>
+      <c r="AF22" s="1">
         <v>0</v>
       </c>
     </row>
@@ -9804,94 +10040,101 @@
         <v>2395</v>
       </c>
       <c r="E23">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F23),-D23,F23-D23)</f>
         <v>14</v>
       </c>
       <c r="F23" s="1">
         <v>2409</v>
       </c>
       <c r="G23">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H23),-F23,H23-F23)</f>
         <v>-2409</v>
       </c>
       <c r="H23" s="1">
         <v>0</v>
       </c>
       <c r="I23">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J23),-H23,J23-H23)</f>
         <v>0</v>
       </c>
       <c r="J23" s="1">
         <v>0</v>
       </c>
       <c r="K23">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L23),-J23,L23-J23)</f>
         <v>0</v>
       </c>
       <c r="L23" s="1">
         <v>0</v>
       </c>
       <c r="M23">
-        <f t="shared" si="4"/>
+        <f>IF(ISBLANK(N23),-L23,N23-L23)</f>
         <v>0</v>
       </c>
       <c r="N23" s="1">
         <v>0</v>
       </c>
       <c r="O23">
-        <f t="shared" si="5"/>
+        <f>IF(ISBLANK(P23),-N23,P23-N23)</f>
         <v>0</v>
       </c>
       <c r="P23" s="1">
         <v>0</v>
       </c>
       <c r="Q23">
-        <f t="shared" si="6"/>
+        <f>IF(ISBLANK(R23),-P23,R23-P23)</f>
         <v>0</v>
       </c>
       <c r="R23" s="1">
         <v>0</v>
       </c>
       <c r="S23">
-        <f t="shared" si="7"/>
+        <f>IF(ISBLANK(T23),-R23,T23-R23)</f>
         <v>0</v>
       </c>
       <c r="T23" s="1">
         <v>0</v>
       </c>
       <c r="U23">
-        <f t="shared" si="8"/>
+        <f>IF(ISBLANK(V23),-T23,V23-T23)</f>
         <v>0</v>
       </c>
       <c r="V23" s="1">
         <v>0</v>
       </c>
       <c r="W23">
-        <f t="shared" si="9"/>
+        <f>IF(ISBLANK(X23),-V23,X23-V23)</f>
         <v>0</v>
       </c>
       <c r="X23" s="1">
         <v>0</v>
       </c>
       <c r="Y23">
-        <f t="shared" si="10"/>
+        <f>IF(ISBLANK(Z23),-X23,Z23-X23)</f>
         <v>0</v>
       </c>
       <c r="Z23" s="1">
         <v>0</v>
       </c>
       <c r="AA23">
-        <f t="shared" si="11"/>
+        <f>IF(ISBLANK(AB23),-Z23,AB23-Z23)</f>
         <v>0</v>
       </c>
       <c r="AB23" s="1">
         <v>0</v>
       </c>
       <c r="AC23">
-        <f t="shared" si="12"/>
+        <f>IF(ISBLANK(AD23),-AB23,AD23-AB23)</f>
         <v>0</v>
       </c>
       <c r="AD23" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE23">
+        <f>IF(ISBLANK(AF23),-AD23,AF23-AD23)</f>
+        <v>0</v>
+      </c>
+      <c r="AF23" s="1">
         <v>0</v>
       </c>
     </row>
@@ -9906,94 +10149,101 @@
         <v>1423</v>
       </c>
       <c r="E24">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F24),-D24,F24-D24)</f>
         <v>-1423</v>
       </c>
       <c r="F24" s="1">
         <v>0</v>
       </c>
       <c r="G24">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H24),-F24,H24-F24)</f>
         <v>0</v>
       </c>
       <c r="H24" s="1">
         <v>0</v>
       </c>
       <c r="I24">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J24),-H24,J24-H24)</f>
         <v>0</v>
       </c>
       <c r="J24" s="1">
         <v>0</v>
       </c>
       <c r="K24">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L24),-J24,L24-J24)</f>
         <v>0</v>
       </c>
       <c r="L24" s="1">
         <v>0</v>
       </c>
       <c r="M24">
-        <f t="shared" si="4"/>
+        <f>IF(ISBLANK(N24),-L24,N24-L24)</f>
         <v>0</v>
       </c>
       <c r="N24" s="1">
         <v>0</v>
       </c>
       <c r="O24">
-        <f t="shared" si="5"/>
+        <f>IF(ISBLANK(P24),-N24,P24-N24)</f>
         <v>0</v>
       </c>
       <c r="P24" s="1">
         <v>0</v>
       </c>
       <c r="Q24">
-        <f t="shared" si="6"/>
+        <f>IF(ISBLANK(R24),-P24,R24-P24)</f>
         <v>0</v>
       </c>
       <c r="R24" s="1">
         <v>0</v>
       </c>
       <c r="S24">
-        <f t="shared" si="7"/>
+        <f>IF(ISBLANK(T24),-R24,T24-R24)</f>
         <v>0</v>
       </c>
       <c r="T24" s="1">
         <v>0</v>
       </c>
       <c r="U24">
-        <f t="shared" si="8"/>
+        <f>IF(ISBLANK(V24),-T24,V24-T24)</f>
         <v>0</v>
       </c>
       <c r="V24" s="1">
         <v>0</v>
       </c>
       <c r="W24">
-        <f t="shared" si="9"/>
+        <f>IF(ISBLANK(X24),-V24,X24-V24)</f>
         <v>0</v>
       </c>
       <c r="X24" s="1">
         <v>0</v>
       </c>
       <c r="Y24">
-        <f t="shared" si="10"/>
+        <f>IF(ISBLANK(Z24),-X24,Z24-X24)</f>
         <v>0</v>
       </c>
       <c r="Z24" s="1">
         <v>0</v>
       </c>
       <c r="AA24">
-        <f t="shared" si="11"/>
+        <f>IF(ISBLANK(AB24),-Z24,AB24-Z24)</f>
         <v>0</v>
       </c>
       <c r="AB24" s="1">
         <v>0</v>
       </c>
       <c r="AC24">
-        <f t="shared" si="12"/>
+        <f>IF(ISBLANK(AD24),-AB24,AD24-AB24)</f>
         <v>0</v>
       </c>
       <c r="AD24" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE24">
+        <f>IF(ISBLANK(AF24),-AD24,AF24-AD24)</f>
+        <v>0</v>
+      </c>
+      <c r="AF24" s="1">
         <v>0</v>
       </c>
     </row>
@@ -10086,19 +10336,19 @@
         <v>148</v>
       </c>
       <c r="E27">
-        <f t="shared" ref="E27:E48" si="13">FIND(",",B27)</f>
+        <f t="shared" ref="E27:E48" si="0">FIND(",",B27)</f>
         <v>9</v>
       </c>
       <c r="F27" t="str">
-        <f t="shared" ref="F27:F48" si="14">LEFT(B27,E27-1)</f>
+        <f t="shared" ref="F27:F48" si="1">LEFT(B27,E27-1)</f>
         <v>Kelleher</v>
       </c>
       <c r="G27" t="str">
-        <f t="shared" ref="G27:G48" si="15">RIGHT(B27,LEN(B27)-(E27+1))</f>
+        <f t="shared" ref="G27:G48" si="2">RIGHT(B27,LEN(B27)-(E27+1))</f>
         <v>Billy</v>
       </c>
       <c r="H27" t="str">
-        <f t="shared" ref="H27:H48" si="16">G27&amp;" "&amp;F27</f>
+        <f t="shared" ref="H27:H48" si="3">G27&amp;" "&amp;F27</f>
         <v>Billy Kelleher</v>
       </c>
       <c r="J27" t="s">
@@ -10151,19 +10401,19 @@
         <v>149</v>
       </c>
       <c r="E28">
-        <f t="shared" si="13"/>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="F28" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="1"/>
         <v>Wallace</v>
       </c>
       <c r="G28" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="2"/>
         <v>Mick</v>
       </c>
       <c r="H28" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="3"/>
         <v>Mick Wallace</v>
       </c>
       <c r="J28" t="s">
@@ -10232,19 +10482,19 @@
         <v>150</v>
       </c>
       <c r="E29">
-        <f t="shared" si="13"/>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="F29" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="1"/>
         <v>Ní Riada</v>
       </c>
       <c r="G29" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="2"/>
         <v>Liadh</v>
       </c>
       <c r="H29" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="3"/>
         <v>Liadh Ní Riada</v>
       </c>
       <c r="J29" t="s">
@@ -10313,19 +10563,19 @@
         <v>151</v>
       </c>
       <c r="E30">
-        <f t="shared" si="13"/>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="F30" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="1"/>
         <v>O'Sullivan</v>
       </c>
       <c r="G30" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="2"/>
         <v>Grace</v>
       </c>
       <c r="H30" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="3"/>
         <v>Grace O'Sullivan</v>
       </c>
       <c r="J30" t="s">
@@ -10394,19 +10644,19 @@
         <v>152</v>
       </c>
       <c r="E31">
-        <f t="shared" si="13"/>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="F31" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="1"/>
         <v>Byrne</v>
       </c>
       <c r="G31" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="2"/>
         <v>Malcolm</v>
       </c>
       <c r="H31" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="3"/>
         <v>Malcolm Byrne</v>
       </c>
       <c r="J31" t="s">
@@ -10475,19 +10725,19 @@
         <v>153</v>
       </c>
       <c r="E32">
-        <f t="shared" si="13"/>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="F32" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="1"/>
         <v>Clune</v>
       </c>
       <c r="G32" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="2"/>
         <v>Deirdre</v>
       </c>
       <c r="H32" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="3"/>
         <v>Deirdre Clune</v>
       </c>
       <c r="J32" t="s">
@@ -10556,19 +10806,19 @@
         <v>154</v>
       </c>
       <c r="E33">
-        <f t="shared" si="13"/>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="F33" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="1"/>
         <v>Doyle</v>
       </c>
       <c r="G33" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="2"/>
         <v>Andrew</v>
       </c>
       <c r="H33" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="3"/>
         <v>Andrew Doyle</v>
       </c>
       <c r="J33" t="s">
@@ -10637,19 +10887,19 @@
         <v>155</v>
       </c>
       <c r="E34">
-        <f t="shared" si="13"/>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="F34" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="1"/>
         <v>Nunan</v>
       </c>
       <c r="G34" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="2"/>
         <v>Sheila</v>
       </c>
       <c r="H34" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="3"/>
         <v>Sheila Nunan</v>
       </c>
       <c r="J34" t="s">
@@ -10718,19 +10968,19 @@
         <v>156</v>
       </c>
       <c r="E35">
-        <f t="shared" si="13"/>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="F35" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="1"/>
         <v>Wallace</v>
       </c>
       <c r="G35" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="2"/>
         <v>Adrienne</v>
       </c>
       <c r="H35" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="3"/>
         <v>Adrienne Wallace</v>
       </c>
       <c r="J35" t="s">
@@ -10799,19 +11049,19 @@
         <v>157</v>
       </c>
       <c r="E36">
-        <f t="shared" si="13"/>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="F36" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="1"/>
         <v>Cahill</v>
       </c>
       <c r="G36" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="2"/>
         <v>Dolores</v>
       </c>
       <c r="H36" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="3"/>
         <v>Dolores Cahill</v>
       </c>
       <c r="J36" t="s">
@@ -10880,19 +11130,19 @@
         <v>158</v>
       </c>
       <c r="E37">
-        <f t="shared" si="13"/>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="F37" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="1"/>
         <v>O'Flynn</v>
       </c>
       <c r="G37" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="2"/>
         <v>Diarmuid Patrick</v>
       </c>
       <c r="H37" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="3"/>
         <v>Diarmuid Patrick O'Flynn</v>
       </c>
       <c r="J37" t="s">
@@ -10958,19 +11208,19 @@
         <v>159</v>
       </c>
       <c r="E38">
-        <f t="shared" si="13"/>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="F38" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="1"/>
         <v>Minehan</v>
       </c>
       <c r="G38" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="2"/>
         <v>Liam</v>
       </c>
       <c r="H38" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="3"/>
         <v>Liam Minehan</v>
       </c>
       <c r="J38" t="s">
@@ -11030,19 +11280,19 @@
         <v>160</v>
       </c>
       <c r="E39">
-        <f t="shared" si="13"/>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="F39" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="1"/>
         <v>Gardner</v>
       </c>
       <c r="G39" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="2"/>
         <v>Breda Patricia</v>
       </c>
       <c r="H39" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="3"/>
         <v>Breda Patricia Gardner</v>
       </c>
       <c r="J39" t="s">
@@ -11105,19 +11355,19 @@
         <v>161</v>
       </c>
       <c r="E40">
-        <f t="shared" si="13"/>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="F40" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="1"/>
         <v>Heaney</v>
       </c>
       <c r="G40" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="2"/>
         <v>Theresa</v>
       </c>
       <c r="H40" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="3"/>
         <v>Theresa Heaney</v>
       </c>
       <c r="J40" t="s">
@@ -11178,19 +11428,19 @@
         <v>162</v>
       </c>
       <c r="E41">
-        <f t="shared" si="13"/>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="F41" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="1"/>
         <v>Brennan</v>
       </c>
       <c r="G41" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="2"/>
         <v>Allan</v>
       </c>
       <c r="H41" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="3"/>
         <v>Allan Brennan</v>
       </c>
       <c r="J41" t="s">
@@ -11248,19 +11498,19 @@
         <v>163</v>
       </c>
       <c r="E42">
-        <f t="shared" si="13"/>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="F42" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="1"/>
         <v>O'Loughlin</v>
       </c>
       <c r="G42" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="2"/>
         <v>Peter</v>
       </c>
       <c r="H42" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="3"/>
         <v>Peter O'Loughlin</v>
       </c>
       <c r="J42" t="s">
@@ -11314,19 +11564,19 @@
         <v>164</v>
       </c>
       <c r="E43">
-        <f t="shared" si="13"/>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="F43" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="1"/>
         <v>Worthington</v>
       </c>
       <c r="G43" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="2"/>
         <v>Colleen</v>
       </c>
       <c r="H43" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="3"/>
         <v>Colleen Worthington</v>
       </c>
       <c r="J43" t="s">
@@ -11376,19 +11626,19 @@
         <v>165</v>
       </c>
       <c r="E44">
-        <f t="shared" si="13"/>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="F44" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="1"/>
         <v>Fitzgerald</v>
       </c>
       <c r="G44" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="2"/>
         <v>Paddy</v>
       </c>
       <c r="H44" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="3"/>
         <v>Paddy Fitzgerald</v>
       </c>
       <c r="J44" t="s">
@@ -11434,19 +11684,19 @@
         <v>166</v>
       </c>
       <c r="E45">
-        <f t="shared" si="13"/>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="F45" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="1"/>
         <v>Ryan-Purcell</v>
       </c>
       <c r="G45" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="2"/>
         <v>Walter</v>
       </c>
       <c r="H45" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="3"/>
         <v>Walter Ryan-Purcell</v>
       </c>
       <c r="J45" t="s">
@@ -11488,19 +11738,19 @@
         <v>167</v>
       </c>
       <c r="E46">
-        <f t="shared" si="13"/>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="F46" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="1"/>
         <v>Sexton</v>
       </c>
       <c r="G46" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="2"/>
         <v>Joesph</v>
       </c>
       <c r="H46" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="3"/>
         <v>Joesph Sexton</v>
       </c>
       <c r="J46" t="s">
@@ -11534,19 +11784,19 @@
         <v>168</v>
       </c>
       <c r="E47">
-        <f t="shared" si="13"/>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="F47" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="1"/>
         <v>Madden</v>
       </c>
       <c r="G47" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="2"/>
         <v>Peter</v>
       </c>
       <c r="H47" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="3"/>
         <v>Peter Madden</v>
       </c>
       <c r="J47" t="s">
@@ -11573,19 +11823,19 @@
         <v>169</v>
       </c>
       <c r="E48">
-        <f t="shared" si="13"/>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="F48" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="1"/>
         <v>Van de Ven</v>
       </c>
       <c r="G48" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="2"/>
         <v>Jan</v>
       </c>
       <c r="H48" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="3"/>
         <v>Jan Van de Ven</v>
       </c>
       <c r="J48" t="s">
@@ -11610,7 +11860,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:AD24">
+  <sortState ref="A2:AF24">
     <sortCondition ref="A2:A24"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Stages 16 & 17 South, Stage 12 Midlands added Signed-off-by: Gerry Mulvenna <git@movingwifi.com>
</commit_message>
<xml_diff>
--- a/europarl/europarl-ireland-2019.xlsx
+++ b/europarl/europarl-ireland-2019.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="14220" windowHeight="8580" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="14220" windowHeight="8580" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Candidates" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="262">
   <si>
     <t>Candidate</t>
   </si>
@@ -800,6 +800,9 @@
   </si>
   <si>
     <t>Count 16</t>
+  </si>
+  <si>
+    <t>Count 17</t>
   </si>
 </sst>
 </file>
@@ -5161,16 +5164,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="S2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="U2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="W2" sqref="W2:X18"/>
+      <selection pane="bottomRight" activeCell="Y2" sqref="Y2:Z18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>256</v>
       </c>
@@ -5210,8 +5213,11 @@
       <c r="X1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Z1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>11</v>
       </c>
@@ -5279,7 +5285,7 @@
         <v>0</v>
       </c>
       <c r="U2">
-        <f t="shared" ref="U2:W18" si="8">IF(ISBLANK(V2),-T2,V2-T2)</f>
+        <f t="shared" ref="U2:Y18" si="8">IF(ISBLANK(V2),-T2,V2-T2)</f>
         <v>0</v>
       </c>
       <c r="V2" s="1">
@@ -5292,8 +5298,15 @@
       <c r="X2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y2">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Z2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
@@ -5374,8 +5387,15 @@
       <c r="X3" s="1">
         <v>84825</v>
       </c>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y3">
+        <f t="shared" si="8"/>
+        <v>6571</v>
+      </c>
+      <c r="Z3" s="1">
+        <v>91396</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>5</v>
       </c>
@@ -5456,8 +5476,15 @@
       <c r="X4" s="1">
         <v>66565</v>
       </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y4">
+        <f t="shared" si="8"/>
+        <v>3358</v>
+      </c>
+      <c r="Z4" s="1">
+        <v>69923</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>9</v>
       </c>
@@ -5538,8 +5565,15 @@
       <c r="X5" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y5">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Z5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -5620,8 +5654,15 @@
       <c r="X6" s="1">
         <v>97319</v>
       </c>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y6">
+        <f t="shared" si="8"/>
+        <v>15441</v>
+      </c>
+      <c r="Z6" s="1">
+        <v>112760</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>15</v>
       </c>
@@ -5702,8 +5743,15 @@
       <c r="X7" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y7">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Z7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>10</v>
       </c>
@@ -5784,8 +5832,15 @@
       <c r="X8" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y8">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Z8" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>14</v>
       </c>
@@ -5866,8 +5921,15 @@
       <c r="X9" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y9">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Z9" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
@@ -5948,8 +6010,15 @@
       <c r="X10">
         <v>118986</v>
       </c>
-    </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y10">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Z10">
+        <v>118986</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>6</v>
       </c>
@@ -6030,8 +6099,15 @@
       <c r="X11" s="1">
         <v>61957</v>
       </c>
-    </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y11">
+        <f t="shared" si="8"/>
+        <v>-61957</v>
+      </c>
+      <c r="Z11" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>16</v>
       </c>
@@ -6112,8 +6188,15 @@
       <c r="X12" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y12">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Z12" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>17</v>
       </c>
@@ -6194,8 +6277,15 @@
       <c r="X13" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y13">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Z13" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -6276,8 +6366,15 @@
       <c r="X14" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y14">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Z14" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>12</v>
       </c>
@@ -6358,8 +6455,15 @@
       <c r="X15" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y15">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Z15" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>8</v>
       </c>
@@ -6440,6 +6544,13 @@
       <c r="X16" s="1">
         <v>0</v>
       </c>
+      <c r="Y16">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Z16" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A17">
@@ -6522,6 +6633,13 @@
       <c r="X17" s="1">
         <v>64532</v>
       </c>
+      <c r="Y17">
+        <f t="shared" si="8"/>
+        <v>4145</v>
+      </c>
+      <c r="Z17" s="1">
+        <v>68677</v>
+      </c>
     </row>
     <row r="18" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A18">
@@ -6603,6 +6721,13 @@
       </c>
       <c r="X18" s="1">
         <v>80338</v>
+      </c>
+      <c r="Y18">
+        <f t="shared" si="8"/>
+        <v>15825</v>
+      </c>
+      <c r="Z18" s="1">
+        <v>96163</v>
       </c>
     </row>
     <row r="20" spans="1:32" x14ac:dyDescent="0.25">
@@ -7591,8 +7716,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="AG2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="AG2" sqref="AG2:AJ24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7653,1259 +7781,1367 @@
       <c r="AF1" t="s">
         <v>258</v>
       </c>
+      <c r="AH1" t="s">
+        <v>260</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>261</v>
+      </c>
     </row>
     <row r="2" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>124</v>
+        <v>139</v>
       </c>
       <c r="D2" s="1">
-        <v>118444</v>
+        <v>4665</v>
       </c>
       <c r="E2">
         <f>IF(ISBLANK(F2),-D2,F2-D2)</f>
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="F2" s="1">
-        <v>118489</v>
+        <v>4691</v>
       </c>
       <c r="G2">
         <f>IF(ISBLANK(H2),-F2,H2-F2)</f>
-        <v>186</v>
+        <v>43</v>
       </c>
       <c r="H2" s="1">
-        <v>118675</v>
+        <v>4734</v>
       </c>
       <c r="I2">
         <f>IF(ISBLANK(J2),-H2,J2-H2)</f>
-        <v>98</v>
+        <v>57</v>
       </c>
       <c r="J2" s="1">
-        <v>118773</v>
+        <v>4791</v>
       </c>
       <c r="K2">
         <f>IF(ISBLANK(L2),-J2,L2-J2)</f>
-        <v>350</v>
+        <v>50</v>
       </c>
       <c r="L2" s="1">
-        <v>119123</v>
+        <v>4841</v>
       </c>
       <c r="M2">
         <f>IF(ISBLANK(N2),-L2,N2-L2)</f>
-        <v>257</v>
+        <v>115</v>
       </c>
       <c r="N2" s="1">
-        <v>119380</v>
+        <v>4956</v>
       </c>
       <c r="O2">
         <f>IF(ISBLANK(P2),-N2,P2-N2)</f>
-        <v>165</v>
+        <v>72</v>
       </c>
       <c r="P2" s="1">
-        <v>119545</v>
+        <v>5028</v>
       </c>
       <c r="Q2">
         <f>IF(ISBLANK(R2),-P2,R2-P2)</f>
-        <v>170</v>
+        <v>104</v>
       </c>
       <c r="R2" s="1">
-        <v>119715</v>
+        <v>5132</v>
       </c>
       <c r="S2">
         <f>IF(ISBLANK(T2),-R2,T2-R2)</f>
-        <v>168</v>
+        <v>-5132</v>
       </c>
       <c r="T2" s="1">
-        <v>119883</v>
+        <v>0</v>
       </c>
       <c r="U2">
         <f>IF(ISBLANK(V2),-T2,V2-T2)</f>
         <v>0</v>
       </c>
       <c r="V2" s="1">
-        <v>119883</v>
+        <v>0</v>
       </c>
       <c r="W2">
         <f>IF(ISBLANK(X2),-V2,X2-V2)</f>
         <v>0</v>
       </c>
       <c r="X2" s="1">
-        <v>119883</v>
+        <v>0</v>
       </c>
       <c r="Y2">
         <f>IF(ISBLANK(Z2),-X2,Z2-X2)</f>
         <v>0</v>
       </c>
       <c r="Z2" s="1">
-        <v>119883</v>
+        <v>0</v>
       </c>
       <c r="AA2">
         <f>IF(ISBLANK(AB2),-Z2,AB2-Z2)</f>
         <v>0</v>
       </c>
       <c r="AB2" s="1">
-        <v>119883</v>
+        <v>0</v>
       </c>
       <c r="AC2">
         <f>IF(ISBLANK(AD2),-AB2,AD2-AB2)</f>
         <v>0</v>
       </c>
       <c r="AD2" s="1">
-        <v>119883</v>
+        <v>0</v>
       </c>
       <c r="AE2">
         <f>IF(ISBLANK(AF2),-AD2,AF2-AD2)</f>
         <v>0</v>
       </c>
       <c r="AF2" s="1">
-        <v>119883</v>
-      </c>
-      <c r="AG2" s="1"/>
-      <c r="AH2" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="AG2">
+        <f>IF(ISBLANK(AH2),-AF2,AH2-AF2)</f>
+        <v>0</v>
+      </c>
+      <c r="AH2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AI2">
+        <f>IF(ISBLANK(AJ2),-AH2,AJ2-AH2)</f>
+        <v>0</v>
+      </c>
+      <c r="AJ2" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="D3" s="1">
-        <v>84083</v>
+        <v>69166</v>
       </c>
       <c r="E3">
         <f>IF(ISBLANK(F3),-D3,F3-D3)</f>
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="F3" s="1">
-        <v>84106</v>
+        <v>69201</v>
       </c>
       <c r="G3">
         <f>IF(ISBLANK(H3),-F3,H3-F3)</f>
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="H3" s="1">
-        <v>84164</v>
+        <v>69272</v>
       </c>
       <c r="I3">
         <f>IF(ISBLANK(J3),-H3,J3-H3)</f>
-        <v>74</v>
+        <v>44</v>
       </c>
       <c r="J3" s="1">
-        <v>84238</v>
+        <v>69316</v>
       </c>
       <c r="K3">
         <f>IF(ISBLANK(L3),-J3,L3-J3)</f>
-        <v>150</v>
+        <v>66</v>
       </c>
       <c r="L3" s="1">
-        <v>84388</v>
+        <v>69382</v>
       </c>
       <c r="M3">
         <f>IF(ISBLANK(N3),-L3,N3-L3)</f>
-        <v>171</v>
+        <v>129</v>
       </c>
       <c r="N3" s="1">
-        <v>84559</v>
+        <v>69511</v>
       </c>
       <c r="O3">
         <f>IF(ISBLANK(P3),-N3,P3-N3)</f>
-        <v>95</v>
+        <v>45</v>
       </c>
       <c r="P3" s="1">
-        <v>84654</v>
+        <v>69556</v>
       </c>
       <c r="Q3">
         <f>IF(ISBLANK(R3),-P3,R3-P3)</f>
-        <v>187</v>
+        <v>116</v>
       </c>
       <c r="R3" s="1">
-        <v>84841</v>
+        <v>69672</v>
       </c>
       <c r="S3">
         <f>IF(ISBLANK(T3),-R3,T3-R3)</f>
-        <v>130</v>
+        <v>1226</v>
       </c>
       <c r="T3" s="1">
-        <v>84971</v>
+        <v>70898</v>
       </c>
       <c r="U3">
         <f>IF(ISBLANK(V3),-T3,V3-T3)</f>
-        <v>480</v>
+        <v>270</v>
       </c>
       <c r="V3" s="1">
-        <v>85451</v>
+        <v>71168</v>
       </c>
       <c r="W3">
         <f>IF(ISBLANK(X3),-V3,X3-V3)</f>
-        <v>575</v>
+        <v>674</v>
       </c>
       <c r="X3" s="1">
-        <v>86026</v>
+        <v>71842</v>
       </c>
       <c r="Y3">
         <f>IF(ISBLANK(Z3),-X3,Z3-X3)</f>
-        <v>1010</v>
+        <v>291</v>
       </c>
       <c r="Z3" s="1">
-        <v>87036</v>
+        <v>72133</v>
       </c>
       <c r="AA3">
         <f>IF(ISBLANK(AB3),-Z3,AB3-Z3)</f>
-        <v>928</v>
+        <v>720</v>
       </c>
       <c r="AB3" s="1">
-        <v>87964</v>
+        <v>72853</v>
       </c>
       <c r="AC3">
         <f>IF(ISBLANK(AD3),-AB3,AD3-AB3)</f>
-        <v>637</v>
+        <v>929</v>
       </c>
       <c r="AD3" s="1">
-        <v>88601</v>
+        <v>73782</v>
       </c>
       <c r="AE3">
         <f>IF(ISBLANK(AF3),-AD3,AF3-AD3)</f>
-        <v>435</v>
+        <v>588</v>
       </c>
       <c r="AF3" s="1">
-        <v>89036</v>
-      </c>
-      <c r="AG3" s="1"/>
-      <c r="AH3" s="1"/>
-      <c r="AI3" s="1"/>
-      <c r="AJ3" s="1"/>
+        <v>74370</v>
+      </c>
+      <c r="AG3">
+        <f>IF(ISBLANK(AH3),-AF3,AH3-AF3)</f>
+        <v>6253</v>
+      </c>
+      <c r="AH3" s="1">
+        <v>80623</v>
+      </c>
+      <c r="AI3">
+        <f>IF(ISBLANK(AJ3),-AH3,AJ3-AH3)</f>
+        <v>-80623</v>
+      </c>
+      <c r="AJ3" s="1">
+        <v>0</v>
+      </c>
       <c r="AK3" s="1"/>
       <c r="AL3" s="1"/>
       <c r="AM3" s="1"/>
     </row>
     <row r="4" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="D4" s="1">
-        <v>81741</v>
+        <v>10582</v>
       </c>
       <c r="E4">
         <f>IF(ISBLANK(F4),-D4,F4-D4)</f>
-        <v>253</v>
+        <v>57</v>
       </c>
       <c r="F4" s="1">
-        <v>81994</v>
+        <v>10639</v>
       </c>
       <c r="G4">
         <f>IF(ISBLANK(H4),-F4,H4-F4)</f>
-        <v>130</v>
+        <v>106</v>
       </c>
       <c r="H4" s="1">
-        <v>82124</v>
+        <v>10745</v>
       </c>
       <c r="I4">
         <f>IF(ISBLANK(J4),-H4,J4-H4)</f>
-        <v>211</v>
+        <v>138</v>
       </c>
       <c r="J4" s="1">
-        <v>82335</v>
+        <v>10883</v>
       </c>
       <c r="K4">
         <f>IF(ISBLANK(L4),-J4,L4-J4)</f>
-        <v>323</v>
+        <v>54</v>
       </c>
       <c r="L4" s="1">
-        <v>82658</v>
+        <v>10937</v>
       </c>
       <c r="M4">
         <f>IF(ISBLANK(N4),-L4,N4-L4)</f>
-        <v>206</v>
+        <v>300</v>
       </c>
       <c r="N4" s="1">
-        <v>82864</v>
+        <v>11237</v>
       </c>
       <c r="O4">
         <f>IF(ISBLANK(P4),-N4,P4-N4)</f>
-        <v>556</v>
+        <v>159</v>
       </c>
       <c r="P4" s="1">
-        <v>83420</v>
+        <v>11396</v>
       </c>
       <c r="Q4">
         <f>IF(ISBLANK(R4),-P4,R4-P4)</f>
-        <v>351</v>
+        <v>322</v>
       </c>
       <c r="R4" s="1">
-        <v>83771</v>
+        <v>11718</v>
       </c>
       <c r="S4">
         <f>IF(ISBLANK(T4),-R4,T4-R4)</f>
-        <v>217</v>
+        <v>908</v>
       </c>
       <c r="T4" s="1">
-        <v>83988</v>
+        <v>12626</v>
       </c>
       <c r="U4">
         <f>IF(ISBLANK(V4),-T4,V4-T4)</f>
-        <v>247</v>
+        <v>1585</v>
       </c>
       <c r="V4" s="1">
-        <v>84235</v>
+        <v>14211</v>
       </c>
       <c r="W4">
         <f>IF(ISBLANK(X4),-V4,X4-V4)</f>
-        <v>1001</v>
+        <v>826</v>
       </c>
       <c r="X4" s="1">
-        <v>85236</v>
+        <v>15037</v>
       </c>
       <c r="Y4">
         <f>IF(ISBLANK(Z4),-X4,Z4-X4)</f>
-        <v>2333</v>
+        <v>429</v>
       </c>
       <c r="Z4" s="1">
-        <v>87569</v>
+        <v>15466</v>
       </c>
       <c r="AA4">
         <f>IF(ISBLANK(AB4),-Z4,AB4-Z4)</f>
-        <v>1190</v>
+        <v>1664</v>
       </c>
       <c r="AB4" s="1">
-        <v>88759</v>
+        <v>17130</v>
       </c>
       <c r="AC4">
         <f>IF(ISBLANK(AD4),-AB4,AD4-AB4)</f>
-        <v>1476</v>
+        <v>-17130</v>
       </c>
       <c r="AD4" s="1">
-        <v>90235</v>
+        <v>0</v>
       </c>
       <c r="AE4">
         <f>IF(ISBLANK(AF4),-AD4,AF4-AD4)</f>
-        <v>5545</v>
+        <v>0</v>
       </c>
       <c r="AF4" s="1">
-        <v>95780</v>
-      </c>
-      <c r="AG4" s="1"/>
-      <c r="AH4" s="1"/>
-      <c r="AI4" s="1"/>
-      <c r="AJ4" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="AG4">
+        <f>IF(ISBLANK(AH4),-AF4,AH4-AF4)</f>
+        <v>0</v>
+      </c>
+      <c r="AH4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AI4">
+        <f>IF(ISBLANK(AJ4),-AH4,AJ4-AH4)</f>
+        <v>0</v>
+      </c>
+      <c r="AJ4" s="1">
+        <v>0</v>
+      </c>
       <c r="AK4" s="1"/>
       <c r="AL4" s="1"/>
       <c r="AM4" s="1"/>
     </row>
     <row r="5" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="D5" s="1">
-        <v>79072</v>
+        <v>64605</v>
       </c>
       <c r="E5">
         <f>IF(ISBLANK(F5),-D5,F5-D5)</f>
-        <v>68</v>
+        <v>26</v>
       </c>
       <c r="F5" s="1">
-        <v>79140</v>
+        <v>64631</v>
       </c>
       <c r="G5">
         <f>IF(ISBLANK(H5),-F5,H5-F5)</f>
-        <v>142</v>
+        <v>61</v>
       </c>
       <c r="H5" s="1">
-        <v>79282</v>
+        <v>64692</v>
       </c>
       <c r="I5">
         <f>IF(ISBLANK(J5),-H5,J5-H5)</f>
-        <v>105</v>
+        <v>71</v>
       </c>
       <c r="J5" s="1">
-        <v>79387</v>
+        <v>64763</v>
       </c>
       <c r="K5">
         <f>IF(ISBLANK(L5),-J5,L5-J5)</f>
-        <v>186</v>
+        <v>136</v>
       </c>
       <c r="L5" s="1">
-        <v>79573</v>
+        <v>64899</v>
       </c>
       <c r="M5">
         <f>IF(ISBLANK(N5),-L5,N5-L5)</f>
-        <v>168</v>
+        <v>106</v>
       </c>
       <c r="N5" s="1">
-        <v>79741</v>
+        <v>65005</v>
       </c>
       <c r="O5">
         <f>IF(ISBLANK(P5),-N5,P5-N5)</f>
-        <v>204</v>
+        <v>110</v>
       </c>
       <c r="P5" s="1">
-        <v>79945</v>
+        <v>65115</v>
       </c>
       <c r="Q5">
         <f>IF(ISBLANK(R5),-P5,R5-P5)</f>
-        <v>305</v>
+        <v>137</v>
       </c>
       <c r="R5" s="1">
-        <v>80250</v>
+        <v>65252</v>
       </c>
       <c r="S5">
         <f>IF(ISBLANK(T5),-R5,T5-R5)</f>
-        <v>127</v>
+        <v>306</v>
       </c>
       <c r="T5" s="1">
-        <v>80377</v>
+        <v>65558</v>
       </c>
       <c r="U5">
         <f>IF(ISBLANK(V5),-T5,V5-T5)</f>
-        <v>446</v>
+        <v>491</v>
       </c>
       <c r="V5" s="1">
-        <v>80823</v>
+        <v>66049</v>
       </c>
       <c r="W5">
         <f>IF(ISBLANK(X5),-V5,X5-V5)</f>
-        <v>991</v>
+        <v>683</v>
       </c>
       <c r="X5" s="1">
-        <v>81814</v>
+        <v>66732</v>
       </c>
       <c r="Y5">
         <f>IF(ISBLANK(Z5),-X5,Z5-X5)</f>
-        <v>1119</v>
+        <v>542</v>
       </c>
       <c r="Z5" s="1">
-        <v>82933</v>
+        <v>67274</v>
       </c>
       <c r="AA5">
         <f>IF(ISBLANK(AB5),-Z5,AB5-Z5)</f>
-        <v>958</v>
+        <v>622</v>
       </c>
       <c r="AB5" s="1">
-        <v>83891</v>
+        <v>67896</v>
       </c>
       <c r="AC5">
         <f>IF(ISBLANK(AD5),-AB5,AD5-AB5)</f>
-        <v>1108</v>
+        <v>1194</v>
       </c>
       <c r="AD5" s="1">
-        <v>84999</v>
+        <v>69090</v>
       </c>
       <c r="AE5">
         <f>IF(ISBLANK(AF5),-AD5,AF5-AD5)</f>
-        <v>2323</v>
+        <v>470</v>
       </c>
       <c r="AF5" s="1">
-        <v>87322</v>
-      </c>
-      <c r="AG5" s="1"/>
-      <c r="AH5" s="1"/>
-      <c r="AI5" s="1"/>
-      <c r="AJ5" s="1"/>
+        <v>69560</v>
+      </c>
+      <c r="AG5">
+        <f>IF(ISBLANK(AH5),-AF5,AH5-AF5)</f>
+        <v>20183</v>
+      </c>
+      <c r="AH5" s="1">
+        <v>89743</v>
+      </c>
+      <c r="AI5">
+        <f>IF(ISBLANK(AJ5),-AH5,AJ5-AH5)</f>
+        <v>8192</v>
+      </c>
+      <c r="AJ5" s="1">
+        <v>97935</v>
+      </c>
       <c r="AK5" s="1"/>
       <c r="AL5" s="1"/>
       <c r="AM5" s="1"/>
     </row>
     <row r="6" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D6" s="1">
-        <v>75946</v>
+        <v>38738</v>
       </c>
       <c r="E6">
         <f>IF(ISBLANK(F6),-D6,F6-D6)</f>
-        <v>100</v>
+        <v>17</v>
       </c>
       <c r="F6" s="1">
-        <v>76046</v>
+        <v>38755</v>
       </c>
       <c r="G6">
         <f>IF(ISBLANK(H6),-F6,H6-F6)</f>
-        <v>201</v>
+        <v>33</v>
       </c>
       <c r="H6" s="1">
-        <v>76247</v>
+        <v>38788</v>
       </c>
       <c r="I6">
         <f>IF(ISBLANK(J6),-H6,J6-H6)</f>
-        <v>126</v>
+        <v>16</v>
       </c>
       <c r="J6" s="1">
-        <v>76373</v>
+        <v>38804</v>
       </c>
       <c r="K6">
         <f>IF(ISBLANK(L6),-J6,L6-J6)</f>
-        <v>272</v>
+        <v>38</v>
       </c>
       <c r="L6" s="1">
-        <v>76645</v>
+        <v>38842</v>
       </c>
       <c r="M6">
         <f>IF(ISBLANK(N6),-L6,N6-L6)</f>
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="N6" s="1">
-        <v>76719</v>
+        <v>38926</v>
       </c>
       <c r="O6">
         <f>IF(ISBLANK(P6),-N6,P6-N6)</f>
-        <v>301</v>
+        <v>24</v>
       </c>
       <c r="P6" s="1">
-        <v>77020</v>
+        <v>38950</v>
       </c>
       <c r="Q6">
         <f>IF(ISBLANK(R6),-P6,R6-P6)</f>
-        <v>283</v>
+        <v>46</v>
       </c>
       <c r="R6" s="1">
-        <v>77303</v>
+        <v>38996</v>
       </c>
       <c r="S6">
         <f>IF(ISBLANK(T6),-R6,T6-R6)</f>
-        <v>112</v>
+        <v>298</v>
       </c>
       <c r="T6" s="1">
-        <v>77415</v>
+        <v>39294</v>
       </c>
       <c r="U6">
         <f>IF(ISBLANK(V6),-T6,V6-T6)</f>
-        <v>339</v>
+        <v>135</v>
       </c>
       <c r="V6" s="1">
-        <v>77754</v>
+        <v>39429</v>
       </c>
       <c r="W6">
         <f>IF(ISBLANK(X6),-V6,X6-V6)</f>
-        <v>1066</v>
+        <v>426</v>
       </c>
       <c r="X6" s="1">
-        <v>78820</v>
+        <v>39855</v>
       </c>
       <c r="Y6">
         <f>IF(ISBLANK(Z6),-X6,Z6-X6)</f>
-        <v>1295</v>
+        <v>159</v>
       </c>
       <c r="Z6" s="1">
-        <v>80115</v>
+        <v>40014</v>
       </c>
       <c r="AA6">
         <f>IF(ISBLANK(AB6),-Z6,AB6-Z6)</f>
-        <v>593</v>
+        <v>572</v>
       </c>
       <c r="AB6" s="1">
-        <v>80708</v>
+        <v>40586</v>
       </c>
       <c r="AC6">
         <f>IF(ISBLANK(AD6),-AB6,AD6-AB6)</f>
-        <v>1290</v>
+        <v>483</v>
       </c>
       <c r="AD6" s="1">
-        <v>81998</v>
+        <v>41069</v>
       </c>
       <c r="AE6">
         <f>IF(ISBLANK(AF6),-AD6,AF6-AD6)</f>
-        <v>2743</v>
+        <v>347</v>
       </c>
       <c r="AF6" s="1">
-        <v>84741</v>
-      </c>
-      <c r="AG6" s="1"/>
-      <c r="AH6" s="1"/>
-      <c r="AI6" s="1"/>
-      <c r="AJ6" s="1"/>
+        <v>41416</v>
+      </c>
+      <c r="AG6">
+        <f>IF(ISBLANK(AH6),-AF6,AH6-AF6)</f>
+        <v>-41416</v>
+      </c>
+      <c r="AH6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AI6">
+        <f>IF(ISBLANK(AJ6),-AH6,AJ6-AH6)</f>
+        <v>0</v>
+      </c>
+      <c r="AJ6" s="1">
+        <v>0</v>
+      </c>
       <c r="AK6" s="1"/>
       <c r="AL6" s="1"/>
       <c r="AM6" s="1"/>
     </row>
     <row r="7" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>129</v>
+        <v>142</v>
       </c>
       <c r="D7" s="1">
-        <v>69166</v>
+        <v>3182</v>
       </c>
       <c r="E7">
         <f>IF(ISBLANK(F7),-D7,F7-D7)</f>
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="F7" s="1">
-        <v>69201</v>
+        <v>3197</v>
       </c>
       <c r="G7">
         <f>IF(ISBLANK(H7),-F7,H7-F7)</f>
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="H7" s="1">
-        <v>69272</v>
+        <v>3257</v>
       </c>
       <c r="I7">
         <f>IF(ISBLANK(J7),-H7,J7-H7)</f>
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J7" s="1">
-        <v>69316</v>
+        <v>3300</v>
       </c>
       <c r="K7">
         <f>IF(ISBLANK(L7),-J7,L7-J7)</f>
-        <v>66</v>
+        <v>32</v>
       </c>
       <c r="L7" s="1">
-        <v>69382</v>
+        <v>3332</v>
       </c>
       <c r="M7">
         <f>IF(ISBLANK(N7),-L7,N7-L7)</f>
-        <v>129</v>
+        <v>-3332</v>
       </c>
       <c r="N7" s="1">
-        <v>69511</v>
+        <v>0</v>
       </c>
       <c r="O7">
         <f>IF(ISBLANK(P7),-N7,P7-N7)</f>
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="P7" s="1">
-        <v>69556</v>
+        <v>0</v>
       </c>
       <c r="Q7">
         <f>IF(ISBLANK(R7),-P7,R7-P7)</f>
-        <v>116</v>
+        <v>0</v>
       </c>
       <c r="R7" s="1">
-        <v>69672</v>
+        <v>0</v>
       </c>
       <c r="S7">
         <f>IF(ISBLANK(T7),-R7,T7-R7)</f>
-        <v>1226</v>
+        <v>0</v>
       </c>
       <c r="T7" s="1">
-        <v>70898</v>
+        <v>0</v>
       </c>
       <c r="U7">
         <f>IF(ISBLANK(V7),-T7,V7-T7)</f>
-        <v>270</v>
+        <v>0</v>
       </c>
       <c r="V7" s="1">
-        <v>71168</v>
+        <v>0</v>
       </c>
       <c r="W7">
         <f>IF(ISBLANK(X7),-V7,X7-V7)</f>
-        <v>674</v>
+        <v>0</v>
       </c>
       <c r="X7" s="1">
-        <v>71842</v>
+        <v>0</v>
       </c>
       <c r="Y7">
         <f>IF(ISBLANK(Z7),-X7,Z7-X7)</f>
-        <v>291</v>
+        <v>0</v>
       </c>
       <c r="Z7" s="1">
-        <v>72133</v>
+        <v>0</v>
       </c>
       <c r="AA7">
         <f>IF(ISBLANK(AB7),-Z7,AB7-Z7)</f>
-        <v>720</v>
+        <v>0</v>
       </c>
       <c r="AB7" s="1">
-        <v>72853</v>
+        <v>0</v>
       </c>
       <c r="AC7">
         <f>IF(ISBLANK(AD7),-AB7,AD7-AB7)</f>
-        <v>929</v>
+        <v>0</v>
       </c>
       <c r="AD7" s="1">
-        <v>73782</v>
+        <v>0</v>
       </c>
       <c r="AE7">
         <f>IF(ISBLANK(AF7),-AD7,AF7-AD7)</f>
-        <v>588</v>
+        <v>0</v>
       </c>
       <c r="AF7" s="1">
-        <v>74370</v>
-      </c>
-      <c r="AG7" s="1"/>
-      <c r="AH7" s="1"/>
-      <c r="AI7" s="1"/>
-      <c r="AJ7" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="AG7">
+        <f>IF(ISBLANK(AH7),-AF7,AH7-AF7)</f>
+        <v>0</v>
+      </c>
+      <c r="AH7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AI7">
+        <f>IF(ISBLANK(AJ7),-AH7,AJ7-AH7)</f>
+        <v>0</v>
+      </c>
+      <c r="AJ7" s="1">
+        <v>0</v>
+      </c>
       <c r="AK7" s="1"/>
       <c r="AL7" s="1"/>
       <c r="AM7" s="1"/>
     </row>
     <row r="8" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="D8" s="1">
-        <v>64605</v>
+        <v>9306</v>
       </c>
       <c r="E8">
         <f>IF(ISBLANK(F8),-D8,F8-D8)</f>
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F8" s="1">
-        <v>64631</v>
+        <v>9331</v>
       </c>
       <c r="G8">
         <f>IF(ISBLANK(H8),-F8,H8-F8)</f>
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="H8" s="1">
-        <v>64692</v>
+        <v>9401</v>
       </c>
       <c r="I8">
         <f>IF(ISBLANK(J8),-H8,J8-H8)</f>
-        <v>71</v>
+        <v>35</v>
       </c>
       <c r="J8" s="1">
-        <v>64763</v>
+        <v>9436</v>
       </c>
       <c r="K8">
         <f>IF(ISBLANK(L8),-J8,L8-J8)</f>
-        <v>136</v>
+        <v>60</v>
       </c>
       <c r="L8" s="1">
-        <v>64899</v>
+        <v>9496</v>
       </c>
       <c r="M8">
         <f>IF(ISBLANK(N8),-L8,N8-L8)</f>
-        <v>106</v>
+        <v>228</v>
       </c>
       <c r="N8" s="1">
-        <v>65005</v>
+        <v>9724</v>
       </c>
       <c r="O8">
         <f>IF(ISBLANK(P8),-N8,P8-N8)</f>
-        <v>110</v>
+        <v>145</v>
       </c>
       <c r="P8" s="1">
-        <v>65115</v>
+        <v>9869</v>
       </c>
       <c r="Q8">
         <f>IF(ISBLANK(R8),-P8,R8-P8)</f>
-        <v>137</v>
+        <v>106</v>
       </c>
       <c r="R8" s="1">
-        <v>65252</v>
+        <v>9975</v>
       </c>
       <c r="S8">
         <f>IF(ISBLANK(T8),-R8,T8-R8)</f>
-        <v>306</v>
+        <v>247</v>
       </c>
       <c r="T8" s="1">
-        <v>65558</v>
+        <v>10222</v>
       </c>
       <c r="U8">
         <f>IF(ISBLANK(V8),-T8,V8-T8)</f>
-        <v>491</v>
+        <v>616</v>
       </c>
       <c r="V8" s="1">
-        <v>66049</v>
+        <v>10838</v>
       </c>
       <c r="W8">
         <f>IF(ISBLANK(X8),-V8,X8-V8)</f>
-        <v>683</v>
+        <v>-10838</v>
       </c>
       <c r="X8" s="1">
-        <v>66732</v>
+        <v>0</v>
       </c>
       <c r="Y8">
         <f>IF(ISBLANK(Z8),-X8,Z8-X8)</f>
-        <v>542</v>
+        <v>0</v>
       </c>
       <c r="Z8" s="1">
-        <v>67274</v>
+        <v>0</v>
       </c>
       <c r="AA8">
         <f>IF(ISBLANK(AB8),-Z8,AB8-Z8)</f>
-        <v>622</v>
+        <v>0</v>
       </c>
       <c r="AB8" s="1">
-        <v>67896</v>
+        <v>0</v>
       </c>
       <c r="AC8">
         <f>IF(ISBLANK(AD8),-AB8,AD8-AB8)</f>
-        <v>1194</v>
+        <v>0</v>
       </c>
       <c r="AD8" s="1">
-        <v>69090</v>
+        <v>0</v>
       </c>
       <c r="AE8">
         <f>IF(ISBLANK(AF8),-AD8,AF8-AD8)</f>
-        <v>470</v>
+        <v>0</v>
       </c>
       <c r="AF8" s="1">
-        <v>69560</v>
-      </c>
-      <c r="AG8" s="1"/>
-      <c r="AH8" s="1"/>
-      <c r="AI8" s="1"/>
-      <c r="AJ8" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="AG8">
+        <f>IF(ISBLANK(AH8),-AF8,AH8-AF8)</f>
+        <v>0</v>
+      </c>
+      <c r="AH8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AI8">
+        <f>IF(ISBLANK(AJ8),-AH8,AJ8-AH8)</f>
+        <v>0</v>
+      </c>
+      <c r="AJ8" s="1">
+        <v>0</v>
+      </c>
       <c r="AK8" s="1"/>
       <c r="AL8" s="1"/>
       <c r="AM8" s="1"/>
     </row>
     <row r="9" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="D9" s="1">
-        <v>38738</v>
+        <v>7475</v>
       </c>
       <c r="E9">
         <f>IF(ISBLANK(F9),-D9,F9-D9)</f>
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="F9" s="1">
-        <v>38755</v>
+        <v>7498</v>
       </c>
       <c r="G9">
         <f>IF(ISBLANK(H9),-F9,H9-F9)</f>
-        <v>33</v>
+        <v>98</v>
       </c>
       <c r="H9" s="1">
-        <v>38788</v>
+        <v>7596</v>
       </c>
       <c r="I9">
         <f>IF(ISBLANK(J9),-H9,J9-H9)</f>
-        <v>16</v>
+        <v>142</v>
       </c>
       <c r="J9" s="1">
-        <v>38804</v>
+        <v>7738</v>
       </c>
       <c r="K9">
         <f>IF(ISBLANK(L9),-J9,L9-J9)</f>
-        <v>38</v>
+        <v>70</v>
       </c>
       <c r="L9" s="1">
-        <v>38842</v>
+        <v>7808</v>
       </c>
       <c r="M9">
         <f>IF(ISBLANK(N9),-L9,N9-L9)</f>
-        <v>84</v>
+        <v>197</v>
       </c>
       <c r="N9" s="1">
-        <v>38926</v>
+        <v>8005</v>
       </c>
       <c r="O9">
         <f>IF(ISBLANK(P9),-N9,P9-N9)</f>
-        <v>24</v>
+        <v>192</v>
       </c>
       <c r="P9" s="1">
-        <v>38950</v>
+        <v>8197</v>
       </c>
       <c r="Q9">
         <f>IF(ISBLANK(R9),-P9,R9-P9)</f>
-        <v>46</v>
+        <v>176</v>
       </c>
       <c r="R9" s="1">
-        <v>38996</v>
+        <v>8373</v>
       </c>
       <c r="S9">
         <f>IF(ISBLANK(T9),-R9,T9-R9)</f>
-        <v>298</v>
+        <v>188</v>
       </c>
       <c r="T9" s="1">
-        <v>39294</v>
+        <v>8561</v>
       </c>
       <c r="U9">
         <f>IF(ISBLANK(V9),-T9,V9-T9)</f>
-        <v>135</v>
+        <v>-8561</v>
       </c>
       <c r="V9" s="1">
-        <v>39429</v>
+        <v>0</v>
       </c>
       <c r="W9">
         <f>IF(ISBLANK(X9),-V9,X9-V9)</f>
-        <v>426</v>
+        <v>0</v>
       </c>
       <c r="X9" s="1">
-        <v>39855</v>
+        <v>0</v>
       </c>
       <c r="Y9">
         <f>IF(ISBLANK(Z9),-X9,Z9-X9)</f>
-        <v>159</v>
+        <v>0</v>
       </c>
       <c r="Z9" s="1">
-        <v>40014</v>
+        <v>0</v>
       </c>
       <c r="AA9">
         <f>IF(ISBLANK(AB9),-Z9,AB9-Z9)</f>
-        <v>572</v>
+        <v>0</v>
       </c>
       <c r="AB9" s="1">
-        <v>40586</v>
+        <v>0</v>
       </c>
       <c r="AC9">
         <f>IF(ISBLANK(AD9),-AB9,AD9-AB9)</f>
-        <v>483</v>
+        <v>0</v>
       </c>
       <c r="AD9" s="1">
-        <v>41069</v>
+        <v>0</v>
       </c>
       <c r="AE9">
         <f>IF(ISBLANK(AF9),-AD9,AF9-AD9)</f>
-        <v>347</v>
+        <v>0</v>
       </c>
       <c r="AF9" s="1">
-        <v>41416</v>
-      </c>
-      <c r="AG9" s="1"/>
-      <c r="AH9" s="1"/>
-      <c r="AI9" s="1"/>
-      <c r="AJ9" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="AG9">
+        <f>IF(ISBLANK(AH9),-AF9,AH9-AF9)</f>
+        <v>0</v>
+      </c>
+      <c r="AH9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AI9">
+        <f>IF(ISBLANK(AJ9),-AH9,AJ9-AH9)</f>
+        <v>0</v>
+      </c>
+      <c r="AJ9" s="1">
+        <v>0</v>
+      </c>
       <c r="AK9" s="1"/>
       <c r="AL9" s="1"/>
       <c r="AM9" s="1"/>
     </row>
     <row r="10" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="D10" s="1">
-        <v>22075</v>
+        <v>84083</v>
       </c>
       <c r="E10">
         <f>IF(ISBLANK(F10),-D10,F10-D10)</f>
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="F10" s="1">
-        <v>22113</v>
+        <v>84106</v>
       </c>
       <c r="G10">
         <f>IF(ISBLANK(H10),-F10,H10-F10)</f>
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="H10" s="1">
-        <v>22193</v>
+        <v>84164</v>
       </c>
       <c r="I10">
         <f>IF(ISBLANK(J10),-H10,J10-H10)</f>
-        <v>58</v>
+        <v>74</v>
       </c>
       <c r="J10" s="1">
-        <v>22251</v>
+        <v>84238</v>
       </c>
       <c r="K10">
         <f>IF(ISBLANK(L10),-J10,L10-J10)</f>
-        <v>70</v>
+        <v>150</v>
       </c>
       <c r="L10" s="1">
-        <v>22321</v>
+        <v>84388</v>
       </c>
       <c r="M10">
         <f>IF(ISBLANK(N10),-L10,N10-L10)</f>
-        <v>62</v>
+        <v>171</v>
       </c>
       <c r="N10" s="1">
-        <v>22383</v>
+        <v>84559</v>
       </c>
       <c r="O10">
         <f>IF(ISBLANK(P10),-N10,P10-N10)</f>
-        <v>70</v>
+        <v>95</v>
       </c>
       <c r="P10" s="1">
-        <v>22453</v>
+        <v>84654</v>
       </c>
       <c r="Q10">
         <f>IF(ISBLANK(R10),-P10,R10-P10)</f>
-        <v>173</v>
+        <v>187</v>
       </c>
       <c r="R10" s="1">
-        <v>22626</v>
+        <v>84841</v>
       </c>
       <c r="S10">
         <f>IF(ISBLANK(T10),-R10,T10-R10)</f>
-        <v>74</v>
+        <v>130</v>
       </c>
       <c r="T10" s="1">
-        <v>22700</v>
+        <v>84971</v>
       </c>
       <c r="U10">
         <f>IF(ISBLANK(V10),-T10,V10-T10)</f>
-        <v>193</v>
+        <v>480</v>
       </c>
       <c r="V10" s="1">
-        <v>22893</v>
+        <v>85451</v>
       </c>
       <c r="W10">
         <f>IF(ISBLANK(X10),-V10,X10-V10)</f>
-        <v>626</v>
+        <v>575</v>
       </c>
       <c r="X10" s="1">
-        <v>23519</v>
+        <v>86026</v>
       </c>
       <c r="Y10">
         <f>IF(ISBLANK(Z10),-X10,Z10-X10)</f>
-        <v>330</v>
+        <v>1010</v>
       </c>
       <c r="Z10" s="1">
-        <v>23849</v>
+        <v>87036</v>
       </c>
       <c r="AA10">
         <f>IF(ISBLANK(AB10),-Z10,AB10-Z10)</f>
-        <v>483</v>
+        <v>928</v>
       </c>
       <c r="AB10" s="1">
-        <v>24332</v>
+        <v>87964</v>
       </c>
       <c r="AC10">
         <f>IF(ISBLANK(AD10),-AB10,AD10-AB10)</f>
-        <v>600</v>
+        <v>637</v>
       </c>
       <c r="AD10" s="1">
-        <v>24932</v>
+        <v>88601</v>
       </c>
       <c r="AE10">
         <f>IF(ISBLANK(AF10),-AD10,AF10-AD10)</f>
-        <v>1026</v>
+        <v>435</v>
       </c>
       <c r="AF10" s="1">
-        <v>25958</v>
-      </c>
-      <c r="AG10" s="1"/>
-      <c r="AH10" s="1"/>
-      <c r="AI10" s="1"/>
-      <c r="AJ10" s="1"/>
+        <v>89036</v>
+      </c>
+      <c r="AG10">
+        <f>IF(ISBLANK(AH10),-AF10,AH10-AF10)</f>
+        <v>3849</v>
+      </c>
+      <c r="AH10" s="1">
+        <v>92885</v>
+      </c>
+      <c r="AI10">
+        <f>IF(ISBLANK(AJ10),-AH10,AJ10-AH10)</f>
+        <v>38767</v>
+      </c>
+      <c r="AJ10" s="1">
+        <v>131652</v>
+      </c>
       <c r="AK10" s="1"/>
       <c r="AL10" s="1"/>
       <c r="AM10" s="1"/>
     </row>
     <row r="11" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="D11" s="1">
-        <v>14802</v>
+        <v>118444</v>
       </c>
       <c r="E11">
         <f>IF(ISBLANK(F11),-D11,F11-D11)</f>
-        <v>156</v>
+        <v>45</v>
       </c>
       <c r="F11" s="1">
-        <v>14958</v>
+        <v>118489</v>
       </c>
       <c r="G11">
         <f>IF(ISBLANK(H11),-F11,H11-F11)</f>
-        <v>51</v>
+        <v>186</v>
       </c>
       <c r="H11" s="1">
-        <v>15009</v>
+        <v>118675</v>
       </c>
       <c r="I11">
         <f>IF(ISBLANK(J11),-H11,J11-H11)</f>
-        <v>198</v>
+        <v>98</v>
       </c>
       <c r="J11" s="1">
-        <v>15207</v>
+        <v>118773</v>
       </c>
       <c r="K11">
         <f>IF(ISBLANK(L11),-J11,L11-J11)</f>
-        <v>146</v>
+        <v>350</v>
       </c>
       <c r="L11" s="1">
-        <v>15353</v>
+        <v>119123</v>
       </c>
       <c r="M11">
         <f>IF(ISBLANK(N11),-L11,N11-L11)</f>
-        <v>41</v>
+        <v>257</v>
       </c>
       <c r="N11" s="1">
-        <v>15394</v>
+        <v>119380</v>
       </c>
       <c r="O11">
         <f>IF(ISBLANK(P11),-N11,P11-N11)</f>
-        <v>392</v>
+        <v>165</v>
       </c>
       <c r="P11" s="1">
-        <v>15786</v>
+        <v>119545</v>
       </c>
       <c r="Q11">
         <f>IF(ISBLANK(R11),-P11,R11-P11)</f>
-        <v>321</v>
+        <v>170</v>
       </c>
       <c r="R11" s="1">
-        <v>16107</v>
+        <v>119715</v>
       </c>
       <c r="S11">
         <f>IF(ISBLANK(T11),-R11,T11-R11)</f>
-        <v>101</v>
+        <v>168</v>
       </c>
       <c r="T11" s="1">
-        <v>16208</v>
+        <v>119883</v>
       </c>
       <c r="U11">
         <f>IF(ISBLANK(V11),-T11,V11-T11)</f>
-        <v>170</v>
+        <v>0</v>
       </c>
       <c r="V11" s="1">
-        <v>16378</v>
+        <v>119883</v>
       </c>
       <c r="W11">
         <f>IF(ISBLANK(X11),-V11,X11-V11)</f>
-        <v>530</v>
+        <v>0</v>
       </c>
       <c r="X11" s="1">
-        <v>16908</v>
+        <v>119883</v>
       </c>
       <c r="Y11">
         <f>IF(ISBLANK(Z11),-X11,Z11-X11)</f>
-        <v>490</v>
+        <v>0</v>
       </c>
       <c r="Z11" s="1">
-        <v>17398</v>
+        <v>119883</v>
       </c>
       <c r="AA11">
         <f>IF(ISBLANK(AB11),-Z11,AB11-Z11)</f>
-        <v>329</v>
+        <v>0</v>
       </c>
       <c r="AB11" s="1">
-        <v>17727</v>
+        <v>119883</v>
       </c>
       <c r="AC11">
         <f>IF(ISBLANK(AD11),-AB11,AD11-AB11)</f>
-        <v>749</v>
+        <v>0</v>
       </c>
       <c r="AD11" s="1">
-        <v>18476</v>
+        <v>119883</v>
       </c>
       <c r="AE11">
         <f>IF(ISBLANK(AF11),-AD11,AF11-AD11)</f>
-        <v>-18476</v>
+        <v>0</v>
       </c>
       <c r="AF11" s="1">
-        <v>0</v>
-      </c>
-      <c r="AG11" s="1"/>
-      <c r="AH11" s="1"/>
-      <c r="AI11" s="1"/>
-      <c r="AJ11" s="1"/>
+        <v>119883</v>
+      </c>
+      <c r="AG11">
+        <f>IF(ISBLANK(AH11),-AF11,AH11-AF11)</f>
+        <v>0</v>
+      </c>
+      <c r="AH11" s="1">
+        <v>119883</v>
+      </c>
+      <c r="AI11">
+        <f>IF(ISBLANK(AJ11),-AH11,AJ11-AH11)</f>
+        <v>0</v>
+      </c>
+      <c r="AJ11" s="1">
+        <v>119883</v>
+      </c>
       <c r="AK11" s="1"/>
       <c r="AL11" s="1"/>
       <c r="AM11" s="1"/>
     </row>
     <row r="12" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>134</v>
+        <v>145</v>
       </c>
       <c r="D12" s="1">
-        <v>10582</v>
+        <v>2395</v>
       </c>
       <c r="E12">
         <f>IF(ISBLANK(F12),-D12,F12-D12)</f>
-        <v>57</v>
+        <v>14</v>
       </c>
       <c r="F12" s="1">
-        <v>10639</v>
+        <v>2409</v>
       </c>
       <c r="G12">
         <f>IF(ISBLANK(H12),-F12,H12-F12)</f>
-        <v>106</v>
+        <v>-2409</v>
       </c>
       <c r="H12" s="1">
-        <v>10745</v>
+        <v>0</v>
       </c>
       <c r="I12">
         <f>IF(ISBLANK(J12),-H12,J12-H12)</f>
-        <v>138</v>
+        <v>0</v>
       </c>
       <c r="J12" s="1">
-        <v>10883</v>
+        <v>0</v>
       </c>
       <c r="K12">
         <f>IF(ISBLANK(L12),-J12,L12-J12)</f>
-        <v>54</v>
+        <v>0</v>
       </c>
       <c r="L12" s="1">
-        <v>10937</v>
+        <v>0</v>
       </c>
       <c r="M12">
         <f>IF(ISBLANK(N12),-L12,N12-L12)</f>
-        <v>300</v>
+        <v>0</v>
       </c>
       <c r="N12" s="1">
-        <v>11237</v>
+        <v>0</v>
       </c>
       <c r="O12">
         <f>IF(ISBLANK(P12),-N12,P12-N12)</f>
-        <v>159</v>
+        <v>0</v>
       </c>
       <c r="P12" s="1">
-        <v>11396</v>
+        <v>0</v>
       </c>
       <c r="Q12">
         <f>IF(ISBLANK(R12),-P12,R12-P12)</f>
-        <v>322</v>
+        <v>0</v>
       </c>
       <c r="R12" s="1">
-        <v>11718</v>
+        <v>0</v>
       </c>
       <c r="S12">
         <f>IF(ISBLANK(T12),-R12,T12-R12)</f>
-        <v>908</v>
+        <v>0</v>
       </c>
       <c r="T12" s="1">
-        <v>12626</v>
+        <v>0</v>
       </c>
       <c r="U12">
         <f>IF(ISBLANK(V12),-T12,V12-T12)</f>
-        <v>1585</v>
+        <v>0</v>
       </c>
       <c r="V12" s="1">
-        <v>14211</v>
+        <v>0</v>
       </c>
       <c r="W12">
         <f>IF(ISBLANK(X12),-V12,X12-V12)</f>
-        <v>826</v>
+        <v>0</v>
       </c>
       <c r="X12" s="1">
-        <v>15037</v>
+        <v>0</v>
       </c>
       <c r="Y12">
         <f>IF(ISBLANK(Z12),-X12,Z12-X12)</f>
-        <v>429</v>
+        <v>0</v>
       </c>
       <c r="Z12" s="1">
-        <v>15466</v>
+        <v>0</v>
       </c>
       <c r="AA12">
         <f>IF(ISBLANK(AB12),-Z12,AB12-Z12)</f>
-        <v>1664</v>
+        <v>0</v>
       </c>
       <c r="AB12" s="1">
-        <v>17130</v>
+        <v>0</v>
       </c>
       <c r="AC12">
         <f>IF(ISBLANK(AD12),-AB12,AD12-AB12)</f>
-        <v>-17130</v>
+        <v>0</v>
       </c>
       <c r="AD12" s="1">
         <v>0</v>
@@ -8917,103 +9153,113 @@
       <c r="AF12" s="1">
         <v>0</v>
       </c>
-      <c r="AG12" s="1"/>
-      <c r="AH12" s="1"/>
-      <c r="AI12" s="1"/>
-      <c r="AJ12" s="1"/>
+      <c r="AG12">
+        <f>IF(ISBLANK(AH12),-AF12,AH12-AF12)</f>
+        <v>0</v>
+      </c>
+      <c r="AH12" s="1">
+        <v>0</v>
+      </c>
+      <c r="AI12">
+        <f>IF(ISBLANK(AJ12),-AH12,AJ12-AH12)</f>
+        <v>0</v>
+      </c>
+      <c r="AJ12" s="1">
+        <v>0</v>
+      </c>
       <c r="AK12" s="1"/>
       <c r="AL12" s="1"/>
     </row>
     <row r="13" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D13" s="1">
-        <v>9823</v>
+        <v>9423</v>
       </c>
       <c r="E13">
         <f>IF(ISBLANK(F13),-D13,F13-D13)</f>
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="F13" s="1">
-        <v>9860</v>
+        <v>9455</v>
       </c>
       <c r="G13">
         <f>IF(ISBLANK(H13),-F13,H13-F13)</f>
-        <v>76</v>
+        <v>325</v>
       </c>
       <c r="H13" s="1">
-        <v>9936</v>
+        <v>9780</v>
       </c>
       <c r="I13">
         <f>IF(ISBLANK(J13),-H13,J13-H13)</f>
-        <v>54</v>
+        <v>75</v>
       </c>
       <c r="J13" s="1">
-        <v>9990</v>
+        <v>9855</v>
       </c>
       <c r="K13">
         <f>IF(ISBLANK(L13),-J13,L13-J13)</f>
-        <v>184</v>
+        <v>114</v>
       </c>
       <c r="L13" s="1">
-        <v>10174</v>
+        <v>9969</v>
       </c>
       <c r="M13">
         <f>IF(ISBLANK(N13),-L13,N13-L13)</f>
-        <v>52</v>
+        <v>280</v>
       </c>
       <c r="N13" s="1">
-        <v>10226</v>
+        <v>10249</v>
       </c>
       <c r="O13">
         <f>IF(ISBLANK(P13),-N13,P13-N13)</f>
-        <v>168</v>
+        <v>78</v>
       </c>
       <c r="P13" s="1">
-        <v>10394</v>
+        <v>10327</v>
       </c>
       <c r="Q13">
         <f>IF(ISBLANK(R13),-P13,R13-P13)</f>
-        <v>214</v>
+        <v>137</v>
       </c>
       <c r="R13" s="1">
-        <v>10608</v>
+        <v>10464</v>
       </c>
       <c r="S13">
         <f>IF(ISBLANK(T13),-R13,T13-R13)</f>
-        <v>48</v>
+        <v>79</v>
       </c>
       <c r="T13" s="1">
-        <v>10656</v>
+        <v>10543</v>
       </c>
       <c r="U13">
         <f>IF(ISBLANK(V13),-T13,V13-T13)</f>
-        <v>286</v>
+        <v>1160</v>
       </c>
       <c r="V13" s="1">
-        <v>10942</v>
+        <v>11703</v>
       </c>
       <c r="W13">
         <f>IF(ISBLANK(X13),-V13,X13-V13)</f>
-        <v>208</v>
+        <v>568</v>
       </c>
       <c r="X13" s="1">
-        <v>11150</v>
+        <v>12271</v>
       </c>
       <c r="Y13">
         <f>IF(ISBLANK(Z13),-X13,Z13-X13)</f>
-        <v>-11150</v>
+        <v>499</v>
       </c>
       <c r="Z13" s="1">
-        <v>0</v>
+        <v>12770</v>
       </c>
       <c r="AA13">
         <f>IF(ISBLANK(AB13),-Z13,AB13-Z13)</f>
-        <v>0</v>
+        <v>-12770</v>
       </c>
       <c r="AB13" s="1">
         <v>0</v>
@@ -9032,320 +9278,351 @@
       <c r="AF13" s="1">
         <v>0</v>
       </c>
-      <c r="AG13" s="1"/>
-      <c r="AH13" s="1"/>
-      <c r="AI13" s="1"/>
-      <c r="AJ13" s="1"/>
+      <c r="AG13">
+        <f>IF(ISBLANK(AH13),-AF13,AH13-AF13)</f>
+        <v>0</v>
+      </c>
+      <c r="AH13" s="1">
+        <v>0</v>
+      </c>
+      <c r="AI13">
+        <f>IF(ISBLANK(AJ13),-AH13,AJ13-AH13)</f>
+        <v>0</v>
+      </c>
+      <c r="AJ13" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="D14" s="1">
-        <v>9423</v>
+        <v>79072</v>
       </c>
       <c r="E14">
         <f>IF(ISBLANK(F14),-D14,F14-D14)</f>
-        <v>32</v>
+        <v>68</v>
       </c>
       <c r="F14" s="1">
-        <v>9455</v>
+        <v>79140</v>
       </c>
       <c r="G14">
         <f>IF(ISBLANK(H14),-F14,H14-F14)</f>
-        <v>325</v>
+        <v>142</v>
       </c>
       <c r="H14" s="1">
-        <v>9780</v>
+        <v>79282</v>
       </c>
       <c r="I14">
         <f>IF(ISBLANK(J14),-H14,J14-H14)</f>
-        <v>75</v>
+        <v>105</v>
       </c>
       <c r="J14" s="1">
-        <v>9855</v>
+        <v>79387</v>
       </c>
       <c r="K14">
         <f>IF(ISBLANK(L14),-J14,L14-J14)</f>
-        <v>114</v>
+        <v>186</v>
       </c>
       <c r="L14" s="1">
-        <v>9969</v>
+        <v>79573</v>
       </c>
       <c r="M14">
         <f>IF(ISBLANK(N14),-L14,N14-L14)</f>
-        <v>280</v>
+        <v>168</v>
       </c>
       <c r="N14" s="1">
-        <v>10249</v>
+        <v>79741</v>
       </c>
       <c r="O14">
         <f>IF(ISBLANK(P14),-N14,P14-N14)</f>
-        <v>78</v>
+        <v>204</v>
       </c>
       <c r="P14" s="1">
-        <v>10327</v>
+        <v>79945</v>
       </c>
       <c r="Q14">
         <f>IF(ISBLANK(R14),-P14,R14-P14)</f>
-        <v>137</v>
+        <v>305</v>
       </c>
       <c r="R14" s="1">
-        <v>10464</v>
+        <v>80250</v>
       </c>
       <c r="S14">
         <f>IF(ISBLANK(T14),-R14,T14-R14)</f>
-        <v>79</v>
+        <v>127</v>
       </c>
       <c r="T14" s="1">
-        <v>10543</v>
+        <v>80377</v>
       </c>
       <c r="U14">
         <f>IF(ISBLANK(V14),-T14,V14-T14)</f>
-        <v>1160</v>
+        <v>446</v>
       </c>
       <c r="V14" s="1">
-        <v>11703</v>
+        <v>80823</v>
       </c>
       <c r="W14">
         <f>IF(ISBLANK(X14),-V14,X14-V14)</f>
-        <v>568</v>
+        <v>991</v>
       </c>
       <c r="X14" s="1">
-        <v>12271</v>
+        <v>81814</v>
       </c>
       <c r="Y14">
         <f>IF(ISBLANK(Z14),-X14,Z14-X14)</f>
-        <v>499</v>
+        <v>1119</v>
       </c>
       <c r="Z14" s="1">
-        <v>12770</v>
+        <v>82933</v>
       </c>
       <c r="AA14">
         <f>IF(ISBLANK(AB14),-Z14,AB14-Z14)</f>
-        <v>-12770</v>
+        <v>958</v>
       </c>
       <c r="AB14" s="1">
-        <v>0</v>
+        <v>83891</v>
       </c>
       <c r="AC14">
         <f>IF(ISBLANK(AD14),-AB14,AD14-AB14)</f>
-        <v>0</v>
+        <v>1108</v>
       </c>
       <c r="AD14" s="1">
-        <v>0</v>
+        <v>84999</v>
       </c>
       <c r="AE14">
         <f>IF(ISBLANK(AF14),-AD14,AF14-AD14)</f>
-        <v>0</v>
+        <v>2323</v>
       </c>
       <c r="AF14" s="1">
-        <v>0</v>
-      </c>
-      <c r="AG14" s="1"/>
-      <c r="AH14" s="1"/>
-      <c r="AI14" s="1"/>
-      <c r="AJ14" s="1"/>
+        <v>87322</v>
+      </c>
+      <c r="AG14">
+        <f>IF(ISBLANK(AH14),-AF14,AH14-AF14)</f>
+        <v>4517</v>
+      </c>
+      <c r="AH14" s="1">
+        <v>91839</v>
+      </c>
+      <c r="AI14">
+        <f>IF(ISBLANK(AJ14),-AH14,AJ14-AH14)</f>
+        <v>3734</v>
+      </c>
+      <c r="AJ14" s="1">
+        <v>95573</v>
+      </c>
       <c r="AK14" s="1"/>
     </row>
     <row r="15" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="D15" s="1">
-        <v>9306</v>
+        <v>22075</v>
       </c>
       <c r="E15">
         <f>IF(ISBLANK(F15),-D15,F15-D15)</f>
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="F15" s="1">
-        <v>9331</v>
+        <v>22113</v>
       </c>
       <c r="G15">
         <f>IF(ISBLANK(H15),-F15,H15-F15)</f>
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="H15" s="1">
-        <v>9401</v>
+        <v>22193</v>
       </c>
       <c r="I15">
         <f>IF(ISBLANK(J15),-H15,J15-H15)</f>
-        <v>35</v>
+        <v>58</v>
       </c>
       <c r="J15" s="1">
-        <v>9436</v>
+        <v>22251</v>
       </c>
       <c r="K15">
         <f>IF(ISBLANK(L15),-J15,L15-J15)</f>
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="L15" s="1">
-        <v>9496</v>
+        <v>22321</v>
       </c>
       <c r="M15">
         <f>IF(ISBLANK(N15),-L15,N15-L15)</f>
-        <v>228</v>
+        <v>62</v>
       </c>
       <c r="N15" s="1">
-        <v>9724</v>
+        <v>22383</v>
       </c>
       <c r="O15">
         <f>IF(ISBLANK(P15),-N15,P15-N15)</f>
-        <v>145</v>
+        <v>70</v>
       </c>
       <c r="P15" s="1">
-        <v>9869</v>
+        <v>22453</v>
       </c>
       <c r="Q15">
         <f>IF(ISBLANK(R15),-P15,R15-P15)</f>
-        <v>106</v>
+        <v>173</v>
       </c>
       <c r="R15" s="1">
-        <v>9975</v>
+        <v>22626</v>
       </c>
       <c r="S15">
         <f>IF(ISBLANK(T15),-R15,T15-R15)</f>
-        <v>247</v>
+        <v>74</v>
       </c>
       <c r="T15" s="1">
-        <v>10222</v>
+        <v>22700</v>
       </c>
       <c r="U15">
         <f>IF(ISBLANK(V15),-T15,V15-T15)</f>
-        <v>616</v>
+        <v>193</v>
       </c>
       <c r="V15" s="1">
-        <v>10838</v>
+        <v>22893</v>
       </c>
       <c r="W15">
         <f>IF(ISBLANK(X15),-V15,X15-V15)</f>
-        <v>-10838</v>
+        <v>626</v>
       </c>
       <c r="X15" s="1">
-        <v>0</v>
+        <v>23519</v>
       </c>
       <c r="Y15">
         <f>IF(ISBLANK(Z15),-X15,Z15-X15)</f>
-        <v>0</v>
+        <v>330</v>
       </c>
       <c r="Z15" s="1">
-        <v>0</v>
+        <v>23849</v>
       </c>
       <c r="AA15">
         <f>IF(ISBLANK(AB15),-Z15,AB15-Z15)</f>
-        <v>0</v>
+        <v>483</v>
       </c>
       <c r="AB15" s="1">
-        <v>0</v>
+        <v>24332</v>
       </c>
       <c r="AC15">
         <f>IF(ISBLANK(AD15),-AB15,AD15-AB15)</f>
-        <v>0</v>
+        <v>600</v>
       </c>
       <c r="AD15" s="1">
-        <v>0</v>
+        <v>24932</v>
       </c>
       <c r="AE15">
         <f>IF(ISBLANK(AF15),-AD15,AF15-AD15)</f>
-        <v>0</v>
+        <v>1026</v>
       </c>
       <c r="AF15" s="1">
-        <v>0</v>
-      </c>
-      <c r="AG15" s="1"/>
-      <c r="AH15" s="1"/>
-      <c r="AI15" s="1"/>
+        <v>25958</v>
+      </c>
+      <c r="AG15">
+        <f>IF(ISBLANK(AH15),-AF15,AH15-AF15)</f>
+        <v>-25958</v>
+      </c>
+      <c r="AH15" s="1">
+        <v>0</v>
+      </c>
+      <c r="AI15">
+        <f>IF(ISBLANK(AJ15),-AH15,AJ15-AH15)</f>
+        <v>0</v>
+      </c>
+      <c r="AJ15" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D16" s="1">
-        <v>7475</v>
+        <v>9823</v>
       </c>
       <c r="E16">
         <f>IF(ISBLANK(F16),-D16,F16-D16)</f>
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="F16" s="1">
-        <v>7498</v>
+        <v>9860</v>
       </c>
       <c r="G16">
         <f>IF(ISBLANK(H16),-F16,H16-F16)</f>
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="H16" s="1">
-        <v>7596</v>
+        <v>9936</v>
       </c>
       <c r="I16">
         <f>IF(ISBLANK(J16),-H16,J16-H16)</f>
-        <v>142</v>
+        <v>54</v>
       </c>
       <c r="J16" s="1">
-        <v>7738</v>
+        <v>9990</v>
       </c>
       <c r="K16">
         <f>IF(ISBLANK(L16),-J16,L16-J16)</f>
-        <v>70</v>
+        <v>184</v>
       </c>
       <c r="L16" s="1">
-        <v>7808</v>
+        <v>10174</v>
       </c>
       <c r="M16">
         <f>IF(ISBLANK(N16),-L16,N16-L16)</f>
-        <v>197</v>
+        <v>52</v>
       </c>
       <c r="N16" s="1">
-        <v>8005</v>
+        <v>10226</v>
       </c>
       <c r="O16">
         <f>IF(ISBLANK(P16),-N16,P16-N16)</f>
-        <v>192</v>
+        <v>168</v>
       </c>
       <c r="P16" s="1">
-        <v>8197</v>
+        <v>10394</v>
       </c>
       <c r="Q16">
         <f>IF(ISBLANK(R16),-P16,R16-P16)</f>
-        <v>176</v>
+        <v>214</v>
       </c>
       <c r="R16" s="1">
-        <v>8373</v>
+        <v>10608</v>
       </c>
       <c r="S16">
         <f>IF(ISBLANK(T16),-R16,T16-R16)</f>
-        <v>188</v>
+        <v>48</v>
       </c>
       <c r="T16" s="1">
-        <v>8561</v>
+        <v>10656</v>
       </c>
       <c r="U16">
         <f>IF(ISBLANK(V16),-T16,V16-T16)</f>
-        <v>-8561</v>
+        <v>286</v>
       </c>
       <c r="V16" s="1">
-        <v>0</v>
+        <v>10942</v>
       </c>
       <c r="W16">
         <f>IF(ISBLANK(X16),-V16,X16-V16)</f>
-        <v>0</v>
+        <v>208</v>
       </c>
       <c r="X16" s="1">
-        <v>0</v>
+        <v>11150</v>
       </c>
       <c r="Y16">
         <f>IF(ISBLANK(Z16),-X16,Z16-X16)</f>
-        <v>0</v>
+        <v>-11150</v>
       </c>
       <c r="Z16" s="1">
         <v>0</v>
@@ -9371,71 +9648,83 @@
       <c r="AF16" s="1">
         <v>0</v>
       </c>
-      <c r="AG16" s="1"/>
-      <c r="AH16" s="1"/>
-    </row>
-    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AG16">
+        <f>IF(ISBLANK(AH16),-AF16,AH16-AF16)</f>
+        <v>0</v>
+      </c>
+      <c r="AH16" s="1">
+        <v>0</v>
+      </c>
+      <c r="AI16">
+        <f>IF(ISBLANK(AJ16),-AH16,AJ16-AH16)</f>
+        <v>0</v>
+      </c>
+      <c r="AJ16" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D17" s="1">
-        <v>4665</v>
+        <v>3682</v>
       </c>
       <c r="E17">
         <f>IF(ISBLANK(F17),-D17,F17-D17)</f>
-        <v>26</v>
+        <v>77</v>
       </c>
       <c r="F17" s="1">
-        <v>4691</v>
+        <v>3759</v>
       </c>
       <c r="G17">
         <f>IF(ISBLANK(H17),-F17,H17-F17)</f>
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H17" s="1">
-        <v>4734</v>
+        <v>3803</v>
       </c>
       <c r="I17">
         <f>IF(ISBLANK(J17),-H17,J17-H17)</f>
-        <v>57</v>
+        <v>116</v>
       </c>
       <c r="J17" s="1">
-        <v>4791</v>
+        <v>3919</v>
       </c>
       <c r="K17">
         <f>IF(ISBLANK(L17),-J17,L17-J17)</f>
-        <v>50</v>
+        <v>87</v>
       </c>
       <c r="L17" s="1">
-        <v>4841</v>
+        <v>4006</v>
       </c>
       <c r="M17">
         <f>IF(ISBLANK(N17),-L17,N17-L17)</f>
-        <v>115</v>
+        <v>41</v>
       </c>
       <c r="N17" s="1">
-        <v>4956</v>
+        <v>4047</v>
       </c>
       <c r="O17">
         <f>IF(ISBLANK(P17),-N17,P17-N17)</f>
-        <v>72</v>
+        <v>134</v>
       </c>
       <c r="P17" s="1">
-        <v>5028</v>
+        <v>4181</v>
       </c>
       <c r="Q17">
         <f>IF(ISBLANK(R17),-P17,R17-P17)</f>
-        <v>104</v>
+        <v>-4181</v>
       </c>
       <c r="R17" s="1">
-        <v>5132</v>
+        <v>0</v>
       </c>
       <c r="S17">
         <f>IF(ISBLANK(T17),-R17,T17-R17)</f>
-        <v>-5132</v>
+        <v>0</v>
       </c>
       <c r="T17" s="1">
         <v>0</v>
@@ -9482,165 +9771,192 @@
       <c r="AF17" s="1">
         <v>0</v>
       </c>
-      <c r="AG17" s="1"/>
-    </row>
-    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AG17">
+        <f>IF(ISBLANK(AH17),-AF17,AH17-AF17)</f>
+        <v>0</v>
+      </c>
+      <c r="AH17" s="1">
+        <v>0</v>
+      </c>
+      <c r="AI17">
+        <f>IF(ISBLANK(AJ17),-AH17,AJ17-AH17)</f>
+        <v>0</v>
+      </c>
+      <c r="AJ17" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="B18" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="D18" s="1">
-        <v>3682</v>
+        <v>75946</v>
       </c>
       <c r="E18">
         <f>IF(ISBLANK(F18),-D18,F18-D18)</f>
-        <v>77</v>
+        <v>100</v>
       </c>
       <c r="F18" s="1">
-        <v>3759</v>
+        <v>76046</v>
       </c>
       <c r="G18">
         <f>IF(ISBLANK(H18),-F18,H18-F18)</f>
-        <v>44</v>
+        <v>201</v>
       </c>
       <c r="H18" s="1">
-        <v>3803</v>
+        <v>76247</v>
       </c>
       <c r="I18">
         <f>IF(ISBLANK(J18),-H18,J18-H18)</f>
-        <v>116</v>
+        <v>126</v>
       </c>
       <c r="J18" s="1">
-        <v>3919</v>
+        <v>76373</v>
       </c>
       <c r="K18">
         <f>IF(ISBLANK(L18),-J18,L18-J18)</f>
-        <v>87</v>
+        <v>272</v>
       </c>
       <c r="L18" s="1">
-        <v>4006</v>
+        <v>76645</v>
       </c>
       <c r="M18">
         <f>IF(ISBLANK(N18),-L18,N18-L18)</f>
-        <v>41</v>
+        <v>74</v>
       </c>
       <c r="N18" s="1">
-        <v>4047</v>
+        <v>76719</v>
       </c>
       <c r="O18">
         <f>IF(ISBLANK(P18),-N18,P18-N18)</f>
-        <v>134</v>
+        <v>301</v>
       </c>
       <c r="P18" s="1">
-        <v>4181</v>
+        <v>77020</v>
       </c>
       <c r="Q18">
         <f>IF(ISBLANK(R18),-P18,R18-P18)</f>
-        <v>-4181</v>
+        <v>283</v>
       </c>
       <c r="R18" s="1">
-        <v>0</v>
+        <v>77303</v>
       </c>
       <c r="S18">
         <f>IF(ISBLANK(T18),-R18,T18-R18)</f>
-        <v>0</v>
+        <v>112</v>
       </c>
       <c r="T18" s="1">
-        <v>0</v>
+        <v>77415</v>
       </c>
       <c r="U18">
         <f>IF(ISBLANK(V18),-T18,V18-T18)</f>
-        <v>0</v>
+        <v>339</v>
       </c>
       <c r="V18" s="1">
-        <v>0</v>
+        <v>77754</v>
       </c>
       <c r="W18">
         <f>IF(ISBLANK(X18),-V18,X18-V18)</f>
-        <v>0</v>
+        <v>1066</v>
       </c>
       <c r="X18" s="1">
-        <v>0</v>
+        <v>78820</v>
       </c>
       <c r="Y18">
         <f>IF(ISBLANK(Z18),-X18,Z18-X18)</f>
-        <v>0</v>
+        <v>1295</v>
       </c>
       <c r="Z18" s="1">
-        <v>0</v>
+        <v>80115</v>
       </c>
       <c r="AA18">
         <f>IF(ISBLANK(AB18),-Z18,AB18-Z18)</f>
-        <v>0</v>
+        <v>593</v>
       </c>
       <c r="AB18" s="1">
-        <v>0</v>
+        <v>80708</v>
       </c>
       <c r="AC18">
         <f>IF(ISBLANK(AD18),-AB18,AD18-AB18)</f>
-        <v>0</v>
+        <v>1290</v>
       </c>
       <c r="AD18" s="1">
-        <v>0</v>
+        <v>81998</v>
       </c>
       <c r="AE18">
         <f>IF(ISBLANK(AF18),-AD18,AF18-AD18)</f>
-        <v>0</v>
+        <v>2743</v>
       </c>
       <c r="AF18" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:33" x14ac:dyDescent="0.25">
+        <v>84741</v>
+      </c>
+      <c r="AG18">
+        <f>IF(ISBLANK(AH18),-AF18,AH18-AF18)</f>
+        <v>8382</v>
+      </c>
+      <c r="AH18" s="1">
+        <v>93123</v>
+      </c>
+      <c r="AI18">
+        <f>IF(ISBLANK(AJ18),-AH18,AJ18-AH18)</f>
+        <v>2972</v>
+      </c>
+      <c r="AJ18" s="1">
+        <v>96095</v>
+      </c>
+    </row>
+    <row r="19" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D19" s="1">
-        <v>3286</v>
+        <v>2864</v>
       </c>
       <c r="E19">
         <f>IF(ISBLANK(F19),-D19,F19-D19)</f>
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="F19" s="1">
-        <v>3307</v>
+        <v>2898</v>
       </c>
       <c r="G19">
         <f>IF(ISBLANK(H19),-F19,H19-F19)</f>
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="H19" s="1">
-        <v>3320</v>
+        <v>2919</v>
       </c>
       <c r="I19">
         <f>IF(ISBLANK(J19),-H19,J19-H19)</f>
-        <v>232</v>
+        <v>148</v>
       </c>
       <c r="J19" s="1">
-        <v>3552</v>
+        <v>3067</v>
       </c>
       <c r="K19">
         <f>IF(ISBLANK(L19),-J19,L19-J19)</f>
-        <v>102</v>
+        <v>-3067</v>
       </c>
       <c r="L19" s="1">
-        <v>3654</v>
+        <v>0</v>
       </c>
       <c r="M19">
         <f>IF(ISBLANK(N19),-L19,N19-L19)</f>
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="N19" s="1">
-        <v>3714</v>
+        <v>0</v>
       </c>
       <c r="O19">
         <f>IF(ISBLANK(P19),-N19,P19-N19)</f>
-        <v>-3714</v>
+        <v>0</v>
       </c>
       <c r="P19" s="1">
         <v>0</v>
@@ -9701,48 +10017,62 @@
       <c r="AF19" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AG19">
+        <f>IF(ISBLANK(AH19),-AF19,AH19-AF19)</f>
+        <v>0</v>
+      </c>
+      <c r="AH19" s="1">
+        <v>0</v>
+      </c>
+      <c r="AI19">
+        <f>IF(ISBLANK(AJ19),-AH19,AJ19-AH19)</f>
+        <v>0</v>
+      </c>
+      <c r="AJ19" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B20" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D20" s="1">
-        <v>3182</v>
+        <v>2416</v>
       </c>
       <c r="E20">
         <f>IF(ISBLANK(F20),-D20,F20-D20)</f>
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="F20" s="1">
-        <v>3197</v>
+        <v>2464</v>
       </c>
       <c r="G20">
         <f>IF(ISBLANK(H20),-F20,H20-F20)</f>
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="H20" s="1">
-        <v>3257</v>
+        <v>2542</v>
       </c>
       <c r="I20">
         <f>IF(ISBLANK(J20),-H20,J20-H20)</f>
-        <v>43</v>
+        <v>-2542</v>
       </c>
       <c r="J20" s="1">
-        <v>3300</v>
+        <v>0</v>
       </c>
       <c r="K20">
         <f>IF(ISBLANK(L20),-J20,L20-J20)</f>
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="L20" s="1">
-        <v>3332</v>
+        <v>0</v>
       </c>
       <c r="M20">
         <f>IF(ISBLANK(N20),-L20,N20-L20)</f>
-        <v>-3332</v>
+        <v>0</v>
       </c>
       <c r="N20" s="1">
         <v>0</v>
@@ -9810,41 +10140,55 @@
       <c r="AF20" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AG20">
+        <f>IF(ISBLANK(AH20),-AF20,AH20-AF20)</f>
+        <v>0</v>
+      </c>
+      <c r="AH20" s="1">
+        <v>0</v>
+      </c>
+      <c r="AI20">
+        <f>IF(ISBLANK(AJ20),-AH20,AJ20-AH20)</f>
+        <v>0</v>
+      </c>
+      <c r="AJ20" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B21" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="D21" s="1">
-        <v>2864</v>
+        <v>1423</v>
       </c>
       <c r="E21">
         <f>IF(ISBLANK(F21),-D21,F21-D21)</f>
-        <v>34</v>
+        <v>-1423</v>
       </c>
       <c r="F21" s="1">
-        <v>2898</v>
+        <v>0</v>
       </c>
       <c r="G21">
         <f>IF(ISBLANK(H21),-F21,H21-F21)</f>
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="H21" s="1">
-        <v>2919</v>
+        <v>0</v>
       </c>
       <c r="I21">
         <f>IF(ISBLANK(J21),-H21,J21-H21)</f>
-        <v>148</v>
+        <v>0</v>
       </c>
       <c r="J21" s="1">
-        <v>3067</v>
+        <v>0</v>
       </c>
       <c r="K21">
         <f>IF(ISBLANK(L21),-J21,L21-J21)</f>
-        <v>-3067</v>
+        <v>0</v>
       </c>
       <c r="L21" s="1">
         <v>0</v>
@@ -9919,273 +10263,315 @@
       <c r="AF21" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AG21">
+        <f>IF(ISBLANK(AH21),-AF21,AH21-AF21)</f>
+        <v>0</v>
+      </c>
+      <c r="AH21" s="1">
+        <v>0</v>
+      </c>
+      <c r="AI21">
+        <f>IF(ISBLANK(AJ21),-AH21,AJ21-AH21)</f>
+        <v>0</v>
+      </c>
+      <c r="AJ21" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="B22" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="D22" s="1">
-        <v>2416</v>
+        <v>14802</v>
       </c>
       <c r="E22">
         <f>IF(ISBLANK(F22),-D22,F22-D22)</f>
-        <v>48</v>
+        <v>156</v>
       </c>
       <c r="F22" s="1">
-        <v>2464</v>
+        <v>14958</v>
       </c>
       <c r="G22">
         <f>IF(ISBLANK(H22),-F22,H22-F22)</f>
-        <v>78</v>
+        <v>51</v>
       </c>
       <c r="H22" s="1">
-        <v>2542</v>
+        <v>15009</v>
       </c>
       <c r="I22">
         <f>IF(ISBLANK(J22),-H22,J22-H22)</f>
-        <v>-2542</v>
+        <v>198</v>
       </c>
       <c r="J22" s="1">
-        <v>0</v>
+        <v>15207</v>
       </c>
       <c r="K22">
         <f>IF(ISBLANK(L22),-J22,L22-J22)</f>
-        <v>0</v>
+        <v>146</v>
       </c>
       <c r="L22" s="1">
-        <v>0</v>
+        <v>15353</v>
       </c>
       <c r="M22">
         <f>IF(ISBLANK(N22),-L22,N22-L22)</f>
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="N22" s="1">
-        <v>0</v>
+        <v>15394</v>
       </c>
       <c r="O22">
         <f>IF(ISBLANK(P22),-N22,P22-N22)</f>
-        <v>0</v>
+        <v>392</v>
       </c>
       <c r="P22" s="1">
-        <v>0</v>
+        <v>15786</v>
       </c>
       <c r="Q22">
         <f>IF(ISBLANK(R22),-P22,R22-P22)</f>
-        <v>0</v>
+        <v>321</v>
       </c>
       <c r="R22" s="1">
-        <v>0</v>
+        <v>16107</v>
       </c>
       <c r="S22">
         <f>IF(ISBLANK(T22),-R22,T22-R22)</f>
-        <v>0</v>
+        <v>101</v>
       </c>
       <c r="T22" s="1">
-        <v>0</v>
+        <v>16208</v>
       </c>
       <c r="U22">
         <f>IF(ISBLANK(V22),-T22,V22-T22)</f>
-        <v>0</v>
+        <v>170</v>
       </c>
       <c r="V22" s="1">
-        <v>0</v>
+        <v>16378</v>
       </c>
       <c r="W22">
         <f>IF(ISBLANK(X22),-V22,X22-V22)</f>
-        <v>0</v>
+        <v>530</v>
       </c>
       <c r="X22" s="1">
-        <v>0</v>
+        <v>16908</v>
       </c>
       <c r="Y22">
         <f>IF(ISBLANK(Z22),-X22,Z22-X22)</f>
-        <v>0</v>
+        <v>490</v>
       </c>
       <c r="Z22" s="1">
-        <v>0</v>
+        <v>17398</v>
       </c>
       <c r="AA22">
         <f>IF(ISBLANK(AB22),-Z22,AB22-Z22)</f>
-        <v>0</v>
+        <v>329</v>
       </c>
       <c r="AB22" s="1">
-        <v>0</v>
+        <v>17727</v>
       </c>
       <c r="AC22">
         <f>IF(ISBLANK(AD22),-AB22,AD22-AB22)</f>
-        <v>0</v>
+        <v>749</v>
       </c>
       <c r="AD22" s="1">
-        <v>0</v>
+        <v>18476</v>
       </c>
       <c r="AE22">
         <f>IF(ISBLANK(AF22),-AD22,AF22-AD22)</f>
-        <v>0</v>
+        <v>-18476</v>
       </c>
       <c r="AF22" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AG22">
+        <f>IF(ISBLANK(AH22),-AF22,AH22-AF22)</f>
+        <v>0</v>
+      </c>
+      <c r="AH22" s="1">
+        <v>0</v>
+      </c>
+      <c r="AI22">
+        <f>IF(ISBLANK(AJ22),-AH22,AJ22-AH22)</f>
+        <v>0</v>
+      </c>
+      <c r="AJ22" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="B23" t="s">
-        <v>145</v>
+        <v>126</v>
       </c>
       <c r="D23" s="1">
-        <v>2395</v>
+        <v>81741</v>
       </c>
       <c r="E23">
         <f>IF(ISBLANK(F23),-D23,F23-D23)</f>
-        <v>14</v>
+        <v>253</v>
       </c>
       <c r="F23" s="1">
-        <v>2409</v>
+        <v>81994</v>
       </c>
       <c r="G23">
         <f>IF(ISBLANK(H23),-F23,H23-F23)</f>
-        <v>-2409</v>
+        <v>130</v>
       </c>
       <c r="H23" s="1">
-        <v>0</v>
+        <v>82124</v>
       </c>
       <c r="I23">
         <f>IF(ISBLANK(J23),-H23,J23-H23)</f>
-        <v>0</v>
+        <v>211</v>
       </c>
       <c r="J23" s="1">
-        <v>0</v>
+        <v>82335</v>
       </c>
       <c r="K23">
         <f>IF(ISBLANK(L23),-J23,L23-J23)</f>
-        <v>0</v>
+        <v>323</v>
       </c>
       <c r="L23" s="1">
-        <v>0</v>
+        <v>82658</v>
       </c>
       <c r="M23">
         <f>IF(ISBLANK(N23),-L23,N23-L23)</f>
-        <v>0</v>
+        <v>206</v>
       </c>
       <c r="N23" s="1">
-        <v>0</v>
+        <v>82864</v>
       </c>
       <c r="O23">
         <f>IF(ISBLANK(P23),-N23,P23-N23)</f>
-        <v>0</v>
+        <v>556</v>
       </c>
       <c r="P23" s="1">
-        <v>0</v>
+        <v>83420</v>
       </c>
       <c r="Q23">
         <f>IF(ISBLANK(R23),-P23,R23-P23)</f>
-        <v>0</v>
+        <v>351</v>
       </c>
       <c r="R23" s="1">
-        <v>0</v>
+        <v>83771</v>
       </c>
       <c r="S23">
         <f>IF(ISBLANK(T23),-R23,T23-R23)</f>
-        <v>0</v>
+        <v>217</v>
       </c>
       <c r="T23" s="1">
-        <v>0</v>
+        <v>83988</v>
       </c>
       <c r="U23">
         <f>IF(ISBLANK(V23),-T23,V23-T23)</f>
-        <v>0</v>
+        <v>247</v>
       </c>
       <c r="V23" s="1">
-        <v>0</v>
+        <v>84235</v>
       </c>
       <c r="W23">
         <f>IF(ISBLANK(X23),-V23,X23-V23)</f>
-        <v>0</v>
+        <v>1001</v>
       </c>
       <c r="X23" s="1">
-        <v>0</v>
+        <v>85236</v>
       </c>
       <c r="Y23">
         <f>IF(ISBLANK(Z23),-X23,Z23-X23)</f>
-        <v>0</v>
+        <v>2333</v>
       </c>
       <c r="Z23" s="1">
-        <v>0</v>
+        <v>87569</v>
       </c>
       <c r="AA23">
         <f>IF(ISBLANK(AB23),-Z23,AB23-Z23)</f>
-        <v>0</v>
+        <v>1190</v>
       </c>
       <c r="AB23" s="1">
-        <v>0</v>
+        <v>88759</v>
       </c>
       <c r="AC23">
         <f>IF(ISBLANK(AD23),-AB23,AD23-AB23)</f>
-        <v>0</v>
+        <v>1476</v>
       </c>
       <c r="AD23" s="1">
-        <v>0</v>
+        <v>90235</v>
       </c>
       <c r="AE23">
         <f>IF(ISBLANK(AF23),-AD23,AF23-AD23)</f>
-        <v>0</v>
+        <v>5545</v>
       </c>
       <c r="AF23" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:33" x14ac:dyDescent="0.25">
+        <v>95780</v>
+      </c>
+      <c r="AG23">
+        <f>IF(ISBLANK(AH23),-AF23,AH23-AF23)</f>
+        <v>5945</v>
+      </c>
+      <c r="AH23" s="1">
+        <v>101725</v>
+      </c>
+      <c r="AI23">
+        <f>IF(ISBLANK(AJ23),-AH23,AJ23-AH23)</f>
+        <v>7424</v>
+      </c>
+      <c r="AJ23" s="1">
+        <v>109149</v>
+      </c>
+    </row>
+    <row r="24" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B24" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="D24" s="1">
-        <v>1423</v>
+        <v>3286</v>
       </c>
       <c r="E24">
         <f>IF(ISBLANK(F24),-D24,F24-D24)</f>
-        <v>-1423</v>
+        <v>21</v>
       </c>
       <c r="F24" s="1">
-        <v>0</v>
+        <v>3307</v>
       </c>
       <c r="G24">
         <f>IF(ISBLANK(H24),-F24,H24-F24)</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="H24" s="1">
-        <v>0</v>
+        <v>3320</v>
       </c>
       <c r="I24">
         <f>IF(ISBLANK(J24),-H24,J24-H24)</f>
-        <v>0</v>
+        <v>232</v>
       </c>
       <c r="J24" s="1">
-        <v>0</v>
+        <v>3552</v>
       </c>
       <c r="K24">
         <f>IF(ISBLANK(L24),-J24,L24-J24)</f>
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="L24" s="1">
-        <v>0</v>
+        <v>3654</v>
       </c>
       <c r="M24">
         <f>IF(ISBLANK(N24),-L24,N24-L24)</f>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="N24" s="1">
-        <v>0</v>
+        <v>3714</v>
       </c>
       <c r="O24">
         <f>IF(ISBLANK(P24),-N24,P24-N24)</f>
-        <v>0</v>
+        <v>-3714</v>
       </c>
       <c r="P24" s="1">
         <v>0</v>
@@ -10246,8 +10632,22 @@
       <c r="AF24" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AG24">
+        <f>IF(ISBLANK(AH24),-AF24,AH24-AF24)</f>
+        <v>0</v>
+      </c>
+      <c r="AH24" s="1">
+        <v>0</v>
+      </c>
+      <c r="AI24">
+        <f>IF(ISBLANK(AJ24),-AH24,AJ24-AH24)</f>
+        <v>0</v>
+      </c>
+      <c r="AJ24" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>147</v>
       </c>
@@ -10330,8 +10730,17 @@
       <c r="AD26" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="27" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AE26" t="s">
+        <v>258</v>
+      </c>
+      <c r="AF26" t="s">
+        <v>260</v>
+      </c>
+      <c r="AG26" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="27" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>148</v>
       </c>
@@ -10393,10 +10802,8 @@
       <c r="Y27" s="1">
         <v>119883</v>
       </c>
-      <c r="AE27" s="1"/>
-      <c r="AF27" s="1"/>
-    </row>
-    <row r="28" spans="1:33" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>149</v>
       </c>
@@ -10473,11 +10880,20 @@
       <c r="AD28" s="1">
         <v>88601</v>
       </c>
-      <c r="AE28" s="1"/>
-      <c r="AF28" s="1"/>
-      <c r="AG28" s="1"/>
-    </row>
-    <row r="29" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AE28" s="1">
+        <v>89036</v>
+      </c>
+      <c r="AF28" s="1">
+        <v>92885</v>
+      </c>
+      <c r="AG28" s="1">
+        <v>131652</v>
+      </c>
+      <c r="AH28" s="1"/>
+      <c r="AI28" s="1"/>
+      <c r="AJ28" s="1"/>
+    </row>
+    <row r="29" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>150</v>
       </c>
@@ -10554,11 +10970,20 @@
       <c r="AD29" s="1">
         <v>90235</v>
       </c>
-      <c r="AE29" s="1"/>
-      <c r="AF29" s="1"/>
-      <c r="AG29" s="1"/>
-    </row>
-    <row r="30" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AE29" s="1">
+        <v>95780</v>
+      </c>
+      <c r="AF29" s="1">
+        <v>101725</v>
+      </c>
+      <c r="AG29" s="1">
+        <v>109149</v>
+      </c>
+      <c r="AH29" s="1"/>
+      <c r="AI29" s="1"/>
+      <c r="AJ29" s="1"/>
+    </row>
+    <row r="30" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>151</v>
       </c>
@@ -10635,11 +11060,20 @@
       <c r="AD30" s="1">
         <v>84999</v>
       </c>
-      <c r="AE30" s="1"/>
-      <c r="AF30" s="1"/>
-      <c r="AG30" s="1"/>
-    </row>
-    <row r="31" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AE30" s="1">
+        <v>87322</v>
+      </c>
+      <c r="AF30" s="1">
+        <v>91839</v>
+      </c>
+      <c r="AG30" s="1">
+        <v>95573</v>
+      </c>
+      <c r="AH30" s="1"/>
+      <c r="AI30" s="1"/>
+      <c r="AJ30" s="1"/>
+    </row>
+    <row r="31" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>152</v>
       </c>
@@ -10716,11 +11150,20 @@
       <c r="AD31" s="1">
         <v>81998</v>
       </c>
-      <c r="AE31" s="1"/>
-      <c r="AF31" s="1"/>
-      <c r="AG31" s="1"/>
-    </row>
-    <row r="32" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AE31" s="1">
+        <v>84741</v>
+      </c>
+      <c r="AF31" s="1">
+        <v>93123</v>
+      </c>
+      <c r="AG31" s="1">
+        <v>96095</v>
+      </c>
+      <c r="AH31" s="1"/>
+      <c r="AI31" s="1"/>
+      <c r="AJ31" s="1"/>
+    </row>
+    <row r="32" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>153</v>
       </c>
@@ -10797,11 +11240,17 @@
       <c r="AD32" s="1">
         <v>73782</v>
       </c>
-      <c r="AE32" s="1"/>
-      <c r="AF32" s="1"/>
-      <c r="AG32" s="1"/>
-    </row>
-    <row r="33" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="AE32" s="1">
+        <v>74370</v>
+      </c>
+      <c r="AF32" s="1">
+        <v>80623</v>
+      </c>
+      <c r="AH32" s="1"/>
+      <c r="AI32" s="1"/>
+      <c r="AJ32" s="1"/>
+    </row>
+    <row r="33" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>154</v>
       </c>
@@ -10878,11 +11327,20 @@
       <c r="AD33" s="1">
         <v>69090</v>
       </c>
-      <c r="AE33" s="1"/>
-      <c r="AF33" s="1"/>
-      <c r="AG33" s="1"/>
-    </row>
-    <row r="34" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="AE33" s="1">
+        <v>69560</v>
+      </c>
+      <c r="AF33" s="1">
+        <v>89743</v>
+      </c>
+      <c r="AG33" s="1">
+        <v>97935</v>
+      </c>
+      <c r="AH33" s="1"/>
+      <c r="AI33" s="1"/>
+      <c r="AJ33" s="1"/>
+    </row>
+    <row r="34" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>155</v>
       </c>
@@ -10959,11 +11417,14 @@
       <c r="AD34" s="1">
         <v>41069</v>
       </c>
-      <c r="AE34" s="1"/>
-      <c r="AF34" s="1"/>
-      <c r="AG34" s="1"/>
-    </row>
-    <row r="35" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="AE34" s="1">
+        <v>41416</v>
+      </c>
+      <c r="AH34" s="1"/>
+      <c r="AI34" s="1"/>
+      <c r="AJ34" s="1"/>
+    </row>
+    <row r="35" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>156</v>
       </c>
@@ -11044,7 +11505,7 @@
       <c r="AF35" s="1"/>
       <c r="AG35" s="1"/>
     </row>
-    <row r="36" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>157</v>
       </c>
@@ -11125,7 +11586,7 @@
       <c r="AF36" s="1"/>
       <c r="AG36" s="1"/>
     </row>
-    <row r="37" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>158</v>
       </c>
@@ -11203,7 +11664,7 @@
       <c r="AF37" s="1"/>
       <c r="AG37" s="1"/>
     </row>
-    <row r="38" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>159</v>
       </c>
@@ -11275,7 +11736,7 @@
       <c r="AF38" s="1"/>
       <c r="AG38" s="1"/>
     </row>
-    <row r="39" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>160</v>
       </c>
@@ -11350,7 +11811,7 @@
       <c r="AF39" s="1"/>
       <c r="AG39" s="1"/>
     </row>
-    <row r="40" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>161</v>
       </c>
@@ -11423,7 +11884,7 @@
       <c r="AF40" s="1"/>
       <c r="AG40" s="1"/>
     </row>
-    <row r="41" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>162</v>
       </c>
@@ -11493,7 +11954,7 @@
       <c r="AE41" s="1"/>
       <c r="AF41" s="1"/>
     </row>
-    <row r="42" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>163</v>
       </c>
@@ -11559,7 +12020,7 @@
       <c r="AD42" s="1"/>
       <c r="AE42" s="1"/>
     </row>
-    <row r="43" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>164</v>
       </c>
@@ -11621,7 +12082,7 @@
       <c r="AC43" s="1"/>
       <c r="AD43" s="1"/>
     </row>
-    <row r="44" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>165</v>
       </c>
@@ -11679,7 +12140,7 @@
       <c r="AB44" s="1"/>
       <c r="AC44" s="1"/>
     </row>
-    <row r="45" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>166</v>
       </c>
@@ -11733,7 +12194,7 @@
       <c r="AA45" s="1"/>
       <c r="AB45" s="1"/>
     </row>
-    <row r="46" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>167</v>
       </c>
@@ -11779,7 +12240,7 @@
       </c>
       <c r="Z46" s="1"/>
     </row>
-    <row r="47" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>168</v>
       </c>
@@ -11818,7 +12279,7 @@
         <v>2542</v>
       </c>
     </row>
-    <row r="48" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>169</v>
       </c>
@@ -11860,8 +12321,8 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:AF24">
-    <sortCondition ref="A2:A24"/>
+  <sortState ref="A2:AJ24">
+    <sortCondition ref="B2:B24"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Stage 13 midlands added Signed-off-by: Gerry Mulvenna <git@movingwifi.com>
</commit_message>
<xml_diff>
--- a/europarl/europarl-ireland-2019.xlsx
+++ b/europarl/europarl-ireland-2019.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="262">
   <si>
     <t>Candidate</t>
   </si>
@@ -5165,15 +5165,15 @@
   <dimension ref="A1:AF37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="U2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="W2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Y2" sqref="Y2:Z18"/>
+      <selection pane="bottomRight" activeCell="AA2" sqref="AA2:AB18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>256</v>
       </c>
@@ -5216,8 +5216,11 @@
       <c r="Z1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AB1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>11</v>
       </c>
@@ -5285,7 +5288,7 @@
         <v>0</v>
       </c>
       <c r="U2">
-        <f t="shared" ref="U2:Y18" si="8">IF(ISBLANK(V2),-T2,V2-T2)</f>
+        <f t="shared" ref="U2:AA18" si="8">IF(ISBLANK(V2),-T2,V2-T2)</f>
         <v>0</v>
       </c>
       <c r="V2" s="1">
@@ -5305,8 +5308,15 @@
       <c r="Z2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA2">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AB2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
@@ -5394,8 +5404,15 @@
       <c r="Z3" s="1">
         <v>91396</v>
       </c>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA3">
+        <f t="shared" si="8"/>
+        <v>7336</v>
+      </c>
+      <c r="AB3" s="1">
+        <v>98732</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>5</v>
       </c>
@@ -5483,8 +5500,15 @@
       <c r="Z4" s="1">
         <v>69923</v>
       </c>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA4">
+        <f t="shared" si="8"/>
+        <v>-69923</v>
+      </c>
+      <c r="AB4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>9</v>
       </c>
@@ -5572,8 +5596,15 @@
       <c r="Z5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA5">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AB5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -5661,8 +5692,15 @@
       <c r="Z6" s="1">
         <v>112760</v>
       </c>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA6">
+        <f t="shared" si="8"/>
+        <v>9064</v>
+      </c>
+      <c r="AB6" s="1">
+        <v>121824</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>15</v>
       </c>
@@ -5750,8 +5788,15 @@
       <c r="Z7" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA7">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AB7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>10</v>
       </c>
@@ -5839,8 +5884,15 @@
       <c r="Z8" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA8">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AB8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>14</v>
       </c>
@@ -5928,8 +5980,15 @@
       <c r="Z9" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA9">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AB9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
@@ -6017,8 +6076,15 @@
       <c r="Z10">
         <v>118986</v>
       </c>
-    </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA10">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AB10">
+        <v>118986</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>6</v>
       </c>
@@ -6106,8 +6172,15 @@
       <c r="Z11" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA11">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AB11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>16</v>
       </c>
@@ -6195,8 +6268,15 @@
       <c r="Z12" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA12">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AB12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>17</v>
       </c>
@@ -6284,8 +6364,15 @@
       <c r="Z13" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA13">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AB13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -6373,8 +6460,15 @@
       <c r="Z14" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA14">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AB14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>12</v>
       </c>
@@ -6462,8 +6556,15 @@
       <c r="Z15" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA15">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AB15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>8</v>
       </c>
@@ -6551,6 +6652,13 @@
       <c r="Z16" s="1">
         <v>0</v>
       </c>
+      <c r="AA16">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AB16">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A17">
@@ -6640,6 +6748,13 @@
       <c r="Z17" s="1">
         <v>68677</v>
       </c>
+      <c r="AA17">
+        <f t="shared" si="8"/>
+        <v>-68677</v>
+      </c>
+      <c r="AB17">
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A18">
@@ -6728,6 +6843,13 @@
       </c>
       <c r="Z18" s="1">
         <v>96163</v>
+      </c>
+      <c r="AA18">
+        <f t="shared" si="8"/>
+        <v>11035</v>
+      </c>
+      <c r="AB18" s="1">
+        <v>107198</v>
       </c>
     </row>
     <row r="20" spans="1:32" x14ac:dyDescent="0.25">
@@ -7799,112 +7921,112 @@
         <v>4665</v>
       </c>
       <c r="E2">
-        <f>IF(ISBLANK(F2),-D2,F2-D2)</f>
+        <f t="shared" ref="E2:E24" si="0">IF(ISBLANK(F2),-D2,F2-D2)</f>
         <v>26</v>
       </c>
       <c r="F2" s="1">
         <v>4691</v>
       </c>
       <c r="G2">
-        <f>IF(ISBLANK(H2),-F2,H2-F2)</f>
+        <f t="shared" ref="G2:G24" si="1">IF(ISBLANK(H2),-F2,H2-F2)</f>
         <v>43</v>
       </c>
       <c r="H2" s="1">
         <v>4734</v>
       </c>
       <c r="I2">
-        <f>IF(ISBLANK(J2),-H2,J2-H2)</f>
+        <f t="shared" ref="I2:I24" si="2">IF(ISBLANK(J2),-H2,J2-H2)</f>
         <v>57</v>
       </c>
       <c r="J2" s="1">
         <v>4791</v>
       </c>
       <c r="K2">
-        <f>IF(ISBLANK(L2),-J2,L2-J2)</f>
+        <f t="shared" ref="K2:K24" si="3">IF(ISBLANK(L2),-J2,L2-J2)</f>
         <v>50</v>
       </c>
       <c r="L2" s="1">
         <v>4841</v>
       </c>
       <c r="M2">
-        <f>IF(ISBLANK(N2),-L2,N2-L2)</f>
+        <f t="shared" ref="M2:M24" si="4">IF(ISBLANK(N2),-L2,N2-L2)</f>
         <v>115</v>
       </c>
       <c r="N2" s="1">
         <v>4956</v>
       </c>
       <c r="O2">
-        <f>IF(ISBLANK(P2),-N2,P2-N2)</f>
+        <f t="shared" ref="O2:O24" si="5">IF(ISBLANK(P2),-N2,P2-N2)</f>
         <v>72</v>
       </c>
       <c r="P2" s="1">
         <v>5028</v>
       </c>
       <c r="Q2">
-        <f>IF(ISBLANK(R2),-P2,R2-P2)</f>
+        <f t="shared" ref="Q2:Q24" si="6">IF(ISBLANK(R2),-P2,R2-P2)</f>
         <v>104</v>
       </c>
       <c r="R2" s="1">
         <v>5132</v>
       </c>
       <c r="S2">
-        <f>IF(ISBLANK(T2),-R2,T2-R2)</f>
+        <f t="shared" ref="S2:S24" si="7">IF(ISBLANK(T2),-R2,T2-R2)</f>
         <v>-5132</v>
       </c>
       <c r="T2" s="1">
         <v>0</v>
       </c>
       <c r="U2">
-        <f>IF(ISBLANK(V2),-T2,V2-T2)</f>
+        <f t="shared" ref="U2:U24" si="8">IF(ISBLANK(V2),-T2,V2-T2)</f>
         <v>0</v>
       </c>
       <c r="V2" s="1">
         <v>0</v>
       </c>
       <c r="W2">
-        <f>IF(ISBLANK(X2),-V2,X2-V2)</f>
+        <f t="shared" ref="W2:W24" si="9">IF(ISBLANK(X2),-V2,X2-V2)</f>
         <v>0</v>
       </c>
       <c r="X2" s="1">
         <v>0</v>
       </c>
       <c r="Y2">
-        <f>IF(ISBLANK(Z2),-X2,Z2-X2)</f>
+        <f t="shared" ref="Y2:Y24" si="10">IF(ISBLANK(Z2),-X2,Z2-X2)</f>
         <v>0</v>
       </c>
       <c r="Z2" s="1">
         <v>0</v>
       </c>
       <c r="AA2">
-        <f>IF(ISBLANK(AB2),-Z2,AB2-Z2)</f>
+        <f t="shared" ref="AA2:AA24" si="11">IF(ISBLANK(AB2),-Z2,AB2-Z2)</f>
         <v>0</v>
       </c>
       <c r="AB2" s="1">
         <v>0</v>
       </c>
       <c r="AC2">
-        <f>IF(ISBLANK(AD2),-AB2,AD2-AB2)</f>
+        <f t="shared" ref="AC2:AC24" si="12">IF(ISBLANK(AD2),-AB2,AD2-AB2)</f>
         <v>0</v>
       </c>
       <c r="AD2" s="1">
         <v>0</v>
       </c>
       <c r="AE2">
-        <f>IF(ISBLANK(AF2),-AD2,AF2-AD2)</f>
+        <f t="shared" ref="AE2:AE24" si="13">IF(ISBLANK(AF2),-AD2,AF2-AD2)</f>
         <v>0</v>
       </c>
       <c r="AF2" s="1">
         <v>0</v>
       </c>
       <c r="AG2">
-        <f>IF(ISBLANK(AH2),-AF2,AH2-AF2)</f>
+        <f t="shared" ref="AG2:AG24" si="14">IF(ISBLANK(AH2),-AF2,AH2-AF2)</f>
         <v>0</v>
       </c>
       <c r="AH2" s="1">
         <v>0</v>
       </c>
       <c r="AI2">
-        <f>IF(ISBLANK(AJ2),-AH2,AJ2-AH2)</f>
+        <f t="shared" ref="AI2:AI24" si="15">IF(ISBLANK(AJ2),-AH2,AJ2-AH2)</f>
         <v>0</v>
       </c>
       <c r="AJ2" s="1">
@@ -7922,112 +8044,112 @@
         <v>69166</v>
       </c>
       <c r="E3">
-        <f>IF(ISBLANK(F3),-D3,F3-D3)</f>
+        <f t="shared" si="0"/>
         <v>35</v>
       </c>
       <c r="F3" s="1">
         <v>69201</v>
       </c>
       <c r="G3">
-        <f>IF(ISBLANK(H3),-F3,H3-F3)</f>
+        <f t="shared" si="1"/>
         <v>71</v>
       </c>
       <c r="H3" s="1">
         <v>69272</v>
       </c>
       <c r="I3">
-        <f>IF(ISBLANK(J3),-H3,J3-H3)</f>
+        <f t="shared" si="2"/>
         <v>44</v>
       </c>
       <c r="J3" s="1">
         <v>69316</v>
       </c>
       <c r="K3">
-        <f>IF(ISBLANK(L3),-J3,L3-J3)</f>
+        <f t="shared" si="3"/>
         <v>66</v>
       </c>
       <c r="L3" s="1">
         <v>69382</v>
       </c>
       <c r="M3">
-        <f>IF(ISBLANK(N3),-L3,N3-L3)</f>
+        <f t="shared" si="4"/>
         <v>129</v>
       </c>
       <c r="N3" s="1">
         <v>69511</v>
       </c>
       <c r="O3">
-        <f>IF(ISBLANK(P3),-N3,P3-N3)</f>
+        <f t="shared" si="5"/>
         <v>45</v>
       </c>
       <c r="P3" s="1">
         <v>69556</v>
       </c>
       <c r="Q3">
-        <f>IF(ISBLANK(R3),-P3,R3-P3)</f>
+        <f t="shared" si="6"/>
         <v>116</v>
       </c>
       <c r="R3" s="1">
         <v>69672</v>
       </c>
       <c r="S3">
-        <f>IF(ISBLANK(T3),-R3,T3-R3)</f>
+        <f t="shared" si="7"/>
         <v>1226</v>
       </c>
       <c r="T3" s="1">
         <v>70898</v>
       </c>
       <c r="U3">
-        <f>IF(ISBLANK(V3),-T3,V3-T3)</f>
+        <f t="shared" si="8"/>
         <v>270</v>
       </c>
       <c r="V3" s="1">
         <v>71168</v>
       </c>
       <c r="W3">
-        <f>IF(ISBLANK(X3),-V3,X3-V3)</f>
+        <f t="shared" si="9"/>
         <v>674</v>
       </c>
       <c r="X3" s="1">
         <v>71842</v>
       </c>
       <c r="Y3">
-        <f>IF(ISBLANK(Z3),-X3,Z3-X3)</f>
+        <f t="shared" si="10"/>
         <v>291</v>
       </c>
       <c r="Z3" s="1">
         <v>72133</v>
       </c>
       <c r="AA3">
-        <f>IF(ISBLANK(AB3),-Z3,AB3-Z3)</f>
+        <f t="shared" si="11"/>
         <v>720</v>
       </c>
       <c r="AB3" s="1">
         <v>72853</v>
       </c>
       <c r="AC3">
-        <f>IF(ISBLANK(AD3),-AB3,AD3-AB3)</f>
+        <f t="shared" si="12"/>
         <v>929</v>
       </c>
       <c r="AD3" s="1">
         <v>73782</v>
       </c>
       <c r="AE3">
-        <f>IF(ISBLANK(AF3),-AD3,AF3-AD3)</f>
+        <f t="shared" si="13"/>
         <v>588</v>
       </c>
       <c r="AF3" s="1">
         <v>74370</v>
       </c>
       <c r="AG3">
-        <f>IF(ISBLANK(AH3),-AF3,AH3-AF3)</f>
+        <f t="shared" si="14"/>
         <v>6253</v>
       </c>
       <c r="AH3" s="1">
         <v>80623</v>
       </c>
       <c r="AI3">
-        <f>IF(ISBLANK(AJ3),-AH3,AJ3-AH3)</f>
+        <f t="shared" si="15"/>
         <v>-80623</v>
       </c>
       <c r="AJ3" s="1">
@@ -8048,112 +8170,112 @@
         <v>10582</v>
       </c>
       <c r="E4">
-        <f>IF(ISBLANK(F4),-D4,F4-D4)</f>
+        <f t="shared" si="0"/>
         <v>57</v>
       </c>
       <c r="F4" s="1">
         <v>10639</v>
       </c>
       <c r="G4">
-        <f>IF(ISBLANK(H4),-F4,H4-F4)</f>
+        <f t="shared" si="1"/>
         <v>106</v>
       </c>
       <c r="H4" s="1">
         <v>10745</v>
       </c>
       <c r="I4">
-        <f>IF(ISBLANK(J4),-H4,J4-H4)</f>
+        <f t="shared" si="2"/>
         <v>138</v>
       </c>
       <c r="J4" s="1">
         <v>10883</v>
       </c>
       <c r="K4">
-        <f>IF(ISBLANK(L4),-J4,L4-J4)</f>
+        <f t="shared" si="3"/>
         <v>54</v>
       </c>
       <c r="L4" s="1">
         <v>10937</v>
       </c>
       <c r="M4">
-        <f>IF(ISBLANK(N4),-L4,N4-L4)</f>
+        <f t="shared" si="4"/>
         <v>300</v>
       </c>
       <c r="N4" s="1">
         <v>11237</v>
       </c>
       <c r="O4">
-        <f>IF(ISBLANK(P4),-N4,P4-N4)</f>
+        <f t="shared" si="5"/>
         <v>159</v>
       </c>
       <c r="P4" s="1">
         <v>11396</v>
       </c>
       <c r="Q4">
-        <f>IF(ISBLANK(R4),-P4,R4-P4)</f>
+        <f t="shared" si="6"/>
         <v>322</v>
       </c>
       <c r="R4" s="1">
         <v>11718</v>
       </c>
       <c r="S4">
-        <f>IF(ISBLANK(T4),-R4,T4-R4)</f>
+        <f t="shared" si="7"/>
         <v>908</v>
       </c>
       <c r="T4" s="1">
         <v>12626</v>
       </c>
       <c r="U4">
-        <f>IF(ISBLANK(V4),-T4,V4-T4)</f>
+        <f t="shared" si="8"/>
         <v>1585</v>
       </c>
       <c r="V4" s="1">
         <v>14211</v>
       </c>
       <c r="W4">
-        <f>IF(ISBLANK(X4),-V4,X4-V4)</f>
+        <f t="shared" si="9"/>
         <v>826</v>
       </c>
       <c r="X4" s="1">
         <v>15037</v>
       </c>
       <c r="Y4">
-        <f>IF(ISBLANK(Z4),-X4,Z4-X4)</f>
+        <f t="shared" si="10"/>
         <v>429</v>
       </c>
       <c r="Z4" s="1">
         <v>15466</v>
       </c>
       <c r="AA4">
-        <f>IF(ISBLANK(AB4),-Z4,AB4-Z4)</f>
+        <f t="shared" si="11"/>
         <v>1664</v>
       </c>
       <c r="AB4" s="1">
         <v>17130</v>
       </c>
       <c r="AC4">
-        <f>IF(ISBLANK(AD4),-AB4,AD4-AB4)</f>
+        <f t="shared" si="12"/>
         <v>-17130</v>
       </c>
       <c r="AD4" s="1">
         <v>0</v>
       </c>
       <c r="AE4">
-        <f>IF(ISBLANK(AF4),-AD4,AF4-AD4)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AF4" s="1">
         <v>0</v>
       </c>
       <c r="AG4">
-        <f>IF(ISBLANK(AH4),-AF4,AH4-AF4)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AH4" s="1">
         <v>0</v>
       </c>
       <c r="AI4">
-        <f>IF(ISBLANK(AJ4),-AH4,AJ4-AH4)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AJ4" s="1">
@@ -8174,112 +8296,112 @@
         <v>64605</v>
       </c>
       <c r="E5">
-        <f>IF(ISBLANK(F5),-D5,F5-D5)</f>
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="F5" s="1">
         <v>64631</v>
       </c>
       <c r="G5">
-        <f>IF(ISBLANK(H5),-F5,H5-F5)</f>
+        <f t="shared" si="1"/>
         <v>61</v>
       </c>
       <c r="H5" s="1">
         <v>64692</v>
       </c>
       <c r="I5">
-        <f>IF(ISBLANK(J5),-H5,J5-H5)</f>
+        <f t="shared" si="2"/>
         <v>71</v>
       </c>
       <c r="J5" s="1">
         <v>64763</v>
       </c>
       <c r="K5">
-        <f>IF(ISBLANK(L5),-J5,L5-J5)</f>
+        <f t="shared" si="3"/>
         <v>136</v>
       </c>
       <c r="L5" s="1">
         <v>64899</v>
       </c>
       <c r="M5">
-        <f>IF(ISBLANK(N5),-L5,N5-L5)</f>
+        <f t="shared" si="4"/>
         <v>106</v>
       </c>
       <c r="N5" s="1">
         <v>65005</v>
       </c>
       <c r="O5">
-        <f>IF(ISBLANK(P5),-N5,P5-N5)</f>
+        <f t="shared" si="5"/>
         <v>110</v>
       </c>
       <c r="P5" s="1">
         <v>65115</v>
       </c>
       <c r="Q5">
-        <f>IF(ISBLANK(R5),-P5,R5-P5)</f>
+        <f t="shared" si="6"/>
         <v>137</v>
       </c>
       <c r="R5" s="1">
         <v>65252</v>
       </c>
       <c r="S5">
-        <f>IF(ISBLANK(T5),-R5,T5-R5)</f>
+        <f t="shared" si="7"/>
         <v>306</v>
       </c>
       <c r="T5" s="1">
         <v>65558</v>
       </c>
       <c r="U5">
-        <f>IF(ISBLANK(V5),-T5,V5-T5)</f>
+        <f t="shared" si="8"/>
         <v>491</v>
       </c>
       <c r="V5" s="1">
         <v>66049</v>
       </c>
       <c r="W5">
-        <f>IF(ISBLANK(X5),-V5,X5-V5)</f>
+        <f t="shared" si="9"/>
         <v>683</v>
       </c>
       <c r="X5" s="1">
         <v>66732</v>
       </c>
       <c r="Y5">
-        <f>IF(ISBLANK(Z5),-X5,Z5-X5)</f>
+        <f t="shared" si="10"/>
         <v>542</v>
       </c>
       <c r="Z5" s="1">
         <v>67274</v>
       </c>
       <c r="AA5">
-        <f>IF(ISBLANK(AB5),-Z5,AB5-Z5)</f>
+        <f t="shared" si="11"/>
         <v>622</v>
       </c>
       <c r="AB5" s="1">
         <v>67896</v>
       </c>
       <c r="AC5">
-        <f>IF(ISBLANK(AD5),-AB5,AD5-AB5)</f>
+        <f t="shared" si="12"/>
         <v>1194</v>
       </c>
       <c r="AD5" s="1">
         <v>69090</v>
       </c>
       <c r="AE5">
-        <f>IF(ISBLANK(AF5),-AD5,AF5-AD5)</f>
+        <f t="shared" si="13"/>
         <v>470</v>
       </c>
       <c r="AF5" s="1">
         <v>69560</v>
       </c>
       <c r="AG5">
-        <f>IF(ISBLANK(AH5),-AF5,AH5-AF5)</f>
+        <f t="shared" si="14"/>
         <v>20183</v>
       </c>
       <c r="AH5" s="1">
         <v>89743</v>
       </c>
       <c r="AI5">
-        <f>IF(ISBLANK(AJ5),-AH5,AJ5-AH5)</f>
+        <f t="shared" si="15"/>
         <v>8192</v>
       </c>
       <c r="AJ5" s="1">
@@ -8300,112 +8422,112 @@
         <v>38738</v>
       </c>
       <c r="E6">
-        <f>IF(ISBLANK(F6),-D6,F6-D6)</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="F6" s="1">
         <v>38755</v>
       </c>
       <c r="G6">
-        <f>IF(ISBLANK(H6),-F6,H6-F6)</f>
+        <f t="shared" si="1"/>
         <v>33</v>
       </c>
       <c r="H6" s="1">
         <v>38788</v>
       </c>
       <c r="I6">
-        <f>IF(ISBLANK(J6),-H6,J6-H6)</f>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="J6" s="1">
         <v>38804</v>
       </c>
       <c r="K6">
-        <f>IF(ISBLANK(L6),-J6,L6-J6)</f>
+        <f t="shared" si="3"/>
         <v>38</v>
       </c>
       <c r="L6" s="1">
         <v>38842</v>
       </c>
       <c r="M6">
-        <f>IF(ISBLANK(N6),-L6,N6-L6)</f>
+        <f t="shared" si="4"/>
         <v>84</v>
       </c>
       <c r="N6" s="1">
         <v>38926</v>
       </c>
       <c r="O6">
-        <f>IF(ISBLANK(P6),-N6,P6-N6)</f>
+        <f t="shared" si="5"/>
         <v>24</v>
       </c>
       <c r="P6" s="1">
         <v>38950</v>
       </c>
       <c r="Q6">
-        <f>IF(ISBLANK(R6),-P6,R6-P6)</f>
+        <f t="shared" si="6"/>
         <v>46</v>
       </c>
       <c r="R6" s="1">
         <v>38996</v>
       </c>
       <c r="S6">
-        <f>IF(ISBLANK(T6),-R6,T6-R6)</f>
+        <f t="shared" si="7"/>
         <v>298</v>
       </c>
       <c r="T6" s="1">
         <v>39294</v>
       </c>
       <c r="U6">
-        <f>IF(ISBLANK(V6),-T6,V6-T6)</f>
+        <f t="shared" si="8"/>
         <v>135</v>
       </c>
       <c r="V6" s="1">
         <v>39429</v>
       </c>
       <c r="W6">
-        <f>IF(ISBLANK(X6),-V6,X6-V6)</f>
+        <f t="shared" si="9"/>
         <v>426</v>
       </c>
       <c r="X6" s="1">
         <v>39855</v>
       </c>
       <c r="Y6">
-        <f>IF(ISBLANK(Z6),-X6,Z6-X6)</f>
+        <f t="shared" si="10"/>
         <v>159</v>
       </c>
       <c r="Z6" s="1">
         <v>40014</v>
       </c>
       <c r="AA6">
-        <f>IF(ISBLANK(AB6),-Z6,AB6-Z6)</f>
+        <f t="shared" si="11"/>
         <v>572</v>
       </c>
       <c r="AB6" s="1">
         <v>40586</v>
       </c>
       <c r="AC6">
-        <f>IF(ISBLANK(AD6),-AB6,AD6-AB6)</f>
+        <f t="shared" si="12"/>
         <v>483</v>
       </c>
       <c r="AD6" s="1">
         <v>41069</v>
       </c>
       <c r="AE6">
-        <f>IF(ISBLANK(AF6),-AD6,AF6-AD6)</f>
+        <f t="shared" si="13"/>
         <v>347</v>
       </c>
       <c r="AF6" s="1">
         <v>41416</v>
       </c>
       <c r="AG6">
-        <f>IF(ISBLANK(AH6),-AF6,AH6-AF6)</f>
+        <f t="shared" si="14"/>
         <v>-41416</v>
       </c>
       <c r="AH6" s="1">
         <v>0</v>
       </c>
       <c r="AI6">
-        <f>IF(ISBLANK(AJ6),-AH6,AJ6-AH6)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AJ6" s="1">
@@ -8426,112 +8548,112 @@
         <v>3182</v>
       </c>
       <c r="E7">
-        <f>IF(ISBLANK(F7),-D7,F7-D7)</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="F7" s="1">
         <v>3197</v>
       </c>
       <c r="G7">
-        <f>IF(ISBLANK(H7),-F7,H7-F7)</f>
+        <f t="shared" si="1"/>
         <v>60</v>
       </c>
       <c r="H7" s="1">
         <v>3257</v>
       </c>
       <c r="I7">
-        <f>IF(ISBLANK(J7),-H7,J7-H7)</f>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="J7" s="1">
         <v>3300</v>
       </c>
       <c r="K7">
-        <f>IF(ISBLANK(L7),-J7,L7-J7)</f>
+        <f t="shared" si="3"/>
         <v>32</v>
       </c>
       <c r="L7" s="1">
         <v>3332</v>
       </c>
       <c r="M7">
-        <f>IF(ISBLANK(N7),-L7,N7-L7)</f>
+        <f t="shared" si="4"/>
         <v>-3332</v>
       </c>
       <c r="N7" s="1">
         <v>0</v>
       </c>
       <c r="O7">
-        <f>IF(ISBLANK(P7),-N7,P7-N7)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P7" s="1">
         <v>0</v>
       </c>
       <c r="Q7">
-        <f>IF(ISBLANK(R7),-P7,R7-P7)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="R7" s="1">
         <v>0</v>
       </c>
       <c r="S7">
-        <f>IF(ISBLANK(T7),-R7,T7-R7)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="T7" s="1">
         <v>0</v>
       </c>
       <c r="U7">
-        <f>IF(ISBLANK(V7),-T7,V7-T7)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="V7" s="1">
         <v>0</v>
       </c>
       <c r="W7">
-        <f>IF(ISBLANK(X7),-V7,X7-V7)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="X7" s="1">
         <v>0</v>
       </c>
       <c r="Y7">
-        <f>IF(ISBLANK(Z7),-X7,Z7-X7)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Z7" s="1">
         <v>0</v>
       </c>
       <c r="AA7">
-        <f>IF(ISBLANK(AB7),-Z7,AB7-Z7)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AB7" s="1">
         <v>0</v>
       </c>
       <c r="AC7">
-        <f>IF(ISBLANK(AD7),-AB7,AD7-AB7)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AD7" s="1">
         <v>0</v>
       </c>
       <c r="AE7">
-        <f>IF(ISBLANK(AF7),-AD7,AF7-AD7)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AF7" s="1">
         <v>0</v>
       </c>
       <c r="AG7">
-        <f>IF(ISBLANK(AH7),-AF7,AH7-AF7)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AH7" s="1">
         <v>0</v>
       </c>
       <c r="AI7">
-        <f>IF(ISBLANK(AJ7),-AH7,AJ7-AH7)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AJ7" s="1">
@@ -8552,112 +8674,112 @@
         <v>9306</v>
       </c>
       <c r="E8">
-        <f>IF(ISBLANK(F8),-D8,F8-D8)</f>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="F8" s="1">
         <v>9331</v>
       </c>
       <c r="G8">
-        <f>IF(ISBLANK(H8),-F8,H8-F8)</f>
+        <f t="shared" si="1"/>
         <v>70</v>
       </c>
       <c r="H8" s="1">
         <v>9401</v>
       </c>
       <c r="I8">
-        <f>IF(ISBLANK(J8),-H8,J8-H8)</f>
+        <f t="shared" si="2"/>
         <v>35</v>
       </c>
       <c r="J8" s="1">
         <v>9436</v>
       </c>
       <c r="K8">
-        <f>IF(ISBLANK(L8),-J8,L8-J8)</f>
+        <f t="shared" si="3"/>
         <v>60</v>
       </c>
       <c r="L8" s="1">
         <v>9496</v>
       </c>
       <c r="M8">
-        <f>IF(ISBLANK(N8),-L8,N8-L8)</f>
+        <f t="shared" si="4"/>
         <v>228</v>
       </c>
       <c r="N8" s="1">
         <v>9724</v>
       </c>
       <c r="O8">
-        <f>IF(ISBLANK(P8),-N8,P8-N8)</f>
+        <f t="shared" si="5"/>
         <v>145</v>
       </c>
       <c r="P8" s="1">
         <v>9869</v>
       </c>
       <c r="Q8">
-        <f>IF(ISBLANK(R8),-P8,R8-P8)</f>
+        <f t="shared" si="6"/>
         <v>106</v>
       </c>
       <c r="R8" s="1">
         <v>9975</v>
       </c>
       <c r="S8">
-        <f>IF(ISBLANK(T8),-R8,T8-R8)</f>
+        <f t="shared" si="7"/>
         <v>247</v>
       </c>
       <c r="T8" s="1">
         <v>10222</v>
       </c>
       <c r="U8">
-        <f>IF(ISBLANK(V8),-T8,V8-T8)</f>
+        <f t="shared" si="8"/>
         <v>616</v>
       </c>
       <c r="V8" s="1">
         <v>10838</v>
       </c>
       <c r="W8">
-        <f>IF(ISBLANK(X8),-V8,X8-V8)</f>
+        <f t="shared" si="9"/>
         <v>-10838</v>
       </c>
       <c r="X8" s="1">
         <v>0</v>
       </c>
       <c r="Y8">
-        <f>IF(ISBLANK(Z8),-X8,Z8-X8)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Z8" s="1">
         <v>0</v>
       </c>
       <c r="AA8">
-        <f>IF(ISBLANK(AB8),-Z8,AB8-Z8)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AB8" s="1">
         <v>0</v>
       </c>
       <c r="AC8">
-        <f>IF(ISBLANK(AD8),-AB8,AD8-AB8)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AD8" s="1">
         <v>0</v>
       </c>
       <c r="AE8">
-        <f>IF(ISBLANK(AF8),-AD8,AF8-AD8)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AF8" s="1">
         <v>0</v>
       </c>
       <c r="AG8">
-        <f>IF(ISBLANK(AH8),-AF8,AH8-AF8)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AH8" s="1">
         <v>0</v>
       </c>
       <c r="AI8">
-        <f>IF(ISBLANK(AJ8),-AH8,AJ8-AH8)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AJ8" s="1">
@@ -8678,112 +8800,112 @@
         <v>7475</v>
       </c>
       <c r="E9">
-        <f>IF(ISBLANK(F9),-D9,F9-D9)</f>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="F9" s="1">
         <v>7498</v>
       </c>
       <c r="G9">
-        <f>IF(ISBLANK(H9),-F9,H9-F9)</f>
+        <f t="shared" si="1"/>
         <v>98</v>
       </c>
       <c r="H9" s="1">
         <v>7596</v>
       </c>
       <c r="I9">
-        <f>IF(ISBLANK(J9),-H9,J9-H9)</f>
+        <f t="shared" si="2"/>
         <v>142</v>
       </c>
       <c r="J9" s="1">
         <v>7738</v>
       </c>
       <c r="K9">
-        <f>IF(ISBLANK(L9),-J9,L9-J9)</f>
+        <f t="shared" si="3"/>
         <v>70</v>
       </c>
       <c r="L9" s="1">
         <v>7808</v>
       </c>
       <c r="M9">
-        <f>IF(ISBLANK(N9),-L9,N9-L9)</f>
+        <f t="shared" si="4"/>
         <v>197</v>
       </c>
       <c r="N9" s="1">
         <v>8005</v>
       </c>
       <c r="O9">
-        <f>IF(ISBLANK(P9),-N9,P9-N9)</f>
+        <f t="shared" si="5"/>
         <v>192</v>
       </c>
       <c r="P9" s="1">
         <v>8197</v>
       </c>
       <c r="Q9">
-        <f>IF(ISBLANK(R9),-P9,R9-P9)</f>
+        <f t="shared" si="6"/>
         <v>176</v>
       </c>
       <c r="R9" s="1">
         <v>8373</v>
       </c>
       <c r="S9">
-        <f>IF(ISBLANK(T9),-R9,T9-R9)</f>
+        <f t="shared" si="7"/>
         <v>188</v>
       </c>
       <c r="T9" s="1">
         <v>8561</v>
       </c>
       <c r="U9">
-        <f>IF(ISBLANK(V9),-T9,V9-T9)</f>
+        <f t="shared" si="8"/>
         <v>-8561</v>
       </c>
       <c r="V9" s="1">
         <v>0</v>
       </c>
       <c r="W9">
-        <f>IF(ISBLANK(X9),-V9,X9-V9)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="X9" s="1">
         <v>0</v>
       </c>
       <c r="Y9">
-        <f>IF(ISBLANK(Z9),-X9,Z9-X9)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Z9" s="1">
         <v>0</v>
       </c>
       <c r="AA9">
-        <f>IF(ISBLANK(AB9),-Z9,AB9-Z9)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AB9" s="1">
         <v>0</v>
       </c>
       <c r="AC9">
-        <f>IF(ISBLANK(AD9),-AB9,AD9-AB9)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AD9" s="1">
         <v>0</v>
       </c>
       <c r="AE9">
-        <f>IF(ISBLANK(AF9),-AD9,AF9-AD9)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AF9" s="1">
         <v>0</v>
       </c>
       <c r="AG9">
-        <f>IF(ISBLANK(AH9),-AF9,AH9-AF9)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AH9" s="1">
         <v>0</v>
       </c>
       <c r="AI9">
-        <f>IF(ISBLANK(AJ9),-AH9,AJ9-AH9)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AJ9" s="1">
@@ -8804,112 +8926,112 @@
         <v>84083</v>
       </c>
       <c r="E10">
-        <f>IF(ISBLANK(F10),-D10,F10-D10)</f>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="F10" s="1">
         <v>84106</v>
       </c>
       <c r="G10">
-        <f>IF(ISBLANK(H10),-F10,H10-F10)</f>
+        <f t="shared" si="1"/>
         <v>58</v>
       </c>
       <c r="H10" s="1">
         <v>84164</v>
       </c>
       <c r="I10">
-        <f>IF(ISBLANK(J10),-H10,J10-H10)</f>
+        <f t="shared" si="2"/>
         <v>74</v>
       </c>
       <c r="J10" s="1">
         <v>84238</v>
       </c>
       <c r="K10">
-        <f>IF(ISBLANK(L10),-J10,L10-J10)</f>
+        <f t="shared" si="3"/>
         <v>150</v>
       </c>
       <c r="L10" s="1">
         <v>84388</v>
       </c>
       <c r="M10">
-        <f>IF(ISBLANK(N10),-L10,N10-L10)</f>
+        <f t="shared" si="4"/>
         <v>171</v>
       </c>
       <c r="N10" s="1">
         <v>84559</v>
       </c>
       <c r="O10">
-        <f>IF(ISBLANK(P10),-N10,P10-N10)</f>
+        <f t="shared" si="5"/>
         <v>95</v>
       </c>
       <c r="P10" s="1">
         <v>84654</v>
       </c>
       <c r="Q10">
-        <f>IF(ISBLANK(R10),-P10,R10-P10)</f>
+        <f t="shared" si="6"/>
         <v>187</v>
       </c>
       <c r="R10" s="1">
         <v>84841</v>
       </c>
       <c r="S10">
-        <f>IF(ISBLANK(T10),-R10,T10-R10)</f>
+        <f t="shared" si="7"/>
         <v>130</v>
       </c>
       <c r="T10" s="1">
         <v>84971</v>
       </c>
       <c r="U10">
-        <f>IF(ISBLANK(V10),-T10,V10-T10)</f>
+        <f t="shared" si="8"/>
         <v>480</v>
       </c>
       <c r="V10" s="1">
         <v>85451</v>
       </c>
       <c r="W10">
-        <f>IF(ISBLANK(X10),-V10,X10-V10)</f>
+        <f t="shared" si="9"/>
         <v>575</v>
       </c>
       <c r="X10" s="1">
         <v>86026</v>
       </c>
       <c r="Y10">
-        <f>IF(ISBLANK(Z10),-X10,Z10-X10)</f>
+        <f t="shared" si="10"/>
         <v>1010</v>
       </c>
       <c r="Z10" s="1">
         <v>87036</v>
       </c>
       <c r="AA10">
-        <f>IF(ISBLANK(AB10),-Z10,AB10-Z10)</f>
+        <f t="shared" si="11"/>
         <v>928</v>
       </c>
       <c r="AB10" s="1">
         <v>87964</v>
       </c>
       <c r="AC10">
-        <f>IF(ISBLANK(AD10),-AB10,AD10-AB10)</f>
+        <f t="shared" si="12"/>
         <v>637</v>
       </c>
       <c r="AD10" s="1">
         <v>88601</v>
       </c>
       <c r="AE10">
-        <f>IF(ISBLANK(AF10),-AD10,AF10-AD10)</f>
+        <f t="shared" si="13"/>
         <v>435</v>
       </c>
       <c r="AF10" s="1">
         <v>89036</v>
       </c>
       <c r="AG10">
-        <f>IF(ISBLANK(AH10),-AF10,AH10-AF10)</f>
+        <f t="shared" si="14"/>
         <v>3849</v>
       </c>
       <c r="AH10" s="1">
         <v>92885</v>
       </c>
       <c r="AI10">
-        <f>IF(ISBLANK(AJ10),-AH10,AJ10-AH10)</f>
+        <f t="shared" si="15"/>
         <v>38767</v>
       </c>
       <c r="AJ10" s="1">
@@ -8930,112 +9052,112 @@
         <v>118444</v>
       </c>
       <c r="E11">
-        <f>IF(ISBLANK(F11),-D11,F11-D11)</f>
+        <f t="shared" si="0"/>
         <v>45</v>
       </c>
       <c r="F11" s="1">
         <v>118489</v>
       </c>
       <c r="G11">
-        <f>IF(ISBLANK(H11),-F11,H11-F11)</f>
+        <f t="shared" si="1"/>
         <v>186</v>
       </c>
       <c r="H11" s="1">
         <v>118675</v>
       </c>
       <c r="I11">
-        <f>IF(ISBLANK(J11),-H11,J11-H11)</f>
+        <f t="shared" si="2"/>
         <v>98</v>
       </c>
       <c r="J11" s="1">
         <v>118773</v>
       </c>
       <c r="K11">
-        <f>IF(ISBLANK(L11),-J11,L11-J11)</f>
+        <f t="shared" si="3"/>
         <v>350</v>
       </c>
       <c r="L11" s="1">
         <v>119123</v>
       </c>
       <c r="M11">
-        <f>IF(ISBLANK(N11),-L11,N11-L11)</f>
+        <f t="shared" si="4"/>
         <v>257</v>
       </c>
       <c r="N11" s="1">
         <v>119380</v>
       </c>
       <c r="O11">
-        <f>IF(ISBLANK(P11),-N11,P11-N11)</f>
+        <f t="shared" si="5"/>
         <v>165</v>
       </c>
       <c r="P11" s="1">
         <v>119545</v>
       </c>
       <c r="Q11">
-        <f>IF(ISBLANK(R11),-P11,R11-P11)</f>
+        <f t="shared" si="6"/>
         <v>170</v>
       </c>
       <c r="R11" s="1">
         <v>119715</v>
       </c>
       <c r="S11">
-        <f>IF(ISBLANK(T11),-R11,T11-R11)</f>
+        <f t="shared" si="7"/>
         <v>168</v>
       </c>
       <c r="T11" s="1">
         <v>119883</v>
       </c>
       <c r="U11">
-        <f>IF(ISBLANK(V11),-T11,V11-T11)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="V11" s="1">
         <v>119883</v>
       </c>
       <c r="W11">
-        <f>IF(ISBLANK(X11),-V11,X11-V11)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="X11" s="1">
         <v>119883</v>
       </c>
       <c r="Y11">
-        <f>IF(ISBLANK(Z11),-X11,Z11-X11)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Z11" s="1">
         <v>119883</v>
       </c>
       <c r="AA11">
-        <f>IF(ISBLANK(AB11),-Z11,AB11-Z11)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AB11" s="1">
         <v>119883</v>
       </c>
       <c r="AC11">
-        <f>IF(ISBLANK(AD11),-AB11,AD11-AB11)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AD11" s="1">
         <v>119883</v>
       </c>
       <c r="AE11">
-        <f>IF(ISBLANK(AF11),-AD11,AF11-AD11)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AF11" s="1">
         <v>119883</v>
       </c>
       <c r="AG11">
-        <f>IF(ISBLANK(AH11),-AF11,AH11-AF11)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AH11" s="1">
         <v>119883</v>
       </c>
       <c r="AI11">
-        <f>IF(ISBLANK(AJ11),-AH11,AJ11-AH11)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AJ11" s="1">
@@ -9056,112 +9178,112 @@
         <v>2395</v>
       </c>
       <c r="E12">
-        <f>IF(ISBLANK(F12),-D12,F12-D12)</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="F12" s="1">
         <v>2409</v>
       </c>
       <c r="G12">
-        <f>IF(ISBLANK(H12),-F12,H12-F12)</f>
+        <f t="shared" si="1"/>
         <v>-2409</v>
       </c>
       <c r="H12" s="1">
         <v>0</v>
       </c>
       <c r="I12">
-        <f>IF(ISBLANK(J12),-H12,J12-H12)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J12" s="1">
         <v>0</v>
       </c>
       <c r="K12">
-        <f>IF(ISBLANK(L12),-J12,L12-J12)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L12" s="1">
         <v>0</v>
       </c>
       <c r="M12">
-        <f>IF(ISBLANK(N12),-L12,N12-L12)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N12" s="1">
         <v>0</v>
       </c>
       <c r="O12">
-        <f>IF(ISBLANK(P12),-N12,P12-N12)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P12" s="1">
         <v>0</v>
       </c>
       <c r="Q12">
-        <f>IF(ISBLANK(R12),-P12,R12-P12)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="R12" s="1">
         <v>0</v>
       </c>
       <c r="S12">
-        <f>IF(ISBLANK(T12),-R12,T12-R12)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="T12" s="1">
         <v>0</v>
       </c>
       <c r="U12">
-        <f>IF(ISBLANK(V12),-T12,V12-T12)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="V12" s="1">
         <v>0</v>
       </c>
       <c r="W12">
-        <f>IF(ISBLANK(X12),-V12,X12-V12)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="X12" s="1">
         <v>0</v>
       </c>
       <c r="Y12">
-        <f>IF(ISBLANK(Z12),-X12,Z12-X12)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Z12" s="1">
         <v>0</v>
       </c>
       <c r="AA12">
-        <f>IF(ISBLANK(AB12),-Z12,AB12-Z12)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AB12" s="1">
         <v>0</v>
       </c>
       <c r="AC12">
-        <f>IF(ISBLANK(AD12),-AB12,AD12-AB12)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AD12" s="1">
         <v>0</v>
       </c>
       <c r="AE12">
-        <f>IF(ISBLANK(AF12),-AD12,AF12-AD12)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AF12" s="1">
         <v>0</v>
       </c>
       <c r="AG12">
-        <f>IF(ISBLANK(AH12),-AF12,AH12-AF12)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AH12" s="1">
         <v>0</v>
       </c>
       <c r="AI12">
-        <f>IF(ISBLANK(AJ12),-AH12,AJ12-AH12)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AJ12" s="1">
@@ -9181,112 +9303,112 @@
         <v>9423</v>
       </c>
       <c r="E13">
-        <f>IF(ISBLANK(F13),-D13,F13-D13)</f>
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="F13" s="1">
         <v>9455</v>
       </c>
       <c r="G13">
-        <f>IF(ISBLANK(H13),-F13,H13-F13)</f>
+        <f t="shared" si="1"/>
         <v>325</v>
       </c>
       <c r="H13" s="1">
         <v>9780</v>
       </c>
       <c r="I13">
-        <f>IF(ISBLANK(J13),-H13,J13-H13)</f>
+        <f t="shared" si="2"/>
         <v>75</v>
       </c>
       <c r="J13" s="1">
         <v>9855</v>
       </c>
       <c r="K13">
-        <f>IF(ISBLANK(L13),-J13,L13-J13)</f>
+        <f t="shared" si="3"/>
         <v>114</v>
       </c>
       <c r="L13" s="1">
         <v>9969</v>
       </c>
       <c r="M13">
-        <f>IF(ISBLANK(N13),-L13,N13-L13)</f>
+        <f t="shared" si="4"/>
         <v>280</v>
       </c>
       <c r="N13" s="1">
         <v>10249</v>
       </c>
       <c r="O13">
-        <f>IF(ISBLANK(P13),-N13,P13-N13)</f>
+        <f t="shared" si="5"/>
         <v>78</v>
       </c>
       <c r="P13" s="1">
         <v>10327</v>
       </c>
       <c r="Q13">
-        <f>IF(ISBLANK(R13),-P13,R13-P13)</f>
+        <f t="shared" si="6"/>
         <v>137</v>
       </c>
       <c r="R13" s="1">
         <v>10464</v>
       </c>
       <c r="S13">
-        <f>IF(ISBLANK(T13),-R13,T13-R13)</f>
+        <f t="shared" si="7"/>
         <v>79</v>
       </c>
       <c r="T13" s="1">
         <v>10543</v>
       </c>
       <c r="U13">
-        <f>IF(ISBLANK(V13),-T13,V13-T13)</f>
+        <f t="shared" si="8"/>
         <v>1160</v>
       </c>
       <c r="V13" s="1">
         <v>11703</v>
       </c>
       <c r="W13">
-        <f>IF(ISBLANK(X13),-V13,X13-V13)</f>
+        <f t="shared" si="9"/>
         <v>568</v>
       </c>
       <c r="X13" s="1">
         <v>12271</v>
       </c>
       <c r="Y13">
-        <f>IF(ISBLANK(Z13),-X13,Z13-X13)</f>
+        <f t="shared" si="10"/>
         <v>499</v>
       </c>
       <c r="Z13" s="1">
         <v>12770</v>
       </c>
       <c r="AA13">
-        <f>IF(ISBLANK(AB13),-Z13,AB13-Z13)</f>
+        <f t="shared" si="11"/>
         <v>-12770</v>
       </c>
       <c r="AB13" s="1">
         <v>0</v>
       </c>
       <c r="AC13">
-        <f>IF(ISBLANK(AD13),-AB13,AD13-AB13)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AD13" s="1">
         <v>0</v>
       </c>
       <c r="AE13">
-        <f>IF(ISBLANK(AF13),-AD13,AF13-AD13)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AF13" s="1">
         <v>0</v>
       </c>
       <c r="AG13">
-        <f>IF(ISBLANK(AH13),-AF13,AH13-AF13)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AH13" s="1">
         <v>0</v>
       </c>
       <c r="AI13">
-        <f>IF(ISBLANK(AJ13),-AH13,AJ13-AH13)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AJ13" s="1">
@@ -9304,112 +9426,112 @@
         <v>79072</v>
       </c>
       <c r="E14">
-        <f>IF(ISBLANK(F14),-D14,F14-D14)</f>
+        <f t="shared" si="0"/>
         <v>68</v>
       </c>
       <c r="F14" s="1">
         <v>79140</v>
       </c>
       <c r="G14">
-        <f>IF(ISBLANK(H14),-F14,H14-F14)</f>
+        <f t="shared" si="1"/>
         <v>142</v>
       </c>
       <c r="H14" s="1">
         <v>79282</v>
       </c>
       <c r="I14">
-        <f>IF(ISBLANK(J14),-H14,J14-H14)</f>
+        <f t="shared" si="2"/>
         <v>105</v>
       </c>
       <c r="J14" s="1">
         <v>79387</v>
       </c>
       <c r="K14">
-        <f>IF(ISBLANK(L14),-J14,L14-J14)</f>
+        <f t="shared" si="3"/>
         <v>186</v>
       </c>
       <c r="L14" s="1">
         <v>79573</v>
       </c>
       <c r="M14">
-        <f>IF(ISBLANK(N14),-L14,N14-L14)</f>
+        <f t="shared" si="4"/>
         <v>168</v>
       </c>
       <c r="N14" s="1">
         <v>79741</v>
       </c>
       <c r="O14">
-        <f>IF(ISBLANK(P14),-N14,P14-N14)</f>
+        <f t="shared" si="5"/>
         <v>204</v>
       </c>
       <c r="P14" s="1">
         <v>79945</v>
       </c>
       <c r="Q14">
-        <f>IF(ISBLANK(R14),-P14,R14-P14)</f>
+        <f t="shared" si="6"/>
         <v>305</v>
       </c>
       <c r="R14" s="1">
         <v>80250</v>
       </c>
       <c r="S14">
-        <f>IF(ISBLANK(T14),-R14,T14-R14)</f>
+        <f t="shared" si="7"/>
         <v>127</v>
       </c>
       <c r="T14" s="1">
         <v>80377</v>
       </c>
       <c r="U14">
-        <f>IF(ISBLANK(V14),-T14,V14-T14)</f>
+        <f t="shared" si="8"/>
         <v>446</v>
       </c>
       <c r="V14" s="1">
         <v>80823</v>
       </c>
       <c r="W14">
-        <f>IF(ISBLANK(X14),-V14,X14-V14)</f>
+        <f t="shared" si="9"/>
         <v>991</v>
       </c>
       <c r="X14" s="1">
         <v>81814</v>
       </c>
       <c r="Y14">
-        <f>IF(ISBLANK(Z14),-X14,Z14-X14)</f>
+        <f t="shared" si="10"/>
         <v>1119</v>
       </c>
       <c r="Z14" s="1">
         <v>82933</v>
       </c>
       <c r="AA14">
-        <f>IF(ISBLANK(AB14),-Z14,AB14-Z14)</f>
+        <f t="shared" si="11"/>
         <v>958</v>
       </c>
       <c r="AB14" s="1">
         <v>83891</v>
       </c>
       <c r="AC14">
-        <f>IF(ISBLANK(AD14),-AB14,AD14-AB14)</f>
+        <f t="shared" si="12"/>
         <v>1108</v>
       </c>
       <c r="AD14" s="1">
         <v>84999</v>
       </c>
       <c r="AE14">
-        <f>IF(ISBLANK(AF14),-AD14,AF14-AD14)</f>
+        <f t="shared" si="13"/>
         <v>2323</v>
       </c>
       <c r="AF14" s="1">
         <v>87322</v>
       </c>
       <c r="AG14">
-        <f>IF(ISBLANK(AH14),-AF14,AH14-AF14)</f>
+        <f t="shared" si="14"/>
         <v>4517</v>
       </c>
       <c r="AH14" s="1">
         <v>91839</v>
       </c>
       <c r="AI14">
-        <f>IF(ISBLANK(AJ14),-AH14,AJ14-AH14)</f>
+        <f t="shared" si="15"/>
         <v>3734</v>
       </c>
       <c r="AJ14" s="1">
@@ -9428,112 +9550,112 @@
         <v>22075</v>
       </c>
       <c r="E15">
-        <f>IF(ISBLANK(F15),-D15,F15-D15)</f>
+        <f t="shared" si="0"/>
         <v>38</v>
       </c>
       <c r="F15" s="1">
         <v>22113</v>
       </c>
       <c r="G15">
-        <f>IF(ISBLANK(H15),-F15,H15-F15)</f>
+        <f t="shared" si="1"/>
         <v>80</v>
       </c>
       <c r="H15" s="1">
         <v>22193</v>
       </c>
       <c r="I15">
-        <f>IF(ISBLANK(J15),-H15,J15-H15)</f>
+        <f t="shared" si="2"/>
         <v>58</v>
       </c>
       <c r="J15" s="1">
         <v>22251</v>
       </c>
       <c r="K15">
-        <f>IF(ISBLANK(L15),-J15,L15-J15)</f>
+        <f t="shared" si="3"/>
         <v>70</v>
       </c>
       <c r="L15" s="1">
         <v>22321</v>
       </c>
       <c r="M15">
-        <f>IF(ISBLANK(N15),-L15,N15-L15)</f>
+        <f t="shared" si="4"/>
         <v>62</v>
       </c>
       <c r="N15" s="1">
         <v>22383</v>
       </c>
       <c r="O15">
-        <f>IF(ISBLANK(P15),-N15,P15-N15)</f>
+        <f t="shared" si="5"/>
         <v>70</v>
       </c>
       <c r="P15" s="1">
         <v>22453</v>
       </c>
       <c r="Q15">
-        <f>IF(ISBLANK(R15),-P15,R15-P15)</f>
+        <f t="shared" si="6"/>
         <v>173</v>
       </c>
       <c r="R15" s="1">
         <v>22626</v>
       </c>
       <c r="S15">
-        <f>IF(ISBLANK(T15),-R15,T15-R15)</f>
+        <f t="shared" si="7"/>
         <v>74</v>
       </c>
       <c r="T15" s="1">
         <v>22700</v>
       </c>
       <c r="U15">
-        <f>IF(ISBLANK(V15),-T15,V15-T15)</f>
+        <f t="shared" si="8"/>
         <v>193</v>
       </c>
       <c r="V15" s="1">
         <v>22893</v>
       </c>
       <c r="W15">
-        <f>IF(ISBLANK(X15),-V15,X15-V15)</f>
+        <f t="shared" si="9"/>
         <v>626</v>
       </c>
       <c r="X15" s="1">
         <v>23519</v>
       </c>
       <c r="Y15">
-        <f>IF(ISBLANK(Z15),-X15,Z15-X15)</f>
+        <f t="shared" si="10"/>
         <v>330</v>
       </c>
       <c r="Z15" s="1">
         <v>23849</v>
       </c>
       <c r="AA15">
-        <f>IF(ISBLANK(AB15),-Z15,AB15-Z15)</f>
+        <f t="shared" si="11"/>
         <v>483</v>
       </c>
       <c r="AB15" s="1">
         <v>24332</v>
       </c>
       <c r="AC15">
-        <f>IF(ISBLANK(AD15),-AB15,AD15-AB15)</f>
+        <f t="shared" si="12"/>
         <v>600</v>
       </c>
       <c r="AD15" s="1">
         <v>24932</v>
       </c>
       <c r="AE15">
-        <f>IF(ISBLANK(AF15),-AD15,AF15-AD15)</f>
+        <f t="shared" si="13"/>
         <v>1026</v>
       </c>
       <c r="AF15" s="1">
         <v>25958</v>
       </c>
       <c r="AG15">
-        <f>IF(ISBLANK(AH15),-AF15,AH15-AF15)</f>
+        <f t="shared" si="14"/>
         <v>-25958</v>
       </c>
       <c r="AH15" s="1">
         <v>0</v>
       </c>
       <c r="AI15">
-        <f>IF(ISBLANK(AJ15),-AH15,AJ15-AH15)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AJ15" s="1">
@@ -9551,112 +9673,112 @@
         <v>9823</v>
       </c>
       <c r="E16">
-        <f>IF(ISBLANK(F16),-D16,F16-D16)</f>
+        <f t="shared" si="0"/>
         <v>37</v>
       </c>
       <c r="F16" s="1">
         <v>9860</v>
       </c>
       <c r="G16">
-        <f>IF(ISBLANK(H16),-F16,H16-F16)</f>
+        <f t="shared" si="1"/>
         <v>76</v>
       </c>
       <c r="H16" s="1">
         <v>9936</v>
       </c>
       <c r="I16">
-        <f>IF(ISBLANK(J16),-H16,J16-H16)</f>
+        <f t="shared" si="2"/>
         <v>54</v>
       </c>
       <c r="J16" s="1">
         <v>9990</v>
       </c>
       <c r="K16">
-        <f>IF(ISBLANK(L16),-J16,L16-J16)</f>
+        <f t="shared" si="3"/>
         <v>184</v>
       </c>
       <c r="L16" s="1">
         <v>10174</v>
       </c>
       <c r="M16">
-        <f>IF(ISBLANK(N16),-L16,N16-L16)</f>
+        <f t="shared" si="4"/>
         <v>52</v>
       </c>
       <c r="N16" s="1">
         <v>10226</v>
       </c>
       <c r="O16">
-        <f>IF(ISBLANK(P16),-N16,P16-N16)</f>
+        <f t="shared" si="5"/>
         <v>168</v>
       </c>
       <c r="P16" s="1">
         <v>10394</v>
       </c>
       <c r="Q16">
-        <f>IF(ISBLANK(R16),-P16,R16-P16)</f>
+        <f t="shared" si="6"/>
         <v>214</v>
       </c>
       <c r="R16" s="1">
         <v>10608</v>
       </c>
       <c r="S16">
-        <f>IF(ISBLANK(T16),-R16,T16-R16)</f>
+        <f t="shared" si="7"/>
         <v>48</v>
       </c>
       <c r="T16" s="1">
         <v>10656</v>
       </c>
       <c r="U16">
-        <f>IF(ISBLANK(V16),-T16,V16-T16)</f>
+        <f t="shared" si="8"/>
         <v>286</v>
       </c>
       <c r="V16" s="1">
         <v>10942</v>
       </c>
       <c r="W16">
-        <f>IF(ISBLANK(X16),-V16,X16-V16)</f>
+        <f t="shared" si="9"/>
         <v>208</v>
       </c>
       <c r="X16" s="1">
         <v>11150</v>
       </c>
       <c r="Y16">
-        <f>IF(ISBLANK(Z16),-X16,Z16-X16)</f>
+        <f t="shared" si="10"/>
         <v>-11150</v>
       </c>
       <c r="Z16" s="1">
         <v>0</v>
       </c>
       <c r="AA16">
-        <f>IF(ISBLANK(AB16),-Z16,AB16-Z16)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AB16" s="1">
         <v>0</v>
       </c>
       <c r="AC16">
-        <f>IF(ISBLANK(AD16),-AB16,AD16-AB16)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AD16" s="1">
         <v>0</v>
       </c>
       <c r="AE16">
-        <f>IF(ISBLANK(AF16),-AD16,AF16-AD16)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AF16" s="1">
         <v>0</v>
       </c>
       <c r="AG16">
-        <f>IF(ISBLANK(AH16),-AF16,AH16-AF16)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AH16" s="1">
         <v>0</v>
       </c>
       <c r="AI16">
-        <f>IF(ISBLANK(AJ16),-AH16,AJ16-AH16)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AJ16" s="1">
@@ -9674,112 +9796,112 @@
         <v>3682</v>
       </c>
       <c r="E17">
-        <f>IF(ISBLANK(F17),-D17,F17-D17)</f>
+        <f t="shared" si="0"/>
         <v>77</v>
       </c>
       <c r="F17" s="1">
         <v>3759</v>
       </c>
       <c r="G17">
-        <f>IF(ISBLANK(H17),-F17,H17-F17)</f>
+        <f t="shared" si="1"/>
         <v>44</v>
       </c>
       <c r="H17" s="1">
         <v>3803</v>
       </c>
       <c r="I17">
-        <f>IF(ISBLANK(J17),-H17,J17-H17)</f>
+        <f t="shared" si="2"/>
         <v>116</v>
       </c>
       <c r="J17" s="1">
         <v>3919</v>
       </c>
       <c r="K17">
-        <f>IF(ISBLANK(L17),-J17,L17-J17)</f>
+        <f t="shared" si="3"/>
         <v>87</v>
       </c>
       <c r="L17" s="1">
         <v>4006</v>
       </c>
       <c r="M17">
-        <f>IF(ISBLANK(N17),-L17,N17-L17)</f>
+        <f t="shared" si="4"/>
         <v>41</v>
       </c>
       <c r="N17" s="1">
         <v>4047</v>
       </c>
       <c r="O17">
-        <f>IF(ISBLANK(P17),-N17,P17-N17)</f>
+        <f t="shared" si="5"/>
         <v>134</v>
       </c>
       <c r="P17" s="1">
         <v>4181</v>
       </c>
       <c r="Q17">
-        <f>IF(ISBLANK(R17),-P17,R17-P17)</f>
+        <f t="shared" si="6"/>
         <v>-4181</v>
       </c>
       <c r="R17" s="1">
         <v>0</v>
       </c>
       <c r="S17">
-        <f>IF(ISBLANK(T17),-R17,T17-R17)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="T17" s="1">
         <v>0</v>
       </c>
       <c r="U17">
-        <f>IF(ISBLANK(V17),-T17,V17-T17)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="V17" s="1">
         <v>0</v>
       </c>
       <c r="W17">
-        <f>IF(ISBLANK(X17),-V17,X17-V17)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="X17" s="1">
         <v>0</v>
       </c>
       <c r="Y17">
-        <f>IF(ISBLANK(Z17),-X17,Z17-X17)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Z17" s="1">
         <v>0</v>
       </c>
       <c r="AA17">
-        <f>IF(ISBLANK(AB17),-Z17,AB17-Z17)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AB17" s="1">
         <v>0</v>
       </c>
       <c r="AC17">
-        <f>IF(ISBLANK(AD17),-AB17,AD17-AB17)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AD17" s="1">
         <v>0</v>
       </c>
       <c r="AE17">
-        <f>IF(ISBLANK(AF17),-AD17,AF17-AD17)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AF17" s="1">
         <v>0</v>
       </c>
       <c r="AG17">
-        <f>IF(ISBLANK(AH17),-AF17,AH17-AF17)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AH17" s="1">
         <v>0</v>
       </c>
       <c r="AI17">
-        <f>IF(ISBLANK(AJ17),-AH17,AJ17-AH17)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AJ17" s="1">
@@ -9797,112 +9919,112 @@
         <v>75946</v>
       </c>
       <c r="E18">
-        <f>IF(ISBLANK(F18),-D18,F18-D18)</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="F18" s="1">
         <v>76046</v>
       </c>
       <c r="G18">
-        <f>IF(ISBLANK(H18),-F18,H18-F18)</f>
+        <f t="shared" si="1"/>
         <v>201</v>
       </c>
       <c r="H18" s="1">
         <v>76247</v>
       </c>
       <c r="I18">
-        <f>IF(ISBLANK(J18),-H18,J18-H18)</f>
+        <f t="shared" si="2"/>
         <v>126</v>
       </c>
       <c r="J18" s="1">
         <v>76373</v>
       </c>
       <c r="K18">
-        <f>IF(ISBLANK(L18),-J18,L18-J18)</f>
+        <f t="shared" si="3"/>
         <v>272</v>
       </c>
       <c r="L18" s="1">
         <v>76645</v>
       </c>
       <c r="M18">
-        <f>IF(ISBLANK(N18),-L18,N18-L18)</f>
+        <f t="shared" si="4"/>
         <v>74</v>
       </c>
       <c r="N18" s="1">
         <v>76719</v>
       </c>
       <c r="O18">
-        <f>IF(ISBLANK(P18),-N18,P18-N18)</f>
+        <f t="shared" si="5"/>
         <v>301</v>
       </c>
       <c r="P18" s="1">
         <v>77020</v>
       </c>
       <c r="Q18">
-        <f>IF(ISBLANK(R18),-P18,R18-P18)</f>
+        <f t="shared" si="6"/>
         <v>283</v>
       </c>
       <c r="R18" s="1">
         <v>77303</v>
       </c>
       <c r="S18">
-        <f>IF(ISBLANK(T18),-R18,T18-R18)</f>
+        <f t="shared" si="7"/>
         <v>112</v>
       </c>
       <c r="T18" s="1">
         <v>77415</v>
       </c>
       <c r="U18">
-        <f>IF(ISBLANK(V18),-T18,V18-T18)</f>
+        <f t="shared" si="8"/>
         <v>339</v>
       </c>
       <c r="V18" s="1">
         <v>77754</v>
       </c>
       <c r="W18">
-        <f>IF(ISBLANK(X18),-V18,X18-V18)</f>
+        <f t="shared" si="9"/>
         <v>1066</v>
       </c>
       <c r="X18" s="1">
         <v>78820</v>
       </c>
       <c r="Y18">
-        <f>IF(ISBLANK(Z18),-X18,Z18-X18)</f>
+        <f t="shared" si="10"/>
         <v>1295</v>
       </c>
       <c r="Z18" s="1">
         <v>80115</v>
       </c>
       <c r="AA18">
-        <f>IF(ISBLANK(AB18),-Z18,AB18-Z18)</f>
+        <f t="shared" si="11"/>
         <v>593</v>
       </c>
       <c r="AB18" s="1">
         <v>80708</v>
       </c>
       <c r="AC18">
-        <f>IF(ISBLANK(AD18),-AB18,AD18-AB18)</f>
+        <f t="shared" si="12"/>
         <v>1290</v>
       </c>
       <c r="AD18" s="1">
         <v>81998</v>
       </c>
       <c r="AE18">
-        <f>IF(ISBLANK(AF18),-AD18,AF18-AD18)</f>
+        <f t="shared" si="13"/>
         <v>2743</v>
       </c>
       <c r="AF18" s="1">
         <v>84741</v>
       </c>
       <c r="AG18">
-        <f>IF(ISBLANK(AH18),-AF18,AH18-AF18)</f>
+        <f t="shared" si="14"/>
         <v>8382</v>
       </c>
       <c r="AH18" s="1">
         <v>93123</v>
       </c>
       <c r="AI18">
-        <f>IF(ISBLANK(AJ18),-AH18,AJ18-AH18)</f>
+        <f t="shared" si="15"/>
         <v>2972</v>
       </c>
       <c r="AJ18" s="1">
@@ -9920,112 +10042,112 @@
         <v>2864</v>
       </c>
       <c r="E19">
-        <f>IF(ISBLANK(F19),-D19,F19-D19)</f>
+        <f t="shared" si="0"/>
         <v>34</v>
       </c>
       <c r="F19" s="1">
         <v>2898</v>
       </c>
       <c r="G19">
-        <f>IF(ISBLANK(H19),-F19,H19-F19)</f>
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="H19" s="1">
         <v>2919</v>
       </c>
       <c r="I19">
-        <f>IF(ISBLANK(J19),-H19,J19-H19)</f>
+        <f t="shared" si="2"/>
         <v>148</v>
       </c>
       <c r="J19" s="1">
         <v>3067</v>
       </c>
       <c r="K19">
-        <f>IF(ISBLANK(L19),-J19,L19-J19)</f>
+        <f t="shared" si="3"/>
         <v>-3067</v>
       </c>
       <c r="L19" s="1">
         <v>0</v>
       </c>
       <c r="M19">
-        <f>IF(ISBLANK(N19),-L19,N19-L19)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N19" s="1">
         <v>0</v>
       </c>
       <c r="O19">
-        <f>IF(ISBLANK(P19),-N19,P19-N19)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P19" s="1">
         <v>0</v>
       </c>
       <c r="Q19">
-        <f>IF(ISBLANK(R19),-P19,R19-P19)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="R19" s="1">
         <v>0</v>
       </c>
       <c r="S19">
-        <f>IF(ISBLANK(T19),-R19,T19-R19)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="T19" s="1">
         <v>0</v>
       </c>
       <c r="U19">
-        <f>IF(ISBLANK(V19),-T19,V19-T19)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="V19" s="1">
         <v>0</v>
       </c>
       <c r="W19">
-        <f>IF(ISBLANK(X19),-V19,X19-V19)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="X19" s="1">
         <v>0</v>
       </c>
       <c r="Y19">
-        <f>IF(ISBLANK(Z19),-X19,Z19-X19)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Z19" s="1">
         <v>0</v>
       </c>
       <c r="AA19">
-        <f>IF(ISBLANK(AB19),-Z19,AB19-Z19)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AB19" s="1">
         <v>0</v>
       </c>
       <c r="AC19">
-        <f>IF(ISBLANK(AD19),-AB19,AD19-AB19)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AD19" s="1">
         <v>0</v>
       </c>
       <c r="AE19">
-        <f>IF(ISBLANK(AF19),-AD19,AF19-AD19)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AF19" s="1">
         <v>0</v>
       </c>
       <c r="AG19">
-        <f>IF(ISBLANK(AH19),-AF19,AH19-AF19)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AH19" s="1">
         <v>0</v>
       </c>
       <c r="AI19">
-        <f>IF(ISBLANK(AJ19),-AH19,AJ19-AH19)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AJ19" s="1">
@@ -10043,112 +10165,112 @@
         <v>2416</v>
       </c>
       <c r="E20">
-        <f>IF(ISBLANK(F20),-D20,F20-D20)</f>
+        <f t="shared" si="0"/>
         <v>48</v>
       </c>
       <c r="F20" s="1">
         <v>2464</v>
       </c>
       <c r="G20">
-        <f>IF(ISBLANK(H20),-F20,H20-F20)</f>
+        <f t="shared" si="1"/>
         <v>78</v>
       </c>
       <c r="H20" s="1">
         <v>2542</v>
       </c>
       <c r="I20">
-        <f>IF(ISBLANK(J20),-H20,J20-H20)</f>
+        <f t="shared" si="2"/>
         <v>-2542</v>
       </c>
       <c r="J20" s="1">
         <v>0</v>
       </c>
       <c r="K20">
-        <f>IF(ISBLANK(L20),-J20,L20-J20)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L20" s="1">
         <v>0</v>
       </c>
       <c r="M20">
-        <f>IF(ISBLANK(N20),-L20,N20-L20)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N20" s="1">
         <v>0</v>
       </c>
       <c r="O20">
-        <f>IF(ISBLANK(P20),-N20,P20-N20)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P20" s="1">
         <v>0</v>
       </c>
       <c r="Q20">
-        <f>IF(ISBLANK(R20),-P20,R20-P20)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="R20" s="1">
         <v>0</v>
       </c>
       <c r="S20">
-        <f>IF(ISBLANK(T20),-R20,T20-R20)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="T20" s="1">
         <v>0</v>
       </c>
       <c r="U20">
-        <f>IF(ISBLANK(V20),-T20,V20-T20)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="V20" s="1">
         <v>0</v>
       </c>
       <c r="W20">
-        <f>IF(ISBLANK(X20),-V20,X20-V20)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="X20" s="1">
         <v>0</v>
       </c>
       <c r="Y20">
-        <f>IF(ISBLANK(Z20),-X20,Z20-X20)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Z20" s="1">
         <v>0</v>
       </c>
       <c r="AA20">
-        <f>IF(ISBLANK(AB20),-Z20,AB20-Z20)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AB20" s="1">
         <v>0</v>
       </c>
       <c r="AC20">
-        <f>IF(ISBLANK(AD20),-AB20,AD20-AB20)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AD20" s="1">
         <v>0</v>
       </c>
       <c r="AE20">
-        <f>IF(ISBLANK(AF20),-AD20,AF20-AD20)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AF20" s="1">
         <v>0</v>
       </c>
       <c r="AG20">
-        <f>IF(ISBLANK(AH20),-AF20,AH20-AF20)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AH20" s="1">
         <v>0</v>
       </c>
       <c r="AI20">
-        <f>IF(ISBLANK(AJ20),-AH20,AJ20-AH20)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AJ20" s="1">
@@ -10166,112 +10288,112 @@
         <v>1423</v>
       </c>
       <c r="E21">
-        <f>IF(ISBLANK(F21),-D21,F21-D21)</f>
+        <f t="shared" si="0"/>
         <v>-1423</v>
       </c>
       <c r="F21" s="1">
         <v>0</v>
       </c>
       <c r="G21">
-        <f>IF(ISBLANK(H21),-F21,H21-F21)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H21" s="1">
         <v>0</v>
       </c>
       <c r="I21">
-        <f>IF(ISBLANK(J21),-H21,J21-H21)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J21" s="1">
         <v>0</v>
       </c>
       <c r="K21">
-        <f>IF(ISBLANK(L21),-J21,L21-J21)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L21" s="1">
         <v>0</v>
       </c>
       <c r="M21">
-        <f>IF(ISBLANK(N21),-L21,N21-L21)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N21" s="1">
         <v>0</v>
       </c>
       <c r="O21">
-        <f>IF(ISBLANK(P21),-N21,P21-N21)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P21" s="1">
         <v>0</v>
       </c>
       <c r="Q21">
-        <f>IF(ISBLANK(R21),-P21,R21-P21)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="R21" s="1">
         <v>0</v>
       </c>
       <c r="S21">
-        <f>IF(ISBLANK(T21),-R21,T21-R21)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="T21" s="1">
         <v>0</v>
       </c>
       <c r="U21">
-        <f>IF(ISBLANK(V21),-T21,V21-T21)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="V21" s="1">
         <v>0</v>
       </c>
       <c r="W21">
-        <f>IF(ISBLANK(X21),-V21,X21-V21)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="X21" s="1">
         <v>0</v>
       </c>
       <c r="Y21">
-        <f>IF(ISBLANK(Z21),-X21,Z21-X21)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Z21" s="1">
         <v>0</v>
       </c>
       <c r="AA21">
-        <f>IF(ISBLANK(AB21),-Z21,AB21-Z21)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AB21" s="1">
         <v>0</v>
       </c>
       <c r="AC21">
-        <f>IF(ISBLANK(AD21),-AB21,AD21-AB21)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AD21" s="1">
         <v>0</v>
       </c>
       <c r="AE21">
-        <f>IF(ISBLANK(AF21),-AD21,AF21-AD21)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AF21" s="1">
         <v>0</v>
       </c>
       <c r="AG21">
-        <f>IF(ISBLANK(AH21),-AF21,AH21-AF21)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AH21" s="1">
         <v>0</v>
       </c>
       <c r="AI21">
-        <f>IF(ISBLANK(AJ21),-AH21,AJ21-AH21)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AJ21" s="1">
@@ -10289,112 +10411,112 @@
         <v>14802</v>
       </c>
       <c r="E22">
-        <f>IF(ISBLANK(F22),-D22,F22-D22)</f>
+        <f t="shared" si="0"/>
         <v>156</v>
       </c>
       <c r="F22" s="1">
         <v>14958</v>
       </c>
       <c r="G22">
-        <f>IF(ISBLANK(H22),-F22,H22-F22)</f>
+        <f t="shared" si="1"/>
         <v>51</v>
       </c>
       <c r="H22" s="1">
         <v>15009</v>
       </c>
       <c r="I22">
-        <f>IF(ISBLANK(J22),-H22,J22-H22)</f>
+        <f t="shared" si="2"/>
         <v>198</v>
       </c>
       <c r="J22" s="1">
         <v>15207</v>
       </c>
       <c r="K22">
-        <f>IF(ISBLANK(L22),-J22,L22-J22)</f>
+        <f t="shared" si="3"/>
         <v>146</v>
       </c>
       <c r="L22" s="1">
         <v>15353</v>
       </c>
       <c r="M22">
-        <f>IF(ISBLANK(N22),-L22,N22-L22)</f>
+        <f t="shared" si="4"/>
         <v>41</v>
       </c>
       <c r="N22" s="1">
         <v>15394</v>
       </c>
       <c r="O22">
-        <f>IF(ISBLANK(P22),-N22,P22-N22)</f>
+        <f t="shared" si="5"/>
         <v>392</v>
       </c>
       <c r="P22" s="1">
         <v>15786</v>
       </c>
       <c r="Q22">
-        <f>IF(ISBLANK(R22),-P22,R22-P22)</f>
+        <f t="shared" si="6"/>
         <v>321</v>
       </c>
       <c r="R22" s="1">
         <v>16107</v>
       </c>
       <c r="S22">
-        <f>IF(ISBLANK(T22),-R22,T22-R22)</f>
+        <f t="shared" si="7"/>
         <v>101</v>
       </c>
       <c r="T22" s="1">
         <v>16208</v>
       </c>
       <c r="U22">
-        <f>IF(ISBLANK(V22),-T22,V22-T22)</f>
+        <f t="shared" si="8"/>
         <v>170</v>
       </c>
       <c r="V22" s="1">
         <v>16378</v>
       </c>
       <c r="W22">
-        <f>IF(ISBLANK(X22),-V22,X22-V22)</f>
+        <f t="shared" si="9"/>
         <v>530</v>
       </c>
       <c r="X22" s="1">
         <v>16908</v>
       </c>
       <c r="Y22">
-        <f>IF(ISBLANK(Z22),-X22,Z22-X22)</f>
+        <f t="shared" si="10"/>
         <v>490</v>
       </c>
       <c r="Z22" s="1">
         <v>17398</v>
       </c>
       <c r="AA22">
-        <f>IF(ISBLANK(AB22),-Z22,AB22-Z22)</f>
+        <f t="shared" si="11"/>
         <v>329</v>
       </c>
       <c r="AB22" s="1">
         <v>17727</v>
       </c>
       <c r="AC22">
-        <f>IF(ISBLANK(AD22),-AB22,AD22-AB22)</f>
+        <f t="shared" si="12"/>
         <v>749</v>
       </c>
       <c r="AD22" s="1">
         <v>18476</v>
       </c>
       <c r="AE22">
-        <f>IF(ISBLANK(AF22),-AD22,AF22-AD22)</f>
+        <f t="shared" si="13"/>
         <v>-18476</v>
       </c>
       <c r="AF22" s="1">
         <v>0</v>
       </c>
       <c r="AG22">
-        <f>IF(ISBLANK(AH22),-AF22,AH22-AF22)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AH22" s="1">
         <v>0</v>
       </c>
       <c r="AI22">
-        <f>IF(ISBLANK(AJ22),-AH22,AJ22-AH22)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AJ22" s="1">
@@ -10412,112 +10534,112 @@
         <v>81741</v>
       </c>
       <c r="E23">
-        <f>IF(ISBLANK(F23),-D23,F23-D23)</f>
+        <f t="shared" si="0"/>
         <v>253</v>
       </c>
       <c r="F23" s="1">
         <v>81994</v>
       </c>
       <c r="G23">
-        <f>IF(ISBLANK(H23),-F23,H23-F23)</f>
+        <f t="shared" si="1"/>
         <v>130</v>
       </c>
       <c r="H23" s="1">
         <v>82124</v>
       </c>
       <c r="I23">
-        <f>IF(ISBLANK(J23),-H23,J23-H23)</f>
+        <f t="shared" si="2"/>
         <v>211</v>
       </c>
       <c r="J23" s="1">
         <v>82335</v>
       </c>
       <c r="K23">
-        <f>IF(ISBLANK(L23),-J23,L23-J23)</f>
+        <f t="shared" si="3"/>
         <v>323</v>
       </c>
       <c r="L23" s="1">
         <v>82658</v>
       </c>
       <c r="M23">
-        <f>IF(ISBLANK(N23),-L23,N23-L23)</f>
+        <f t="shared" si="4"/>
         <v>206</v>
       </c>
       <c r="N23" s="1">
         <v>82864</v>
       </c>
       <c r="O23">
-        <f>IF(ISBLANK(P23),-N23,P23-N23)</f>
+        <f t="shared" si="5"/>
         <v>556</v>
       </c>
       <c r="P23" s="1">
         <v>83420</v>
       </c>
       <c r="Q23">
-        <f>IF(ISBLANK(R23),-P23,R23-P23)</f>
+        <f t="shared" si="6"/>
         <v>351</v>
       </c>
       <c r="R23" s="1">
         <v>83771</v>
       </c>
       <c r="S23">
-        <f>IF(ISBLANK(T23),-R23,T23-R23)</f>
+        <f t="shared" si="7"/>
         <v>217</v>
       </c>
       <c r="T23" s="1">
         <v>83988</v>
       </c>
       <c r="U23">
-        <f>IF(ISBLANK(V23),-T23,V23-T23)</f>
+        <f t="shared" si="8"/>
         <v>247</v>
       </c>
       <c r="V23" s="1">
         <v>84235</v>
       </c>
       <c r="W23">
-        <f>IF(ISBLANK(X23),-V23,X23-V23)</f>
+        <f t="shared" si="9"/>
         <v>1001</v>
       </c>
       <c r="X23" s="1">
         <v>85236</v>
       </c>
       <c r="Y23">
-        <f>IF(ISBLANK(Z23),-X23,Z23-X23)</f>
+        <f t="shared" si="10"/>
         <v>2333</v>
       </c>
       <c r="Z23" s="1">
         <v>87569</v>
       </c>
       <c r="AA23">
-        <f>IF(ISBLANK(AB23),-Z23,AB23-Z23)</f>
+        <f t="shared" si="11"/>
         <v>1190</v>
       </c>
       <c r="AB23" s="1">
         <v>88759</v>
       </c>
       <c r="AC23">
-        <f>IF(ISBLANK(AD23),-AB23,AD23-AB23)</f>
+        <f t="shared" si="12"/>
         <v>1476</v>
       </c>
       <c r="AD23" s="1">
         <v>90235</v>
       </c>
       <c r="AE23">
-        <f>IF(ISBLANK(AF23),-AD23,AF23-AD23)</f>
+        <f t="shared" si="13"/>
         <v>5545</v>
       </c>
       <c r="AF23" s="1">
         <v>95780</v>
       </c>
       <c r="AG23">
-        <f>IF(ISBLANK(AH23),-AF23,AH23-AF23)</f>
+        <f t="shared" si="14"/>
         <v>5945</v>
       </c>
       <c r="AH23" s="1">
         <v>101725</v>
       </c>
       <c r="AI23">
-        <f>IF(ISBLANK(AJ23),-AH23,AJ23-AH23)</f>
+        <f t="shared" si="15"/>
         <v>7424</v>
       </c>
       <c r="AJ23" s="1">
@@ -10535,112 +10657,112 @@
         <v>3286</v>
       </c>
       <c r="E24">
-        <f>IF(ISBLANK(F24),-D24,F24-D24)</f>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="F24" s="1">
         <v>3307</v>
       </c>
       <c r="G24">
-        <f>IF(ISBLANK(H24),-F24,H24-F24)</f>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="H24" s="1">
         <v>3320</v>
       </c>
       <c r="I24">
-        <f>IF(ISBLANK(J24),-H24,J24-H24)</f>
+        <f t="shared" si="2"/>
         <v>232</v>
       </c>
       <c r="J24" s="1">
         <v>3552</v>
       </c>
       <c r="K24">
-        <f>IF(ISBLANK(L24),-J24,L24-J24)</f>
+        <f t="shared" si="3"/>
         <v>102</v>
       </c>
       <c r="L24" s="1">
         <v>3654</v>
       </c>
       <c r="M24">
-        <f>IF(ISBLANK(N24),-L24,N24-L24)</f>
+        <f t="shared" si="4"/>
         <v>60</v>
       </c>
       <c r="N24" s="1">
         <v>3714</v>
       </c>
       <c r="O24">
-        <f>IF(ISBLANK(P24),-N24,P24-N24)</f>
+        <f t="shared" si="5"/>
         <v>-3714</v>
       </c>
       <c r="P24" s="1">
         <v>0</v>
       </c>
       <c r="Q24">
-        <f>IF(ISBLANK(R24),-P24,R24-P24)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="R24" s="1">
         <v>0</v>
       </c>
       <c r="S24">
-        <f>IF(ISBLANK(T24),-R24,T24-R24)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="T24" s="1">
         <v>0</v>
       </c>
       <c r="U24">
-        <f>IF(ISBLANK(V24),-T24,V24-T24)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="V24" s="1">
         <v>0</v>
       </c>
       <c r="W24">
-        <f>IF(ISBLANK(X24),-V24,X24-V24)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="X24" s="1">
         <v>0</v>
       </c>
       <c r="Y24">
-        <f>IF(ISBLANK(Z24),-X24,Z24-X24)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Z24" s="1">
         <v>0</v>
       </c>
       <c r="AA24">
-        <f>IF(ISBLANK(AB24),-Z24,AB24-Z24)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AB24" s="1">
         <v>0</v>
       </c>
       <c r="AC24">
-        <f>IF(ISBLANK(AD24),-AB24,AD24-AB24)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AD24" s="1">
         <v>0</v>
       </c>
       <c r="AE24">
-        <f>IF(ISBLANK(AF24),-AD24,AF24-AD24)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AF24" s="1">
         <v>0</v>
       </c>
       <c r="AG24">
-        <f>IF(ISBLANK(AH24),-AF24,AH24-AF24)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AH24" s="1">
         <v>0</v>
       </c>
       <c r="AI24">
-        <f>IF(ISBLANK(AJ24),-AH24,AJ24-AH24)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AJ24" s="1">
@@ -10745,19 +10867,19 @@
         <v>148</v>
       </c>
       <c r="E27">
-        <f t="shared" ref="E27:E48" si="0">FIND(",",B27)</f>
+        <f t="shared" ref="E27:E48" si="16">FIND(",",B27)</f>
         <v>9</v>
       </c>
       <c r="F27" t="str">
-        <f t="shared" ref="F27:F48" si="1">LEFT(B27,E27-1)</f>
+        <f t="shared" ref="F27:F48" si="17">LEFT(B27,E27-1)</f>
         <v>Kelleher</v>
       </c>
       <c r="G27" t="str">
-        <f t="shared" ref="G27:G48" si="2">RIGHT(B27,LEN(B27)-(E27+1))</f>
+        <f t="shared" ref="G27:G48" si="18">RIGHT(B27,LEN(B27)-(E27+1))</f>
         <v>Billy</v>
       </c>
       <c r="H27" t="str">
-        <f t="shared" ref="H27:H48" si="3">G27&amp;" "&amp;F27</f>
+        <f t="shared" ref="H27:H48" si="19">G27&amp;" "&amp;F27</f>
         <v>Billy Kelleher</v>
       </c>
       <c r="J27" t="s">
@@ -10808,19 +10930,19 @@
         <v>149</v>
       </c>
       <c r="E28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="16"/>
         <v>8</v>
       </c>
       <c r="F28" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="17"/>
         <v>Wallace</v>
       </c>
       <c r="G28" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="18"/>
         <v>Mick</v>
       </c>
       <c r="H28" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="19"/>
         <v>Mick Wallace</v>
       </c>
       <c r="J28" t="s">
@@ -10898,19 +11020,19 @@
         <v>150</v>
       </c>
       <c r="E29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="16"/>
         <v>9</v>
       </c>
       <c r="F29" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="17"/>
         <v>Ní Riada</v>
       </c>
       <c r="G29" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="18"/>
         <v>Liadh</v>
       </c>
       <c r="H29" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="19"/>
         <v>Liadh Ní Riada</v>
       </c>
       <c r="J29" t="s">
@@ -10988,19 +11110,19 @@
         <v>151</v>
       </c>
       <c r="E30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="16"/>
         <v>11</v>
       </c>
       <c r="F30" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="17"/>
         <v>O'Sullivan</v>
       </c>
       <c r="G30" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="18"/>
         <v>Grace</v>
       </c>
       <c r="H30" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="19"/>
         <v>Grace O'Sullivan</v>
       </c>
       <c r="J30" t="s">
@@ -11078,19 +11200,19 @@
         <v>152</v>
       </c>
       <c r="E31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="16"/>
         <v>6</v>
       </c>
       <c r="F31" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="17"/>
         <v>Byrne</v>
       </c>
       <c r="G31" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="18"/>
         <v>Malcolm</v>
       </c>
       <c r="H31" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="19"/>
         <v>Malcolm Byrne</v>
       </c>
       <c r="J31" t="s">
@@ -11168,19 +11290,19 @@
         <v>153</v>
       </c>
       <c r="E32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="16"/>
         <v>6</v>
       </c>
       <c r="F32" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="17"/>
         <v>Clune</v>
       </c>
       <c r="G32" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="18"/>
         <v>Deirdre</v>
       </c>
       <c r="H32" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="19"/>
         <v>Deirdre Clune</v>
       </c>
       <c r="J32" t="s">
@@ -11255,19 +11377,19 @@
         <v>154</v>
       </c>
       <c r="E33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="16"/>
         <v>6</v>
       </c>
       <c r="F33" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="17"/>
         <v>Doyle</v>
       </c>
       <c r="G33" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="18"/>
         <v>Andrew</v>
       </c>
       <c r="H33" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="19"/>
         <v>Andrew Doyle</v>
       </c>
       <c r="J33" t="s">
@@ -11345,19 +11467,19 @@
         <v>155</v>
       </c>
       <c r="E34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="16"/>
         <v>6</v>
       </c>
       <c r="F34" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="17"/>
         <v>Nunan</v>
       </c>
       <c r="G34" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="18"/>
         <v>Sheila</v>
       </c>
       <c r="H34" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="19"/>
         <v>Sheila Nunan</v>
       </c>
       <c r="J34" t="s">
@@ -11429,19 +11551,19 @@
         <v>156</v>
       </c>
       <c r="E35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="16"/>
         <v>8</v>
       </c>
       <c r="F35" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="17"/>
         <v>Wallace</v>
       </c>
       <c r="G35" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="18"/>
         <v>Adrienne</v>
       </c>
       <c r="H35" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="19"/>
         <v>Adrienne Wallace</v>
       </c>
       <c r="J35" t="s">
@@ -11510,19 +11632,19 @@
         <v>157</v>
       </c>
       <c r="E36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="16"/>
         <v>7</v>
       </c>
       <c r="F36" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="17"/>
         <v>Cahill</v>
       </c>
       <c r="G36" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="18"/>
         <v>Dolores</v>
       </c>
       <c r="H36" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="19"/>
         <v>Dolores Cahill</v>
       </c>
       <c r="J36" t="s">
@@ -11591,19 +11713,19 @@
         <v>158</v>
       </c>
       <c r="E37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="16"/>
         <v>8</v>
       </c>
       <c r="F37" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="17"/>
         <v>O'Flynn</v>
       </c>
       <c r="G37" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="18"/>
         <v>Diarmuid Patrick</v>
       </c>
       <c r="H37" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="19"/>
         <v>Diarmuid Patrick O'Flynn</v>
       </c>
       <c r="J37" t="s">
@@ -11669,19 +11791,19 @@
         <v>159</v>
       </c>
       <c r="E38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="16"/>
         <v>8</v>
       </c>
       <c r="F38" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="17"/>
         <v>Minehan</v>
       </c>
       <c r="G38" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="18"/>
         <v>Liam</v>
       </c>
       <c r="H38" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="19"/>
         <v>Liam Minehan</v>
       </c>
       <c r="J38" t="s">
@@ -11741,19 +11863,19 @@
         <v>160</v>
       </c>
       <c r="E39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="16"/>
         <v>8</v>
       </c>
       <c r="F39" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="17"/>
         <v>Gardner</v>
       </c>
       <c r="G39" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="18"/>
         <v>Breda Patricia</v>
       </c>
       <c r="H39" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="19"/>
         <v>Breda Patricia Gardner</v>
       </c>
       <c r="J39" t="s">
@@ -11816,19 +11938,19 @@
         <v>161</v>
       </c>
       <c r="E40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="16"/>
         <v>7</v>
       </c>
       <c r="F40" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="17"/>
         <v>Heaney</v>
       </c>
       <c r="G40" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="18"/>
         <v>Theresa</v>
       </c>
       <c r="H40" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="19"/>
         <v>Theresa Heaney</v>
       </c>
       <c r="J40" t="s">
@@ -11889,19 +12011,19 @@
         <v>162</v>
       </c>
       <c r="E41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="16"/>
         <v>8</v>
       </c>
       <c r="F41" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="17"/>
         <v>Brennan</v>
       </c>
       <c r="G41" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="18"/>
         <v>Allan</v>
       </c>
       <c r="H41" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="19"/>
         <v>Allan Brennan</v>
       </c>
       <c r="J41" t="s">
@@ -11959,19 +12081,19 @@
         <v>163</v>
       </c>
       <c r="E42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="16"/>
         <v>11</v>
       </c>
       <c r="F42" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="17"/>
         <v>O'Loughlin</v>
       </c>
       <c r="G42" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="18"/>
         <v>Peter</v>
       </c>
       <c r="H42" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="19"/>
         <v>Peter O'Loughlin</v>
       </c>
       <c r="J42" t="s">
@@ -12025,19 +12147,19 @@
         <v>164</v>
       </c>
       <c r="E43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="16"/>
         <v>12</v>
       </c>
       <c r="F43" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="17"/>
         <v>Worthington</v>
       </c>
       <c r="G43" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="18"/>
         <v>Colleen</v>
       </c>
       <c r="H43" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="19"/>
         <v>Colleen Worthington</v>
       </c>
       <c r="J43" t="s">
@@ -12087,19 +12209,19 @@
         <v>165</v>
       </c>
       <c r="E44">
-        <f t="shared" si="0"/>
+        <f t="shared" si="16"/>
         <v>11</v>
       </c>
       <c r="F44" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="17"/>
         <v>Fitzgerald</v>
       </c>
       <c r="G44" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="18"/>
         <v>Paddy</v>
       </c>
       <c r="H44" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="19"/>
         <v>Paddy Fitzgerald</v>
       </c>
       <c r="J44" t="s">
@@ -12145,19 +12267,19 @@
         <v>166</v>
       </c>
       <c r="E45">
-        <f t="shared" si="0"/>
+        <f t="shared" si="16"/>
         <v>13</v>
       </c>
       <c r="F45" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="17"/>
         <v>Ryan-Purcell</v>
       </c>
       <c r="G45" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="18"/>
         <v>Walter</v>
       </c>
       <c r="H45" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="19"/>
         <v>Walter Ryan-Purcell</v>
       </c>
       <c r="J45" t="s">
@@ -12199,19 +12321,19 @@
         <v>167</v>
       </c>
       <c r="E46">
-        <f t="shared" si="0"/>
+        <f t="shared" si="16"/>
         <v>7</v>
       </c>
       <c r="F46" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="17"/>
         <v>Sexton</v>
       </c>
       <c r="G46" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="18"/>
         <v>Joesph</v>
       </c>
       <c r="H46" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="19"/>
         <v>Joesph Sexton</v>
       </c>
       <c r="J46" t="s">
@@ -12245,19 +12367,19 @@
         <v>168</v>
       </c>
       <c r="E47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="16"/>
         <v>7</v>
       </c>
       <c r="F47" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="17"/>
         <v>Madden</v>
       </c>
       <c r="G47" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="18"/>
         <v>Peter</v>
       </c>
       <c r="H47" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="19"/>
         <v>Peter Madden</v>
       </c>
       <c r="J47" t="s">
@@ -12284,19 +12406,19 @@
         <v>169</v>
       </c>
       <c r="E48">
-        <f t="shared" si="0"/>
+        <f t="shared" si="16"/>
         <v>11</v>
       </c>
       <c r="F48" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="17"/>
         <v>Van de Ven</v>
       </c>
       <c r="G48" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="18"/>
         <v>Jan</v>
       </c>
       <c r="H48" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="19"/>
         <v>Jan Van de Ven</v>
       </c>
       <c r="J48" t="s">

</xml_diff>

<commit_message>
Correct Ni Riada sorting error on the South data Signed-off-by: Gerry Mulvenna <git@movingwifi.com>
</commit_message>
<xml_diff>
--- a/europarl/europarl-ireland-2019.xlsx
+++ b/europarl/europarl-ireland-2019.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="14220" windowHeight="8580" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="14220" windowHeight="8580" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Candidates" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="263">
   <si>
     <t>Candidate</t>
   </si>
@@ -803,6 +803,9 @@
   </si>
   <si>
     <t>Count 17</t>
+  </si>
+  <si>
+    <t>Riada, Liadh Ninot-elected</t>
   </si>
 </sst>
 </file>
@@ -5164,11 +5167,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="W2" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AA2" sqref="AA2:AB18"/>
+      <selection pane="bottomRight" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7838,11 +7841,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="AG2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AG2" sqref="AG2:AJ24"/>
+      <selection pane="bottomRight" activeCell="D2" sqref="D2:AJ24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7921,112 +7924,112 @@
         <v>4665</v>
       </c>
       <c r="E2">
-        <f t="shared" ref="E2:E24" si="0">IF(ISBLANK(F2),-D2,F2-D2)</f>
+        <f>IF(ISBLANK(F2),-D2,F2-D2)</f>
         <v>26</v>
       </c>
       <c r="F2" s="1">
         <v>4691</v>
       </c>
       <c r="G2">
-        <f t="shared" ref="G2:G24" si="1">IF(ISBLANK(H2),-F2,H2-F2)</f>
+        <f>IF(ISBLANK(H2),-F2,H2-F2)</f>
         <v>43</v>
       </c>
       <c r="H2" s="1">
         <v>4734</v>
       </c>
       <c r="I2">
-        <f t="shared" ref="I2:I24" si="2">IF(ISBLANK(J2),-H2,J2-H2)</f>
+        <f>IF(ISBLANK(J2),-H2,J2-H2)</f>
         <v>57</v>
       </c>
       <c r="J2" s="1">
         <v>4791</v>
       </c>
       <c r="K2">
-        <f t="shared" ref="K2:K24" si="3">IF(ISBLANK(L2),-J2,L2-J2)</f>
+        <f>IF(ISBLANK(L2),-J2,L2-J2)</f>
         <v>50</v>
       </c>
       <c r="L2" s="1">
         <v>4841</v>
       </c>
       <c r="M2">
-        <f t="shared" ref="M2:M24" si="4">IF(ISBLANK(N2),-L2,N2-L2)</f>
+        <f>IF(ISBLANK(N2),-L2,N2-L2)</f>
         <v>115</v>
       </c>
       <c r="N2" s="1">
         <v>4956</v>
       </c>
       <c r="O2">
-        <f t="shared" ref="O2:O24" si="5">IF(ISBLANK(P2),-N2,P2-N2)</f>
+        <f>IF(ISBLANK(P2),-N2,P2-N2)</f>
         <v>72</v>
       </c>
       <c r="P2" s="1">
         <v>5028</v>
       </c>
       <c r="Q2">
-        <f t="shared" ref="Q2:Q24" si="6">IF(ISBLANK(R2),-P2,R2-P2)</f>
+        <f>IF(ISBLANK(R2),-P2,R2-P2)</f>
         <v>104</v>
       </c>
       <c r="R2" s="1">
         <v>5132</v>
       </c>
       <c r="S2">
-        <f t="shared" ref="S2:S24" si="7">IF(ISBLANK(T2),-R2,T2-R2)</f>
+        <f>IF(ISBLANK(T2),-R2,T2-R2)</f>
         <v>-5132</v>
       </c>
       <c r="T2" s="1">
         <v>0</v>
       </c>
       <c r="U2">
-        <f t="shared" ref="U2:U24" si="8">IF(ISBLANK(V2),-T2,V2-T2)</f>
+        <f>IF(ISBLANK(V2),-T2,V2-T2)</f>
         <v>0</v>
       </c>
       <c r="V2" s="1">
         <v>0</v>
       </c>
       <c r="W2">
-        <f t="shared" ref="W2:W24" si="9">IF(ISBLANK(X2),-V2,X2-V2)</f>
+        <f>IF(ISBLANK(X2),-V2,X2-V2)</f>
         <v>0</v>
       </c>
       <c r="X2" s="1">
         <v>0</v>
       </c>
       <c r="Y2">
-        <f t="shared" ref="Y2:Y24" si="10">IF(ISBLANK(Z2),-X2,Z2-X2)</f>
+        <f>IF(ISBLANK(Z2),-X2,Z2-X2)</f>
         <v>0</v>
       </c>
       <c r="Z2" s="1">
         <v>0</v>
       </c>
       <c r="AA2">
-        <f t="shared" ref="AA2:AA24" si="11">IF(ISBLANK(AB2),-Z2,AB2-Z2)</f>
+        <f>IF(ISBLANK(AB2),-Z2,AB2-Z2)</f>
         <v>0</v>
       </c>
       <c r="AB2" s="1">
         <v>0</v>
       </c>
       <c r="AC2">
-        <f t="shared" ref="AC2:AC24" si="12">IF(ISBLANK(AD2),-AB2,AD2-AB2)</f>
+        <f>IF(ISBLANK(AD2),-AB2,AD2-AB2)</f>
         <v>0</v>
       </c>
       <c r="AD2" s="1">
         <v>0</v>
       </c>
       <c r="AE2">
-        <f t="shared" ref="AE2:AE24" si="13">IF(ISBLANK(AF2),-AD2,AF2-AD2)</f>
+        <f>IF(ISBLANK(AF2),-AD2,AF2-AD2)</f>
         <v>0</v>
       </c>
       <c r="AF2" s="1">
         <v>0</v>
       </c>
       <c r="AG2">
-        <f t="shared" ref="AG2:AG24" si="14">IF(ISBLANK(AH2),-AF2,AH2-AF2)</f>
+        <f>IF(ISBLANK(AH2),-AF2,AH2-AF2)</f>
         <v>0</v>
       </c>
       <c r="AH2" s="1">
         <v>0</v>
       </c>
       <c r="AI2">
-        <f t="shared" ref="AI2:AI24" si="15">IF(ISBLANK(AJ2),-AH2,AJ2-AH2)</f>
+        <f>IF(ISBLANK(AJ2),-AH2,AJ2-AH2)</f>
         <v>0</v>
       </c>
       <c r="AJ2" s="1">
@@ -8044,112 +8047,112 @@
         <v>69166</v>
       </c>
       <c r="E3">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F3),-D3,F3-D3)</f>
         <v>35</v>
       </c>
       <c r="F3" s="1">
         <v>69201</v>
       </c>
       <c r="G3">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H3),-F3,H3-F3)</f>
         <v>71</v>
       </c>
       <c r="H3" s="1">
         <v>69272</v>
       </c>
       <c r="I3">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J3),-H3,J3-H3)</f>
         <v>44</v>
       </c>
       <c r="J3" s="1">
         <v>69316</v>
       </c>
       <c r="K3">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L3),-J3,L3-J3)</f>
         <v>66</v>
       </c>
       <c r="L3" s="1">
         <v>69382</v>
       </c>
       <c r="M3">
-        <f t="shared" si="4"/>
+        <f>IF(ISBLANK(N3),-L3,N3-L3)</f>
         <v>129</v>
       </c>
       <c r="N3" s="1">
         <v>69511</v>
       </c>
       <c r="O3">
-        <f t="shared" si="5"/>
+        <f>IF(ISBLANK(P3),-N3,P3-N3)</f>
         <v>45</v>
       </c>
       <c r="P3" s="1">
         <v>69556</v>
       </c>
       <c r="Q3">
-        <f t="shared" si="6"/>
+        <f>IF(ISBLANK(R3),-P3,R3-P3)</f>
         <v>116</v>
       </c>
       <c r="R3" s="1">
         <v>69672</v>
       </c>
       <c r="S3">
-        <f t="shared" si="7"/>
+        <f>IF(ISBLANK(T3),-R3,T3-R3)</f>
         <v>1226</v>
       </c>
       <c r="T3" s="1">
         <v>70898</v>
       </c>
       <c r="U3">
-        <f t="shared" si="8"/>
+        <f>IF(ISBLANK(V3),-T3,V3-T3)</f>
         <v>270</v>
       </c>
       <c r="V3" s="1">
         <v>71168</v>
       </c>
       <c r="W3">
-        <f t="shared" si="9"/>
+        <f>IF(ISBLANK(X3),-V3,X3-V3)</f>
         <v>674</v>
       </c>
       <c r="X3" s="1">
         <v>71842</v>
       </c>
       <c r="Y3">
-        <f t="shared" si="10"/>
+        <f>IF(ISBLANK(Z3),-X3,Z3-X3)</f>
         <v>291</v>
       </c>
       <c r="Z3" s="1">
         <v>72133</v>
       </c>
       <c r="AA3">
-        <f t="shared" si="11"/>
+        <f>IF(ISBLANK(AB3),-Z3,AB3-Z3)</f>
         <v>720</v>
       </c>
       <c r="AB3" s="1">
         <v>72853</v>
       </c>
       <c r="AC3">
-        <f t="shared" si="12"/>
+        <f>IF(ISBLANK(AD3),-AB3,AD3-AB3)</f>
         <v>929</v>
       </c>
       <c r="AD3" s="1">
         <v>73782</v>
       </c>
       <c r="AE3">
-        <f t="shared" si="13"/>
+        <f>IF(ISBLANK(AF3),-AD3,AF3-AD3)</f>
         <v>588</v>
       </c>
       <c r="AF3" s="1">
         <v>74370</v>
       </c>
       <c r="AG3">
-        <f t="shared" si="14"/>
+        <f>IF(ISBLANK(AH3),-AF3,AH3-AF3)</f>
         <v>6253</v>
       </c>
       <c r="AH3" s="1">
         <v>80623</v>
       </c>
       <c r="AI3">
-        <f t="shared" si="15"/>
+        <f>IF(ISBLANK(AJ3),-AH3,AJ3-AH3)</f>
         <v>-80623</v>
       </c>
       <c r="AJ3" s="1">
@@ -8170,112 +8173,112 @@
         <v>10582</v>
       </c>
       <c r="E4">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F4),-D4,F4-D4)</f>
         <v>57</v>
       </c>
       <c r="F4" s="1">
         <v>10639</v>
       </c>
       <c r="G4">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H4),-F4,H4-F4)</f>
         <v>106</v>
       </c>
       <c r="H4" s="1">
         <v>10745</v>
       </c>
       <c r="I4">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J4),-H4,J4-H4)</f>
         <v>138</v>
       </c>
       <c r="J4" s="1">
         <v>10883</v>
       </c>
       <c r="K4">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L4),-J4,L4-J4)</f>
         <v>54</v>
       </c>
       <c r="L4" s="1">
         <v>10937</v>
       </c>
       <c r="M4">
-        <f t="shared" si="4"/>
+        <f>IF(ISBLANK(N4),-L4,N4-L4)</f>
         <v>300</v>
       </c>
       <c r="N4" s="1">
         <v>11237</v>
       </c>
       <c r="O4">
-        <f t="shared" si="5"/>
+        <f>IF(ISBLANK(P4),-N4,P4-N4)</f>
         <v>159</v>
       </c>
       <c r="P4" s="1">
         <v>11396</v>
       </c>
       <c r="Q4">
-        <f t="shared" si="6"/>
+        <f>IF(ISBLANK(R4),-P4,R4-P4)</f>
         <v>322</v>
       </c>
       <c r="R4" s="1">
         <v>11718</v>
       </c>
       <c r="S4">
-        <f t="shared" si="7"/>
+        <f>IF(ISBLANK(T4),-R4,T4-R4)</f>
         <v>908</v>
       </c>
       <c r="T4" s="1">
         <v>12626</v>
       </c>
       <c r="U4">
-        <f t="shared" si="8"/>
+        <f>IF(ISBLANK(V4),-T4,V4-T4)</f>
         <v>1585</v>
       </c>
       <c r="V4" s="1">
         <v>14211</v>
       </c>
       <c r="W4">
-        <f t="shared" si="9"/>
+        <f>IF(ISBLANK(X4),-V4,X4-V4)</f>
         <v>826</v>
       </c>
       <c r="X4" s="1">
         <v>15037</v>
       </c>
       <c r="Y4">
-        <f t="shared" si="10"/>
+        <f>IF(ISBLANK(Z4),-X4,Z4-X4)</f>
         <v>429</v>
       </c>
       <c r="Z4" s="1">
         <v>15466</v>
       </c>
       <c r="AA4">
-        <f t="shared" si="11"/>
+        <f>IF(ISBLANK(AB4),-Z4,AB4-Z4)</f>
         <v>1664</v>
       </c>
       <c r="AB4" s="1">
         <v>17130</v>
       </c>
       <c r="AC4">
-        <f t="shared" si="12"/>
+        <f>IF(ISBLANK(AD4),-AB4,AD4-AB4)</f>
         <v>-17130</v>
       </c>
       <c r="AD4" s="1">
         <v>0</v>
       </c>
       <c r="AE4">
-        <f t="shared" si="13"/>
+        <f>IF(ISBLANK(AF4),-AD4,AF4-AD4)</f>
         <v>0</v>
       </c>
       <c r="AF4" s="1">
         <v>0</v>
       </c>
       <c r="AG4">
-        <f t="shared" si="14"/>
+        <f>IF(ISBLANK(AH4),-AF4,AH4-AF4)</f>
         <v>0</v>
       </c>
       <c r="AH4" s="1">
         <v>0</v>
       </c>
       <c r="AI4">
-        <f t="shared" si="15"/>
+        <f>IF(ISBLANK(AJ4),-AH4,AJ4-AH4)</f>
         <v>0</v>
       </c>
       <c r="AJ4" s="1">
@@ -8296,112 +8299,112 @@
         <v>64605</v>
       </c>
       <c r="E5">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F5),-D5,F5-D5)</f>
         <v>26</v>
       </c>
       <c r="F5" s="1">
         <v>64631</v>
       </c>
       <c r="G5">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H5),-F5,H5-F5)</f>
         <v>61</v>
       </c>
       <c r="H5" s="1">
         <v>64692</v>
       </c>
       <c r="I5">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J5),-H5,J5-H5)</f>
         <v>71</v>
       </c>
       <c r="J5" s="1">
         <v>64763</v>
       </c>
       <c r="K5">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L5),-J5,L5-J5)</f>
         <v>136</v>
       </c>
       <c r="L5" s="1">
         <v>64899</v>
       </c>
       <c r="M5">
-        <f t="shared" si="4"/>
+        <f>IF(ISBLANK(N5),-L5,N5-L5)</f>
         <v>106</v>
       </c>
       <c r="N5" s="1">
         <v>65005</v>
       </c>
       <c r="O5">
-        <f t="shared" si="5"/>
+        <f>IF(ISBLANK(P5),-N5,P5-N5)</f>
         <v>110</v>
       </c>
       <c r="P5" s="1">
         <v>65115</v>
       </c>
       <c r="Q5">
-        <f t="shared" si="6"/>
+        <f>IF(ISBLANK(R5),-P5,R5-P5)</f>
         <v>137</v>
       </c>
       <c r="R5" s="1">
         <v>65252</v>
       </c>
       <c r="S5">
-        <f t="shared" si="7"/>
+        <f>IF(ISBLANK(T5),-R5,T5-R5)</f>
         <v>306</v>
       </c>
       <c r="T5" s="1">
         <v>65558</v>
       </c>
       <c r="U5">
-        <f t="shared" si="8"/>
+        <f>IF(ISBLANK(V5),-T5,V5-T5)</f>
         <v>491</v>
       </c>
       <c r="V5" s="1">
         <v>66049</v>
       </c>
       <c r="W5">
-        <f t="shared" si="9"/>
+        <f>IF(ISBLANK(X5),-V5,X5-V5)</f>
         <v>683</v>
       </c>
       <c r="X5" s="1">
         <v>66732</v>
       </c>
       <c r="Y5">
-        <f t="shared" si="10"/>
+        <f>IF(ISBLANK(Z5),-X5,Z5-X5)</f>
         <v>542</v>
       </c>
       <c r="Z5" s="1">
         <v>67274</v>
       </c>
       <c r="AA5">
-        <f t="shared" si="11"/>
+        <f>IF(ISBLANK(AB5),-Z5,AB5-Z5)</f>
         <v>622</v>
       </c>
       <c r="AB5" s="1">
         <v>67896</v>
       </c>
       <c r="AC5">
-        <f t="shared" si="12"/>
+        <f>IF(ISBLANK(AD5),-AB5,AD5-AB5)</f>
         <v>1194</v>
       </c>
       <c r="AD5" s="1">
         <v>69090</v>
       </c>
       <c r="AE5">
-        <f t="shared" si="13"/>
+        <f>IF(ISBLANK(AF5),-AD5,AF5-AD5)</f>
         <v>470</v>
       </c>
       <c r="AF5" s="1">
         <v>69560</v>
       </c>
       <c r="AG5">
-        <f t="shared" si="14"/>
+        <f>IF(ISBLANK(AH5),-AF5,AH5-AF5)</f>
         <v>20183</v>
       </c>
       <c r="AH5" s="1">
         <v>89743</v>
       </c>
       <c r="AI5">
-        <f t="shared" si="15"/>
+        <f>IF(ISBLANK(AJ5),-AH5,AJ5-AH5)</f>
         <v>8192</v>
       </c>
       <c r="AJ5" s="1">
@@ -8422,112 +8425,112 @@
         <v>38738</v>
       </c>
       <c r="E6">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F6),-D6,F6-D6)</f>
         <v>17</v>
       </c>
       <c r="F6" s="1">
         <v>38755</v>
       </c>
       <c r="G6">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H6),-F6,H6-F6)</f>
         <v>33</v>
       </c>
       <c r="H6" s="1">
         <v>38788</v>
       </c>
       <c r="I6">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J6),-H6,J6-H6)</f>
         <v>16</v>
       </c>
       <c r="J6" s="1">
         <v>38804</v>
       </c>
       <c r="K6">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L6),-J6,L6-J6)</f>
         <v>38</v>
       </c>
       <c r="L6" s="1">
         <v>38842</v>
       </c>
       <c r="M6">
-        <f t="shared" si="4"/>
+        <f>IF(ISBLANK(N6),-L6,N6-L6)</f>
         <v>84</v>
       </c>
       <c r="N6" s="1">
         <v>38926</v>
       </c>
       <c r="O6">
-        <f t="shared" si="5"/>
+        <f>IF(ISBLANK(P6),-N6,P6-N6)</f>
         <v>24</v>
       </c>
       <c r="P6" s="1">
         <v>38950</v>
       </c>
       <c r="Q6">
-        <f t="shared" si="6"/>
+        <f>IF(ISBLANK(R6),-P6,R6-P6)</f>
         <v>46</v>
       </c>
       <c r="R6" s="1">
         <v>38996</v>
       </c>
       <c r="S6">
-        <f t="shared" si="7"/>
+        <f>IF(ISBLANK(T6),-R6,T6-R6)</f>
         <v>298</v>
       </c>
       <c r="T6" s="1">
         <v>39294</v>
       </c>
       <c r="U6">
-        <f t="shared" si="8"/>
+        <f>IF(ISBLANK(V6),-T6,V6-T6)</f>
         <v>135</v>
       </c>
       <c r="V6" s="1">
         <v>39429</v>
       </c>
       <c r="W6">
-        <f t="shared" si="9"/>
+        <f>IF(ISBLANK(X6),-V6,X6-V6)</f>
         <v>426</v>
       </c>
       <c r="X6" s="1">
         <v>39855</v>
       </c>
       <c r="Y6">
-        <f t="shared" si="10"/>
+        <f>IF(ISBLANK(Z6),-X6,Z6-X6)</f>
         <v>159</v>
       </c>
       <c r="Z6" s="1">
         <v>40014</v>
       </c>
       <c r="AA6">
-        <f t="shared" si="11"/>
+        <f>IF(ISBLANK(AB6),-Z6,AB6-Z6)</f>
         <v>572</v>
       </c>
       <c r="AB6" s="1">
         <v>40586</v>
       </c>
       <c r="AC6">
-        <f t="shared" si="12"/>
+        <f>IF(ISBLANK(AD6),-AB6,AD6-AB6)</f>
         <v>483</v>
       </c>
       <c r="AD6" s="1">
         <v>41069</v>
       </c>
       <c r="AE6">
-        <f t="shared" si="13"/>
+        <f>IF(ISBLANK(AF6),-AD6,AF6-AD6)</f>
         <v>347</v>
       </c>
       <c r="AF6" s="1">
         <v>41416</v>
       </c>
       <c r="AG6">
-        <f t="shared" si="14"/>
+        <f>IF(ISBLANK(AH6),-AF6,AH6-AF6)</f>
         <v>-41416</v>
       </c>
       <c r="AH6" s="1">
         <v>0</v>
       </c>
       <c r="AI6">
-        <f t="shared" si="15"/>
+        <f>IF(ISBLANK(AJ6),-AH6,AJ6-AH6)</f>
         <v>0</v>
       </c>
       <c r="AJ6" s="1">
@@ -8548,112 +8551,112 @@
         <v>3182</v>
       </c>
       <c r="E7">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F7),-D7,F7-D7)</f>
         <v>15</v>
       </c>
       <c r="F7" s="1">
         <v>3197</v>
       </c>
       <c r="G7">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H7),-F7,H7-F7)</f>
         <v>60</v>
       </c>
       <c r="H7" s="1">
         <v>3257</v>
       </c>
       <c r="I7">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J7),-H7,J7-H7)</f>
         <v>43</v>
       </c>
       <c r="J7" s="1">
         <v>3300</v>
       </c>
       <c r="K7">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L7),-J7,L7-J7)</f>
         <v>32</v>
       </c>
       <c r="L7" s="1">
         <v>3332</v>
       </c>
       <c r="M7">
-        <f t="shared" si="4"/>
+        <f>IF(ISBLANK(N7),-L7,N7-L7)</f>
         <v>-3332</v>
       </c>
       <c r="N7" s="1">
         <v>0</v>
       </c>
       <c r="O7">
-        <f t="shared" si="5"/>
+        <f>IF(ISBLANK(P7),-N7,P7-N7)</f>
         <v>0</v>
       </c>
       <c r="P7" s="1">
         <v>0</v>
       </c>
       <c r="Q7">
-        <f t="shared" si="6"/>
+        <f>IF(ISBLANK(R7),-P7,R7-P7)</f>
         <v>0</v>
       </c>
       <c r="R7" s="1">
         <v>0</v>
       </c>
       <c r="S7">
-        <f t="shared" si="7"/>
+        <f>IF(ISBLANK(T7),-R7,T7-R7)</f>
         <v>0</v>
       </c>
       <c r="T7" s="1">
         <v>0</v>
       </c>
       <c r="U7">
-        <f t="shared" si="8"/>
+        <f>IF(ISBLANK(V7),-T7,V7-T7)</f>
         <v>0</v>
       </c>
       <c r="V7" s="1">
         <v>0</v>
       </c>
       <c r="W7">
-        <f t="shared" si="9"/>
+        <f>IF(ISBLANK(X7),-V7,X7-V7)</f>
         <v>0</v>
       </c>
       <c r="X7" s="1">
         <v>0</v>
       </c>
       <c r="Y7">
-        <f t="shared" si="10"/>
+        <f>IF(ISBLANK(Z7),-X7,Z7-X7)</f>
         <v>0</v>
       </c>
       <c r="Z7" s="1">
         <v>0</v>
       </c>
       <c r="AA7">
-        <f t="shared" si="11"/>
+        <f>IF(ISBLANK(AB7),-Z7,AB7-Z7)</f>
         <v>0</v>
       </c>
       <c r="AB7" s="1">
         <v>0</v>
       </c>
       <c r="AC7">
-        <f t="shared" si="12"/>
+        <f>IF(ISBLANK(AD7),-AB7,AD7-AB7)</f>
         <v>0</v>
       </c>
       <c r="AD7" s="1">
         <v>0</v>
       </c>
       <c r="AE7">
-        <f t="shared" si="13"/>
+        <f>IF(ISBLANK(AF7),-AD7,AF7-AD7)</f>
         <v>0</v>
       </c>
       <c r="AF7" s="1">
         <v>0</v>
       </c>
       <c r="AG7">
-        <f t="shared" si="14"/>
+        <f>IF(ISBLANK(AH7),-AF7,AH7-AF7)</f>
         <v>0</v>
       </c>
       <c r="AH7" s="1">
         <v>0</v>
       </c>
       <c r="AI7">
-        <f t="shared" si="15"/>
+        <f>IF(ISBLANK(AJ7),-AH7,AJ7-AH7)</f>
         <v>0</v>
       </c>
       <c r="AJ7" s="1">
@@ -8674,112 +8677,112 @@
         <v>9306</v>
       </c>
       <c r="E8">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F8),-D8,F8-D8)</f>
         <v>25</v>
       </c>
       <c r="F8" s="1">
         <v>9331</v>
       </c>
       <c r="G8">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H8),-F8,H8-F8)</f>
         <v>70</v>
       </c>
       <c r="H8" s="1">
         <v>9401</v>
       </c>
       <c r="I8">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J8),-H8,J8-H8)</f>
         <v>35</v>
       </c>
       <c r="J8" s="1">
         <v>9436</v>
       </c>
       <c r="K8">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L8),-J8,L8-J8)</f>
         <v>60</v>
       </c>
       <c r="L8" s="1">
         <v>9496</v>
       </c>
       <c r="M8">
-        <f t="shared" si="4"/>
+        <f>IF(ISBLANK(N8),-L8,N8-L8)</f>
         <v>228</v>
       </c>
       <c r="N8" s="1">
         <v>9724</v>
       </c>
       <c r="O8">
-        <f t="shared" si="5"/>
+        <f>IF(ISBLANK(P8),-N8,P8-N8)</f>
         <v>145</v>
       </c>
       <c r="P8" s="1">
         <v>9869</v>
       </c>
       <c r="Q8">
-        <f t="shared" si="6"/>
+        <f>IF(ISBLANK(R8),-P8,R8-P8)</f>
         <v>106</v>
       </c>
       <c r="R8" s="1">
         <v>9975</v>
       </c>
       <c r="S8">
-        <f t="shared" si="7"/>
+        <f>IF(ISBLANK(T8),-R8,T8-R8)</f>
         <v>247</v>
       </c>
       <c r="T8" s="1">
         <v>10222</v>
       </c>
       <c r="U8">
-        <f t="shared" si="8"/>
+        <f>IF(ISBLANK(V8),-T8,V8-T8)</f>
         <v>616</v>
       </c>
       <c r="V8" s="1">
         <v>10838</v>
       </c>
       <c r="W8">
-        <f t="shared" si="9"/>
+        <f>IF(ISBLANK(X8),-V8,X8-V8)</f>
         <v>-10838</v>
       </c>
       <c r="X8" s="1">
         <v>0</v>
       </c>
       <c r="Y8">
-        <f t="shared" si="10"/>
+        <f>IF(ISBLANK(Z8),-X8,Z8-X8)</f>
         <v>0</v>
       </c>
       <c r="Z8" s="1">
         <v>0</v>
       </c>
       <c r="AA8">
-        <f t="shared" si="11"/>
+        <f>IF(ISBLANK(AB8),-Z8,AB8-Z8)</f>
         <v>0</v>
       </c>
       <c r="AB8" s="1">
         <v>0</v>
       </c>
       <c r="AC8">
-        <f t="shared" si="12"/>
+        <f>IF(ISBLANK(AD8),-AB8,AD8-AB8)</f>
         <v>0</v>
       </c>
       <c r="AD8" s="1">
         <v>0</v>
       </c>
       <c r="AE8">
-        <f t="shared" si="13"/>
+        <f>IF(ISBLANK(AF8),-AD8,AF8-AD8)</f>
         <v>0</v>
       </c>
       <c r="AF8" s="1">
         <v>0</v>
       </c>
       <c r="AG8">
-        <f t="shared" si="14"/>
+        <f>IF(ISBLANK(AH8),-AF8,AH8-AF8)</f>
         <v>0</v>
       </c>
       <c r="AH8" s="1">
         <v>0</v>
       </c>
       <c r="AI8">
-        <f t="shared" si="15"/>
+        <f>IF(ISBLANK(AJ8),-AH8,AJ8-AH8)</f>
         <v>0</v>
       </c>
       <c r="AJ8" s="1">
@@ -8800,112 +8803,112 @@
         <v>7475</v>
       </c>
       <c r="E9">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F9),-D9,F9-D9)</f>
         <v>23</v>
       </c>
       <c r="F9" s="1">
         <v>7498</v>
       </c>
       <c r="G9">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H9),-F9,H9-F9)</f>
         <v>98</v>
       </c>
       <c r="H9" s="1">
         <v>7596</v>
       </c>
       <c r="I9">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J9),-H9,J9-H9)</f>
         <v>142</v>
       </c>
       <c r="J9" s="1">
         <v>7738</v>
       </c>
       <c r="K9">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L9),-J9,L9-J9)</f>
         <v>70</v>
       </c>
       <c r="L9" s="1">
         <v>7808</v>
       </c>
       <c r="M9">
-        <f t="shared" si="4"/>
+        <f>IF(ISBLANK(N9),-L9,N9-L9)</f>
         <v>197</v>
       </c>
       <c r="N9" s="1">
         <v>8005</v>
       </c>
       <c r="O9">
-        <f t="shared" si="5"/>
+        <f>IF(ISBLANK(P9),-N9,P9-N9)</f>
         <v>192</v>
       </c>
       <c r="P9" s="1">
         <v>8197</v>
       </c>
       <c r="Q9">
-        <f t="shared" si="6"/>
+        <f>IF(ISBLANK(R9),-P9,R9-P9)</f>
         <v>176</v>
       </c>
       <c r="R9" s="1">
         <v>8373</v>
       </c>
       <c r="S9">
-        <f t="shared" si="7"/>
+        <f>IF(ISBLANK(T9),-R9,T9-R9)</f>
         <v>188</v>
       </c>
       <c r="T9" s="1">
         <v>8561</v>
       </c>
       <c r="U9">
-        <f t="shared" si="8"/>
+        <f>IF(ISBLANK(V9),-T9,V9-T9)</f>
         <v>-8561</v>
       </c>
       <c r="V9" s="1">
         <v>0</v>
       </c>
       <c r="W9">
-        <f t="shared" si="9"/>
+        <f>IF(ISBLANK(X9),-V9,X9-V9)</f>
         <v>0</v>
       </c>
       <c r="X9" s="1">
         <v>0</v>
       </c>
       <c r="Y9">
-        <f t="shared" si="10"/>
+        <f>IF(ISBLANK(Z9),-X9,Z9-X9)</f>
         <v>0</v>
       </c>
       <c r="Z9" s="1">
         <v>0</v>
       </c>
       <c r="AA9">
-        <f t="shared" si="11"/>
+        <f>IF(ISBLANK(AB9),-Z9,AB9-Z9)</f>
         <v>0</v>
       </c>
       <c r="AB9" s="1">
         <v>0</v>
       </c>
       <c r="AC9">
-        <f t="shared" si="12"/>
+        <f>IF(ISBLANK(AD9),-AB9,AD9-AB9)</f>
         <v>0</v>
       </c>
       <c r="AD9" s="1">
         <v>0</v>
       </c>
       <c r="AE9">
-        <f t="shared" si="13"/>
+        <f>IF(ISBLANK(AF9),-AD9,AF9-AD9)</f>
         <v>0</v>
       </c>
       <c r="AF9" s="1">
         <v>0</v>
       </c>
       <c r="AG9">
-        <f t="shared" si="14"/>
+        <f>IF(ISBLANK(AH9),-AF9,AH9-AF9)</f>
         <v>0</v>
       </c>
       <c r="AH9" s="1">
         <v>0</v>
       </c>
       <c r="AI9">
-        <f t="shared" si="15"/>
+        <f>IF(ISBLANK(AJ9),-AH9,AJ9-AH9)</f>
         <v>0</v>
       </c>
       <c r="AJ9" s="1">
@@ -8926,112 +8929,112 @@
         <v>84083</v>
       </c>
       <c r="E10">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F10),-D10,F10-D10)</f>
         <v>23</v>
       </c>
       <c r="F10" s="1">
         <v>84106</v>
       </c>
       <c r="G10">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H10),-F10,H10-F10)</f>
         <v>58</v>
       </c>
       <c r="H10" s="1">
         <v>84164</v>
       </c>
       <c r="I10">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J10),-H10,J10-H10)</f>
         <v>74</v>
       </c>
       <c r="J10" s="1">
         <v>84238</v>
       </c>
       <c r="K10">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L10),-J10,L10-J10)</f>
         <v>150</v>
       </c>
       <c r="L10" s="1">
         <v>84388</v>
       </c>
       <c r="M10">
-        <f t="shared" si="4"/>
+        <f>IF(ISBLANK(N10),-L10,N10-L10)</f>
         <v>171</v>
       </c>
       <c r="N10" s="1">
         <v>84559</v>
       </c>
       <c r="O10">
-        <f t="shared" si="5"/>
+        <f>IF(ISBLANK(P10),-N10,P10-N10)</f>
         <v>95</v>
       </c>
       <c r="P10" s="1">
         <v>84654</v>
       </c>
       <c r="Q10">
-        <f t="shared" si="6"/>
+        <f>IF(ISBLANK(R10),-P10,R10-P10)</f>
         <v>187</v>
       </c>
       <c r="R10" s="1">
         <v>84841</v>
       </c>
       <c r="S10">
-        <f t="shared" si="7"/>
+        <f>IF(ISBLANK(T10),-R10,T10-R10)</f>
         <v>130</v>
       </c>
       <c r="T10" s="1">
         <v>84971</v>
       </c>
       <c r="U10">
-        <f t="shared" si="8"/>
+        <f>IF(ISBLANK(V10),-T10,V10-T10)</f>
         <v>480</v>
       </c>
       <c r="V10" s="1">
         <v>85451</v>
       </c>
       <c r="W10">
-        <f t="shared" si="9"/>
+        <f>IF(ISBLANK(X10),-V10,X10-V10)</f>
         <v>575</v>
       </c>
       <c r="X10" s="1">
         <v>86026</v>
       </c>
       <c r="Y10">
-        <f t="shared" si="10"/>
+        <f>IF(ISBLANK(Z10),-X10,Z10-X10)</f>
         <v>1010</v>
       </c>
       <c r="Z10" s="1">
         <v>87036</v>
       </c>
       <c r="AA10">
-        <f t="shared" si="11"/>
+        <f>IF(ISBLANK(AB10),-Z10,AB10-Z10)</f>
         <v>928</v>
       </c>
       <c r="AB10" s="1">
         <v>87964</v>
       </c>
       <c r="AC10">
-        <f t="shared" si="12"/>
+        <f>IF(ISBLANK(AD10),-AB10,AD10-AB10)</f>
         <v>637</v>
       </c>
       <c r="AD10" s="1">
         <v>88601</v>
       </c>
       <c r="AE10">
-        <f t="shared" si="13"/>
+        <f>IF(ISBLANK(AF10),-AD10,AF10-AD10)</f>
         <v>435</v>
       </c>
       <c r="AF10" s="1">
         <v>89036</v>
       </c>
       <c r="AG10">
-        <f t="shared" si="14"/>
+        <f>IF(ISBLANK(AH10),-AF10,AH10-AF10)</f>
         <v>3849</v>
       </c>
       <c r="AH10" s="1">
         <v>92885</v>
       </c>
       <c r="AI10">
-        <f t="shared" si="15"/>
+        <f>IF(ISBLANK(AJ10),-AH10,AJ10-AH10)</f>
         <v>38767</v>
       </c>
       <c r="AJ10" s="1">
@@ -9052,112 +9055,112 @@
         <v>118444</v>
       </c>
       <c r="E11">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F11),-D11,F11-D11)</f>
         <v>45</v>
       </c>
       <c r="F11" s="1">
         <v>118489</v>
       </c>
       <c r="G11">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H11),-F11,H11-F11)</f>
         <v>186</v>
       </c>
       <c r="H11" s="1">
         <v>118675</v>
       </c>
       <c r="I11">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J11),-H11,J11-H11)</f>
         <v>98</v>
       </c>
       <c r="J11" s="1">
         <v>118773</v>
       </c>
       <c r="K11">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L11),-J11,L11-J11)</f>
         <v>350</v>
       </c>
       <c r="L11" s="1">
         <v>119123</v>
       </c>
       <c r="M11">
-        <f t="shared" si="4"/>
+        <f>IF(ISBLANK(N11),-L11,N11-L11)</f>
         <v>257</v>
       </c>
       <c r="N11" s="1">
         <v>119380</v>
       </c>
       <c r="O11">
-        <f t="shared" si="5"/>
+        <f>IF(ISBLANK(P11),-N11,P11-N11)</f>
         <v>165</v>
       </c>
       <c r="P11" s="1">
         <v>119545</v>
       </c>
       <c r="Q11">
-        <f t="shared" si="6"/>
+        <f>IF(ISBLANK(R11),-P11,R11-P11)</f>
         <v>170</v>
       </c>
       <c r="R11" s="1">
         <v>119715</v>
       </c>
       <c r="S11">
-        <f t="shared" si="7"/>
+        <f>IF(ISBLANK(T11),-R11,T11-R11)</f>
         <v>168</v>
       </c>
       <c r="T11" s="1">
         <v>119883</v>
       </c>
       <c r="U11">
-        <f t="shared" si="8"/>
+        <f>IF(ISBLANK(V11),-T11,V11-T11)</f>
         <v>0</v>
       </c>
       <c r="V11" s="1">
         <v>119883</v>
       </c>
       <c r="W11">
-        <f t="shared" si="9"/>
+        <f>IF(ISBLANK(X11),-V11,X11-V11)</f>
         <v>0</v>
       </c>
       <c r="X11" s="1">
         <v>119883</v>
       </c>
       <c r="Y11">
-        <f t="shared" si="10"/>
+        <f>IF(ISBLANK(Z11),-X11,Z11-X11)</f>
         <v>0</v>
       </c>
       <c r="Z11" s="1">
         <v>119883</v>
       </c>
       <c r="AA11">
-        <f t="shared" si="11"/>
+        <f>IF(ISBLANK(AB11),-Z11,AB11-Z11)</f>
         <v>0</v>
       </c>
       <c r="AB11" s="1">
         <v>119883</v>
       </c>
       <c r="AC11">
-        <f t="shared" si="12"/>
+        <f>IF(ISBLANK(AD11),-AB11,AD11-AB11)</f>
         <v>0</v>
       </c>
       <c r="AD11" s="1">
         <v>119883</v>
       </c>
       <c r="AE11">
-        <f t="shared" si="13"/>
+        <f>IF(ISBLANK(AF11),-AD11,AF11-AD11)</f>
         <v>0</v>
       </c>
       <c r="AF11" s="1">
         <v>119883</v>
       </c>
       <c r="AG11">
-        <f t="shared" si="14"/>
+        <f>IF(ISBLANK(AH11),-AF11,AH11-AF11)</f>
         <v>0</v>
       </c>
       <c r="AH11" s="1">
         <v>119883</v>
       </c>
       <c r="AI11">
-        <f t="shared" si="15"/>
+        <f>IF(ISBLANK(AJ11),-AH11,AJ11-AH11)</f>
         <v>0</v>
       </c>
       <c r="AJ11" s="1">
@@ -9178,112 +9181,112 @@
         <v>2395</v>
       </c>
       <c r="E12">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F12),-D12,F12-D12)</f>
         <v>14</v>
       </c>
       <c r="F12" s="1">
         <v>2409</v>
       </c>
       <c r="G12">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H12),-F12,H12-F12)</f>
         <v>-2409</v>
       </c>
       <c r="H12" s="1">
         <v>0</v>
       </c>
       <c r="I12">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J12),-H12,J12-H12)</f>
         <v>0</v>
       </c>
       <c r="J12" s="1">
         <v>0</v>
       </c>
       <c r="K12">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L12),-J12,L12-J12)</f>
         <v>0</v>
       </c>
       <c r="L12" s="1">
         <v>0</v>
       </c>
       <c r="M12">
-        <f t="shared" si="4"/>
+        <f>IF(ISBLANK(N12),-L12,N12-L12)</f>
         <v>0</v>
       </c>
       <c r="N12" s="1">
         <v>0</v>
       </c>
       <c r="O12">
-        <f t="shared" si="5"/>
+        <f>IF(ISBLANK(P12),-N12,P12-N12)</f>
         <v>0</v>
       </c>
       <c r="P12" s="1">
         <v>0</v>
       </c>
       <c r="Q12">
-        <f t="shared" si="6"/>
+        <f>IF(ISBLANK(R12),-P12,R12-P12)</f>
         <v>0</v>
       </c>
       <c r="R12" s="1">
         <v>0</v>
       </c>
       <c r="S12">
-        <f t="shared" si="7"/>
+        <f>IF(ISBLANK(T12),-R12,T12-R12)</f>
         <v>0</v>
       </c>
       <c r="T12" s="1">
         <v>0</v>
       </c>
       <c r="U12">
-        <f t="shared" si="8"/>
+        <f>IF(ISBLANK(V12),-T12,V12-T12)</f>
         <v>0</v>
       </c>
       <c r="V12" s="1">
         <v>0</v>
       </c>
       <c r="W12">
-        <f t="shared" si="9"/>
+        <f>IF(ISBLANK(X12),-V12,X12-V12)</f>
         <v>0</v>
       </c>
       <c r="X12" s="1">
         <v>0</v>
       </c>
       <c r="Y12">
-        <f t="shared" si="10"/>
+        <f>IF(ISBLANK(Z12),-X12,Z12-X12)</f>
         <v>0</v>
       </c>
       <c r="Z12" s="1">
         <v>0</v>
       </c>
       <c r="AA12">
-        <f t="shared" si="11"/>
+        <f>IF(ISBLANK(AB12),-Z12,AB12-Z12)</f>
         <v>0</v>
       </c>
       <c r="AB12" s="1">
         <v>0</v>
       </c>
       <c r="AC12">
-        <f t="shared" si="12"/>
+        <f>IF(ISBLANK(AD12),-AB12,AD12-AB12)</f>
         <v>0</v>
       </c>
       <c r="AD12" s="1">
         <v>0</v>
       </c>
       <c r="AE12">
-        <f t="shared" si="13"/>
+        <f>IF(ISBLANK(AF12),-AD12,AF12-AD12)</f>
         <v>0</v>
       </c>
       <c r="AF12" s="1">
         <v>0</v>
       </c>
       <c r="AG12">
-        <f t="shared" si="14"/>
+        <f>IF(ISBLANK(AH12),-AF12,AH12-AF12)</f>
         <v>0</v>
       </c>
       <c r="AH12" s="1">
         <v>0</v>
       </c>
       <c r="AI12">
-        <f t="shared" si="15"/>
+        <f>IF(ISBLANK(AJ12),-AH12,AJ12-AH12)</f>
         <v>0</v>
       </c>
       <c r="AJ12" s="1">
@@ -9303,112 +9306,112 @@
         <v>9423</v>
       </c>
       <c r="E13">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F13),-D13,F13-D13)</f>
         <v>32</v>
       </c>
       <c r="F13" s="1">
         <v>9455</v>
       </c>
       <c r="G13">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H13),-F13,H13-F13)</f>
         <v>325</v>
       </c>
       <c r="H13" s="1">
         <v>9780</v>
       </c>
       <c r="I13">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J13),-H13,J13-H13)</f>
         <v>75</v>
       </c>
       <c r="J13" s="1">
         <v>9855</v>
       </c>
       <c r="K13">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L13),-J13,L13-J13)</f>
         <v>114</v>
       </c>
       <c r="L13" s="1">
         <v>9969</v>
       </c>
       <c r="M13">
-        <f t="shared" si="4"/>
+        <f>IF(ISBLANK(N13),-L13,N13-L13)</f>
         <v>280</v>
       </c>
       <c r="N13" s="1">
         <v>10249</v>
       </c>
       <c r="O13">
-        <f t="shared" si="5"/>
+        <f>IF(ISBLANK(P13),-N13,P13-N13)</f>
         <v>78</v>
       </c>
       <c r="P13" s="1">
         <v>10327</v>
       </c>
       <c r="Q13">
-        <f t="shared" si="6"/>
+        <f>IF(ISBLANK(R13),-P13,R13-P13)</f>
         <v>137</v>
       </c>
       <c r="R13" s="1">
         <v>10464</v>
       </c>
       <c r="S13">
-        <f t="shared" si="7"/>
+        <f>IF(ISBLANK(T13),-R13,T13-R13)</f>
         <v>79</v>
       </c>
       <c r="T13" s="1">
         <v>10543</v>
       </c>
       <c r="U13">
-        <f t="shared" si="8"/>
+        <f>IF(ISBLANK(V13),-T13,V13-T13)</f>
         <v>1160</v>
       </c>
       <c r="V13" s="1">
         <v>11703</v>
       </c>
       <c r="W13">
-        <f t="shared" si="9"/>
+        <f>IF(ISBLANK(X13),-V13,X13-V13)</f>
         <v>568</v>
       </c>
       <c r="X13" s="1">
         <v>12271</v>
       </c>
       <c r="Y13">
-        <f t="shared" si="10"/>
+        <f>IF(ISBLANK(Z13),-X13,Z13-X13)</f>
         <v>499</v>
       </c>
       <c r="Z13" s="1">
         <v>12770</v>
       </c>
       <c r="AA13">
-        <f t="shared" si="11"/>
+        <f>IF(ISBLANK(AB13),-Z13,AB13-Z13)</f>
         <v>-12770</v>
       </c>
       <c r="AB13" s="1">
         <v>0</v>
       </c>
       <c r="AC13">
-        <f t="shared" si="12"/>
+        <f>IF(ISBLANK(AD13),-AB13,AD13-AB13)</f>
         <v>0</v>
       </c>
       <c r="AD13" s="1">
         <v>0</v>
       </c>
       <c r="AE13">
-        <f t="shared" si="13"/>
+        <f>IF(ISBLANK(AF13),-AD13,AF13-AD13)</f>
         <v>0</v>
       </c>
       <c r="AF13" s="1">
         <v>0</v>
       </c>
       <c r="AG13">
-        <f t="shared" si="14"/>
+        <f>IF(ISBLANK(AH13),-AF13,AH13-AF13)</f>
         <v>0</v>
       </c>
       <c r="AH13" s="1">
         <v>0</v>
       </c>
       <c r="AI13">
-        <f t="shared" si="15"/>
+        <f>IF(ISBLANK(AJ13),-AH13,AJ13-AH13)</f>
         <v>0</v>
       </c>
       <c r="AJ13" s="1">
@@ -9417,245 +9420,245 @@
     </row>
     <row r="14" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="D14" s="1">
-        <v>79072</v>
+        <v>22075</v>
       </c>
       <c r="E14">
-        <f t="shared" si="0"/>
-        <v>68</v>
+        <f>IF(ISBLANK(F14),-D14,F14-D14)</f>
+        <v>38</v>
       </c>
       <c r="F14" s="1">
-        <v>79140</v>
+        <v>22113</v>
       </c>
       <c r="G14">
-        <f t="shared" si="1"/>
-        <v>142</v>
+        <f>IF(ISBLANK(H14),-F14,H14-F14)</f>
+        <v>80</v>
       </c>
       <c r="H14" s="1">
-        <v>79282</v>
+        <v>22193</v>
       </c>
       <c r="I14">
-        <f t="shared" si="2"/>
-        <v>105</v>
+        <f>IF(ISBLANK(J14),-H14,J14-H14)</f>
+        <v>58</v>
       </c>
       <c r="J14" s="1">
-        <v>79387</v>
+        <v>22251</v>
       </c>
       <c r="K14">
-        <f t="shared" si="3"/>
-        <v>186</v>
+        <f>IF(ISBLANK(L14),-J14,L14-J14)</f>
+        <v>70</v>
       </c>
       <c r="L14" s="1">
-        <v>79573</v>
+        <v>22321</v>
       </c>
       <c r="M14">
-        <f t="shared" si="4"/>
-        <v>168</v>
+        <f>IF(ISBLANK(N14),-L14,N14-L14)</f>
+        <v>62</v>
       </c>
       <c r="N14" s="1">
-        <v>79741</v>
+        <v>22383</v>
       </c>
       <c r="O14">
-        <f t="shared" si="5"/>
-        <v>204</v>
+        <f>IF(ISBLANK(P14),-N14,P14-N14)</f>
+        <v>70</v>
       </c>
       <c r="P14" s="1">
-        <v>79945</v>
+        <v>22453</v>
       </c>
       <c r="Q14">
-        <f t="shared" si="6"/>
-        <v>305</v>
+        <f>IF(ISBLANK(R14),-P14,R14-P14)</f>
+        <v>173</v>
       </c>
       <c r="R14" s="1">
-        <v>80250</v>
+        <v>22626</v>
       </c>
       <c r="S14">
-        <f t="shared" si="7"/>
-        <v>127</v>
+        <f>IF(ISBLANK(T14),-R14,T14-R14)</f>
+        <v>74</v>
       </c>
       <c r="T14" s="1">
-        <v>80377</v>
+        <v>22700</v>
       </c>
       <c r="U14">
-        <f t="shared" si="8"/>
-        <v>446</v>
+        <f>IF(ISBLANK(V14),-T14,V14-T14)</f>
+        <v>193</v>
       </c>
       <c r="V14" s="1">
-        <v>80823</v>
+        <v>22893</v>
       </c>
       <c r="W14">
-        <f t="shared" si="9"/>
-        <v>991</v>
+        <f>IF(ISBLANK(X14),-V14,X14-V14)</f>
+        <v>626</v>
       </c>
       <c r="X14" s="1">
-        <v>81814</v>
+        <v>23519</v>
       </c>
       <c r="Y14">
-        <f t="shared" si="10"/>
-        <v>1119</v>
+        <f>IF(ISBLANK(Z14),-X14,Z14-X14)</f>
+        <v>330</v>
       </c>
       <c r="Z14" s="1">
-        <v>82933</v>
+        <v>23849</v>
       </c>
       <c r="AA14">
-        <f t="shared" si="11"/>
-        <v>958</v>
+        <f>IF(ISBLANK(AB14),-Z14,AB14-Z14)</f>
+        <v>483</v>
       </c>
       <c r="AB14" s="1">
-        <v>83891</v>
+        <v>24332</v>
       </c>
       <c r="AC14">
-        <f t="shared" si="12"/>
-        <v>1108</v>
+        <f>IF(ISBLANK(AD14),-AB14,AD14-AB14)</f>
+        <v>600</v>
       </c>
       <c r="AD14" s="1">
-        <v>84999</v>
+        <v>24932</v>
       </c>
       <c r="AE14">
-        <f t="shared" si="13"/>
-        <v>2323</v>
+        <f>IF(ISBLANK(AF14),-AD14,AF14-AD14)</f>
+        <v>1026</v>
       </c>
       <c r="AF14" s="1">
-        <v>87322</v>
+        <v>25958</v>
       </c>
       <c r="AG14">
-        <f t="shared" si="14"/>
-        <v>4517</v>
+        <f>IF(ISBLANK(AH14),-AF14,AH14-AF14)</f>
+        <v>-25958</v>
       </c>
       <c r="AH14" s="1">
-        <v>91839</v>
+        <v>0</v>
       </c>
       <c r="AI14">
-        <f t="shared" si="15"/>
-        <v>3734</v>
+        <f>IF(ISBLANK(AJ14),-AH14,AJ14-AH14)</f>
+        <v>0</v>
       </c>
       <c r="AJ14" s="1">
-        <v>95573</v>
+        <v>0</v>
       </c>
       <c r="AK14" s="1"/>
     </row>
     <row r="15" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="D15" s="1">
-        <v>22075</v>
+        <v>9823</v>
       </c>
       <c r="E15">
-        <f t="shared" si="0"/>
-        <v>38</v>
+        <f>IF(ISBLANK(F15),-D15,F15-D15)</f>
+        <v>37</v>
       </c>
       <c r="F15" s="1">
-        <v>22113</v>
+        <v>9860</v>
       </c>
       <c r="G15">
-        <f t="shared" si="1"/>
-        <v>80</v>
+        <f>IF(ISBLANK(H15),-F15,H15-F15)</f>
+        <v>76</v>
       </c>
       <c r="H15" s="1">
-        <v>22193</v>
+        <v>9936</v>
       </c>
       <c r="I15">
-        <f t="shared" si="2"/>
-        <v>58</v>
+        <f>IF(ISBLANK(J15),-H15,J15-H15)</f>
+        <v>54</v>
       </c>
       <c r="J15" s="1">
-        <v>22251</v>
+        <v>9990</v>
       </c>
       <c r="K15">
-        <f t="shared" si="3"/>
-        <v>70</v>
+        <f>IF(ISBLANK(L15),-J15,L15-J15)</f>
+        <v>184</v>
       </c>
       <c r="L15" s="1">
-        <v>22321</v>
+        <v>10174</v>
       </c>
       <c r="M15">
-        <f t="shared" si="4"/>
-        <v>62</v>
+        <f>IF(ISBLANK(N15),-L15,N15-L15)</f>
+        <v>52</v>
       </c>
       <c r="N15" s="1">
-        <v>22383</v>
+        <v>10226</v>
       </c>
       <c r="O15">
-        <f t="shared" si="5"/>
-        <v>70</v>
+        <f>IF(ISBLANK(P15),-N15,P15-N15)</f>
+        <v>168</v>
       </c>
       <c r="P15" s="1">
-        <v>22453</v>
+        <v>10394</v>
       </c>
       <c r="Q15">
-        <f t="shared" si="6"/>
-        <v>173</v>
+        <f>IF(ISBLANK(R15),-P15,R15-P15)</f>
+        <v>214</v>
       </c>
       <c r="R15" s="1">
-        <v>22626</v>
+        <v>10608</v>
       </c>
       <c r="S15">
-        <f t="shared" si="7"/>
-        <v>74</v>
+        <f>IF(ISBLANK(T15),-R15,T15-R15)</f>
+        <v>48</v>
       </c>
       <c r="T15" s="1">
-        <v>22700</v>
+        <v>10656</v>
       </c>
       <c r="U15">
-        <f t="shared" si="8"/>
-        <v>193</v>
+        <f>IF(ISBLANK(V15),-T15,V15-T15)</f>
+        <v>286</v>
       </c>
       <c r="V15" s="1">
-        <v>22893</v>
+        <v>10942</v>
       </c>
       <c r="W15">
-        <f t="shared" si="9"/>
-        <v>626</v>
+        <f>IF(ISBLANK(X15),-V15,X15-V15)</f>
+        <v>208</v>
       </c>
       <c r="X15" s="1">
-        <v>23519</v>
+        <v>11150</v>
       </c>
       <c r="Y15">
-        <f t="shared" si="10"/>
-        <v>330</v>
+        <f>IF(ISBLANK(Z15),-X15,Z15-X15)</f>
+        <v>-11150</v>
       </c>
       <c r="Z15" s="1">
-        <v>23849</v>
+        <v>0</v>
       </c>
       <c r="AA15">
-        <f t="shared" si="11"/>
-        <v>483</v>
+        <f>IF(ISBLANK(AB15),-Z15,AB15-Z15)</f>
+        <v>0</v>
       </c>
       <c r="AB15" s="1">
-        <v>24332</v>
+        <v>0</v>
       </c>
       <c r="AC15">
-        <f t="shared" si="12"/>
-        <v>600</v>
+        <f>IF(ISBLANK(AD15),-AB15,AD15-AB15)</f>
+        <v>0</v>
       </c>
       <c r="AD15" s="1">
-        <v>24932</v>
+        <v>0</v>
       </c>
       <c r="AE15">
-        <f t="shared" si="13"/>
-        <v>1026</v>
+        <f>IF(ISBLANK(AF15),-AD15,AF15-AD15)</f>
+        <v>0</v>
       </c>
       <c r="AF15" s="1">
-        <v>25958</v>
+        <v>0</v>
       </c>
       <c r="AG15">
-        <f t="shared" si="14"/>
-        <v>-25958</v>
+        <f>IF(ISBLANK(AH15),-AF15,AH15-AF15)</f>
+        <v>0</v>
       </c>
       <c r="AH15" s="1">
         <v>0</v>
       </c>
       <c r="AI15">
-        <f t="shared" si="15"/>
+        <f>IF(ISBLANK(AJ15),-AH15,AJ15-AH15)</f>
         <v>0</v>
       </c>
       <c r="AJ15" s="1">
@@ -9664,121 +9667,121 @@
     </row>
     <row r="16" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="D16" s="1">
-        <v>9823</v>
+        <v>3682</v>
       </c>
       <c r="E16">
-        <f t="shared" si="0"/>
-        <v>37</v>
+        <f>IF(ISBLANK(F16),-D16,F16-D16)</f>
+        <v>77</v>
       </c>
       <c r="F16" s="1">
-        <v>9860</v>
+        <v>3759</v>
       </c>
       <c r="G16">
-        <f t="shared" si="1"/>
-        <v>76</v>
+        <f>IF(ISBLANK(H16),-F16,H16-F16)</f>
+        <v>44</v>
       </c>
       <c r="H16" s="1">
-        <v>9936</v>
+        <v>3803</v>
       </c>
       <c r="I16">
-        <f t="shared" si="2"/>
-        <v>54</v>
+        <f>IF(ISBLANK(J16),-H16,J16-H16)</f>
+        <v>116</v>
       </c>
       <c r="J16" s="1">
-        <v>9990</v>
+        <v>3919</v>
       </c>
       <c r="K16">
-        <f t="shared" si="3"/>
-        <v>184</v>
+        <f>IF(ISBLANK(L16),-J16,L16-J16)</f>
+        <v>87</v>
       </c>
       <c r="L16" s="1">
-        <v>10174</v>
+        <v>4006</v>
       </c>
       <c r="M16">
-        <f t="shared" si="4"/>
-        <v>52</v>
+        <f>IF(ISBLANK(N16),-L16,N16-L16)</f>
+        <v>41</v>
       </c>
       <c r="N16" s="1">
-        <v>10226</v>
+        <v>4047</v>
       </c>
       <c r="O16">
-        <f t="shared" si="5"/>
-        <v>168</v>
+        <f>IF(ISBLANK(P16),-N16,P16-N16)</f>
+        <v>134</v>
       </c>
       <c r="P16" s="1">
-        <v>10394</v>
+        <v>4181</v>
       </c>
       <c r="Q16">
-        <f t="shared" si="6"/>
-        <v>214</v>
+        <f>IF(ISBLANK(R16),-P16,R16-P16)</f>
+        <v>-4181</v>
       </c>
       <c r="R16" s="1">
-        <v>10608</v>
+        <v>0</v>
       </c>
       <c r="S16">
-        <f t="shared" si="7"/>
-        <v>48</v>
+        <f>IF(ISBLANK(T16),-R16,T16-R16)</f>
+        <v>0</v>
       </c>
       <c r="T16" s="1">
-        <v>10656</v>
+        <v>0</v>
       </c>
       <c r="U16">
-        <f t="shared" si="8"/>
-        <v>286</v>
+        <f>IF(ISBLANK(V16),-T16,V16-T16)</f>
+        <v>0</v>
       </c>
       <c r="V16" s="1">
-        <v>10942</v>
+        <v>0</v>
       </c>
       <c r="W16">
-        <f t="shared" si="9"/>
-        <v>208</v>
+        <f>IF(ISBLANK(X16),-V16,X16-V16)</f>
+        <v>0</v>
       </c>
       <c r="X16" s="1">
-        <v>11150</v>
+        <v>0</v>
       </c>
       <c r="Y16">
-        <f t="shared" si="10"/>
-        <v>-11150</v>
+        <f>IF(ISBLANK(Z16),-X16,Z16-X16)</f>
+        <v>0</v>
       </c>
       <c r="Z16" s="1">
         <v>0</v>
       </c>
       <c r="AA16">
-        <f t="shared" si="11"/>
+        <f>IF(ISBLANK(AB16),-Z16,AB16-Z16)</f>
         <v>0</v>
       </c>
       <c r="AB16" s="1">
         <v>0</v>
       </c>
       <c r="AC16">
-        <f t="shared" si="12"/>
+        <f>IF(ISBLANK(AD16),-AB16,AD16-AB16)</f>
         <v>0</v>
       </c>
       <c r="AD16" s="1">
         <v>0</v>
       </c>
       <c r="AE16">
-        <f t="shared" si="13"/>
+        <f>IF(ISBLANK(AF16),-AD16,AF16-AD16)</f>
         <v>0</v>
       </c>
       <c r="AF16" s="1">
         <v>0</v>
       </c>
       <c r="AG16">
-        <f t="shared" si="14"/>
+        <f>IF(ISBLANK(AH16),-AF16,AH16-AF16)</f>
         <v>0</v>
       </c>
       <c r="AH16" s="1">
         <v>0</v>
       </c>
       <c r="AI16">
-        <f t="shared" si="15"/>
+        <f>IF(ISBLANK(AJ16),-AH16,AJ16-AH16)</f>
         <v>0</v>
       </c>
       <c r="AJ16" s="1">
@@ -9787,248 +9790,248 @@
     </row>
     <row r="17" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="B17" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="D17" s="1">
-        <v>3682</v>
+        <v>75946</v>
       </c>
       <c r="E17">
-        <f t="shared" si="0"/>
-        <v>77</v>
+        <f>IF(ISBLANK(F17),-D17,F17-D17)</f>
+        <v>100</v>
       </c>
       <c r="F17" s="1">
-        <v>3759</v>
+        <v>76046</v>
       </c>
       <c r="G17">
-        <f t="shared" si="1"/>
-        <v>44</v>
+        <f>IF(ISBLANK(H17),-F17,H17-F17)</f>
+        <v>201</v>
       </c>
       <c r="H17" s="1">
-        <v>3803</v>
+        <v>76247</v>
       </c>
       <c r="I17">
-        <f t="shared" si="2"/>
-        <v>116</v>
+        <f>IF(ISBLANK(J17),-H17,J17-H17)</f>
+        <v>126</v>
       </c>
       <c r="J17" s="1">
-        <v>3919</v>
+        <v>76373</v>
       </c>
       <c r="K17">
-        <f t="shared" si="3"/>
-        <v>87</v>
+        <f>IF(ISBLANK(L17),-J17,L17-J17)</f>
+        <v>272</v>
       </c>
       <c r="L17" s="1">
-        <v>4006</v>
+        <v>76645</v>
       </c>
       <c r="M17">
-        <f t="shared" si="4"/>
-        <v>41</v>
+        <f>IF(ISBLANK(N17),-L17,N17-L17)</f>
+        <v>74</v>
       </c>
       <c r="N17" s="1">
-        <v>4047</v>
+        <v>76719</v>
       </c>
       <c r="O17">
-        <f t="shared" si="5"/>
-        <v>134</v>
+        <f>IF(ISBLANK(P17),-N17,P17-N17)</f>
+        <v>301</v>
       </c>
       <c r="P17" s="1">
-        <v>4181</v>
+        <v>77020</v>
       </c>
       <c r="Q17">
-        <f t="shared" si="6"/>
-        <v>-4181</v>
+        <f>IF(ISBLANK(R17),-P17,R17-P17)</f>
+        <v>283</v>
       </c>
       <c r="R17" s="1">
-        <v>0</v>
+        <v>77303</v>
       </c>
       <c r="S17">
-        <f t="shared" si="7"/>
-        <v>0</v>
+        <f>IF(ISBLANK(T17),-R17,T17-R17)</f>
+        <v>112</v>
       </c>
       <c r="T17" s="1">
-        <v>0</v>
+        <v>77415</v>
       </c>
       <c r="U17">
-        <f t="shared" si="8"/>
-        <v>0</v>
+        <f>IF(ISBLANK(V17),-T17,V17-T17)</f>
+        <v>339</v>
       </c>
       <c r="V17" s="1">
-        <v>0</v>
+        <v>77754</v>
       </c>
       <c r="W17">
-        <f t="shared" si="9"/>
-        <v>0</v>
+        <f>IF(ISBLANK(X17),-V17,X17-V17)</f>
+        <v>1066</v>
       </c>
       <c r="X17" s="1">
-        <v>0</v>
+        <v>78820</v>
       </c>
       <c r="Y17">
-        <f t="shared" si="10"/>
-        <v>0</v>
+        <f>IF(ISBLANK(Z17),-X17,Z17-X17)</f>
+        <v>1295</v>
       </c>
       <c r="Z17" s="1">
-        <v>0</v>
+        <v>80115</v>
       </c>
       <c r="AA17">
-        <f t="shared" si="11"/>
-        <v>0</v>
+        <f>IF(ISBLANK(AB17),-Z17,AB17-Z17)</f>
+        <v>593</v>
       </c>
       <c r="AB17" s="1">
-        <v>0</v>
+        <v>80708</v>
       </c>
       <c r="AC17">
-        <f t="shared" si="12"/>
-        <v>0</v>
+        <f>IF(ISBLANK(AD17),-AB17,AD17-AB17)</f>
+        <v>1290</v>
       </c>
       <c r="AD17" s="1">
-        <v>0</v>
+        <v>81998</v>
       </c>
       <c r="AE17">
-        <f t="shared" si="13"/>
-        <v>0</v>
+        <f>IF(ISBLANK(AF17),-AD17,AF17-AD17)</f>
+        <v>2743</v>
       </c>
       <c r="AF17" s="1">
-        <v>0</v>
+        <v>84741</v>
       </c>
       <c r="AG17">
-        <f t="shared" si="14"/>
-        <v>0</v>
+        <f>IF(ISBLANK(AH17),-AF17,AH17-AF17)</f>
+        <v>8382</v>
       </c>
       <c r="AH17" s="1">
-        <v>0</v>
+        <v>93123</v>
       </c>
       <c r="AI17">
-        <f t="shared" si="15"/>
-        <v>0</v>
+        <f>IF(ISBLANK(AJ17),-AH17,AJ17-AH17)</f>
+        <v>2972</v>
       </c>
       <c r="AJ17" s="1">
-        <v>0</v>
+        <v>96095</v>
       </c>
     </row>
     <row r="18" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B18" t="s">
-        <v>128</v>
+        <v>262</v>
       </c>
       <c r="D18" s="1">
-        <v>75946</v>
+        <v>79072</v>
       </c>
       <c r="E18">
-        <f t="shared" si="0"/>
-        <v>100</v>
+        <f>IF(ISBLANK(F18),-D18,F18-D18)</f>
+        <v>68</v>
       </c>
       <c r="F18" s="1">
-        <v>76046</v>
+        <v>79140</v>
       </c>
       <c r="G18">
-        <f t="shared" si="1"/>
-        <v>201</v>
+        <f>IF(ISBLANK(H18),-F18,H18-F18)</f>
+        <v>142</v>
       </c>
       <c r="H18" s="1">
-        <v>76247</v>
+        <v>79282</v>
       </c>
       <c r="I18">
-        <f t="shared" si="2"/>
-        <v>126</v>
+        <f>IF(ISBLANK(J18),-H18,J18-H18)</f>
+        <v>105</v>
       </c>
       <c r="J18" s="1">
-        <v>76373</v>
+        <v>79387</v>
       </c>
       <c r="K18">
-        <f t="shared" si="3"/>
-        <v>272</v>
+        <f>IF(ISBLANK(L18),-J18,L18-J18)</f>
+        <v>186</v>
       </c>
       <c r="L18" s="1">
-        <v>76645</v>
+        <v>79573</v>
       </c>
       <c r="M18">
-        <f t="shared" si="4"/>
-        <v>74</v>
+        <f>IF(ISBLANK(N18),-L18,N18-L18)</f>
+        <v>168</v>
       </c>
       <c r="N18" s="1">
-        <v>76719</v>
+        <v>79741</v>
       </c>
       <c r="O18">
-        <f t="shared" si="5"/>
-        <v>301</v>
+        <f>IF(ISBLANK(P18),-N18,P18-N18)</f>
+        <v>204</v>
       </c>
       <c r="P18" s="1">
-        <v>77020</v>
+        <v>79945</v>
       </c>
       <c r="Q18">
-        <f t="shared" si="6"/>
-        <v>283</v>
+        <f>IF(ISBLANK(R18),-P18,R18-P18)</f>
+        <v>305</v>
       </c>
       <c r="R18" s="1">
-        <v>77303</v>
+        <v>80250</v>
       </c>
       <c r="S18">
-        <f t="shared" si="7"/>
-        <v>112</v>
+        <f>IF(ISBLANK(T18),-R18,T18-R18)</f>
+        <v>127</v>
       </c>
       <c r="T18" s="1">
-        <v>77415</v>
+        <v>80377</v>
       </c>
       <c r="U18">
-        <f t="shared" si="8"/>
-        <v>339</v>
+        <f>IF(ISBLANK(V18),-T18,V18-T18)</f>
+        <v>446</v>
       </c>
       <c r="V18" s="1">
-        <v>77754</v>
+        <v>80823</v>
       </c>
       <c r="W18">
-        <f t="shared" si="9"/>
-        <v>1066</v>
+        <f>IF(ISBLANK(X18),-V18,X18-V18)</f>
+        <v>991</v>
       </c>
       <c r="X18" s="1">
-        <v>78820</v>
+        <v>81814</v>
       </c>
       <c r="Y18">
-        <f t="shared" si="10"/>
-        <v>1295</v>
+        <f>IF(ISBLANK(Z18),-X18,Z18-X18)</f>
+        <v>1119</v>
       </c>
       <c r="Z18" s="1">
-        <v>80115</v>
+        <v>82933</v>
       </c>
       <c r="AA18">
-        <f t="shared" si="11"/>
-        <v>593</v>
+        <f>IF(ISBLANK(AB18),-Z18,AB18-Z18)</f>
+        <v>958</v>
       </c>
       <c r="AB18" s="1">
-        <v>80708</v>
+        <v>83891</v>
       </c>
       <c r="AC18">
-        <f t="shared" si="12"/>
-        <v>1290</v>
+        <f>IF(ISBLANK(AD18),-AB18,AD18-AB18)</f>
+        <v>1108</v>
       </c>
       <c r="AD18" s="1">
-        <v>81998</v>
+        <v>84999</v>
       </c>
       <c r="AE18">
-        <f t="shared" si="13"/>
-        <v>2743</v>
+        <f>IF(ISBLANK(AF18),-AD18,AF18-AD18)</f>
+        <v>2323</v>
       </c>
       <c r="AF18" s="1">
-        <v>84741</v>
+        <v>87322</v>
       </c>
       <c r="AG18">
-        <f t="shared" si="14"/>
-        <v>8382</v>
+        <f>IF(ISBLANK(AH18),-AF18,AH18-AF18)</f>
+        <v>4517</v>
       </c>
       <c r="AH18" s="1">
-        <v>93123</v>
+        <v>91839</v>
       </c>
       <c r="AI18">
-        <f t="shared" si="15"/>
-        <v>2972</v>
+        <f>IF(ISBLANK(AJ18),-AH18,AJ18-AH18)</f>
+        <v>3734</v>
       </c>
       <c r="AJ18" s="1">
-        <v>96095</v>
+        <v>95573</v>
       </c>
     </row>
     <row r="19" spans="1:36" x14ac:dyDescent="0.25">
@@ -10042,112 +10045,112 @@
         <v>2864</v>
       </c>
       <c r="E19">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F19),-D19,F19-D19)</f>
         <v>34</v>
       </c>
       <c r="F19" s="1">
         <v>2898</v>
       </c>
       <c r="G19">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H19),-F19,H19-F19)</f>
         <v>21</v>
       </c>
       <c r="H19" s="1">
         <v>2919</v>
       </c>
       <c r="I19">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J19),-H19,J19-H19)</f>
         <v>148</v>
       </c>
       <c r="J19" s="1">
         <v>3067</v>
       </c>
       <c r="K19">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L19),-J19,L19-J19)</f>
         <v>-3067</v>
       </c>
       <c r="L19" s="1">
         <v>0</v>
       </c>
       <c r="M19">
-        <f t="shared" si="4"/>
+        <f>IF(ISBLANK(N19),-L19,N19-L19)</f>
         <v>0</v>
       </c>
       <c r="N19" s="1">
         <v>0</v>
       </c>
       <c r="O19">
-        <f t="shared" si="5"/>
+        <f>IF(ISBLANK(P19),-N19,P19-N19)</f>
         <v>0</v>
       </c>
       <c r="P19" s="1">
         <v>0</v>
       </c>
       <c r="Q19">
-        <f t="shared" si="6"/>
+        <f>IF(ISBLANK(R19),-P19,R19-P19)</f>
         <v>0</v>
       </c>
       <c r="R19" s="1">
         <v>0</v>
       </c>
       <c r="S19">
-        <f t="shared" si="7"/>
+        <f>IF(ISBLANK(T19),-R19,T19-R19)</f>
         <v>0</v>
       </c>
       <c r="T19" s="1">
         <v>0</v>
       </c>
       <c r="U19">
-        <f t="shared" si="8"/>
+        <f>IF(ISBLANK(V19),-T19,V19-T19)</f>
         <v>0</v>
       </c>
       <c r="V19" s="1">
         <v>0</v>
       </c>
       <c r="W19">
-        <f t="shared" si="9"/>
+        <f>IF(ISBLANK(X19),-V19,X19-V19)</f>
         <v>0</v>
       </c>
       <c r="X19" s="1">
         <v>0</v>
       </c>
       <c r="Y19">
-        <f t="shared" si="10"/>
+        <f>IF(ISBLANK(Z19),-X19,Z19-X19)</f>
         <v>0</v>
       </c>
       <c r="Z19" s="1">
         <v>0</v>
       </c>
       <c r="AA19">
-        <f t="shared" si="11"/>
+        <f>IF(ISBLANK(AB19),-Z19,AB19-Z19)</f>
         <v>0</v>
       </c>
       <c r="AB19" s="1">
         <v>0</v>
       </c>
       <c r="AC19">
-        <f t="shared" si="12"/>
+        <f>IF(ISBLANK(AD19),-AB19,AD19-AB19)</f>
         <v>0</v>
       </c>
       <c r="AD19" s="1">
         <v>0</v>
       </c>
       <c r="AE19">
-        <f t="shared" si="13"/>
+        <f>IF(ISBLANK(AF19),-AD19,AF19-AD19)</f>
         <v>0</v>
       </c>
       <c r="AF19" s="1">
         <v>0</v>
       </c>
       <c r="AG19">
-        <f t="shared" si="14"/>
+        <f>IF(ISBLANK(AH19),-AF19,AH19-AF19)</f>
         <v>0</v>
       </c>
       <c r="AH19" s="1">
         <v>0</v>
       </c>
       <c r="AI19">
-        <f t="shared" si="15"/>
+        <f>IF(ISBLANK(AJ19),-AH19,AJ19-AH19)</f>
         <v>0</v>
       </c>
       <c r="AJ19" s="1">
@@ -10165,112 +10168,112 @@
         <v>2416</v>
       </c>
       <c r="E20">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F20),-D20,F20-D20)</f>
         <v>48</v>
       </c>
       <c r="F20" s="1">
         <v>2464</v>
       </c>
       <c r="G20">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H20),-F20,H20-F20)</f>
         <v>78</v>
       </c>
       <c r="H20" s="1">
         <v>2542</v>
       </c>
       <c r="I20">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J20),-H20,J20-H20)</f>
         <v>-2542</v>
       </c>
       <c r="J20" s="1">
         <v>0</v>
       </c>
       <c r="K20">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L20),-J20,L20-J20)</f>
         <v>0</v>
       </c>
       <c r="L20" s="1">
         <v>0</v>
       </c>
       <c r="M20">
-        <f t="shared" si="4"/>
+        <f>IF(ISBLANK(N20),-L20,N20-L20)</f>
         <v>0</v>
       </c>
       <c r="N20" s="1">
         <v>0</v>
       </c>
       <c r="O20">
-        <f t="shared" si="5"/>
+        <f>IF(ISBLANK(P20),-N20,P20-N20)</f>
         <v>0</v>
       </c>
       <c r="P20" s="1">
         <v>0</v>
       </c>
       <c r="Q20">
-        <f t="shared" si="6"/>
+        <f>IF(ISBLANK(R20),-P20,R20-P20)</f>
         <v>0</v>
       </c>
       <c r="R20" s="1">
         <v>0</v>
       </c>
       <c r="S20">
-        <f t="shared" si="7"/>
+        <f>IF(ISBLANK(T20),-R20,T20-R20)</f>
         <v>0</v>
       </c>
       <c r="T20" s="1">
         <v>0</v>
       </c>
       <c r="U20">
-        <f t="shared" si="8"/>
+        <f>IF(ISBLANK(V20),-T20,V20-T20)</f>
         <v>0</v>
       </c>
       <c r="V20" s="1">
         <v>0</v>
       </c>
       <c r="W20">
-        <f t="shared" si="9"/>
+        <f>IF(ISBLANK(X20),-V20,X20-V20)</f>
         <v>0</v>
       </c>
       <c r="X20" s="1">
         <v>0</v>
       </c>
       <c r="Y20">
-        <f t="shared" si="10"/>
+        <f>IF(ISBLANK(Z20),-X20,Z20-X20)</f>
         <v>0</v>
       </c>
       <c r="Z20" s="1">
         <v>0</v>
       </c>
       <c r="AA20">
-        <f t="shared" si="11"/>
+        <f>IF(ISBLANK(AB20),-Z20,AB20-Z20)</f>
         <v>0</v>
       </c>
       <c r="AB20" s="1">
         <v>0</v>
       </c>
       <c r="AC20">
-        <f t="shared" si="12"/>
+        <f>IF(ISBLANK(AD20),-AB20,AD20-AB20)</f>
         <v>0</v>
       </c>
       <c r="AD20" s="1">
         <v>0</v>
       </c>
       <c r="AE20">
-        <f t="shared" si="13"/>
+        <f>IF(ISBLANK(AF20),-AD20,AF20-AD20)</f>
         <v>0</v>
       </c>
       <c r="AF20" s="1">
         <v>0</v>
       </c>
       <c r="AG20">
-        <f t="shared" si="14"/>
+        <f>IF(ISBLANK(AH20),-AF20,AH20-AF20)</f>
         <v>0</v>
       </c>
       <c r="AH20" s="1">
         <v>0</v>
       </c>
       <c r="AI20">
-        <f t="shared" si="15"/>
+        <f>IF(ISBLANK(AJ20),-AH20,AJ20-AH20)</f>
         <v>0</v>
       </c>
       <c r="AJ20" s="1">
@@ -10288,112 +10291,112 @@
         <v>1423</v>
       </c>
       <c r="E21">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F21),-D21,F21-D21)</f>
         <v>-1423</v>
       </c>
       <c r="F21" s="1">
         <v>0</v>
       </c>
       <c r="G21">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H21),-F21,H21-F21)</f>
         <v>0</v>
       </c>
       <c r="H21" s="1">
         <v>0</v>
       </c>
       <c r="I21">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J21),-H21,J21-H21)</f>
         <v>0</v>
       </c>
       <c r="J21" s="1">
         <v>0</v>
       </c>
       <c r="K21">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L21),-J21,L21-J21)</f>
         <v>0</v>
       </c>
       <c r="L21" s="1">
         <v>0</v>
       </c>
       <c r="M21">
-        <f t="shared" si="4"/>
+        <f>IF(ISBLANK(N21),-L21,N21-L21)</f>
         <v>0</v>
       </c>
       <c r="N21" s="1">
         <v>0</v>
       </c>
       <c r="O21">
-        <f t="shared" si="5"/>
+        <f>IF(ISBLANK(P21),-N21,P21-N21)</f>
         <v>0</v>
       </c>
       <c r="P21" s="1">
         <v>0</v>
       </c>
       <c r="Q21">
-        <f t="shared" si="6"/>
+        <f>IF(ISBLANK(R21),-P21,R21-P21)</f>
         <v>0</v>
       </c>
       <c r="R21" s="1">
         <v>0</v>
       </c>
       <c r="S21">
-        <f t="shared" si="7"/>
+        <f>IF(ISBLANK(T21),-R21,T21-R21)</f>
         <v>0</v>
       </c>
       <c r="T21" s="1">
         <v>0</v>
       </c>
       <c r="U21">
-        <f t="shared" si="8"/>
+        <f>IF(ISBLANK(V21),-T21,V21-T21)</f>
         <v>0</v>
       </c>
       <c r="V21" s="1">
         <v>0</v>
       </c>
       <c r="W21">
-        <f t="shared" si="9"/>
+        <f>IF(ISBLANK(X21),-V21,X21-V21)</f>
         <v>0</v>
       </c>
       <c r="X21" s="1">
         <v>0</v>
       </c>
       <c r="Y21">
-        <f t="shared" si="10"/>
+        <f>IF(ISBLANK(Z21),-X21,Z21-X21)</f>
         <v>0</v>
       </c>
       <c r="Z21" s="1">
         <v>0</v>
       </c>
       <c r="AA21">
-        <f t="shared" si="11"/>
+        <f>IF(ISBLANK(AB21),-Z21,AB21-Z21)</f>
         <v>0</v>
       </c>
       <c r="AB21" s="1">
         <v>0</v>
       </c>
       <c r="AC21">
-        <f t="shared" si="12"/>
+        <f>IF(ISBLANK(AD21),-AB21,AD21-AB21)</f>
         <v>0</v>
       </c>
       <c r="AD21" s="1">
         <v>0</v>
       </c>
       <c r="AE21">
-        <f t="shared" si="13"/>
+        <f>IF(ISBLANK(AF21),-AD21,AF21-AD21)</f>
         <v>0</v>
       </c>
       <c r="AF21" s="1">
         <v>0</v>
       </c>
       <c r="AG21">
-        <f t="shared" si="14"/>
+        <f>IF(ISBLANK(AH21),-AF21,AH21-AF21)</f>
         <v>0</v>
       </c>
       <c r="AH21" s="1">
         <v>0</v>
       </c>
       <c r="AI21">
-        <f t="shared" si="15"/>
+        <f>IF(ISBLANK(AJ21),-AH21,AJ21-AH21)</f>
         <v>0</v>
       </c>
       <c r="AJ21" s="1">
@@ -10411,112 +10414,112 @@
         <v>14802</v>
       </c>
       <c r="E22">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F22),-D22,F22-D22)</f>
         <v>156</v>
       </c>
       <c r="F22" s="1">
         <v>14958</v>
       </c>
       <c r="G22">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H22),-F22,H22-F22)</f>
         <v>51</v>
       </c>
       <c r="H22" s="1">
         <v>15009</v>
       </c>
       <c r="I22">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J22),-H22,J22-H22)</f>
         <v>198</v>
       </c>
       <c r="J22" s="1">
         <v>15207</v>
       </c>
       <c r="K22">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L22),-J22,L22-J22)</f>
         <v>146</v>
       </c>
       <c r="L22" s="1">
         <v>15353</v>
       </c>
       <c r="M22">
-        <f t="shared" si="4"/>
+        <f>IF(ISBLANK(N22),-L22,N22-L22)</f>
         <v>41</v>
       </c>
       <c r="N22" s="1">
         <v>15394</v>
       </c>
       <c r="O22">
-        <f t="shared" si="5"/>
+        <f>IF(ISBLANK(P22),-N22,P22-N22)</f>
         <v>392</v>
       </c>
       <c r="P22" s="1">
         <v>15786</v>
       </c>
       <c r="Q22">
-        <f t="shared" si="6"/>
+        <f>IF(ISBLANK(R22),-P22,R22-P22)</f>
         <v>321</v>
       </c>
       <c r="R22" s="1">
         <v>16107</v>
       </c>
       <c r="S22">
-        <f t="shared" si="7"/>
+        <f>IF(ISBLANK(T22),-R22,T22-R22)</f>
         <v>101</v>
       </c>
       <c r="T22" s="1">
         <v>16208</v>
       </c>
       <c r="U22">
-        <f t="shared" si="8"/>
+        <f>IF(ISBLANK(V22),-T22,V22-T22)</f>
         <v>170</v>
       </c>
       <c r="V22" s="1">
         <v>16378</v>
       </c>
       <c r="W22">
-        <f t="shared" si="9"/>
+        <f>IF(ISBLANK(X22),-V22,X22-V22)</f>
         <v>530</v>
       </c>
       <c r="X22" s="1">
         <v>16908</v>
       </c>
       <c r="Y22">
-        <f t="shared" si="10"/>
+        <f>IF(ISBLANK(Z22),-X22,Z22-X22)</f>
         <v>490</v>
       </c>
       <c r="Z22" s="1">
         <v>17398</v>
       </c>
       <c r="AA22">
-        <f t="shared" si="11"/>
+        <f>IF(ISBLANK(AB22),-Z22,AB22-Z22)</f>
         <v>329</v>
       </c>
       <c r="AB22" s="1">
         <v>17727</v>
       </c>
       <c r="AC22">
-        <f t="shared" si="12"/>
+        <f>IF(ISBLANK(AD22),-AB22,AD22-AB22)</f>
         <v>749</v>
       </c>
       <c r="AD22" s="1">
         <v>18476</v>
       </c>
       <c r="AE22">
-        <f t="shared" si="13"/>
+        <f>IF(ISBLANK(AF22),-AD22,AF22-AD22)</f>
         <v>-18476</v>
       </c>
       <c r="AF22" s="1">
         <v>0</v>
       </c>
       <c r="AG22">
-        <f t="shared" si="14"/>
+        <f>IF(ISBLANK(AH22),-AF22,AH22-AF22)</f>
         <v>0</v>
       </c>
       <c r="AH22" s="1">
         <v>0</v>
       </c>
       <c r="AI22">
-        <f t="shared" si="15"/>
+        <f>IF(ISBLANK(AJ22),-AH22,AJ22-AH22)</f>
         <v>0</v>
       </c>
       <c r="AJ22" s="1">
@@ -10534,112 +10537,112 @@
         <v>81741</v>
       </c>
       <c r="E23">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F23),-D23,F23-D23)</f>
         <v>253</v>
       </c>
       <c r="F23" s="1">
         <v>81994</v>
       </c>
       <c r="G23">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H23),-F23,H23-F23)</f>
         <v>130</v>
       </c>
       <c r="H23" s="1">
         <v>82124</v>
       </c>
       <c r="I23">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J23),-H23,J23-H23)</f>
         <v>211</v>
       </c>
       <c r="J23" s="1">
         <v>82335</v>
       </c>
       <c r="K23">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L23),-J23,L23-J23)</f>
         <v>323</v>
       </c>
       <c r="L23" s="1">
         <v>82658</v>
       </c>
       <c r="M23">
-        <f t="shared" si="4"/>
+        <f>IF(ISBLANK(N23),-L23,N23-L23)</f>
         <v>206</v>
       </c>
       <c r="N23" s="1">
         <v>82864</v>
       </c>
       <c r="O23">
-        <f t="shared" si="5"/>
+        <f>IF(ISBLANK(P23),-N23,P23-N23)</f>
         <v>556</v>
       </c>
       <c r="P23" s="1">
         <v>83420</v>
       </c>
       <c r="Q23">
-        <f t="shared" si="6"/>
+        <f>IF(ISBLANK(R23),-P23,R23-P23)</f>
         <v>351</v>
       </c>
       <c r="R23" s="1">
         <v>83771</v>
       </c>
       <c r="S23">
-        <f t="shared" si="7"/>
+        <f>IF(ISBLANK(T23),-R23,T23-R23)</f>
         <v>217</v>
       </c>
       <c r="T23" s="1">
         <v>83988</v>
       </c>
       <c r="U23">
-        <f t="shared" si="8"/>
+        <f>IF(ISBLANK(V23),-T23,V23-T23)</f>
         <v>247</v>
       </c>
       <c r="V23" s="1">
         <v>84235</v>
       </c>
       <c r="W23">
-        <f t="shared" si="9"/>
+        <f>IF(ISBLANK(X23),-V23,X23-V23)</f>
         <v>1001</v>
       </c>
       <c r="X23" s="1">
         <v>85236</v>
       </c>
       <c r="Y23">
-        <f t="shared" si="10"/>
+        <f>IF(ISBLANK(Z23),-X23,Z23-X23)</f>
         <v>2333</v>
       </c>
       <c r="Z23" s="1">
         <v>87569</v>
       </c>
       <c r="AA23">
-        <f t="shared" si="11"/>
+        <f>IF(ISBLANK(AB23),-Z23,AB23-Z23)</f>
         <v>1190</v>
       </c>
       <c r="AB23" s="1">
         <v>88759</v>
       </c>
       <c r="AC23">
-        <f t="shared" si="12"/>
+        <f>IF(ISBLANK(AD23),-AB23,AD23-AB23)</f>
         <v>1476</v>
       </c>
       <c r="AD23" s="1">
         <v>90235</v>
       </c>
       <c r="AE23">
-        <f t="shared" si="13"/>
+        <f>IF(ISBLANK(AF23),-AD23,AF23-AD23)</f>
         <v>5545</v>
       </c>
       <c r="AF23" s="1">
         <v>95780</v>
       </c>
       <c r="AG23">
-        <f t="shared" si="14"/>
+        <f>IF(ISBLANK(AH23),-AF23,AH23-AF23)</f>
         <v>5945</v>
       </c>
       <c r="AH23" s="1">
         <v>101725</v>
       </c>
       <c r="AI23">
-        <f t="shared" si="15"/>
+        <f>IF(ISBLANK(AJ23),-AH23,AJ23-AH23)</f>
         <v>7424</v>
       </c>
       <c r="AJ23" s="1">
@@ -10657,112 +10660,112 @@
         <v>3286</v>
       </c>
       <c r="E24">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(F24),-D24,F24-D24)</f>
         <v>21</v>
       </c>
       <c r="F24" s="1">
         <v>3307</v>
       </c>
       <c r="G24">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(H24),-F24,H24-F24)</f>
         <v>13</v>
       </c>
       <c r="H24" s="1">
         <v>3320</v>
       </c>
       <c r="I24">
-        <f t="shared" si="2"/>
+        <f>IF(ISBLANK(J24),-H24,J24-H24)</f>
         <v>232</v>
       </c>
       <c r="J24" s="1">
         <v>3552</v>
       </c>
       <c r="K24">
-        <f t="shared" si="3"/>
+        <f>IF(ISBLANK(L24),-J24,L24-J24)</f>
         <v>102</v>
       </c>
       <c r="L24" s="1">
         <v>3654</v>
       </c>
       <c r="M24">
-        <f t="shared" si="4"/>
+        <f>IF(ISBLANK(N24),-L24,N24-L24)</f>
         <v>60</v>
       </c>
       <c r="N24" s="1">
         <v>3714</v>
       </c>
       <c r="O24">
-        <f t="shared" si="5"/>
+        <f>IF(ISBLANK(P24),-N24,P24-N24)</f>
         <v>-3714</v>
       </c>
       <c r="P24" s="1">
         <v>0</v>
       </c>
       <c r="Q24">
-        <f t="shared" si="6"/>
+        <f>IF(ISBLANK(R24),-P24,R24-P24)</f>
         <v>0</v>
       </c>
       <c r="R24" s="1">
         <v>0</v>
       </c>
       <c r="S24">
-        <f t="shared" si="7"/>
+        <f>IF(ISBLANK(T24),-R24,T24-R24)</f>
         <v>0</v>
       </c>
       <c r="T24" s="1">
         <v>0</v>
       </c>
       <c r="U24">
-        <f t="shared" si="8"/>
+        <f>IF(ISBLANK(V24),-T24,V24-T24)</f>
         <v>0</v>
       </c>
       <c r="V24" s="1">
         <v>0</v>
       </c>
       <c r="W24">
-        <f t="shared" si="9"/>
+        <f>IF(ISBLANK(X24),-V24,X24-V24)</f>
         <v>0</v>
       </c>
       <c r="X24" s="1">
         <v>0</v>
       </c>
       <c r="Y24">
-        <f t="shared" si="10"/>
+        <f>IF(ISBLANK(Z24),-X24,Z24-X24)</f>
         <v>0</v>
       </c>
       <c r="Z24" s="1">
         <v>0</v>
       </c>
       <c r="AA24">
-        <f t="shared" si="11"/>
+        <f>IF(ISBLANK(AB24),-Z24,AB24-Z24)</f>
         <v>0</v>
       </c>
       <c r="AB24" s="1">
         <v>0</v>
       </c>
       <c r="AC24">
-        <f t="shared" si="12"/>
+        <f>IF(ISBLANK(AD24),-AB24,AD24-AB24)</f>
         <v>0</v>
       </c>
       <c r="AD24" s="1">
         <v>0</v>
       </c>
       <c r="AE24">
-        <f t="shared" si="13"/>
+        <f>IF(ISBLANK(AF24),-AD24,AF24-AD24)</f>
         <v>0</v>
       </c>
       <c r="AF24" s="1">
         <v>0</v>
       </c>
       <c r="AG24">
-        <f t="shared" si="14"/>
+        <f>IF(ISBLANK(AH24),-AF24,AH24-AF24)</f>
         <v>0</v>
       </c>
       <c r="AH24" s="1">
         <v>0</v>
       </c>
       <c r="AI24">
-        <f t="shared" si="15"/>
+        <f>IF(ISBLANK(AJ24),-AH24,AJ24-AH24)</f>
         <v>0</v>
       </c>
       <c r="AJ24" s="1">
@@ -10867,19 +10870,19 @@
         <v>148</v>
       </c>
       <c r="E27">
-        <f t="shared" ref="E27:E48" si="16">FIND(",",B27)</f>
+        <f t="shared" ref="E27:E48" si="0">FIND(",",B27)</f>
         <v>9</v>
       </c>
       <c r="F27" t="str">
-        <f t="shared" ref="F27:F48" si="17">LEFT(B27,E27-1)</f>
+        <f t="shared" ref="F27:F48" si="1">LEFT(B27,E27-1)</f>
         <v>Kelleher</v>
       </c>
       <c r="G27" t="str">
-        <f t="shared" ref="G27:G48" si="18">RIGHT(B27,LEN(B27)-(E27+1))</f>
+        <f t="shared" ref="G27:G48" si="2">RIGHT(B27,LEN(B27)-(E27+1))</f>
         <v>Billy</v>
       </c>
       <c r="H27" t="str">
-        <f t="shared" ref="H27:H48" si="19">G27&amp;" "&amp;F27</f>
+        <f t="shared" ref="H27:H48" si="3">G27&amp;" "&amp;F27</f>
         <v>Billy Kelleher</v>
       </c>
       <c r="J27" t="s">
@@ -10930,19 +10933,19 @@
         <v>149</v>
       </c>
       <c r="E28">
-        <f t="shared" si="16"/>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="F28" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="1"/>
         <v>Wallace</v>
       </c>
       <c r="G28" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="2"/>
         <v>Mick</v>
       </c>
       <c r="H28" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="3"/>
         <v>Mick Wallace</v>
       </c>
       <c r="J28" t="s">
@@ -11020,19 +11023,19 @@
         <v>150</v>
       </c>
       <c r="E29">
-        <f t="shared" si="16"/>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="F29" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="1"/>
         <v>Ní Riada</v>
       </c>
       <c r="G29" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="2"/>
         <v>Liadh</v>
       </c>
       <c r="H29" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="3"/>
         <v>Liadh Ní Riada</v>
       </c>
       <c r="J29" t="s">
@@ -11110,19 +11113,19 @@
         <v>151</v>
       </c>
       <c r="E30">
-        <f t="shared" si="16"/>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="F30" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="1"/>
         <v>O'Sullivan</v>
       </c>
       <c r="G30" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="2"/>
         <v>Grace</v>
       </c>
       <c r="H30" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="3"/>
         <v>Grace O'Sullivan</v>
       </c>
       <c r="J30" t="s">
@@ -11200,19 +11203,19 @@
         <v>152</v>
       </c>
       <c r="E31">
-        <f t="shared" si="16"/>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="F31" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="1"/>
         <v>Byrne</v>
       </c>
       <c r="G31" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="2"/>
         <v>Malcolm</v>
       </c>
       <c r="H31" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="3"/>
         <v>Malcolm Byrne</v>
       </c>
       <c r="J31" t="s">
@@ -11290,19 +11293,19 @@
         <v>153</v>
       </c>
       <c r="E32">
-        <f t="shared" si="16"/>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="F32" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="1"/>
         <v>Clune</v>
       </c>
       <c r="G32" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="2"/>
         <v>Deirdre</v>
       </c>
       <c r="H32" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="3"/>
         <v>Deirdre Clune</v>
       </c>
       <c r="J32" t="s">
@@ -11377,19 +11380,19 @@
         <v>154</v>
       </c>
       <c r="E33">
-        <f t="shared" si="16"/>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="F33" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="1"/>
         <v>Doyle</v>
       </c>
       <c r="G33" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="2"/>
         <v>Andrew</v>
       </c>
       <c r="H33" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="3"/>
         <v>Andrew Doyle</v>
       </c>
       <c r="J33" t="s">
@@ -11467,19 +11470,19 @@
         <v>155</v>
       </c>
       <c r="E34">
-        <f t="shared" si="16"/>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="F34" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="1"/>
         <v>Nunan</v>
       </c>
       <c r="G34" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="2"/>
         <v>Sheila</v>
       </c>
       <c r="H34" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="3"/>
         <v>Sheila Nunan</v>
       </c>
       <c r="J34" t="s">
@@ -11551,19 +11554,19 @@
         <v>156</v>
       </c>
       <c r="E35">
-        <f t="shared" si="16"/>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="F35" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="1"/>
         <v>Wallace</v>
       </c>
       <c r="G35" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="2"/>
         <v>Adrienne</v>
       </c>
       <c r="H35" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="3"/>
         <v>Adrienne Wallace</v>
       </c>
       <c r="J35" t="s">
@@ -11632,19 +11635,19 @@
         <v>157</v>
       </c>
       <c r="E36">
-        <f t="shared" si="16"/>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="F36" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="1"/>
         <v>Cahill</v>
       </c>
       <c r="G36" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="2"/>
         <v>Dolores</v>
       </c>
       <c r="H36" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="3"/>
         <v>Dolores Cahill</v>
       </c>
       <c r="J36" t="s">
@@ -11713,19 +11716,19 @@
         <v>158</v>
       </c>
       <c r="E37">
-        <f t="shared" si="16"/>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="F37" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="1"/>
         <v>O'Flynn</v>
       </c>
       <c r="G37" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="2"/>
         <v>Diarmuid Patrick</v>
       </c>
       <c r="H37" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="3"/>
         <v>Diarmuid Patrick O'Flynn</v>
       </c>
       <c r="J37" t="s">
@@ -11791,19 +11794,19 @@
         <v>159</v>
       </c>
       <c r="E38">
-        <f t="shared" si="16"/>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="F38" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="1"/>
         <v>Minehan</v>
       </c>
       <c r="G38" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="2"/>
         <v>Liam</v>
       </c>
       <c r="H38" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="3"/>
         <v>Liam Minehan</v>
       </c>
       <c r="J38" t="s">
@@ -11863,19 +11866,19 @@
         <v>160</v>
       </c>
       <c r="E39">
-        <f t="shared" si="16"/>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="F39" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="1"/>
         <v>Gardner</v>
       </c>
       <c r="G39" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="2"/>
         <v>Breda Patricia</v>
       </c>
       <c r="H39" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="3"/>
         <v>Breda Patricia Gardner</v>
       </c>
       <c r="J39" t="s">
@@ -11938,19 +11941,19 @@
         <v>161</v>
       </c>
       <c r="E40">
-        <f t="shared" si="16"/>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="F40" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="1"/>
         <v>Heaney</v>
       </c>
       <c r="G40" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="2"/>
         <v>Theresa</v>
       </c>
       <c r="H40" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="3"/>
         <v>Theresa Heaney</v>
       </c>
       <c r="J40" t="s">
@@ -12011,19 +12014,19 @@
         <v>162</v>
       </c>
       <c r="E41">
-        <f t="shared" si="16"/>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="F41" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="1"/>
         <v>Brennan</v>
       </c>
       <c r="G41" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="2"/>
         <v>Allan</v>
       </c>
       <c r="H41" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="3"/>
         <v>Allan Brennan</v>
       </c>
       <c r="J41" t="s">
@@ -12081,19 +12084,19 @@
         <v>163</v>
       </c>
       <c r="E42">
-        <f t="shared" si="16"/>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="F42" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="1"/>
         <v>O'Loughlin</v>
       </c>
       <c r="G42" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="2"/>
         <v>Peter</v>
       </c>
       <c r="H42" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="3"/>
         <v>Peter O'Loughlin</v>
       </c>
       <c r="J42" t="s">
@@ -12147,19 +12150,19 @@
         <v>164</v>
       </c>
       <c r="E43">
-        <f t="shared" si="16"/>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="F43" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="1"/>
         <v>Worthington</v>
       </c>
       <c r="G43" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="2"/>
         <v>Colleen</v>
       </c>
       <c r="H43" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="3"/>
         <v>Colleen Worthington</v>
       </c>
       <c r="J43" t="s">
@@ -12209,19 +12212,19 @@
         <v>165</v>
       </c>
       <c r="E44">
-        <f t="shared" si="16"/>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="F44" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="1"/>
         <v>Fitzgerald</v>
       </c>
       <c r="G44" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="2"/>
         <v>Paddy</v>
       </c>
       <c r="H44" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="3"/>
         <v>Paddy Fitzgerald</v>
       </c>
       <c r="J44" t="s">
@@ -12267,19 +12270,19 @@
         <v>166</v>
       </c>
       <c r="E45">
-        <f t="shared" si="16"/>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="F45" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="1"/>
         <v>Ryan-Purcell</v>
       </c>
       <c r="G45" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="2"/>
         <v>Walter</v>
       </c>
       <c r="H45" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="3"/>
         <v>Walter Ryan-Purcell</v>
       </c>
       <c r="J45" t="s">
@@ -12321,19 +12324,19 @@
         <v>167</v>
       </c>
       <c r="E46">
-        <f t="shared" si="16"/>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="F46" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="1"/>
         <v>Sexton</v>
       </c>
       <c r="G46" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="2"/>
         <v>Joesph</v>
       </c>
       <c r="H46" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="3"/>
         <v>Joesph Sexton</v>
       </c>
       <c r="J46" t="s">
@@ -12367,19 +12370,19 @@
         <v>168</v>
       </c>
       <c r="E47">
-        <f t="shared" si="16"/>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="F47" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="1"/>
         <v>Madden</v>
       </c>
       <c r="G47" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="2"/>
         <v>Peter</v>
       </c>
       <c r="H47" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="3"/>
         <v>Peter Madden</v>
       </c>
       <c r="J47" t="s">
@@ -12406,19 +12409,19 @@
         <v>169</v>
       </c>
       <c r="E48">
-        <f t="shared" si="16"/>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="F48" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="1"/>
         <v>Van de Ven</v>
       </c>
       <c r="G48" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="2"/>
         <v>Jan</v>
       </c>
       <c r="H48" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="3"/>
         <v>Jan Van de Ven</v>
       </c>
       <c r="J48" t="s">

</xml_diff>

<commit_message>
Stage 18 south added Signed-off-by: Gerry Mulvenna <git@movingwifi.com>
</commit_message>
<xml_diff>
--- a/europarl/europarl-ireland-2019.xlsx
+++ b/europarl/europarl-ireland-2019.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="264">
   <si>
     <t>Candidate</t>
   </si>
@@ -806,6 +806,9 @@
   </si>
   <si>
     <t>Riada, Liadh Ninot-elected</t>
+  </si>
+  <si>
+    <t>Count 18</t>
   </si>
 </sst>
 </file>
@@ -7842,10 +7845,10 @@
   <dimension ref="A1:AM49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="AG2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="AH2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D2" sqref="D2:AJ24"/>
+      <selection pane="bottomRight" activeCell="D2" sqref="D2:AL24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7912,6 +7915,9 @@
       <c r="AJ1" t="s">
         <v>261</v>
       </c>
+      <c r="AL1" t="s">
+        <v>263</v>
+      </c>
     </row>
     <row r="2" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A2">
@@ -7924,115 +7930,122 @@
         <v>4665</v>
       </c>
       <c r="E2">
-        <f>IF(ISBLANK(F2),-D2,F2-D2)</f>
+        <f t="shared" ref="E2:E24" si="0">IF(ISBLANK(F2),-D2,F2-D2)</f>
         <v>26</v>
       </c>
       <c r="F2" s="1">
         <v>4691</v>
       </c>
       <c r="G2">
-        <f>IF(ISBLANK(H2),-F2,H2-F2)</f>
+        <f t="shared" ref="G2:G24" si="1">IF(ISBLANK(H2),-F2,H2-F2)</f>
         <v>43</v>
       </c>
       <c r="H2" s="1">
         <v>4734</v>
       </c>
       <c r="I2">
-        <f>IF(ISBLANK(J2),-H2,J2-H2)</f>
+        <f t="shared" ref="I2:I24" si="2">IF(ISBLANK(J2),-H2,J2-H2)</f>
         <v>57</v>
       </c>
       <c r="J2" s="1">
         <v>4791</v>
       </c>
       <c r="K2">
-        <f>IF(ISBLANK(L2),-J2,L2-J2)</f>
+        <f t="shared" ref="K2:K24" si="3">IF(ISBLANK(L2),-J2,L2-J2)</f>
         <v>50</v>
       </c>
       <c r="L2" s="1">
         <v>4841</v>
       </c>
       <c r="M2">
-        <f>IF(ISBLANK(N2),-L2,N2-L2)</f>
+        <f t="shared" ref="M2:M24" si="4">IF(ISBLANK(N2),-L2,N2-L2)</f>
         <v>115</v>
       </c>
       <c r="N2" s="1">
         <v>4956</v>
       </c>
       <c r="O2">
-        <f>IF(ISBLANK(P2),-N2,P2-N2)</f>
+        <f t="shared" ref="O2:O24" si="5">IF(ISBLANK(P2),-N2,P2-N2)</f>
         <v>72</v>
       </c>
       <c r="P2" s="1">
         <v>5028</v>
       </c>
       <c r="Q2">
-        <f>IF(ISBLANK(R2),-P2,R2-P2)</f>
+        <f t="shared" ref="Q2:Q24" si="6">IF(ISBLANK(R2),-P2,R2-P2)</f>
         <v>104</v>
       </c>
       <c r="R2" s="1">
         <v>5132</v>
       </c>
       <c r="S2">
-        <f>IF(ISBLANK(T2),-R2,T2-R2)</f>
+        <f t="shared" ref="S2:S24" si="7">IF(ISBLANK(T2),-R2,T2-R2)</f>
         <v>-5132</v>
       </c>
       <c r="T2" s="1">
         <v>0</v>
       </c>
       <c r="U2">
-        <f>IF(ISBLANK(V2),-T2,V2-T2)</f>
+        <f t="shared" ref="U2:U24" si="8">IF(ISBLANK(V2),-T2,V2-T2)</f>
         <v>0</v>
       </c>
       <c r="V2" s="1">
         <v>0</v>
       </c>
       <c r="W2">
-        <f>IF(ISBLANK(X2),-V2,X2-V2)</f>
+        <f t="shared" ref="W2:W24" si="9">IF(ISBLANK(X2),-V2,X2-V2)</f>
         <v>0</v>
       </c>
       <c r="X2" s="1">
         <v>0</v>
       </c>
       <c r="Y2">
-        <f>IF(ISBLANK(Z2),-X2,Z2-X2)</f>
+        <f t="shared" ref="Y2:Y24" si="10">IF(ISBLANK(Z2),-X2,Z2-X2)</f>
         <v>0</v>
       </c>
       <c r="Z2" s="1">
         <v>0</v>
       </c>
       <c r="AA2">
-        <f>IF(ISBLANK(AB2),-Z2,AB2-Z2)</f>
+        <f t="shared" ref="AA2:AA24" si="11">IF(ISBLANK(AB2),-Z2,AB2-Z2)</f>
         <v>0</v>
       </c>
       <c r="AB2" s="1">
         <v>0</v>
       </c>
       <c r="AC2">
-        <f>IF(ISBLANK(AD2),-AB2,AD2-AB2)</f>
+        <f t="shared" ref="AC2:AC24" si="12">IF(ISBLANK(AD2),-AB2,AD2-AB2)</f>
         <v>0</v>
       </c>
       <c r="AD2" s="1">
         <v>0</v>
       </c>
       <c r="AE2">
-        <f>IF(ISBLANK(AF2),-AD2,AF2-AD2)</f>
+        <f t="shared" ref="AE2:AE24" si="13">IF(ISBLANK(AF2),-AD2,AF2-AD2)</f>
         <v>0</v>
       </c>
       <c r="AF2" s="1">
         <v>0</v>
       </c>
       <c r="AG2">
-        <f>IF(ISBLANK(AH2),-AF2,AH2-AF2)</f>
+        <f t="shared" ref="AG2:AG24" si="14">IF(ISBLANK(AH2),-AF2,AH2-AF2)</f>
         <v>0</v>
       </c>
       <c r="AH2" s="1">
         <v>0</v>
       </c>
       <c r="AI2">
-        <f>IF(ISBLANK(AJ2),-AH2,AJ2-AH2)</f>
+        <f t="shared" ref="AI2:AK24" si="15">IF(ISBLANK(AJ2),-AH2,AJ2-AH2)</f>
         <v>0</v>
       </c>
       <c r="AJ2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK2">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AL2" s="1">
         <v>0</v>
       </c>
     </row>
@@ -8047,119 +8060,124 @@
         <v>69166</v>
       </c>
       <c r="E3">
-        <f>IF(ISBLANK(F3),-D3,F3-D3)</f>
+        <f t="shared" si="0"/>
         <v>35</v>
       </c>
       <c r="F3" s="1">
         <v>69201</v>
       </c>
       <c r="G3">
-        <f>IF(ISBLANK(H3),-F3,H3-F3)</f>
+        <f t="shared" si="1"/>
         <v>71</v>
       </c>
       <c r="H3" s="1">
         <v>69272</v>
       </c>
       <c r="I3">
-        <f>IF(ISBLANK(J3),-H3,J3-H3)</f>
+        <f t="shared" si="2"/>
         <v>44</v>
       </c>
       <c r="J3" s="1">
         <v>69316</v>
       </c>
       <c r="K3">
-        <f>IF(ISBLANK(L3),-J3,L3-J3)</f>
+        <f t="shared" si="3"/>
         <v>66</v>
       </c>
       <c r="L3" s="1">
         <v>69382</v>
       </c>
       <c r="M3">
-        <f>IF(ISBLANK(N3),-L3,N3-L3)</f>
+        <f t="shared" si="4"/>
         <v>129</v>
       </c>
       <c r="N3" s="1">
         <v>69511</v>
       </c>
       <c r="O3">
-        <f>IF(ISBLANK(P3),-N3,P3-N3)</f>
+        <f t="shared" si="5"/>
         <v>45</v>
       </c>
       <c r="P3" s="1">
         <v>69556</v>
       </c>
       <c r="Q3">
-        <f>IF(ISBLANK(R3),-P3,R3-P3)</f>
+        <f t="shared" si="6"/>
         <v>116</v>
       </c>
       <c r="R3" s="1">
         <v>69672</v>
       </c>
       <c r="S3">
-        <f>IF(ISBLANK(T3),-R3,T3-R3)</f>
+        <f t="shared" si="7"/>
         <v>1226</v>
       </c>
       <c r="T3" s="1">
         <v>70898</v>
       </c>
       <c r="U3">
-        <f>IF(ISBLANK(V3),-T3,V3-T3)</f>
+        <f t="shared" si="8"/>
         <v>270</v>
       </c>
       <c r="V3" s="1">
         <v>71168</v>
       </c>
       <c r="W3">
-        <f>IF(ISBLANK(X3),-V3,X3-V3)</f>
+        <f t="shared" si="9"/>
         <v>674</v>
       </c>
       <c r="X3" s="1">
         <v>71842</v>
       </c>
       <c r="Y3">
-        <f>IF(ISBLANK(Z3),-X3,Z3-X3)</f>
+        <f t="shared" si="10"/>
         <v>291</v>
       </c>
       <c r="Z3" s="1">
         <v>72133</v>
       </c>
       <c r="AA3">
-        <f>IF(ISBLANK(AB3),-Z3,AB3-Z3)</f>
+        <f t="shared" si="11"/>
         <v>720</v>
       </c>
       <c r="AB3" s="1">
         <v>72853</v>
       </c>
       <c r="AC3">
-        <f>IF(ISBLANK(AD3),-AB3,AD3-AB3)</f>
+        <f t="shared" si="12"/>
         <v>929</v>
       </c>
       <c r="AD3" s="1">
         <v>73782</v>
       </c>
       <c r="AE3">
-        <f>IF(ISBLANK(AF3),-AD3,AF3-AD3)</f>
+        <f t="shared" si="13"/>
         <v>588</v>
       </c>
       <c r="AF3" s="1">
         <v>74370</v>
       </c>
       <c r="AG3">
-        <f>IF(ISBLANK(AH3),-AF3,AH3-AF3)</f>
+        <f t="shared" si="14"/>
         <v>6253</v>
       </c>
       <c r="AH3" s="1">
         <v>80623</v>
       </c>
       <c r="AI3">
-        <f>IF(ISBLANK(AJ3),-AH3,AJ3-AH3)</f>
+        <f t="shared" si="15"/>
         <v>-80623</v>
       </c>
       <c r="AJ3" s="1">
         <v>0</v>
       </c>
-      <c r="AK3" s="1"/>
-      <c r="AL3" s="1"/>
+      <c r="AK3">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AL3" s="1">
+        <v>0</v>
+      </c>
       <c r="AM3" s="1"/>
     </row>
     <row r="4" spans="1:39" x14ac:dyDescent="0.25">
@@ -8173,119 +8191,124 @@
         <v>10582</v>
       </c>
       <c r="E4">
-        <f>IF(ISBLANK(F4),-D4,F4-D4)</f>
+        <f t="shared" si="0"/>
         <v>57</v>
       </c>
       <c r="F4" s="1">
         <v>10639</v>
       </c>
       <c r="G4">
-        <f>IF(ISBLANK(H4),-F4,H4-F4)</f>
+        <f t="shared" si="1"/>
         <v>106</v>
       </c>
       <c r="H4" s="1">
         <v>10745</v>
       </c>
       <c r="I4">
-        <f>IF(ISBLANK(J4),-H4,J4-H4)</f>
+        <f t="shared" si="2"/>
         <v>138</v>
       </c>
       <c r="J4" s="1">
         <v>10883</v>
       </c>
       <c r="K4">
-        <f>IF(ISBLANK(L4),-J4,L4-J4)</f>
+        <f t="shared" si="3"/>
         <v>54</v>
       </c>
       <c r="L4" s="1">
         <v>10937</v>
       </c>
       <c r="M4">
-        <f>IF(ISBLANK(N4),-L4,N4-L4)</f>
+        <f t="shared" si="4"/>
         <v>300</v>
       </c>
       <c r="N4" s="1">
         <v>11237</v>
       </c>
       <c r="O4">
-        <f>IF(ISBLANK(P4),-N4,P4-N4)</f>
+        <f t="shared" si="5"/>
         <v>159</v>
       </c>
       <c r="P4" s="1">
         <v>11396</v>
       </c>
       <c r="Q4">
-        <f>IF(ISBLANK(R4),-P4,R4-P4)</f>
+        <f t="shared" si="6"/>
         <v>322</v>
       </c>
       <c r="R4" s="1">
         <v>11718</v>
       </c>
       <c r="S4">
-        <f>IF(ISBLANK(T4),-R4,T4-R4)</f>
+        <f t="shared" si="7"/>
         <v>908</v>
       </c>
       <c r="T4" s="1">
         <v>12626</v>
       </c>
       <c r="U4">
-        <f>IF(ISBLANK(V4),-T4,V4-T4)</f>
+        <f t="shared" si="8"/>
         <v>1585</v>
       </c>
       <c r="V4" s="1">
         <v>14211</v>
       </c>
       <c r="W4">
-        <f>IF(ISBLANK(X4),-V4,X4-V4)</f>
+        <f t="shared" si="9"/>
         <v>826</v>
       </c>
       <c r="X4" s="1">
         <v>15037</v>
       </c>
       <c r="Y4">
-        <f>IF(ISBLANK(Z4),-X4,Z4-X4)</f>
+        <f t="shared" si="10"/>
         <v>429</v>
       </c>
       <c r="Z4" s="1">
         <v>15466</v>
       </c>
       <c r="AA4">
-        <f>IF(ISBLANK(AB4),-Z4,AB4-Z4)</f>
+        <f t="shared" si="11"/>
         <v>1664</v>
       </c>
       <c r="AB4" s="1">
         <v>17130</v>
       </c>
       <c r="AC4">
-        <f>IF(ISBLANK(AD4),-AB4,AD4-AB4)</f>
+        <f t="shared" si="12"/>
         <v>-17130</v>
       </c>
       <c r="AD4" s="1">
         <v>0</v>
       </c>
       <c r="AE4">
-        <f>IF(ISBLANK(AF4),-AD4,AF4-AD4)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AF4" s="1">
         <v>0</v>
       </c>
       <c r="AG4">
-        <f>IF(ISBLANK(AH4),-AF4,AH4-AF4)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AH4" s="1">
         <v>0</v>
       </c>
       <c r="AI4">
-        <f>IF(ISBLANK(AJ4),-AH4,AJ4-AH4)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AJ4" s="1">
         <v>0</v>
       </c>
-      <c r="AK4" s="1"/>
-      <c r="AL4" s="1"/>
+      <c r="AK4">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AL4" s="1">
+        <v>0</v>
+      </c>
       <c r="AM4" s="1"/>
     </row>
     <row r="5" spans="1:39" x14ac:dyDescent="0.25">
@@ -8299,119 +8322,124 @@
         <v>64605</v>
       </c>
       <c r="E5">
-        <f>IF(ISBLANK(F5),-D5,F5-D5)</f>
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="F5" s="1">
         <v>64631</v>
       </c>
       <c r="G5">
-        <f>IF(ISBLANK(H5),-F5,H5-F5)</f>
+        <f t="shared" si="1"/>
         <v>61</v>
       </c>
       <c r="H5" s="1">
         <v>64692</v>
       </c>
       <c r="I5">
-        <f>IF(ISBLANK(J5),-H5,J5-H5)</f>
+        <f t="shared" si="2"/>
         <v>71</v>
       </c>
       <c r="J5" s="1">
         <v>64763</v>
       </c>
       <c r="K5">
-        <f>IF(ISBLANK(L5),-J5,L5-J5)</f>
+        <f t="shared" si="3"/>
         <v>136</v>
       </c>
       <c r="L5" s="1">
         <v>64899</v>
       </c>
       <c r="M5">
-        <f>IF(ISBLANK(N5),-L5,N5-L5)</f>
+        <f t="shared" si="4"/>
         <v>106</v>
       </c>
       <c r="N5" s="1">
         <v>65005</v>
       </c>
       <c r="O5">
-        <f>IF(ISBLANK(P5),-N5,P5-N5)</f>
+        <f t="shared" si="5"/>
         <v>110</v>
       </c>
       <c r="P5" s="1">
         <v>65115</v>
       </c>
       <c r="Q5">
-        <f>IF(ISBLANK(R5),-P5,R5-P5)</f>
+        <f t="shared" si="6"/>
         <v>137</v>
       </c>
       <c r="R5" s="1">
         <v>65252</v>
       </c>
       <c r="S5">
-        <f>IF(ISBLANK(T5),-R5,T5-R5)</f>
+        <f t="shared" si="7"/>
         <v>306</v>
       </c>
       <c r="T5" s="1">
         <v>65558</v>
       </c>
       <c r="U5">
-        <f>IF(ISBLANK(V5),-T5,V5-T5)</f>
+        <f t="shared" si="8"/>
         <v>491</v>
       </c>
       <c r="V5" s="1">
         <v>66049</v>
       </c>
       <c r="W5">
-        <f>IF(ISBLANK(X5),-V5,X5-V5)</f>
+        <f t="shared" si="9"/>
         <v>683</v>
       </c>
       <c r="X5" s="1">
         <v>66732</v>
       </c>
       <c r="Y5">
-        <f>IF(ISBLANK(Z5),-X5,Z5-X5)</f>
+        <f t="shared" si="10"/>
         <v>542</v>
       </c>
       <c r="Z5" s="1">
         <v>67274</v>
       </c>
       <c r="AA5">
-        <f>IF(ISBLANK(AB5),-Z5,AB5-Z5)</f>
+        <f t="shared" si="11"/>
         <v>622</v>
       </c>
       <c r="AB5" s="1">
         <v>67896</v>
       </c>
       <c r="AC5">
-        <f>IF(ISBLANK(AD5),-AB5,AD5-AB5)</f>
+        <f t="shared" si="12"/>
         <v>1194</v>
       </c>
       <c r="AD5" s="1">
         <v>69090</v>
       </c>
       <c r="AE5">
-        <f>IF(ISBLANK(AF5),-AD5,AF5-AD5)</f>
+        <f t="shared" si="13"/>
         <v>470</v>
       </c>
       <c r="AF5" s="1">
         <v>69560</v>
       </c>
       <c r="AG5">
-        <f>IF(ISBLANK(AH5),-AF5,AH5-AF5)</f>
+        <f t="shared" si="14"/>
         <v>20183</v>
       </c>
       <c r="AH5" s="1">
         <v>89743</v>
       </c>
       <c r="AI5">
-        <f>IF(ISBLANK(AJ5),-AH5,AJ5-AH5)</f>
+        <f t="shared" si="15"/>
         <v>8192</v>
       </c>
       <c r="AJ5" s="1">
         <v>97935</v>
       </c>
-      <c r="AK5" s="1"/>
-      <c r="AL5" s="1"/>
+      <c r="AK5">
+        <f t="shared" si="15"/>
+        <v>3077</v>
+      </c>
+      <c r="AL5" s="1">
+        <v>101012</v>
+      </c>
       <c r="AM5" s="1"/>
     </row>
     <row r="6" spans="1:39" x14ac:dyDescent="0.25">
@@ -8425,119 +8453,124 @@
         <v>38738</v>
       </c>
       <c r="E6">
-        <f>IF(ISBLANK(F6),-D6,F6-D6)</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="F6" s="1">
         <v>38755</v>
       </c>
       <c r="G6">
-        <f>IF(ISBLANK(H6),-F6,H6-F6)</f>
+        <f t="shared" si="1"/>
         <v>33</v>
       </c>
       <c r="H6" s="1">
         <v>38788</v>
       </c>
       <c r="I6">
-        <f>IF(ISBLANK(J6),-H6,J6-H6)</f>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="J6" s="1">
         <v>38804</v>
       </c>
       <c r="K6">
-        <f>IF(ISBLANK(L6),-J6,L6-J6)</f>
+        <f t="shared" si="3"/>
         <v>38</v>
       </c>
       <c r="L6" s="1">
         <v>38842</v>
       </c>
       <c r="M6">
-        <f>IF(ISBLANK(N6),-L6,N6-L6)</f>
+        <f t="shared" si="4"/>
         <v>84</v>
       </c>
       <c r="N6" s="1">
         <v>38926</v>
       </c>
       <c r="O6">
-        <f>IF(ISBLANK(P6),-N6,P6-N6)</f>
+        <f t="shared" si="5"/>
         <v>24</v>
       </c>
       <c r="P6" s="1">
         <v>38950</v>
       </c>
       <c r="Q6">
-        <f>IF(ISBLANK(R6),-P6,R6-P6)</f>
+        <f t="shared" si="6"/>
         <v>46</v>
       </c>
       <c r="R6" s="1">
         <v>38996</v>
       </c>
       <c r="S6">
-        <f>IF(ISBLANK(T6),-R6,T6-R6)</f>
+        <f t="shared" si="7"/>
         <v>298</v>
       </c>
       <c r="T6" s="1">
         <v>39294</v>
       </c>
       <c r="U6">
-        <f>IF(ISBLANK(V6),-T6,V6-T6)</f>
+        <f t="shared" si="8"/>
         <v>135</v>
       </c>
       <c r="V6" s="1">
         <v>39429</v>
       </c>
       <c r="W6">
-        <f>IF(ISBLANK(X6),-V6,X6-V6)</f>
+        <f t="shared" si="9"/>
         <v>426</v>
       </c>
       <c r="X6" s="1">
         <v>39855</v>
       </c>
       <c r="Y6">
-        <f>IF(ISBLANK(Z6),-X6,Z6-X6)</f>
+        <f t="shared" si="10"/>
         <v>159</v>
       </c>
       <c r="Z6" s="1">
         <v>40014</v>
       </c>
       <c r="AA6">
-        <f>IF(ISBLANK(AB6),-Z6,AB6-Z6)</f>
+        <f t="shared" si="11"/>
         <v>572</v>
       </c>
       <c r="AB6" s="1">
         <v>40586</v>
       </c>
       <c r="AC6">
-        <f>IF(ISBLANK(AD6),-AB6,AD6-AB6)</f>
+        <f t="shared" si="12"/>
         <v>483</v>
       </c>
       <c r="AD6" s="1">
         <v>41069</v>
       </c>
       <c r="AE6">
-        <f>IF(ISBLANK(AF6),-AD6,AF6-AD6)</f>
+        <f t="shared" si="13"/>
         <v>347</v>
       </c>
       <c r="AF6" s="1">
         <v>41416</v>
       </c>
       <c r="AG6">
-        <f>IF(ISBLANK(AH6),-AF6,AH6-AF6)</f>
+        <f t="shared" si="14"/>
         <v>-41416</v>
       </c>
       <c r="AH6" s="1">
         <v>0</v>
       </c>
       <c r="AI6">
-        <f>IF(ISBLANK(AJ6),-AH6,AJ6-AH6)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AJ6" s="1">
         <v>0</v>
       </c>
-      <c r="AK6" s="1"/>
-      <c r="AL6" s="1"/>
+      <c r="AK6">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AL6" s="1">
+        <v>0</v>
+      </c>
       <c r="AM6" s="1"/>
     </row>
     <row r="7" spans="1:39" x14ac:dyDescent="0.25">
@@ -8551,119 +8584,124 @@
         <v>3182</v>
       </c>
       <c r="E7">
-        <f>IF(ISBLANK(F7),-D7,F7-D7)</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="F7" s="1">
         <v>3197</v>
       </c>
       <c r="G7">
-        <f>IF(ISBLANK(H7),-F7,H7-F7)</f>
+        <f t="shared" si="1"/>
         <v>60</v>
       </c>
       <c r="H7" s="1">
         <v>3257</v>
       </c>
       <c r="I7">
-        <f>IF(ISBLANK(J7),-H7,J7-H7)</f>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="J7" s="1">
         <v>3300</v>
       </c>
       <c r="K7">
-        <f>IF(ISBLANK(L7),-J7,L7-J7)</f>
+        <f t="shared" si="3"/>
         <v>32</v>
       </c>
       <c r="L7" s="1">
         <v>3332</v>
       </c>
       <c r="M7">
-        <f>IF(ISBLANK(N7),-L7,N7-L7)</f>
+        <f t="shared" si="4"/>
         <v>-3332</v>
       </c>
       <c r="N7" s="1">
         <v>0</v>
       </c>
       <c r="O7">
-        <f>IF(ISBLANK(P7),-N7,P7-N7)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P7" s="1">
         <v>0</v>
       </c>
       <c r="Q7">
-        <f>IF(ISBLANK(R7),-P7,R7-P7)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="R7" s="1">
         <v>0</v>
       </c>
       <c r="S7">
-        <f>IF(ISBLANK(T7),-R7,T7-R7)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="T7" s="1">
         <v>0</v>
       </c>
       <c r="U7">
-        <f>IF(ISBLANK(V7),-T7,V7-T7)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="V7" s="1">
         <v>0</v>
       </c>
       <c r="W7">
-        <f>IF(ISBLANK(X7),-V7,X7-V7)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="X7" s="1">
         <v>0</v>
       </c>
       <c r="Y7">
-        <f>IF(ISBLANK(Z7),-X7,Z7-X7)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Z7" s="1">
         <v>0</v>
       </c>
       <c r="AA7">
-        <f>IF(ISBLANK(AB7),-Z7,AB7-Z7)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AB7" s="1">
         <v>0</v>
       </c>
       <c r="AC7">
-        <f>IF(ISBLANK(AD7),-AB7,AD7-AB7)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AD7" s="1">
         <v>0</v>
       </c>
       <c r="AE7">
-        <f>IF(ISBLANK(AF7),-AD7,AF7-AD7)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AF7" s="1">
         <v>0</v>
       </c>
       <c r="AG7">
-        <f>IF(ISBLANK(AH7),-AF7,AH7-AF7)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AH7" s="1">
         <v>0</v>
       </c>
       <c r="AI7">
-        <f>IF(ISBLANK(AJ7),-AH7,AJ7-AH7)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AJ7" s="1">
         <v>0</v>
       </c>
-      <c r="AK7" s="1"/>
-      <c r="AL7" s="1"/>
+      <c r="AK7">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AL7" s="1">
+        <v>0</v>
+      </c>
       <c r="AM7" s="1"/>
     </row>
     <row r="8" spans="1:39" x14ac:dyDescent="0.25">
@@ -8677,119 +8715,124 @@
         <v>9306</v>
       </c>
       <c r="E8">
-        <f>IF(ISBLANK(F8),-D8,F8-D8)</f>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="F8" s="1">
         <v>9331</v>
       </c>
       <c r="G8">
-        <f>IF(ISBLANK(H8),-F8,H8-F8)</f>
+        <f t="shared" si="1"/>
         <v>70</v>
       </c>
       <c r="H8" s="1">
         <v>9401</v>
       </c>
       <c r="I8">
-        <f>IF(ISBLANK(J8),-H8,J8-H8)</f>
+        <f t="shared" si="2"/>
         <v>35</v>
       </c>
       <c r="J8" s="1">
         <v>9436</v>
       </c>
       <c r="K8">
-        <f>IF(ISBLANK(L8),-J8,L8-J8)</f>
+        <f t="shared" si="3"/>
         <v>60</v>
       </c>
       <c r="L8" s="1">
         <v>9496</v>
       </c>
       <c r="M8">
-        <f>IF(ISBLANK(N8),-L8,N8-L8)</f>
+        <f t="shared" si="4"/>
         <v>228</v>
       </c>
       <c r="N8" s="1">
         <v>9724</v>
       </c>
       <c r="O8">
-        <f>IF(ISBLANK(P8),-N8,P8-N8)</f>
+        <f t="shared" si="5"/>
         <v>145</v>
       </c>
       <c r="P8" s="1">
         <v>9869</v>
       </c>
       <c r="Q8">
-        <f>IF(ISBLANK(R8),-P8,R8-P8)</f>
+        <f t="shared" si="6"/>
         <v>106</v>
       </c>
       <c r="R8" s="1">
         <v>9975</v>
       </c>
       <c r="S8">
-        <f>IF(ISBLANK(T8),-R8,T8-R8)</f>
+        <f t="shared" si="7"/>
         <v>247</v>
       </c>
       <c r="T8" s="1">
         <v>10222</v>
       </c>
       <c r="U8">
-        <f>IF(ISBLANK(V8),-T8,V8-T8)</f>
+        <f t="shared" si="8"/>
         <v>616</v>
       </c>
       <c r="V8" s="1">
         <v>10838</v>
       </c>
       <c r="W8">
-        <f>IF(ISBLANK(X8),-V8,X8-V8)</f>
+        <f t="shared" si="9"/>
         <v>-10838</v>
       </c>
       <c r="X8" s="1">
         <v>0</v>
       </c>
       <c r="Y8">
-        <f>IF(ISBLANK(Z8),-X8,Z8-X8)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Z8" s="1">
         <v>0</v>
       </c>
       <c r="AA8">
-        <f>IF(ISBLANK(AB8),-Z8,AB8-Z8)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AB8" s="1">
         <v>0</v>
       </c>
       <c r="AC8">
-        <f>IF(ISBLANK(AD8),-AB8,AD8-AB8)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AD8" s="1">
         <v>0</v>
       </c>
       <c r="AE8">
-        <f>IF(ISBLANK(AF8),-AD8,AF8-AD8)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AF8" s="1">
         <v>0</v>
       </c>
       <c r="AG8">
-        <f>IF(ISBLANK(AH8),-AF8,AH8-AF8)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AH8" s="1">
         <v>0</v>
       </c>
       <c r="AI8">
-        <f>IF(ISBLANK(AJ8),-AH8,AJ8-AH8)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AJ8" s="1">
         <v>0</v>
       </c>
-      <c r="AK8" s="1"/>
-      <c r="AL8" s="1"/>
+      <c r="AK8">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AL8" s="1">
+        <v>0</v>
+      </c>
       <c r="AM8" s="1"/>
     </row>
     <row r="9" spans="1:39" x14ac:dyDescent="0.25">
@@ -8803,119 +8846,124 @@
         <v>7475</v>
       </c>
       <c r="E9">
-        <f>IF(ISBLANK(F9),-D9,F9-D9)</f>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="F9" s="1">
         <v>7498</v>
       </c>
       <c r="G9">
-        <f>IF(ISBLANK(H9),-F9,H9-F9)</f>
+        <f t="shared" si="1"/>
         <v>98</v>
       </c>
       <c r="H9" s="1">
         <v>7596</v>
       </c>
       <c r="I9">
-        <f>IF(ISBLANK(J9),-H9,J9-H9)</f>
+        <f t="shared" si="2"/>
         <v>142</v>
       </c>
       <c r="J9" s="1">
         <v>7738</v>
       </c>
       <c r="K9">
-        <f>IF(ISBLANK(L9),-J9,L9-J9)</f>
+        <f t="shared" si="3"/>
         <v>70</v>
       </c>
       <c r="L9" s="1">
         <v>7808</v>
       </c>
       <c r="M9">
-        <f>IF(ISBLANK(N9),-L9,N9-L9)</f>
+        <f t="shared" si="4"/>
         <v>197</v>
       </c>
       <c r="N9" s="1">
         <v>8005</v>
       </c>
       <c r="O9">
-        <f>IF(ISBLANK(P9),-N9,P9-N9)</f>
+        <f t="shared" si="5"/>
         <v>192</v>
       </c>
       <c r="P9" s="1">
         <v>8197</v>
       </c>
       <c r="Q9">
-        <f>IF(ISBLANK(R9),-P9,R9-P9)</f>
+        <f t="shared" si="6"/>
         <v>176</v>
       </c>
       <c r="R9" s="1">
         <v>8373</v>
       </c>
       <c r="S9">
-        <f>IF(ISBLANK(T9),-R9,T9-R9)</f>
+        <f t="shared" si="7"/>
         <v>188</v>
       </c>
       <c r="T9" s="1">
         <v>8561</v>
       </c>
       <c r="U9">
-        <f>IF(ISBLANK(V9),-T9,V9-T9)</f>
+        <f t="shared" si="8"/>
         <v>-8561</v>
       </c>
       <c r="V9" s="1">
         <v>0</v>
       </c>
       <c r="W9">
-        <f>IF(ISBLANK(X9),-V9,X9-V9)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="X9" s="1">
         <v>0</v>
       </c>
       <c r="Y9">
-        <f>IF(ISBLANK(Z9),-X9,Z9-X9)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Z9" s="1">
         <v>0</v>
       </c>
       <c r="AA9">
-        <f>IF(ISBLANK(AB9),-Z9,AB9-Z9)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AB9" s="1">
         <v>0</v>
       </c>
       <c r="AC9">
-        <f>IF(ISBLANK(AD9),-AB9,AD9-AB9)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AD9" s="1">
         <v>0</v>
       </c>
       <c r="AE9">
-        <f>IF(ISBLANK(AF9),-AD9,AF9-AD9)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AF9" s="1">
         <v>0</v>
       </c>
       <c r="AG9">
-        <f>IF(ISBLANK(AH9),-AF9,AH9-AF9)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AH9" s="1">
         <v>0</v>
       </c>
       <c r="AI9">
-        <f>IF(ISBLANK(AJ9),-AH9,AJ9-AH9)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AJ9" s="1">
         <v>0</v>
       </c>
-      <c r="AK9" s="1"/>
-      <c r="AL9" s="1"/>
+      <c r="AK9">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AL9" s="1">
+        <v>0</v>
+      </c>
       <c r="AM9" s="1"/>
     </row>
     <row r="10" spans="1:39" x14ac:dyDescent="0.25">
@@ -8929,119 +8977,124 @@
         <v>84083</v>
       </c>
       <c r="E10">
-        <f>IF(ISBLANK(F10),-D10,F10-D10)</f>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="F10" s="1">
         <v>84106</v>
       </c>
       <c r="G10">
-        <f>IF(ISBLANK(H10),-F10,H10-F10)</f>
+        <f t="shared" si="1"/>
         <v>58</v>
       </c>
       <c r="H10" s="1">
         <v>84164</v>
       </c>
       <c r="I10">
-        <f>IF(ISBLANK(J10),-H10,J10-H10)</f>
+        <f t="shared" si="2"/>
         <v>74</v>
       </c>
       <c r="J10" s="1">
         <v>84238</v>
       </c>
       <c r="K10">
-        <f>IF(ISBLANK(L10),-J10,L10-J10)</f>
+        <f t="shared" si="3"/>
         <v>150</v>
       </c>
       <c r="L10" s="1">
         <v>84388</v>
       </c>
       <c r="M10">
-        <f>IF(ISBLANK(N10),-L10,N10-L10)</f>
+        <f t="shared" si="4"/>
         <v>171</v>
       </c>
       <c r="N10" s="1">
         <v>84559</v>
       </c>
       <c r="O10">
-        <f>IF(ISBLANK(P10),-N10,P10-N10)</f>
+        <f t="shared" si="5"/>
         <v>95</v>
       </c>
       <c r="P10" s="1">
         <v>84654</v>
       </c>
       <c r="Q10">
-        <f>IF(ISBLANK(R10),-P10,R10-P10)</f>
+        <f t="shared" si="6"/>
         <v>187</v>
       </c>
       <c r="R10" s="1">
         <v>84841</v>
       </c>
       <c r="S10">
-        <f>IF(ISBLANK(T10),-R10,T10-R10)</f>
+        <f t="shared" si="7"/>
         <v>130</v>
       </c>
       <c r="T10" s="1">
         <v>84971</v>
       </c>
       <c r="U10">
-        <f>IF(ISBLANK(V10),-T10,V10-T10)</f>
+        <f t="shared" si="8"/>
         <v>480</v>
       </c>
       <c r="V10" s="1">
         <v>85451</v>
       </c>
       <c r="W10">
-        <f>IF(ISBLANK(X10),-V10,X10-V10)</f>
+        <f t="shared" si="9"/>
         <v>575</v>
       </c>
       <c r="X10" s="1">
         <v>86026</v>
       </c>
       <c r="Y10">
-        <f>IF(ISBLANK(Z10),-X10,Z10-X10)</f>
+        <f t="shared" si="10"/>
         <v>1010</v>
       </c>
       <c r="Z10" s="1">
         <v>87036</v>
       </c>
       <c r="AA10">
-        <f>IF(ISBLANK(AB10),-Z10,AB10-Z10)</f>
+        <f t="shared" si="11"/>
         <v>928</v>
       </c>
       <c r="AB10" s="1">
         <v>87964</v>
       </c>
       <c r="AC10">
-        <f>IF(ISBLANK(AD10),-AB10,AD10-AB10)</f>
+        <f t="shared" si="12"/>
         <v>637</v>
       </c>
       <c r="AD10" s="1">
         <v>88601</v>
       </c>
       <c r="AE10">
-        <f>IF(ISBLANK(AF10),-AD10,AF10-AD10)</f>
+        <f t="shared" si="13"/>
         <v>435</v>
       </c>
       <c r="AF10" s="1">
         <v>89036</v>
       </c>
       <c r="AG10">
-        <f>IF(ISBLANK(AH10),-AF10,AH10-AF10)</f>
+        <f t="shared" si="14"/>
         <v>3849</v>
       </c>
       <c r="AH10" s="1">
         <v>92885</v>
       </c>
       <c r="AI10">
-        <f>IF(ISBLANK(AJ10),-AH10,AJ10-AH10)</f>
+        <f t="shared" si="15"/>
         <v>38767</v>
       </c>
       <c r="AJ10" s="1">
         <v>131652</v>
       </c>
-      <c r="AK10" s="1"/>
-      <c r="AL10" s="1"/>
+      <c r="AK10">
+        <f t="shared" si="15"/>
+        <v>-11786</v>
+      </c>
+      <c r="AL10" s="1">
+        <v>119866</v>
+      </c>
       <c r="AM10" s="1"/>
     </row>
     <row r="11" spans="1:39" x14ac:dyDescent="0.25">
@@ -9055,119 +9108,124 @@
         <v>118444</v>
       </c>
       <c r="E11">
-        <f>IF(ISBLANK(F11),-D11,F11-D11)</f>
+        <f t="shared" si="0"/>
         <v>45</v>
       </c>
       <c r="F11" s="1">
         <v>118489</v>
       </c>
       <c r="G11">
-        <f>IF(ISBLANK(H11),-F11,H11-F11)</f>
+        <f t="shared" si="1"/>
         <v>186</v>
       </c>
       <c r="H11" s="1">
         <v>118675</v>
       </c>
       <c r="I11">
-        <f>IF(ISBLANK(J11),-H11,J11-H11)</f>
+        <f t="shared" si="2"/>
         <v>98</v>
       </c>
       <c r="J11" s="1">
         <v>118773</v>
       </c>
       <c r="K11">
-        <f>IF(ISBLANK(L11),-J11,L11-J11)</f>
+        <f t="shared" si="3"/>
         <v>350</v>
       </c>
       <c r="L11" s="1">
         <v>119123</v>
       </c>
       <c r="M11">
-        <f>IF(ISBLANK(N11),-L11,N11-L11)</f>
+        <f t="shared" si="4"/>
         <v>257</v>
       </c>
       <c r="N11" s="1">
         <v>119380</v>
       </c>
       <c r="O11">
-        <f>IF(ISBLANK(P11),-N11,P11-N11)</f>
+        <f t="shared" si="5"/>
         <v>165</v>
       </c>
       <c r="P11" s="1">
         <v>119545</v>
       </c>
       <c r="Q11">
-        <f>IF(ISBLANK(R11),-P11,R11-P11)</f>
+        <f t="shared" si="6"/>
         <v>170</v>
       </c>
       <c r="R11" s="1">
         <v>119715</v>
       </c>
       <c r="S11">
-        <f>IF(ISBLANK(T11),-R11,T11-R11)</f>
+        <f t="shared" si="7"/>
         <v>168</v>
       </c>
       <c r="T11" s="1">
         <v>119883</v>
       </c>
       <c r="U11">
-        <f>IF(ISBLANK(V11),-T11,V11-T11)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="V11" s="1">
         <v>119883</v>
       </c>
       <c r="W11">
-        <f>IF(ISBLANK(X11),-V11,X11-V11)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="X11" s="1">
         <v>119883</v>
       </c>
       <c r="Y11">
-        <f>IF(ISBLANK(Z11),-X11,Z11-X11)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Z11" s="1">
         <v>119883</v>
       </c>
       <c r="AA11">
-        <f>IF(ISBLANK(AB11),-Z11,AB11-Z11)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AB11" s="1">
         <v>119883</v>
       </c>
       <c r="AC11">
-        <f>IF(ISBLANK(AD11),-AB11,AD11-AB11)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AD11" s="1">
         <v>119883</v>
       </c>
       <c r="AE11">
-        <f>IF(ISBLANK(AF11),-AD11,AF11-AD11)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AF11" s="1">
         <v>119883</v>
       </c>
       <c r="AG11">
-        <f>IF(ISBLANK(AH11),-AF11,AH11-AF11)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AH11" s="1">
         <v>119883</v>
       </c>
       <c r="AI11">
-        <f>IF(ISBLANK(AJ11),-AH11,AJ11-AH11)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AJ11" s="1">
         <v>119883</v>
       </c>
-      <c r="AK11" s="1"/>
-      <c r="AL11" s="1"/>
+      <c r="AK11">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AL11" s="1">
+        <v>119883</v>
+      </c>
       <c r="AM11" s="1"/>
     </row>
     <row r="12" spans="1:39" x14ac:dyDescent="0.25">
@@ -9181,119 +9239,124 @@
         <v>2395</v>
       </c>
       <c r="E12">
-        <f>IF(ISBLANK(F12),-D12,F12-D12)</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="F12" s="1">
         <v>2409</v>
       </c>
       <c r="G12">
-        <f>IF(ISBLANK(H12),-F12,H12-F12)</f>
+        <f t="shared" si="1"/>
         <v>-2409</v>
       </c>
       <c r="H12" s="1">
         <v>0</v>
       </c>
       <c r="I12">
-        <f>IF(ISBLANK(J12),-H12,J12-H12)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J12" s="1">
         <v>0</v>
       </c>
       <c r="K12">
-        <f>IF(ISBLANK(L12),-J12,L12-J12)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L12" s="1">
         <v>0</v>
       </c>
       <c r="M12">
-        <f>IF(ISBLANK(N12),-L12,N12-L12)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N12" s="1">
         <v>0</v>
       </c>
       <c r="O12">
-        <f>IF(ISBLANK(P12),-N12,P12-N12)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P12" s="1">
         <v>0</v>
       </c>
       <c r="Q12">
-        <f>IF(ISBLANK(R12),-P12,R12-P12)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="R12" s="1">
         <v>0</v>
       </c>
       <c r="S12">
-        <f>IF(ISBLANK(T12),-R12,T12-R12)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="T12" s="1">
         <v>0</v>
       </c>
       <c r="U12">
-        <f>IF(ISBLANK(V12),-T12,V12-T12)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="V12" s="1">
         <v>0</v>
       </c>
       <c r="W12">
-        <f>IF(ISBLANK(X12),-V12,X12-V12)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="X12" s="1">
         <v>0</v>
       </c>
       <c r="Y12">
-        <f>IF(ISBLANK(Z12),-X12,Z12-X12)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Z12" s="1">
         <v>0</v>
       </c>
       <c r="AA12">
-        <f>IF(ISBLANK(AB12),-Z12,AB12-Z12)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AB12" s="1">
         <v>0</v>
       </c>
       <c r="AC12">
-        <f>IF(ISBLANK(AD12),-AB12,AD12-AB12)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AD12" s="1">
         <v>0</v>
       </c>
       <c r="AE12">
-        <f>IF(ISBLANK(AF12),-AD12,AF12-AD12)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AF12" s="1">
         <v>0</v>
       </c>
       <c r="AG12">
-        <f>IF(ISBLANK(AH12),-AF12,AH12-AF12)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AH12" s="1">
         <v>0</v>
       </c>
       <c r="AI12">
-        <f>IF(ISBLANK(AJ12),-AH12,AJ12-AH12)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AJ12" s="1">
         <v>0</v>
       </c>
-      <c r="AK12" s="1"/>
-      <c r="AL12" s="1"/>
+      <c r="AK12">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AL12" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -9306,115 +9369,122 @@
         <v>9423</v>
       </c>
       <c r="E13">
-        <f>IF(ISBLANK(F13),-D13,F13-D13)</f>
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="F13" s="1">
         <v>9455</v>
       </c>
       <c r="G13">
-        <f>IF(ISBLANK(H13),-F13,H13-F13)</f>
+        <f t="shared" si="1"/>
         <v>325</v>
       </c>
       <c r="H13" s="1">
         <v>9780</v>
       </c>
       <c r="I13">
-        <f>IF(ISBLANK(J13),-H13,J13-H13)</f>
+        <f t="shared" si="2"/>
         <v>75</v>
       </c>
       <c r="J13" s="1">
         <v>9855</v>
       </c>
       <c r="K13">
-        <f>IF(ISBLANK(L13),-J13,L13-J13)</f>
+        <f t="shared" si="3"/>
         <v>114</v>
       </c>
       <c r="L13" s="1">
         <v>9969</v>
       </c>
       <c r="M13">
-        <f>IF(ISBLANK(N13),-L13,N13-L13)</f>
+        <f t="shared" si="4"/>
         <v>280</v>
       </c>
       <c r="N13" s="1">
         <v>10249</v>
       </c>
       <c r="O13">
-        <f>IF(ISBLANK(P13),-N13,P13-N13)</f>
+        <f t="shared" si="5"/>
         <v>78</v>
       </c>
       <c r="P13" s="1">
         <v>10327</v>
       </c>
       <c r="Q13">
-        <f>IF(ISBLANK(R13),-P13,R13-P13)</f>
+        <f t="shared" si="6"/>
         <v>137</v>
       </c>
       <c r="R13" s="1">
         <v>10464</v>
       </c>
       <c r="S13">
-        <f>IF(ISBLANK(T13),-R13,T13-R13)</f>
+        <f t="shared" si="7"/>
         <v>79</v>
       </c>
       <c r="T13" s="1">
         <v>10543</v>
       </c>
       <c r="U13">
-        <f>IF(ISBLANK(V13),-T13,V13-T13)</f>
+        <f t="shared" si="8"/>
         <v>1160</v>
       </c>
       <c r="V13" s="1">
         <v>11703</v>
       </c>
       <c r="W13">
-        <f>IF(ISBLANK(X13),-V13,X13-V13)</f>
+        <f t="shared" si="9"/>
         <v>568</v>
       </c>
       <c r="X13" s="1">
         <v>12271</v>
       </c>
       <c r="Y13">
-        <f>IF(ISBLANK(Z13),-X13,Z13-X13)</f>
+        <f t="shared" si="10"/>
         <v>499</v>
       </c>
       <c r="Z13" s="1">
         <v>12770</v>
       </c>
       <c r="AA13">
-        <f>IF(ISBLANK(AB13),-Z13,AB13-Z13)</f>
+        <f t="shared" si="11"/>
         <v>-12770</v>
       </c>
       <c r="AB13" s="1">
         <v>0</v>
       </c>
       <c r="AC13">
-        <f>IF(ISBLANK(AD13),-AB13,AD13-AB13)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AD13" s="1">
         <v>0</v>
       </c>
       <c r="AE13">
-        <f>IF(ISBLANK(AF13),-AD13,AF13-AD13)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AF13" s="1">
         <v>0</v>
       </c>
       <c r="AG13">
-        <f>IF(ISBLANK(AH13),-AF13,AH13-AF13)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AH13" s="1">
         <v>0</v>
       </c>
       <c r="AI13">
-        <f>IF(ISBLANK(AJ13),-AH13,AJ13-AH13)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AJ13" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK13">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AL13" s="1">
         <v>0</v>
       </c>
     </row>
@@ -9429,118 +9499,124 @@
         <v>22075</v>
       </c>
       <c r="E14">
-        <f>IF(ISBLANK(F14),-D14,F14-D14)</f>
+        <f t="shared" si="0"/>
         <v>38</v>
       </c>
       <c r="F14" s="1">
         <v>22113</v>
       </c>
       <c r="G14">
-        <f>IF(ISBLANK(H14),-F14,H14-F14)</f>
+        <f t="shared" si="1"/>
         <v>80</v>
       </c>
       <c r="H14" s="1">
         <v>22193</v>
       </c>
       <c r="I14">
-        <f>IF(ISBLANK(J14),-H14,J14-H14)</f>
+        <f t="shared" si="2"/>
         <v>58</v>
       </c>
       <c r="J14" s="1">
         <v>22251</v>
       </c>
       <c r="K14">
-        <f>IF(ISBLANK(L14),-J14,L14-J14)</f>
+        <f t="shared" si="3"/>
         <v>70</v>
       </c>
       <c r="L14" s="1">
         <v>22321</v>
       </c>
       <c r="M14">
-        <f>IF(ISBLANK(N14),-L14,N14-L14)</f>
+        <f t="shared" si="4"/>
         <v>62</v>
       </c>
       <c r="N14" s="1">
         <v>22383</v>
       </c>
       <c r="O14">
-        <f>IF(ISBLANK(P14),-N14,P14-N14)</f>
+        <f t="shared" si="5"/>
         <v>70</v>
       </c>
       <c r="P14" s="1">
         <v>22453</v>
       </c>
       <c r="Q14">
-        <f>IF(ISBLANK(R14),-P14,R14-P14)</f>
+        <f t="shared" si="6"/>
         <v>173</v>
       </c>
       <c r="R14" s="1">
         <v>22626</v>
       </c>
       <c r="S14">
-        <f>IF(ISBLANK(T14),-R14,T14-R14)</f>
+        <f t="shared" si="7"/>
         <v>74</v>
       </c>
       <c r="T14" s="1">
         <v>22700</v>
       </c>
       <c r="U14">
-        <f>IF(ISBLANK(V14),-T14,V14-T14)</f>
+        <f t="shared" si="8"/>
         <v>193</v>
       </c>
       <c r="V14" s="1">
         <v>22893</v>
       </c>
       <c r="W14">
-        <f>IF(ISBLANK(X14),-V14,X14-V14)</f>
+        <f t="shared" si="9"/>
         <v>626</v>
       </c>
       <c r="X14" s="1">
         <v>23519</v>
       </c>
       <c r="Y14">
-        <f>IF(ISBLANK(Z14),-X14,Z14-X14)</f>
+        <f t="shared" si="10"/>
         <v>330</v>
       </c>
       <c r="Z14" s="1">
         <v>23849</v>
       </c>
       <c r="AA14">
-        <f>IF(ISBLANK(AB14),-Z14,AB14-Z14)</f>
+        <f t="shared" si="11"/>
         <v>483</v>
       </c>
       <c r="AB14" s="1">
         <v>24332</v>
       </c>
       <c r="AC14">
-        <f>IF(ISBLANK(AD14),-AB14,AD14-AB14)</f>
+        <f t="shared" si="12"/>
         <v>600</v>
       </c>
       <c r="AD14" s="1">
         <v>24932</v>
       </c>
       <c r="AE14">
-        <f>IF(ISBLANK(AF14),-AD14,AF14-AD14)</f>
+        <f t="shared" si="13"/>
         <v>1026</v>
       </c>
       <c r="AF14" s="1">
         <v>25958</v>
       </c>
       <c r="AG14">
-        <f>IF(ISBLANK(AH14),-AF14,AH14-AF14)</f>
+        <f t="shared" si="14"/>
         <v>-25958</v>
       </c>
       <c r="AH14" s="1">
         <v>0</v>
       </c>
       <c r="AI14">
-        <f>IF(ISBLANK(AJ14),-AH14,AJ14-AH14)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AJ14" s="1">
         <v>0</v>
       </c>
-      <c r="AK14" s="1"/>
+      <c r="AK14">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AL14" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A15">
@@ -9553,115 +9629,122 @@
         <v>9823</v>
       </c>
       <c r="E15">
-        <f>IF(ISBLANK(F15),-D15,F15-D15)</f>
+        <f t="shared" si="0"/>
         <v>37</v>
       </c>
       <c r="F15" s="1">
         <v>9860</v>
       </c>
       <c r="G15">
-        <f>IF(ISBLANK(H15),-F15,H15-F15)</f>
+        <f t="shared" si="1"/>
         <v>76</v>
       </c>
       <c r="H15" s="1">
         <v>9936</v>
       </c>
       <c r="I15">
-        <f>IF(ISBLANK(J15),-H15,J15-H15)</f>
+        <f t="shared" si="2"/>
         <v>54</v>
       </c>
       <c r="J15" s="1">
         <v>9990</v>
       </c>
       <c r="K15">
-        <f>IF(ISBLANK(L15),-J15,L15-J15)</f>
+        <f t="shared" si="3"/>
         <v>184</v>
       </c>
       <c r="L15" s="1">
         <v>10174</v>
       </c>
       <c r="M15">
-        <f>IF(ISBLANK(N15),-L15,N15-L15)</f>
+        <f t="shared" si="4"/>
         <v>52</v>
       </c>
       <c r="N15" s="1">
         <v>10226</v>
       </c>
       <c r="O15">
-        <f>IF(ISBLANK(P15),-N15,P15-N15)</f>
+        <f t="shared" si="5"/>
         <v>168</v>
       </c>
       <c r="P15" s="1">
         <v>10394</v>
       </c>
       <c r="Q15">
-        <f>IF(ISBLANK(R15),-P15,R15-P15)</f>
+        <f t="shared" si="6"/>
         <v>214</v>
       </c>
       <c r="R15" s="1">
         <v>10608</v>
       </c>
       <c r="S15">
-        <f>IF(ISBLANK(T15),-R15,T15-R15)</f>
+        <f t="shared" si="7"/>
         <v>48</v>
       </c>
       <c r="T15" s="1">
         <v>10656</v>
       </c>
       <c r="U15">
-        <f>IF(ISBLANK(V15),-T15,V15-T15)</f>
+        <f t="shared" si="8"/>
         <v>286</v>
       </c>
       <c r="V15" s="1">
         <v>10942</v>
       </c>
       <c r="W15">
-        <f>IF(ISBLANK(X15),-V15,X15-V15)</f>
+        <f t="shared" si="9"/>
         <v>208</v>
       </c>
       <c r="X15" s="1">
         <v>11150</v>
       </c>
       <c r="Y15">
-        <f>IF(ISBLANK(Z15),-X15,Z15-X15)</f>
+        <f t="shared" si="10"/>
         <v>-11150</v>
       </c>
       <c r="Z15" s="1">
         <v>0</v>
       </c>
       <c r="AA15">
-        <f>IF(ISBLANK(AB15),-Z15,AB15-Z15)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AB15" s="1">
         <v>0</v>
       </c>
       <c r="AC15">
-        <f>IF(ISBLANK(AD15),-AB15,AD15-AB15)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AD15" s="1">
         <v>0</v>
       </c>
       <c r="AE15">
-        <f>IF(ISBLANK(AF15),-AD15,AF15-AD15)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AF15" s="1">
         <v>0</v>
       </c>
       <c r="AG15">
-        <f>IF(ISBLANK(AH15),-AF15,AH15-AF15)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AH15" s="1">
         <v>0</v>
       </c>
       <c r="AI15">
-        <f>IF(ISBLANK(AJ15),-AH15,AJ15-AH15)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AJ15" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK15">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AL15" s="1">
         <v>0</v>
       </c>
     </row>
@@ -9676,119 +9759,126 @@
         <v>3682</v>
       </c>
       <c r="E16">
-        <f>IF(ISBLANK(F16),-D16,F16-D16)</f>
+        <f t="shared" si="0"/>
         <v>77</v>
       </c>
       <c r="F16" s="1">
         <v>3759</v>
       </c>
       <c r="G16">
-        <f>IF(ISBLANK(H16),-F16,H16-F16)</f>
+        <f t="shared" si="1"/>
         <v>44</v>
       </c>
       <c r="H16" s="1">
         <v>3803</v>
       </c>
       <c r="I16">
-        <f>IF(ISBLANK(J16),-H16,J16-H16)</f>
+        <f t="shared" si="2"/>
         <v>116</v>
       </c>
       <c r="J16" s="1">
         <v>3919</v>
       </c>
       <c r="K16">
-        <f>IF(ISBLANK(L16),-J16,L16-J16)</f>
+        <f t="shared" si="3"/>
         <v>87</v>
       </c>
       <c r="L16" s="1">
         <v>4006</v>
       </c>
       <c r="M16">
-        <f>IF(ISBLANK(N16),-L16,N16-L16)</f>
+        <f t="shared" si="4"/>
         <v>41</v>
       </c>
       <c r="N16" s="1">
         <v>4047</v>
       </c>
       <c r="O16">
-        <f>IF(ISBLANK(P16),-N16,P16-N16)</f>
+        <f t="shared" si="5"/>
         <v>134</v>
       </c>
       <c r="P16" s="1">
         <v>4181</v>
       </c>
       <c r="Q16">
-        <f>IF(ISBLANK(R16),-P16,R16-P16)</f>
+        <f t="shared" si="6"/>
         <v>-4181</v>
       </c>
       <c r="R16" s="1">
         <v>0</v>
       </c>
       <c r="S16">
-        <f>IF(ISBLANK(T16),-R16,T16-R16)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="T16" s="1">
         <v>0</v>
       </c>
       <c r="U16">
-        <f>IF(ISBLANK(V16),-T16,V16-T16)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="V16" s="1">
         <v>0</v>
       </c>
       <c r="W16">
-        <f>IF(ISBLANK(X16),-V16,X16-V16)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="X16" s="1">
         <v>0</v>
       </c>
       <c r="Y16">
-        <f>IF(ISBLANK(Z16),-X16,Z16-X16)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Z16" s="1">
         <v>0</v>
       </c>
       <c r="AA16">
-        <f>IF(ISBLANK(AB16),-Z16,AB16-Z16)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AB16" s="1">
         <v>0</v>
       </c>
       <c r="AC16">
-        <f>IF(ISBLANK(AD16),-AB16,AD16-AB16)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AD16" s="1">
         <v>0</v>
       </c>
       <c r="AE16">
-        <f>IF(ISBLANK(AF16),-AD16,AF16-AD16)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AF16" s="1">
         <v>0</v>
       </c>
       <c r="AG16">
-        <f>IF(ISBLANK(AH16),-AF16,AH16-AF16)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AH16" s="1">
         <v>0</v>
       </c>
       <c r="AI16">
-        <f>IF(ISBLANK(AJ16),-AH16,AJ16-AH16)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AJ16" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK16">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AL16" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>5</v>
       </c>
@@ -9799,119 +9889,126 @@
         <v>75946</v>
       </c>
       <c r="E17">
-        <f>IF(ISBLANK(F17),-D17,F17-D17)</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="F17" s="1">
         <v>76046</v>
       </c>
       <c r="G17">
-        <f>IF(ISBLANK(H17),-F17,H17-F17)</f>
+        <f t="shared" si="1"/>
         <v>201</v>
       </c>
       <c r="H17" s="1">
         <v>76247</v>
       </c>
       <c r="I17">
-        <f>IF(ISBLANK(J17),-H17,J17-H17)</f>
+        <f t="shared" si="2"/>
         <v>126</v>
       </c>
       <c r="J17" s="1">
         <v>76373</v>
       </c>
       <c r="K17">
-        <f>IF(ISBLANK(L17),-J17,L17-J17)</f>
+        <f t="shared" si="3"/>
         <v>272</v>
       </c>
       <c r="L17" s="1">
         <v>76645</v>
       </c>
       <c r="M17">
-        <f>IF(ISBLANK(N17),-L17,N17-L17)</f>
+        <f t="shared" si="4"/>
         <v>74</v>
       </c>
       <c r="N17" s="1">
         <v>76719</v>
       </c>
       <c r="O17">
-        <f>IF(ISBLANK(P17),-N17,P17-N17)</f>
+        <f t="shared" si="5"/>
         <v>301</v>
       </c>
       <c r="P17" s="1">
         <v>77020</v>
       </c>
       <c r="Q17">
-        <f>IF(ISBLANK(R17),-P17,R17-P17)</f>
+        <f t="shared" si="6"/>
         <v>283</v>
       </c>
       <c r="R17" s="1">
         <v>77303</v>
       </c>
       <c r="S17">
-        <f>IF(ISBLANK(T17),-R17,T17-R17)</f>
+        <f t="shared" si="7"/>
         <v>112</v>
       </c>
       <c r="T17" s="1">
         <v>77415</v>
       </c>
       <c r="U17">
-        <f>IF(ISBLANK(V17),-T17,V17-T17)</f>
+        <f t="shared" si="8"/>
         <v>339</v>
       </c>
       <c r="V17" s="1">
         <v>77754</v>
       </c>
       <c r="W17">
-        <f>IF(ISBLANK(X17),-V17,X17-V17)</f>
+        <f t="shared" si="9"/>
         <v>1066</v>
       </c>
       <c r="X17" s="1">
         <v>78820</v>
       </c>
       <c r="Y17">
-        <f>IF(ISBLANK(Z17),-X17,Z17-X17)</f>
+        <f t="shared" si="10"/>
         <v>1295</v>
       </c>
       <c r="Z17" s="1">
         <v>80115</v>
       </c>
       <c r="AA17">
-        <f>IF(ISBLANK(AB17),-Z17,AB17-Z17)</f>
+        <f t="shared" si="11"/>
         <v>593</v>
       </c>
       <c r="AB17" s="1">
         <v>80708</v>
       </c>
       <c r="AC17">
-        <f>IF(ISBLANK(AD17),-AB17,AD17-AB17)</f>
+        <f t="shared" si="12"/>
         <v>1290</v>
       </c>
       <c r="AD17" s="1">
         <v>81998</v>
       </c>
       <c r="AE17">
-        <f>IF(ISBLANK(AF17),-AD17,AF17-AD17)</f>
+        <f t="shared" si="13"/>
         <v>2743</v>
       </c>
       <c r="AF17" s="1">
         <v>84741</v>
       </c>
       <c r="AG17">
-        <f>IF(ISBLANK(AH17),-AF17,AH17-AF17)</f>
+        <f t="shared" si="14"/>
         <v>8382</v>
       </c>
       <c r="AH17" s="1">
         <v>93123</v>
       </c>
       <c r="AI17">
-        <f>IF(ISBLANK(AJ17),-AH17,AJ17-AH17)</f>
+        <f t="shared" si="15"/>
         <v>2972</v>
       </c>
       <c r="AJ17" s="1">
         <v>96095</v>
       </c>
-    </row>
-    <row r="18" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK17">
+        <f t="shared" si="15"/>
+        <v>2611</v>
+      </c>
+      <c r="AL17">
+        <v>98706</v>
+      </c>
+    </row>
+    <row r="18" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>4</v>
       </c>
@@ -9922,119 +10019,126 @@
         <v>79072</v>
       </c>
       <c r="E18">
-        <f>IF(ISBLANK(F18),-D18,F18-D18)</f>
+        <f t="shared" si="0"/>
         <v>68</v>
       </c>
       <c r="F18" s="1">
         <v>79140</v>
       </c>
       <c r="G18">
-        <f>IF(ISBLANK(H18),-F18,H18-F18)</f>
+        <f t="shared" si="1"/>
         <v>142</v>
       </c>
       <c r="H18" s="1">
         <v>79282</v>
       </c>
       <c r="I18">
-        <f>IF(ISBLANK(J18),-H18,J18-H18)</f>
+        <f t="shared" si="2"/>
         <v>105</v>
       </c>
       <c r="J18" s="1">
         <v>79387</v>
       </c>
       <c r="K18">
-        <f>IF(ISBLANK(L18),-J18,L18-J18)</f>
+        <f t="shared" si="3"/>
         <v>186</v>
       </c>
       <c r="L18" s="1">
         <v>79573</v>
       </c>
       <c r="M18">
-        <f>IF(ISBLANK(N18),-L18,N18-L18)</f>
+        <f t="shared" si="4"/>
         <v>168</v>
       </c>
       <c r="N18" s="1">
         <v>79741</v>
       </c>
       <c r="O18">
-        <f>IF(ISBLANK(P18),-N18,P18-N18)</f>
+        <f t="shared" si="5"/>
         <v>204</v>
       </c>
       <c r="P18" s="1">
         <v>79945</v>
       </c>
       <c r="Q18">
-        <f>IF(ISBLANK(R18),-P18,R18-P18)</f>
+        <f t="shared" si="6"/>
         <v>305</v>
       </c>
       <c r="R18" s="1">
         <v>80250</v>
       </c>
       <c r="S18">
-        <f>IF(ISBLANK(T18),-R18,T18-R18)</f>
+        <f t="shared" si="7"/>
         <v>127</v>
       </c>
       <c r="T18" s="1">
         <v>80377</v>
       </c>
       <c r="U18">
-        <f>IF(ISBLANK(V18),-T18,V18-T18)</f>
+        <f t="shared" si="8"/>
         <v>446</v>
       </c>
       <c r="V18" s="1">
         <v>80823</v>
       </c>
       <c r="W18">
-        <f>IF(ISBLANK(X18),-V18,X18-V18)</f>
+        <f t="shared" si="9"/>
         <v>991</v>
       </c>
       <c r="X18" s="1">
         <v>81814</v>
       </c>
       <c r="Y18">
-        <f>IF(ISBLANK(Z18),-X18,Z18-X18)</f>
+        <f t="shared" si="10"/>
         <v>1119</v>
       </c>
       <c r="Z18" s="1">
         <v>82933</v>
       </c>
       <c r="AA18">
-        <f>IF(ISBLANK(AB18),-Z18,AB18-Z18)</f>
+        <f t="shared" si="11"/>
         <v>958</v>
       </c>
       <c r="AB18" s="1">
         <v>83891</v>
       </c>
       <c r="AC18">
-        <f>IF(ISBLANK(AD18),-AB18,AD18-AB18)</f>
+        <f t="shared" si="12"/>
         <v>1108</v>
       </c>
       <c r="AD18" s="1">
         <v>84999</v>
       </c>
       <c r="AE18">
-        <f>IF(ISBLANK(AF18),-AD18,AF18-AD18)</f>
+        <f t="shared" si="13"/>
         <v>2323</v>
       </c>
       <c r="AF18" s="1">
         <v>87322</v>
       </c>
       <c r="AG18">
-        <f>IF(ISBLANK(AH18),-AF18,AH18-AF18)</f>
+        <f t="shared" si="14"/>
         <v>4517</v>
       </c>
       <c r="AH18" s="1">
         <v>91839</v>
       </c>
       <c r="AI18">
-        <f>IF(ISBLANK(AJ18),-AH18,AJ18-AH18)</f>
+        <f t="shared" si="15"/>
         <v>3734</v>
       </c>
       <c r="AJ18" s="1">
         <v>95573</v>
       </c>
-    </row>
-    <row r="19" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK18">
+        <f t="shared" si="15"/>
+        <v>2806</v>
+      </c>
+      <c r="AL18">
+        <v>98379</v>
+      </c>
+    </row>
+    <row r="19" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>20</v>
       </c>
@@ -10045,119 +10149,126 @@
         <v>2864</v>
       </c>
       <c r="E19">
-        <f>IF(ISBLANK(F19),-D19,F19-D19)</f>
+        <f t="shared" si="0"/>
         <v>34</v>
       </c>
       <c r="F19" s="1">
         <v>2898</v>
       </c>
       <c r="G19">
-        <f>IF(ISBLANK(H19),-F19,H19-F19)</f>
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="H19" s="1">
         <v>2919</v>
       </c>
       <c r="I19">
-        <f>IF(ISBLANK(J19),-H19,J19-H19)</f>
+        <f t="shared" si="2"/>
         <v>148</v>
       </c>
       <c r="J19" s="1">
         <v>3067</v>
       </c>
       <c r="K19">
-        <f>IF(ISBLANK(L19),-J19,L19-J19)</f>
+        <f t="shared" si="3"/>
         <v>-3067</v>
       </c>
       <c r="L19" s="1">
         <v>0</v>
       </c>
       <c r="M19">
-        <f>IF(ISBLANK(N19),-L19,N19-L19)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N19" s="1">
         <v>0</v>
       </c>
       <c r="O19">
-        <f>IF(ISBLANK(P19),-N19,P19-N19)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P19" s="1">
         <v>0</v>
       </c>
       <c r="Q19">
-        <f>IF(ISBLANK(R19),-P19,R19-P19)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="R19" s="1">
         <v>0</v>
       </c>
       <c r="S19">
-        <f>IF(ISBLANK(T19),-R19,T19-R19)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="T19" s="1">
         <v>0</v>
       </c>
       <c r="U19">
-        <f>IF(ISBLANK(V19),-T19,V19-T19)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="V19" s="1">
         <v>0</v>
       </c>
       <c r="W19">
-        <f>IF(ISBLANK(X19),-V19,X19-V19)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="X19" s="1">
         <v>0</v>
       </c>
       <c r="Y19">
-        <f>IF(ISBLANK(Z19),-X19,Z19-X19)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Z19" s="1">
         <v>0</v>
       </c>
       <c r="AA19">
-        <f>IF(ISBLANK(AB19),-Z19,AB19-Z19)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AB19" s="1">
         <v>0</v>
       </c>
       <c r="AC19">
-        <f>IF(ISBLANK(AD19),-AB19,AD19-AB19)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AD19" s="1">
         <v>0</v>
       </c>
       <c r="AE19">
-        <f>IF(ISBLANK(AF19),-AD19,AF19-AD19)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AF19" s="1">
         <v>0</v>
       </c>
       <c r="AG19">
-        <f>IF(ISBLANK(AH19),-AF19,AH19-AF19)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AH19" s="1">
         <v>0</v>
       </c>
       <c r="AI19">
-        <f>IF(ISBLANK(AJ19),-AH19,AJ19-AH19)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AJ19" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK19">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AL19" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>21</v>
       </c>
@@ -10168,119 +10279,126 @@
         <v>2416</v>
       </c>
       <c r="E20">
-        <f>IF(ISBLANK(F20),-D20,F20-D20)</f>
+        <f t="shared" si="0"/>
         <v>48</v>
       </c>
       <c r="F20" s="1">
         <v>2464</v>
       </c>
       <c r="G20">
-        <f>IF(ISBLANK(H20),-F20,H20-F20)</f>
+        <f t="shared" si="1"/>
         <v>78</v>
       </c>
       <c r="H20" s="1">
         <v>2542</v>
       </c>
       <c r="I20">
-        <f>IF(ISBLANK(J20),-H20,J20-H20)</f>
+        <f t="shared" si="2"/>
         <v>-2542</v>
       </c>
       <c r="J20" s="1">
         <v>0</v>
       </c>
       <c r="K20">
-        <f>IF(ISBLANK(L20),-J20,L20-J20)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L20" s="1">
         <v>0</v>
       </c>
       <c r="M20">
-        <f>IF(ISBLANK(N20),-L20,N20-L20)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N20" s="1">
         <v>0</v>
       </c>
       <c r="O20">
-        <f>IF(ISBLANK(P20),-N20,P20-N20)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P20" s="1">
         <v>0</v>
       </c>
       <c r="Q20">
-        <f>IF(ISBLANK(R20),-P20,R20-P20)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="R20" s="1">
         <v>0</v>
       </c>
       <c r="S20">
-        <f>IF(ISBLANK(T20),-R20,T20-R20)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="T20" s="1">
         <v>0</v>
       </c>
       <c r="U20">
-        <f>IF(ISBLANK(V20),-T20,V20-T20)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="V20" s="1">
         <v>0</v>
       </c>
       <c r="W20">
-        <f>IF(ISBLANK(X20),-V20,X20-V20)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="X20" s="1">
         <v>0</v>
       </c>
       <c r="Y20">
-        <f>IF(ISBLANK(Z20),-X20,Z20-X20)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Z20" s="1">
         <v>0</v>
       </c>
       <c r="AA20">
-        <f>IF(ISBLANK(AB20),-Z20,AB20-Z20)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AB20" s="1">
         <v>0</v>
       </c>
       <c r="AC20">
-        <f>IF(ISBLANK(AD20),-AB20,AD20-AB20)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AD20" s="1">
         <v>0</v>
       </c>
       <c r="AE20">
-        <f>IF(ISBLANK(AF20),-AD20,AF20-AD20)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AF20" s="1">
         <v>0</v>
       </c>
       <c r="AG20">
-        <f>IF(ISBLANK(AH20),-AF20,AH20-AF20)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AH20" s="1">
         <v>0</v>
       </c>
       <c r="AI20">
-        <f>IF(ISBLANK(AJ20),-AH20,AJ20-AH20)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AJ20" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AL20" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>23</v>
       </c>
@@ -10291,119 +10409,126 @@
         <v>1423</v>
       </c>
       <c r="E21">
-        <f>IF(ISBLANK(F21),-D21,F21-D21)</f>
+        <f t="shared" si="0"/>
         <v>-1423</v>
       </c>
       <c r="F21" s="1">
         <v>0</v>
       </c>
       <c r="G21">
-        <f>IF(ISBLANK(H21),-F21,H21-F21)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H21" s="1">
         <v>0</v>
       </c>
       <c r="I21">
-        <f>IF(ISBLANK(J21),-H21,J21-H21)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J21" s="1">
         <v>0</v>
       </c>
       <c r="K21">
-        <f>IF(ISBLANK(L21),-J21,L21-J21)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L21" s="1">
         <v>0</v>
       </c>
       <c r="M21">
-        <f>IF(ISBLANK(N21),-L21,N21-L21)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N21" s="1">
         <v>0</v>
       </c>
       <c r="O21">
-        <f>IF(ISBLANK(P21),-N21,P21-N21)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P21" s="1">
         <v>0</v>
       </c>
       <c r="Q21">
-        <f>IF(ISBLANK(R21),-P21,R21-P21)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="R21" s="1">
         <v>0</v>
       </c>
       <c r="S21">
-        <f>IF(ISBLANK(T21),-R21,T21-R21)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="T21" s="1">
         <v>0</v>
       </c>
       <c r="U21">
-        <f>IF(ISBLANK(V21),-T21,V21-T21)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="V21" s="1">
         <v>0</v>
       </c>
       <c r="W21">
-        <f>IF(ISBLANK(X21),-V21,X21-V21)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="X21" s="1">
         <v>0</v>
       </c>
       <c r="Y21">
-        <f>IF(ISBLANK(Z21),-X21,Z21-X21)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Z21" s="1">
         <v>0</v>
       </c>
       <c r="AA21">
-        <f>IF(ISBLANK(AB21),-Z21,AB21-Z21)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AB21" s="1">
         <v>0</v>
       </c>
       <c r="AC21">
-        <f>IF(ISBLANK(AD21),-AB21,AD21-AB21)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AD21" s="1">
         <v>0</v>
       </c>
       <c r="AE21">
-        <f>IF(ISBLANK(AF21),-AD21,AF21-AD21)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AF21" s="1">
         <v>0</v>
       </c>
       <c r="AG21">
-        <f>IF(ISBLANK(AH21),-AF21,AH21-AF21)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AH21" s="1">
         <v>0</v>
       </c>
       <c r="AI21">
-        <f>IF(ISBLANK(AJ21),-AH21,AJ21-AH21)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AJ21" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK21">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AL21" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>10</v>
       </c>
@@ -10414,119 +10539,126 @@
         <v>14802</v>
       </c>
       <c r="E22">
-        <f>IF(ISBLANK(F22),-D22,F22-D22)</f>
+        <f t="shared" si="0"/>
         <v>156</v>
       </c>
       <c r="F22" s="1">
         <v>14958</v>
       </c>
       <c r="G22">
-        <f>IF(ISBLANK(H22),-F22,H22-F22)</f>
+        <f t="shared" si="1"/>
         <v>51</v>
       </c>
       <c r="H22" s="1">
         <v>15009</v>
       </c>
       <c r="I22">
-        <f>IF(ISBLANK(J22),-H22,J22-H22)</f>
+        <f t="shared" si="2"/>
         <v>198</v>
       </c>
       <c r="J22" s="1">
         <v>15207</v>
       </c>
       <c r="K22">
-        <f>IF(ISBLANK(L22),-J22,L22-J22)</f>
+        <f t="shared" si="3"/>
         <v>146</v>
       </c>
       <c r="L22" s="1">
         <v>15353</v>
       </c>
       <c r="M22">
-        <f>IF(ISBLANK(N22),-L22,N22-L22)</f>
+        <f t="shared" si="4"/>
         <v>41</v>
       </c>
       <c r="N22" s="1">
         <v>15394</v>
       </c>
       <c r="O22">
-        <f>IF(ISBLANK(P22),-N22,P22-N22)</f>
+        <f t="shared" si="5"/>
         <v>392</v>
       </c>
       <c r="P22" s="1">
         <v>15786</v>
       </c>
       <c r="Q22">
-        <f>IF(ISBLANK(R22),-P22,R22-P22)</f>
+        <f t="shared" si="6"/>
         <v>321</v>
       </c>
       <c r="R22" s="1">
         <v>16107</v>
       </c>
       <c r="S22">
-        <f>IF(ISBLANK(T22),-R22,T22-R22)</f>
+        <f t="shared" si="7"/>
         <v>101</v>
       </c>
       <c r="T22" s="1">
         <v>16208</v>
       </c>
       <c r="U22">
-        <f>IF(ISBLANK(V22),-T22,V22-T22)</f>
+        <f t="shared" si="8"/>
         <v>170</v>
       </c>
       <c r="V22" s="1">
         <v>16378</v>
       </c>
       <c r="W22">
-        <f>IF(ISBLANK(X22),-V22,X22-V22)</f>
+        <f t="shared" si="9"/>
         <v>530</v>
       </c>
       <c r="X22" s="1">
         <v>16908</v>
       </c>
       <c r="Y22">
-        <f>IF(ISBLANK(Z22),-X22,Z22-X22)</f>
+        <f t="shared" si="10"/>
         <v>490</v>
       </c>
       <c r="Z22" s="1">
         <v>17398</v>
       </c>
       <c r="AA22">
-        <f>IF(ISBLANK(AB22),-Z22,AB22-Z22)</f>
+        <f t="shared" si="11"/>
         <v>329</v>
       </c>
       <c r="AB22" s="1">
         <v>17727</v>
       </c>
       <c r="AC22">
-        <f>IF(ISBLANK(AD22),-AB22,AD22-AB22)</f>
+        <f t="shared" si="12"/>
         <v>749</v>
       </c>
       <c r="AD22" s="1">
         <v>18476</v>
       </c>
       <c r="AE22">
-        <f>IF(ISBLANK(AF22),-AD22,AF22-AD22)</f>
+        <f t="shared" si="13"/>
         <v>-18476</v>
       </c>
       <c r="AF22" s="1">
         <v>0</v>
       </c>
       <c r="AG22">
-        <f>IF(ISBLANK(AH22),-AF22,AH22-AF22)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AH22" s="1">
         <v>0</v>
       </c>
       <c r="AI22">
-        <f>IF(ISBLANK(AJ22),-AH22,AJ22-AH22)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AJ22" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK22">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AL22" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>3</v>
       </c>
@@ -10537,119 +10669,126 @@
         <v>81741</v>
       </c>
       <c r="E23">
-        <f>IF(ISBLANK(F23),-D23,F23-D23)</f>
+        <f t="shared" si="0"/>
         <v>253</v>
       </c>
       <c r="F23" s="1">
         <v>81994</v>
       </c>
       <c r="G23">
-        <f>IF(ISBLANK(H23),-F23,H23-F23)</f>
+        <f t="shared" si="1"/>
         <v>130</v>
       </c>
       <c r="H23" s="1">
         <v>82124</v>
       </c>
       <c r="I23">
-        <f>IF(ISBLANK(J23),-H23,J23-H23)</f>
+        <f t="shared" si="2"/>
         <v>211</v>
       </c>
       <c r="J23" s="1">
         <v>82335</v>
       </c>
       <c r="K23">
-        <f>IF(ISBLANK(L23),-J23,L23-J23)</f>
+        <f t="shared" si="3"/>
         <v>323</v>
       </c>
       <c r="L23" s="1">
         <v>82658</v>
       </c>
       <c r="M23">
-        <f>IF(ISBLANK(N23),-L23,N23-L23)</f>
+        <f t="shared" si="4"/>
         <v>206</v>
       </c>
       <c r="N23" s="1">
         <v>82864</v>
       </c>
       <c r="O23">
-        <f>IF(ISBLANK(P23),-N23,P23-N23)</f>
+        <f t="shared" si="5"/>
         <v>556</v>
       </c>
       <c r="P23" s="1">
         <v>83420</v>
       </c>
       <c r="Q23">
-        <f>IF(ISBLANK(R23),-P23,R23-P23)</f>
+        <f t="shared" si="6"/>
         <v>351</v>
       </c>
       <c r="R23" s="1">
         <v>83771</v>
       </c>
       <c r="S23">
-        <f>IF(ISBLANK(T23),-R23,T23-R23)</f>
+        <f t="shared" si="7"/>
         <v>217</v>
       </c>
       <c r="T23" s="1">
         <v>83988</v>
       </c>
       <c r="U23">
-        <f>IF(ISBLANK(V23),-T23,V23-T23)</f>
+        <f t="shared" si="8"/>
         <v>247</v>
       </c>
       <c r="V23" s="1">
         <v>84235</v>
       </c>
       <c r="W23">
-        <f>IF(ISBLANK(X23),-V23,X23-V23)</f>
+        <f t="shared" si="9"/>
         <v>1001</v>
       </c>
       <c r="X23" s="1">
         <v>85236</v>
       </c>
       <c r="Y23">
-        <f>IF(ISBLANK(Z23),-X23,Z23-X23)</f>
+        <f t="shared" si="10"/>
         <v>2333</v>
       </c>
       <c r="Z23" s="1">
         <v>87569</v>
       </c>
       <c r="AA23">
-        <f>IF(ISBLANK(AB23),-Z23,AB23-Z23)</f>
+        <f t="shared" si="11"/>
         <v>1190</v>
       </c>
       <c r="AB23" s="1">
         <v>88759</v>
       </c>
       <c r="AC23">
-        <f>IF(ISBLANK(AD23),-AB23,AD23-AB23)</f>
+        <f t="shared" si="12"/>
         <v>1476</v>
       </c>
       <c r="AD23" s="1">
         <v>90235</v>
       </c>
       <c r="AE23">
-        <f>IF(ISBLANK(AF23),-AD23,AF23-AD23)</f>
+        <f t="shared" si="13"/>
         <v>5545</v>
       </c>
       <c r="AF23" s="1">
         <v>95780</v>
       </c>
       <c r="AG23">
-        <f>IF(ISBLANK(AH23),-AF23,AH23-AF23)</f>
+        <f t="shared" si="14"/>
         <v>5945</v>
       </c>
       <c r="AH23" s="1">
         <v>101725</v>
       </c>
       <c r="AI23">
-        <f>IF(ISBLANK(AJ23),-AH23,AJ23-AH23)</f>
+        <f t="shared" si="15"/>
         <v>7424</v>
       </c>
       <c r="AJ23" s="1">
         <v>109149</v>
       </c>
-    </row>
-    <row r="24" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK23">
+        <f t="shared" si="15"/>
+        <v>3292</v>
+      </c>
+      <c r="AL23">
+        <v>112441</v>
+      </c>
+    </row>
+    <row r="24" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>18</v>
       </c>
@@ -10660,119 +10799,126 @@
         <v>3286</v>
       </c>
       <c r="E24">
-        <f>IF(ISBLANK(F24),-D24,F24-D24)</f>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="F24" s="1">
         <v>3307</v>
       </c>
       <c r="G24">
-        <f>IF(ISBLANK(H24),-F24,H24-F24)</f>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="H24" s="1">
         <v>3320</v>
       </c>
       <c r="I24">
-        <f>IF(ISBLANK(J24),-H24,J24-H24)</f>
+        <f t="shared" si="2"/>
         <v>232</v>
       </c>
       <c r="J24" s="1">
         <v>3552</v>
       </c>
       <c r="K24">
-        <f>IF(ISBLANK(L24),-J24,L24-J24)</f>
+        <f t="shared" si="3"/>
         <v>102</v>
       </c>
       <c r="L24" s="1">
         <v>3654</v>
       </c>
       <c r="M24">
-        <f>IF(ISBLANK(N24),-L24,N24-L24)</f>
+        <f t="shared" si="4"/>
         <v>60</v>
       </c>
       <c r="N24" s="1">
         <v>3714</v>
       </c>
       <c r="O24">
-        <f>IF(ISBLANK(P24),-N24,P24-N24)</f>
+        <f t="shared" si="5"/>
         <v>-3714</v>
       </c>
       <c r="P24" s="1">
         <v>0</v>
       </c>
       <c r="Q24">
-        <f>IF(ISBLANK(R24),-P24,R24-P24)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="R24" s="1">
         <v>0</v>
       </c>
       <c r="S24">
-        <f>IF(ISBLANK(T24),-R24,T24-R24)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="T24" s="1">
         <v>0</v>
       </c>
       <c r="U24">
-        <f>IF(ISBLANK(V24),-T24,V24-T24)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="V24" s="1">
         <v>0</v>
       </c>
       <c r="W24">
-        <f>IF(ISBLANK(X24),-V24,X24-V24)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="X24" s="1">
         <v>0</v>
       </c>
       <c r="Y24">
-        <f>IF(ISBLANK(Z24),-X24,Z24-X24)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Z24" s="1">
         <v>0</v>
       </c>
       <c r="AA24">
-        <f>IF(ISBLANK(AB24),-Z24,AB24-Z24)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AB24" s="1">
         <v>0</v>
       </c>
       <c r="AC24">
-        <f>IF(ISBLANK(AD24),-AB24,AD24-AB24)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AD24" s="1">
         <v>0</v>
       </c>
       <c r="AE24">
-        <f>IF(ISBLANK(AF24),-AD24,AF24-AD24)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AF24" s="1">
         <v>0</v>
       </c>
       <c r="AG24">
-        <f>IF(ISBLANK(AH24),-AF24,AH24-AF24)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AH24" s="1">
         <v>0</v>
       </c>
       <c r="AI24">
-        <f>IF(ISBLANK(AJ24),-AH24,AJ24-AH24)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AJ24" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK24">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AL24" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>147</v>
       </c>
@@ -10865,24 +11011,24 @@
         <v>261</v>
       </c>
     </row>
-    <row r="27" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>148</v>
       </c>
       <c r="E27">
-        <f t="shared" ref="E27:E48" si="0">FIND(",",B27)</f>
+        <f t="shared" ref="E27:E48" si="16">FIND(",",B27)</f>
         <v>9</v>
       </c>
       <c r="F27" t="str">
-        <f t="shared" ref="F27:F48" si="1">LEFT(B27,E27-1)</f>
+        <f t="shared" ref="F27:F48" si="17">LEFT(B27,E27-1)</f>
         <v>Kelleher</v>
       </c>
       <c r="G27" t="str">
-        <f t="shared" ref="G27:G48" si="2">RIGHT(B27,LEN(B27)-(E27+1))</f>
+        <f t="shared" ref="G27:G48" si="18">RIGHT(B27,LEN(B27)-(E27+1))</f>
         <v>Billy</v>
       </c>
       <c r="H27" t="str">
-        <f t="shared" ref="H27:H48" si="3">G27&amp;" "&amp;F27</f>
+        <f t="shared" ref="H27:H48" si="19">G27&amp;" "&amp;F27</f>
         <v>Billy Kelleher</v>
       </c>
       <c r="J27" t="s">
@@ -10928,24 +11074,24 @@
         <v>119883</v>
       </c>
     </row>
-    <row r="28" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>149</v>
       </c>
       <c r="E28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="16"/>
         <v>8</v>
       </c>
       <c r="F28" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="17"/>
         <v>Wallace</v>
       </c>
       <c r="G28" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="18"/>
         <v>Mick</v>
       </c>
       <c r="H28" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="19"/>
         <v>Mick Wallace</v>
       </c>
       <c r="J28" t="s">
@@ -11018,24 +11164,24 @@
       <c r="AI28" s="1"/>
       <c r="AJ28" s="1"/>
     </row>
-    <row r="29" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>150</v>
       </c>
       <c r="E29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="16"/>
         <v>9</v>
       </c>
       <c r="F29" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="17"/>
         <v>Ní Riada</v>
       </c>
       <c r="G29" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="18"/>
         <v>Liadh</v>
       </c>
       <c r="H29" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="19"/>
         <v>Liadh Ní Riada</v>
       </c>
       <c r="J29" t="s">
@@ -11108,24 +11254,24 @@
       <c r="AI29" s="1"/>
       <c r="AJ29" s="1"/>
     </row>
-    <row r="30" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>151</v>
       </c>
       <c r="E30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="16"/>
         <v>11</v>
       </c>
       <c r="F30" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="17"/>
         <v>O'Sullivan</v>
       </c>
       <c r="G30" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="18"/>
         <v>Grace</v>
       </c>
       <c r="H30" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="19"/>
         <v>Grace O'Sullivan</v>
       </c>
       <c r="J30" t="s">
@@ -11198,24 +11344,24 @@
       <c r="AI30" s="1"/>
       <c r="AJ30" s="1"/>
     </row>
-    <row r="31" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>152</v>
       </c>
       <c r="E31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="16"/>
         <v>6</v>
       </c>
       <c r="F31" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="17"/>
         <v>Byrne</v>
       </c>
       <c r="G31" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="18"/>
         <v>Malcolm</v>
       </c>
       <c r="H31" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="19"/>
         <v>Malcolm Byrne</v>
       </c>
       <c r="J31" t="s">
@@ -11288,24 +11434,24 @@
       <c r="AI31" s="1"/>
       <c r="AJ31" s="1"/>
     </row>
-    <row r="32" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>153</v>
       </c>
       <c r="E32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="16"/>
         <v>6</v>
       </c>
       <c r="F32" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="17"/>
         <v>Clune</v>
       </c>
       <c r="G32" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="18"/>
         <v>Deirdre</v>
       </c>
       <c r="H32" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="19"/>
         <v>Deirdre Clune</v>
       </c>
       <c r="J32" t="s">
@@ -11380,19 +11526,19 @@
         <v>154</v>
       </c>
       <c r="E33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="16"/>
         <v>6</v>
       </c>
       <c r="F33" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="17"/>
         <v>Doyle</v>
       </c>
       <c r="G33" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="18"/>
         <v>Andrew</v>
       </c>
       <c r="H33" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="19"/>
         <v>Andrew Doyle</v>
       </c>
       <c r="J33" t="s">
@@ -11470,19 +11616,19 @@
         <v>155</v>
       </c>
       <c r="E34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="16"/>
         <v>6</v>
       </c>
       <c r="F34" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="17"/>
         <v>Nunan</v>
       </c>
       <c r="G34" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="18"/>
         <v>Sheila</v>
       </c>
       <c r="H34" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="19"/>
         <v>Sheila Nunan</v>
       </c>
       <c r="J34" t="s">
@@ -11554,19 +11700,19 @@
         <v>156</v>
       </c>
       <c r="E35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="16"/>
         <v>8</v>
       </c>
       <c r="F35" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="17"/>
         <v>Wallace</v>
       </c>
       <c r="G35" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="18"/>
         <v>Adrienne</v>
       </c>
       <c r="H35" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="19"/>
         <v>Adrienne Wallace</v>
       </c>
       <c r="J35" t="s">
@@ -11635,19 +11781,19 @@
         <v>157</v>
       </c>
       <c r="E36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="16"/>
         <v>7</v>
       </c>
       <c r="F36" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="17"/>
         <v>Cahill</v>
       </c>
       <c r="G36" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="18"/>
         <v>Dolores</v>
       </c>
       <c r="H36" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="19"/>
         <v>Dolores Cahill</v>
       </c>
       <c r="J36" t="s">
@@ -11716,19 +11862,19 @@
         <v>158</v>
       </c>
       <c r="E37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="16"/>
         <v>8</v>
       </c>
       <c r="F37" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="17"/>
         <v>O'Flynn</v>
       </c>
       <c r="G37" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="18"/>
         <v>Diarmuid Patrick</v>
       </c>
       <c r="H37" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="19"/>
         <v>Diarmuid Patrick O'Flynn</v>
       </c>
       <c r="J37" t="s">
@@ -11794,19 +11940,19 @@
         <v>159</v>
       </c>
       <c r="E38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="16"/>
         <v>8</v>
       </c>
       <c r="F38" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="17"/>
         <v>Minehan</v>
       </c>
       <c r="G38" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="18"/>
         <v>Liam</v>
       </c>
       <c r="H38" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="19"/>
         <v>Liam Minehan</v>
       </c>
       <c r="J38" t="s">
@@ -11866,19 +12012,19 @@
         <v>160</v>
       </c>
       <c r="E39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="16"/>
         <v>8</v>
       </c>
       <c r="F39" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="17"/>
         <v>Gardner</v>
       </c>
       <c r="G39" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="18"/>
         <v>Breda Patricia</v>
       </c>
       <c r="H39" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="19"/>
         <v>Breda Patricia Gardner</v>
       </c>
       <c r="J39" t="s">
@@ -11941,19 +12087,19 @@
         <v>161</v>
       </c>
       <c r="E40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="16"/>
         <v>7</v>
       </c>
       <c r="F40" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="17"/>
         <v>Heaney</v>
       </c>
       <c r="G40" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="18"/>
         <v>Theresa</v>
       </c>
       <c r="H40" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="19"/>
         <v>Theresa Heaney</v>
       </c>
       <c r="J40" t="s">
@@ -12014,19 +12160,19 @@
         <v>162</v>
       </c>
       <c r="E41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="16"/>
         <v>8</v>
       </c>
       <c r="F41" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="17"/>
         <v>Brennan</v>
       </c>
       <c r="G41" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="18"/>
         <v>Allan</v>
       </c>
       <c r="H41" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="19"/>
         <v>Allan Brennan</v>
       </c>
       <c r="J41" t="s">
@@ -12084,19 +12230,19 @@
         <v>163</v>
       </c>
       <c r="E42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="16"/>
         <v>11</v>
       </c>
       <c r="F42" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="17"/>
         <v>O'Loughlin</v>
       </c>
       <c r="G42" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="18"/>
         <v>Peter</v>
       </c>
       <c r="H42" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="19"/>
         <v>Peter O'Loughlin</v>
       </c>
       <c r="J42" t="s">
@@ -12150,19 +12296,19 @@
         <v>164</v>
       </c>
       <c r="E43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="16"/>
         <v>12</v>
       </c>
       <c r="F43" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="17"/>
         <v>Worthington</v>
       </c>
       <c r="G43" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="18"/>
         <v>Colleen</v>
       </c>
       <c r="H43" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="19"/>
         <v>Colleen Worthington</v>
       </c>
       <c r="J43" t="s">
@@ -12212,19 +12358,19 @@
         <v>165</v>
       </c>
       <c r="E44">
-        <f t="shared" si="0"/>
+        <f t="shared" si="16"/>
         <v>11</v>
       </c>
       <c r="F44" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="17"/>
         <v>Fitzgerald</v>
       </c>
       <c r="G44" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="18"/>
         <v>Paddy</v>
       </c>
       <c r="H44" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="19"/>
         <v>Paddy Fitzgerald</v>
       </c>
       <c r="J44" t="s">
@@ -12270,19 +12416,19 @@
         <v>166</v>
       </c>
       <c r="E45">
-        <f t="shared" si="0"/>
+        <f t="shared" si="16"/>
         <v>13</v>
       </c>
       <c r="F45" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="17"/>
         <v>Ryan-Purcell</v>
       </c>
       <c r="G45" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="18"/>
         <v>Walter</v>
       </c>
       <c r="H45" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="19"/>
         <v>Walter Ryan-Purcell</v>
       </c>
       <c r="J45" t="s">
@@ -12324,19 +12470,19 @@
         <v>167</v>
       </c>
       <c r="E46">
-        <f t="shared" si="0"/>
+        <f t="shared" si="16"/>
         <v>7</v>
       </c>
       <c r="F46" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="17"/>
         <v>Sexton</v>
       </c>
       <c r="G46" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="18"/>
         <v>Joesph</v>
       </c>
       <c r="H46" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="19"/>
         <v>Joesph Sexton</v>
       </c>
       <c r="J46" t="s">
@@ -12370,19 +12516,19 @@
         <v>168</v>
       </c>
       <c r="E47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="16"/>
         <v>7</v>
       </c>
       <c r="F47" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="17"/>
         <v>Madden</v>
       </c>
       <c r="G47" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="18"/>
         <v>Peter</v>
       </c>
       <c r="H47" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="19"/>
         <v>Peter Madden</v>
       </c>
       <c r="J47" t="s">
@@ -12409,19 +12555,19 @@
         <v>169</v>
       </c>
       <c r="E48">
-        <f t="shared" si="0"/>
+        <f t="shared" si="16"/>
         <v>11</v>
       </c>
       <c r="F48" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="17"/>
         <v>Van de Ven</v>
       </c>
       <c r="G48" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="18"/>
         <v>Jan</v>
       </c>
       <c r="H48" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="19"/>
         <v>Jan Van de Ven</v>
       </c>
       <c r="J48" t="s">

</xml_diff>

<commit_message>
Corrected Stage 13 midlands Added stage 20 south Signed-off-by: Gerry Mulvenna <git@movingwifi.com>
</commit_message>
<xml_diff>
--- a/europarl/europarl-ireland-2019.xlsx
+++ b/europarl/europarl-ireland-2019.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="14220" windowHeight="8580" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="14220" windowHeight="8580" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Candidates" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="265">
   <si>
     <t>Candidate</t>
   </si>
@@ -5173,7 +5173,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="Y2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -5511,10 +5511,10 @@
       </c>
       <c r="AA4">
         <f t="shared" si="11"/>
-        <v>-69923</v>
+        <v>8439</v>
       </c>
       <c r="AB4">
-        <v>0</v>
+        <v>78362</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
@@ -7845,13 +7845,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AN49"/>
+  <dimension ref="A1:AP49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="AI2" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="AL2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AN22" sqref="AN22"/>
+      <selection pane="bottomRight" activeCell="AO2" sqref="AO2:AP24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7860,7 +7860,7 @@
     <col min="3" max="3" width="4.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>232</v>
       </c>
@@ -7924,8 +7924,11 @@
       <c r="AN1" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AP1" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="2" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>16</v>
       </c>
@@ -8048,7 +8051,7 @@
         <v>0</v>
       </c>
       <c r="AK2">
-        <f t="shared" ref="AK2:AM24" si="16">IF(ISBLANK(AL2),-AJ2,AL2-AJ2)</f>
+        <f t="shared" ref="AK2:AO24" si="16">IF(ISBLANK(AL2),-AJ2,AL2-AJ2)</f>
         <v>0</v>
       </c>
       <c r="AL2" s="1">
@@ -8061,8 +8064,15 @@
       <c r="AN2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO2">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="AP2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>6</v>
       </c>
@@ -8198,8 +8208,15 @@
       <c r="AN3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO3">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="AP3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>11</v>
       </c>
@@ -8335,8 +8352,15 @@
       <c r="AN4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO4">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="AP4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>7</v>
       </c>
@@ -8472,8 +8496,15 @@
       <c r="AN5">
         <v>110085</v>
       </c>
-    </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO5">
+        <f t="shared" si="16"/>
+        <v>2077</v>
+      </c>
+      <c r="AP5" s="1">
+        <v>112162</v>
+      </c>
+    </row>
+    <row r="6" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>8</v>
       </c>
@@ -8609,8 +8640,15 @@
       <c r="AN6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO6">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="AP6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>19</v>
       </c>
@@ -8746,8 +8784,15 @@
       <c r="AN7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO7">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="AP7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>14</v>
       </c>
@@ -8883,8 +8928,15 @@
       <c r="AN8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO8">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="AP8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>15</v>
       </c>
@@ -9020,8 +9072,15 @@
       <c r="AN9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO9">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="AP9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2</v>
       </c>
@@ -9157,8 +9216,15 @@
       <c r="AN10" s="1">
         <v>119866</v>
       </c>
-    </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO10">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="AP10" s="1">
+        <v>119866</v>
+      </c>
+    </row>
+    <row r="11" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
@@ -9294,8 +9360,15 @@
       <c r="AN11" s="1">
         <v>119883</v>
       </c>
-    </row>
-    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO11">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="AP11" s="1">
+        <v>119883</v>
+      </c>
+    </row>
+    <row r="12" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>22</v>
       </c>
@@ -9431,8 +9504,15 @@
       <c r="AN12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO12">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="AP12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>13</v>
       </c>
@@ -9568,8 +9648,15 @@
       <c r="AN13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO13">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="AP13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>4</v>
       </c>
@@ -9705,8 +9792,15 @@
       <c r="AN14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO14">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="AP14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>9</v>
       </c>
@@ -9842,8 +9936,15 @@
       <c r="AN15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO15">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="AP15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>12</v>
       </c>
@@ -9979,8 +10080,15 @@
       <c r="AN16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO16">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="AP16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>17</v>
       </c>
@@ -10116,8 +10224,15 @@
       <c r="AN17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO17">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="AP17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>5</v>
       </c>
@@ -10253,8 +10368,15 @@
       <c r="AN18">
         <v>114287</v>
       </c>
-    </row>
-    <row r="19" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO18">
+        <f t="shared" si="16"/>
+        <v>5414</v>
+      </c>
+      <c r="AP18" s="1">
+        <v>119701</v>
+      </c>
+    </row>
+    <row r="19" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>20</v>
       </c>
@@ -10390,8 +10512,15 @@
       <c r="AN19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO19">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="AP19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>21</v>
       </c>
@@ -10527,8 +10656,15 @@
       <c r="AN20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO20">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="AP20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>23</v>
       </c>
@@ -10664,8 +10800,15 @@
       <c r="AN21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO21">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="AP21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>10</v>
       </c>
@@ -10801,8 +10944,15 @@
       <c r="AN22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO22">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="AP22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>3</v>
       </c>
@@ -10938,8 +11088,15 @@
       <c r="AN23">
         <v>139529</v>
       </c>
-    </row>
-    <row r="24" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO23">
+        <f t="shared" si="16"/>
+        <v>-19663</v>
+      </c>
+      <c r="AP23" s="1">
+        <v>119866</v>
+      </c>
+    </row>
+    <row r="24" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>18</v>
       </c>
@@ -11075,8 +11232,15 @@
       <c r="AN24">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO24">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="AP24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:42" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>147</v>
       </c>
@@ -11169,7 +11333,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="27" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:42" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>148</v>
       </c>
@@ -11232,7 +11396,7 @@
         <v>119883</v>
       </c>
     </row>
-    <row r="28" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:42" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>149</v>
       </c>
@@ -11322,7 +11486,7 @@
       <c r="AI28" s="1"/>
       <c r="AJ28" s="1"/>
     </row>
-    <row r="29" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:42" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>150</v>
       </c>
@@ -11412,7 +11576,7 @@
       <c r="AI29" s="1"/>
       <c r="AJ29" s="1"/>
     </row>
-    <row r="30" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:42" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>151</v>
       </c>
@@ -11502,7 +11666,7 @@
       <c r="AI30" s="1"/>
       <c r="AJ30" s="1"/>
     </row>
-    <row r="31" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:42" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>152</v>
       </c>
@@ -11592,7 +11756,7 @@
       <c r="AI31" s="1"/>
       <c r="AJ31" s="1"/>
     </row>
-    <row r="32" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:42" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>153</v>
       </c>

</xml_diff>

<commit_message>
Surname Van de Ven corrected in south Signed-off-by: Gerry Mulvenna <git@movingwifi.com>
</commit_message>
<xml_diff>
--- a/europarl/europarl-ireland-2019.xlsx
+++ b/europarl/europarl-ireland-2019.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="14220" windowHeight="8580" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="14220" windowHeight="8580" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Candidates" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="266">
   <si>
     <t>Candidate</t>
   </si>
@@ -812,6 +812,9 @@
   </si>
   <si>
     <t>Count 19</t>
+  </si>
+  <si>
+    <t>Count 20</t>
   </si>
 </sst>
 </file>
@@ -5173,7 +5176,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="Y2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -7847,11 +7850,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AP49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="AL2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="AN2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AO2" sqref="AO2:AP24"/>
+      <selection pane="bottomRight" activeCell="D2" sqref="D2:AP24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7925,7 +7928,7 @@
         <v>264</v>
       </c>
       <c r="AP1" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="2" spans="1:42" x14ac:dyDescent="0.25">

</xml_diff>